<commit_message>
start adding in the LED operations
</commit_message>
<xml_diff>
--- a/RBG_arduino/StateTable_minimal.xlsx
+++ b/RBG_arduino/StateTable_minimal.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub-Mark-MDO47\RubberBandGun\RBG_arduino\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9DBFFBF9-61DF-4421-8931-4022E349AF88}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C9F1E84-71AF-414A-8D77-5DFFF27DB7BD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="690" yWindow="690" windowWidth="32760" windowHeight="16875" xr2:uid="{CCADFEE4-B0E1-4363-9617-1683960BED03}"/>
   </bookViews>
@@ -681,7 +681,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C4" sqref="C4"/>
+      <selection pane="bottomLeft" activeCell="F1" sqref="F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
make use of state table to simplify special handlers
</commit_message>
<xml_diff>
--- a/RBG_arduino/StateTable_minimal.xlsx
+++ b/RBG_arduino/StateTable_minimal.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub-Mark-MDO47\RubberBandGun\RBG_arduino\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1234B7B4-6FE4-4824-8353-A705EEDC1864}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{634CB5ED-7638-4D8C-92ED-20DB2CBC470F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4935" yWindow="2025" windowWidth="32760" windowHeight="16875" xr2:uid="{CCADFEE4-B0E1-4363-9617-1683960BED03}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="79">
   <si>
     <t>trigOnly</t>
   </si>
@@ -238,6 +238,36 @@
   </si>
   <si>
     <t>mROW_LOKLOD</t>
+  </si>
+  <si>
+    <t>mROW_SHOOT</t>
+  </si>
+  <si>
+    <t>mROW_SHOOT_WINDUP</t>
+  </si>
+  <si>
+    <t>mEFCT_SHOOT</t>
+  </si>
+  <si>
+    <t>mEFCT_WIND_UP</t>
+  </si>
+  <si>
+    <t>mROW_SOLENOID</t>
+  </si>
+  <si>
+    <t>mSPCL_HANDLER | mSPCL_HANDLER_SOLENOID</t>
+  </si>
+  <si>
+    <t>… and the WINDUP</t>
+  </si>
+  <si>
+    <t>POW!!!</t>
+  </si>
+  <si>
+    <t>release solenoid</t>
+  </si>
+  <si>
+    <t>mEFCT_UNIQ_SILENCE</t>
   </si>
 </sst>
 </file>
@@ -683,17 +713,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{90E8DFC6-94F4-4A82-A874-2F16F2CF0145}">
-  <dimension ref="A1:R13"/>
+  <dimension ref="A1:R17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I2" sqref="I2:J10"/>
+      <selection pane="bottomLeft" activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="22.85546875" customWidth="1"/>
-    <col min="2" max="2" width="26.5703125" customWidth="1"/>
+    <col min="2" max="2" width="26.7109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="18.7109375" bestFit="1" customWidth="1"/>
     <col min="4" max="5" width="42.5703125" customWidth="1"/>
     <col min="6" max="6" width="10" bestFit="1" customWidth="1"/>
@@ -827,9 +857,6 @@
     </row>
     <row r="4" spans="1:18" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" s="9"/>
-      <c r="B4" s="10" t="s">
-        <v>62</v>
-      </c>
       <c r="C4" s="9" t="s">
         <v>65</v>
       </c>
@@ -844,8 +871,8 @@
       </c>
       <c r="G4" s="9"/>
       <c r="H4" s="9"/>
-      <c r="I4" s="9" t="s">
-        <v>65</v>
+      <c r="I4" t="s">
+        <v>70</v>
       </c>
       <c r="J4" s="9"/>
       <c r="L4" t="s">
@@ -1043,6 +1070,21 @@
       </c>
     </row>
     <row r="12" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>75</v>
+      </c>
+      <c r="C12" t="s">
+        <v>70</v>
+      </c>
+      <c r="D12" t="s">
+        <v>72</v>
+      </c>
+      <c r="E12" t="s">
+        <v>72</v>
+      </c>
+      <c r="J12" t="s">
+        <v>69</v>
+      </c>
       <c r="L12" s="4" t="s">
         <v>19</v>
       </c>
@@ -1052,6 +1094,49 @@
     </row>
     <row r="13" spans="1:18" x14ac:dyDescent="0.25">
       <c r="N13" s="7"/>
+    </row>
+    <row r="14" spans="1:18" ht="30" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>76</v>
+      </c>
+      <c r="B14" s="10" t="s">
+        <v>62</v>
+      </c>
+      <c r="C14" t="s">
+        <v>69</v>
+      </c>
+      <c r="D14" t="s">
+        <v>71</v>
+      </c>
+      <c r="E14" t="s">
+        <v>71</v>
+      </c>
+      <c r="J14" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="16" spans="1:18" ht="30" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>77</v>
+      </c>
+      <c r="B16" s="10" t="s">
+        <v>74</v>
+      </c>
+      <c r="C16" t="s">
+        <v>73</v>
+      </c>
+      <c r="D16" t="s">
+        <v>78</v>
+      </c>
+      <c r="E16" t="s">
+        <v>78</v>
+      </c>
+      <c r="J16" s="9" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="17" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B17" s="10"/>
     </row>
   </sheetData>
   <sortState ref="R3:R52">

</xml_diff>

<commit_message>
skeletons for RBG_specialProcSolenoid() and RBG_specialProcShoot()
</commit_message>
<xml_diff>
--- a/RBG_arduino/StateTable_minimal.xlsx
+++ b/RBG_arduino/StateTable_minimal.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub-Mark-MDO47\RubberBandGun\RBG_arduino\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{634CB5ED-7638-4D8C-92ED-20DB2CBC470F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F58B3E4-3267-4B7D-89E4-E7D793BBCC56}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4935" yWindow="2025" windowWidth="32760" windowHeight="16875" xr2:uid="{CCADFEE4-B0E1-4363-9617-1683960BED03}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="81">
   <si>
     <t>trigOnly</t>
   </si>
@@ -243,9 +243,6 @@
     <t>mROW_SHOOT</t>
   </si>
   <si>
-    <t>mROW_SHOOT_WINDUP</t>
-  </si>
-  <si>
     <t>mEFCT_SHOOT</t>
   </si>
   <si>
@@ -267,7 +264,16 @@
     <t>release solenoid</t>
   </si>
   <si>
-    <t>mEFCT_UNIQ_SILENCE</t>
+    <t>mROW_SHOOT_SOUND</t>
+  </si>
+  <si>
+    <t>POW SOUND</t>
+  </si>
+  <si>
+    <t>mROW_WINDUP</t>
+  </si>
+  <si>
+    <t>mROW_WINDUP_SOUND</t>
   </si>
 </sst>
 </file>
@@ -713,24 +719,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{90E8DFC6-94F4-4A82-A874-2F16F2CF0145}">
-  <dimension ref="A1:R17"/>
+  <dimension ref="A1:R22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E16" sqref="E16"/>
+      <selection pane="bottomLeft" activeCell="D21" sqref="D21:E21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="22.85546875" customWidth="1"/>
     <col min="2" max="2" width="26.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="23.28515625" bestFit="1" customWidth="1"/>
     <col min="4" max="5" width="42.5703125" customWidth="1"/>
     <col min="6" max="6" width="10" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="13.7109375" customWidth="1"/>
     <col min="8" max="8" width="20" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="16" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="17.42578125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="23.5703125" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="8" customWidth="1"/>
     <col min="12" max="12" width="19.28515625" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="16" bestFit="1" customWidth="1"/>
@@ -872,7 +878,7 @@
       <c r="G4" s="9"/>
       <c r="H4" s="9"/>
       <c r="I4" t="s">
-        <v>70</v>
+        <v>79</v>
       </c>
       <c r="J4" s="9"/>
       <c r="L4" t="s">
@@ -1071,19 +1077,13 @@
     </row>
     <row r="12" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C12" t="s">
-        <v>70</v>
-      </c>
-      <c r="D12" t="s">
-        <v>72</v>
-      </c>
-      <c r="E12" t="s">
-        <v>72</v>
+        <v>79</v>
       </c>
       <c r="J12" t="s">
-        <v>69</v>
+        <v>80</v>
       </c>
       <c r="L12" s="4" t="s">
         <v>19</v>
@@ -1093,17 +1093,12 @@
       </c>
     </row>
     <row r="13" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="N13" s="7"/>
-    </row>
-    <row r="14" spans="1:18" ht="30" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>76</v>
-      </c>
-      <c r="B14" s="10" t="s">
-        <v>62</v>
-      </c>
+      <c r="L13" s="4"/>
+      <c r="M13" s="4"/>
+    </row>
+    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
       <c r="C14" t="s">
-        <v>69</v>
+        <v>80</v>
       </c>
       <c r="D14" t="s">
         <v>71</v>
@@ -1112,35 +1107,72 @@
         <v>71</v>
       </c>
       <c r="J14" t="s">
-        <v>73</v>
-      </c>
+        <v>69</v>
+      </c>
+      <c r="L14" s="4"/>
+      <c r="M14" s="4"/>
+    </row>
+    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="N15" s="7"/>
     </row>
     <row r="16" spans="1:18" ht="30" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
+        <v>75</v>
+      </c>
+      <c r="B16" s="10" t="s">
+        <v>62</v>
+      </c>
+      <c r="C16" t="s">
+        <v>69</v>
+      </c>
+      <c r="J16" t="s">
         <v>77</v>
       </c>
-      <c r="B16" s="10" t="s">
-        <v>74</v>
-      </c>
-      <c r="C16" t="s">
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B17" s="10"/>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>78</v>
+      </c>
+      <c r="B18" s="10"/>
+      <c r="C18" t="s">
+        <v>77</v>
+      </c>
+      <c r="D18" t="s">
+        <v>70</v>
+      </c>
+      <c r="E18" t="s">
+        <v>70</v>
+      </c>
+      <c r="J18" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B19" s="10"/>
+    </row>
+    <row r="21" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>76</v>
+      </c>
+      <c r="B21" s="10" t="s">
         <v>73</v>
       </c>
-      <c r="D16" t="s">
-        <v>78</v>
-      </c>
-      <c r="E16" t="s">
-        <v>78</v>
-      </c>
-      <c r="J16" s="9" t="s">
+      <c r="C21" t="s">
+        <v>72</v>
+      </c>
+      <c r="J21" s="9" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="17" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B17" s="10"/>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B22" s="10"/>
     </row>
   </sheetData>
-  <sortState ref="R3:R52">
-    <sortCondition ref="R3:R52"/>
+  <sortState ref="R3:R57">
+    <sortCondition ref="R3:R57"/>
   </sortState>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
still debugging special processing
</commit_message>
<xml_diff>
--- a/RBG_arduino/StateTable_minimal.xlsx
+++ b/RBG_arduino/StateTable_minimal.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub-Mark-MDO47\RubberBandGun\RBG_arduino\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72351FAB-EF98-4700-9B01-0FFECB6F737A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B70DBDA-9E94-4F9C-B781-6E68EEB1F516}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="435" yWindow="1155" windowWidth="17460" windowHeight="19170" activeTab="2" xr2:uid="{CCADFEE4-B0E1-4363-9617-1683960BED03}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21840" activeTab="1" xr2:uid="{CCADFEE4-B0E1-4363-9617-1683960BED03}"/>
   </bookViews>
   <sheets>
     <sheet name="StateTable" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2199" uniqueCount="1797">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2363" uniqueCount="1856">
   <si>
     <t>trigOnly</t>
   </si>
@@ -5441,6 +5441,183 @@
   </si>
   <si>
     <t>18177:DEBUG loop() - nowVinputRBG 0x40 loo</t>
+  </si>
+  <si>
+    <t>disable ACK and turn off loop command and shorten timeout</t>
+  </si>
+  <si>
+    <t>29:DEBUG loop() - nowVinputRBG 0x40 loopCount 0</t>
+  </si>
+  <si>
+    <t>32: RBG_startEffectSound ln 485 EFCT num 0x28 final num 41 loopCount 0</t>
+  </si>
+  <si>
+    <t>33: RBG_startEffectSound ln 519 myDFPlayer problem after check busy</t>
+  </si>
+  <si>
+    <t>891:DEBUG loop() - nowVinputRBG 0x40 loopCount 748</t>
+  </si>
+  <si>
+    <t>900: RBG_startRow ln 275 from row 0 to row 1 loopCount 749</t>
+  </si>
+  <si>
+    <t>903: RBG_startEffectSound ln 485 EFCT num 0x66 final num 102 loopCount 749</t>
+  </si>
+  <si>
+    <t>904: RBG_startEffectSound ln 512 myDFPlayer problem after play</t>
+  </si>
+  <si>
+    <t>905:Number:48 Play Finished!</t>
+  </si>
+  <si>
+    <t>906: RBG_startEffectSound ln 519 myDFPlayer problem after check busy</t>
+  </si>
+  <si>
+    <t>907:Number:48 Play Finished!</t>
+  </si>
+  <si>
+    <t>936: RBG_startEffectSound ln 470 wait msec 100 AUDIO_BUSY LOW</t>
+  </si>
+  <si>
+    <t>938: RBG_startEffectSound ln 485 EFCT num 0x66 final num 102 loopCount 750</t>
+  </si>
+  <si>
+    <t>940:DEBUG loop() - nowVinputRBG 0x240 loopCount 751</t>
+  </si>
+  <si>
+    <t>4645:DEBUG loop() - nowVinputRBG 0x40 loopCount 946</t>
+  </si>
+  <si>
+    <t>4664: RBG_startEffectSound ln 485 EFCT num 0x66 final num 102 loopCount 946</t>
+  </si>
+  <si>
+    <t>4665: RBG_startEffectSound ln 512 myDFPlayer problem after play</t>
+  </si>
+  <si>
+    <t>4666:Number:51 Play Finished!</t>
+  </si>
+  <si>
+    <t>4667: RBG_startEffectSound ln 519 myDFPlayer problem after check busy</t>
+  </si>
+  <si>
+    <t>4668:Number:51 Play Finished!</t>
+  </si>
+  <si>
+    <t>4689: RBG_startEffectSound ln 470 wait msec 100 AUDIO_BUSY LOW</t>
+  </si>
+  <si>
+    <t>4691: RBG_startEffectSound ln 485 EFCT num 0x66 final num 102 loopCount 947</t>
+  </si>
+  <si>
+    <t>4693:DEBUG loop() - nowVinputRBG 0x240 loopCount 948</t>
+  </si>
+  <si>
+    <t>4712:DEBUG loop() - nowVinputRBG 0x40 loopCount 949</t>
+  </si>
+  <si>
+    <t>4731: RBG_startEffectSound ln 470 wait msec 100 AUDIO_BUSY LOW</t>
+  </si>
+  <si>
+    <t>4733: RBG_startEffectSound ln 485 EFCT num 0x66 final num 102 loopCount 949</t>
+  </si>
+  <si>
+    <t>4735:DEBUG loop() - nowVinputRBG 0x240 loopCount 950</t>
+  </si>
+  <si>
+    <t>8421:DEBUG loop() - nowVinputRBG 0x40 loopCount 1144</t>
+  </si>
+  <si>
+    <t>8440: RBG_startEffectSound ln 485 EFCT num 0x66 final num 102 loopCount 1144</t>
+  </si>
+  <si>
+    <t>8441: RBG_startEffectSound ln 512 myDFPlayer problem after play</t>
+  </si>
+  <si>
+    <t>8442:Number:51 Play Finished!</t>
+  </si>
+  <si>
+    <t>8443: RBG_startEffectSound ln 519 myDFPlayer problem after check busy</t>
+  </si>
+  <si>
+    <t>8444:Number:51 Play Finished!</t>
+  </si>
+  <si>
+    <t>8465: RBG_startEffectSound ln 470 wait msec 100 AUDIO_BUSY LOW</t>
+  </si>
+  <si>
+    <t>8467: RBG_startEffectSound ln 485 EFCT num 0x66 final num 102 loopCount 1145</t>
+  </si>
+  <si>
+    <t>8469:DEBUG loop() - nowVinputRBG 0x240 loopCount 1146</t>
+  </si>
+  <si>
+    <t>8488:DEBUG loop() - nowVinputRBG 0x40 loopCount 1147</t>
+  </si>
+  <si>
+    <t>8507: RBG_startEffectSound ln 470 wait msec 100 AUDIO_BUSY LOW</t>
+  </si>
+  <si>
+    <t>8509: RBG_startEffectSound ln 485 EFCT num 0x66 final num 102 loopCount 1147</t>
+  </si>
+  <si>
+    <t>8511:DEBUG loop() - nowVinputRBG 0x240 loopCount 1148</t>
+  </si>
+  <si>
+    <t>11342:DEBUG loop() - nowVinputRBG 0x260 loopCount 1297</t>
+  </si>
+  <si>
+    <t>11359: RBG_startRow ln 275 from row 1 to row 4 loopCount 1298</t>
+  </si>
+  <si>
+    <t>11362: RBG_startEffectSound ln 470 wait msec 100 AUDIO_BUSY LOW</t>
+  </si>
+  <si>
+    <t>11364: RBG_startEffectSound ln 485 EFCT num 0x0 final num 1 loopCount 1298</t>
+  </si>
+  <si>
+    <t>11375:DEBUG loop() - nowVinputRBG 0x40 loopCount 1299</t>
+  </si>
+  <si>
+    <t>11384: RBG_startRow ln 275 from row 4 to row 7 loopCount 1300</t>
+  </si>
+  <si>
+    <t>11385: RBG_startEffectSound ln 470 wait msec 100 AUDIO_BUSY LOW</t>
+  </si>
+  <si>
+    <t>11394:DEBUG loop() - nowVinputRBG 0x240 loopCount 1301</t>
+  </si>
+  <si>
+    <t>14535:DEBUG loop() - nowVinputRBG 0x40 loopCount 4442</t>
+  </si>
+  <si>
+    <t>16769:DEBUG loop() - nowVinputRBG 0x60 loopCount 6676</t>
+  </si>
+  <si>
+    <t>16844:DEBUG loop() - nowVinputRBG 0x40 loopCount 6751</t>
+  </si>
+  <si>
+    <t>go from 0 to 1</t>
+  </si>
+  <si>
+    <t>go from 1 to 1</t>
+  </si>
+  <si>
+    <t>go from 1 to 4</t>
+  </si>
+  <si>
+    <t>go from 4 to 7</t>
+  </si>
+  <si>
+    <t>mVINP_LOCK|mVINP_SOUNDACTV</t>
+  </si>
+  <si>
+    <t>mVINP_LOCK|mVINP_SOUNDACTV|mVINP_TRIG</t>
+  </si>
+  <si>
+    <t>mVINP_LOCK|mVINP_TRIG</t>
+  </si>
+  <si>
+    <t>// special processing should happen in exactly one call, then we move on to .gotoWithoutInput</t>
   </si>
 </sst>
 </file>
@@ -6001,7 +6178,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E30" sqref="E30"/>
+      <selection pane="bottomLeft" activeCell="J19" sqref="J19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6471,10 +6648,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0B3F56F7-7110-4AD7-8B0D-AA537E4015D5}">
-  <dimension ref="A1:C14"/>
+  <dimension ref="A1:C15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="M17" sqref="M17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6536,16 +6713,21 @@
         <v>88</v>
       </c>
     </row>
-    <row r="12" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="13" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="1" t="s">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C12" t="s">
+        <v>1855</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="14" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="C13" t="s">
+      <c r="C14" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="14" spans="1:3" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
+    <row r="15" spans="1:3" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -6553,10 +6735,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F57F550E-21B4-4ED7-B7FF-211D228584A7}">
-  <dimension ref="A1:H1572"/>
+  <dimension ref="A1:L1666"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A1510" workbookViewId="0">
-      <selection activeCell="B1567" sqref="B1566:B1567"/>
+    <sheetView topLeftCell="A1629" workbookViewId="0">
+      <selection activeCell="B1681" sqref="B1681"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -19050,11 +19232,920 @@
         <v>1796</v>
       </c>
     </row>
+    <row r="1575" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="1576" spans="1:2" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B1576" s="1" t="s">
+        <v>1797</v>
+      </c>
+    </row>
+    <row r="1577" spans="1:2" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
+    <row r="1578" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B1578" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="1579" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B1579" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="1580" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B1580" t="s">
+        <v>925</v>
+      </c>
+    </row>
+    <row r="1581" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B1581" t="s">
+        <v>926</v>
+      </c>
+    </row>
+    <row r="1582" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B1582" t="s">
+        <v>430</v>
+      </c>
+    </row>
+    <row r="1585" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1585">
+        <v>29</v>
+      </c>
+      <c r="B1585" t="s">
+        <v>1798</v>
+      </c>
+    </row>
+    <row r="1586" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1586">
+        <v>32</v>
+      </c>
+      <c r="B1586" t="s">
+        <v>1799</v>
+      </c>
+    </row>
+    <row r="1587" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1587">
+        <v>33</v>
+      </c>
+      <c r="B1587" t="s">
+        <v>1800</v>
+      </c>
+    </row>
+    <row r="1588" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1588">
+        <v>67</v>
+      </c>
+      <c r="B1588" s="25" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="1589" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1589">
+        <v>891</v>
+      </c>
+      <c r="B1589" s="25" t="s">
+        <v>1801</v>
+      </c>
+    </row>
+    <row r="1590" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1590">
+        <v>900</v>
+      </c>
+      <c r="B1590" t="s">
+        <v>1802</v>
+      </c>
+    </row>
+    <row r="1591" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1591">
+        <v>903</v>
+      </c>
+      <c r="B1591" t="s">
+        <v>1803</v>
+      </c>
+    </row>
+    <row r="1592" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1592">
+        <v>904</v>
+      </c>
+      <c r="B1592" t="s">
+        <v>1804</v>
+      </c>
+    </row>
+    <row r="1593" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1593">
+        <v>905</v>
+      </c>
+      <c r="B1593" t="s">
+        <v>1805</v>
+      </c>
+    </row>
+    <row r="1594" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1594">
+        <v>906</v>
+      </c>
+      <c r="B1594" t="s">
+        <v>1806</v>
+      </c>
+    </row>
+    <row r="1595" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1595">
+        <v>907</v>
+      </c>
+      <c r="B1595" t="s">
+        <v>1807</v>
+      </c>
+    </row>
+    <row r="1596" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1596">
+        <v>936</v>
+      </c>
+      <c r="B1596" t="s">
+        <v>1808</v>
+      </c>
+    </row>
+    <row r="1597" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1597">
+        <v>938</v>
+      </c>
+      <c r="B1597" t="s">
+        <v>1809</v>
+      </c>
+    </row>
+    <row r="1598" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1598">
+        <v>940</v>
+      </c>
+      <c r="B1598" s="25" t="s">
+        <v>1810</v>
+      </c>
+    </row>
+    <row r="1599" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1599">
+        <v>4645</v>
+      </c>
+      <c r="B1599" s="25" t="s">
+        <v>1811</v>
+      </c>
+    </row>
+    <row r="1600" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1600">
+        <v>4664</v>
+      </c>
+      <c r="B1600" t="s">
+        <v>1812</v>
+      </c>
+    </row>
+    <row r="1601" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1601">
+        <v>4665</v>
+      </c>
+      <c r="B1601" t="s">
+        <v>1813</v>
+      </c>
+    </row>
+    <row r="1602" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1602">
+        <v>4666</v>
+      </c>
+      <c r="B1602" t="s">
+        <v>1814</v>
+      </c>
+    </row>
+    <row r="1603" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1603">
+        <v>4667</v>
+      </c>
+      <c r="B1603" t="s">
+        <v>1815</v>
+      </c>
+    </row>
+    <row r="1604" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1604">
+        <v>4668</v>
+      </c>
+      <c r="B1604" t="s">
+        <v>1816</v>
+      </c>
+    </row>
+    <row r="1605" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1605">
+        <v>4689</v>
+      </c>
+      <c r="B1605" t="s">
+        <v>1817</v>
+      </c>
+    </row>
+    <row r="1606" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1606">
+        <v>4691</v>
+      </c>
+      <c r="B1606" t="s">
+        <v>1818</v>
+      </c>
+    </row>
+    <row r="1607" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1607">
+        <v>4693</v>
+      </c>
+      <c r="B1607" s="4" t="s">
+        <v>1819</v>
+      </c>
+    </row>
+    <row r="1608" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1608">
+        <v>4712</v>
+      </c>
+      <c r="B1608" s="4" t="s">
+        <v>1820</v>
+      </c>
+    </row>
+    <row r="1609" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1609">
+        <v>4731</v>
+      </c>
+      <c r="B1609" t="s">
+        <v>1821</v>
+      </c>
+    </row>
+    <row r="1610" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1610">
+        <v>4733</v>
+      </c>
+      <c r="B1610" t="s">
+        <v>1822</v>
+      </c>
+    </row>
+    <row r="1611" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1611">
+        <v>4735</v>
+      </c>
+      <c r="B1611" s="25" t="s">
+        <v>1823</v>
+      </c>
+    </row>
+    <row r="1612" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1612">
+        <v>8421</v>
+      </c>
+      <c r="B1612" s="25" t="s">
+        <v>1824</v>
+      </c>
+    </row>
+    <row r="1613" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1613">
+        <v>8440</v>
+      </c>
+      <c r="B1613" t="s">
+        <v>1825</v>
+      </c>
+    </row>
+    <row r="1614" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1614">
+        <v>8441</v>
+      </c>
+      <c r="B1614" t="s">
+        <v>1826</v>
+      </c>
+    </row>
+    <row r="1615" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1615">
+        <v>8442</v>
+      </c>
+      <c r="B1615" t="s">
+        <v>1827</v>
+      </c>
+    </row>
+    <row r="1616" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1616">
+        <v>8443</v>
+      </c>
+      <c r="B1616" t="s">
+        <v>1828</v>
+      </c>
+    </row>
+    <row r="1617" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1617">
+        <v>8444</v>
+      </c>
+      <c r="B1617" t="s">
+        <v>1829</v>
+      </c>
+    </row>
+    <row r="1618" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1618">
+        <v>8465</v>
+      </c>
+      <c r="B1618" t="s">
+        <v>1830</v>
+      </c>
+    </row>
+    <row r="1619" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1619">
+        <v>8467</v>
+      </c>
+      <c r="B1619" t="s">
+        <v>1831</v>
+      </c>
+    </row>
+    <row r="1620" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1620">
+        <v>8469</v>
+      </c>
+      <c r="B1620" s="4" t="s">
+        <v>1832</v>
+      </c>
+    </row>
+    <row r="1621" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1621">
+        <v>8488</v>
+      </c>
+      <c r="B1621" s="4" t="s">
+        <v>1833</v>
+      </c>
+    </row>
+    <row r="1622" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1622">
+        <v>8507</v>
+      </c>
+      <c r="B1622" t="s">
+        <v>1834</v>
+      </c>
+    </row>
+    <row r="1623" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1623">
+        <v>8509</v>
+      </c>
+      <c r="B1623" t="s">
+        <v>1835</v>
+      </c>
+    </row>
+    <row r="1624" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1624">
+        <v>8511</v>
+      </c>
+      <c r="B1624" s="25" t="s">
+        <v>1836</v>
+      </c>
+    </row>
+    <row r="1625" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1625">
+        <v>11342</v>
+      </c>
+      <c r="B1625" s="25" t="s">
+        <v>1837</v>
+      </c>
+    </row>
+    <row r="1626" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1626">
+        <v>11359</v>
+      </c>
+      <c r="B1626" s="16" t="s">
+        <v>1838</v>
+      </c>
+    </row>
+    <row r="1627" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1627">
+        <v>11362</v>
+      </c>
+      <c r="B1627" t="s">
+        <v>1839</v>
+      </c>
+    </row>
+    <row r="1628" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1628">
+        <v>11364</v>
+      </c>
+      <c r="B1628" s="16" t="s">
+        <v>1840</v>
+      </c>
+    </row>
+    <row r="1629" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1629">
+        <v>11375</v>
+      </c>
+      <c r="B1629" t="s">
+        <v>1841</v>
+      </c>
+    </row>
+    <row r="1630" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1630">
+        <v>11384</v>
+      </c>
+      <c r="B1630" s="16" t="s">
+        <v>1842</v>
+      </c>
+    </row>
+    <row r="1631" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1631">
+        <v>11385</v>
+      </c>
+      <c r="B1631" t="s">
+        <v>1843</v>
+      </c>
+    </row>
+    <row r="1632" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1632">
+        <v>11394</v>
+      </c>
+      <c r="B1632" s="25" t="s">
+        <v>1844</v>
+      </c>
+    </row>
+    <row r="1633" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A1633">
+        <v>14535</v>
+      </c>
+      <c r="B1633" s="25" t="s">
+        <v>1845</v>
+      </c>
+    </row>
+    <row r="1634" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A1634">
+        <v>16769</v>
+      </c>
+      <c r="B1634" t="s">
+        <v>1846</v>
+      </c>
+    </row>
+    <row r="1635" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A1635">
+        <v>16844</v>
+      </c>
+      <c r="B1635" t="s">
+        <v>1847</v>
+      </c>
+    </row>
+    <row r="1642" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B1642" t="s">
+        <v>1798</v>
+      </c>
+      <c r="C1642" t="s">
+        <v>97</v>
+      </c>
+      <c r="F1642" t="str">
+        <f>"mVINP_LOCK"&amp;IF(LEN(D1642)&gt;0,"|"&amp;D1642,"")&amp;IF(LEN(E1642)&gt;0,"|"&amp;E1642,"")</f>
+        <v>mVINP_LOCK</v>
+      </c>
+      <c r="J1642" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="1643" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B1643" t="s">
+        <v>106</v>
+      </c>
+      <c r="C1643" t="s">
+        <v>97</v>
+      </c>
+      <c r="D1643" t="s">
+        <v>96</v>
+      </c>
+      <c r="F1643" t="str">
+        <f t="shared" ref="F1643:F1666" si="8">"mVINP_LOCK"&amp;IF(LEN(D1643)&gt;0,"|"&amp;D1643,"")&amp;IF(LEN(E1643)&gt;0,"|"&amp;E1643,"")</f>
+        <v>mVINP_LOCK|mVINP_SOUNDACTV</v>
+      </c>
+      <c r="J1643" t="s">
+        <v>1852</v>
+      </c>
+    </row>
+    <row r="1644" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B1644" t="s">
+        <v>106</v>
+      </c>
+      <c r="C1644" t="s">
+        <v>97</v>
+      </c>
+      <c r="D1644" t="s">
+        <v>96</v>
+      </c>
+      <c r="F1644" t="str">
+        <f t="shared" si="8"/>
+        <v>mVINP_LOCK|mVINP_SOUNDACTV</v>
+      </c>
+      <c r="J1644" t="s">
+        <v>1852</v>
+      </c>
+    </row>
+    <row r="1645" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B1645" t="s">
+        <v>1801</v>
+      </c>
+      <c r="C1645" t="s">
+        <v>97</v>
+      </c>
+      <c r="F1645" t="str">
+        <f t="shared" si="8"/>
+        <v>mVINP_LOCK</v>
+      </c>
+      <c r="H1645" t="s">
+        <v>1848</v>
+      </c>
+      <c r="J1645" t="s">
+        <v>97</v>
+      </c>
+      <c r="L1645" t="s">
+        <v>1848</v>
+      </c>
+    </row>
+    <row r="1646" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B1646" t="s">
+        <v>1810</v>
+      </c>
+      <c r="C1646" t="s">
+        <v>97</v>
+      </c>
+      <c r="D1646" t="s">
+        <v>96</v>
+      </c>
+      <c r="F1646" t="str">
+        <f t="shared" si="8"/>
+        <v>mVINP_LOCK|mVINP_SOUNDACTV</v>
+      </c>
+      <c r="J1646" t="s">
+        <v>1852</v>
+      </c>
+    </row>
+    <row r="1647" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B1647" t="s">
+        <v>1810</v>
+      </c>
+      <c r="C1647" t="s">
+        <v>97</v>
+      </c>
+      <c r="D1647" t="s">
+        <v>96</v>
+      </c>
+      <c r="F1647" t="str">
+        <f t="shared" si="8"/>
+        <v>mVINP_LOCK|mVINP_SOUNDACTV</v>
+      </c>
+      <c r="J1647" t="s">
+        <v>1852</v>
+      </c>
+    </row>
+    <row r="1648" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B1648" t="s">
+        <v>1811</v>
+      </c>
+      <c r="C1648" t="s">
+        <v>97</v>
+      </c>
+      <c r="F1648" t="str">
+        <f t="shared" si="8"/>
+        <v>mVINP_LOCK</v>
+      </c>
+      <c r="H1648" t="s">
+        <v>1849</v>
+      </c>
+      <c r="J1648" t="s">
+        <v>97</v>
+      </c>
+      <c r="L1648" t="s">
+        <v>1849</v>
+      </c>
+    </row>
+    <row r="1649" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B1649" t="s">
+        <v>1819</v>
+      </c>
+      <c r="C1649" t="s">
+        <v>97</v>
+      </c>
+      <c r="D1649" t="s">
+        <v>96</v>
+      </c>
+      <c r="F1649" t="str">
+        <f t="shared" si="8"/>
+        <v>mVINP_LOCK|mVINP_SOUNDACTV</v>
+      </c>
+      <c r="J1649" t="s">
+        <v>1852</v>
+      </c>
+    </row>
+    <row r="1650" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B1650" t="s">
+        <v>1819</v>
+      </c>
+      <c r="C1650" t="s">
+        <v>97</v>
+      </c>
+      <c r="D1650" t="s">
+        <v>96</v>
+      </c>
+      <c r="F1650" t="str">
+        <f t="shared" si="8"/>
+        <v>mVINP_LOCK|mVINP_SOUNDACTV</v>
+      </c>
+      <c r="J1650" t="s">
+        <v>1852</v>
+      </c>
+    </row>
+    <row r="1651" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B1651" t="s">
+        <v>1820</v>
+      </c>
+      <c r="C1651" t="s">
+        <v>97</v>
+      </c>
+      <c r="F1651" t="str">
+        <f t="shared" si="8"/>
+        <v>mVINP_LOCK</v>
+      </c>
+      <c r="H1651" t="s">
+        <v>1849</v>
+      </c>
+      <c r="J1651" t="s">
+        <v>97</v>
+      </c>
+      <c r="L1651" t="s">
+        <v>1849</v>
+      </c>
+    </row>
+    <row r="1652" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B1652" t="s">
+        <v>1823</v>
+      </c>
+      <c r="C1652" t="s">
+        <v>97</v>
+      </c>
+      <c r="D1652" t="s">
+        <v>96</v>
+      </c>
+      <c r="F1652" t="str">
+        <f t="shared" si="8"/>
+        <v>mVINP_LOCK|mVINP_SOUNDACTV</v>
+      </c>
+      <c r="J1652" t="s">
+        <v>1852</v>
+      </c>
+    </row>
+    <row r="1653" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B1653" t="s">
+        <v>1823</v>
+      </c>
+      <c r="C1653" t="s">
+        <v>97</v>
+      </c>
+      <c r="D1653" t="s">
+        <v>96</v>
+      </c>
+      <c r="F1653" t="str">
+        <f t="shared" si="8"/>
+        <v>mVINP_LOCK|mVINP_SOUNDACTV</v>
+      </c>
+      <c r="J1653" t="s">
+        <v>1852</v>
+      </c>
+    </row>
+    <row r="1654" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B1654" t="s">
+        <v>1824</v>
+      </c>
+      <c r="C1654" t="s">
+        <v>97</v>
+      </c>
+      <c r="F1654" t="str">
+        <f t="shared" si="8"/>
+        <v>mVINP_LOCK</v>
+      </c>
+      <c r="H1654" t="s">
+        <v>1849</v>
+      </c>
+      <c r="J1654" t="s">
+        <v>97</v>
+      </c>
+      <c r="L1654" t="s">
+        <v>1849</v>
+      </c>
+    </row>
+    <row r="1655" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B1655" t="s">
+        <v>1832</v>
+      </c>
+      <c r="C1655" t="s">
+        <v>97</v>
+      </c>
+      <c r="D1655" t="s">
+        <v>96</v>
+      </c>
+      <c r="F1655" t="str">
+        <f t="shared" si="8"/>
+        <v>mVINP_LOCK|mVINP_SOUNDACTV</v>
+      </c>
+      <c r="J1655" t="s">
+        <v>1852</v>
+      </c>
+    </row>
+    <row r="1656" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B1656" t="s">
+        <v>1832</v>
+      </c>
+      <c r="C1656" t="s">
+        <v>97</v>
+      </c>
+      <c r="D1656" t="s">
+        <v>96</v>
+      </c>
+      <c r="F1656" t="str">
+        <f t="shared" si="8"/>
+        <v>mVINP_LOCK|mVINP_SOUNDACTV</v>
+      </c>
+      <c r="J1656" t="s">
+        <v>1852</v>
+      </c>
+    </row>
+    <row r="1657" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B1657" t="s">
+        <v>1833</v>
+      </c>
+      <c r="C1657" t="s">
+        <v>97</v>
+      </c>
+      <c r="F1657" t="str">
+        <f t="shared" si="8"/>
+        <v>mVINP_LOCK</v>
+      </c>
+      <c r="H1657" t="s">
+        <v>1849</v>
+      </c>
+      <c r="J1657" t="s">
+        <v>97</v>
+      </c>
+      <c r="L1657" t="s">
+        <v>1849</v>
+      </c>
+    </row>
+    <row r="1658" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B1658" t="s">
+        <v>1836</v>
+      </c>
+      <c r="C1658" t="s">
+        <v>97</v>
+      </c>
+      <c r="D1658" t="s">
+        <v>96</v>
+      </c>
+      <c r="F1658" t="str">
+        <f t="shared" si="8"/>
+        <v>mVINP_LOCK|mVINP_SOUNDACTV</v>
+      </c>
+      <c r="J1658" t="s">
+        <v>1852</v>
+      </c>
+    </row>
+    <row r="1659" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B1659" t="s">
+        <v>1836</v>
+      </c>
+      <c r="C1659" t="s">
+        <v>97</v>
+      </c>
+      <c r="D1659" t="s">
+        <v>96</v>
+      </c>
+      <c r="F1659" t="str">
+        <f t="shared" si="8"/>
+        <v>mVINP_LOCK|mVINP_SOUNDACTV</v>
+      </c>
+      <c r="J1659" t="s">
+        <v>1852</v>
+      </c>
+    </row>
+    <row r="1660" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B1660" t="s">
+        <v>1837</v>
+      </c>
+      <c r="C1660" t="s">
+        <v>97</v>
+      </c>
+      <c r="D1660" t="s">
+        <v>96</v>
+      </c>
+      <c r="E1660" t="s">
+        <v>98</v>
+      </c>
+      <c r="F1660" t="str">
+        <f t="shared" si="8"/>
+        <v>mVINP_LOCK|mVINP_SOUNDACTV|mVINP_TRIG</v>
+      </c>
+      <c r="H1660" t="s">
+        <v>1850</v>
+      </c>
+      <c r="J1660" t="s">
+        <v>1853</v>
+      </c>
+      <c r="L1660" t="s">
+        <v>1850</v>
+      </c>
+    </row>
+    <row r="1661" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B1661" t="s">
+        <v>1841</v>
+      </c>
+      <c r="C1661" t="s">
+        <v>97</v>
+      </c>
+      <c r="F1661" t="str">
+        <f t="shared" si="8"/>
+        <v>mVINP_LOCK</v>
+      </c>
+      <c r="J1661" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="1662" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B1662" t="s">
+        <v>1844</v>
+      </c>
+      <c r="C1662" t="s">
+        <v>97</v>
+      </c>
+      <c r="D1662" t="s">
+        <v>96</v>
+      </c>
+      <c r="F1662" t="str">
+        <f t="shared" si="8"/>
+        <v>mVINP_LOCK|mVINP_SOUNDACTV</v>
+      </c>
+      <c r="J1662" t="s">
+        <v>1852</v>
+      </c>
+    </row>
+    <row r="1663" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B1663" t="s">
+        <v>1844</v>
+      </c>
+      <c r="C1663" t="s">
+        <v>97</v>
+      </c>
+      <c r="D1663" t="s">
+        <v>96</v>
+      </c>
+      <c r="F1663" t="str">
+        <f t="shared" si="8"/>
+        <v>mVINP_LOCK|mVINP_SOUNDACTV</v>
+      </c>
+      <c r="J1663" t="s">
+        <v>1852</v>
+      </c>
+    </row>
+    <row r="1664" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B1664" t="s">
+        <v>1845</v>
+      </c>
+      <c r="C1664" t="s">
+        <v>97</v>
+      </c>
+      <c r="F1664" t="str">
+        <f t="shared" si="8"/>
+        <v>mVINP_LOCK</v>
+      </c>
+      <c r="H1664" t="s">
+        <v>1851</v>
+      </c>
+      <c r="J1664" t="s">
+        <v>97</v>
+      </c>
+      <c r="L1664" t="s">
+        <v>1851</v>
+      </c>
+    </row>
+    <row r="1665" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B1665" t="s">
+        <v>1846</v>
+      </c>
+      <c r="C1665" t="s">
+        <v>97</v>
+      </c>
+      <c r="E1665" t="s">
+        <v>98</v>
+      </c>
+      <c r="F1665" t="str">
+        <f t="shared" si="8"/>
+        <v>mVINP_LOCK|mVINP_TRIG</v>
+      </c>
+      <c r="J1665" t="s">
+        <v>1854</v>
+      </c>
+    </row>
+    <row r="1666" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B1666" t="s">
+        <v>1847</v>
+      </c>
+      <c r="C1666" t="s">
+        <v>97</v>
+      </c>
+      <c r="F1666" t="str">
+        <f t="shared" si="8"/>
+        <v>mVINP_LOCK</v>
+      </c>
+      <c r="J1666" t="s">
+        <v>97</v>
+      </c>
+    </row>
   </sheetData>
   <sortState ref="A540:B846">
     <sortCondition ref="A540:A846"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
state table seems to work; still issues with reliably starting sound
</commit_message>
<xml_diff>
--- a/RBG_arduino/StateTable_minimal.xlsx
+++ b/RBG_arduino/StateTable_minimal.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub-Mark-MDO47\RubberBandGun\RBG_arduino\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B70DBDA-9E94-4F9C-B781-6E68EEB1F516}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D79B7AC0-30A6-48D1-8904-504395D452E9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21840" activeTab="1" xr2:uid="{CCADFEE4-B0E1-4363-9617-1683960BED03}"/>
+    <workbookView xWindow="435" yWindow="1155" windowWidth="17460" windowHeight="19170" activeTab="2" xr2:uid="{CCADFEE4-B0E1-4363-9617-1683960BED03}"/>
   </bookViews>
   <sheets>
     <sheet name="StateTable" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2363" uniqueCount="1856">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2491" uniqueCount="1953">
   <si>
     <t>trigOnly</t>
   </si>
@@ -5618,6 +5618,297 @@
   </si>
   <si>
     <t>// special processing should happen in exactly one call, then we move on to .gotoWithoutInput</t>
+  </si>
+  <si>
+    <t>disable ACK and turn off loop command and shorten timeout and change special proc</t>
+  </si>
+  <si>
+    <t>33: RBG_startEffectSound ln 484 EFCT num 0x28 final num 41 loopCount 0</t>
+  </si>
+  <si>
+    <t>34: RBG_startEffectSound ln 518 myDFPlayer problem after check busy</t>
+  </si>
+  <si>
+    <t>891:DEBUG loop() - nowVinputRBG 0x40 loopCount 747</t>
+  </si>
+  <si>
+    <t>900: RBG_startRow ln 275 from row 0 to row 1 loopCount 748</t>
+  </si>
+  <si>
+    <t>903: RBG_startEffectSound ln 484 EFCT num 0x66 final num 102 loopCount 748</t>
+  </si>
+  <si>
+    <t>904: RBG_startEffectSound ln 511 myDFPlayer problem after play</t>
+  </si>
+  <si>
+    <t>906: RBG_startEffectSound ln 518 myDFPlayer problem after check busy</t>
+  </si>
+  <si>
+    <t>935: RBG_startEffectSound ln 484 EFCT num 0x66 final num 102 loopCount 749</t>
+  </si>
+  <si>
+    <t>956: RBG_startEffectSound ln 484 EFCT num 0x66 final num 102 loopCount 750</t>
+  </si>
+  <si>
+    <t>958:DEBUG loop() - nowVinputRBG 0x240 loopCount 751</t>
+  </si>
+  <si>
+    <t>4663:DEBUG loop() - nowVinputRBG 0x40 loopCount 946</t>
+  </si>
+  <si>
+    <t>4682: RBG_startEffectSound ln 484 EFCT num 0x66 final num 102 loopCount 946</t>
+  </si>
+  <si>
+    <t>4683: RBG_startEffectSound ln 518 myDFPlayer problem after check busy</t>
+  </si>
+  <si>
+    <t>4684:Number:51 Play Finished!</t>
+  </si>
+  <si>
+    <t>4705: RBG_startEffectSound ln 484 EFCT num 0x66 final num 102 loopCount 947</t>
+  </si>
+  <si>
+    <t>4707:DEBUG loop() - nowVinputRBG 0x240 loopCount 948</t>
+  </si>
+  <si>
+    <t>5334:DEBUG loop() - nowVinputRBG 0x260 loopCount 981</t>
+  </si>
+  <si>
+    <t>5351: RBG_startRow ln 275 from row 1 to row 4 loopCount 982</t>
+  </si>
+  <si>
+    <t>5354: RBG_startEffectSound ln 484 EFCT num 0x0 final num 1 loopCount 982</t>
+  </si>
+  <si>
+    <t>5366:DEBUG loop() - nowVinputRBG 0x60 loopCount 984</t>
+  </si>
+  <si>
+    <t>5375: RBG_startRow ln 275 from row 4 to row 7 loopCount 985</t>
+  </si>
+  <si>
+    <t>5383:DEBUG loop() - nowVinputRBG 0x260 loopCount 986</t>
+  </si>
+  <si>
+    <t>5384:DEBUG loop() - nowVinputRBG 0x240 loopCount 987</t>
+  </si>
+  <si>
+    <t>9234:DEBUG loop() - nowVinputRBG 0x40 loopCount 2912</t>
+  </si>
+  <si>
+    <t>12800:DEBUG loop() - nowVinputRBG 0x40</t>
+  </si>
+  <si>
+    <t>Still stuck at 7</t>
+  </si>
+  <si>
+    <t>more debugging and changes</t>
+  </si>
+  <si>
+    <t>32: RBG_startEffectSound ln 478 EFCT num 0x28 final num 41 loopCount 0</t>
+  </si>
+  <si>
+    <t>33: RBG_startEffectSound ln 512 myDFPlayer problem after check busy</t>
+  </si>
+  <si>
+    <t>890:DEBUG loop() - nowVinputRBG 0x40 loopCount 747</t>
+  </si>
+  <si>
+    <t>899: RBG_startRow ln 276 from row 0 to row 1 loopCount 748</t>
+  </si>
+  <si>
+    <t>902: RBG_startEffectSound ln 478 EFCT num 0x66 final num 102 loopCount 748</t>
+  </si>
+  <si>
+    <t>903: RBG_startEffectSound ln 505 myDFPlayer problem after play</t>
+  </si>
+  <si>
+    <t>904:Number:48 Play Finished!</t>
+  </si>
+  <si>
+    <t>905: RBG_startEffectSound ln 512 myDFPlayer problem after check busy</t>
+  </si>
+  <si>
+    <t>934: RBG_startEffectSound ln 478 EFCT num 0x66 final num 102 loopCount 749</t>
+  </si>
+  <si>
+    <t>936:DEBUG loop() - nowVinputRBG 0x240 loopCount 750</t>
+  </si>
+  <si>
+    <t>2304:DEBUG loop() - nowVinputRBG 0x260 loopCount 822</t>
+  </si>
+  <si>
+    <t>2321: RBG_startRow ln 276 from row 1 to row 4 loopCount 823</t>
+  </si>
+  <si>
+    <t>2324: RBG_startEffectSound ln 478 EFCT num 0x0 final num 1 loopCount 823</t>
+  </si>
+  <si>
+    <t>2335:DEBUG loop() - nowVinputRBG 0x40 loopCount 824</t>
+  </si>
+  <si>
+    <t>2344: RBG_startRow ln 276 from row 4 to row 7 loopCount 825</t>
+  </si>
+  <si>
+    <t>2352:DEBUG loop() - nowVinputRBG 0x240 loopCount 826</t>
+  </si>
+  <si>
+    <t>2354: RBG_startRow ln 276 from row 7 to row 8 loopCount 827</t>
+  </si>
+  <si>
+    <t>2357: RBG_startEffectSound ln 478 EFCT num 0xA final num 11 loopCount 827</t>
+  </si>
+  <si>
+    <t>2364:DEBUG loop() - nowVinputRBG 0x40 loopCount 830</t>
+  </si>
+  <si>
+    <t>2366: RBG_startRow ln 276 from row 8 to row 9 loopCount 831</t>
+  </si>
+  <si>
+    <t>2370: RBG_startRow ln 276 from row 9 to row 1 loopCount 833</t>
+  </si>
+  <si>
+    <t>2373: RBG_startEffectSound ln 478 EFCT num 0x66 final num 102 loopCount 833</t>
+  </si>
+  <si>
+    <t>2396: RBG_startEffectSound ln 478 EFCT num 0x66 final num 102 loopCount 834</t>
+  </si>
+  <si>
+    <t>2398:DEBUG loop() - nowVinputRBG 0x240 loopCount 835</t>
+  </si>
+  <si>
+    <t>6103:DEBUG loop() - nowVinputRBG 0x40 loopCount 1030</t>
+  </si>
+  <si>
+    <t>6122: RBG_startEffectSound ln 478 EFCT num 0x66 final num 102 loopCount 1030</t>
+  </si>
+  <si>
+    <t>6123: RBG_startEffectSound ln 512 myDFPlayer problem after check busy</t>
+  </si>
+  <si>
+    <t>6124:Number:51 Play Finished!</t>
+  </si>
+  <si>
+    <t>6145: RBG_startEffectSound ln 478 EFCT num 0x66 final num 102 loopCount 1031</t>
+  </si>
+  <si>
+    <t>6147:DEBUG loop() - nowVinputRBG 0x240 loopCount 1032</t>
+  </si>
+  <si>
+    <t>7040:DEBUG loop() - nowVinputRBG 0x260 loopCount 1079</t>
+  </si>
+  <si>
+    <t>7057: RBG_startRow ln 276 from row 1 to row 4 loopCount 1080</t>
+  </si>
+  <si>
+    <t>7060: RBG_startEffectSound ln 478 EFCT num 0x0 final num 1 loopCount 1080</t>
+  </si>
+  <si>
+    <t>7068:DEBUG loop() - nowVinputRBG 0x60 loopCount 1084</t>
+  </si>
+  <si>
+    <t>7070: RBG_startRow ln 276 from row 4 to row 7 loopCount 1085</t>
+  </si>
+  <si>
+    <t>7073:DEBUG loop() - nowVinputRBG 0x240 loopCount 1087</t>
+  </si>
+  <si>
+    <t>7074: RBG_startRow ln 276 from row 7 to row 8 loopCount 1087</t>
+  </si>
+  <si>
+    <t>7077: RBG_startEffectSound ln 478 EFCT num 0xA final num 11 loopCount 1087</t>
+  </si>
+  <si>
+    <t>7078: RBG_startEffectSound ln 512 myDFPlayer problem after check busy</t>
+  </si>
+  <si>
+    <t>7083:DEBUG loop() - nowVinputRBG 0x40 loopCount 1088</t>
+  </si>
+  <si>
+    <t>7085: RBG_startRow ln 276 from row 8 to row 9 loopCount 1089</t>
+  </si>
+  <si>
+    <t>7089: RBG_startRow ln 276 from row 9 to row 1 loopCount 1091</t>
+  </si>
+  <si>
+    <t>7092: RBG_startEffectSound ln 478 EFCT num 0x66 final num 102 loopCount 1091</t>
+  </si>
+  <si>
+    <t>7096:DEBUG loop() - nowVinputRBG 0x240 loopCount 1092</t>
+  </si>
+  <si>
+    <t>10782:DEBUG loop() - nowVinputRBG 0x40 loopCount 1286</t>
+  </si>
+  <si>
+    <t>10801: RBG_startEffectSound ln 478 EFCT num 0x66 final num 102 loopCount 1286</t>
+  </si>
+  <si>
+    <t>10802: RBG_startEffectSound ln 505 myDFPlayer problem after play</t>
+  </si>
+  <si>
+    <t>10803:Number:51 Play Finished!</t>
+  </si>
+  <si>
+    <t>10804: RBG_startEffectSound ln 512 myDFPlayer problem after check busy</t>
+  </si>
+  <si>
+    <t>10805:Number:51 Play Finished!</t>
+  </si>
+  <si>
+    <t>10826: RBG_startEffectSound ln 478 EFCT num 0x66 final num 102 loopCount 1287</t>
+  </si>
+  <si>
+    <t>10828:DEBUG loop() - nowVinputRBG 0x240 loopCount 1288</t>
+  </si>
+  <si>
+    <t>10847:DEBUG loop() - nowVinputRBG 0x40 loopCount 1289</t>
+  </si>
+  <si>
+    <t>10866: RBG_startEffectSound ln 478 EFCT num 0x66 final num 102 loopCount 1289</t>
+  </si>
+  <si>
+    <t>10868:DEBUG loop() - nowVinputRBG 0x240 loopCount 1290</t>
+  </si>
+  <si>
+    <t>11438:DEBUG loop() - nowVinputRBG 0x260 loopCount 1320</t>
+  </si>
+  <si>
+    <t>11455: RBG_startRow ln 276 from row 1 to row 4 loopCount 1321</t>
+  </si>
+  <si>
+    <t>11458: RBG_startEffectSound ln 478 EFCT num 0x0 final num 1 loopCount 1321</t>
+  </si>
+  <si>
+    <t>11466:DEBUG loop() - nowVinputRBG 0x60 loopCount 1325</t>
+  </si>
+  <si>
+    <t>11468: RBG_startRow ln 276 from row 4 to row 7 loopCount 1326</t>
+  </si>
+  <si>
+    <t>11471:DEBUG loop() - nowVinputRBG 0x240 loopCount 1328</t>
+  </si>
+  <si>
+    <t>11472: RBG_startRow ln 276 from row 7 to row 8 loopCount 1328</t>
+  </si>
+  <si>
+    <t>11475: RBG_startEffectSound ln 478 EFCT num 0xA final num 11 loopCount 1328</t>
+  </si>
+  <si>
+    <t>11484:DEBUG loop() - nowVinputRBG 0x40 loopCount 1333</t>
+  </si>
+  <si>
+    <t>11486: RBG_startRow ln 276 from row 8 to row 9 loopCount 1334</t>
+  </si>
+  <si>
+    <t>11490: RBG_startRow ln 276 from row 9 to row 1 loopCount 1336</t>
+  </si>
+  <si>
+    <t>11493: RBG_startEffectSound ln 478 EFCT num 0x66 final num 102 loopCount 1336</t>
+  </si>
+  <si>
+    <t>11497:DEBUG loop() - nowVinputRBG 0x240 loopCount 1337</t>
+  </si>
+  <si>
+    <t>maybe worked</t>
   </si>
 </sst>
 </file>
@@ -6650,7 +6941,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0B3F56F7-7110-4AD7-8B0D-AA537E4015D5}">
   <dimension ref="A1:C15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
@@ -6735,10 +7026,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F57F550E-21B4-4ED7-B7FF-211D228584A7}">
-  <dimension ref="A1:L1666"/>
+  <dimension ref="A1:L1789"/>
   <sheetViews>
-    <sheetView topLeftCell="A1629" workbookViewId="0">
-      <selection activeCell="B1681" sqref="B1681"/>
+    <sheetView tabSelected="1" topLeftCell="A1732" workbookViewId="0">
+      <selection activeCell="E1775" sqref="E1775"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -20138,6 +20429,961 @@
       </c>
       <c r="J1666" t="s">
         <v>97</v>
+      </c>
+    </row>
+    <row r="1670" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="1671" spans="2:10" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B1671" s="1" t="s">
+        <v>1856</v>
+      </c>
+    </row>
+    <row r="1672" spans="2:10" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
+    <row r="1673" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B1673" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="1674" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B1674" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="1675" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B1675" t="s">
+        <v>925</v>
+      </c>
+    </row>
+    <row r="1676" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B1676" t="s">
+        <v>926</v>
+      </c>
+    </row>
+    <row r="1677" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B1677" t="s">
+        <v>430</v>
+      </c>
+    </row>
+    <row r="1681" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1681">
+        <v>30</v>
+      </c>
+      <c r="B1681" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="1682" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1682">
+        <v>33</v>
+      </c>
+      <c r="B1682" t="s">
+        <v>1857</v>
+      </c>
+    </row>
+    <row r="1683" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1683">
+        <v>34</v>
+      </c>
+      <c r="B1683" t="s">
+        <v>1858</v>
+      </c>
+    </row>
+    <row r="1684" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1684">
+        <v>68</v>
+      </c>
+      <c r="B1684" t="s">
+        <v>1734</v>
+      </c>
+    </row>
+    <row r="1685" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1685">
+        <v>891</v>
+      </c>
+      <c r="B1685" t="s">
+        <v>1859</v>
+      </c>
+    </row>
+    <row r="1686" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1686">
+        <v>900</v>
+      </c>
+      <c r="B1686" t="s">
+        <v>1860</v>
+      </c>
+    </row>
+    <row r="1687" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1687">
+        <v>903</v>
+      </c>
+      <c r="B1687" t="s">
+        <v>1861</v>
+      </c>
+    </row>
+    <row r="1688" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1688">
+        <v>904</v>
+      </c>
+      <c r="B1688" t="s">
+        <v>1862</v>
+      </c>
+    </row>
+    <row r="1689" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1689">
+        <v>905</v>
+      </c>
+      <c r="B1689" t="s">
+        <v>1805</v>
+      </c>
+    </row>
+    <row r="1690" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1690">
+        <v>906</v>
+      </c>
+      <c r="B1690" t="s">
+        <v>1863</v>
+      </c>
+    </row>
+    <row r="1691" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1691">
+        <v>935</v>
+      </c>
+      <c r="B1691" t="s">
+        <v>1864</v>
+      </c>
+    </row>
+    <row r="1692" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1692">
+        <v>956</v>
+      </c>
+      <c r="B1692" t="s">
+        <v>1865</v>
+      </c>
+    </row>
+    <row r="1693" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1693">
+        <v>958</v>
+      </c>
+      <c r="B1693" t="s">
+        <v>1866</v>
+      </c>
+    </row>
+    <row r="1694" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1694">
+        <v>4663</v>
+      </c>
+      <c r="B1694" t="s">
+        <v>1867</v>
+      </c>
+    </row>
+    <row r="1695" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1695">
+        <v>4682</v>
+      </c>
+      <c r="B1695" t="s">
+        <v>1868</v>
+      </c>
+    </row>
+    <row r="1696" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1696">
+        <v>4683</v>
+      </c>
+      <c r="B1696" t="s">
+        <v>1869</v>
+      </c>
+    </row>
+    <row r="1697" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1697">
+        <v>4684</v>
+      </c>
+      <c r="B1697" t="s">
+        <v>1870</v>
+      </c>
+    </row>
+    <row r="1698" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1698">
+        <v>4705</v>
+      </c>
+      <c r="B1698" t="s">
+        <v>1871</v>
+      </c>
+    </row>
+    <row r="1699" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1699">
+        <v>4707</v>
+      </c>
+      <c r="B1699" t="s">
+        <v>1872</v>
+      </c>
+    </row>
+    <row r="1700" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1700">
+        <v>5334</v>
+      </c>
+      <c r="B1700" t="s">
+        <v>1873</v>
+      </c>
+    </row>
+    <row r="1701" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1701">
+        <v>5351</v>
+      </c>
+      <c r="B1701" t="s">
+        <v>1874</v>
+      </c>
+    </row>
+    <row r="1702" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1702">
+        <v>5354</v>
+      </c>
+      <c r="B1702" t="s">
+        <v>1875</v>
+      </c>
+    </row>
+    <row r="1703" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1703">
+        <v>5366</v>
+      </c>
+      <c r="B1703" t="s">
+        <v>1876</v>
+      </c>
+    </row>
+    <row r="1704" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1704">
+        <v>5375</v>
+      </c>
+      <c r="B1704" s="4" t="s">
+        <v>1877</v>
+      </c>
+      <c r="D1704" t="s">
+        <v>1882</v>
+      </c>
+    </row>
+    <row r="1705" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1705">
+        <v>5383</v>
+      </c>
+      <c r="B1705" t="s">
+        <v>1878</v>
+      </c>
+    </row>
+    <row r="1706" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1706">
+        <v>5384</v>
+      </c>
+      <c r="B1706" t="s">
+        <v>1879</v>
+      </c>
+    </row>
+    <row r="1707" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1707">
+        <v>9234</v>
+      </c>
+      <c r="B1707" t="s">
+        <v>1880</v>
+      </c>
+    </row>
+    <row r="1708" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1708">
+        <v>12800</v>
+      </c>
+      <c r="B1708" t="s">
+        <v>1881</v>
+      </c>
+    </row>
+    <row r="1710" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="1711" spans="1:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B1711" s="1" t="s">
+        <v>1883</v>
+      </c>
+    </row>
+    <row r="1712" spans="1:4" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
+    <row r="1713" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B1713" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="1714" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B1714" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="1715" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B1715" t="s">
+        <v>925</v>
+      </c>
+    </row>
+    <row r="1716" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B1716" t="s">
+        <v>926</v>
+      </c>
+    </row>
+    <row r="1717" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B1717" t="s">
+        <v>430</v>
+      </c>
+    </row>
+    <row r="1720" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1720">
+        <v>29</v>
+      </c>
+      <c r="B1720" t="s">
+        <v>1798</v>
+      </c>
+    </row>
+    <row r="1721" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1721">
+        <v>32</v>
+      </c>
+      <c r="B1721" s="16" t="s">
+        <v>1884</v>
+      </c>
+      <c r="E1721" t="s">
+        <v>1352</v>
+      </c>
+    </row>
+    <row r="1722" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1722">
+        <v>33</v>
+      </c>
+      <c r="B1722" t="s">
+        <v>1885</v>
+      </c>
+      <c r="C1722" s="14"/>
+    </row>
+    <row r="1723" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1723">
+        <v>67</v>
+      </c>
+      <c r="B1723" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="1724" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1724">
+        <v>890</v>
+      </c>
+      <c r="B1724" t="s">
+        <v>1886</v>
+      </c>
+    </row>
+    <row r="1725" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1725">
+        <v>899</v>
+      </c>
+      <c r="B1725" s="12" t="s">
+        <v>1887</v>
+      </c>
+    </row>
+    <row r="1726" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1726">
+        <v>902</v>
+      </c>
+      <c r="B1726" s="16" t="s">
+        <v>1888</v>
+      </c>
+      <c r="D1726" t="s">
+        <v>1351</v>
+      </c>
+    </row>
+    <row r="1727" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1727">
+        <v>903</v>
+      </c>
+      <c r="B1727" t="s">
+        <v>1889</v>
+      </c>
+      <c r="C1727" s="4"/>
+    </row>
+    <row r="1728" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1728">
+        <v>904</v>
+      </c>
+      <c r="B1728" t="s">
+        <v>1890</v>
+      </c>
+    </row>
+    <row r="1729" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1729">
+        <v>905</v>
+      </c>
+      <c r="B1729" t="s">
+        <v>1891</v>
+      </c>
+      <c r="C1729" s="14"/>
+    </row>
+    <row r="1730" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1730">
+        <v>934</v>
+      </c>
+      <c r="B1730" s="16" t="s">
+        <v>1892</v>
+      </c>
+      <c r="C1730" s="16"/>
+      <c r="D1730" s="16"/>
+      <c r="E1730" s="16" t="s">
+        <v>1352</v>
+      </c>
+      <c r="F1730" s="16"/>
+    </row>
+    <row r="1731" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1731">
+        <v>936</v>
+      </c>
+      <c r="B1731" t="s">
+        <v>1893</v>
+      </c>
+      <c r="C1731" s="12"/>
+    </row>
+    <row r="1732" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1732">
+        <v>2304</v>
+      </c>
+      <c r="B1732" t="s">
+        <v>1894</v>
+      </c>
+    </row>
+    <row r="1733" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1733">
+        <v>2321</v>
+      </c>
+      <c r="B1733" s="12" t="s">
+        <v>1895</v>
+      </c>
+    </row>
+    <row r="1734" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1734">
+        <v>2324</v>
+      </c>
+      <c r="B1734" s="16" t="s">
+        <v>1896</v>
+      </c>
+      <c r="C1734" s="16"/>
+      <c r="D1734" s="16" t="s">
+        <v>1351</v>
+      </c>
+      <c r="E1734" s="16"/>
+      <c r="F1734" s="16"/>
+    </row>
+    <row r="1735" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1735">
+        <v>2335</v>
+      </c>
+      <c r="B1735" t="s">
+        <v>1897</v>
+      </c>
+    </row>
+    <row r="1736" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1736">
+        <v>2344</v>
+      </c>
+      <c r="B1736" s="12" t="s">
+        <v>1898</v>
+      </c>
+    </row>
+    <row r="1737" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1737">
+        <v>2352</v>
+      </c>
+      <c r="B1737" t="s">
+        <v>1899</v>
+      </c>
+    </row>
+    <row r="1738" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1738">
+        <v>2354</v>
+      </c>
+      <c r="B1738" s="12" t="s">
+        <v>1900</v>
+      </c>
+    </row>
+    <row r="1739" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1739">
+        <v>2357</v>
+      </c>
+      <c r="B1739" s="16" t="s">
+        <v>1901</v>
+      </c>
+      <c r="C1739" s="16"/>
+      <c r="D1739" s="16" t="s">
+        <v>1351</v>
+      </c>
+      <c r="E1739" s="16"/>
+      <c r="F1739" s="16"/>
+    </row>
+    <row r="1740" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1740">
+        <v>2364</v>
+      </c>
+      <c r="B1740" t="s">
+        <v>1902</v>
+      </c>
+    </row>
+    <row r="1741" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1741">
+        <v>2366</v>
+      </c>
+      <c r="B1741" s="12" t="s">
+        <v>1903</v>
+      </c>
+    </row>
+    <row r="1742" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1742">
+        <v>2370</v>
+      </c>
+      <c r="B1742" s="12" t="s">
+        <v>1904</v>
+      </c>
+    </row>
+    <row r="1743" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1743">
+        <v>2373</v>
+      </c>
+      <c r="B1743" s="16" t="s">
+        <v>1905</v>
+      </c>
+      <c r="C1743" s="16"/>
+      <c r="D1743" s="16" t="s">
+        <v>1351</v>
+      </c>
+      <c r="E1743" s="16"/>
+      <c r="F1743" s="16"/>
+    </row>
+    <row r="1744" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1744">
+        <v>2396</v>
+      </c>
+      <c r="B1744" s="16" t="s">
+        <v>1906</v>
+      </c>
+      <c r="C1744" s="16"/>
+      <c r="D1744" s="16"/>
+      <c r="E1744" s="17" t="s">
+        <v>1352</v>
+      </c>
+      <c r="F1744" s="16"/>
+    </row>
+    <row r="1745" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1745">
+        <v>2398</v>
+      </c>
+      <c r="B1745" t="s">
+        <v>1907</v>
+      </c>
+    </row>
+    <row r="1746" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1746">
+        <v>6103</v>
+      </c>
+      <c r="B1746" t="s">
+        <v>1908</v>
+      </c>
+    </row>
+    <row r="1747" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1747">
+        <v>6122</v>
+      </c>
+      <c r="B1747" s="16" t="s">
+        <v>1909</v>
+      </c>
+      <c r="C1747" s="16"/>
+      <c r="D1747" s="16" t="s">
+        <v>1351</v>
+      </c>
+      <c r="E1747" s="16"/>
+      <c r="F1747" s="16"/>
+    </row>
+    <row r="1748" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1748">
+        <v>6123</v>
+      </c>
+      <c r="B1748" t="s">
+        <v>1910</v>
+      </c>
+      <c r="C1748" s="14"/>
+    </row>
+    <row r="1749" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1749">
+        <v>6124</v>
+      </c>
+      <c r="B1749" t="s">
+        <v>1911</v>
+      </c>
+    </row>
+    <row r="1750" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1750">
+        <v>6145</v>
+      </c>
+      <c r="B1750" s="16" t="s">
+        <v>1912</v>
+      </c>
+      <c r="C1750" s="16"/>
+      <c r="D1750" s="16"/>
+      <c r="E1750" s="17" t="s">
+        <v>1352</v>
+      </c>
+      <c r="F1750" s="16"/>
+    </row>
+    <row r="1751" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1751">
+        <v>6147</v>
+      </c>
+      <c r="B1751" t="s">
+        <v>1913</v>
+      </c>
+    </row>
+    <row r="1752" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1752">
+        <v>7040</v>
+      </c>
+      <c r="B1752" t="s">
+        <v>1914</v>
+      </c>
+    </row>
+    <row r="1753" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1753">
+        <v>7057</v>
+      </c>
+      <c r="B1753" s="12" t="s">
+        <v>1915</v>
+      </c>
+    </row>
+    <row r="1754" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1754">
+        <v>7060</v>
+      </c>
+      <c r="B1754" s="16" t="s">
+        <v>1916</v>
+      </c>
+      <c r="C1754" s="16"/>
+      <c r="D1754" s="16"/>
+      <c r="E1754" s="16"/>
+      <c r="F1754" s="16" t="s">
+        <v>1952</v>
+      </c>
+    </row>
+    <row r="1755" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1755">
+        <v>7068</v>
+      </c>
+      <c r="B1755" t="s">
+        <v>1917</v>
+      </c>
+    </row>
+    <row r="1756" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1756">
+        <v>7070</v>
+      </c>
+      <c r="B1756" s="12" t="s">
+        <v>1918</v>
+      </c>
+    </row>
+    <row r="1757" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1757">
+        <v>7073</v>
+      </c>
+      <c r="B1757" t="s">
+        <v>1919</v>
+      </c>
+    </row>
+    <row r="1758" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1758">
+        <v>7074</v>
+      </c>
+      <c r="B1758" s="12" t="s">
+        <v>1920</v>
+      </c>
+    </row>
+    <row r="1759" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1759">
+        <v>7077</v>
+      </c>
+      <c r="B1759" s="16" t="s">
+        <v>1921</v>
+      </c>
+      <c r="C1759" s="16"/>
+      <c r="D1759" s="16" t="s">
+        <v>1351</v>
+      </c>
+      <c r="E1759" s="16"/>
+      <c r="F1759" s="16"/>
+    </row>
+    <row r="1760" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1760">
+        <v>7078</v>
+      </c>
+      <c r="B1760" t="s">
+        <v>1922</v>
+      </c>
+      <c r="C1760" s="14"/>
+    </row>
+    <row r="1761" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1761">
+        <v>7083</v>
+      </c>
+      <c r="B1761" t="s">
+        <v>1923</v>
+      </c>
+    </row>
+    <row r="1762" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1762">
+        <v>7085</v>
+      </c>
+      <c r="B1762" s="12" t="s">
+        <v>1924</v>
+      </c>
+    </row>
+    <row r="1763" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1763">
+        <v>7089</v>
+      </c>
+      <c r="B1763" s="12" t="s">
+        <v>1925</v>
+      </c>
+    </row>
+    <row r="1764" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1764">
+        <v>7092</v>
+      </c>
+      <c r="B1764" s="16" t="s">
+        <v>1926</v>
+      </c>
+      <c r="C1764" s="16"/>
+      <c r="D1764" s="16" t="s">
+        <v>1351</v>
+      </c>
+      <c r="E1764" s="16"/>
+      <c r="F1764" s="16"/>
+    </row>
+    <row r="1765" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1765">
+        <v>7096</v>
+      </c>
+      <c r="B1765" t="s">
+        <v>1927</v>
+      </c>
+    </row>
+    <row r="1766" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1766">
+        <v>10782</v>
+      </c>
+      <c r="B1766" t="s">
+        <v>1928</v>
+      </c>
+    </row>
+    <row r="1767" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1767">
+        <v>10801</v>
+      </c>
+      <c r="B1767" s="16" t="s">
+        <v>1929</v>
+      </c>
+      <c r="C1767" s="16"/>
+      <c r="D1767" s="16" t="s">
+        <v>1351</v>
+      </c>
+      <c r="E1767" s="16"/>
+      <c r="F1767" s="16"/>
+    </row>
+    <row r="1768" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1768">
+        <v>10802</v>
+      </c>
+      <c r="B1768" t="s">
+        <v>1930</v>
+      </c>
+      <c r="C1768" s="4"/>
+    </row>
+    <row r="1769" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1769">
+        <v>10803</v>
+      </c>
+      <c r="B1769" t="s">
+        <v>1931</v>
+      </c>
+    </row>
+    <row r="1770" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1770">
+        <v>10804</v>
+      </c>
+      <c r="B1770" t="s">
+        <v>1932</v>
+      </c>
+      <c r="C1770" s="14"/>
+    </row>
+    <row r="1771" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1771">
+        <v>10805</v>
+      </c>
+      <c r="B1771" t="s">
+        <v>1933</v>
+      </c>
+    </row>
+    <row r="1772" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1772">
+        <v>10826</v>
+      </c>
+      <c r="B1772" s="16" t="s">
+        <v>1934</v>
+      </c>
+      <c r="C1772" s="16"/>
+      <c r="D1772" s="16" t="s">
+        <v>1351</v>
+      </c>
+      <c r="E1772" s="16"/>
+      <c r="F1772" s="16"/>
+    </row>
+    <row r="1773" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1773">
+        <v>10828</v>
+      </c>
+      <c r="B1773" t="s">
+        <v>1935</v>
+      </c>
+    </row>
+    <row r="1774" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1774">
+        <v>10847</v>
+      </c>
+      <c r="B1774" t="s">
+        <v>1936</v>
+      </c>
+    </row>
+    <row r="1775" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1775">
+        <v>10866</v>
+      </c>
+      <c r="B1775" s="16" t="s">
+        <v>1937</v>
+      </c>
+      <c r="C1775" s="16"/>
+      <c r="D1775" s="16"/>
+      <c r="E1775" s="17" t="s">
+        <v>1352</v>
+      </c>
+      <c r="F1775" s="16"/>
+    </row>
+    <row r="1776" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1776">
+        <v>10868</v>
+      </c>
+      <c r="B1776" t="s">
+        <v>1938</v>
+      </c>
+    </row>
+    <row r="1777" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1777">
+        <v>11438</v>
+      </c>
+      <c r="B1777" t="s">
+        <v>1939</v>
+      </c>
+    </row>
+    <row r="1778" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1778">
+        <v>11455</v>
+      </c>
+      <c r="B1778" s="12" t="s">
+        <v>1940</v>
+      </c>
+    </row>
+    <row r="1779" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1779">
+        <v>11458</v>
+      </c>
+      <c r="B1779" s="16" t="s">
+        <v>1941</v>
+      </c>
+      <c r="C1779" s="16"/>
+      <c r="D1779" s="16" t="s">
+        <v>1351</v>
+      </c>
+      <c r="E1779" s="16"/>
+      <c r="F1779" s="16"/>
+    </row>
+    <row r="1780" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1780">
+        <v>11466</v>
+      </c>
+      <c r="B1780" t="s">
+        <v>1942</v>
+      </c>
+    </row>
+    <row r="1781" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1781">
+        <v>11468</v>
+      </c>
+      <c r="B1781" s="12" t="s">
+        <v>1943</v>
+      </c>
+    </row>
+    <row r="1782" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1782">
+        <v>11471</v>
+      </c>
+      <c r="B1782" t="s">
+        <v>1944</v>
+      </c>
+    </row>
+    <row r="1783" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1783">
+        <v>11472</v>
+      </c>
+      <c r="B1783" s="12" t="s">
+        <v>1945</v>
+      </c>
+    </row>
+    <row r="1784" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1784">
+        <v>11475</v>
+      </c>
+      <c r="B1784" s="16" t="s">
+        <v>1946</v>
+      </c>
+      <c r="C1784" s="16"/>
+      <c r="D1784" s="16" t="s">
+        <v>1351</v>
+      </c>
+      <c r="E1784" s="16"/>
+      <c r="F1784" s="16"/>
+    </row>
+    <row r="1785" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1785">
+        <v>11484</v>
+      </c>
+      <c r="B1785" t="s">
+        <v>1947</v>
+      </c>
+    </row>
+    <row r="1786" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1786">
+        <v>11486</v>
+      </c>
+      <c r="B1786" s="12" t="s">
+        <v>1948</v>
+      </c>
+    </row>
+    <row r="1787" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1787">
+        <v>11490</v>
+      </c>
+      <c r="B1787" s="12" t="s">
+        <v>1949</v>
+      </c>
+    </row>
+    <row r="1788" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1788">
+        <v>11493</v>
+      </c>
+      <c r="B1788" s="16" t="s">
+        <v>1950</v>
+      </c>
+    </row>
+    <row r="1789" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1789">
+        <v>11497</v>
+      </c>
+      <c r="B1789" t="s">
+        <v>1951</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
going back to primitive play() command makes it work much better; still curiosities
</commit_message>
<xml_diff>
--- a/RBG_arduino/StateTable_minimal.xlsx
+++ b/RBG_arduino/StateTable_minimal.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub-Mark-MDO47\RubberBandGun\RBG_arduino\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{490D424D-A303-445D-A1F0-F9D28A6D2B99}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96245999-C64E-4917-8EE1-727677320667}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="435" yWindow="1155" windowWidth="17460" windowHeight="19170" activeTab="4" xr2:uid="{CCADFEE4-B0E1-4363-9617-1683960BED03}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21840" activeTab="2" xr2:uid="{CCADFEE4-B0E1-4363-9617-1683960BED03}"/>
   </bookViews>
   <sheets>
     <sheet name="StateTable" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
     <sheet name="ThingsToTry" sheetId="5" r:id="rId5"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">debugging!$A$2172:$B$2245</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">debugging!$A$2256:$B$2321</definedName>
     <definedName name="yxcmd">'YX5200 info'!$A$2:$C$44</definedName>
   </definedNames>
   <calcPr calcId="181029"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2990" uniqueCount="2388">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3065" uniqueCount="2455">
   <si>
     <t>trigOnly</t>
   </si>
@@ -7215,6 +7215,207 @@
   </si>
   <si>
     <t>reformat SD and copy shortened files in correct order to MP3 directory DFRobotDFPlayerMini::playMp3Folder</t>
+  </si>
+  <si>
+    <t>assume minimum play time 1.5 sec; implement check and retry if not playing after that time</t>
+  </si>
+  <si>
+    <t>18:DEBUG loop() - nowVinputRBG 0x40 loopCount 0</t>
+  </si>
+  <si>
+    <t>40:DEBUG loop() - nowVinputRBG 0x240 loopCount 1</t>
+  </si>
+  <si>
+    <t>453:DEBUG loop() - nowVinputRBG 0x40 loopCount 134</t>
+  </si>
+  <si>
+    <t>483:DEBUG loop() - nowVinputRBG 0x240 loopCount 136</t>
+  </si>
+  <si>
+    <t>3633:DEBUG loop() - nowVinputRBG 0x40 loopCount 286</t>
+  </si>
+  <si>
+    <t>3658:DEBUG loop() - nowVinputRBG 0x240 loopCount 287</t>
+  </si>
+  <si>
+    <t>4141:DEBUG loop() - nowVinputRBG 0x260 loopCount 310</t>
+  </si>
+  <si>
+    <t>4178:DEBUG loop() - nowVinputRBG 0x240 loopCount 312</t>
+  </si>
+  <si>
+    <t>5855:DEBUG loop() - nowVinputRBG 0x40 loopCount 871</t>
+  </si>
+  <si>
+    <t>5894:DEBUG loop() - nowVinputRBG 0x240 loopCount 875</t>
+  </si>
+  <si>
+    <t>6209:DEBUG loop() - nowVinputRBG 0x40 loopCount 980</t>
+  </si>
+  <si>
+    <t>6232:DEBUG loop() - nowVinputRBG 0x240 loopCount 984</t>
+  </si>
+  <si>
+    <t>6862:DEBUG loop() - nowVinputRBG 0x80 loopCount 1014</t>
+  </si>
+  <si>
+    <t>7325:DEBUG loop() - nowVinputRBG 0x240 loopCount 1036</t>
+  </si>
+  <si>
+    <t>464: RBG_startRow ln 276 from row 0 to row 1 loopCount 135</t>
+  </si>
+  <si>
+    <t>4160: RBG_startRow ln 276 from row 1 to row 4 loopCount 311</t>
+  </si>
+  <si>
+    <t>5866: RBG_startRow ln 276 from row 4 to row 7 loopCount 872</t>
+  </si>
+  <si>
+    <t>5880: RBG_startRow ln 276 from row 7 to row 8 loopCount 874</t>
+  </si>
+  <si>
+    <t>6213: RBG_startRow ln 276 from row 8 to row 9 loopCount 981</t>
+  </si>
+  <si>
+    <t>6221: RBG_startRow ln 276 from row 9 to row 1 loopCount 983</t>
+  </si>
+  <si>
+    <t>6885: RBG_startRow ln 276 from row 1 to row 5 loopCount 1015</t>
+  </si>
+  <si>
+    <t>6899: RBG_startRow ln 276 from row 5 to row 1 loopCount 1017</t>
+  </si>
+  <si>
+    <t>21: RBG_startEffectSound ln 478 EFCT num 0x28 final num 41 loopCount 0</t>
+  </si>
+  <si>
+    <t>22: RBG_startEffectSound ln 513 myDFPlayer problem after check busy</t>
+  </si>
+  <si>
+    <t>467: RBG_startEffectSound ln 478 EFCT num 0x66 final num 102 loopCount 135</t>
+  </si>
+  <si>
+    <t>468: RBG_startEffectSound ln 506 myDFPlayer problem after play</t>
+  </si>
+  <si>
+    <t>470: RBG_startEffectSound ln 513 myDFPlayer problem after check busy</t>
+  </si>
+  <si>
+    <t>3652: RBG_startEffectSound ln 478 EFCT num 0x66 final num 102 loopCount 286</t>
+  </si>
+  <si>
+    <t>3653: RBG_startEffectSound ln 506 myDFPlayer problem after play</t>
+  </si>
+  <si>
+    <t>4163: RBG_startEffectSound ln 478 EFCT num 0x0 final num 1 loopCount 311</t>
+  </si>
+  <si>
+    <t>4164: RBG_startEffectSound ln 506 myDFPlayer problem after play</t>
+  </si>
+  <si>
+    <t>5883: RBG_startEffectSound ln 478 EFCT num 0xA final num 11 loopCount 874</t>
+  </si>
+  <si>
+    <t>5884: RBG_startEffectSound ln 506 myDFPlayer problem after play</t>
+  </si>
+  <si>
+    <t>5886: RBG_startEffectSound ln 513 myDFPlayer problem after check busy</t>
+  </si>
+  <si>
+    <t>6224: RBG_startEffectSound ln 478 EFCT num 0x66 final num 102 loopCount 983</t>
+  </si>
+  <si>
+    <t>6225: RBG_startEffectSound ln 513 myDFPlayer problem after check busy</t>
+  </si>
+  <si>
+    <t>6888: RBG_startEffectSound ln 478 EFCT num 0x14 final num 21 loopCount 1015</t>
+  </si>
+  <si>
+    <t>6902: RBG_startEffectSound ln 478 EFCT num 0x66 final num 102 loopCount 1017</t>
+  </si>
+  <si>
+    <t>6927: RBG_startEffectSound ln 478 EFCT num 0x66 final num 102 loopCount 1018</t>
+  </si>
+  <si>
+    <t>6950: RBG_startEffectSound ln 478 EFCT num 0x66 final num 102 loopCount 1019</t>
+  </si>
+  <si>
+    <t>6973: RBG_startEffectSound ln 478 EFCT num 0x66 final num 102 loopCount 1020</t>
+  </si>
+  <si>
+    <t>6996: RBG_startEffectSound ln 478 EFCT num 0x66 final num 102 loopCount 1021</t>
+  </si>
+  <si>
+    <t>7019: RBG_startEffectSound ln 478 EFCT num 0x66 final num 102 loopCount 1022</t>
+  </si>
+  <si>
+    <t>7042: RBG_startEffectSound ln 478 EFCT num 0x66 final num 102 loopCount 1023</t>
+  </si>
+  <si>
+    <t>7065: RBG_startEffectSound ln 478 EFCT num 0x66 final num 102 loopCount 1024</t>
+  </si>
+  <si>
+    <t>7088: RBG_startEffectSound ln 478 EFCT num 0x66 final num 102 loopCount 1025</t>
+  </si>
+  <si>
+    <t>7111: RBG_startEffectSound ln 478 EFCT num 0x66 final num 102 loopCount 1026</t>
+  </si>
+  <si>
+    <t>7134: RBG_startEffectSound ln 478 EFCT num 0x66 final num 102 loopCount 1027</t>
+  </si>
+  <si>
+    <t>7157: RBG_startEffectSound ln 478 EFCT num 0x66 final num 102 loopCount 1028</t>
+  </si>
+  <si>
+    <t>7180: RBG_startEffectSound ln 478 EFCT num 0x66 final num 102 loopCount 1029</t>
+  </si>
+  <si>
+    <t>7203: RBG_startEffectSound ln 478 EFCT num 0x66 final num 102 loopCount 1030</t>
+  </si>
+  <si>
+    <t>7204: RBG_startEffectSound ln 513 myDFPlayer problem after check busy</t>
+  </si>
+  <si>
+    <t>7227: RBG_startEffectSound ln 478 EFCT num 0x66 final num 102 loopCount 1031</t>
+  </si>
+  <si>
+    <t>7228: RBG_startEffectSound ln 513 myDFPlayer problem after check busy</t>
+  </si>
+  <si>
+    <t>7251: RBG_startEffectSound ln 478 EFCT num 0x66 final num 102 loopCount 1032</t>
+  </si>
+  <si>
+    <t>7252: RBG_startEffectSound ln 513 myDFPlayer problem after check busy</t>
+  </si>
+  <si>
+    <t>7275: RBG_startEffectSound ln 478 EFCT num 0x66 final num 102 loopCount 1033</t>
+  </si>
+  <si>
+    <t>7298: RBG_startEffectSound ln 478 EFCT num 0x66 final num 102 loopCount 1034</t>
+  </si>
+  <si>
+    <t>7321: RBG_startEffectSound ln 478 EFCT num 0x66 final num 102 loopCount 1035</t>
+  </si>
+  <si>
+    <t>469:Number:42 Play Finished!</t>
+  </si>
+  <si>
+    <t>471:Number:42 Play Finished!</t>
+  </si>
+  <si>
+    <t>3654:Number:103 Play Finished!</t>
+  </si>
+  <si>
+    <t>4165:Number:103 Play Finished!</t>
+  </si>
+  <si>
+    <t>5885:Number:2 Play Finished!</t>
+  </si>
+  <si>
+    <t>5887:Number:2 Play Finished!</t>
+  </si>
+  <si>
+    <t>hmm - problem here</t>
   </si>
 </sst>
 </file>
@@ -8332,10 +8533,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F57F550E-21B4-4ED7-B7FF-211D228584A7}">
-  <dimension ref="A1:L2245"/>
+  <dimension ref="A1:L2321"/>
   <sheetViews>
-    <sheetView topLeftCell="A2162" workbookViewId="0">
-      <selection activeCell="B2176" sqref="B2176"/>
+    <sheetView tabSelected="1" topLeftCell="A2275" workbookViewId="0">
+      <selection activeCell="B2295" sqref="B2295"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -26117,10 +26318,573 @@
         <v>2340</v>
       </c>
     </row>
+    <row r="2247" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="2248" spans="1:2" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B2248" s="1" t="s">
+        <v>2384</v>
+      </c>
+    </row>
+    <row r="2249" spans="1:2" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
+    <row r="2250" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B2250" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="2251" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B2251" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="2252" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B2252" t="s">
+        <v>924</v>
+      </c>
+    </row>
+    <row r="2253" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B2253" t="s">
+        <v>925</v>
+      </c>
+    </row>
+    <row r="2254" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B2254" t="s">
+        <v>430</v>
+      </c>
+    </row>
+    <row r="2256" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2256" t="s">
+        <v>2097</v>
+      </c>
+      <c r="B2256" t="s">
+        <v>617</v>
+      </c>
+    </row>
+    <row r="2257" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2257">
+        <v>18</v>
+      </c>
+      <c r="B2257" t="s">
+        <v>2389</v>
+      </c>
+    </row>
+    <row r="2258" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2258">
+        <v>21</v>
+      </c>
+      <c r="B2258" s="16" t="s">
+        <v>2411</v>
+      </c>
+    </row>
+    <row r="2259" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2259">
+        <v>22</v>
+      </c>
+      <c r="B2259" t="s">
+        <v>2412</v>
+      </c>
+    </row>
+    <row r="2260" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2260">
+        <v>40</v>
+      </c>
+      <c r="B2260" t="s">
+        <v>2390</v>
+      </c>
+    </row>
+    <row r="2261" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2261">
+        <v>453</v>
+      </c>
+      <c r="B2261" t="s">
+        <v>2391</v>
+      </c>
+    </row>
+    <row r="2262" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2262">
+        <v>464</v>
+      </c>
+      <c r="B2262" s="12" t="s">
+        <v>2403</v>
+      </c>
+    </row>
+    <row r="2263" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2263">
+        <v>467</v>
+      </c>
+      <c r="B2263" s="16" t="s">
+        <v>2413</v>
+      </c>
+    </row>
+    <row r="2264" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2264">
+        <v>468</v>
+      </c>
+      <c r="B2264" t="s">
+        <v>2414</v>
+      </c>
+    </row>
+    <row r="2265" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2265">
+        <v>469</v>
+      </c>
+      <c r="B2265" t="s">
+        <v>2448</v>
+      </c>
+    </row>
+    <row r="2266" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2266">
+        <v>470</v>
+      </c>
+      <c r="B2266" t="s">
+        <v>2415</v>
+      </c>
+    </row>
+    <row r="2267" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2267">
+        <v>471</v>
+      </c>
+      <c r="B2267" t="s">
+        <v>2449</v>
+      </c>
+    </row>
+    <row r="2268" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2268">
+        <v>483</v>
+      </c>
+      <c r="B2268" t="s">
+        <v>2392</v>
+      </c>
+    </row>
+    <row r="2269" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2269">
+        <v>3633</v>
+      </c>
+      <c r="B2269" t="s">
+        <v>2393</v>
+      </c>
+    </row>
+    <row r="2270" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2270">
+        <v>3652</v>
+      </c>
+      <c r="B2270" s="16" t="s">
+        <v>2416</v>
+      </c>
+    </row>
+    <row r="2271" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2271">
+        <v>3653</v>
+      </c>
+      <c r="B2271" t="s">
+        <v>2417</v>
+      </c>
+    </row>
+    <row r="2272" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2272">
+        <v>3654</v>
+      </c>
+      <c r="B2272" t="s">
+        <v>2450</v>
+      </c>
+    </row>
+    <row r="2273" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2273">
+        <v>3658</v>
+      </c>
+      <c r="B2273" t="s">
+        <v>2394</v>
+      </c>
+    </row>
+    <row r="2274" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2274">
+        <v>4141</v>
+      </c>
+      <c r="B2274" t="s">
+        <v>2395</v>
+      </c>
+    </row>
+    <row r="2275" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2275">
+        <v>4160</v>
+      </c>
+      <c r="B2275" s="12" t="s">
+        <v>2404</v>
+      </c>
+    </row>
+    <row r="2276" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2276">
+        <v>4163</v>
+      </c>
+      <c r="B2276" s="16" t="s">
+        <v>2418</v>
+      </c>
+    </row>
+    <row r="2277" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2277">
+        <v>4164</v>
+      </c>
+      <c r="B2277" t="s">
+        <v>2419</v>
+      </c>
+    </row>
+    <row r="2278" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2278">
+        <v>4165</v>
+      </c>
+      <c r="B2278" t="s">
+        <v>2451</v>
+      </c>
+    </row>
+    <row r="2279" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2279">
+        <v>4178</v>
+      </c>
+      <c r="B2279" t="s">
+        <v>2396</v>
+      </c>
+    </row>
+    <row r="2280" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2280">
+        <v>5855</v>
+      </c>
+      <c r="B2280" t="s">
+        <v>2397</v>
+      </c>
+    </row>
+    <row r="2281" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2281">
+        <v>5866</v>
+      </c>
+      <c r="B2281" s="12" t="s">
+        <v>2405</v>
+      </c>
+    </row>
+    <row r="2282" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2282">
+        <v>5880</v>
+      </c>
+      <c r="B2282" s="12" t="s">
+        <v>2406</v>
+      </c>
+    </row>
+    <row r="2283" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2283">
+        <v>5883</v>
+      </c>
+      <c r="B2283" s="16" t="s">
+        <v>2420</v>
+      </c>
+    </row>
+    <row r="2284" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2284">
+        <v>5884</v>
+      </c>
+      <c r="B2284" t="s">
+        <v>2421</v>
+      </c>
+    </row>
+    <row r="2285" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2285">
+        <v>5885</v>
+      </c>
+      <c r="B2285" t="s">
+        <v>2452</v>
+      </c>
+    </row>
+    <row r="2286" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2286">
+        <v>5886</v>
+      </c>
+      <c r="B2286" t="s">
+        <v>2422</v>
+      </c>
+    </row>
+    <row r="2287" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2287">
+        <v>5887</v>
+      </c>
+      <c r="B2287" t="s">
+        <v>2453</v>
+      </c>
+    </row>
+    <row r="2288" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2288">
+        <v>5894</v>
+      </c>
+      <c r="B2288" t="s">
+        <v>2398</v>
+      </c>
+    </row>
+    <row r="2289" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2289">
+        <v>6209</v>
+      </c>
+      <c r="B2289" t="s">
+        <v>2399</v>
+      </c>
+    </row>
+    <row r="2290" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2290">
+        <v>6213</v>
+      </c>
+      <c r="B2290" s="12" t="s">
+        <v>2407</v>
+      </c>
+    </row>
+    <row r="2291" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2291">
+        <v>6221</v>
+      </c>
+      <c r="B2291" s="12" t="s">
+        <v>2408</v>
+      </c>
+    </row>
+    <row r="2292" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2292">
+        <v>6224</v>
+      </c>
+      <c r="B2292" s="16" t="s">
+        <v>2423</v>
+      </c>
+    </row>
+    <row r="2293" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2293">
+        <v>6225</v>
+      </c>
+      <c r="B2293" t="s">
+        <v>2424</v>
+      </c>
+    </row>
+    <row r="2294" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2294">
+        <v>6232</v>
+      </c>
+      <c r="B2294" t="s">
+        <v>2400</v>
+      </c>
+    </row>
+    <row r="2295" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2295">
+        <v>6862</v>
+      </c>
+      <c r="B2295" t="s">
+        <v>2401</v>
+      </c>
+    </row>
+    <row r="2296" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2296">
+        <v>6885</v>
+      </c>
+      <c r="B2296" s="12" t="s">
+        <v>2409</v>
+      </c>
+    </row>
+    <row r="2297" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2297">
+        <v>6888</v>
+      </c>
+      <c r="B2297" s="16" t="s">
+        <v>2425</v>
+      </c>
+    </row>
+    <row r="2298" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2298">
+        <v>6899</v>
+      </c>
+      <c r="B2298" s="12" t="s">
+        <v>2410</v>
+      </c>
+    </row>
+    <row r="2299" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2299">
+        <v>6902</v>
+      </c>
+      <c r="B2299" s="16" t="s">
+        <v>2426</v>
+      </c>
+      <c r="D2299" t="s">
+        <v>2454</v>
+      </c>
+    </row>
+    <row r="2300" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2300">
+        <v>6927</v>
+      </c>
+      <c r="B2300" s="16" t="s">
+        <v>2427</v>
+      </c>
+    </row>
+    <row r="2301" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2301">
+        <v>6950</v>
+      </c>
+      <c r="B2301" s="16" t="s">
+        <v>2428</v>
+      </c>
+    </row>
+    <row r="2302" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2302">
+        <v>6973</v>
+      </c>
+      <c r="B2302" s="16" t="s">
+        <v>2429</v>
+      </c>
+    </row>
+    <row r="2303" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2303">
+        <v>6996</v>
+      </c>
+      <c r="B2303" s="16" t="s">
+        <v>2430</v>
+      </c>
+    </row>
+    <row r="2304" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2304">
+        <v>7019</v>
+      </c>
+      <c r="B2304" s="16" t="s">
+        <v>2431</v>
+      </c>
+    </row>
+    <row r="2305" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2305">
+        <v>7042</v>
+      </c>
+      <c r="B2305" s="16" t="s">
+        <v>2432</v>
+      </c>
+    </row>
+    <row r="2306" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2306">
+        <v>7065</v>
+      </c>
+      <c r="B2306" s="16" t="s">
+        <v>2433</v>
+      </c>
+    </row>
+    <row r="2307" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2307">
+        <v>7088</v>
+      </c>
+      <c r="B2307" s="16" t="s">
+        <v>2434</v>
+      </c>
+    </row>
+    <row r="2308" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2308">
+        <v>7111</v>
+      </c>
+      <c r="B2308" s="16" t="s">
+        <v>2435</v>
+      </c>
+    </row>
+    <row r="2309" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2309">
+        <v>7134</v>
+      </c>
+      <c r="B2309" s="16" t="s">
+        <v>2436</v>
+      </c>
+    </row>
+    <row r="2310" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2310">
+        <v>7157</v>
+      </c>
+      <c r="B2310" s="16" t="s">
+        <v>2437</v>
+      </c>
+    </row>
+    <row r="2311" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2311">
+        <v>7180</v>
+      </c>
+      <c r="B2311" s="16" t="s">
+        <v>2438</v>
+      </c>
+    </row>
+    <row r="2312" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2312">
+        <v>7203</v>
+      </c>
+      <c r="B2312" s="16" t="s">
+        <v>2439</v>
+      </c>
+    </row>
+    <row r="2313" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2313">
+        <v>7204</v>
+      </c>
+      <c r="B2313" t="s">
+        <v>2440</v>
+      </c>
+    </row>
+    <row r="2314" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2314">
+        <v>7227</v>
+      </c>
+      <c r="B2314" s="16" t="s">
+        <v>2441</v>
+      </c>
+    </row>
+    <row r="2315" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2315">
+        <v>7228</v>
+      </c>
+      <c r="B2315" t="s">
+        <v>2442</v>
+      </c>
+    </row>
+    <row r="2316" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2316">
+        <v>7251</v>
+      </c>
+      <c r="B2316" s="16" t="s">
+        <v>2443</v>
+      </c>
+    </row>
+    <row r="2317" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2317">
+        <v>7252</v>
+      </c>
+      <c r="B2317" t="s">
+        <v>2444</v>
+      </c>
+    </row>
+    <row r="2318" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2318">
+        <v>7275</v>
+      </c>
+      <c r="B2318" s="16" t="s">
+        <v>2445</v>
+      </c>
+    </row>
+    <row r="2319" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2319">
+        <v>7298</v>
+      </c>
+      <c r="B2319" s="16" t="s">
+        <v>2446</v>
+      </c>
+    </row>
+    <row r="2320" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2320">
+        <v>7321</v>
+      </c>
+      <c r="B2320" s="16" t="s">
+        <v>2447</v>
+      </c>
+    </row>
+    <row r="2321" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2321">
+        <v>7325</v>
+      </c>
+      <c r="B2321" t="s">
+        <v>2402</v>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter ref="A2172:B2245" xr:uid="{00BC6913-1260-4FDB-BC1F-F2231612BD43}"/>
-  <sortState ref="A1802:B1946">
-    <sortCondition ref="A1802:A1946"/>
+  <autoFilter ref="A2256:B2321" xr:uid="{AA991574-F325-4C54-AC69-6022E43693E7}"/>
+  <sortState ref="A2257:L2321">
+    <sortCondition ref="A2257:A2321"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -28580,10 +29344,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A827A58D-C8A4-4858-A89B-E853C083564F}">
-  <dimension ref="A1:I24"/>
+  <dimension ref="A1:I26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B22" sqref="B22"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -28770,22 +29534,17 @@
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
-        <v>2342</v>
-      </c>
-    </row>
-    <row r="20" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B20" t="s">
-        <v>2386</v>
+        <v>2384</v>
       </c>
     </row>
     <row r="21" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B21" t="s">
-        <v>2387</v>
+        <v>2386</v>
       </c>
     </row>
     <row r="22" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B22" t="s">
-        <v>2384</v>
+        <v>2387</v>
       </c>
     </row>
     <row r="23" spans="2:2" x14ac:dyDescent="0.25">
@@ -28796,6 +29555,16 @@
     <row r="24" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B24" t="s">
         <v>2362</v>
+      </c>
+    </row>
+    <row r="25" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B25" t="s">
+        <v>2342</v>
+      </c>
+    </row>
+    <row r="26" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B26" t="s">
+        <v>2388</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
mix input and go to without input
</commit_message>
<xml_diff>
--- a/RBG_arduino/StateTable_minimal.xlsx
+++ b/RBG_arduino/StateTable_minimal.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/markdolson/GitHub-Mark-MDO47/RubberBandGun/RBG_arduino/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9363237C-F3CA-A14A-A3BD-83446585470F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C824E99-92A9-274C-9BEF-CA4BBA42D1A4}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1100" yWindow="960" windowWidth="25600" windowHeight="15540" xr2:uid="{CCADFEE4-B0E1-4363-9617-1683960BED03}"/>
+    <workbookView xWindow="1100" yWindow="960" windowWidth="25600" windowHeight="15540" activeTab="2" xr2:uid="{CCADFEE4-B0E1-4363-9617-1683960BED03}"/>
   </bookViews>
   <sheets>
     <sheet name="StateTable" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
     <sheet name="ThingsToTry" sheetId="5" r:id="rId5"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">debugging!$A$2518:$B$2537</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">debugging!$A$2649:$B$2695</definedName>
     <definedName name="yxcmd">'YX5200 info'!$A$2:$C$44</definedName>
   </definedNames>
   <calcPr calcId="181029"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3620" uniqueCount="2716">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3555" uniqueCount="2752">
   <si>
     <t>trigOnly</t>
   </si>
@@ -8060,261 +8060,6 @@
     <t xml:space="preserve"> RBG_waitForInput ln 383 thisReturn 255 loopCount 205</t>
   </si>
   <si>
-    <t>DEBUG loop() - nowVinputRBG 0x280 loopCount 206</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> RBG_waitForInput entry ln 337 tmpVinputRBG 0x280 loopCount 206</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> RBG_waitForInput ln 342 idx 1 thisRowPtr-&gt;inputRBG 0x30 loopCount 206</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> RBG_waitForInput ln 342 idx 2 thisRowPtr-&gt;inputRBG 0x80 loopCount 206</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> RBG_waitForInput ln 342 idx 3 thisRowPtr-&gt;inputRBG 0x40 loopCount 206</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> RBG_waitForInput ln 370 loopCount 206</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> RBG_waitForInput ln 383 thisReturn 255 loopCount 206</t>
-  </si>
-  <si>
-    <t>DEBUG loop() - nowVinputRBG 0x280 loopCount 207</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> RBG_waitForInput entry ln 337 tmpVinputRBG 0x280 loopCount 207</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> RBG_waitForInput ln 342 idx 1 thisRowPtr-&gt;inputRBG 0x30 loopCount 207</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> RBG_waitForInput ln 342 idx 2 thisRowPtr-&gt;inputRBG 0x80 loopCount 207</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> RBG_waitForInput ln 342 idx 3 thisRowPtr-&gt;inputRBG 0x40 loopCount 207</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> RBG_waitForInput ln 370 loopCount 207</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> RBG_waitForInput ln 383 thisReturn 255 loopCount 207</t>
-  </si>
-  <si>
-    <t>DEBUG loop() - nowVinputRBG 0x280 loopCount 208</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> RBG_waitForInput entry ln 337 tmpVinputRBG 0x280 loopCount 208</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> RBG_waitForInput ln 342 idx 1 thisRowPtr-&gt;inputRBG 0x30 loopCount 208</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> RBG_waitForInput ln 342 idx 2 thisRowPtr-&gt;inputRBG 0x80 loopCount 208</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> RBG_waitForInput ln 342 idx 3 thisRowPtr-&gt;inputRBG 0x40 loopCount 208</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> RBG_waitForInput ln 370 loopCount 208</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> RBG_waitForInput ln 383 thisReturn 255 loopCount 208</t>
-  </si>
-  <si>
-    <t>DEBUG loop() - nowVinputRBG 0x280 loopCount 209</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> RBG_waitForInput entry ln 337 tmpVinputRBG 0x280 loopCount 209</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> RBG_waitForInput ln 342 idx 1 thisRowPtr-&gt;inputRBG 0x30 loopCount 209</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> RBG_waitForInput ln 342 idx 2 thisRowPtr-&gt;inputRBG 0x80 loopCount 209</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> RBG_waitForInput ln 342 idx 3 thisRowPtr-&gt;inputRBG 0x40 loopCount 209</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> RBG_waitForInput ln 370 loopCount 209</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> RBG_waitForInput ln 383 thisReturn 255 loopCount 209</t>
-  </si>
-  <si>
-    <t>DEBUG loop() - nowVinputRBG 0x280 loopCount 210</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> RBG_waitForInput entry ln 337 tmpVinputRBG 0x280 loopCount 210</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> RBG_waitForInput ln 342 idx 1 thisRowPtr-&gt;inputRBG 0x30 loopCount 210</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> RBG_waitForInput ln 342 idx 2 thisRowPtr-&gt;inputRBG 0x80 loopCount 210</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> RBG_waitForInput ln 342 idx 3 thisRowPtr-&gt;inputRBG 0x40 loopCount 210</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> RBG_waitForInput ln 370 loopCount 210</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> RBG_waitForInput ln 383 thisReturn 255 loopCount 210</t>
-  </si>
-  <si>
-    <t>DEBUG loop() - nowVinputRBG 0x280 loopCount 211</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> RBG_waitForInput entry ln 337 tmpVinputRBG 0x280 loopCount 211</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> RBG_waitForInput ln 342 idx 1 thisRowPtr-&gt;inputRBG 0x30 loopCount 211</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> RBG_waitForInput ln 342 idx 2 thisRowPtr-&gt;inputRBG 0x80 loopCount 211</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> RBG_waitForInput ln 342 idx 3 thisRowPtr-&gt;inputRBG 0x40 loopCount 211</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> RBG_waitForInput ln 370 loopCount 211</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> RBG_waitForInput ln 383 thisReturn 255 loopCount 211</t>
-  </si>
-  <si>
-    <t>DEBUG loop() - nowVinputRBG 0x280 loopCount 212</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> RBG_waitForInput entry ln 337 tmpVinputRBG 0x280 loopCount 212</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> RBG_waitForInput ln 342 idx 1 thisRowPtr-&gt;inputRBG 0x30 loopCount 212</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> RBG_waitForInput ln 342 idx 2 thisRowPtr-&gt;inputRBG 0x80 loopCount 212</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> RBG_waitForInput ln 342 idx 3 thisRowPtr-&gt;inputRBG 0x40 loopCount 212</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> RBG_waitForInput ln 370 loopCount 212</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> RBG_waitForInput ln 383 thisReturn 255 loopCount 212</t>
-  </si>
-  <si>
-    <t>DEBUG loop() - nowVinputRBG 0x280 loopCount 213</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> RBG_waitForInput entry ln 337 tmpVinputRBG 0x280 loopCount 213</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> RBG_waitForInput ln 342 idx 1 thisRowPtr-&gt;inputRBG 0x30 loopCount 213</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> RBG_waitForInput ln 342 idx 2 thisRowPtr-&gt;inputRBG 0x80 loopCount 213</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> RBG_waitForInput ln 342 idx 3 thisRowPtr-&gt;inputRBG 0x40 loopCount 213</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> RBG_waitForInput ln 370 loopCount 213</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> RBG_waitForInput ln 383 thisReturn 255 loopCount 213</t>
-  </si>
-  <si>
-    <t>DEBUG loop() - nowVinputRBG 0x280 loopCount 214</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> RBG_waitForInput entry ln 337 tmpVinputRBG 0x280 loopCount 214</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> RBG_waitForInput ln 342 idx 1 thisRowPtr-&gt;inputRBG 0x30 loopCount 214</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> RBG_waitForInput ln 342 idx 2 thisRowPtr-&gt;inputRBG 0x80 loopCount 214</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> RBG_waitForInput ln 342 idx 3 thisRowPtr-&gt;inputRBG 0x40 loopCount 214</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> RBG_waitForInput ln 370 loopCount 214</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> RBG_waitForInput ln 383 thisReturn 255 loopCount 214</t>
-  </si>
-  <si>
-    <t>DEBUG loop() - nowVinputRBG 0x280 loopCount 215</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> RBG_waitForInput entry ln 337 tmpVinputRBG 0x280 loopCount 215</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> RBG_waitForInput ln 342 idx 1 thisRowPtr-&gt;inputRBG 0x30 loopCount 215</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> RBG_waitForInput ln 342 idx 2 thisRowPtr-&gt;inputRBG 0x80 loopCount 215</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> RBG_waitForInput ln 342 idx 3 thisRowPtr-&gt;inputRBG 0x40 loopCount 215</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> RBG_waitForInput ln 370 loopCount 215</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> RBG_waitForInput ln 383 thisReturn 255 loopCount 215</t>
-  </si>
-  <si>
-    <t>DEBUG loop() - nowVinputRBG 0x280 loopCount 216</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> RBG_waitForInput entry ln 337 tmpVinputRBG 0x280 loopCount 216</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> RBG_waitForInput ln 342 idx 1 thisRowPtr-&gt;inputRBG 0x30 loopCount 216</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> RBG_waitForInput ln 342 idx 2 thisRowPtr-&gt;inputRBG 0x80 loopCount 216</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> RBG_waitForInput ln 342 idx 3 thisRowPtr-&gt;inputRBG 0x40 loopCount 216</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> RBG_waitForInput ln 370 loopCount 216</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> RBG_waitForInput ln 383 thisReturn 255 loopCount 216</t>
-  </si>
-  <si>
-    <t>DEBUG loop() - nowVinputRBG 0x280 loopCount 217</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> RBG_waitForInput entry ln 337 tmpVinputRBG 0x280 loopCount 217</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> RBG_waitForInput ln 342 idx 1 thisRowPtr-&gt;inputRBG 0x30 loopCount 217</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> RBG_waitForInput ln 342 idx 2 thisRowPtr-&gt;inputRBG 0x80 loopCount 217</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> RBG_waitForInput ln 342 idx 3 thisRowPtr-&gt;inputRBG 0x40 loopCount 217</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> RBG_waitForInput ln 370 loopCount 217</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> RBG_waitForInput ln 383 thisReturn 255 loopCount 217</t>
-  </si>
-  <si>
-    <t>c</t>
-  </si>
-  <si>
     <r>
       <t xml:space="preserve">checkButtons() called: DEBUG - printAllMyInputs: DPIN_BTN_TRIGGER HIGH DPIN_BTN_YELLOW HIGH DPIN_BTN_GREEN HIGH DPIN_BTN_BLACK HIGH </t>
     </r>
@@ -8405,6 +8150,369 @@
       </rPr>
       <t xml:space="preserve"> loopCount 205</t>
     </r>
+  </si>
+  <si>
+    <t>17: RBG_startEffectSound ln 476 EFCT num 0x28 final num 41 loopCount 0</t>
+  </si>
+  <si>
+    <t>18: RBG_startEffectSound ln 511 myDFPlayer problem after check busy</t>
+  </si>
+  <si>
+    <t>449:DEBUG loop() - nowVinputRBG 0x40 loopCount 134</t>
+  </si>
+  <si>
+    <t>460: RBG_startRow ln 276 from row 0 to row 1 loopCount 135</t>
+  </si>
+  <si>
+    <t>492: RBG_startRow ln 276 from row 1 to row 5 loopCount 137</t>
+  </si>
+  <si>
+    <t>495: RBG_startEffectSound ln 476 EFCT num 0x66 final num 102 loopCount 137</t>
+  </si>
+  <si>
+    <t>496: RBG_startEffectSound ln 504 myDFPlayer problem after play</t>
+  </si>
+  <si>
+    <t>497:Number:41 Play Finished!</t>
+  </si>
+  <si>
+    <t>498: RBG_startEffectSound ln 511 myDFPlayer problem after check busy</t>
+  </si>
+  <si>
+    <t>499:Number:41 Play Finished!</t>
+  </si>
+  <si>
+    <t>511:DEBUG loop() - nowVinputRBG 0x240 loopCount 138</t>
+  </si>
+  <si>
+    <t>1933:DEBUG loop() - nowVinputRBG 0x260 loopCount 217</t>
+  </si>
+  <si>
+    <t>1951: RBG_startRow ln 276 from row 5 to row 7 loopCount 218</t>
+  </si>
+  <si>
+    <t>1954: RBG_startEffectSound ln 476 EFCT num 0x0 final num 1 loopCount 218</t>
+  </si>
+  <si>
+    <t>1967:DEBUG loop() - nowVinputRBG 0x240 loopCount 219</t>
+  </si>
+  <si>
+    <t>3644:DEBUG loop() - nowVinputRBG 0x40 loopCount 778</t>
+  </si>
+  <si>
+    <t>3655: RBG_startRow ln 276 from row 7 to row 8 loopCount 779</t>
+  </si>
+  <si>
+    <t>3663: RBG_startRow ln 276 from row 8 to row 9 loopCount 781</t>
+  </si>
+  <si>
+    <t>3666: RBG_startEffectSound ln 476 EFCT num 0xA final num 11 loopCount 781</t>
+  </si>
+  <si>
+    <t>3667: RBG_startEffectSound ln 504 myDFPlayer problem after play</t>
+  </si>
+  <si>
+    <t>3668:Number:1 Play Finished!</t>
+  </si>
+  <si>
+    <t>3669: RBG_startEffectSound ln 511 myDFPlayer problem after check busy</t>
+  </si>
+  <si>
+    <t>3670:Number:1 Play Finished!</t>
+  </si>
+  <si>
+    <t>3677:DEBUG loop() - nowVinputRBG 0x240 loopCount 782</t>
+  </si>
+  <si>
+    <t>3992:DEBUG loop() - nowVinputRBG 0x40 loopCount 887</t>
+  </si>
+  <si>
+    <t>3996: RBG_startRow ln 276 from row 9 to row 10 loopCount 888</t>
+  </si>
+  <si>
+    <t>4004: RBG_startRow ln 276 from row 10 to row 1 loopCount 890</t>
+  </si>
+  <si>
+    <t>4030: RBG_startRow ln 276 from row 1 to row 5 loopCount 892</t>
+  </si>
+  <si>
+    <t>4033: RBG_startEffectSound ln 476 EFCT num 0x66 final num 102 loopCount 892</t>
+  </si>
+  <si>
+    <t>4034: RBG_startEffectSound ln 511 myDFPlayer problem after check busy</t>
+  </si>
+  <si>
+    <t>4041:DEBUG loop() - nowVinputRBG 0x240 loopCount 893</t>
+  </si>
+  <si>
+    <t>4383:DEBUG loop() - nowVinputRBG 0x280 loopCount 912</t>
+  </si>
+  <si>
+    <t>4404: RBG_startRow ln 276 from row 5 to row 11 loopCount 913</t>
+  </si>
+  <si>
+    <t>4407: RBG_startEffectSound ln 476 EFCT num 0x14 final num 21 loopCount 913</t>
+  </si>
+  <si>
+    <t>4840:DEBUG loop() - nowVinputRBG 0x80 loopCount 1056</t>
+  </si>
+  <si>
+    <t>4844: RBG_startRow ln 276 from row 11 to row 1 loopCount 1057</t>
+  </si>
+  <si>
+    <t>4849:DEBUG loop() - nowVinputRBG 0x40 loopCount 1058</t>
+  </si>
+  <si>
+    <t>4870: RBG_startRow ln 276 from row 1 to row 5 loopCount 1059</t>
+  </si>
+  <si>
+    <t>4873: RBG_startEffectSound ln 476 EFCT num 0x66 final num 102 loopCount 1059</t>
+  </si>
+  <si>
+    <t>4874: RBG_startEffectSound ln 504 myDFPlayer problem after play</t>
+  </si>
+  <si>
+    <t>4875:Number:21 Play Finished!</t>
+  </si>
+  <si>
+    <t>4876: RBG_startEffectSound ln 511 myDFPlayer problem after check busy</t>
+  </si>
+  <si>
+    <t>4877:Number:21 Play Finished!</t>
+  </si>
+  <si>
+    <t>4883:DEBUG loop() - nowVinputRBG 0x240 loopCount 1060</t>
+  </si>
+  <si>
+    <t>5639:DEBUG loop() - nowVinputRBG 0x280 loopCount 1102</t>
+  </si>
+  <si>
+    <t>5660: RBG_startRow ln 276 from row 5 to row 11 loopCount 1103</t>
+  </si>
+  <si>
+    <t>5663: RBG_startEffectSound ln 476 EFCT num 0x14 final num 21 loopCount 1103</t>
+  </si>
+  <si>
+    <t>5670:DEBUG loop() - nowVinputRBG 0x80 loopCount 1104</t>
+  </si>
+  <si>
+    <t>5673:DEBUG loop() - nowVinputRBG 0x280 loopCount 1105</t>
+  </si>
+  <si>
+    <t>5674: RBG_startRow ln 276 from row 11 to row 1 loopCount 1105</t>
+  </si>
+  <si>
+    <t>5690: RBG_startRow ln 276 from row 1 to row 3 loopCount 1107</t>
+  </si>
+  <si>
+    <t>5693: RBG_startEffectSound ln 476 EFCT num 0x66 final num 102 loopCount 1107</t>
+  </si>
+  <si>
+    <t>5699:DEBUG loop() - nowVinputRBG 0x80 loopCount 1108</t>
+  </si>
+  <si>
+    <t>5711: RBG_startEffectSound ln 476 EFCT num 0x66 final num 102 loopCount 1108</t>
+  </si>
+  <si>
+    <t>5715:DEBUG loop() - nowVinputRBG 0x280 loopCount 1109</t>
+  </si>
+  <si>
+    <t>6947:DEBUG loop() - nowVinputRBG 0x240 loopCount 1197</t>
+  </si>
+  <si>
+    <t>6962: RBG_startRow ln 276 from row 3 to row 12 loopCount 1198</t>
+  </si>
+  <si>
+    <t>6965: RBG_startEffectSound ln 476 EFCT num 0x1E final num 31 loopCount 1198</t>
+  </si>
+  <si>
+    <t>7407:DEBUG loop() - nowVinputRBG 0x40 loopCount 1344</t>
+  </si>
+  <si>
+    <t>7411: RBG_startRow ln 276 from row 12 to row 1 loopCount 1345</t>
+  </si>
+  <si>
+    <t>7431: RBG_startRow ln 276 from row 1 to row 5 loopCount 1347</t>
+  </si>
+  <si>
+    <t>7434: RBG_startEffectSound ln 476 EFCT num 0x66 final num 102 loopCount 1347</t>
+  </si>
+  <si>
+    <t>7435: RBG_startEffectSound ln 504 myDFPlayer problem after play</t>
+  </si>
+  <si>
+    <t>7436:Number:31 Play Finished!</t>
+  </si>
+  <si>
+    <t>7437: RBG_startEffectSound ln 511 myDFPlayer problem after check busy</t>
+  </si>
+  <si>
+    <t>7443:DEBUG loop() - nowVinputRBG 0x240 loopCount 1348</t>
+  </si>
+  <si>
+    <t>10377:DEBUG loop() - nowVinputRBG 0x40 loopCount 1511</t>
+  </si>
+  <si>
+    <t>#define mROW_MENU 1</t>
+  </si>
+  <si>
+    <t>#define mROW_MENU_OPEN 3</t>
+  </si>
+  <si>
+    <t>#define mROW_MENU_CLOSED 5</t>
+  </si>
+  <si>
+    <t>#define mROW_WINDUP_SOUND 7</t>
+  </si>
+  <si>
+    <t>#define mROW_SHOOT 8</t>
+  </si>
+  <si>
+    <t>#define mROW_SHOOT_SOUND 9</t>
+  </si>
+  <si>
+    <t>#define mROW_SOLENOID 10</t>
+  </si>
+  <si>
+    <t>#define mROW_OPNBRL 11</t>
+  </si>
+  <si>
+    <t>#define mROW_LOKLOD 12</t>
+  </si>
+  <si>
+    <t>menu_closed</t>
+  </si>
+  <si>
+    <t>WINDUP_SOUND</t>
+  </si>
+  <si>
+    <t>trigger</t>
+  </si>
+  <si>
+    <t>mix input and go to without input</t>
+  </si>
+  <si>
+    <t>495: RBG_startRow ln 276 from row 1 to row 5 loopCount 138</t>
+  </si>
+  <si>
+    <t>498: RBG_startEffectSound ln 476 EFCT num 0x66 final num 102 loopCount 138</t>
+  </si>
+  <si>
+    <t>499: RBG_startEffectSound ln 504 myDFPlayer problem after play</t>
+  </si>
+  <si>
+    <t>500:Number:41 Play Finished!</t>
+  </si>
+  <si>
+    <t>501: RBG_startEffectSound ln 511 myDFPlayer problem after check busy</t>
+  </si>
+  <si>
+    <t>502:Number:41 Play Finished!</t>
+  </si>
+  <si>
+    <t>514:DEBUG loop() - nowVinputRBG 0x240 loopCount 139</t>
+  </si>
+  <si>
+    <t>2890:DEBUG loop() - nowVinputRBG 0x280 loopCount 271</t>
+  </si>
+  <si>
+    <t>2911: RBG_startRow ln 276 from row 5 to row 11 loopCount 272</t>
+  </si>
+  <si>
+    <t>2914: RBG_startEffectSound ln 476 EFCT num 0x14 final num 21 loopCount 272</t>
+  </si>
+  <si>
+    <t>3320:DEBUG loop() - nowVinputRBG 0x240 loopCount 404</t>
+  </si>
+  <si>
+    <t>3353:DEBUG loop() - nowVinputRBG 0x40 loopCount 415</t>
+  </si>
+  <si>
+    <t>3364: RBG_startRow ln 276 from row 11 to row 1 loopCount 416</t>
+  </si>
+  <si>
+    <t>3390: RBG_startRow ln 276 from row 1 to row 5 loopCount 418</t>
+  </si>
+  <si>
+    <t>3393: RBG_startEffectSound ln 476 EFCT num 0x66 final num 102 loopCount 418</t>
+  </si>
+  <si>
+    <t>3394: RBG_startEffectSound ln 504 myDFPlayer problem after play</t>
+  </si>
+  <si>
+    <t>3395:Number:21 Play Finished!</t>
+  </si>
+  <si>
+    <t>3396: RBG_startEffectSound ln 511 myDFPlayer problem after check busy</t>
+  </si>
+  <si>
+    <t>3402:DEBUG loop() - nowVinputRBG 0x240 loopCount 419</t>
+  </si>
+  <si>
+    <t>3600:DEBUG loop() - nowVinputRBG 0x280 loopCount 430</t>
+  </si>
+  <si>
+    <t>3621: RBG_startRow ln 276 from row 5 to row 11 loopCount 431</t>
+  </si>
+  <si>
+    <t>3624: RBG_startEffectSound ln 476 EFCT num 0x14 final num 21 loopCount 431</t>
+  </si>
+  <si>
+    <t>3631:DEBUG loop() - nowVinputRBG 0x80 loopCount 432</t>
+  </si>
+  <si>
+    <t>3634:DEBUG loop() - nowVinputRBG 0x280 loopCount 433</t>
+  </si>
+  <si>
+    <t>3635: RBG_startRow ln 276 from row 11 to row 1 loopCount 433</t>
+  </si>
+  <si>
+    <t>3657: RBG_startRow ln 276 from row 1 to row 3 loopCount 435</t>
+  </si>
+  <si>
+    <t>3660: RBG_startEffectSound ln 476 EFCT num 0x66 final num 102 loopCount 435</t>
+  </si>
+  <si>
+    <t>3666:DEBUG loop() - nowVinputRBG 0x80 loopCount 436</t>
+  </si>
+  <si>
+    <t>3678: RBG_startEffectSound ln 476 EFCT num 0x66 final num 102 loopCount 436</t>
+  </si>
+  <si>
+    <t>3694: RBG_startEffectSound ln 476 EFCT num 0x66 final num 102 loopCount 437</t>
+  </si>
+  <si>
+    <t>3698:DEBUG loop() - nowVinputRBG 0x240 loopCount 438</t>
+  </si>
+  <si>
+    <t>3719: RBG_startRow ln 276 from row 3 to row 13 loopCount 439</t>
+  </si>
+  <si>
+    <t>3722: RBG_startEffectSound ln 476 EFCT num 0x1E final num 31 loopCount 439</t>
+  </si>
+  <si>
+    <t>4164:DEBUG loop() - nowVinputRBG 0x40 loopCount 585</t>
+  </si>
+  <si>
+    <t>4168: RBG_startRow ln 276 from row 13 to row 1 loopCount 586</t>
+  </si>
+  <si>
+    <t>4188: RBG_startRow ln 276 from row 1 to row 5 loopCount 588</t>
+  </si>
+  <si>
+    <t>4191: RBG_startEffectSound ln 476 EFCT num 0x66 final num 102 loopCount 588</t>
+  </si>
+  <si>
+    <t>4192: RBG_startEffectSound ln 511 myDFPlayer problem after check busy</t>
+  </si>
+  <si>
+    <t>4193:Number:31 Play Finished!</t>
+  </si>
+  <si>
+    <t>4199:DEBUG loop() - nowVinputRBG 0x240 loopCount 589</t>
+  </si>
+  <si>
+    <t>#define mROW_LOKLOD 13</t>
   </si>
 </sst>
 </file>
@@ -8492,7 +8600,7 @@
       <name val="Calibri (Body)_x0000_"/>
     </font>
   </fonts>
-  <fills count="9">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -8533,6 +8641,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF7030A0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -8608,7 +8728,7 @@
     <xf numFmtId="0" fontId="5" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="6" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -8648,6 +8768,8 @@
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="9" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="9" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Bad" xfId="2" builtinId="27"/>
@@ -8969,9 +9091,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{90E8DFC6-94F4-4A82-A874-2F16F2CF0145}">
   <dimension ref="A1:R28"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C4" sqref="C4"/>
+      <selection pane="bottomLeft" activeCell="I27" sqref="I27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
@@ -9485,48 +9607,69 @@
         <v>66</v>
       </c>
     </row>
-    <row r="24" spans="1:14">
+    <row r="24" spans="1:14" ht="16">
       <c r="A24" s="9"/>
       <c r="B24" s="9"/>
-      <c r="C24" s="9" t="s">
-        <v>67</v>
-      </c>
-      <c r="D24" s="9"/>
-      <c r="E24" s="9"/>
-      <c r="F24" s="9"/>
+      <c r="C24" s="13" t="s">
+        <v>68</v>
+      </c>
+      <c r="D24" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="E24" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="F24" s="9" t="s">
+        <v>4</v>
+      </c>
       <c r="G24" s="9"/>
       <c r="H24" s="9"/>
-      <c r="I24" s="9"/>
+      <c r="I24" s="9" t="s">
+        <v>69</v>
+      </c>
       <c r="J24" s="9"/>
     </row>
-    <row r="25" spans="1:14" ht="16">
-      <c r="A25" s="9" t="s">
-        <v>63</v>
-      </c>
-      <c r="B25" s="9"/>
-      <c r="C25" s="9" t="s">
-        <v>69</v>
-      </c>
-      <c r="D25" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="E25" s="3" t="s">
-        <v>59</v>
-      </c>
+    <row r="25" spans="1:14">
       <c r="F25" s="9"/>
       <c r="G25" s="9"/>
       <c r="H25" s="9"/>
       <c r="I25" s="9"/>
-      <c r="J25" s="9" t="s">
+    </row>
+    <row r="26" spans="1:14" ht="16">
+      <c r="A26" s="9" t="s">
+        <v>63</v>
+      </c>
+      <c r="B26" s="9"/>
+      <c r="C26" s="9" t="s">
+        <v>69</v>
+      </c>
+      <c r="D26" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="E26" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="J26" s="9" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="26" spans="1:14">
-      <c r="C26" s="9"/>
-    </row>
-    <row r="27" spans="1:14">
+    <row r="27" spans="1:14" ht="16">
       <c r="B27" s="9"/>
-      <c r="D27" s="3"/>
+      <c r="C27" s="13" t="s">
+        <v>69</v>
+      </c>
+      <c r="D27" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="E27" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="F27" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="I27" s="9" t="s">
+        <v>68</v>
+      </c>
     </row>
     <row r="28" spans="1:14">
       <c r="N28" s="7"/>
@@ -9630,10 +9773,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F57F550E-21B4-4ED7-B7FF-211D228584A7}">
-  <dimension ref="A1:L2815"/>
+  <dimension ref="A1:L2695"/>
   <sheetViews>
-    <sheetView topLeftCell="B2521" workbookViewId="0">
-      <selection activeCell="B2545" sqref="B2545"/>
+    <sheetView tabSelected="1" topLeftCell="A2639" workbookViewId="0">
+      <selection activeCell="E2657" sqref="E2657"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
@@ -29189,7 +29332,7 @@
         <v>2590</v>
       </c>
       <c r="F2522" t="s">
-        <v>2712</v>
+        <v>2627</v>
       </c>
     </row>
     <row r="2523" spans="1:6">
@@ -29200,7 +29343,7 @@
         <v>2591</v>
       </c>
       <c r="F2523" t="s">
-        <v>2713</v>
+        <v>2628</v>
       </c>
     </row>
     <row r="2524" spans="1:6">
@@ -29379,7 +29522,7 @@
     </row>
     <row r="2542" spans="1:6">
       <c r="F2542" t="s">
-        <v>2714</v>
+        <v>2629</v>
       </c>
     </row>
     <row r="2543" spans="1:6">
@@ -29389,1362 +29532,1227 @@
     </row>
     <row r="2544" spans="1:6">
       <c r="F2544" t="s">
-        <v>2715</v>
-      </c>
-    </row>
-    <row r="2545" spans="6:6">
+        <v>2630</v>
+      </c>
+    </row>
+    <row r="2545" spans="2:6">
       <c r="F2545" t="s">
         <v>2618</v>
       </c>
     </row>
-    <row r="2546" spans="6:6">
+    <row r="2546" spans="2:6">
       <c r="F2546" t="s">
         <v>2619</v>
       </c>
     </row>
-    <row r="2547" spans="6:6">
+    <row r="2547" spans="2:6">
       <c r="F2547" t="s">
         <v>2459</v>
       </c>
     </row>
-    <row r="2548" spans="6:6">
+    <row r="2548" spans="2:6">
       <c r="F2548" t="s">
         <v>2620</v>
       </c>
     </row>
-    <row r="2549" spans="6:6">
+    <row r="2549" spans="2:6">
       <c r="F2549" t="s">
         <v>2462</v>
       </c>
     </row>
-    <row r="2550" spans="6:6">
+    <row r="2550" spans="2:6">
       <c r="F2550" t="s">
         <v>2621</v>
       </c>
     </row>
-    <row r="2551" spans="6:6">
+    <row r="2551" spans="2:6">
       <c r="F2551" t="s">
         <v>2622</v>
       </c>
     </row>
-    <row r="2552" spans="6:6">
+    <row r="2552" spans="2:6">
       <c r="F2552" t="s">
         <v>2464</v>
       </c>
     </row>
-    <row r="2553" spans="6:6">
+    <row r="2553" spans="2:6" ht="16" thickBot="1">
       <c r="F2553" t="s">
         <v>2623</v>
       </c>
     </row>
-    <row r="2554" spans="6:6">
+    <row r="2554" spans="2:6" ht="17" thickTop="1" thickBot="1">
+      <c r="B2554" s="1" t="s">
+        <v>2515</v>
+      </c>
       <c r="F2554" t="s">
         <v>2462</v>
       </c>
     </row>
-    <row r="2555" spans="6:6">
+    <row r="2555" spans="2:6" ht="16" thickTop="1">
       <c r="F2555" t="s">
         <v>2621</v>
       </c>
     </row>
-    <row r="2556" spans="6:6">
+    <row r="2556" spans="2:6">
+      <c r="B2556" t="s">
+        <v>129</v>
+      </c>
       <c r="F2556" t="s">
         <v>2624</v>
       </c>
     </row>
-    <row r="2557" spans="6:6">
+    <row r="2557" spans="2:6">
+      <c r="B2557" t="s">
+        <v>130</v>
+      </c>
       <c r="F2557" t="s">
         <v>2464</v>
       </c>
     </row>
-    <row r="2558" spans="6:6">
+    <row r="2558" spans="2:6">
+      <c r="B2558" t="s">
+        <v>924</v>
+      </c>
       <c r="F2558" t="s">
         <v>2620</v>
       </c>
     </row>
-    <row r="2559" spans="6:6">
+    <row r="2559" spans="2:6">
+      <c r="B2559" t="s">
+        <v>925</v>
+      </c>
+      <c r="C2559" t="s">
+        <v>2698</v>
+      </c>
       <c r="F2559" t="s">
         <v>2497</v>
       </c>
     </row>
-    <row r="2560" spans="6:6">
+    <row r="2560" spans="2:6">
+      <c r="B2560" t="s">
+        <v>430</v>
+      </c>
+      <c r="C2560" t="s">
+        <v>2699</v>
+      </c>
       <c r="F2560" t="s">
         <v>2621</v>
       </c>
     </row>
-    <row r="2561" spans="6:6">
+    <row r="2561" spans="1:6">
+      <c r="C2561" t="s">
+        <v>2700</v>
+      </c>
       <c r="F2561" t="s">
         <v>2625</v>
       </c>
     </row>
-    <row r="2562" spans="6:6">
+    <row r="2562" spans="1:6">
+      <c r="A2562" t="s">
+        <v>2097</v>
+      </c>
+      <c r="B2562" t="s">
+        <v>617</v>
+      </c>
+      <c r="C2562" t="s">
+        <v>2701</v>
+      </c>
       <c r="F2562" t="s">
         <v>2626</v>
       </c>
     </row>
-    <row r="2563" spans="6:6">
+    <row r="2563" spans="1:6">
+      <c r="A2563">
+        <v>14</v>
+      </c>
+      <c r="B2563" s="28" t="s">
+        <v>2587</v>
+      </c>
+      <c r="C2563" t="s">
+        <v>2702</v>
+      </c>
       <c r="F2563" t="s">
         <v>2456</v>
       </c>
     </row>
-    <row r="2564" spans="6:6">
+    <row r="2564" spans="1:6">
+      <c r="A2564">
+        <v>17</v>
+      </c>
+      <c r="B2564" s="16" t="s">
+        <v>2631</v>
+      </c>
+      <c r="C2564" t="s">
+        <v>2703</v>
+      </c>
       <c r="F2564" t="s">
         <v>2456</v>
       </c>
     </row>
-    <row r="2565" spans="6:6">
-      <c r="F2565" t="s">
-        <v>2627</v>
-      </c>
-    </row>
-    <row r="2566" spans="6:6">
-      <c r="F2566" t="s">
-        <v>2628</v>
-      </c>
-    </row>
-    <row r="2567" spans="6:6">
-      <c r="F2567" t="s">
-        <v>2629</v>
-      </c>
-    </row>
-    <row r="2568" spans="6:6">
-      <c r="F2568" t="s">
-        <v>2459</v>
-      </c>
-    </row>
-    <row r="2569" spans="6:6">
-      <c r="F2569" t="s">
-        <v>2620</v>
-      </c>
-    </row>
-    <row r="2570" spans="6:6">
-      <c r="F2570" t="s">
-        <v>2462</v>
-      </c>
-    </row>
-    <row r="2571" spans="6:6">
-      <c r="F2571" t="s">
-        <v>2621</v>
-      </c>
-    </row>
-    <row r="2572" spans="6:6">
-      <c r="F2572" t="s">
-        <v>2630</v>
-      </c>
-    </row>
-    <row r="2573" spans="6:6">
-      <c r="F2573" t="s">
-        <v>2464</v>
-      </c>
-    </row>
-    <row r="2574" spans="6:6">
-      <c r="F2574" t="s">
-        <v>2623</v>
-      </c>
-    </row>
-    <row r="2575" spans="6:6">
-      <c r="F2575" t="s">
-        <v>2462</v>
-      </c>
-    </row>
-    <row r="2576" spans="6:6">
-      <c r="F2576" t="s">
-        <v>2621</v>
-      </c>
-    </row>
-    <row r="2577" spans="6:6">
-      <c r="F2577" t="s">
+    <row r="2565" spans="1:6">
+      <c r="A2565">
+        <v>18</v>
+      </c>
+      <c r="B2565" t="s">
+        <v>2632</v>
+      </c>
+      <c r="C2565" t="s">
+        <v>2704</v>
+      </c>
+    </row>
+    <row r="2566" spans="1:6">
+      <c r="A2566">
+        <v>36</v>
+      </c>
+      <c r="B2566" s="28" t="s">
+        <v>2590</v>
+      </c>
+      <c r="C2566" t="s">
+        <v>2705</v>
+      </c>
+    </row>
+    <row r="2567" spans="1:6">
+      <c r="A2567">
+        <v>449</v>
+      </c>
+      <c r="B2567" s="28" t="s">
+        <v>2633</v>
+      </c>
+      <c r="C2567" t="s">
+        <v>2706</v>
+      </c>
+    </row>
+    <row r="2568" spans="1:6">
+      <c r="A2568">
+        <v>460</v>
+      </c>
+      <c r="B2568" s="12" t="s">
+        <v>2634</v>
+      </c>
+    </row>
+    <row r="2569" spans="1:6">
+      <c r="A2569">
+        <v>492</v>
+      </c>
+      <c r="B2569" s="12" t="s">
+        <v>2635</v>
+      </c>
+      <c r="C2569" t="s">
+        <v>2707</v>
+      </c>
+    </row>
+    <row r="2570" spans="1:6">
+      <c r="A2570">
+        <v>495</v>
+      </c>
+      <c r="B2570" s="16" t="s">
+        <v>2636</v>
+      </c>
+    </row>
+    <row r="2571" spans="1:6">
+      <c r="A2571">
+        <v>496</v>
+      </c>
+      <c r="B2571" t="s">
+        <v>2637</v>
+      </c>
+    </row>
+    <row r="2572" spans="1:6">
+      <c r="A2572">
+        <v>497</v>
+      </c>
+      <c r="B2572" s="27" t="s">
+        <v>2638</v>
+      </c>
+    </row>
+    <row r="2573" spans="1:6">
+      <c r="A2573">
+        <v>498</v>
+      </c>
+      <c r="B2573" t="s">
+        <v>2639</v>
+      </c>
+    </row>
+    <row r="2574" spans="1:6">
+      <c r="A2574">
+        <v>499</v>
+      </c>
+      <c r="B2574" s="27" t="s">
+        <v>2640</v>
+      </c>
+    </row>
+    <row r="2575" spans="1:6">
+      <c r="A2575">
+        <v>511</v>
+      </c>
+      <c r="B2575" s="28" t="s">
+        <v>2641</v>
+      </c>
+    </row>
+    <row r="2576" spans="1:6">
+      <c r="A2576">
+        <v>1933</v>
+      </c>
+      <c r="B2576" s="28" t="s">
+        <v>2642</v>
+      </c>
+      <c r="D2576" t="s">
+        <v>2709</v>
+      </c>
+    </row>
+    <row r="2577" spans="1:3">
+      <c r="A2577">
+        <v>1951</v>
+      </c>
+      <c r="B2577" s="12" t="s">
+        <v>2643</v>
+      </c>
+      <c r="C2577" t="s">
+        <v>2708</v>
+      </c>
+    </row>
+    <row r="2578" spans="1:3">
+      <c r="A2578">
+        <v>1954</v>
+      </c>
+      <c r="B2578" s="16" t="s">
+        <v>2644</v>
+      </c>
+    </row>
+    <row r="2579" spans="1:3">
+      <c r="A2579">
+        <v>1967</v>
+      </c>
+      <c r="B2579" s="28" t="s">
+        <v>2645</v>
+      </c>
+    </row>
+    <row r="2580" spans="1:3">
+      <c r="A2580">
+        <v>3644</v>
+      </c>
+      <c r="B2580" s="28" t="s">
+        <v>2646</v>
+      </c>
+    </row>
+    <row r="2581" spans="1:3">
+      <c r="A2581">
+        <v>3655</v>
+      </c>
+      <c r="B2581" s="12" t="s">
+        <v>2647</v>
+      </c>
+      <c r="C2581" t="s">
+        <v>2702</v>
+      </c>
+    </row>
+    <row r="2582" spans="1:3">
+      <c r="A2582">
+        <v>3663</v>
+      </c>
+      <c r="B2582" s="12" t="s">
+        <v>2648</v>
+      </c>
+      <c r="C2582" t="s">
+        <v>2703</v>
+      </c>
+    </row>
+    <row r="2583" spans="1:3">
+      <c r="A2583">
+        <v>3666</v>
+      </c>
+      <c r="B2583" s="16" t="s">
+        <v>2649</v>
+      </c>
+    </row>
+    <row r="2584" spans="1:3">
+      <c r="A2584">
+        <v>3667</v>
+      </c>
+      <c r="B2584" t="s">
+        <v>2650</v>
+      </c>
+    </row>
+    <row r="2585" spans="1:3">
+      <c r="A2585">
+        <v>3668</v>
+      </c>
+      <c r="B2585" s="27" t="s">
+        <v>2651</v>
+      </c>
+    </row>
+    <row r="2586" spans="1:3">
+      <c r="A2586">
+        <v>3669</v>
+      </c>
+      <c r="B2586" t="s">
+        <v>2652</v>
+      </c>
+    </row>
+    <row r="2587" spans="1:3">
+      <c r="A2587">
+        <v>3670</v>
+      </c>
+      <c r="B2587" s="27" t="s">
+        <v>2653</v>
+      </c>
+    </row>
+    <row r="2588" spans="1:3">
+      <c r="A2588">
+        <v>3677</v>
+      </c>
+      <c r="B2588" s="28" t="s">
+        <v>2654</v>
+      </c>
+    </row>
+    <row r="2589" spans="1:3">
+      <c r="A2589">
+        <v>3992</v>
+      </c>
+      <c r="B2589" s="28" t="s">
+        <v>2655</v>
+      </c>
+    </row>
+    <row r="2590" spans="1:3">
+      <c r="A2590">
+        <v>3996</v>
+      </c>
+      <c r="B2590" s="12" t="s">
+        <v>2656</v>
+      </c>
+      <c r="C2590" t="s">
+        <v>2704</v>
+      </c>
+    </row>
+    <row r="2591" spans="1:3">
+      <c r="A2591">
+        <v>4004</v>
+      </c>
+      <c r="B2591" s="12" t="s">
+        <v>2657</v>
+      </c>
+      <c r="C2591" t="s">
+        <v>2705</v>
+      </c>
+    </row>
+    <row r="2592" spans="1:3">
+      <c r="A2592">
+        <v>4030</v>
+      </c>
+      <c r="B2592" s="12" t="s">
+        <v>2658</v>
+      </c>
+      <c r="C2592" t="s">
+        <v>2706</v>
+      </c>
+    </row>
+    <row r="2593" spans="1:4">
+      <c r="A2593">
+        <v>4033</v>
+      </c>
+      <c r="B2593" s="16" t="s">
+        <v>2659</v>
+      </c>
+    </row>
+    <row r="2594" spans="1:4">
+      <c r="A2594">
+        <v>4034</v>
+      </c>
+      <c r="B2594" t="s">
+        <v>2660</v>
+      </c>
+    </row>
+    <row r="2595" spans="1:4">
+      <c r="A2595">
+        <v>4041</v>
+      </c>
+      <c r="B2595" s="28" t="s">
+        <v>2661</v>
+      </c>
+    </row>
+    <row r="2596" spans="1:4">
+      <c r="A2596">
+        <v>4383</v>
+      </c>
+      <c r="B2596" s="28" t="s">
+        <v>2662</v>
+      </c>
+      <c r="D2596" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2597" spans="1:4">
+      <c r="A2597">
+        <v>4404</v>
+      </c>
+      <c r="B2597" s="12" t="s">
+        <v>2663</v>
+      </c>
+      <c r="C2597" t="s">
+        <v>2705</v>
+      </c>
+    </row>
+    <row r="2598" spans="1:4">
+      <c r="A2598">
+        <v>4407</v>
+      </c>
+      <c r="B2598" s="16" t="s">
+        <v>2664</v>
+      </c>
+    </row>
+    <row r="2599" spans="1:4">
+      <c r="A2599">
+        <v>4840</v>
+      </c>
+      <c r="B2599" s="28" t="s">
+        <v>2665</v>
+      </c>
+    </row>
+    <row r="2600" spans="1:4">
+      <c r="A2600">
+        <v>4844</v>
+      </c>
+      <c r="B2600" s="12" t="s">
+        <v>2666</v>
+      </c>
+      <c r="C2600" t="s">
+        <v>2698</v>
+      </c>
+    </row>
+    <row r="2601" spans="1:4">
+      <c r="A2601">
+        <v>4849</v>
+      </c>
+      <c r="B2601" s="28" t="s">
+        <v>2667</v>
+      </c>
+      <c r="D2601" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2602" spans="1:4">
+      <c r="A2602">
+        <v>4870</v>
+      </c>
+      <c r="B2602" s="12" t="s">
+        <v>2668</v>
+      </c>
+      <c r="C2602" t="s">
+        <v>2700</v>
+      </c>
+    </row>
+    <row r="2603" spans="1:4">
+      <c r="A2603">
+        <v>4873</v>
+      </c>
+      <c r="B2603" s="16" t="s">
+        <v>2669</v>
+      </c>
+    </row>
+    <row r="2604" spans="1:4">
+      <c r="A2604">
+        <v>4874</v>
+      </c>
+      <c r="B2604" t="s">
+        <v>2670</v>
+      </c>
+    </row>
+    <row r="2605" spans="1:4">
+      <c r="A2605">
+        <v>4875</v>
+      </c>
+      <c r="B2605" s="27" t="s">
+        <v>2671</v>
+      </c>
+    </row>
+    <row r="2606" spans="1:4">
+      <c r="A2606">
+        <v>4876</v>
+      </c>
+      <c r="B2606" t="s">
+        <v>2672</v>
+      </c>
+    </row>
+    <row r="2607" spans="1:4">
+      <c r="A2607">
+        <v>4877</v>
+      </c>
+      <c r="B2607" s="27" t="s">
+        <v>2673</v>
+      </c>
+    </row>
+    <row r="2608" spans="1:4">
+      <c r="A2608">
+        <v>4883</v>
+      </c>
+      <c r="B2608" s="28" t="s">
+        <v>2674</v>
+      </c>
+    </row>
+    <row r="2609" spans="1:4">
+      <c r="A2609">
+        <v>5639</v>
+      </c>
+      <c r="B2609" s="28" t="s">
+        <v>2675</v>
+      </c>
+      <c r="D2609" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2610" spans="1:4">
+      <c r="A2610">
+        <v>5660</v>
+      </c>
+      <c r="B2610" s="12" t="s">
+        <v>2676</v>
+      </c>
+      <c r="C2610" t="s">
+        <v>2705</v>
+      </c>
+    </row>
+    <row r="2611" spans="1:4">
+      <c r="A2611">
+        <v>5663</v>
+      </c>
+      <c r="B2611" s="16" t="s">
+        <v>2677</v>
+      </c>
+    </row>
+    <row r="2612" spans="1:4">
+      <c r="A2612">
+        <v>5670</v>
+      </c>
+      <c r="B2612" s="28" t="s">
+        <v>2678</v>
+      </c>
+    </row>
+    <row r="2613" spans="1:4">
+      <c r="A2613">
+        <v>5673</v>
+      </c>
+      <c r="B2613" s="28" t="s">
+        <v>2679</v>
+      </c>
+    </row>
+    <row r="2614" spans="1:4">
+      <c r="A2614">
+        <v>5674</v>
+      </c>
+      <c r="B2614" s="12" t="s">
+        <v>2680</v>
+      </c>
+      <c r="C2614" t="s">
+        <v>2698</v>
+      </c>
+    </row>
+    <row r="2615" spans="1:4">
+      <c r="A2615">
+        <v>5690</v>
+      </c>
+      <c r="B2615" s="12" t="s">
+        <v>2681</v>
+      </c>
+      <c r="C2615" t="s">
+        <v>2699</v>
+      </c>
+    </row>
+    <row r="2616" spans="1:4">
+      <c r="A2616">
+        <v>5693</v>
+      </c>
+      <c r="B2616" s="16" t="s">
+        <v>2682</v>
+      </c>
+    </row>
+    <row r="2617" spans="1:4">
+      <c r="A2617">
+        <v>5699</v>
+      </c>
+      <c r="B2617" s="28" t="s">
+        <v>2683</v>
+      </c>
+    </row>
+    <row r="2618" spans="1:4">
+      <c r="A2618">
+        <v>5711</v>
+      </c>
+      <c r="B2618" s="16" t="s">
+        <v>2684</v>
+      </c>
+    </row>
+    <row r="2619" spans="1:4">
+      <c r="A2619">
+        <v>5715</v>
+      </c>
+      <c r="B2619" s="28" t="s">
+        <v>2685</v>
+      </c>
+    </row>
+    <row r="2620" spans="1:4">
+      <c r="A2620">
+        <v>6947</v>
+      </c>
+      <c r="B2620" s="28" t="s">
+        <v>2686</v>
+      </c>
+      <c r="D2620" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2621" spans="1:4">
+      <c r="A2621">
+        <v>6962</v>
+      </c>
+      <c r="B2621" s="12" t="s">
+        <v>2687</v>
+      </c>
+      <c r="C2621" t="s">
+        <v>2706</v>
+      </c>
+    </row>
+    <row r="2622" spans="1:4">
+      <c r="A2622">
+        <v>6965</v>
+      </c>
+      <c r="B2622" s="16" t="s">
+        <v>2688</v>
+      </c>
+    </row>
+    <row r="2623" spans="1:4">
+      <c r="A2623">
+        <v>7407</v>
+      </c>
+      <c r="B2623" s="28" t="s">
+        <v>2689</v>
+      </c>
+    </row>
+    <row r="2624" spans="1:4">
+      <c r="A2624">
+        <v>7411</v>
+      </c>
+      <c r="B2624" s="12" t="s">
+        <v>2690</v>
+      </c>
+      <c r="C2624" t="s">
+        <v>2698</v>
+      </c>
+    </row>
+    <row r="2625" spans="1:3">
+      <c r="A2625">
+        <v>7431</v>
+      </c>
+      <c r="B2625" s="12" t="s">
+        <v>2691</v>
+      </c>
+      <c r="C2625" t="s">
+        <v>2700</v>
+      </c>
+    </row>
+    <row r="2626" spans="1:3">
+      <c r="A2626">
+        <v>7434</v>
+      </c>
+      <c r="B2626" s="16" t="s">
+        <v>2692</v>
+      </c>
+    </row>
+    <row r="2627" spans="1:3">
+      <c r="A2627">
+        <v>7435</v>
+      </c>
+      <c r="B2627" t="s">
+        <v>2693</v>
+      </c>
+    </row>
+    <row r="2628" spans="1:3">
+      <c r="A2628">
+        <v>7436</v>
+      </c>
+      <c r="B2628" s="27" t="s">
+        <v>2694</v>
+      </c>
+    </row>
+    <row r="2629" spans="1:3">
+      <c r="A2629">
+        <v>7437</v>
+      </c>
+      <c r="B2629" t="s">
+        <v>2695</v>
+      </c>
+    </row>
+    <row r="2630" spans="1:3">
+      <c r="A2630">
+        <v>7443</v>
+      </c>
+      <c r="B2630" s="28" t="s">
+        <v>2696</v>
+      </c>
+    </row>
+    <row r="2631" spans="1:3">
+      <c r="A2631">
+        <v>10377</v>
+      </c>
+      <c r="B2631" s="28" t="s">
+        <v>2697</v>
+      </c>
+    </row>
+    <row r="2640" spans="1:3" ht="16" thickBot="1"/>
+    <row r="2641" spans="1:3" ht="17" thickTop="1" thickBot="1">
+      <c r="B2641" s="1" t="s">
+        <v>2710</v>
+      </c>
+    </row>
+    <row r="2642" spans="1:3" ht="16" thickTop="1"/>
+    <row r="2643" spans="1:3">
+      <c r="B2643" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="2644" spans="1:3">
+      <c r="B2644" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="2645" spans="1:3">
+      <c r="B2645" t="s">
+        <v>924</v>
+      </c>
+      <c r="C2645" t="s">
+        <v>2698</v>
+      </c>
+    </row>
+    <row r="2646" spans="1:3">
+      <c r="B2646" t="s">
+        <v>925</v>
+      </c>
+      <c r="C2646" t="s">
+        <v>2699</v>
+      </c>
+    </row>
+    <row r="2647" spans="1:3">
+      <c r="B2647" t="s">
+        <v>430</v>
+      </c>
+      <c r="C2647" t="s">
+        <v>2700</v>
+      </c>
+    </row>
+    <row r="2648" spans="1:3">
+      <c r="C2648" t="s">
+        <v>2701</v>
+      </c>
+    </row>
+    <row r="2649" spans="1:3">
+      <c r="A2649" t="s">
+        <v>2097</v>
+      </c>
+      <c r="B2649" t="s">
+        <v>617</v>
+      </c>
+      <c r="C2649" t="s">
+        <v>2702</v>
+      </c>
+    </row>
+    <row r="2650" spans="1:3">
+      <c r="A2650">
+        <v>14</v>
+      </c>
+      <c r="B2650" s="28" t="s">
+        <v>2587</v>
+      </c>
+      <c r="C2650" t="s">
+        <v>2703</v>
+      </c>
+    </row>
+    <row r="2651" spans="1:3">
+      <c r="A2651">
+        <v>17</v>
+      </c>
+      <c r="B2651" s="16" t="s">
         <v>2631</v>
       </c>
-    </row>
-    <row r="2578" spans="6:6">
-      <c r="F2578" t="s">
-        <v>2464</v>
-      </c>
-    </row>
-    <row r="2579" spans="6:6">
-      <c r="F2579" t="s">
-        <v>2620</v>
-      </c>
-    </row>
-    <row r="2580" spans="6:6">
-      <c r="F2580" t="s">
-        <v>2497</v>
-      </c>
-    </row>
-    <row r="2581" spans="6:6">
-      <c r="F2581" t="s">
-        <v>2621</v>
-      </c>
-    </row>
-    <row r="2582" spans="6:6">
-      <c r="F2582" t="s">
+      <c r="C2651" t="s">
+        <v>2704</v>
+      </c>
+    </row>
+    <row r="2652" spans="1:3">
+      <c r="A2652">
+        <v>18</v>
+      </c>
+      <c r="B2652" t="s">
         <v>2632</v>
       </c>
-    </row>
-    <row r="2583" spans="6:6">
-      <c r="F2583" t="s">
-        <v>2633</v>
-      </c>
-    </row>
-    <row r="2584" spans="6:6">
-      <c r="F2584" t="s">
-        <v>2456</v>
-      </c>
-    </row>
-    <row r="2585" spans="6:6">
-      <c r="F2585" t="s">
-        <v>2456</v>
-      </c>
-    </row>
-    <row r="2586" spans="6:6">
-      <c r="F2586" t="s">
-        <v>2634</v>
-      </c>
-    </row>
-    <row r="2587" spans="6:6">
-      <c r="F2587" t="s">
-        <v>2635</v>
-      </c>
-    </row>
-    <row r="2588" spans="6:6">
-      <c r="F2588" t="s">
-        <v>2636</v>
-      </c>
-    </row>
-    <row r="2589" spans="6:6">
-      <c r="F2589" t="s">
-        <v>2459</v>
-      </c>
-    </row>
-    <row r="2590" spans="6:6">
-      <c r="F2590" t="s">
-        <v>2620</v>
-      </c>
-    </row>
-    <row r="2591" spans="6:6">
-      <c r="F2591" t="s">
-        <v>2462</v>
-      </c>
-    </row>
-    <row r="2592" spans="6:6">
-      <c r="F2592" t="s">
-        <v>2621</v>
-      </c>
-    </row>
-    <row r="2593" spans="6:6">
-      <c r="F2593" t="s">
-        <v>2637</v>
-      </c>
-    </row>
-    <row r="2594" spans="6:6">
-      <c r="F2594" t="s">
-        <v>2464</v>
-      </c>
-    </row>
-    <row r="2595" spans="6:6">
-      <c r="F2595" t="s">
-        <v>2623</v>
-      </c>
-    </row>
-    <row r="2596" spans="6:6">
-      <c r="F2596" t="s">
-        <v>2462</v>
-      </c>
-    </row>
-    <row r="2597" spans="6:6">
-      <c r="F2597" t="s">
-        <v>2621</v>
-      </c>
-    </row>
-    <row r="2598" spans="6:6">
-      <c r="F2598" t="s">
-        <v>2638</v>
-      </c>
-    </row>
-    <row r="2599" spans="6:6">
-      <c r="F2599" t="s">
-        <v>2464</v>
-      </c>
-    </row>
-    <row r="2600" spans="6:6">
-      <c r="F2600" t="s">
-        <v>2620</v>
-      </c>
-    </row>
-    <row r="2601" spans="6:6">
-      <c r="F2601" t="s">
-        <v>2497</v>
-      </c>
-    </row>
-    <row r="2602" spans="6:6">
-      <c r="F2602" t="s">
-        <v>2621</v>
-      </c>
-    </row>
-    <row r="2603" spans="6:6">
-      <c r="F2603" t="s">
-        <v>2639</v>
-      </c>
-    </row>
-    <row r="2604" spans="6:6">
-      <c r="F2604" t="s">
-        <v>2640</v>
-      </c>
-    </row>
-    <row r="2605" spans="6:6">
-      <c r="F2605" t="s">
-        <v>2456</v>
-      </c>
-    </row>
-    <row r="2606" spans="6:6">
-      <c r="F2606" t="s">
-        <v>2456</v>
-      </c>
-    </row>
-    <row r="2607" spans="6:6">
-      <c r="F2607" t="s">
-        <v>2641</v>
-      </c>
-    </row>
-    <row r="2608" spans="6:6">
-      <c r="F2608" t="s">
-        <v>2642</v>
-      </c>
-    </row>
-    <row r="2609" spans="6:6">
-      <c r="F2609" t="s">
-        <v>2643</v>
-      </c>
-    </row>
-    <row r="2610" spans="6:6">
-      <c r="F2610" t="s">
-        <v>2459</v>
-      </c>
-    </row>
-    <row r="2611" spans="6:6">
-      <c r="F2611" t="s">
-        <v>2620</v>
-      </c>
-    </row>
-    <row r="2612" spans="6:6">
-      <c r="F2612" t="s">
-        <v>2462</v>
-      </c>
-    </row>
-    <row r="2613" spans="6:6">
-      <c r="F2613" t="s">
-        <v>2621</v>
-      </c>
-    </row>
-    <row r="2614" spans="6:6">
-      <c r="F2614" t="s">
-        <v>2644</v>
-      </c>
-    </row>
-    <row r="2615" spans="6:6">
-      <c r="F2615" t="s">
-        <v>2464</v>
-      </c>
-    </row>
-    <row r="2616" spans="6:6">
-      <c r="F2616" t="s">
-        <v>2623</v>
-      </c>
-    </row>
-    <row r="2617" spans="6:6">
-      <c r="F2617" t="s">
-        <v>2462</v>
-      </c>
-    </row>
-    <row r="2618" spans="6:6">
-      <c r="F2618" t="s">
-        <v>2621</v>
-      </c>
-    </row>
-    <row r="2619" spans="6:6">
-      <c r="F2619" t="s">
-        <v>2645</v>
-      </c>
-    </row>
-    <row r="2620" spans="6:6">
-      <c r="F2620" t="s">
-        <v>2464</v>
-      </c>
-    </row>
-    <row r="2621" spans="6:6">
-      <c r="F2621" t="s">
-        <v>2620</v>
-      </c>
-    </row>
-    <row r="2622" spans="6:6">
-      <c r="F2622" t="s">
-        <v>2497</v>
-      </c>
-    </row>
-    <row r="2623" spans="6:6">
-      <c r="F2623" t="s">
-        <v>2621</v>
-      </c>
-    </row>
-    <row r="2624" spans="6:6">
-      <c r="F2624" t="s">
-        <v>2646</v>
-      </c>
-    </row>
-    <row r="2625" spans="6:6">
-      <c r="F2625" t="s">
-        <v>2647</v>
-      </c>
-    </row>
-    <row r="2626" spans="6:6">
-      <c r="F2626" t="s">
-        <v>2456</v>
-      </c>
-    </row>
-    <row r="2627" spans="6:6">
-      <c r="F2627" t="s">
-        <v>2456</v>
-      </c>
-    </row>
-    <row r="2628" spans="6:6">
-      <c r="F2628" t="s">
-        <v>2648</v>
-      </c>
-    </row>
-    <row r="2629" spans="6:6">
-      <c r="F2629" t="s">
-        <v>2649</v>
-      </c>
-    </row>
-    <row r="2630" spans="6:6">
-      <c r="F2630" t="s">
-        <v>2650</v>
-      </c>
-    </row>
-    <row r="2631" spans="6:6">
-      <c r="F2631" t="s">
-        <v>2459</v>
-      </c>
-    </row>
-    <row r="2632" spans="6:6">
-      <c r="F2632" t="s">
-        <v>2620</v>
-      </c>
-    </row>
-    <row r="2633" spans="6:6">
-      <c r="F2633" t="s">
-        <v>2462</v>
-      </c>
-    </row>
-    <row r="2634" spans="6:6">
-      <c r="F2634" t="s">
-        <v>2621</v>
-      </c>
-    </row>
-    <row r="2635" spans="6:6">
-      <c r="F2635" t="s">
-        <v>2651</v>
-      </c>
-    </row>
-    <row r="2636" spans="6:6">
-      <c r="F2636" t="s">
-        <v>2464</v>
-      </c>
-    </row>
-    <row r="2637" spans="6:6">
-      <c r="F2637" t="s">
-        <v>2623</v>
-      </c>
-    </row>
-    <row r="2638" spans="6:6">
-      <c r="F2638" t="s">
-        <v>2462</v>
-      </c>
-    </row>
-    <row r="2639" spans="6:6">
-      <c r="F2639" t="s">
-        <v>2621</v>
-      </c>
-    </row>
-    <row r="2640" spans="6:6">
-      <c r="F2640" t="s">
-        <v>2652</v>
-      </c>
-    </row>
-    <row r="2641" spans="6:6">
-      <c r="F2641" t="s">
-        <v>2464</v>
-      </c>
-    </row>
-    <row r="2642" spans="6:6">
-      <c r="F2642" t="s">
-        <v>2620</v>
-      </c>
-    </row>
-    <row r="2643" spans="6:6">
-      <c r="F2643" t="s">
-        <v>2497</v>
-      </c>
-    </row>
-    <row r="2644" spans="6:6">
-      <c r="F2644" t="s">
-        <v>2621</v>
-      </c>
-    </row>
-    <row r="2645" spans="6:6">
-      <c r="F2645" t="s">
-        <v>2653</v>
-      </c>
-    </row>
-    <row r="2646" spans="6:6">
-      <c r="F2646" t="s">
-        <v>2654</v>
-      </c>
-    </row>
-    <row r="2647" spans="6:6">
-      <c r="F2647" t="s">
-        <v>2456</v>
-      </c>
-    </row>
-    <row r="2648" spans="6:6">
-      <c r="F2648" t="s">
-        <v>2456</v>
-      </c>
-    </row>
-    <row r="2649" spans="6:6">
-      <c r="F2649" t="s">
-        <v>2655</v>
-      </c>
-    </row>
-    <row r="2650" spans="6:6">
-      <c r="F2650" t="s">
-        <v>2656</v>
-      </c>
-    </row>
-    <row r="2651" spans="6:6">
-      <c r="F2651" t="s">
-        <v>2657</v>
-      </c>
-    </row>
-    <row r="2652" spans="6:6">
-      <c r="F2652" t="s">
-        <v>2459</v>
-      </c>
-    </row>
-    <row r="2653" spans="6:6">
-      <c r="F2653" t="s">
-        <v>2620</v>
-      </c>
-    </row>
-    <row r="2654" spans="6:6">
-      <c r="F2654" t="s">
-        <v>2462</v>
-      </c>
-    </row>
-    <row r="2655" spans="6:6">
-      <c r="F2655" t="s">
-        <v>2621</v>
-      </c>
-    </row>
-    <row r="2656" spans="6:6">
-      <c r="F2656" t="s">
-        <v>2658</v>
-      </c>
-    </row>
-    <row r="2657" spans="6:6">
-      <c r="F2657" t="s">
-        <v>2464</v>
-      </c>
-    </row>
-    <row r="2658" spans="6:6">
-      <c r="F2658" t="s">
-        <v>2623</v>
-      </c>
-    </row>
-    <row r="2659" spans="6:6">
-      <c r="F2659" t="s">
-        <v>2462</v>
-      </c>
-    </row>
-    <row r="2660" spans="6:6">
-      <c r="F2660" t="s">
-        <v>2621</v>
-      </c>
-    </row>
-    <row r="2661" spans="6:6">
-      <c r="F2661" t="s">
-        <v>2659</v>
-      </c>
-    </row>
-    <row r="2662" spans="6:6">
-      <c r="F2662" t="s">
-        <v>2464</v>
-      </c>
-    </row>
-    <row r="2663" spans="6:6">
-      <c r="F2663" t="s">
-        <v>2620</v>
-      </c>
-    </row>
-    <row r="2664" spans="6:6">
-      <c r="F2664" t="s">
-        <v>2497</v>
-      </c>
-    </row>
-    <row r="2665" spans="6:6">
-      <c r="F2665" t="s">
-        <v>2621</v>
-      </c>
-    </row>
-    <row r="2666" spans="6:6">
-      <c r="F2666" t="s">
-        <v>2660</v>
-      </c>
-    </row>
-    <row r="2667" spans="6:6">
-      <c r="F2667" t="s">
-        <v>2661</v>
-      </c>
-    </row>
-    <row r="2668" spans="6:6">
-      <c r="F2668" t="s">
-        <v>2456</v>
-      </c>
-    </row>
-    <row r="2669" spans="6:6">
-      <c r="F2669" t="s">
-        <v>2456</v>
-      </c>
-    </row>
-    <row r="2670" spans="6:6">
-      <c r="F2670" t="s">
-        <v>2662</v>
-      </c>
-    </row>
-    <row r="2671" spans="6:6">
-      <c r="F2671" t="s">
-        <v>2663</v>
-      </c>
-    </row>
-    <row r="2672" spans="6:6">
-      <c r="F2672" t="s">
-        <v>2664</v>
-      </c>
-    </row>
-    <row r="2673" spans="6:6">
-      <c r="F2673" t="s">
-        <v>2459</v>
-      </c>
-    </row>
-    <row r="2674" spans="6:6">
-      <c r="F2674" t="s">
-        <v>2620</v>
-      </c>
-    </row>
-    <row r="2675" spans="6:6">
-      <c r="F2675" t="s">
-        <v>2462</v>
-      </c>
-    </row>
-    <row r="2676" spans="6:6">
-      <c r="F2676" t="s">
-        <v>2621</v>
-      </c>
-    </row>
-    <row r="2677" spans="6:6">
-      <c r="F2677" t="s">
-        <v>2665</v>
-      </c>
-    </row>
-    <row r="2678" spans="6:6">
-      <c r="F2678" t="s">
-        <v>2464</v>
-      </c>
-    </row>
-    <row r="2679" spans="6:6">
-      <c r="F2679" t="s">
-        <v>2623</v>
-      </c>
-    </row>
-    <row r="2680" spans="6:6">
-      <c r="F2680" t="s">
-        <v>2462</v>
-      </c>
-    </row>
-    <row r="2681" spans="6:6">
-      <c r="F2681" t="s">
-        <v>2621</v>
-      </c>
-    </row>
-    <row r="2682" spans="6:6">
-      <c r="F2682" t="s">
-        <v>2666</v>
-      </c>
-    </row>
-    <row r="2683" spans="6:6">
-      <c r="F2683" t="s">
-        <v>2464</v>
-      </c>
-    </row>
-    <row r="2684" spans="6:6">
-      <c r="F2684" t="s">
-        <v>2620</v>
-      </c>
-    </row>
-    <row r="2685" spans="6:6">
-      <c r="F2685" t="s">
-        <v>2497</v>
-      </c>
-    </row>
-    <row r="2686" spans="6:6">
-      <c r="F2686" t="s">
-        <v>2621</v>
-      </c>
-    </row>
-    <row r="2687" spans="6:6">
-      <c r="F2687" t="s">
-        <v>2667</v>
-      </c>
-    </row>
-    <row r="2688" spans="6:6">
-      <c r="F2688" t="s">
-        <v>2668</v>
-      </c>
-    </row>
-    <row r="2689" spans="6:6">
-      <c r="F2689" t="s">
-        <v>2456</v>
-      </c>
-    </row>
-    <row r="2690" spans="6:6">
-      <c r="F2690" t="s">
-        <v>2456</v>
-      </c>
-    </row>
-    <row r="2691" spans="6:6">
-      <c r="F2691" t="s">
-        <v>2669</v>
-      </c>
-    </row>
-    <row r="2692" spans="6:6">
-      <c r="F2692" t="s">
-        <v>2670</v>
-      </c>
-    </row>
-    <row r="2693" spans="6:6">
-      <c r="F2693" t="s">
-        <v>2671</v>
-      </c>
-    </row>
-    <row r="2694" spans="6:6">
-      <c r="F2694" t="s">
-        <v>2459</v>
-      </c>
-    </row>
-    <row r="2695" spans="6:6">
-      <c r="F2695" t="s">
-        <v>2620</v>
-      </c>
-    </row>
-    <row r="2696" spans="6:6">
-      <c r="F2696" t="s">
-        <v>2462</v>
-      </c>
-    </row>
-    <row r="2697" spans="6:6">
-      <c r="F2697" t="s">
-        <v>2621</v>
-      </c>
-    </row>
-    <row r="2698" spans="6:6">
-      <c r="F2698" t="s">
-        <v>2672</v>
-      </c>
-    </row>
-    <row r="2699" spans="6:6">
-      <c r="F2699" t="s">
-        <v>2464</v>
-      </c>
-    </row>
-    <row r="2700" spans="6:6">
-      <c r="F2700" t="s">
-        <v>2623</v>
-      </c>
-    </row>
-    <row r="2701" spans="6:6">
-      <c r="F2701" t="s">
-        <v>2462</v>
-      </c>
-    </row>
-    <row r="2702" spans="6:6">
-      <c r="F2702" t="s">
-        <v>2621</v>
-      </c>
-    </row>
-    <row r="2703" spans="6:6">
-      <c r="F2703" t="s">
-        <v>2673</v>
-      </c>
-    </row>
-    <row r="2704" spans="6:6">
-      <c r="F2704" t="s">
-        <v>2464</v>
-      </c>
-    </row>
-    <row r="2705" spans="6:6">
-      <c r="F2705" t="s">
-        <v>2620</v>
-      </c>
-    </row>
-    <row r="2706" spans="6:6">
-      <c r="F2706" t="s">
-        <v>2497</v>
-      </c>
-    </row>
-    <row r="2707" spans="6:6">
-      <c r="F2707" t="s">
-        <v>2621</v>
-      </c>
-    </row>
-    <row r="2708" spans="6:6">
-      <c r="F2708" t="s">
-        <v>2674</v>
-      </c>
-    </row>
-    <row r="2709" spans="6:6">
-      <c r="F2709" t="s">
-        <v>2675</v>
-      </c>
-    </row>
-    <row r="2710" spans="6:6">
-      <c r="F2710" t="s">
-        <v>2456</v>
-      </c>
-    </row>
-    <row r="2711" spans="6:6">
-      <c r="F2711" t="s">
-        <v>2456</v>
-      </c>
-    </row>
-    <row r="2712" spans="6:6">
-      <c r="F2712" t="s">
-        <v>2676</v>
-      </c>
-    </row>
-    <row r="2713" spans="6:6">
-      <c r="F2713" t="s">
-        <v>2677</v>
-      </c>
-    </row>
-    <row r="2714" spans="6:6">
-      <c r="F2714" t="s">
-        <v>2678</v>
-      </c>
-    </row>
-    <row r="2715" spans="6:6">
-      <c r="F2715" t="s">
-        <v>2459</v>
-      </c>
-    </row>
-    <row r="2716" spans="6:6">
-      <c r="F2716" t="s">
-        <v>2620</v>
-      </c>
-    </row>
-    <row r="2717" spans="6:6">
-      <c r="F2717" t="s">
-        <v>2462</v>
-      </c>
-    </row>
-    <row r="2718" spans="6:6">
-      <c r="F2718" t="s">
-        <v>2621</v>
-      </c>
-    </row>
-    <row r="2719" spans="6:6">
-      <c r="F2719" t="s">
-        <v>2679</v>
-      </c>
-    </row>
-    <row r="2720" spans="6:6">
-      <c r="F2720" t="s">
-        <v>2464</v>
-      </c>
-    </row>
-    <row r="2721" spans="6:6">
-      <c r="F2721" t="s">
-        <v>2623</v>
-      </c>
-    </row>
-    <row r="2722" spans="6:6">
-      <c r="F2722" t="s">
-        <v>2462</v>
-      </c>
-    </row>
-    <row r="2723" spans="6:6">
-      <c r="F2723" t="s">
-        <v>2621</v>
-      </c>
-    </row>
-    <row r="2724" spans="6:6">
-      <c r="F2724" t="s">
-        <v>2680</v>
-      </c>
-    </row>
-    <row r="2725" spans="6:6">
-      <c r="F2725" t="s">
-        <v>2464</v>
-      </c>
-    </row>
-    <row r="2726" spans="6:6">
-      <c r="F2726" t="s">
-        <v>2620</v>
-      </c>
-    </row>
-    <row r="2727" spans="6:6">
-      <c r="F2727" t="s">
-        <v>2497</v>
-      </c>
-    </row>
-    <row r="2728" spans="6:6">
-      <c r="F2728" t="s">
-        <v>2621</v>
-      </c>
-    </row>
-    <row r="2729" spans="6:6">
-      <c r="F2729" t="s">
-        <v>2681</v>
-      </c>
-    </row>
-    <row r="2730" spans="6:6">
-      <c r="F2730" t="s">
-        <v>2682</v>
-      </c>
-    </row>
-    <row r="2731" spans="6:6">
-      <c r="F2731" t="s">
-        <v>2456</v>
-      </c>
-    </row>
-    <row r="2732" spans="6:6">
-      <c r="F2732" t="s">
-        <v>2456</v>
-      </c>
-    </row>
-    <row r="2733" spans="6:6">
-      <c r="F2733" t="s">
-        <v>2683</v>
-      </c>
-    </row>
-    <row r="2734" spans="6:6">
-      <c r="F2734" t="s">
-        <v>2684</v>
-      </c>
-    </row>
-    <row r="2735" spans="6:6">
-      <c r="F2735" t="s">
-        <v>2685</v>
-      </c>
-    </row>
-    <row r="2736" spans="6:6">
-      <c r="F2736" t="s">
-        <v>2459</v>
-      </c>
-    </row>
-    <row r="2737" spans="6:6">
-      <c r="F2737" t="s">
-        <v>2620</v>
-      </c>
-    </row>
-    <row r="2738" spans="6:6">
-      <c r="F2738" t="s">
-        <v>2462</v>
-      </c>
-    </row>
-    <row r="2739" spans="6:6">
-      <c r="F2739" t="s">
-        <v>2621</v>
-      </c>
-    </row>
-    <row r="2740" spans="6:6">
-      <c r="F2740" t="s">
-        <v>2686</v>
-      </c>
-    </row>
-    <row r="2741" spans="6:6">
-      <c r="F2741" t="s">
-        <v>2464</v>
-      </c>
-    </row>
-    <row r="2742" spans="6:6">
-      <c r="F2742" t="s">
-        <v>2623</v>
-      </c>
-    </row>
-    <row r="2743" spans="6:6">
-      <c r="F2743" t="s">
-        <v>2462</v>
-      </c>
-    </row>
-    <row r="2744" spans="6:6">
-      <c r="F2744" t="s">
-        <v>2621</v>
-      </c>
-    </row>
-    <row r="2745" spans="6:6">
-      <c r="F2745" t="s">
-        <v>2687</v>
-      </c>
-    </row>
-    <row r="2746" spans="6:6">
-      <c r="F2746" t="s">
-        <v>2464</v>
-      </c>
-    </row>
-    <row r="2747" spans="6:6">
-      <c r="F2747" t="s">
-        <v>2620</v>
-      </c>
-    </row>
-    <row r="2748" spans="6:6">
-      <c r="F2748" t="s">
-        <v>2497</v>
-      </c>
-    </row>
-    <row r="2749" spans="6:6">
-      <c r="F2749" t="s">
-        <v>2621</v>
-      </c>
-    </row>
-    <row r="2750" spans="6:6">
-      <c r="F2750" t="s">
-        <v>2688</v>
-      </c>
-    </row>
-    <row r="2751" spans="6:6">
-      <c r="F2751" t="s">
-        <v>2689</v>
-      </c>
-    </row>
-    <row r="2752" spans="6:6">
-      <c r="F2752" t="s">
-        <v>2456</v>
-      </c>
-    </row>
-    <row r="2753" spans="6:6">
-      <c r="F2753" t="s">
-        <v>2456</v>
-      </c>
-    </row>
-    <row r="2754" spans="6:6">
-      <c r="F2754" t="s">
-        <v>2690</v>
-      </c>
-    </row>
-    <row r="2755" spans="6:6">
-      <c r="F2755" t="s">
-        <v>2691</v>
-      </c>
-    </row>
-    <row r="2756" spans="6:6">
-      <c r="F2756" t="s">
-        <v>2692</v>
-      </c>
-    </row>
-    <row r="2757" spans="6:6">
-      <c r="F2757" t="s">
-        <v>2459</v>
-      </c>
-    </row>
-    <row r="2758" spans="6:6">
-      <c r="F2758" t="s">
-        <v>2620</v>
-      </c>
-    </row>
-    <row r="2759" spans="6:6">
-      <c r="F2759" t="s">
-        <v>2462</v>
-      </c>
-    </row>
-    <row r="2760" spans="6:6">
-      <c r="F2760" t="s">
-        <v>2621</v>
-      </c>
-    </row>
-    <row r="2761" spans="6:6">
-      <c r="F2761" t="s">
-        <v>2693</v>
-      </c>
-    </row>
-    <row r="2762" spans="6:6">
-      <c r="F2762" t="s">
-        <v>2464</v>
-      </c>
-    </row>
-    <row r="2763" spans="6:6">
-      <c r="F2763" t="s">
-        <v>2623</v>
-      </c>
-    </row>
-    <row r="2764" spans="6:6">
-      <c r="F2764" t="s">
-        <v>2462</v>
-      </c>
-    </row>
-    <row r="2765" spans="6:6">
-      <c r="F2765" t="s">
-        <v>2621</v>
-      </c>
-    </row>
-    <row r="2766" spans="6:6">
-      <c r="F2766" t="s">
-        <v>2694</v>
-      </c>
-    </row>
-    <row r="2767" spans="6:6">
-      <c r="F2767" t="s">
-        <v>2464</v>
-      </c>
-    </row>
-    <row r="2768" spans="6:6">
-      <c r="F2768" t="s">
-        <v>2620</v>
-      </c>
-    </row>
-    <row r="2769" spans="6:6">
-      <c r="F2769" t="s">
-        <v>2497</v>
-      </c>
-    </row>
-    <row r="2770" spans="6:6">
-      <c r="F2770" t="s">
-        <v>2621</v>
-      </c>
-    </row>
-    <row r="2771" spans="6:6">
-      <c r="F2771" t="s">
-        <v>2695</v>
-      </c>
-    </row>
-    <row r="2772" spans="6:6">
-      <c r="F2772" t="s">
-        <v>2696</v>
-      </c>
-    </row>
-    <row r="2773" spans="6:6">
-      <c r="F2773" t="s">
-        <v>2456</v>
-      </c>
-    </row>
-    <row r="2774" spans="6:6">
-      <c r="F2774" t="s">
-        <v>2456</v>
-      </c>
-    </row>
-    <row r="2775" spans="6:6">
-      <c r="F2775" t="s">
-        <v>2697</v>
-      </c>
-    </row>
-    <row r="2776" spans="6:6">
-      <c r="F2776" t="s">
-        <v>2698</v>
-      </c>
-    </row>
-    <row r="2777" spans="6:6">
-      <c r="F2777" t="s">
+      <c r="C2652" t="s">
+        <v>2705</v>
+      </c>
+    </row>
+    <row r="2653" spans="1:3">
+      <c r="A2653">
+        <v>36</v>
+      </c>
+      <c r="B2653" s="28" t="s">
+        <v>2590</v>
+      </c>
+      <c r="C2653" t="s">
+        <v>2751</v>
+      </c>
+    </row>
+    <row r="2654" spans="1:3">
+      <c r="A2654">
+        <v>452</v>
+      </c>
+      <c r="B2654" s="28" t="s">
+        <v>2591</v>
+      </c>
+    </row>
+    <row r="2655" spans="1:3">
+      <c r="A2655">
+        <v>463</v>
+      </c>
+      <c r="B2655" s="12" t="s">
+        <v>2592</v>
+      </c>
+    </row>
+    <row r="2656" spans="1:3">
+      <c r="A2656">
+        <v>495</v>
+      </c>
+      <c r="B2656" s="12" t="s">
+        <v>2711</v>
+      </c>
+      <c r="C2656" t="s">
+        <v>2700</v>
+      </c>
+    </row>
+    <row r="2657" spans="1:3">
+      <c r="A2657">
+        <v>498</v>
+      </c>
+      <c r="B2657" s="16" t="s">
+        <v>2712</v>
+      </c>
+    </row>
+    <row r="2658" spans="1:3">
+      <c r="A2658">
+        <v>499</v>
+      </c>
+      <c r="B2658" t="s">
+        <v>2713</v>
+      </c>
+    </row>
+    <row r="2659" spans="1:3">
+      <c r="A2659">
+        <v>500</v>
+      </c>
+      <c r="B2659" t="s">
+        <v>2714</v>
+      </c>
+    </row>
+    <row r="2660" spans="1:3">
+      <c r="A2660">
+        <v>501</v>
+      </c>
+      <c r="B2660" t="s">
+        <v>2715</v>
+      </c>
+    </row>
+    <row r="2661" spans="1:3">
+      <c r="A2661">
+        <v>502</v>
+      </c>
+      <c r="B2661" t="s">
+        <v>2716</v>
+      </c>
+    </row>
+    <row r="2662" spans="1:3">
+      <c r="A2662">
+        <v>514</v>
+      </c>
+      <c r="B2662" s="28" t="s">
+        <v>2717</v>
+      </c>
+    </row>
+    <row r="2663" spans="1:3">
+      <c r="A2663">
+        <v>2890</v>
+      </c>
+      <c r="B2663" s="28" t="s">
+        <v>2718</v>
+      </c>
+    </row>
+    <row r="2664" spans="1:3">
+      <c r="A2664">
+        <v>2911</v>
+      </c>
+      <c r="B2664" s="12" t="s">
+        <v>2719</v>
+      </c>
+      <c r="C2664" t="s">
+        <v>2705</v>
+      </c>
+    </row>
+    <row r="2665" spans="1:3">
+      <c r="A2665">
+        <v>2914</v>
+      </c>
+      <c r="B2665" s="16" t="s">
+        <v>2720</v>
+      </c>
+    </row>
+    <row r="2666" spans="1:3">
+      <c r="A2666">
+        <v>3320</v>
+      </c>
+      <c r="B2666" s="28" t="s">
+        <v>2721</v>
+      </c>
+    </row>
+    <row r="2667" spans="1:3">
+      <c r="A2667">
+        <v>3353</v>
+      </c>
+      <c r="B2667" s="28" t="s">
+        <v>2722</v>
+      </c>
+    </row>
+    <row r="2668" spans="1:3">
+      <c r="A2668">
+        <v>3364</v>
+      </c>
+      <c r="B2668" s="12" t="s">
+        <v>2723</v>
+      </c>
+    </row>
+    <row r="2669" spans="1:3">
+      <c r="A2669">
+        <v>3390</v>
+      </c>
+      <c r="B2669" s="12" t="s">
+        <v>2724</v>
+      </c>
+      <c r="C2669" t="s">
+        <v>2700</v>
+      </c>
+    </row>
+    <row r="2670" spans="1:3">
+      <c r="A2670">
+        <v>3393</v>
+      </c>
+      <c r="B2670" s="16" t="s">
+        <v>2725</v>
+      </c>
+    </row>
+    <row r="2671" spans="1:3">
+      <c r="A2671">
+        <v>3394</v>
+      </c>
+      <c r="B2671" t="s">
+        <v>2726</v>
+      </c>
+    </row>
+    <row r="2672" spans="1:3">
+      <c r="A2672">
+        <v>3395</v>
+      </c>
+      <c r="B2672" t="s">
+        <v>2727</v>
+      </c>
+    </row>
+    <row r="2673" spans="1:3">
+      <c r="A2673">
+        <v>3396</v>
+      </c>
+      <c r="B2673" t="s">
+        <v>2728</v>
+      </c>
+    </row>
+    <row r="2674" spans="1:3">
+      <c r="A2674">
+        <v>3402</v>
+      </c>
+      <c r="B2674" s="28" t="s">
+        <v>2729</v>
+      </c>
+    </row>
+    <row r="2675" spans="1:3">
+      <c r="A2675">
+        <v>3600</v>
+      </c>
+      <c r="B2675" s="28" t="s">
+        <v>2730</v>
+      </c>
+    </row>
+    <row r="2676" spans="1:3">
+      <c r="A2676">
+        <v>3621</v>
+      </c>
+      <c r="B2676" s="12" t="s">
+        <v>2731</v>
+      </c>
+      <c r="C2676" t="s">
+        <v>2705</v>
+      </c>
+    </row>
+    <row r="2677" spans="1:3">
+      <c r="A2677">
+        <v>3624</v>
+      </c>
+      <c r="B2677" s="16" t="s">
+        <v>2732</v>
+      </c>
+    </row>
+    <row r="2678" spans="1:3">
+      <c r="A2678">
+        <v>3631</v>
+      </c>
+      <c r="B2678" s="28" t="s">
+        <v>2733</v>
+      </c>
+    </row>
+    <row r="2679" spans="1:3">
+      <c r="A2679">
+        <v>3634</v>
+      </c>
+      <c r="B2679" s="28" t="s">
+        <v>2734</v>
+      </c>
+    </row>
+    <row r="2680" spans="1:3">
+      <c r="A2680">
+        <v>3635</v>
+      </c>
+      <c r="B2680" s="12" t="s">
+        <v>2735</v>
+      </c>
+    </row>
+    <row r="2681" spans="1:3">
+      <c r="A2681">
+        <v>3657</v>
+      </c>
+      <c r="B2681" s="12" t="s">
+        <v>2736</v>
+      </c>
+      <c r="C2681" t="s">
         <v>2699</v>
       </c>
     </row>
-    <row r="2778" spans="6:6">
-      <c r="F2778" t="s">
-        <v>2459</v>
-      </c>
-    </row>
-    <row r="2779" spans="6:6">
-      <c r="F2779" t="s">
-        <v>2620</v>
-      </c>
-    </row>
-    <row r="2780" spans="6:6">
-      <c r="F2780" t="s">
-        <v>2462</v>
-      </c>
-    </row>
-    <row r="2781" spans="6:6">
-      <c r="F2781" t="s">
-        <v>2621</v>
-      </c>
-    </row>
-    <row r="2782" spans="6:6">
-      <c r="F2782" t="s">
+    <row r="2682" spans="1:3">
+      <c r="A2682">
+        <v>3660</v>
+      </c>
+      <c r="B2682" s="16" t="s">
+        <v>2737</v>
+      </c>
+    </row>
+    <row r="2683" spans="1:3">
+      <c r="A2683">
+        <v>3666</v>
+      </c>
+      <c r="B2683" s="28" t="s">
+        <v>2738</v>
+      </c>
+    </row>
+    <row r="2684" spans="1:3">
+      <c r="A2684">
+        <v>3678</v>
+      </c>
+      <c r="B2684" s="16" t="s">
+        <v>2739</v>
+      </c>
+    </row>
+    <row r="2685" spans="1:3">
+      <c r="A2685">
+        <v>3694</v>
+      </c>
+      <c r="B2685" s="16" t="s">
+        <v>2740</v>
+      </c>
+    </row>
+    <row r="2686" spans="1:3">
+      <c r="A2686">
+        <v>3698</v>
+      </c>
+      <c r="B2686" s="28" t="s">
+        <v>2741</v>
+      </c>
+    </row>
+    <row r="2687" spans="1:3">
+      <c r="A2687">
+        <v>3719</v>
+      </c>
+      <c r="B2687" s="12" t="s">
+        <v>2742</v>
+      </c>
+      <c r="C2687" t="s">
+        <v>2751</v>
+      </c>
+    </row>
+    <row r="2688" spans="1:3">
+      <c r="A2688">
+        <v>3722</v>
+      </c>
+      <c r="B2688" s="16" t="s">
+        <v>2743</v>
+      </c>
+    </row>
+    <row r="2689" spans="1:3">
+      <c r="A2689">
+        <v>4164</v>
+      </c>
+      <c r="B2689" s="28" t="s">
+        <v>2744</v>
+      </c>
+    </row>
+    <row r="2690" spans="1:3">
+      <c r="A2690">
+        <v>4168</v>
+      </c>
+      <c r="B2690" s="12" t="s">
+        <v>2745</v>
+      </c>
+    </row>
+    <row r="2691" spans="1:3">
+      <c r="A2691">
+        <v>4188</v>
+      </c>
+      <c r="B2691" s="12" t="s">
+        <v>2746</v>
+      </c>
+      <c r="C2691" t="s">
         <v>2700</v>
       </c>
     </row>
-    <row r="2783" spans="6:6">
-      <c r="F2783" t="s">
-        <v>2464</v>
-      </c>
-    </row>
-    <row r="2784" spans="6:6">
-      <c r="F2784" t="s">
-        <v>2623</v>
-      </c>
-    </row>
-    <row r="2785" spans="6:6">
-      <c r="F2785" t="s">
-        <v>2462</v>
-      </c>
-    </row>
-    <row r="2786" spans="6:6">
-      <c r="F2786" t="s">
-        <v>2621</v>
-      </c>
-    </row>
-    <row r="2787" spans="6:6">
-      <c r="F2787" t="s">
-        <v>2701</v>
-      </c>
-    </row>
-    <row r="2788" spans="6:6">
-      <c r="F2788" t="s">
-        <v>2464</v>
-      </c>
-    </row>
-    <row r="2789" spans="6:6">
-      <c r="F2789" t="s">
-        <v>2620</v>
-      </c>
-    </row>
-    <row r="2790" spans="6:6">
-      <c r="F2790" t="s">
-        <v>2497</v>
-      </c>
-    </row>
-    <row r="2791" spans="6:6">
-      <c r="F2791" t="s">
-        <v>2621</v>
-      </c>
-    </row>
-    <row r="2792" spans="6:6">
-      <c r="F2792" t="s">
-        <v>2702</v>
-      </c>
-    </row>
-    <row r="2793" spans="6:6">
-      <c r="F2793" t="s">
-        <v>2703</v>
-      </c>
-    </row>
-    <row r="2794" spans="6:6">
-      <c r="F2794" t="s">
-        <v>2456</v>
-      </c>
-    </row>
-    <row r="2795" spans="6:6">
-      <c r="F2795" t="s">
-        <v>2456</v>
-      </c>
-    </row>
-    <row r="2796" spans="6:6">
-      <c r="F2796" t="s">
-        <v>2704</v>
-      </c>
-    </row>
-    <row r="2797" spans="6:6">
-      <c r="F2797" t="s">
-        <v>2705</v>
-      </c>
-    </row>
-    <row r="2798" spans="6:6">
-      <c r="F2798" t="s">
-        <v>2706</v>
-      </c>
-    </row>
-    <row r="2799" spans="6:6">
-      <c r="F2799" t="s">
-        <v>2459</v>
-      </c>
-    </row>
-    <row r="2800" spans="6:6">
-      <c r="F2800" t="s">
-        <v>2620</v>
-      </c>
-    </row>
-    <row r="2801" spans="6:6">
-      <c r="F2801" t="s">
-        <v>2462</v>
-      </c>
-    </row>
-    <row r="2802" spans="6:6">
-      <c r="F2802" t="s">
-        <v>2621</v>
-      </c>
-    </row>
-    <row r="2803" spans="6:6">
-      <c r="F2803" t="s">
-        <v>2707</v>
-      </c>
-    </row>
-    <row r="2804" spans="6:6">
-      <c r="F2804" t="s">
-        <v>2464</v>
-      </c>
-    </row>
-    <row r="2805" spans="6:6">
-      <c r="F2805" t="s">
-        <v>2623</v>
-      </c>
-    </row>
-    <row r="2806" spans="6:6">
-      <c r="F2806" t="s">
-        <v>2462</v>
-      </c>
-    </row>
-    <row r="2807" spans="6:6">
-      <c r="F2807" t="s">
-        <v>2621</v>
-      </c>
-    </row>
-    <row r="2808" spans="6:6">
-      <c r="F2808" t="s">
-        <v>2708</v>
-      </c>
-    </row>
-    <row r="2809" spans="6:6">
-      <c r="F2809" t="s">
-        <v>2464</v>
-      </c>
-    </row>
-    <row r="2810" spans="6:6">
-      <c r="F2810" t="s">
-        <v>2620</v>
-      </c>
-    </row>
-    <row r="2811" spans="6:6">
-      <c r="F2811" t="s">
-        <v>2497</v>
-      </c>
-    </row>
-    <row r="2812" spans="6:6">
-      <c r="F2812" t="s">
-        <v>2621</v>
-      </c>
-    </row>
-    <row r="2813" spans="6:6">
-      <c r="F2813" t="s">
-        <v>2709</v>
-      </c>
-    </row>
-    <row r="2814" spans="6:6">
-      <c r="F2814" t="s">
-        <v>2710</v>
-      </c>
-    </row>
-    <row r="2815" spans="6:6">
-      <c r="F2815" t="s">
-        <v>2711</v>
+    <row r="2692" spans="1:3">
+      <c r="A2692">
+        <v>4191</v>
+      </c>
+      <c r="B2692" s="16" t="s">
+        <v>2747</v>
+      </c>
+    </row>
+    <row r="2693" spans="1:3">
+      <c r="A2693">
+        <v>4192</v>
+      </c>
+      <c r="B2693" t="s">
+        <v>2748</v>
+      </c>
+    </row>
+    <row r="2694" spans="1:3">
+      <c r="A2694">
+        <v>4193</v>
+      </c>
+      <c r="B2694" t="s">
+        <v>2749</v>
+      </c>
+    </row>
+    <row r="2695" spans="1:3">
+      <c r="A2695">
+        <v>4199</v>
+      </c>
+      <c r="B2695" s="28" t="s">
+        <v>2750</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fix a couple of typos
</commit_message>
<xml_diff>
--- a/RBG_arduino/StateTable_minimal.xlsx
+++ b/RBG_arduino/StateTable_minimal.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/markdolson/GitHub-Mark-MDO47/RubberBandGun/RBG_arduino/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A868CA1-9BF5-AE4A-8681-FD1886832334}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B53A6D8-D0DA-074E-BC18-F282BFC4D73F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15540" activeTab="1" xr2:uid="{CCADFEE4-B0E1-4363-9617-1683960BED03}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15540" activeTab="2" xr2:uid="{CCADFEE4-B0E1-4363-9617-1683960BED03}"/>
   </bookViews>
   <sheets>
     <sheet name="StateTable" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
     <sheet name="ThingsToTry" sheetId="5" r:id="rId5"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">debugging!$A$2649:$B$2695</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">debugging!$A$2709:$B$2781</definedName>
     <definedName name="yxcmd">'YX5200 info'!$A$2:$C$44</definedName>
   </definedNames>
   <calcPr calcId="181029"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3584" uniqueCount="2773">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3663" uniqueCount="2844">
   <si>
     <t>trigOnly</t>
   </si>
@@ -8530,9 +8530,6 @@
     <t>RBG_waitForInput</t>
   </si>
   <si>
-    <t>foundRow</t>
-  </si>
-  <si>
     <t>need a way to start the first row</t>
   </si>
   <si>
@@ -8586,6 +8583,222 @@
   </si>
   <si>
     <t>if foundInputRow != mNone, myState Row = foundInput</t>
+  </si>
+  <si>
+    <t>complete re-organization: major re-write, depend on rows not state inproc</t>
+  </si>
+  <si>
+    <t>15: RBG_startEffectSound ln 428 EFCT num 40 final num 41 loopCount 0</t>
+  </si>
+  <si>
+    <t>16: RBG_startEffectSound ln 463 myDFPlayer problem after check busy</t>
+  </si>
+  <si>
+    <t>31:DEBUG loop() - nowVinputRBG 0x240 loopCount 1</t>
+  </si>
+  <si>
+    <t>679:DEBUG loop() - nowVinputRBG 0x40 loopCount 65</t>
+  </si>
+  <si>
+    <t>692:DEBUG RBG_processStateTable() - tmpVinputRBG 0x40 from row 0 foundInputRow 1 loopCount 65</t>
+  </si>
+  <si>
+    <t>722:DEBUG RBG_processStateTable() - tmpVinputRBG 0x40 from row 1 foundInputRow 5 loopCount 67</t>
+  </si>
+  <si>
+    <t>726: RBG_startEffectSound ln 428 EFCT num 102 final num 102 loopCount 68</t>
+  </si>
+  <si>
+    <t>728:Number:41 Play Finished!</t>
+  </si>
+  <si>
+    <t>727: RBG_startEffectSound ln 456 myDFPlayer problem after play</t>
+  </si>
+  <si>
+    <t>729: RBG_startEffectSound ln 463 myDFPlayer problem after check busy</t>
+  </si>
+  <si>
+    <t>730:Number:41 Play Finished!</t>
+  </si>
+  <si>
+    <t>740:DEBUG loop() - nowVinputRBG 0x240 loopCount 69</t>
+  </si>
+  <si>
+    <t>3575:DEBUG loop() - nowVinputRBG 0x40 loopCount 258</t>
+  </si>
+  <si>
+    <t>3593: RBG_startEffectSound ln 428 EFCT num 102 final num 102 loopCount 258</t>
+  </si>
+  <si>
+    <t>3594: RBG_startEffectSound ln 456 myDFPlayer problem after play</t>
+  </si>
+  <si>
+    <t>3595:Number:102 Play Finished!</t>
+  </si>
+  <si>
+    <t>3598:DEBUG loop() - nowVinputRBG 0x240 loopCount 259</t>
+  </si>
+  <si>
+    <t>6436:DEBUG loop() - nowVinputRBG 0x40 loopCount 449</t>
+  </si>
+  <si>
+    <t>6454: RBG_startEffectSound ln 428 EFCT num 102 final num 102 loopCount 449</t>
+  </si>
+  <si>
+    <t>6455: RBG_startEffectSound ln 456 myDFPlayer problem after play</t>
+  </si>
+  <si>
+    <t>6456:Number:102 Play Finished!</t>
+  </si>
+  <si>
+    <t>6459:DEBUG loop() - nowVinputRBG 0x240 loopCount 450</t>
+  </si>
+  <si>
+    <t>7059:DEBUG loop() - nowVinputRBG 0x260 loopCount 490</t>
+  </si>
+  <si>
+    <t>7074:DEBUG RBG_processStateTable() - tmpVinputRBG 0x260 from row 5 foundInputRow 7 loopCount 490</t>
+  </si>
+  <si>
+    <t>7078: RBG_startEffectSound ln 428 EFCT num 0 final num 1 loopCount 491</t>
+  </si>
+  <si>
+    <t>7079: RBG_startEffectSound ln 456 myDFPlayer problem after play</t>
+  </si>
+  <si>
+    <t>7080:Number:102 Play Finished!</t>
+  </si>
+  <si>
+    <t>7090:DEBUG loop() - nowVinputRBG 0x240 loopCount 492</t>
+  </si>
+  <si>
+    <t>9734:DEBUG loop() - nowVinputRBG 0x40 loopCount 757</t>
+  </si>
+  <si>
+    <t>9747:DEBUG RBG_processStateTable() - tmpVinputRBG 0x40 from row 7 foundInputRow 8 loopCount 757</t>
+  </si>
+  <si>
+    <t>9771:DEBUG RBG_processStateTable() - tmpVinputRBG 0x40 from row 9 foundInputRow 9 loopCount 759</t>
+  </si>
+  <si>
+    <t>9775: RBG_startEffectSound ln 428 EFCT num 10 final num 11 loopCount 760</t>
+  </si>
+  <si>
+    <t>9776: RBG_startEffectSound ln 456 myDFPlayer problem after play</t>
+  </si>
+  <si>
+    <t>9777:Number:102 Play Finished!</t>
+  </si>
+  <si>
+    <t>9778: RBG_startEffectSound ln 463 myDFPlayer problem after check busy</t>
+  </si>
+  <si>
+    <t>9779:Number:1 Play Finished!</t>
+  </si>
+  <si>
+    <t>9789:DEBUG loop() - nowVinputRBG 0x240 loopCount 761</t>
+  </si>
+  <si>
+    <t>10283:DEBUG loop() - nowVinputRBG 0x40 loopCount 811</t>
+  </si>
+  <si>
+    <t>10296:DEBUG RBG_processStateTable() - tmpVinputRBG 0x40 from row 9 foundInputRow 10 loopCount 811</t>
+  </si>
+  <si>
+    <t>10320:DEBUG RBG_processStateTable() - tmpVinputRBG 0x40 from row 1 foundInputRow 1 loopCount 813</t>
+  </si>
+  <si>
+    <t>10350:DEBUG RBG_processStateTable() - tmpVinputRBG 0x40 from row 1 foundInputRow 5 loopCount 815</t>
+  </si>
+  <si>
+    <t>10354: RBG_startEffectSound ln 428 EFCT num 102 final num 102 loopCount 816</t>
+  </si>
+  <si>
+    <t>10355: RBG_startEffectSound ln 456 myDFPlayer problem after play</t>
+  </si>
+  <si>
+    <t>10356:Number:1 Play Finished!</t>
+  </si>
+  <si>
+    <t>10357: RBG_startEffectSound ln 463 myDFPlayer problem after check busy</t>
+  </si>
+  <si>
+    <t>10358:Number:11 Play Finished!</t>
+  </si>
+  <si>
+    <t>10368:DEBUG loop() - nowVinputRBG 0x240 loopCount 817</t>
+  </si>
+  <si>
+    <t>10968:DEBUG loop() - nowVinputRBG 0x280 loopCount 857</t>
+  </si>
+  <si>
+    <t>10987:DEBUG RBG_processStateTable() - tmpVinputRBG 0x280 from row 5 foundInputRow 11 loopCount 857</t>
+  </si>
+  <si>
+    <t>10991: RBG_startEffectSound ln 428 EFCT num 20 final num 21 loopCount 858</t>
+  </si>
+  <si>
+    <t>11664:DEBUG loop() - nowVinputRBG 0x80 loopCount 926</t>
+  </si>
+  <si>
+    <t>11677:DEBUG RBG_processStateTable() - tmpVinputRBG 0x80 from row 11 foundInputRow 1 loopCount 926</t>
+  </si>
+  <si>
+    <t>11701:DEBUG RBG_processStateTable() - tmpVinputRBG 0x80 from row 1 foundInputRow 3 loopCount 928</t>
+  </si>
+  <si>
+    <t>11705: RBG_startEffectSound ln 428 EFCT num 102 final num 102 loopCount 929</t>
+  </si>
+  <si>
+    <t>11706: RBG_startEffectSound ln 456 myDFPlayer problem after play</t>
+  </si>
+  <si>
+    <t>11707:Number:21 Play Finished!</t>
+  </si>
+  <si>
+    <t>11708: RBG_startEffectSound ln 463 myDFPlayer problem after check busy</t>
+  </si>
+  <si>
+    <t>11709:Number:21 Play Finished!</t>
+  </si>
+  <si>
+    <t>11719:DEBUG loop() - nowVinputRBG 0x280 loopCount 930</t>
+  </si>
+  <si>
+    <t>11944:DEBUG loop() - nowVinputRBG 0x240 loopCount 945</t>
+  </si>
+  <si>
+    <t>11963:DEBUG RBG_processStateTable() - tmpVinputRBG 0x240 from row 3 foundInputRow 13 loopCount 945</t>
+  </si>
+  <si>
+    <t>11967: RBG_startEffectSound ln 428 EFCT num 30 final num 31 loopCount 946</t>
+  </si>
+  <si>
+    <t>12657:DEBUG loop() - nowVinputRBG 0x40 loopCount 1015</t>
+  </si>
+  <si>
+    <t>12670:DEBUG RBG_processStateTable() - tmpVinputRBG 0x40 from row 13 foundInputRow 1 loopCount 1015</t>
+  </si>
+  <si>
+    <t>12700:DEBUG RBG_processStateTable() - tmpVinputRBG 0x40 from row 1 foundInputRow 5 loopCount 1017</t>
+  </si>
+  <si>
+    <t>12704: RBG_startEffectSound ln 428 EFCT num 102 final num 102 loopCount 1018</t>
+  </si>
+  <si>
+    <t>12705: RBG_startEffectSound ln 456 myDFPlayer problem after play</t>
+  </si>
+  <si>
+    <t>12706:Number:31 Play Finished!</t>
+  </si>
+  <si>
+    <t>12707: RBG_startEffectSound ln 463 myDFPlayer problem after check busy</t>
+  </si>
+  <si>
+    <t>12708:Number:31 Play Finished!</t>
+  </si>
+  <si>
+    <t>12718:DEBUG loop() - nowVinputRBG 0x240 loopCount 1019</t>
   </si>
 </sst>
 </file>
@@ -9185,7 +9398,7 @@
   <sheetViews>
     <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A18" sqref="A18"/>
+      <selection pane="bottomLeft" activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
@@ -9264,7 +9477,7 @@
         <v>54</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>2763</v>
+        <v>2762</v>
       </c>
       <c r="C2" s="9" t="s">
         <v>64</v>
@@ -9328,7 +9541,7 @@
     <row r="4" spans="1:18">
       <c r="A4" s="9"/>
       <c r="B4" s="9" t="s">
-        <v>2766</v>
+        <v>2765</v>
       </c>
       <c r="C4" s="9" t="s">
         <v>65</v>
@@ -9366,7 +9579,7 @@
     <row r="5" spans="1:18">
       <c r="A5" s="9"/>
       <c r="B5" s="9" t="s">
-        <v>2766</v>
+        <v>2765</v>
       </c>
       <c r="C5" s="13" t="s">
         <v>65</v>
@@ -9605,7 +9818,7 @@
         <v>80</v>
       </c>
       <c r="B14" t="s">
-        <v>2763</v>
+        <v>2762</v>
       </c>
       <c r="C14" s="9" t="s">
         <v>77</v>
@@ -9628,7 +9841,7 @@
         <v>73</v>
       </c>
       <c r="B16" s="10" t="s">
-        <v>2764</v>
+        <v>2763</v>
       </c>
       <c r="C16" s="9" t="s">
         <v>69</v>
@@ -9646,7 +9859,7 @@
         <v>76</v>
       </c>
       <c r="B18" s="9" t="s">
-        <v>2763</v>
+        <v>2762</v>
       </c>
       <c r="C18" s="9" t="s">
         <v>75</v>
@@ -9673,7 +9886,7 @@
         <v>74</v>
       </c>
       <c r="B21" s="10" t="s">
-        <v>2765</v>
+        <v>2764</v>
       </c>
       <c r="C21" s="9" t="s">
         <v>72</v>
@@ -9693,7 +9906,7 @@
         <v>62</v>
       </c>
       <c r="B23" s="9" t="s">
-        <v>2763</v>
+        <v>2762</v>
       </c>
       <c r="C23" s="9" t="s">
         <v>67</v>
@@ -9715,7 +9928,7 @@
     <row r="24" spans="1:14" ht="16">
       <c r="A24" s="9"/>
       <c r="B24" s="9" t="s">
-        <v>2763</v>
+        <v>2762</v>
       </c>
       <c r="C24" s="13" t="s">
         <v>67</v>
@@ -9747,7 +9960,7 @@
         <v>63</v>
       </c>
       <c r="B26" s="9" t="s">
-        <v>2763</v>
+        <v>2762</v>
       </c>
       <c r="C26" s="9" t="s">
         <v>68</v>
@@ -9764,7 +9977,7 @@
     </row>
     <row r="27" spans="1:14" ht="16">
       <c r="B27" s="9" t="s">
-        <v>2763</v>
+        <v>2762</v>
       </c>
       <c r="C27" s="13" t="s">
         <v>68</v>
@@ -9797,10 +10010,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0B3F56F7-7110-4AD7-8B0D-AA537E4015D5}">
-  <dimension ref="A1:H49"/>
+  <dimension ref="A1:H48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
-      <selection activeCell="E33" sqref="E33"/>
+    <sheetView topLeftCell="A21" workbookViewId="0">
+      <selection activeCell="A41" sqref="A41:XFD41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
@@ -9869,7 +10082,7 @@
     </row>
     <row r="13" spans="1:3">
       <c r="C13" t="s">
-        <v>2762</v>
+        <v>2761</v>
       </c>
     </row>
     <row r="18" spans="1:6" s="29" customFormat="1" ht="16" thickBot="1"/>
@@ -9891,7 +10104,7 @@
     </row>
     <row r="30" spans="1:6">
       <c r="C30" t="s">
-        <v>2760</v>
+        <v>2759</v>
       </c>
     </row>
     <row r="31" spans="1:6">
@@ -9899,12 +10112,12 @@
         <v>2752</v>
       </c>
       <c r="F31" t="s">
-        <v>2758</v>
+        <v>2757</v>
       </c>
     </row>
     <row r="32" spans="1:6" s="29" customFormat="1">
       <c r="D32" s="2" t="s">
-        <v>2759</v>
+        <v>2758</v>
       </c>
     </row>
     <row r="33" spans="2:8">
@@ -9915,27 +10128,27 @@
     <row r="34" spans="2:8" s="29" customFormat="1">
       <c r="C34"/>
       <c r="D34" t="s">
-        <v>2771</v>
+        <v>2770</v>
       </c>
     </row>
     <row r="35" spans="2:8" s="29" customFormat="1">
       <c r="D35" t="s">
-        <v>2772</v>
+        <v>2771</v>
       </c>
     </row>
     <row r="36" spans="2:8" s="29" customFormat="1">
       <c r="E36" s="2" t="s">
-        <v>2770</v>
+        <v>2769</v>
       </c>
     </row>
     <row r="37" spans="2:8" s="29" customFormat="1">
       <c r="D37" t="s">
-        <v>2768</v>
+        <v>2767</v>
       </c>
     </row>
     <row r="38" spans="2:8">
       <c r="E38" t="s">
-        <v>2769</v>
+        <v>2768</v>
       </c>
     </row>
     <row r="40" spans="2:8">
@@ -9945,35 +10158,30 @@
     </row>
     <row r="41" spans="2:8">
       <c r="C41" t="s">
-        <v>2757</v>
+        <v>2753</v>
       </c>
     </row>
     <row r="42" spans="2:8">
-      <c r="C42" t="s">
-        <v>2753</v>
+      <c r="D42" t="s">
+        <v>2754</v>
       </c>
     </row>
     <row r="43" spans="2:8">
       <c r="D43" t="s">
-        <v>2754</v>
-      </c>
-    </row>
-    <row r="44" spans="2:8">
-      <c r="D44" t="s">
         <v>2755</v>
       </c>
-      <c r="H44" t="s">
-        <v>2767</v>
+      <c r="H43" t="s">
+        <v>2766</v>
+      </c>
+    </row>
+    <row r="47" spans="2:8">
+      <c r="B47" t="s">
+        <v>2752</v>
       </c>
     </row>
     <row r="48" spans="2:8">
-      <c r="B48" t="s">
-        <v>2752</v>
-      </c>
-    </row>
-    <row r="49" spans="3:3">
-      <c r="C49" t="s">
-        <v>2761</v>
+      <c r="C48" t="s">
+        <v>2760</v>
       </c>
     </row>
   </sheetData>
@@ -9984,10 +10192,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F57F550E-21B4-4ED7-B7FF-211D228584A7}">
-  <dimension ref="A1:L2695"/>
+  <dimension ref="A1:L2781"/>
   <sheetViews>
-    <sheetView topLeftCell="A2648" workbookViewId="0">
-      <selection activeCell="E2657" sqref="E2657"/>
+    <sheetView tabSelected="1" topLeftCell="A2726" workbookViewId="0">
+      <selection activeCell="B2741" sqref="B2741"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
@@ -30964,6 +31172,694 @@
       </c>
       <c r="B2695" s="28" t="s">
         <v>2748</v>
+      </c>
+    </row>
+    <row r="2700" spans="1:3" ht="16" thickBot="1"/>
+    <row r="2701" spans="1:3" ht="17" thickTop="1" thickBot="1">
+      <c r="B2701" s="1" t="s">
+        <v>2772</v>
+      </c>
+    </row>
+    <row r="2702" spans="1:3" ht="16" thickTop="1"/>
+    <row r="2703" spans="1:3">
+      <c r="B2703" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="2704" spans="1:3">
+      <c r="B2704" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="2705" spans="1:2">
+      <c r="B2705" t="s">
+        <v>922</v>
+      </c>
+    </row>
+    <row r="2706" spans="1:2">
+      <c r="B2706" t="s">
+        <v>923</v>
+      </c>
+    </row>
+    <row r="2707" spans="1:2">
+      <c r="B2707" t="s">
+        <v>428</v>
+      </c>
+    </row>
+    <row r="2709" spans="1:2">
+      <c r="A2709" t="s">
+        <v>2095</v>
+      </c>
+      <c r="B2709" t="s">
+        <v>615</v>
+      </c>
+    </row>
+    <row r="2710" spans="1:2">
+      <c r="A2710">
+        <f>0+LEFT(B2710,FIND(":",B2710)-1)</f>
+        <v>14</v>
+      </c>
+      <c r="B2710" s="28" t="s">
+        <v>2585</v>
+      </c>
+    </row>
+    <row r="2711" spans="1:2">
+      <c r="A2711">
+        <f>0+LEFT(B2711,FIND(":",B2711)-1)</f>
+        <v>15</v>
+      </c>
+      <c r="B2711" s="16" t="s">
+        <v>2773</v>
+      </c>
+    </row>
+    <row r="2712" spans="1:2">
+      <c r="A2712">
+        <f>0+LEFT(B2712,FIND(":",B2712)-1)</f>
+        <v>16</v>
+      </c>
+      <c r="B2712" t="s">
+        <v>2774</v>
+      </c>
+    </row>
+    <row r="2713" spans="1:2">
+      <c r="A2713">
+        <f>0+LEFT(B2713,FIND(":",B2713)-1)</f>
+        <v>31</v>
+      </c>
+      <c r="B2713" s="28" t="s">
+        <v>2775</v>
+      </c>
+    </row>
+    <row r="2714" spans="1:2">
+      <c r="A2714">
+        <f>0+LEFT(B2714,FIND(":",B2714)-1)</f>
+        <v>679</v>
+      </c>
+      <c r="B2714" s="28" t="s">
+        <v>2776</v>
+      </c>
+    </row>
+    <row r="2715" spans="1:2">
+      <c r="A2715">
+        <f>0+LEFT(B2715,FIND(":",B2715)-1)</f>
+        <v>692</v>
+      </c>
+      <c r="B2715" s="12" t="s">
+        <v>2777</v>
+      </c>
+    </row>
+    <row r="2716" spans="1:2">
+      <c r="A2716">
+        <f>0+LEFT(B2716,FIND(":",B2716)-1)</f>
+        <v>722</v>
+      </c>
+      <c r="B2716" s="12" t="s">
+        <v>2778</v>
+      </c>
+    </row>
+    <row r="2717" spans="1:2">
+      <c r="A2717">
+        <f>0+LEFT(B2717,FIND(":",B2717)-1)</f>
+        <v>726</v>
+      </c>
+      <c r="B2717" s="16" t="s">
+        <v>2779</v>
+      </c>
+    </row>
+    <row r="2718" spans="1:2">
+      <c r="A2718">
+        <f>0+LEFT(B2718,FIND(":",B2718)-1)</f>
+        <v>727</v>
+      </c>
+      <c r="B2718" t="s">
+        <v>2781</v>
+      </c>
+    </row>
+    <row r="2719" spans="1:2">
+      <c r="A2719">
+        <f>0+LEFT(B2719,FIND(":",B2719)-1)</f>
+        <v>728</v>
+      </c>
+      <c r="B2719" t="s">
+        <v>2780</v>
+      </c>
+    </row>
+    <row r="2720" spans="1:2">
+      <c r="A2720">
+        <f>0+LEFT(B2720,FIND(":",B2720)-1)</f>
+        <v>729</v>
+      </c>
+      <c r="B2720" t="s">
+        <v>2782</v>
+      </c>
+    </row>
+    <row r="2721" spans="1:2">
+      <c r="A2721">
+        <f>0+LEFT(B2721,FIND(":",B2721)-1)</f>
+        <v>730</v>
+      </c>
+      <c r="B2721" t="s">
+        <v>2783</v>
+      </c>
+    </row>
+    <row r="2722" spans="1:2">
+      <c r="A2722">
+        <f>0+LEFT(B2722,FIND(":",B2722)-1)</f>
+        <v>740</v>
+      </c>
+      <c r="B2722" s="28" t="s">
+        <v>2784</v>
+      </c>
+    </row>
+    <row r="2723" spans="1:2">
+      <c r="A2723">
+        <f>0+LEFT(B2723,FIND(":",B2723)-1)</f>
+        <v>3575</v>
+      </c>
+      <c r="B2723" s="28" t="s">
+        <v>2785</v>
+      </c>
+    </row>
+    <row r="2724" spans="1:2">
+      <c r="A2724">
+        <f>0+LEFT(B2724,FIND(":",B2724)-1)</f>
+        <v>3593</v>
+      </c>
+      <c r="B2724" s="16" t="s">
+        <v>2786</v>
+      </c>
+    </row>
+    <row r="2725" spans="1:2">
+      <c r="A2725">
+        <f>0+LEFT(B2725,FIND(":",B2725)-1)</f>
+        <v>3594</v>
+      </c>
+      <c r="B2725" t="s">
+        <v>2787</v>
+      </c>
+    </row>
+    <row r="2726" spans="1:2">
+      <c r="A2726">
+        <f>0+LEFT(B2726,FIND(":",B2726)-1)</f>
+        <v>3595</v>
+      </c>
+      <c r="B2726" t="s">
+        <v>2788</v>
+      </c>
+    </row>
+    <row r="2727" spans="1:2">
+      <c r="A2727">
+        <f>0+LEFT(B2727,FIND(":",B2727)-1)</f>
+        <v>3598</v>
+      </c>
+      <c r="B2727" s="28" t="s">
+        <v>2789</v>
+      </c>
+    </row>
+    <row r="2728" spans="1:2">
+      <c r="A2728">
+        <f>0+LEFT(B2728,FIND(":",B2728)-1)</f>
+        <v>6436</v>
+      </c>
+      <c r="B2728" s="28" t="s">
+        <v>2790</v>
+      </c>
+    </row>
+    <row r="2729" spans="1:2">
+      <c r="A2729">
+        <f>0+LEFT(B2729,FIND(":",B2729)-1)</f>
+        <v>6454</v>
+      </c>
+      <c r="B2729" s="16" t="s">
+        <v>2791</v>
+      </c>
+    </row>
+    <row r="2730" spans="1:2">
+      <c r="A2730">
+        <f>0+LEFT(B2730,FIND(":",B2730)-1)</f>
+        <v>6455</v>
+      </c>
+      <c r="B2730" t="s">
+        <v>2792</v>
+      </c>
+    </row>
+    <row r="2731" spans="1:2">
+      <c r="A2731">
+        <f>0+LEFT(B2731,FIND(":",B2731)-1)</f>
+        <v>6456</v>
+      </c>
+      <c r="B2731" t="s">
+        <v>2793</v>
+      </c>
+    </row>
+    <row r="2732" spans="1:2">
+      <c r="A2732">
+        <f>0+LEFT(B2732,FIND(":",B2732)-1)</f>
+        <v>6459</v>
+      </c>
+      <c r="B2732" s="28" t="s">
+        <v>2794</v>
+      </c>
+    </row>
+    <row r="2733" spans="1:2">
+      <c r="A2733">
+        <f>0+LEFT(B2733,FIND(":",B2733)-1)</f>
+        <v>7059</v>
+      </c>
+      <c r="B2733" s="28" t="s">
+        <v>2795</v>
+      </c>
+    </row>
+    <row r="2734" spans="1:2">
+      <c r="A2734">
+        <f>0+LEFT(B2734,FIND(":",B2734)-1)</f>
+        <v>7074</v>
+      </c>
+      <c r="B2734" s="12" t="s">
+        <v>2796</v>
+      </c>
+    </row>
+    <row r="2735" spans="1:2">
+      <c r="A2735">
+        <f>0+LEFT(B2735,FIND(":",B2735)-1)</f>
+        <v>7078</v>
+      </c>
+      <c r="B2735" s="16" t="s">
+        <v>2797</v>
+      </c>
+    </row>
+    <row r="2736" spans="1:2">
+      <c r="A2736">
+        <f>0+LEFT(B2736,FIND(":",B2736)-1)</f>
+        <v>7079</v>
+      </c>
+      <c r="B2736" t="s">
+        <v>2798</v>
+      </c>
+    </row>
+    <row r="2737" spans="1:2">
+      <c r="A2737">
+        <f>0+LEFT(B2737,FIND(":",B2737)-1)</f>
+        <v>7080</v>
+      </c>
+      <c r="B2737" t="s">
+        <v>2799</v>
+      </c>
+    </row>
+    <row r="2738" spans="1:2">
+      <c r="A2738">
+        <f>0+LEFT(B2738,FIND(":",B2738)-1)</f>
+        <v>7090</v>
+      </c>
+      <c r="B2738" s="28" t="s">
+        <v>2800</v>
+      </c>
+    </row>
+    <row r="2739" spans="1:2">
+      <c r="A2739">
+        <f>0+LEFT(B2739,FIND(":",B2739)-1)</f>
+        <v>9734</v>
+      </c>
+      <c r="B2739" s="28" t="s">
+        <v>2801</v>
+      </c>
+    </row>
+    <row r="2740" spans="1:2">
+      <c r="A2740">
+        <f>0+LEFT(B2740,FIND(":",B2740)-1)</f>
+        <v>9747</v>
+      </c>
+      <c r="B2740" s="12" t="s">
+        <v>2802</v>
+      </c>
+    </row>
+    <row r="2741" spans="1:2">
+      <c r="A2741">
+        <f>0+LEFT(B2741,FIND(":",B2741)-1)</f>
+        <v>9771</v>
+      </c>
+      <c r="B2741" s="12" t="s">
+        <v>2803</v>
+      </c>
+    </row>
+    <row r="2742" spans="1:2">
+      <c r="A2742">
+        <f>0+LEFT(B2742,FIND(":",B2742)-1)</f>
+        <v>9775</v>
+      </c>
+      <c r="B2742" s="16" t="s">
+        <v>2804</v>
+      </c>
+    </row>
+    <row r="2743" spans="1:2">
+      <c r="A2743">
+        <f>0+LEFT(B2743,FIND(":",B2743)-1)</f>
+        <v>9776</v>
+      </c>
+      <c r="B2743" t="s">
+        <v>2805</v>
+      </c>
+    </row>
+    <row r="2744" spans="1:2">
+      <c r="A2744">
+        <f>0+LEFT(B2744,FIND(":",B2744)-1)</f>
+        <v>9777</v>
+      </c>
+      <c r="B2744" t="s">
+        <v>2806</v>
+      </c>
+    </row>
+    <row r="2745" spans="1:2">
+      <c r="A2745">
+        <f>0+LEFT(B2745,FIND(":",B2745)-1)</f>
+        <v>9778</v>
+      </c>
+      <c r="B2745" t="s">
+        <v>2807</v>
+      </c>
+    </row>
+    <row r="2746" spans="1:2">
+      <c r="A2746">
+        <f>0+LEFT(B2746,FIND(":",B2746)-1)</f>
+        <v>9779</v>
+      </c>
+      <c r="B2746" t="s">
+        <v>2808</v>
+      </c>
+    </row>
+    <row r="2747" spans="1:2">
+      <c r="A2747">
+        <f>0+LEFT(B2747,FIND(":",B2747)-1)</f>
+        <v>9789</v>
+      </c>
+      <c r="B2747" s="28" t="s">
+        <v>2809</v>
+      </c>
+    </row>
+    <row r="2748" spans="1:2">
+      <c r="A2748">
+        <f>0+LEFT(B2748,FIND(":",B2748)-1)</f>
+        <v>10283</v>
+      </c>
+      <c r="B2748" s="28" t="s">
+        <v>2810</v>
+      </c>
+    </row>
+    <row r="2749" spans="1:2">
+      <c r="A2749">
+        <f>0+LEFT(B2749,FIND(":",B2749)-1)</f>
+        <v>10296</v>
+      </c>
+      <c r="B2749" s="12" t="s">
+        <v>2811</v>
+      </c>
+    </row>
+    <row r="2750" spans="1:2">
+      <c r="A2750">
+        <f>0+LEFT(B2750,FIND(":",B2750)-1)</f>
+        <v>10320</v>
+      </c>
+      <c r="B2750" s="12" t="s">
+        <v>2812</v>
+      </c>
+    </row>
+    <row r="2751" spans="1:2">
+      <c r="A2751">
+        <f>0+LEFT(B2751,FIND(":",B2751)-1)</f>
+        <v>10350</v>
+      </c>
+      <c r="B2751" s="12" t="s">
+        <v>2813</v>
+      </c>
+    </row>
+    <row r="2752" spans="1:2">
+      <c r="A2752">
+        <f>0+LEFT(B2752,FIND(":",B2752)-1)</f>
+        <v>10354</v>
+      </c>
+      <c r="B2752" s="16" t="s">
+        <v>2814</v>
+      </c>
+    </row>
+    <row r="2753" spans="1:2">
+      <c r="A2753">
+        <f>0+LEFT(B2753,FIND(":",B2753)-1)</f>
+        <v>10355</v>
+      </c>
+      <c r="B2753" t="s">
+        <v>2815</v>
+      </c>
+    </row>
+    <row r="2754" spans="1:2">
+      <c r="A2754">
+        <f>0+LEFT(B2754,FIND(":",B2754)-1)</f>
+        <v>10356</v>
+      </c>
+      <c r="B2754" t="s">
+        <v>2816</v>
+      </c>
+    </row>
+    <row r="2755" spans="1:2">
+      <c r="A2755">
+        <f>0+LEFT(B2755,FIND(":",B2755)-1)</f>
+        <v>10357</v>
+      </c>
+      <c r="B2755" t="s">
+        <v>2817</v>
+      </c>
+    </row>
+    <row r="2756" spans="1:2">
+      <c r="A2756">
+        <f>0+LEFT(B2756,FIND(":",B2756)-1)</f>
+        <v>10358</v>
+      </c>
+      <c r="B2756" t="s">
+        <v>2818</v>
+      </c>
+    </row>
+    <row r="2757" spans="1:2">
+      <c r="A2757">
+        <f>0+LEFT(B2757,FIND(":",B2757)-1)</f>
+        <v>10368</v>
+      </c>
+      <c r="B2757" s="28" t="s">
+        <v>2819</v>
+      </c>
+    </row>
+    <row r="2758" spans="1:2">
+      <c r="A2758">
+        <f>0+LEFT(B2758,FIND(":",B2758)-1)</f>
+        <v>10968</v>
+      </c>
+      <c r="B2758" s="28" t="s">
+        <v>2820</v>
+      </c>
+    </row>
+    <row r="2759" spans="1:2">
+      <c r="A2759">
+        <f>0+LEFT(B2759,FIND(":",B2759)-1)</f>
+        <v>10987</v>
+      </c>
+      <c r="B2759" s="12" t="s">
+        <v>2821</v>
+      </c>
+    </row>
+    <row r="2760" spans="1:2">
+      <c r="A2760">
+        <f>0+LEFT(B2760,FIND(":",B2760)-1)</f>
+        <v>10991</v>
+      </c>
+      <c r="B2760" s="16" t="s">
+        <v>2822</v>
+      </c>
+    </row>
+    <row r="2761" spans="1:2">
+      <c r="A2761">
+        <f>0+LEFT(B2761,FIND(":",B2761)-1)</f>
+        <v>11664</v>
+      </c>
+      <c r="B2761" s="28" t="s">
+        <v>2823</v>
+      </c>
+    </row>
+    <row r="2762" spans="1:2">
+      <c r="A2762">
+        <f>0+LEFT(B2762,FIND(":",B2762)-1)</f>
+        <v>11677</v>
+      </c>
+      <c r="B2762" s="12" t="s">
+        <v>2824</v>
+      </c>
+    </row>
+    <row r="2763" spans="1:2">
+      <c r="A2763">
+        <f>0+LEFT(B2763,FIND(":",B2763)-1)</f>
+        <v>11701</v>
+      </c>
+      <c r="B2763" s="12" t="s">
+        <v>2825</v>
+      </c>
+    </row>
+    <row r="2764" spans="1:2">
+      <c r="A2764">
+        <f>0+LEFT(B2764,FIND(":",B2764)-1)</f>
+        <v>11705</v>
+      </c>
+      <c r="B2764" s="16" t="s">
+        <v>2826</v>
+      </c>
+    </row>
+    <row r="2765" spans="1:2">
+      <c r="A2765">
+        <f>0+LEFT(B2765,FIND(":",B2765)-1)</f>
+        <v>11706</v>
+      </c>
+      <c r="B2765" t="s">
+        <v>2827</v>
+      </c>
+    </row>
+    <row r="2766" spans="1:2">
+      <c r="A2766">
+        <f>0+LEFT(B2766,FIND(":",B2766)-1)</f>
+        <v>11707</v>
+      </c>
+      <c r="B2766" t="s">
+        <v>2828</v>
+      </c>
+    </row>
+    <row r="2767" spans="1:2">
+      <c r="A2767">
+        <f>0+LEFT(B2767,FIND(":",B2767)-1)</f>
+        <v>11708</v>
+      </c>
+      <c r="B2767" t="s">
+        <v>2829</v>
+      </c>
+    </row>
+    <row r="2768" spans="1:2">
+      <c r="A2768">
+        <f>0+LEFT(B2768,FIND(":",B2768)-1)</f>
+        <v>11709</v>
+      </c>
+      <c r="B2768" t="s">
+        <v>2830</v>
+      </c>
+    </row>
+    <row r="2769" spans="1:2">
+      <c r="A2769">
+        <f>0+LEFT(B2769,FIND(":",B2769)-1)</f>
+        <v>11719</v>
+      </c>
+      <c r="B2769" s="28" t="s">
+        <v>2831</v>
+      </c>
+    </row>
+    <row r="2770" spans="1:2">
+      <c r="A2770">
+        <f>0+LEFT(B2770,FIND(":",B2770)-1)</f>
+        <v>11944</v>
+      </c>
+      <c r="B2770" s="28" t="s">
+        <v>2832</v>
+      </c>
+    </row>
+    <row r="2771" spans="1:2">
+      <c r="A2771">
+        <f>0+LEFT(B2771,FIND(":",B2771)-1)</f>
+        <v>11963</v>
+      </c>
+      <c r="B2771" s="12" t="s">
+        <v>2833</v>
+      </c>
+    </row>
+    <row r="2772" spans="1:2">
+      <c r="A2772">
+        <f>0+LEFT(B2772,FIND(":",B2772)-1)</f>
+        <v>11967</v>
+      </c>
+      <c r="B2772" s="16" t="s">
+        <v>2834</v>
+      </c>
+    </row>
+    <row r="2773" spans="1:2">
+      <c r="A2773">
+        <f>0+LEFT(B2773,FIND(":",B2773)-1)</f>
+        <v>12657</v>
+      </c>
+      <c r="B2773" s="28" t="s">
+        <v>2835</v>
+      </c>
+    </row>
+    <row r="2774" spans="1:2">
+      <c r="A2774">
+        <f>0+LEFT(B2774,FIND(":",B2774)-1)</f>
+        <v>12670</v>
+      </c>
+      <c r="B2774" s="12" t="s">
+        <v>2836</v>
+      </c>
+    </row>
+    <row r="2775" spans="1:2">
+      <c r="A2775">
+        <f>0+LEFT(B2775,FIND(":",B2775)-1)</f>
+        <v>12700</v>
+      </c>
+      <c r="B2775" s="12" t="s">
+        <v>2837</v>
+      </c>
+    </row>
+    <row r="2776" spans="1:2">
+      <c r="A2776">
+        <f>0+LEFT(B2776,FIND(":",B2776)-1)</f>
+        <v>12704</v>
+      </c>
+      <c r="B2776" s="16" t="s">
+        <v>2838</v>
+      </c>
+    </row>
+    <row r="2777" spans="1:2">
+      <c r="A2777">
+        <f>0+LEFT(B2777,FIND(":",B2777)-1)</f>
+        <v>12705</v>
+      </c>
+      <c r="B2777" t="s">
+        <v>2839</v>
+      </c>
+    </row>
+    <row r="2778" spans="1:2">
+      <c r="A2778">
+        <f>0+LEFT(B2778,FIND(":",B2778)-1)</f>
+        <v>12706</v>
+      </c>
+      <c r="B2778" t="s">
+        <v>2840</v>
+      </c>
+    </row>
+    <row r="2779" spans="1:2">
+      <c r="A2779">
+        <f>0+LEFT(B2779,FIND(":",B2779)-1)</f>
+        <v>12707</v>
+      </c>
+      <c r="B2779" t="s">
+        <v>2841</v>
+      </c>
+    </row>
+    <row r="2780" spans="1:2">
+      <c r="A2780">
+        <f>0+LEFT(B2780,FIND(":",B2780)-1)</f>
+        <v>12708</v>
+      </c>
+      <c r="B2780" t="s">
+        <v>2842</v>
+      </c>
+    </row>
+    <row r="2781" spans="1:2">
+      <c r="A2781">
+        <f>0+LEFT(B2781,FIND(":",B2781)-1)</f>
+        <v>12718</v>
+      </c>
+      <c r="B2781" s="28" t="s">
+        <v>2843</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
some additional checks when waiting for input
</commit_message>
<xml_diff>
--- a/RBG_arduino/StateTable_minimal.xlsx
+++ b/RBG_arduino/StateTable_minimal.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/markdolson/GitHub-Mark-MDO47/RubberBandGun/RBG_arduino/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45162EBF-4684-9F4F-8965-4317C47BFE39}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89ACC72D-F7F6-FD43-8B8D-9D2E4F8D0791}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15540" activeTab="2" xr2:uid="{CCADFEE4-B0E1-4363-9617-1683960BED03}"/>
   </bookViews>
@@ -20,7 +20,7 @@
     <sheet name="ThingsToTry" sheetId="5" r:id="rId5"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">debugging!$A$2709:$B$2781</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">debugging!$A$2792:$B$2832</definedName>
     <definedName name="yxcmd">'YX5200 info'!$A$2:$C$44</definedName>
   </definedNames>
   <calcPr calcId="181029"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3663" uniqueCount="2844">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3711" uniqueCount="2886">
   <si>
     <t>trigOnly</t>
   </si>
@@ -8799,6 +8799,132 @@
   </si>
   <si>
     <t>12718:DEBUG loop() - nowVinputRBG 0x240 loopCount 1019</t>
+  </si>
+  <si>
+    <t>complete re-organization: major re-write, depend on rows not state inproc, got rid of inproc state</t>
+  </si>
+  <si>
+    <t>"=0+LEFT(B1,FIND(":",B1)-1)</t>
+  </si>
+  <si>
+    <t>13:DEBUG loop() - nowVinputRBG 0x40 loopCount 0</t>
+  </si>
+  <si>
+    <t>14: RBG_startEffectSound ln 436 EFCT num 40 final num 41 loopCount 0</t>
+  </si>
+  <si>
+    <t>15: RBG_startEffectSound ln 457 myDFPlayer problem after check busy</t>
+  </si>
+  <si>
+    <t>29:DEBUG loop() - nowVinputRBG 0x240 loopCount 1</t>
+  </si>
+  <si>
+    <t>658:DEBUG loop() - nowVinputRBG 0x40 loopCount 70</t>
+  </si>
+  <si>
+    <t>670:DEBUG RBG_processStateTable() - tmpVinputRBG 0x40 from row 0 foundInputRow 1 loopCount 70</t>
+  </si>
+  <si>
+    <t>698:DEBUG RBG_processStateTable() - tmpVinputRBG 0x40 from row 1 foundInputRow 5 loopCount 72</t>
+  </si>
+  <si>
+    <t>702: RBG_startEffectSound ln 436 EFCT num 102 final num 102 loopCount 73</t>
+  </si>
+  <si>
+    <t>703: RBG_startEffectSound ln 451 myDFPlayer problem after play</t>
+  </si>
+  <si>
+    <t>704:Number:41 Play Finished!</t>
+  </si>
+  <si>
+    <t>705: RBG_startEffectSound ln 457 myDFPlayer problem after check busy</t>
+  </si>
+  <si>
+    <t>706:Number:41 Play Finished!</t>
+  </si>
+  <si>
+    <t>715:DEBUG loop() - nowVinputRBG 0x240 loopCount 74</t>
+  </si>
+  <si>
+    <t>1255:DEBUG loop() - nowVinputRBG 0x280 loopCount 110</t>
+  </si>
+  <si>
+    <t>1273:DEBUG RBG_processStateTable() - tmpVinputRBG 0x280 from row 5 foundInputRow 11 loopCount 110</t>
+  </si>
+  <si>
+    <t>1277: RBG_startEffectSound ln 436 EFCT num 20 final num 21 loopCount 111</t>
+  </si>
+  <si>
+    <t>1661:DEBUG loop() - nowVinputRBG 0x240 loopCount 137</t>
+  </si>
+  <si>
+    <t>1679:DEBUG RBG_processStateTable() - tmpVinputRBG 0x240 from row 11 foundInputRow 13 loopCount 137</t>
+  </si>
+  <si>
+    <t>1683: RBG_startEffectSound ln 436 EFCT num 30 final num 31 loopCount 138</t>
+  </si>
+  <si>
+    <t>1684: RBG_startEffectSound ln 457 myDFPlayer problem after check busy</t>
+  </si>
+  <si>
+    <t>1918:DEBUG loop() - nowVinputRBG 0x280 loopCount 154</t>
+  </si>
+  <si>
+    <t>1936:DEBUG RBG_processStateTable() - tmpVinputRBG 0x280 from row 13 foundInputRow 11 loopCount 154</t>
+  </si>
+  <si>
+    <t>1940: RBG_startEffectSound ln 436 EFCT num 20 final num 21 loopCount 155</t>
+  </si>
+  <si>
+    <t>1941: RBG_startEffectSound ln 457 myDFPlayer problem after check busy</t>
+  </si>
+  <si>
+    <t>2055:DEBUG loop() - nowVinputRBG 0x240 loopCount 163</t>
+  </si>
+  <si>
+    <t>2073:DEBUG RBG_processStateTable() - tmpVinputRBG 0x240 from row 11 foundInputRow 13 loopCount 163</t>
+  </si>
+  <si>
+    <t>2077: RBG_startEffectSound ln 436 EFCT num 30 final num 31 loopCount 164</t>
+  </si>
+  <si>
+    <t>2821:DEBUG loop() - nowVinputRBG 0x40 loopCount 214</t>
+  </si>
+  <si>
+    <t>2833:DEBUG RBG_processStateTable() - tmpVinputRBG 0x40 from row 13 foundInputRow 1 loopCount 214</t>
+  </si>
+  <si>
+    <t>2861:DEBUG RBG_processStateTable() - tmpVinputRBG 0x40 from row 1 foundInputRow 5 loopCount 216</t>
+  </si>
+  <si>
+    <t>2865: RBG_startEffectSound ln 436 EFCT num 102 final num 102 loopCount 217</t>
+  </si>
+  <si>
+    <t>2866: RBG_startEffectSound ln 451 myDFPlayer problem after play</t>
+  </si>
+  <si>
+    <t>2867:Number:31 Play Finished!</t>
+  </si>
+  <si>
+    <t>2868: RBG_startEffectSound ln 457 myDFPlayer problem after check busy</t>
+  </si>
+  <si>
+    <t>2869:Number:31 Play Finished!</t>
+  </si>
+  <si>
+    <t>2878:DEBUG loop() - nowVinputRBG 0x240 loopCount 218</t>
+  </si>
+  <si>
+    <t>3013:DEBUG loop() - nowVinputRBG 0x260 loopCount 227</t>
+  </si>
+  <si>
+    <t>3027:DEBUG RBG_processStateTable() - tmpVinputRBG 0x260 from row 5 foundInputRow 7 loopCount 227</t>
+  </si>
+  <si>
+    <t>3030:DEBUG loop() - nowVinputRBG 0x240 loopCount 228</t>
+  </si>
+  <si>
+    <t>3031: RBG_startEffectSound ln 436 EFCT num 0 final num 1 loopCount 228</t>
   </si>
 </sst>
 </file>
@@ -9398,7 +9524,7 @@
   <sheetViews>
     <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C16" sqref="C16"/>
+      <selection pane="bottomLeft" activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
@@ -10192,15 +10318,15 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F57F550E-21B4-4ED7-B7FF-211D228584A7}">
-  <dimension ref="A1:L2781"/>
+  <dimension ref="A1:L2832"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2726" workbookViewId="0">
-      <selection activeCell="B2741" sqref="B2741"/>
+    <sheetView tabSelected="1" topLeftCell="A2810" workbookViewId="0">
+      <selection activeCell="C2807" sqref="C2807"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="2" width="71.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="84.6640625" customWidth="1"/>
     <col min="3" max="3" width="12.6640625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="19.5" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="12.1640625" bestFit="1" customWidth="1"/>
@@ -31860,6 +31986,366 @@
       </c>
       <c r="B2781" s="28" t="s">
         <v>2843</v>
+      </c>
+    </row>
+    <row r="2783" spans="1:2" ht="16" thickBot="1"/>
+    <row r="2784" spans="1:2" ht="17" thickTop="1" thickBot="1">
+      <c r="B2784" s="1" t="s">
+        <v>2844</v>
+      </c>
+    </row>
+    <row r="2785" spans="1:2" ht="16" thickTop="1"/>
+    <row r="2786" spans="1:2">
+      <c r="B2786" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="2787" spans="1:2">
+      <c r="B2787" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="2788" spans="1:2">
+      <c r="B2788" t="s">
+        <v>922</v>
+      </c>
+    </row>
+    <row r="2789" spans="1:2">
+      <c r="B2789" t="s">
+        <v>923</v>
+      </c>
+    </row>
+    <row r="2790" spans="1:2">
+      <c r="B2790" t="s">
+        <v>2845</v>
+      </c>
+    </row>
+    <row r="2792" spans="1:2">
+      <c r="A2792" t="s">
+        <v>2095</v>
+      </c>
+      <c r="B2792" t="s">
+        <v>615</v>
+      </c>
+    </row>
+    <row r="2793" spans="1:2">
+      <c r="A2793">
+        <v>13</v>
+      </c>
+      <c r="B2793" s="28" t="s">
+        <v>2846</v>
+      </c>
+    </row>
+    <row r="2794" spans="1:2">
+      <c r="A2794">
+        <v>14</v>
+      </c>
+      <c r="B2794" s="16" t="s">
+        <v>2847</v>
+      </c>
+    </row>
+    <row r="2795" spans="1:2">
+      <c r="A2795">
+        <v>15</v>
+      </c>
+      <c r="B2795" t="s">
+        <v>2848</v>
+      </c>
+    </row>
+    <row r="2796" spans="1:2">
+      <c r="A2796">
+        <v>29</v>
+      </c>
+      <c r="B2796" s="28" t="s">
+        <v>2849</v>
+      </c>
+    </row>
+    <row r="2797" spans="1:2">
+      <c r="A2797">
+        <v>658</v>
+      </c>
+      <c r="B2797" s="28" t="s">
+        <v>2850</v>
+      </c>
+    </row>
+    <row r="2798" spans="1:2">
+      <c r="A2798">
+        <v>670</v>
+      </c>
+      <c r="B2798" s="12" t="s">
+        <v>2851</v>
+      </c>
+    </row>
+    <row r="2799" spans="1:2">
+      <c r="A2799">
+        <v>698</v>
+      </c>
+      <c r="B2799" s="12" t="s">
+        <v>2852</v>
+      </c>
+    </row>
+    <row r="2800" spans="1:2">
+      <c r="A2800">
+        <v>702</v>
+      </c>
+      <c r="B2800" s="16" t="s">
+        <v>2853</v>
+      </c>
+    </row>
+    <row r="2801" spans="1:2">
+      <c r="A2801">
+        <v>703</v>
+      </c>
+      <c r="B2801" t="s">
+        <v>2854</v>
+      </c>
+    </row>
+    <row r="2802" spans="1:2">
+      <c r="A2802">
+        <v>704</v>
+      </c>
+      <c r="B2802" t="s">
+        <v>2855</v>
+      </c>
+    </row>
+    <row r="2803" spans="1:2">
+      <c r="A2803">
+        <v>705</v>
+      </c>
+      <c r="B2803" t="s">
+        <v>2856</v>
+      </c>
+    </row>
+    <row r="2804" spans="1:2">
+      <c r="A2804">
+        <v>706</v>
+      </c>
+      <c r="B2804" t="s">
+        <v>2857</v>
+      </c>
+    </row>
+    <row r="2805" spans="1:2">
+      <c r="A2805">
+        <v>715</v>
+      </c>
+      <c r="B2805" s="28" t="s">
+        <v>2858</v>
+      </c>
+    </row>
+    <row r="2806" spans="1:2">
+      <c r="A2806">
+        <v>1255</v>
+      </c>
+      <c r="B2806" s="28" t="s">
+        <v>2859</v>
+      </c>
+    </row>
+    <row r="2807" spans="1:2">
+      <c r="A2807">
+        <v>1273</v>
+      </c>
+      <c r="B2807" s="12" t="s">
+        <v>2860</v>
+      </c>
+    </row>
+    <row r="2808" spans="1:2">
+      <c r="A2808">
+        <v>1277</v>
+      </c>
+      <c r="B2808" s="16" t="s">
+        <v>2861</v>
+      </c>
+    </row>
+    <row r="2809" spans="1:2">
+      <c r="A2809">
+        <v>1661</v>
+      </c>
+      <c r="B2809" s="28" t="s">
+        <v>2862</v>
+      </c>
+    </row>
+    <row r="2810" spans="1:2">
+      <c r="A2810">
+        <v>1679</v>
+      </c>
+      <c r="B2810" s="12" t="s">
+        <v>2863</v>
+      </c>
+    </row>
+    <row r="2811" spans="1:2">
+      <c r="A2811">
+        <v>1683</v>
+      </c>
+      <c r="B2811" s="16" t="s">
+        <v>2864</v>
+      </c>
+    </row>
+    <row r="2812" spans="1:2">
+      <c r="A2812">
+        <v>1684</v>
+      </c>
+      <c r="B2812" t="s">
+        <v>2865</v>
+      </c>
+    </row>
+    <row r="2813" spans="1:2">
+      <c r="A2813">
+        <v>1918</v>
+      </c>
+      <c r="B2813" s="28" t="s">
+        <v>2866</v>
+      </c>
+    </row>
+    <row r="2814" spans="1:2">
+      <c r="A2814">
+        <v>1936</v>
+      </c>
+      <c r="B2814" s="12" t="s">
+        <v>2867</v>
+      </c>
+    </row>
+    <row r="2815" spans="1:2">
+      <c r="A2815">
+        <v>1940</v>
+      </c>
+      <c r="B2815" s="16" t="s">
+        <v>2868</v>
+      </c>
+    </row>
+    <row r="2816" spans="1:2">
+      <c r="A2816">
+        <v>1941</v>
+      </c>
+      <c r="B2816" t="s">
+        <v>2869</v>
+      </c>
+    </row>
+    <row r="2817" spans="1:2">
+      <c r="A2817">
+        <v>2055</v>
+      </c>
+      <c r="B2817" s="28" t="s">
+        <v>2870</v>
+      </c>
+    </row>
+    <row r="2818" spans="1:2">
+      <c r="A2818">
+        <v>2073</v>
+      </c>
+      <c r="B2818" s="12" t="s">
+        <v>2871</v>
+      </c>
+    </row>
+    <row r="2819" spans="1:2">
+      <c r="A2819">
+        <v>2077</v>
+      </c>
+      <c r="B2819" s="16" t="s">
+        <v>2872</v>
+      </c>
+    </row>
+    <row r="2820" spans="1:2">
+      <c r="A2820">
+        <v>2821</v>
+      </c>
+      <c r="B2820" s="28" t="s">
+        <v>2873</v>
+      </c>
+    </row>
+    <row r="2821" spans="1:2">
+      <c r="A2821">
+        <v>2833</v>
+      </c>
+      <c r="B2821" s="12" t="s">
+        <v>2874</v>
+      </c>
+    </row>
+    <row r="2822" spans="1:2">
+      <c r="A2822">
+        <v>2861</v>
+      </c>
+      <c r="B2822" s="12" t="s">
+        <v>2875</v>
+      </c>
+    </row>
+    <row r="2823" spans="1:2">
+      <c r="A2823">
+        <v>2865</v>
+      </c>
+      <c r="B2823" s="16" t="s">
+        <v>2876</v>
+      </c>
+    </row>
+    <row r="2824" spans="1:2">
+      <c r="A2824">
+        <v>2866</v>
+      </c>
+      <c r="B2824" t="s">
+        <v>2877</v>
+      </c>
+    </row>
+    <row r="2825" spans="1:2">
+      <c r="A2825">
+        <v>2867</v>
+      </c>
+      <c r="B2825" t="s">
+        <v>2878</v>
+      </c>
+    </row>
+    <row r="2826" spans="1:2">
+      <c r="A2826">
+        <v>2868</v>
+      </c>
+      <c r="B2826" t="s">
+        <v>2879</v>
+      </c>
+    </row>
+    <row r="2827" spans="1:2">
+      <c r="A2827">
+        <v>2869</v>
+      </c>
+      <c r="B2827" t="s">
+        <v>2880</v>
+      </c>
+    </row>
+    <row r="2828" spans="1:2">
+      <c r="A2828">
+        <v>2878</v>
+      </c>
+      <c r="B2828" s="28" t="s">
+        <v>2881</v>
+      </c>
+    </row>
+    <row r="2829" spans="1:2">
+      <c r="A2829">
+        <v>3013</v>
+      </c>
+      <c r="B2829" s="28" t="s">
+        <v>2882</v>
+      </c>
+    </row>
+    <row r="2830" spans="1:2">
+      <c r="A2830">
+        <v>3027</v>
+      </c>
+      <c r="B2830" s="12" t="s">
+        <v>2883</v>
+      </c>
+    </row>
+    <row r="2831" spans="1:2">
+      <c r="A2831">
+        <v>3030</v>
+      </c>
+      <c r="B2831" s="28" t="s">
+        <v>2884</v>
+      </c>
+    </row>
+    <row r="2832" spans="1:2">
+      <c r="A2832">
+        <v>3031</v>
+      </c>
+      <c r="B2832" s="16" t="s">
+        <v>2885</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
some simplification and renaming
</commit_message>
<xml_diff>
--- a/RBG_arduino/StateTable_minimal.xlsx
+++ b/RBG_arduino/StateTable_minimal.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/markdolson/GitHub-Mark-MDO47/RubberBandGun/RBG_arduino/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34908F3D-5275-6241-8B6A-35015779921F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5BE4743-124D-AD48-91B6-391A517549F7}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15540" activeTab="4" xr2:uid="{CCADFEE4-B0E1-4363-9617-1683960BED03}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15540" activeTab="2" xr2:uid="{CCADFEE4-B0E1-4363-9617-1683960BED03}"/>
   </bookViews>
   <sheets>
     <sheet name="StateTable" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
     <sheet name="Sounds" sheetId="5" r:id="rId5"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">debugging!$A$2792:$B$2832</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">debugging!$A$2982:$B$3064</definedName>
     <definedName name="prev">Sounds!$N$2:$N$9</definedName>
     <definedName name="yxcmd">'YX5200 info'!$A$2:$C$44</definedName>
   </definedNames>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3900" uniqueCount="2977">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4290" uniqueCount="3207">
   <si>
     <t>trigOnly</t>
   </si>
@@ -9200,14 +9200,711 @@
   <si>
     <t>https://freesound.org/s/91296/</t>
   </si>
+  <si>
+    <t>| Tag | File Name | URL | Who |</t>
+  </si>
+  <si>
+    <t>| --- | --- | --- | --- |</t>
+  </si>
+  <si>
+    <t>| zero/1.0/ | 407052__sojan__power-charge.flac | https://freesound.org/s/193610/ | crashoverride61088 |</t>
+  </si>
+  <si>
+    <t>10:DEBUG loop() - nowVinputRBG 0x40 loopCount 0</t>
+  </si>
+  <si>
+    <t>31:DEBUG loop() - nowVinputRBG 0x240 loopCount 2</t>
+  </si>
+  <si>
+    <t>61:DEBUG loop() - nowVinputRBG 0x40 loopCount 5</t>
+  </si>
+  <si>
+    <t>79:DEBUG loop() - nowVinputRBG 0x240 loopCount 6</t>
+  </si>
+  <si>
+    <t>140:DEBUG loop() - nowVinputRBG 0x260 loopCount 556380</t>
+  </si>
+  <si>
+    <t>154:DEBUG loop() - nowVinputRBG 0x60 loopCount 556382</t>
+  </si>
+  <si>
+    <t>161:DEBUG loop() - nowVinputRBG 0x260 loopCount 556383</t>
+  </si>
+  <si>
+    <t>172:DEBUG loop() - nowVinputRBG 0x240 loopCount 556385</t>
+  </si>
+  <si>
+    <t>180:DEBUG loop() - nowVinputRBG 0x40 loopCount 557929</t>
+  </si>
+  <si>
+    <t>187:DEBUG loop() - nowVinputRBG 0x240 loopCount 557930</t>
+  </si>
+  <si>
+    <t>215:DEBUG loop() - nowVinputRBG 0x40 loopCount 557935</t>
+  </si>
+  <si>
+    <t>221:DEBUG loop() - nowVinputRBG 0x240 loopCount 557936</t>
+  </si>
+  <si>
+    <t>222:DEBUG loop() - nowVinputRBG 0x260 loopCount 1031537</t>
+  </si>
+  <si>
+    <t>236:DEBUG loop() - nowVinputRBG 0x60 loopCount 1032940</t>
+  </si>
+  <si>
+    <t>243:DEBUG loop() - nowVinputRBG 0x260 loopCount 1032941</t>
+  </si>
+  <si>
+    <t>254:DEBUG loop() - nowVinputRBG 0x240 loopCount 1032943</t>
+  </si>
+  <si>
+    <t>262:DEBUG loop() - nowVinputRBG 0x40 loopCount 1032944</t>
+  </si>
+  <si>
+    <t>273:DEBUG loop() - nowVinputRBG 0x240 loopCount 1032946</t>
+  </si>
+  <si>
+    <t>297:DEBUG loop() - nowVinputRBG 0x40 loopCount 1034620</t>
+  </si>
+  <si>
+    <t>303:DEBUG loop() - nowVinputRBG 0x240 loopCount 1034621</t>
+  </si>
+  <si>
+    <t>30:DEBUG RBG_processStateTable() - tmpVinputRBG 0x40 from row 0 foundInputRow 1 loopCount 1</t>
+  </si>
+  <si>
+    <t>53:DEBUG RBG_processStateTable() - tmpVinputRBG 0x240 from row 1 foundInputRow 5 loopCount 3</t>
+  </si>
+  <si>
+    <t>146:DEBUG RBG_processStateTable() - tmpVinputRBG 0x260 from row 5 foundInputRow 7 loopCount 556380</t>
+  </si>
+  <si>
+    <t>160:DEBUG RBG_processStateTable() - tmpVinputRBG 0x60 from row 7 foundInputRow 8 loopCount 556382</t>
+  </si>
+  <si>
+    <t>171:DEBUG RBG_processStateTable() - tmpVinputRBG 0x260 from row 8 foundInputRow 9 loopCount 556384</t>
+  </si>
+  <si>
+    <t>186:DEBUG RBG_processStateTable() - tmpVinputRBG 0x40 from row 9 foundInputRow 10 loopCount 557929</t>
+  </si>
+  <si>
+    <t>197:DEBUG RBG_processStateTable() - tmpVinputRBG 0x240 from row 10 foundInputRow 1 loopCount 557931</t>
+  </si>
+  <si>
+    <t>207:DEBUG RBG_processStateTable() - tmpVinputRBG 0x240 from row 1 foundInputRow 5 loopCount 557933</t>
+  </si>
+  <si>
+    <t>228:DEBUG RBG_processStateTable() - tmpVinputRBG 0x260 from row 5 foundInputRow 7 loopCount 1031537</t>
+  </si>
+  <si>
+    <t>242:DEBUG RBG_processStateTable() - tmpVinputRBG 0x60 from row 7 foundInputRow 8 loopCount 1032940</t>
+  </si>
+  <si>
+    <t>253:DEBUG RBG_processStateTable() - tmpVinputRBG 0x260 from row 8 foundInputRow 9 loopCount 1032942</t>
+  </si>
+  <si>
+    <t>268:DEBUG RBG_processStateTable() - tmpVinputRBG 0x40 from row 9 foundInputRow 10 loopCount 1032944</t>
+  </si>
+  <si>
+    <t>279:DEBUG RBG_processStateTable() - tmpVinputRBG 0x240 from row 10 foundInputRow 1 loopCount 1032946</t>
+  </si>
+  <si>
+    <t>289:DEBUG RBG_processStateTable() - tmpVinputRBG 0x240 from row 1 foundInputRow 5 loopCount 1032948</t>
+  </si>
+  <si>
+    <t>11: RBG_startEffectSound ln 513 EFCT num 40 final num 41 loopCount 0</t>
+  </si>
+  <si>
+    <t>12: RBG_startEffectSound ln 535 myDFPlayer problem after check busy</t>
+  </si>
+  <si>
+    <t>54: RBG_startEffectSound ln 513 EFCT num 102 final num 102 loopCount 4</t>
+  </si>
+  <si>
+    <t>78: RBG_startEffectSound ln 513 EFCT num 102 final num 102 loopCount 5</t>
+  </si>
+  <si>
+    <t>147: RBG_startEffectSound ln 513 EFCT num 0 final num 1 loopCount 556381</t>
+  </si>
+  <si>
+    <t>173: RBG_startEffectSound ln 513 EFCT num 10 final num 11 loopCount 556385</t>
+  </si>
+  <si>
+    <t>208: RBG_startEffectSound ln 513 EFCT num 102 final num 102 loopCount 557934</t>
+  </si>
+  <si>
+    <t>220: RBG_startEffectSound ln 513 EFCT num 102 final num 102 loopCount 557935</t>
+  </si>
+  <si>
+    <t>229: RBG_startEffectSound ln 513 EFCT num 0 final num 1 loopCount 1031538</t>
+  </si>
+  <si>
+    <t>255: RBG_startEffectSound ln 513 EFCT num 10 final num 11 loopCount 1032943</t>
+  </si>
+  <si>
+    <t>290: RBG_startEffectSound ln 513 EFCT num 102 final num 102 loopCount 1032949</t>
+  </si>
+  <si>
+    <t>302: RBG_startEffectSound ln 513 EFCT num 102 final num 102 loopCount 1034620</t>
+  </si>
+  <si>
+    <t>re-organize timing; sometimes sound doesn't start right. 20 msec delay for state</t>
+  </si>
+  <si>
+    <t>704:DEBUG loop() - nowVinputRBG 0x260 loopCount 58</t>
+  </si>
+  <si>
+    <t>718:DEBUG RBG_processStateTable() - tmpVinputRBG 0x260 from row 5 foundInputRow 7 loopCount 58</t>
+  </si>
+  <si>
+    <t>719: RBG_startEffectSound ln 513 EFCT num 0 final num 1 loopCount 59</t>
+  </si>
+  <si>
+    <t>726:DEBUG loop() - nowVinputRBG 0x60 loopCount 60</t>
+  </si>
+  <si>
+    <t>738:DEBUG RBG_processStateTable() - tmpVinputRBG 0x60 from row 7 foundInputRow 8 loopCount 60</t>
+  </si>
+  <si>
+    <t>739:DEBUG loop() - nowVinputRBG 0x240 loopCount 61</t>
+  </si>
+  <si>
+    <t>755:DEBUG RBG_processStateTable() - tmpVinputRBG 0x240 from row 8 foundInputRow 9 loopCount 62</t>
+  </si>
+  <si>
+    <t>756: RBG_startEffectSound ln 513 EFCT num 10 final num 11 loopCount 63</t>
+  </si>
+  <si>
+    <t>763:DEBUG loop() - nowVinputRBG 0x40 loopCount 64</t>
+  </si>
+  <si>
+    <t>775:DEBUG RBG_processStateTable() - tmpVinputRBG 0x40 from row 9 foundInputRow 10 loopCount 64</t>
+  </si>
+  <si>
+    <t>776:DEBUG loop() - nowVinputRBG 0x240 loopCount 65</t>
+  </si>
+  <si>
+    <t>792:DEBUG RBG_processStateTable() - tmpVinputRBG 0x240 from row 10 foundInputRow 1 loopCount 66</t>
+  </si>
+  <si>
+    <t>814:DEBUG RBG_processStateTable() - tmpVinputRBG 0x240 from row 1 foundInputRow 5 loopCount 68</t>
+  </si>
+  <si>
+    <t>815: RBG_startEffectSound ln 513 EFCT num 102 final num 102 loopCount 69</t>
+  </si>
+  <si>
+    <t>822:DEBUG loop() - nowVinputRBG 0x40 loopCount 70</t>
+  </si>
+  <si>
+    <t>839: RBG_startEffectSound ln 513 EFCT num 102 final num 102 loopCount 70</t>
+  </si>
+  <si>
+    <t>840:DEBUG loop() - nowVinputRBG 0x240 loopCount 71</t>
+  </si>
+  <si>
+    <t>1477:DEBUG loop() - nowVinputRBG 0x260 loopCount 124</t>
+  </si>
+  <si>
+    <t>1491:DEBUG RBG_processStateTable() - tmpVinputRBG 0x260 from row 5 foundInputRow 7 loopCount 124</t>
+  </si>
+  <si>
+    <t>1492: RBG_startEffectSound ln 513 EFCT num 0 final num 1 loopCount 125</t>
+  </si>
+  <si>
+    <t>1511:DEBUG loop() - nowVinputRBG 0x240 loopCount 128</t>
+  </si>
+  <si>
+    <t>re-organize timing; sometimes sound doesn't start right. 40 msec delay for state</t>
+  </si>
+  <si>
+    <t>1976:DEBUG loop() - nowVinputRBG 0x260 loopCount 164</t>
+  </si>
+  <si>
+    <t>1990:DEBUG RBG_processStateTable() - tmpVinputRBG 0x260 from row 5 foundInputRow 7 loopCount 164</t>
+  </si>
+  <si>
+    <t>1991: RBG_startEffectSound ln 513 EFCT num 0 final num 1 loopCount 165</t>
+  </si>
+  <si>
+    <t>1998:DEBUG loop() - nowVinputRBG 0x60 loopCount 166</t>
+  </si>
+  <si>
+    <t>2010:DEBUG RBG_processStateTable() - tmpVinputRBG 0x60 from row 7 foundInputRow 8 loopCount 166</t>
+  </si>
+  <si>
+    <t>2011:DEBUG loop() - nowVinputRBG 0x240 loopCount 167</t>
+  </si>
+  <si>
+    <t>2027:DEBUG RBG_processStateTable() - tmpVinputRBG 0x240 from row 8 foundInputRow 9 loopCount 168</t>
+  </si>
+  <si>
+    <t>2028: RBG_startEffectSound ln 513 EFCT num 10 final num 11 loopCount 169</t>
+  </si>
+  <si>
+    <t>2203:DEBUG loop() - nowVinputRBG 0x260 loopCount 225</t>
+  </si>
+  <si>
+    <t>2228:DEBUG loop() - nowVinputRBG 0x240 loopCount 233</t>
+  </si>
+  <si>
+    <t>2253:DEBUG loop() - nowVinputRBG 0x40 loopCount 592</t>
+  </si>
+  <si>
+    <t>2259:DEBUG RBG_processStateTable() - tmpVinputRBG 0x40 from row 9 foundInputRow 10 loopCount 592</t>
+  </si>
+  <si>
+    <t>2269:DEBUG RBG_processStateTable() - tmpVinputRBG 0x40 from row 10 foundInputRow 1 loopCount 598</t>
+  </si>
+  <si>
+    <t>2279:DEBUG RBG_processStateTable() - tmpVinputRBG 0x40 from row 1 foundInputRow 5 loopCount 605</t>
+  </si>
+  <si>
+    <t>2280: RBG_startEffectSound ln 513 EFCT num 102 final num 102 loopCount 609</t>
+  </si>
+  <si>
+    <t>2281: RBG_startEffectSound ln 535 myDFPlayer problem after check busy</t>
+  </si>
+  <si>
+    <t>2289:DEBUG loop() - nowVinputRBG 0x240 loopCount 609</t>
+  </si>
+  <si>
+    <t>re-organize timing; sometimes sound doesn't start right. 40 msec delay for state; up to 100 msec delay for busy</t>
+  </si>
+  <si>
+    <t>12: RBG_startEffectSound ln 543 waited for AUDIO_BUSY (msec) 10</t>
+  </si>
+  <si>
+    <t>19:DEBUG loop() - nowVinputRBG 0x240 loopCount 1</t>
+  </si>
+  <si>
+    <t>752:DEBUG loop() - nowVinputRBG 0x40 loopCount 242</t>
+  </si>
+  <si>
+    <t>764:DEBUG RBG_processStateTable() - tmpVinputRBG 0x40 from row 0 foundInputRow 1 loopCount 242</t>
+  </si>
+  <si>
+    <t>786:DEBUG RBG_processStateTable() - tmpVinputRBG 0x40 from row 1 foundInputRow 5 loopCount 246</t>
+  </si>
+  <si>
+    <t>787: RBG_startEffectSound ln 513 EFCT num 102 final num 102 loopCount 246</t>
+  </si>
+  <si>
+    <t>788: RBG_startEffectSound ln 543 waited for AUDIO_BUSY (msec) 10</t>
+  </si>
+  <si>
+    <t>795:DEBUG loop() - nowVinputRBG 0x240 loopCount 247</t>
+  </si>
+  <si>
+    <t>1708:DEBUG loop() - nowVinputRBG 0x260 loopCount 1534</t>
+  </si>
+  <si>
+    <t>1714:DEBUG RBG_processStateTable() - tmpVinputRBG 0x260 from row 5 foundInputRow 7 loopCount 1534</t>
+  </si>
+  <si>
+    <t>1715: RBG_startEffectSound ln 513 EFCT num 0 final num 1 loopCount 1537</t>
+  </si>
+  <si>
+    <t>1716: RBG_startEffectSound ln 543 waited for AUDIO_BUSY (msec) 0</t>
+  </si>
+  <si>
+    <t>1723:DEBUG loop() - nowVinputRBG 0x60 loopCount 1537</t>
+  </si>
+  <si>
+    <t>1729:DEBUG RBG_processStateTable() - tmpVinputRBG 0x60 from row 7 foundInputRow 8 loopCount 1537</t>
+  </si>
+  <si>
+    <t>1730:DEBUG loop() - nowVinputRBG 0x260 loopCount 1540</t>
+  </si>
+  <si>
+    <t>1735:DEBUG loop() - nowVinputRBG 0x240 loopCount 1541</t>
+  </si>
+  <si>
+    <t>1741:DEBUG RBG_processStateTable() - tmpVinputRBG 0x240 from row 8 foundInputRow 9 loopCount 1541</t>
+  </si>
+  <si>
+    <t>1742: RBG_startEffectSound ln 513 EFCT num 10 final num 11 loopCount 1541</t>
+  </si>
+  <si>
+    <t>1743: RBG_startEffectSound ln 543 waited for AUDIO_BUSY (msec) 0</t>
+  </si>
+  <si>
+    <t>1750:DEBUG loop() - nowVinputRBG 0x40 loopCount 1542</t>
+  </si>
+  <si>
+    <t>1756:DEBUG RBG_processStateTable() - tmpVinputRBG 0x40 from row 9 foundInputRow 10 loopCount 1542</t>
+  </si>
+  <si>
+    <t>1757:DEBUG loop() - nowVinputRBG 0x240 loopCount 1545</t>
+  </si>
+  <si>
+    <t>1767:DEBUG RBG_processStateTable() - tmpVinputRBG 0x240 from row 10 foundInputRow 1 loopCount 1546</t>
+  </si>
+  <si>
+    <t>1777:DEBUG RBG_processStateTable() - tmpVinputRBG 0x240 from row 1 foundInputRow 5 loopCount 1550</t>
+  </si>
+  <si>
+    <t>1778: RBG_startEffectSound ln 513 EFCT num 102 final num 102 loopCount 1553</t>
+  </si>
+  <si>
+    <t>1779: RBG_startEffectSound ln 543 waited for AUDIO_BUSY (msec) 0</t>
+  </si>
+  <si>
+    <t>1786:DEBUG loop() - nowVinputRBG 0x40 loopCount 1553</t>
+  </si>
+  <si>
+    <t>1791: RBG_startEffectSound ln 513 EFCT num 102 final num 102 loopCount 1553</t>
+  </si>
+  <si>
+    <t>1792: RBG_startEffectSound ln 543 waited for AUDIO_BUSY (msec) 0</t>
+  </si>
+  <si>
+    <t>1793:DEBUG loop() - nowVinputRBG 0x240 loopCount 1554</t>
+  </si>
+  <si>
+    <t>1794:DEBUG loop() - nowVinputRBG 0x40 loopCount 4447</t>
+  </si>
+  <si>
+    <t>1799: RBG_startEffectSound ln 513 EFCT num 102 final num 102 loopCount 4447</t>
+  </si>
+  <si>
+    <t>1800: RBG_startEffectSound ln 543 waited for AUDIO_BUSY (msec) 0</t>
+  </si>
+  <si>
+    <t>1801:DEBUG loop() - nowVinputRBG 0x240 loopCount 4447</t>
+  </si>
+  <si>
+    <t>1802:DEBUG loop() - nowVinputRBG 0x260 loopCount 6161</t>
+  </si>
+  <si>
+    <t>1808:DEBUG RBG_processStateTable() - tmpVinputRBG 0x260 from row 5 foundInputRow 7 loopCount 6161</t>
+  </si>
+  <si>
+    <t>1809: RBG_startEffectSound ln 513 EFCT num 0 final num 1 loopCount 6164</t>
+  </si>
+  <si>
+    <t>1810: RBG_startEffectSound ln 543 waited for AUDIO_BUSY (msec) 0</t>
+  </si>
+  <si>
+    <t>1817:DEBUG loop() - nowVinputRBG 0x240 loopCount 6181</t>
+  </si>
+  <si>
+    <t>1818:DEBUG loop() - nowVinputRBG 0x40 loopCount 9090</t>
+  </si>
+  <si>
+    <t>1824:DEBUG RBG_processStateTable() - tmpVinputRBG 0x40 from row 7 foundInputRow 8 loopCount 9090</t>
+  </si>
+  <si>
+    <t>1834:DEBUG RBG_processStateTable() - tmpVinputRBG 0x40 from row 8 foundInputRow 9 loopCount 9096</t>
+  </si>
+  <si>
+    <t>1835: RBG_startEffectSound ln 513 EFCT num 10 final num 11 loopCount 9096</t>
+  </si>
+  <si>
+    <t>1836: RBG_startEffectSound ln 543 waited for AUDIO_BUSY (msec) 10</t>
+  </si>
+  <si>
+    <t>1843:DEBUG loop() - nowVinputRBG 0x240 loopCount 9097</t>
+  </si>
+  <si>
+    <t>1844:DEBUG loop() - nowVinputRBG 0x40 loopCount 9648</t>
+  </si>
+  <si>
+    <t>1850:DEBUG RBG_processStateTable() - tmpVinputRBG 0x40 from row 9 foundInputRow 10 loopCount 9648</t>
+  </si>
+  <si>
+    <t>1860:DEBUG RBG_processStateTable() - tmpVinputRBG 0x40 from row 10 foundInputRow 1 loopCount 9654</t>
+  </si>
+  <si>
+    <t>1870:DEBUG RBG_processStateTable() - tmpVinputRBG 0x40 from row 1 foundInputRow 5 loopCount 9661</t>
+  </si>
+  <si>
+    <t>1871: RBG_startEffectSound ln 513 EFCT num 102 final num 102 loopCount 9665</t>
+  </si>
+  <si>
+    <t>1872: RBG_startEffectSound ln 543 waited for AUDIO_BUSY (msec) 10</t>
+  </si>
+  <si>
+    <t>1879:DEBUG loop() - nowVinputRBG 0x240 loopCount 9665</t>
+  </si>
+  <si>
+    <t>1880:DEBUG loop() - nowVinputRBG 0x280 loopCount 10238</t>
+  </si>
+  <si>
+    <t>1886:DEBUG RBG_processStateTable() - tmpVinputRBG 0x280 from row 5 foundInputRow 11 loopCount 10238</t>
+  </si>
+  <si>
+    <t>1887: RBG_startEffectSound ln 513 EFCT num 20 final num 21 loopCount 10241</t>
+  </si>
+  <si>
+    <t>1888: RBG_startEffectSound ln 543 waited for AUDIO_BUSY (msec) 0</t>
+  </si>
+  <si>
+    <t>1895:DEBUG loop() - nowVinputRBG 0x80 loopCount 10241</t>
+  </si>
+  <si>
+    <t>1901:DEBUG RBG_processStateTable() - tmpVinputRBG 0x80 from row 11 foundInputRow 1 loopCount 10241</t>
+  </si>
+  <si>
+    <t>1902:DEBUG loop() - nowVinputRBG 0x280 loopCount 10244</t>
+  </si>
+  <si>
+    <t>1912:DEBUG RBG_processStateTable() - tmpVinputRBG 0x280 from row 1 foundInputRow 3 loopCount 10245</t>
+  </si>
+  <si>
+    <t>1913: RBG_startEffectSound ln 513 EFCT num 102 final num 102 loopCount 10248</t>
+  </si>
+  <si>
+    <t>1914: RBG_startEffectSound ln 543 waited for AUDIO_BUSY (msec) 10</t>
+  </si>
+  <si>
+    <t>1921:DEBUG loop() - nowVinputRBG 0x80 loopCount 10248</t>
+  </si>
+  <si>
+    <t>1926: RBG_startEffectSound ln 513 EFCT num 102 final num 102 loopCount 10248</t>
+  </si>
+  <si>
+    <t>1927: RBG_startEffectSound ln 543 waited for AUDIO_BUSY (msec) 0</t>
+  </si>
+  <si>
+    <t>1928:DEBUG loop() - nowVinputRBG 0x280 loopCount 10249</t>
+  </si>
+  <si>
+    <t>1929:DEBUG loop() - nowVinputRBG 0x240 loopCount 10657</t>
+  </si>
+  <si>
+    <t>1935:DEBUG RBG_processStateTable() - tmpVinputRBG 0x240 from row 3 foundInputRow 13 loopCount 10657</t>
+  </si>
+  <si>
+    <t>1936: RBG_startEffectSound ln 513 EFCT num 30 final num 31 loopCount 10660</t>
+  </si>
+  <si>
+    <t>1937: RBG_startEffectSound ln 543 waited for AUDIO_BUSY (msec) 0</t>
+  </si>
+  <si>
+    <t>1944:DEBUG loop() - nowVinputRBG 0x40 loopCount 10660</t>
+  </si>
+  <si>
+    <t>1950:DEBUG RBG_processStateTable() - tmpVinputRBG 0x40 from row 13 foundInputRow 1 loopCount 10660</t>
+  </si>
+  <si>
+    <t>1951:DEBUG loop() - nowVinputRBG 0x240 loopCount 10663</t>
+  </si>
+  <si>
+    <t>1961:DEBUG RBG_processStateTable() - tmpVinputRBG 0x240 from row 1 foundInputRow 5 loopCount 10664</t>
+  </si>
+  <si>
+    <t>1962: RBG_startEffectSound ln 513 EFCT num 102 final num 102 loopCount 10667</t>
+  </si>
+  <si>
+    <t>1963: RBG_startEffectSound ln 543 waited for AUDIO_BUSY (msec) 0</t>
+  </si>
+  <si>
+    <t>1970:DEBUG loop() - nowVinputRBG 0x40 loopCount 10667</t>
+  </si>
+  <si>
+    <t>1975: RBG_startEffectSound ln 513 EFCT num 102 final num 102 loopCount 10667</t>
+  </si>
+  <si>
+    <t>1976: RBG_startEffectSound ln 543 waited for AUDIO_BUSY (msec) 0</t>
+  </si>
+  <si>
+    <t>1977:DEBUG loop() - nowVinputRBG 0x240 loopCount 10668</t>
+  </si>
+  <si>
+    <t>good</t>
+  </si>
+  <si>
+    <t>what</t>
+  </si>
+  <si>
+    <t>trigger ON</t>
+  </si>
+  <si>
+    <t>20 loops</t>
+  </si>
+  <si>
+    <t>8 loops</t>
+  </si>
+  <si>
+    <t>DEBUG loop() - nowVinputRBG 0x260 loopCount 1534</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> RBG_waitForInput mINP_TRIG mINP_BANY thisReturn 7 loopCount 1534</t>
+  </si>
+  <si>
+    <t>DEBUG RBG_processStateTable() - after RBG_waitForInput() call</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  - VinputRBG: 0x0</t>
+  </si>
+  <si>
+    <t>DEBUG RBG_processStateTable() - tmpVinputRBG 0x260 from row 5 foundInputRow 7 loopCount 1534</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> RBG_startEffectSound ln 513 EFCT num 0 final num 1 loopCount 1537</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> RBG_startEffectSound ln 543 waited for AUDIO_BUSY (msec) 0</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> RBG_startEffectLED ln 457 EFCT num 0 final LED num 1 loopCount 1537</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  - tableRow: 7</t>
+  </si>
+  <si>
+    <t>DEBUG RBG_processStateTable() - tmpVinputRBG 0x260 loopCount 1537</t>
+  </si>
+  <si>
+    <t>DEBUG loop() - nowVinputRBG 0x60 loopCount 1537</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> RBG_waitForInput mSPCL_EFCT_ONETIME thisReturn 8 loopCount 1537</t>
+  </si>
+  <si>
+    <t>DEBUG RBG_processStateTable() - tmpVinputRBG 0x60 from row 7 foundInputRow 8 loopCount 1537</t>
+  </si>
+  <si>
+    <t>DEBUG loop() - nowVinputRBG 0x260 loopCount 1540</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  - tableRow: 8</t>
+  </si>
+  <si>
+    <t>DEBUG RBG_processStateTable() - tmpVinputRBG 0x260 loopCount 1540</t>
+  </si>
+  <si>
+    <t>DEBUG loop() - nowVinputRBG 0x240 loopCount 1541</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> RBG_waitForInput mSPCL_HANDLER thisReturn 9 loopCount 1541</t>
+  </si>
+  <si>
+    <t>DEBUG RBG_processStateTable() - tmpVinputRBG 0x240 from row 8 foundInputRow 9 loopCount 1541</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> RBG_startEffectSound ln 513 EFCT num 10 final num 11 loopCount 1541</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> RBG_startEffectLED ln 457 EFCT num 10 final LED num 11 loopCount 1541</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  - tableRow: 9</t>
+  </si>
+  <si>
+    <t>DEBUG RBG_processStateTable() - tmpVinputRBG 0x240 loopCount 1541</t>
+  </si>
+  <si>
+    <t>DEBUG loop() - nowVinputRBG 0x40 loopCount 1542</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> RBG_waitForInput mSPCL_EFCT_ONETIME thisReturn 10 loopCount 1542</t>
+  </si>
+  <si>
+    <t>DEBUG RBG_processStateTable() - tmpVinputRBG 0x40 from row 9 foundInputRow 10 loopCount 1542</t>
+  </si>
+  <si>
+    <t>DEBUG loop() - nowVinputRBG 0x240 loopCount 1545</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  - tableRow: 10</t>
+  </si>
+  <si>
+    <t>DEBUG RBG_processStateTable() - tmpVinputRBG 0x240 loopCount 1545</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> RBG_waitForInput mSPCL_HANDLER thisReturn 1 loopCount 1546</t>
+  </si>
+  <si>
+    <t>DEBUG RBG_processStateTable() - tmpVinputRBG 0x240 from row 10 foundInputRow 1 loopCount 1546</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  - tableRow: 1</t>
+  </si>
+  <si>
+    <t>DEBUG RBG_processStateTable() - tmpVinputRBG 0x240 loopCount 1549</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> RBG_waitForInput mINP_LOCK thisReturn 5 loopCount 1550</t>
+  </si>
+  <si>
+    <t>DEBUG RBG_processStateTable() - tmpVinputRBG 0x240 from row 1 foundInputRow 5 loopCount 1550</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> RBG_startEffectSound ln 513 EFCT num 102 final num 102 loopCount 1553</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> RBG_startEffectLED ln 457 EFCT num 102 final LED num 102 loopCount 1553</t>
+  </si>
+  <si>
+    <t>DEBUG RBG_processStateTable() - tmpVinputRBG 0x240 loopCount 1553</t>
+  </si>
+  <si>
+    <t>DEBUG loop() - nowVinputRBG 0x40 loopCount 1553</t>
+  </si>
+  <si>
+    <t>DEBUG RBG_processStateTable() - tmpVinputRBG 0x40 restart sound 102 loopCount 1553</t>
+  </si>
+  <si>
+    <t>DEBUG loop() - nowVinputRBG 0x240 loopCount 1554</t>
+  </si>
+  <si>
+    <t>DEBUG loop() - nowVinputRBG 0x40 loopCount 4447</t>
+  </si>
+  <si>
+    <t>DEBUG RBG_processStateTable() - tmpVinputRBG 0x40 restart sound 102 loopCount 4447</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> RBG_startEffectSound ln 513 EFCT num 102 final num 102 loopCount 4447</t>
+  </si>
+  <si>
+    <t>DEBUG loop() - nowVinputRBG 0x240 loopCount 4447</t>
+  </si>
+  <si>
+    <t>DEBUG loop() - nowVinputRBG 0x260 loopCount 6161</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> RBG_waitForInput mINP_TRIG mINP_BANY thisReturn 7 loopCount 6161</t>
+  </si>
+  <si>
+    <t>DEBUG RBG_processStateTable() - tmpVinputRBG 0x260 from row 5 foundInputRow 7 loopCount 6161</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> RBG_startEffectSound ln 513 EFCT num 0 final num 1 loopCount 6164</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> RBG_startEffectLED ln 457 EFCT num 0 final LED num 1 loopCount 6164</t>
+  </si>
+  <si>
+    <t>DEBUG RBG_processStateTable() - tmpVinputRBG 0x260 loopCount 6164</t>
+  </si>
+  <si>
+    <t>DEBUG loop() - nowVinputRBG 0x240 loopCount 6181</t>
+  </si>
+  <si>
+    <t>DEBUG loop() - nowVinputRBG 0x40 loopCount 9090</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> RBG_waitForInput mSPCL_EFCT_ONETIME thisReturn 8 loopCount 9090</t>
+  </si>
+  <si>
+    <t>DEBUG RBG_processStateTable() - tmpVinputRBG 0x40 from row 7 foundInputRow 8 loopCount 9090</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="17">
+  <fonts count="19">
     <font>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -9280,6 +9977,13 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="0"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -9469,28 +10173,28 @@
   </borders>
   <cellStyleXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="10" fillId="9" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="9" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="42">
+  <cellXfs count="46">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="2"/>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="3" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="2"/>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="3" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="2" xfId="3" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="2" xfId="3" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -9500,38 +10204,46 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" xfId="4"/>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" xfId="4" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" xfId="4"/>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" xfId="4" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="3"/>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="3"/>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="3" xfId="5"/>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="3" xfId="4" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="3" xfId="5"/>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="3" xfId="4" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="9" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="10" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="9" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="13" fillId="2" borderId="1" xfId="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="7"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="4" xfId="4" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="4" xfId="5" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="15" fillId="2" borderId="1" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="7"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="4" xfId="4" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="4" xfId="5" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="5" xfId="6" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="6" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="3" xfId="6" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="12" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="8">
     <cellStyle name="Bad" xfId="2" builtinId="27"/>
@@ -9857,7 +10569,7 @@
   <sheetViews>
     <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B23" sqref="B23"/>
+      <selection pane="bottomLeft" activeCell="I28" sqref="I28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
@@ -10408,11 +11120,11 @@
       </c>
       <c r="J24" s="9"/>
     </row>
-    <row r="25" spans="1:14">
-      <c r="F25" s="9"/>
-      <c r="G25" s="9"/>
-      <c r="H25" s="9"/>
-      <c r="I25" s="9"/>
+    <row r="25" spans="1:14" s="28" customFormat="1">
+      <c r="F25" s="42"/>
+      <c r="G25" s="42"/>
+      <c r="H25" s="42"/>
+      <c r="I25" s="42"/>
     </row>
     <row r="26" spans="1:14" ht="16">
       <c r="A26" s="9" t="s">
@@ -10454,14 +11166,32 @@
         <v>67</v>
       </c>
     </row>
-    <row r="28" spans="1:14">
+    <row r="28" spans="1:14" ht="16">
+      <c r="B28" s="9" t="s">
+        <v>2738</v>
+      </c>
+      <c r="C28" s="13" t="s">
+        <v>68</v>
+      </c>
+      <c r="D28" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="E28" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="F28" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="I28" s="9" t="s">
+        <v>77</v>
+      </c>
       <c r="N28" s="7"/>
     </row>
   </sheetData>
   <sortState ref="R3:R67">
     <sortCondition ref="R3:R67"/>
   </sortState>
-  <phoneticPr fontId="2" type="noConversion"/>
+  <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
@@ -10651,19 +11381,19 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F57F550E-21B4-4ED7-B7FF-211D228584A7}">
-  <dimension ref="A1:L2832"/>
+  <dimension ref="A1:L3109"/>
   <sheetViews>
-    <sheetView topLeftCell="A2810" workbookViewId="0">
-      <selection activeCell="C2807" sqref="C2807"/>
+    <sheetView tabSelected="1" topLeftCell="B2988" workbookViewId="0">
+      <selection activeCell="E3008" sqref="E3008"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <cols>
     <col min="2" max="2" width="84.6640625" customWidth="1"/>
     <col min="3" max="3" width="12.6640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="19.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="27" customWidth="1"/>
     <col min="5" max="5" width="12.1640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="180.5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="82.1640625" customWidth="1"/>
     <col min="7" max="7" width="16.5" customWidth="1"/>
   </cols>
   <sheetData>
@@ -32681,9 +33411,2587 @@
         <v>2861</v>
       </c>
     </row>
+    <row r="2834" spans="1:2" ht="16" thickBot="1"/>
+    <row r="2835" spans="1:2" ht="17" thickTop="1" thickBot="1">
+      <c r="B2835" s="1" t="s">
+        <v>3026</v>
+      </c>
+    </row>
+    <row r="2836" spans="1:2" ht="16" thickTop="1"/>
+    <row r="2837" spans="1:2">
+      <c r="B2837" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="2838" spans="1:2">
+      <c r="B2838" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="2839" spans="1:2">
+      <c r="B2839" t="s">
+        <v>911</v>
+      </c>
+    </row>
+    <row r="2840" spans="1:2">
+      <c r="B2840" t="s">
+        <v>912</v>
+      </c>
+    </row>
+    <row r="2841" spans="1:2">
+      <c r="B2841" t="s">
+        <v>2821</v>
+      </c>
+    </row>
+    <row r="2843" spans="1:2">
+      <c r="A2843" t="s">
+        <v>2081</v>
+      </c>
+      <c r="B2843" t="s">
+        <v>615</v>
+      </c>
+    </row>
+    <row r="2844" spans="1:2">
+      <c r="A2844">
+        <v>10</v>
+      </c>
+      <c r="B2844" s="27" t="s">
+        <v>2980</v>
+      </c>
+    </row>
+    <row r="2845" spans="1:2">
+      <c r="A2845">
+        <v>11</v>
+      </c>
+      <c r="B2845" s="16" t="s">
+        <v>3014</v>
+      </c>
+    </row>
+    <row r="2846" spans="1:2">
+      <c r="A2846">
+        <v>12</v>
+      </c>
+      <c r="B2846" t="s">
+        <v>3015</v>
+      </c>
+    </row>
+    <row r="2847" spans="1:2">
+      <c r="A2847">
+        <v>30</v>
+      </c>
+      <c r="B2847" s="12" t="s">
+        <v>3000</v>
+      </c>
+    </row>
+    <row r="2848" spans="1:2">
+      <c r="A2848">
+        <v>31</v>
+      </c>
+      <c r="B2848" s="27" t="s">
+        <v>2981</v>
+      </c>
+    </row>
+    <row r="2849" spans="1:2">
+      <c r="A2849">
+        <v>53</v>
+      </c>
+      <c r="B2849" s="12" t="s">
+        <v>3001</v>
+      </c>
+    </row>
+    <row r="2850" spans="1:2">
+      <c r="A2850">
+        <v>54</v>
+      </c>
+      <c r="B2850" s="16" t="s">
+        <v>3016</v>
+      </c>
+    </row>
+    <row r="2851" spans="1:2">
+      <c r="A2851">
+        <v>61</v>
+      </c>
+      <c r="B2851" s="27" t="s">
+        <v>2982</v>
+      </c>
+    </row>
+    <row r="2852" spans="1:2">
+      <c r="A2852">
+        <v>78</v>
+      </c>
+      <c r="B2852" s="16" t="s">
+        <v>3017</v>
+      </c>
+    </row>
+    <row r="2853" spans="1:2">
+      <c r="A2853">
+        <v>79</v>
+      </c>
+      <c r="B2853" s="27" t="s">
+        <v>2983</v>
+      </c>
+    </row>
+    <row r="2854" spans="1:2">
+      <c r="A2854">
+        <v>140</v>
+      </c>
+      <c r="B2854" s="27" t="s">
+        <v>2984</v>
+      </c>
+    </row>
+    <row r="2855" spans="1:2">
+      <c r="A2855">
+        <v>146</v>
+      </c>
+      <c r="B2855" s="12" t="s">
+        <v>3002</v>
+      </c>
+    </row>
+    <row r="2856" spans="1:2">
+      <c r="A2856">
+        <v>147</v>
+      </c>
+      <c r="B2856" s="16" t="s">
+        <v>3018</v>
+      </c>
+    </row>
+    <row r="2857" spans="1:2">
+      <c r="A2857">
+        <v>154</v>
+      </c>
+      <c r="B2857" s="27" t="s">
+        <v>2985</v>
+      </c>
+    </row>
+    <row r="2858" spans="1:2">
+      <c r="A2858">
+        <v>160</v>
+      </c>
+      <c r="B2858" s="12" t="s">
+        <v>3003</v>
+      </c>
+    </row>
+    <row r="2859" spans="1:2">
+      <c r="A2859">
+        <v>161</v>
+      </c>
+      <c r="B2859" s="27" t="s">
+        <v>2986</v>
+      </c>
+    </row>
+    <row r="2860" spans="1:2">
+      <c r="A2860">
+        <v>171</v>
+      </c>
+      <c r="B2860" s="12" t="s">
+        <v>3004</v>
+      </c>
+    </row>
+    <row r="2861" spans="1:2">
+      <c r="A2861">
+        <v>172</v>
+      </c>
+      <c r="B2861" s="27" t="s">
+        <v>2987</v>
+      </c>
+    </row>
+    <row r="2862" spans="1:2">
+      <c r="A2862">
+        <v>173</v>
+      </c>
+      <c r="B2862" s="16" t="s">
+        <v>3019</v>
+      </c>
+    </row>
+    <row r="2863" spans="1:2">
+      <c r="A2863">
+        <v>180</v>
+      </c>
+      <c r="B2863" s="27" t="s">
+        <v>2988</v>
+      </c>
+    </row>
+    <row r="2864" spans="1:2">
+      <c r="A2864">
+        <v>186</v>
+      </c>
+      <c r="B2864" s="12" t="s">
+        <v>3005</v>
+      </c>
+    </row>
+    <row r="2865" spans="1:2">
+      <c r="A2865">
+        <v>187</v>
+      </c>
+      <c r="B2865" s="27" t="s">
+        <v>2989</v>
+      </c>
+    </row>
+    <row r="2866" spans="1:2">
+      <c r="A2866">
+        <v>197</v>
+      </c>
+      <c r="B2866" s="12" t="s">
+        <v>3006</v>
+      </c>
+    </row>
+    <row r="2867" spans="1:2">
+      <c r="A2867">
+        <v>207</v>
+      </c>
+      <c r="B2867" s="12" t="s">
+        <v>3007</v>
+      </c>
+    </row>
+    <row r="2868" spans="1:2">
+      <c r="A2868">
+        <v>208</v>
+      </c>
+      <c r="B2868" s="16" t="s">
+        <v>3020</v>
+      </c>
+    </row>
+    <row r="2869" spans="1:2">
+      <c r="A2869">
+        <v>215</v>
+      </c>
+      <c r="B2869" s="27" t="s">
+        <v>2990</v>
+      </c>
+    </row>
+    <row r="2870" spans="1:2">
+      <c r="A2870">
+        <v>220</v>
+      </c>
+      <c r="B2870" s="16" t="s">
+        <v>3021</v>
+      </c>
+    </row>
+    <row r="2871" spans="1:2">
+      <c r="A2871">
+        <v>221</v>
+      </c>
+      <c r="B2871" s="27" t="s">
+        <v>2991</v>
+      </c>
+    </row>
+    <row r="2872" spans="1:2">
+      <c r="A2872">
+        <v>222</v>
+      </c>
+      <c r="B2872" s="27" t="s">
+        <v>2992</v>
+      </c>
+    </row>
+    <row r="2873" spans="1:2">
+      <c r="A2873">
+        <v>228</v>
+      </c>
+      <c r="B2873" s="12" t="s">
+        <v>3008</v>
+      </c>
+    </row>
+    <row r="2874" spans="1:2">
+      <c r="A2874">
+        <v>229</v>
+      </c>
+      <c r="B2874" s="16" t="s">
+        <v>3022</v>
+      </c>
+    </row>
+    <row r="2875" spans="1:2">
+      <c r="A2875">
+        <v>236</v>
+      </c>
+      <c r="B2875" s="27" t="s">
+        <v>2993</v>
+      </c>
+    </row>
+    <row r="2876" spans="1:2">
+      <c r="A2876">
+        <v>242</v>
+      </c>
+      <c r="B2876" s="12" t="s">
+        <v>3009</v>
+      </c>
+    </row>
+    <row r="2877" spans="1:2">
+      <c r="A2877">
+        <v>243</v>
+      </c>
+      <c r="B2877" s="27" t="s">
+        <v>2994</v>
+      </c>
+    </row>
+    <row r="2878" spans="1:2">
+      <c r="A2878">
+        <v>253</v>
+      </c>
+      <c r="B2878" s="12" t="s">
+        <v>3010</v>
+      </c>
+    </row>
+    <row r="2879" spans="1:2">
+      <c r="A2879">
+        <v>254</v>
+      </c>
+      <c r="B2879" s="27" t="s">
+        <v>2995</v>
+      </c>
+    </row>
+    <row r="2880" spans="1:2">
+      <c r="A2880">
+        <v>255</v>
+      </c>
+      <c r="B2880" s="16" t="s">
+        <v>3023</v>
+      </c>
+    </row>
+    <row r="2881" spans="1:2">
+      <c r="A2881">
+        <v>262</v>
+      </c>
+      <c r="B2881" s="27" t="s">
+        <v>2996</v>
+      </c>
+    </row>
+    <row r="2882" spans="1:2">
+      <c r="A2882">
+        <v>268</v>
+      </c>
+      <c r="B2882" s="12" t="s">
+        <v>3011</v>
+      </c>
+    </row>
+    <row r="2883" spans="1:2">
+      <c r="A2883">
+        <v>273</v>
+      </c>
+      <c r="B2883" s="27" t="s">
+        <v>2997</v>
+      </c>
+    </row>
+    <row r="2884" spans="1:2">
+      <c r="A2884">
+        <v>279</v>
+      </c>
+      <c r="B2884" s="12" t="s">
+        <v>3012</v>
+      </c>
+    </row>
+    <row r="2885" spans="1:2">
+      <c r="A2885">
+        <v>289</v>
+      </c>
+      <c r="B2885" s="12" t="s">
+        <v>3013</v>
+      </c>
+    </row>
+    <row r="2886" spans="1:2">
+      <c r="A2886">
+        <v>290</v>
+      </c>
+      <c r="B2886" s="16" t="s">
+        <v>3024</v>
+      </c>
+    </row>
+    <row r="2887" spans="1:2">
+      <c r="A2887">
+        <v>297</v>
+      </c>
+      <c r="B2887" s="27" t="s">
+        <v>2998</v>
+      </c>
+    </row>
+    <row r="2888" spans="1:2">
+      <c r="A2888">
+        <v>302</v>
+      </c>
+      <c r="B2888" s="16" t="s">
+        <v>3025</v>
+      </c>
+    </row>
+    <row r="2889" spans="1:2">
+      <c r="A2889">
+        <v>303</v>
+      </c>
+      <c r="B2889" s="27" t="s">
+        <v>2999</v>
+      </c>
+    </row>
+    <row r="2893" spans="1:2" ht="16" thickBot="1"/>
+    <row r="2894" spans="1:2" ht="17" thickTop="1" thickBot="1">
+      <c r="B2894" s="1" t="s">
+        <v>3026</v>
+      </c>
+    </row>
+    <row r="2895" spans="1:2" ht="16" thickTop="1"/>
+    <row r="2896" spans="1:2">
+      <c r="B2896" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="2897" spans="1:2">
+      <c r="B2897" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="2898" spans="1:2">
+      <c r="B2898" t="s">
+        <v>911</v>
+      </c>
+    </row>
+    <row r="2899" spans="1:2">
+      <c r="B2899" t="s">
+        <v>912</v>
+      </c>
+    </row>
+    <row r="2900" spans="1:2">
+      <c r="B2900" t="s">
+        <v>2821</v>
+      </c>
+    </row>
+    <row r="2902" spans="1:2">
+      <c r="A2902" t="s">
+        <v>2081</v>
+      </c>
+      <c r="B2902" t="s">
+        <v>615</v>
+      </c>
+    </row>
+    <row r="2903" spans="1:2">
+      <c r="A2903">
+        <v>10</v>
+      </c>
+      <c r="B2903" s="27" t="s">
+        <v>2980</v>
+      </c>
+    </row>
+    <row r="2904" spans="1:2">
+      <c r="A2904">
+        <v>11</v>
+      </c>
+      <c r="B2904" s="16" t="s">
+        <v>3014</v>
+      </c>
+    </row>
+    <row r="2905" spans="1:2">
+      <c r="A2905">
+        <v>12</v>
+      </c>
+      <c r="B2905" t="s">
+        <v>3015</v>
+      </c>
+    </row>
+    <row r="2906" spans="1:2">
+      <c r="A2906">
+        <v>30</v>
+      </c>
+      <c r="B2906" s="12" t="s">
+        <v>3000</v>
+      </c>
+    </row>
+    <row r="2907" spans="1:2">
+      <c r="A2907">
+        <v>31</v>
+      </c>
+      <c r="B2907" s="27" t="s">
+        <v>2981</v>
+      </c>
+    </row>
+    <row r="2908" spans="1:2">
+      <c r="A2908">
+        <v>53</v>
+      </c>
+      <c r="B2908" s="12" t="s">
+        <v>3001</v>
+      </c>
+    </row>
+    <row r="2909" spans="1:2">
+      <c r="A2909">
+        <v>54</v>
+      </c>
+      <c r="B2909" s="16" t="s">
+        <v>3016</v>
+      </c>
+    </row>
+    <row r="2910" spans="1:2">
+      <c r="A2910">
+        <v>61</v>
+      </c>
+      <c r="B2910" s="27" t="s">
+        <v>2982</v>
+      </c>
+    </row>
+    <row r="2911" spans="1:2">
+      <c r="A2911">
+        <v>78</v>
+      </c>
+      <c r="B2911" s="16" t="s">
+        <v>3017</v>
+      </c>
+    </row>
+    <row r="2912" spans="1:2">
+      <c r="A2912">
+        <v>79</v>
+      </c>
+      <c r="B2912" s="27" t="s">
+        <v>2983</v>
+      </c>
+    </row>
+    <row r="2913" spans="1:2">
+      <c r="A2913">
+        <v>704</v>
+      </c>
+      <c r="B2913" s="27" t="s">
+        <v>3027</v>
+      </c>
+    </row>
+    <row r="2914" spans="1:2">
+      <c r="A2914">
+        <v>718</v>
+      </c>
+      <c r="B2914" s="12" t="s">
+        <v>3028</v>
+      </c>
+    </row>
+    <row r="2915" spans="1:2">
+      <c r="A2915">
+        <v>719</v>
+      </c>
+      <c r="B2915" s="16" t="s">
+        <v>3029</v>
+      </c>
+    </row>
+    <row r="2916" spans="1:2">
+      <c r="A2916">
+        <v>726</v>
+      </c>
+      <c r="B2916" s="27" t="s">
+        <v>3030</v>
+      </c>
+    </row>
+    <row r="2917" spans="1:2">
+      <c r="A2917">
+        <v>738</v>
+      </c>
+      <c r="B2917" s="12" t="s">
+        <v>3031</v>
+      </c>
+    </row>
+    <row r="2918" spans="1:2">
+      <c r="A2918">
+        <v>739</v>
+      </c>
+      <c r="B2918" s="27" t="s">
+        <v>3032</v>
+      </c>
+    </row>
+    <row r="2919" spans="1:2">
+      <c r="A2919">
+        <v>755</v>
+      </c>
+      <c r="B2919" s="12" t="s">
+        <v>3033</v>
+      </c>
+    </row>
+    <row r="2920" spans="1:2">
+      <c r="A2920">
+        <v>756</v>
+      </c>
+      <c r="B2920" s="16" t="s">
+        <v>3034</v>
+      </c>
+    </row>
+    <row r="2921" spans="1:2">
+      <c r="A2921">
+        <v>763</v>
+      </c>
+      <c r="B2921" s="27" t="s">
+        <v>3035</v>
+      </c>
+    </row>
+    <row r="2922" spans="1:2">
+      <c r="A2922">
+        <v>775</v>
+      </c>
+      <c r="B2922" s="12" t="s">
+        <v>3036</v>
+      </c>
+    </row>
+    <row r="2923" spans="1:2">
+      <c r="A2923">
+        <v>776</v>
+      </c>
+      <c r="B2923" s="27" t="s">
+        <v>3037</v>
+      </c>
+    </row>
+    <row r="2924" spans="1:2">
+      <c r="A2924">
+        <v>792</v>
+      </c>
+      <c r="B2924" s="12" t="s">
+        <v>3038</v>
+      </c>
+    </row>
+    <row r="2925" spans="1:2">
+      <c r="A2925">
+        <v>814</v>
+      </c>
+      <c r="B2925" s="12" t="s">
+        <v>3039</v>
+      </c>
+    </row>
+    <row r="2926" spans="1:2">
+      <c r="A2926">
+        <v>815</v>
+      </c>
+      <c r="B2926" s="16" t="s">
+        <v>3040</v>
+      </c>
+    </row>
+    <row r="2927" spans="1:2">
+      <c r="A2927">
+        <v>822</v>
+      </c>
+      <c r="B2927" s="27" t="s">
+        <v>3041</v>
+      </c>
+    </row>
+    <row r="2928" spans="1:2">
+      <c r="A2928">
+        <v>839</v>
+      </c>
+      <c r="B2928" s="16" t="s">
+        <v>3042</v>
+      </c>
+    </row>
+    <row r="2929" spans="1:2">
+      <c r="A2929">
+        <v>840</v>
+      </c>
+      <c r="B2929" s="27" t="s">
+        <v>3043</v>
+      </c>
+    </row>
+    <row r="2930" spans="1:2">
+      <c r="A2930">
+        <v>1477</v>
+      </c>
+      <c r="B2930" s="27" t="s">
+        <v>3044</v>
+      </c>
+    </row>
+    <row r="2931" spans="1:2">
+      <c r="A2931">
+        <v>1491</v>
+      </c>
+      <c r="B2931" s="12" t="s">
+        <v>3045</v>
+      </c>
+    </row>
+    <row r="2932" spans="1:2">
+      <c r="A2932">
+        <v>1492</v>
+      </c>
+      <c r="B2932" s="16" t="s">
+        <v>3046</v>
+      </c>
+    </row>
+    <row r="2933" spans="1:2">
+      <c r="A2933">
+        <v>1511</v>
+      </c>
+      <c r="B2933" s="27" t="s">
+        <v>3047</v>
+      </c>
+    </row>
+    <row r="2935" spans="1:2" ht="16" thickBot="1"/>
+    <row r="2936" spans="1:2" ht="17" thickTop="1" thickBot="1">
+      <c r="B2936" s="1" t="s">
+        <v>3048</v>
+      </c>
+    </row>
+    <row r="2937" spans="1:2" ht="16" thickTop="1"/>
+    <row r="2938" spans="1:2">
+      <c r="B2938" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="2939" spans="1:2">
+      <c r="B2939" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="2940" spans="1:2">
+      <c r="B2940" t="s">
+        <v>911</v>
+      </c>
+    </row>
+    <row r="2941" spans="1:2">
+      <c r="B2941" t="s">
+        <v>912</v>
+      </c>
+    </row>
+    <row r="2942" spans="1:2">
+      <c r="B2942" t="s">
+        <v>2821</v>
+      </c>
+    </row>
+    <row r="2944" spans="1:2">
+      <c r="A2944" t="s">
+        <v>2081</v>
+      </c>
+      <c r="B2944" t="s">
+        <v>615</v>
+      </c>
+    </row>
+    <row r="2945" spans="1:2" ht="16">
+      <c r="A2945" s="43">
+        <v>10</v>
+      </c>
+      <c r="B2945" s="44" t="s">
+        <v>2980</v>
+      </c>
+    </row>
+    <row r="2946" spans="1:2" ht="16">
+      <c r="A2946" s="43">
+        <v>11</v>
+      </c>
+      <c r="B2946" s="16" t="s">
+        <v>3014</v>
+      </c>
+    </row>
+    <row r="2947" spans="1:2" ht="16">
+      <c r="A2947" s="43">
+        <v>12</v>
+      </c>
+      <c r="B2947" s="43" t="s">
+        <v>3015</v>
+      </c>
+    </row>
+    <row r="2948" spans="1:2" ht="16">
+      <c r="A2948" s="43">
+        <v>30</v>
+      </c>
+      <c r="B2948" s="12" t="s">
+        <v>3000</v>
+      </c>
+    </row>
+    <row r="2949" spans="1:2" ht="16">
+      <c r="A2949" s="43">
+        <v>31</v>
+      </c>
+      <c r="B2949" s="44" t="s">
+        <v>2981</v>
+      </c>
+    </row>
+    <row r="2950" spans="1:2" ht="16">
+      <c r="A2950" s="43">
+        <v>53</v>
+      </c>
+      <c r="B2950" s="12" t="s">
+        <v>3001</v>
+      </c>
+    </row>
+    <row r="2951" spans="1:2" ht="16">
+      <c r="A2951" s="43">
+        <v>54</v>
+      </c>
+      <c r="B2951" s="16" t="s">
+        <v>3016</v>
+      </c>
+    </row>
+    <row r="2952" spans="1:2" ht="16">
+      <c r="A2952" s="43">
+        <v>61</v>
+      </c>
+      <c r="B2952" s="44" t="s">
+        <v>2982</v>
+      </c>
+    </row>
+    <row r="2953" spans="1:2" ht="16">
+      <c r="A2953" s="43">
+        <v>78</v>
+      </c>
+      <c r="B2953" s="16" t="s">
+        <v>3017</v>
+      </c>
+    </row>
+    <row r="2954" spans="1:2" ht="16">
+      <c r="A2954" s="43">
+        <v>79</v>
+      </c>
+      <c r="B2954" s="44" t="s">
+        <v>2983</v>
+      </c>
+    </row>
+    <row r="2955" spans="1:2" ht="16">
+      <c r="A2955" s="43">
+        <v>1976</v>
+      </c>
+      <c r="B2955" s="44" t="s">
+        <v>3049</v>
+      </c>
+    </row>
+    <row r="2956" spans="1:2" ht="16">
+      <c r="A2956" s="43">
+        <v>1990</v>
+      </c>
+      <c r="B2956" s="12" t="s">
+        <v>3050</v>
+      </c>
+    </row>
+    <row r="2957" spans="1:2" ht="16">
+      <c r="A2957" s="43">
+        <v>1991</v>
+      </c>
+      <c r="B2957" s="16" t="s">
+        <v>3051</v>
+      </c>
+    </row>
+    <row r="2958" spans="1:2" ht="16">
+      <c r="A2958" s="43">
+        <v>1998</v>
+      </c>
+      <c r="B2958" s="44" t="s">
+        <v>3052</v>
+      </c>
+    </row>
+    <row r="2959" spans="1:2" ht="16">
+      <c r="A2959" s="43">
+        <v>2010</v>
+      </c>
+      <c r="B2959" s="12" t="s">
+        <v>3053</v>
+      </c>
+    </row>
+    <row r="2960" spans="1:2" ht="16">
+      <c r="A2960" s="43">
+        <v>2011</v>
+      </c>
+      <c r="B2960" s="44" t="s">
+        <v>3054</v>
+      </c>
+    </row>
+    <row r="2961" spans="1:2" ht="16">
+      <c r="A2961" s="43">
+        <v>2027</v>
+      </c>
+      <c r="B2961" s="12" t="s">
+        <v>3055</v>
+      </c>
+    </row>
+    <row r="2962" spans="1:2" ht="16">
+      <c r="A2962" s="43">
+        <v>2028</v>
+      </c>
+      <c r="B2962" s="16" t="s">
+        <v>3056</v>
+      </c>
+    </row>
+    <row r="2963" spans="1:2" ht="16">
+      <c r="A2963" s="43">
+        <v>2203</v>
+      </c>
+      <c r="B2963" s="44" t="s">
+        <v>3057</v>
+      </c>
+    </row>
+    <row r="2964" spans="1:2" ht="16">
+      <c r="A2964" s="43">
+        <v>2228</v>
+      </c>
+      <c r="B2964" s="44" t="s">
+        <v>3058</v>
+      </c>
+    </row>
+    <row r="2965" spans="1:2" ht="16">
+      <c r="A2965" s="43">
+        <v>2253</v>
+      </c>
+      <c r="B2965" s="44" t="s">
+        <v>3059</v>
+      </c>
+    </row>
+    <row r="2966" spans="1:2" ht="16">
+      <c r="A2966" s="43">
+        <v>2259</v>
+      </c>
+      <c r="B2966" s="12" t="s">
+        <v>3060</v>
+      </c>
+    </row>
+    <row r="2967" spans="1:2" ht="16">
+      <c r="A2967" s="43">
+        <v>2269</v>
+      </c>
+      <c r="B2967" s="12" t="s">
+        <v>3061</v>
+      </c>
+    </row>
+    <row r="2968" spans="1:2" ht="16">
+      <c r="A2968" s="43">
+        <v>2279</v>
+      </c>
+      <c r="B2968" s="12" t="s">
+        <v>3062</v>
+      </c>
+    </row>
+    <row r="2969" spans="1:2" ht="16">
+      <c r="A2969" s="43">
+        <v>2280</v>
+      </c>
+      <c r="B2969" s="16" t="s">
+        <v>3063</v>
+      </c>
+    </row>
+    <row r="2970" spans="1:2" ht="16">
+      <c r="A2970" s="43">
+        <v>2281</v>
+      </c>
+      <c r="B2970" s="43" t="s">
+        <v>3064</v>
+      </c>
+    </row>
+    <row r="2971" spans="1:2" ht="16">
+      <c r="A2971" s="43">
+        <v>2289</v>
+      </c>
+      <c r="B2971" s="44" t="s">
+        <v>3065</v>
+      </c>
+    </row>
+    <row r="2973" spans="1:2" ht="16" thickBot="1"/>
+    <row r="2974" spans="1:2" ht="17" thickTop="1" thickBot="1">
+      <c r="B2974" s="1" t="s">
+        <v>3066</v>
+      </c>
+    </row>
+    <row r="2975" spans="1:2" ht="16" thickTop="1"/>
+    <row r="2976" spans="1:2">
+      <c r="B2976" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="2977" spans="1:4">
+      <c r="B2977" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="2978" spans="1:4">
+      <c r="B2978" t="s">
+        <v>911</v>
+      </c>
+    </row>
+    <row r="2979" spans="1:4">
+      <c r="B2979" t="s">
+        <v>912</v>
+      </c>
+    </row>
+    <row r="2980" spans="1:4">
+      <c r="B2980" t="s">
+        <v>2821</v>
+      </c>
+    </row>
+    <row r="2982" spans="1:4">
+      <c r="A2982" t="s">
+        <v>2081</v>
+      </c>
+      <c r="B2982" t="s">
+        <v>615</v>
+      </c>
+    </row>
+    <row r="2983" spans="1:4">
+      <c r="A2983">
+        <v>10</v>
+      </c>
+      <c r="B2983" s="27" t="s">
+        <v>2980</v>
+      </c>
+    </row>
+    <row r="2984" spans="1:4">
+      <c r="A2984">
+        <v>11</v>
+      </c>
+      <c r="B2984" s="16" t="s">
+        <v>3014</v>
+      </c>
+      <c r="C2984" t="s">
+        <v>3147</v>
+      </c>
+    </row>
+    <row r="2985" spans="1:4">
+      <c r="A2985">
+        <v>12</v>
+      </c>
+      <c r="B2985" t="s">
+        <v>3067</v>
+      </c>
+    </row>
+    <row r="2986" spans="1:4">
+      <c r="A2986">
+        <v>19</v>
+      </c>
+      <c r="B2986" s="27" t="s">
+        <v>3068</v>
+      </c>
+    </row>
+    <row r="2987" spans="1:4">
+      <c r="A2987">
+        <v>752</v>
+      </c>
+      <c r="B2987" s="27" t="s">
+        <v>3069</v>
+      </c>
+      <c r="C2987" t="s">
+        <v>3147</v>
+      </c>
+    </row>
+    <row r="2988" spans="1:4">
+      <c r="A2988">
+        <v>764</v>
+      </c>
+      <c r="B2988" s="12" t="s">
+        <v>3070</v>
+      </c>
+      <c r="D2988" t="s">
+        <v>2672</v>
+      </c>
+    </row>
+    <row r="2989" spans="1:4">
+      <c r="A2989">
+        <v>786</v>
+      </c>
+      <c r="B2989" s="12" t="s">
+        <v>3071</v>
+      </c>
+      <c r="D2989" t="s">
+        <v>2674</v>
+      </c>
+    </row>
+    <row r="2990" spans="1:4">
+      <c r="A2990">
+        <v>787</v>
+      </c>
+      <c r="B2990" s="16" t="s">
+        <v>3072</v>
+      </c>
+      <c r="C2990" t="s">
+        <v>3147</v>
+      </c>
+    </row>
+    <row r="2991" spans="1:4">
+      <c r="A2991">
+        <v>788</v>
+      </c>
+      <c r="B2991" t="s">
+        <v>3073</v>
+      </c>
+    </row>
+    <row r="2992" spans="1:4">
+      <c r="A2992">
+        <v>795</v>
+      </c>
+      <c r="B2992" s="27" t="s">
+        <v>3074</v>
+      </c>
+    </row>
+    <row r="2993" spans="1:7">
+      <c r="A2993">
+        <v>1708</v>
+      </c>
+      <c r="B2993" s="27" t="s">
+        <v>3075</v>
+      </c>
+      <c r="E2993" t="s">
+        <v>3149</v>
+      </c>
+      <c r="F2993" s="27" t="s">
+        <v>3152</v>
+      </c>
+      <c r="G2993">
+        <v>1708</v>
+      </c>
+    </row>
+    <row r="2994" spans="1:7">
+      <c r="A2994">
+        <v>1714</v>
+      </c>
+      <c r="B2994" s="12" t="s">
+        <v>3076</v>
+      </c>
+      <c r="D2994" t="s">
+        <v>2675</v>
+      </c>
+      <c r="E2994" t="s">
+        <v>3149</v>
+      </c>
+      <c r="F2994" t="s">
+        <v>3153</v>
+      </c>
+      <c r="G2994">
+        <v>1709</v>
+      </c>
+    </row>
+    <row r="2995" spans="1:7">
+      <c r="A2995">
+        <v>1715</v>
+      </c>
+      <c r="B2995" s="16" t="s">
+        <v>3077</v>
+      </c>
+      <c r="C2995" s="4" t="s">
+        <v>3148</v>
+      </c>
+      <c r="E2995" t="s">
+        <v>3149</v>
+      </c>
+      <c r="F2995" t="s">
+        <v>3154</v>
+      </c>
+      <c r="G2995">
+        <v>1710</v>
+      </c>
+    </row>
+    <row r="2996" spans="1:7">
+      <c r="A2996">
+        <v>1716</v>
+      </c>
+      <c r="B2996" t="s">
+        <v>3078</v>
+      </c>
+      <c r="E2996" t="s">
+        <v>3149</v>
+      </c>
+      <c r="F2996" t="s">
+        <v>2443</v>
+      </c>
+      <c r="G2996">
+        <v>1711</v>
+      </c>
+    </row>
+    <row r="2997" spans="1:7">
+      <c r="A2997">
+        <v>1723</v>
+      </c>
+      <c r="B2997" s="27" t="s">
+        <v>3079</v>
+      </c>
+      <c r="C2997" s="4" t="s">
+        <v>3148</v>
+      </c>
+      <c r="E2997" t="s">
+        <v>3149</v>
+      </c>
+      <c r="F2997" t="s">
+        <v>2444</v>
+      </c>
+      <c r="G2997">
+        <v>1712</v>
+      </c>
+    </row>
+    <row r="2998" spans="1:7">
+      <c r="A2998">
+        <v>1729</v>
+      </c>
+      <c r="B2998" s="12" t="s">
+        <v>3080</v>
+      </c>
+      <c r="D2998" t="s">
+        <v>2676</v>
+      </c>
+      <c r="E2998" t="s">
+        <v>3149</v>
+      </c>
+      <c r="F2998" t="s">
+        <v>3155</v>
+      </c>
+      <c r="G2998">
+        <v>1713</v>
+      </c>
+    </row>
+    <row r="2999" spans="1:7">
+      <c r="A2999">
+        <v>1730</v>
+      </c>
+      <c r="B2999" s="27" t="s">
+        <v>3081</v>
+      </c>
+      <c r="E2999" t="s">
+        <v>3149</v>
+      </c>
+      <c r="F2999" t="s">
+        <v>3156</v>
+      </c>
+      <c r="G2999">
+        <v>1714</v>
+      </c>
+    </row>
+    <row r="3000" spans="1:7">
+      <c r="A3000">
+        <v>1735</v>
+      </c>
+      <c r="B3000" s="27" t="s">
+        <v>3082</v>
+      </c>
+      <c r="E3000" t="s">
+        <v>3149</v>
+      </c>
+      <c r="F3000" s="16" t="s">
+        <v>3157</v>
+      </c>
+      <c r="G3000">
+        <v>1715</v>
+      </c>
+    </row>
+    <row r="3001" spans="1:7">
+      <c r="A3001">
+        <v>1741</v>
+      </c>
+      <c r="B3001" s="12" t="s">
+        <v>3083</v>
+      </c>
+      <c r="D3001" t="s">
+        <v>2677</v>
+      </c>
+      <c r="E3001" t="s">
+        <v>3149</v>
+      </c>
+      <c r="F3001" t="s">
+        <v>3158</v>
+      </c>
+      <c r="G3001">
+        <v>1716</v>
+      </c>
+    </row>
+    <row r="3002" spans="1:7">
+      <c r="A3002">
+        <v>1742</v>
+      </c>
+      <c r="B3002" s="16" t="s">
+        <v>3084</v>
+      </c>
+      <c r="C3002" s="4" t="s">
+        <v>3148</v>
+      </c>
+      <c r="E3002" t="s">
+        <v>3149</v>
+      </c>
+      <c r="F3002" t="s">
+        <v>3159</v>
+      </c>
+      <c r="G3002">
+        <v>1717</v>
+      </c>
+    </row>
+    <row r="3003" spans="1:7">
+      <c r="A3003">
+        <v>1743</v>
+      </c>
+      <c r="B3003" t="s">
+        <v>3085</v>
+      </c>
+      <c r="E3003" t="s">
+        <v>3149</v>
+      </c>
+      <c r="F3003" t="s">
+        <v>2453</v>
+      </c>
+      <c r="G3003">
+        <v>1718</v>
+      </c>
+    </row>
+    <row r="3004" spans="1:7">
+      <c r="A3004">
+        <v>1750</v>
+      </c>
+      <c r="B3004" s="27" t="s">
+        <v>3086</v>
+      </c>
+      <c r="C3004" s="4" t="s">
+        <v>3148</v>
+      </c>
+      <c r="E3004" t="s">
+        <v>3151</v>
+      </c>
+      <c r="F3004" t="s">
+        <v>2443</v>
+      </c>
+      <c r="G3004">
+        <v>1719</v>
+      </c>
+    </row>
+    <row r="3005" spans="1:7">
+      <c r="A3005">
+        <v>1756</v>
+      </c>
+      <c r="B3005" s="12" t="s">
+        <v>3087</v>
+      </c>
+      <c r="D3005" t="s">
+        <v>2678</v>
+      </c>
+      <c r="F3005" t="s">
+        <v>3160</v>
+      </c>
+      <c r="G3005">
+        <v>1720</v>
+      </c>
+    </row>
+    <row r="3006" spans="1:7">
+      <c r="A3006">
+        <v>1757</v>
+      </c>
+      <c r="B3006" s="27" t="s">
+        <v>3088</v>
+      </c>
+      <c r="C3006" s="4" t="s">
+        <v>3148</v>
+      </c>
+      <c r="F3006" t="s">
+        <v>3155</v>
+      </c>
+      <c r="G3006">
+        <v>1721</v>
+      </c>
+    </row>
+    <row r="3007" spans="1:7">
+      <c r="A3007">
+        <v>1767</v>
+      </c>
+      <c r="B3007" s="12" t="s">
+        <v>3089</v>
+      </c>
+      <c r="D3007" t="s">
+        <v>2672</v>
+      </c>
+      <c r="F3007" t="s">
+        <v>3161</v>
+      </c>
+      <c r="G3007">
+        <v>1722</v>
+      </c>
+    </row>
+    <row r="3008" spans="1:7">
+      <c r="A3008">
+        <v>1777</v>
+      </c>
+      <c r="B3008" s="12" t="s">
+        <v>3090</v>
+      </c>
+      <c r="D3008" t="s">
+        <v>2674</v>
+      </c>
+      <c r="F3008" s="27" t="s">
+        <v>3162</v>
+      </c>
+      <c r="G3008" s="4">
+        <v>1723</v>
+      </c>
+    </row>
+    <row r="3009" spans="1:7">
+      <c r="A3009">
+        <v>1778</v>
+      </c>
+      <c r="B3009" s="16" t="s">
+        <v>3091</v>
+      </c>
+      <c r="F3009" t="s">
+        <v>3163</v>
+      </c>
+      <c r="G3009">
+        <v>1724</v>
+      </c>
+    </row>
+    <row r="3010" spans="1:7">
+      <c r="A3010">
+        <v>1779</v>
+      </c>
+      <c r="B3010" t="s">
+        <v>3092</v>
+      </c>
+      <c r="F3010" t="s">
+        <v>3154</v>
+      </c>
+      <c r="G3010">
+        <v>1725</v>
+      </c>
+    </row>
+    <row r="3011" spans="1:7">
+      <c r="A3011">
+        <v>1786</v>
+      </c>
+      <c r="B3011" s="27" t="s">
+        <v>3093</v>
+      </c>
+      <c r="C3011" s="4" t="s">
+        <v>3148</v>
+      </c>
+      <c r="F3011" t="s">
+        <v>2443</v>
+      </c>
+      <c r="G3011">
+        <v>1726</v>
+      </c>
+    </row>
+    <row r="3012" spans="1:7">
+      <c r="A3012">
+        <v>1791</v>
+      </c>
+      <c r="B3012" s="16" t="s">
+        <v>3094</v>
+      </c>
+      <c r="F3012" t="s">
+        <v>3160</v>
+      </c>
+      <c r="G3012">
+        <v>1727</v>
+      </c>
+    </row>
+    <row r="3013" spans="1:7">
+      <c r="A3013">
+        <v>1792</v>
+      </c>
+      <c r="B3013" t="s">
+        <v>3095</v>
+      </c>
+      <c r="F3013" t="s">
+        <v>3155</v>
+      </c>
+      <c r="G3013">
+        <v>1728</v>
+      </c>
+    </row>
+    <row r="3014" spans="1:7">
+      <c r="A3014">
+        <v>1793</v>
+      </c>
+      <c r="B3014" s="27" t="s">
+        <v>3096</v>
+      </c>
+      <c r="F3014" t="s">
+        <v>3164</v>
+      </c>
+      <c r="G3014">
+        <v>1729</v>
+      </c>
+    </row>
+    <row r="3015" spans="1:7">
+      <c r="A3015">
+        <v>1794</v>
+      </c>
+      <c r="B3015" s="27" t="s">
+        <v>3097</v>
+      </c>
+      <c r="F3015" s="27" t="s">
+        <v>3165</v>
+      </c>
+      <c r="G3015">
+        <v>1730</v>
+      </c>
+    </row>
+    <row r="3016" spans="1:7">
+      <c r="A3016">
+        <v>1799</v>
+      </c>
+      <c r="B3016" s="16" t="s">
+        <v>3098</v>
+      </c>
+      <c r="F3016" t="s">
+        <v>2443</v>
+      </c>
+      <c r="G3016">
+        <v>1731</v>
+      </c>
+    </row>
+    <row r="3017" spans="1:7">
+      <c r="A3017">
+        <v>1800</v>
+      </c>
+      <c r="B3017" t="s">
+        <v>3099</v>
+      </c>
+      <c r="F3017" t="s">
+        <v>3166</v>
+      </c>
+      <c r="G3017">
+        <v>1732</v>
+      </c>
+    </row>
+    <row r="3018" spans="1:7">
+      <c r="A3018">
+        <v>1801</v>
+      </c>
+      <c r="B3018" s="27" t="s">
+        <v>3100</v>
+      </c>
+      <c r="F3018" t="s">
+        <v>3155</v>
+      </c>
+      <c r="G3018">
+        <v>1733</v>
+      </c>
+    </row>
+    <row r="3019" spans="1:7">
+      <c r="A3019">
+        <v>1802</v>
+      </c>
+      <c r="B3019" s="27" t="s">
+        <v>3101</v>
+      </c>
+      <c r="E3019" t="s">
+        <v>3149</v>
+      </c>
+      <c r="F3019" t="s">
+        <v>3167</v>
+      </c>
+      <c r="G3019">
+        <v>1734</v>
+      </c>
+    </row>
+    <row r="3020" spans="1:7">
+      <c r="A3020">
+        <v>1808</v>
+      </c>
+      <c r="B3020" s="12" t="s">
+        <v>3102</v>
+      </c>
+      <c r="D3020" t="s">
+        <v>2675</v>
+      </c>
+      <c r="E3020" t="s">
+        <v>3149</v>
+      </c>
+      <c r="F3020" s="27" t="s">
+        <v>3168</v>
+      </c>
+      <c r="G3020">
+        <v>1735</v>
+      </c>
+    </row>
+    <row r="3021" spans="1:7">
+      <c r="A3021">
+        <v>1809</v>
+      </c>
+      <c r="B3021" s="16" t="s">
+        <v>3103</v>
+      </c>
+      <c r="E3021" t="s">
+        <v>3149</v>
+      </c>
+      <c r="F3021" t="s">
+        <v>3169</v>
+      </c>
+      <c r="G3021">
+        <v>1736</v>
+      </c>
+    </row>
+    <row r="3022" spans="1:7">
+      <c r="A3022">
+        <v>1810</v>
+      </c>
+      <c r="B3022" t="s">
+        <v>3104</v>
+      </c>
+      <c r="E3022" t="s">
+        <v>3149</v>
+      </c>
+      <c r="F3022" t="s">
+        <v>3154</v>
+      </c>
+      <c r="G3022">
+        <v>1737</v>
+      </c>
+    </row>
+    <row r="3023" spans="1:7">
+      <c r="A3023">
+        <v>1817</v>
+      </c>
+      <c r="B3023" s="27" t="s">
+        <v>3105</v>
+      </c>
+      <c r="E3023" t="s">
+        <v>3150</v>
+      </c>
+      <c r="F3023" s="45" t="s">
+        <v>2443</v>
+      </c>
+      <c r="G3023">
+        <v>1738</v>
+      </c>
+    </row>
+    <row r="3024" spans="1:7">
+      <c r="A3024">
+        <v>1818</v>
+      </c>
+      <c r="B3024" s="27" t="s">
+        <v>3106</v>
+      </c>
+      <c r="F3024" t="s">
+        <v>3166</v>
+      </c>
+      <c r="G3024">
+        <v>1739</v>
+      </c>
+    </row>
+    <row r="3025" spans="1:7">
+      <c r="A3025">
+        <v>1824</v>
+      </c>
+      <c r="B3025" s="12" t="s">
+        <v>3107</v>
+      </c>
+      <c r="D3025" t="s">
+        <v>2676</v>
+      </c>
+      <c r="F3025" t="s">
+        <v>3155</v>
+      </c>
+      <c r="G3025">
+        <v>1740</v>
+      </c>
+    </row>
+    <row r="3026" spans="1:7">
+      <c r="A3026">
+        <v>1834</v>
+      </c>
+      <c r="B3026" s="12" t="s">
+        <v>3108</v>
+      </c>
+      <c r="D3026" t="s">
+        <v>2677</v>
+      </c>
+      <c r="F3026" t="s">
+        <v>3170</v>
+      </c>
+      <c r="G3026">
+        <v>1741</v>
+      </c>
+    </row>
+    <row r="3027" spans="1:7">
+      <c r="A3027">
+        <v>1835</v>
+      </c>
+      <c r="B3027" s="16" t="s">
+        <v>3109</v>
+      </c>
+      <c r="F3027" s="16" t="s">
+        <v>3171</v>
+      </c>
+      <c r="G3027">
+        <v>1742</v>
+      </c>
+    </row>
+    <row r="3028" spans="1:7">
+      <c r="A3028">
+        <v>1836</v>
+      </c>
+      <c r="B3028" t="s">
+        <v>3110</v>
+      </c>
+      <c r="F3028" t="s">
+        <v>3158</v>
+      </c>
+      <c r="G3028">
+        <v>1743</v>
+      </c>
+    </row>
+    <row r="3029" spans="1:7">
+      <c r="A3029">
+        <v>1843</v>
+      </c>
+      <c r="B3029" s="27" t="s">
+        <v>3111</v>
+      </c>
+      <c r="F3029" t="s">
+        <v>3172</v>
+      </c>
+      <c r="G3029">
+        <v>1744</v>
+      </c>
+    </row>
+    <row r="3030" spans="1:7">
+      <c r="A3030">
+        <v>1844</v>
+      </c>
+      <c r="B3030" s="27" t="s">
+        <v>3112</v>
+      </c>
+      <c r="F3030" t="s">
+        <v>2453</v>
+      </c>
+      <c r="G3030">
+        <v>1745</v>
+      </c>
+    </row>
+    <row r="3031" spans="1:7">
+      <c r="A3031">
+        <v>1850</v>
+      </c>
+      <c r="B3031" s="12" t="s">
+        <v>3113</v>
+      </c>
+      <c r="D3031" t="s">
+        <v>2678</v>
+      </c>
+      <c r="F3031" t="s">
+        <v>2443</v>
+      </c>
+      <c r="G3031">
+        <v>1746</v>
+      </c>
+    </row>
+    <row r="3032" spans="1:7">
+      <c r="A3032">
+        <v>1860</v>
+      </c>
+      <c r="B3032" s="12" t="s">
+        <v>3114</v>
+      </c>
+      <c r="D3032" t="s">
+        <v>2672</v>
+      </c>
+      <c r="F3032" t="s">
+        <v>3173</v>
+      </c>
+      <c r="G3032">
+        <v>1747</v>
+      </c>
+    </row>
+    <row r="3033" spans="1:7">
+      <c r="A3033">
+        <v>1870</v>
+      </c>
+      <c r="B3033" s="12" t="s">
+        <v>3115</v>
+      </c>
+      <c r="D3033" t="s">
+        <v>2674</v>
+      </c>
+      <c r="F3033" t="s">
+        <v>3155</v>
+      </c>
+      <c r="G3033">
+        <v>1748</v>
+      </c>
+    </row>
+    <row r="3034" spans="1:7">
+      <c r="A3034">
+        <v>1871</v>
+      </c>
+      <c r="B3034" s="16" t="s">
+        <v>3116</v>
+      </c>
+      <c r="F3034" t="s">
+        <v>3174</v>
+      </c>
+      <c r="G3034">
+        <v>1749</v>
+      </c>
+    </row>
+    <row r="3035" spans="1:7">
+      <c r="A3035">
+        <v>1872</v>
+      </c>
+      <c r="B3035" t="s">
+        <v>3117</v>
+      </c>
+      <c r="F3035" s="27" t="s">
+        <v>3175</v>
+      </c>
+      <c r="G3035">
+        <v>1750</v>
+      </c>
+    </row>
+    <row r="3036" spans="1:7">
+      <c r="A3036">
+        <v>1879</v>
+      </c>
+      <c r="B3036" s="27" t="s">
+        <v>3118</v>
+      </c>
+      <c r="F3036" t="s">
+        <v>3176</v>
+      </c>
+      <c r="G3036">
+        <v>1751</v>
+      </c>
+    </row>
+    <row r="3037" spans="1:7">
+      <c r="A3037">
+        <v>1880</v>
+      </c>
+      <c r="B3037" s="27" t="s">
+        <v>3119</v>
+      </c>
+      <c r="F3037" t="s">
+        <v>3154</v>
+      </c>
+      <c r="G3037">
+        <v>1752</v>
+      </c>
+    </row>
+    <row r="3038" spans="1:7">
+      <c r="A3038">
+        <v>1886</v>
+      </c>
+      <c r="B3038" s="12" t="s">
+        <v>3120</v>
+      </c>
+      <c r="D3038" t="s">
+        <v>2679</v>
+      </c>
+      <c r="F3038" t="s">
+        <v>2443</v>
+      </c>
+      <c r="G3038">
+        <v>1753</v>
+      </c>
+    </row>
+    <row r="3039" spans="1:7">
+      <c r="A3039">
+        <v>1887</v>
+      </c>
+      <c r="B3039" s="16" t="s">
+        <v>3121</v>
+      </c>
+      <c r="F3039" t="s">
+        <v>3173</v>
+      </c>
+      <c r="G3039">
+        <v>1754</v>
+      </c>
+    </row>
+    <row r="3040" spans="1:7">
+      <c r="A3040">
+        <v>1888</v>
+      </c>
+      <c r="B3040" t="s">
+        <v>3122</v>
+      </c>
+      <c r="F3040" t="s">
+        <v>3155</v>
+      </c>
+      <c r="G3040">
+        <v>1755</v>
+      </c>
+    </row>
+    <row r="3041" spans="1:7">
+      <c r="A3041">
+        <v>1895</v>
+      </c>
+      <c r="B3041" s="27" t="s">
+        <v>3123</v>
+      </c>
+      <c r="F3041" t="s">
+        <v>3177</v>
+      </c>
+      <c r="G3041">
+        <v>1756</v>
+      </c>
+    </row>
+    <row r="3042" spans="1:7">
+      <c r="A3042">
+        <v>1901</v>
+      </c>
+      <c r="B3042" s="12" t="s">
+        <v>3124</v>
+      </c>
+      <c r="D3042" t="s">
+        <v>2672</v>
+      </c>
+      <c r="F3042" s="27" t="s">
+        <v>3178</v>
+      </c>
+      <c r="G3042">
+        <v>1757</v>
+      </c>
+    </row>
+    <row r="3043" spans="1:7">
+      <c r="A3043">
+        <v>1902</v>
+      </c>
+      <c r="B3043" s="27" t="s">
+        <v>3125</v>
+      </c>
+      <c r="F3043" t="s">
+        <v>2443</v>
+      </c>
+      <c r="G3043">
+        <v>1758</v>
+      </c>
+    </row>
+    <row r="3044" spans="1:7">
+      <c r="A3044">
+        <v>1912</v>
+      </c>
+      <c r="B3044" s="12" t="s">
+        <v>3126</v>
+      </c>
+      <c r="D3044" t="s">
+        <v>2673</v>
+      </c>
+      <c r="F3044" t="s">
+        <v>3179</v>
+      </c>
+      <c r="G3044">
+        <v>1759</v>
+      </c>
+    </row>
+    <row r="3045" spans="1:7">
+      <c r="A3045">
+        <v>1913</v>
+      </c>
+      <c r="B3045" s="16" t="s">
+        <v>3127</v>
+      </c>
+      <c r="F3045" t="s">
+        <v>3155</v>
+      </c>
+      <c r="G3045">
+        <v>1760</v>
+      </c>
+    </row>
+    <row r="3046" spans="1:7">
+      <c r="A3046">
+        <v>1914</v>
+      </c>
+      <c r="B3046" t="s">
+        <v>3128</v>
+      </c>
+      <c r="F3046" t="s">
+        <v>3180</v>
+      </c>
+      <c r="G3046">
+        <v>1761</v>
+      </c>
+    </row>
+    <row r="3047" spans="1:7">
+      <c r="A3047">
+        <v>1921</v>
+      </c>
+      <c r="B3047" s="27" t="s">
+        <v>3129</v>
+      </c>
+      <c r="F3047" t="s">
+        <v>3181</v>
+      </c>
+      <c r="G3047">
+        <v>1762</v>
+      </c>
+    </row>
+    <row r="3048" spans="1:7">
+      <c r="A3048">
+        <v>1926</v>
+      </c>
+      <c r="B3048" s="16" t="s">
+        <v>3130</v>
+      </c>
+      <c r="F3048" t="s">
+        <v>3154</v>
+      </c>
+      <c r="G3048">
+        <v>1763</v>
+      </c>
+    </row>
+    <row r="3049" spans="1:7">
+      <c r="A3049">
+        <v>1927</v>
+      </c>
+      <c r="B3049" t="s">
+        <v>3131</v>
+      </c>
+      <c r="F3049" t="s">
+        <v>2443</v>
+      </c>
+      <c r="G3049">
+        <v>1764</v>
+      </c>
+    </row>
+    <row r="3050" spans="1:7">
+      <c r="A3050">
+        <v>1928</v>
+      </c>
+      <c r="B3050" s="27" t="s">
+        <v>3132</v>
+      </c>
+      <c r="F3050" t="s">
+        <v>3179</v>
+      </c>
+      <c r="G3050">
+        <v>1765</v>
+      </c>
+    </row>
+    <row r="3051" spans="1:7">
+      <c r="A3051">
+        <v>1929</v>
+      </c>
+      <c r="B3051" s="27" t="s">
+        <v>3133</v>
+      </c>
+      <c r="F3051" t="s">
+        <v>3155</v>
+      </c>
+      <c r="G3051">
+        <v>1766</v>
+      </c>
+    </row>
+    <row r="3052" spans="1:7">
+      <c r="A3052">
+        <v>1935</v>
+      </c>
+      <c r="B3052" s="12" t="s">
+        <v>3134</v>
+      </c>
+      <c r="D3052" t="s">
+        <v>2725</v>
+      </c>
+      <c r="F3052" t="s">
+        <v>3182</v>
+      </c>
+      <c r="G3052">
+        <v>1767</v>
+      </c>
+    </row>
+    <row r="3053" spans="1:7">
+      <c r="A3053">
+        <v>1936</v>
+      </c>
+      <c r="B3053" s="16" t="s">
+        <v>3135</v>
+      </c>
+      <c r="F3053" t="s">
+        <v>2443</v>
+      </c>
+      <c r="G3053">
+        <v>1768</v>
+      </c>
+    </row>
+    <row r="3054" spans="1:7">
+      <c r="A3054">
+        <v>1937</v>
+      </c>
+      <c r="B3054" t="s">
+        <v>3136</v>
+      </c>
+      <c r="F3054" t="s">
+        <v>3183</v>
+      </c>
+      <c r="G3054">
+        <v>1769</v>
+      </c>
+    </row>
+    <row r="3055" spans="1:7">
+      <c r="A3055">
+        <v>1944</v>
+      </c>
+      <c r="B3055" s="27" t="s">
+        <v>3137</v>
+      </c>
+      <c r="F3055" t="s">
+        <v>3155</v>
+      </c>
+      <c r="G3055">
+        <v>1770</v>
+      </c>
+    </row>
+    <row r="3056" spans="1:7">
+      <c r="A3056">
+        <v>1950</v>
+      </c>
+      <c r="B3056" s="12" t="s">
+        <v>3138</v>
+      </c>
+      <c r="D3056" t="s">
+        <v>2672</v>
+      </c>
+      <c r="F3056" t="s">
+        <v>3184</v>
+      </c>
+      <c r="G3056">
+        <v>1771</v>
+      </c>
+    </row>
+    <row r="3057" spans="1:7">
+      <c r="A3057">
+        <v>1951</v>
+      </c>
+      <c r="B3057" s="27" t="s">
+        <v>3139</v>
+      </c>
+      <c r="F3057" t="s">
+        <v>3185</v>
+      </c>
+      <c r="G3057">
+        <v>1772</v>
+      </c>
+    </row>
+    <row r="3058" spans="1:7">
+      <c r="A3058">
+        <v>1961</v>
+      </c>
+      <c r="B3058" s="12" t="s">
+        <v>3140</v>
+      </c>
+      <c r="D3058" t="s">
+        <v>2674</v>
+      </c>
+      <c r="F3058" t="s">
+        <v>3154</v>
+      </c>
+      <c r="G3058">
+        <v>1773</v>
+      </c>
+    </row>
+    <row r="3059" spans="1:7">
+      <c r="A3059">
+        <v>1962</v>
+      </c>
+      <c r="B3059" s="16" t="s">
+        <v>3141</v>
+      </c>
+      <c r="F3059" t="s">
+        <v>2443</v>
+      </c>
+      <c r="G3059">
+        <v>1774</v>
+      </c>
+    </row>
+    <row r="3060" spans="1:7">
+      <c r="A3060">
+        <v>1963</v>
+      </c>
+      <c r="B3060" t="s">
+        <v>3142</v>
+      </c>
+      <c r="F3060" t="s">
+        <v>3183</v>
+      </c>
+      <c r="G3060">
+        <v>1775</v>
+      </c>
+    </row>
+    <row r="3061" spans="1:7">
+      <c r="A3061">
+        <v>1970</v>
+      </c>
+      <c r="B3061" s="27" t="s">
+        <v>3143</v>
+      </c>
+      <c r="F3061" t="s">
+        <v>3155</v>
+      </c>
+      <c r="G3061">
+        <v>1776</v>
+      </c>
+    </row>
+    <row r="3062" spans="1:7">
+      <c r="A3062">
+        <v>1975</v>
+      </c>
+      <c r="B3062" s="16" t="s">
+        <v>3144</v>
+      </c>
+      <c r="F3062" t="s">
+        <v>3186</v>
+      </c>
+      <c r="G3062">
+        <v>1777</v>
+      </c>
+    </row>
+    <row r="3063" spans="1:7">
+      <c r="A3063">
+        <v>1976</v>
+      </c>
+      <c r="B3063" t="s">
+        <v>3145</v>
+      </c>
+      <c r="F3063" s="16" t="s">
+        <v>3187</v>
+      </c>
+      <c r="G3063">
+        <v>1778</v>
+      </c>
+    </row>
+    <row r="3064" spans="1:7">
+      <c r="A3064">
+        <v>1977</v>
+      </c>
+      <c r="B3064" s="27" t="s">
+        <v>3146</v>
+      </c>
+      <c r="F3064" t="s">
+        <v>3158</v>
+      </c>
+      <c r="G3064">
+        <v>1779</v>
+      </c>
+    </row>
+    <row r="3065" spans="1:7">
+      <c r="F3065" t="s">
+        <v>3188</v>
+      </c>
+      <c r="G3065">
+        <v>1780</v>
+      </c>
+    </row>
+    <row r="3066" spans="1:7">
+      <c r="F3066" t="s">
+        <v>2453</v>
+      </c>
+      <c r="G3066">
+        <v>1781</v>
+      </c>
+    </row>
+    <row r="3067" spans="1:7">
+      <c r="F3067" t="s">
+        <v>2443</v>
+      </c>
+      <c r="G3067">
+        <v>1782</v>
+      </c>
+    </row>
+    <row r="3068" spans="1:7">
+      <c r="F3068" t="s">
+        <v>2444</v>
+      </c>
+      <c r="G3068">
+        <v>1783</v>
+      </c>
+    </row>
+    <row r="3069" spans="1:7">
+      <c r="F3069" t="s">
+        <v>3155</v>
+      </c>
+      <c r="G3069">
+        <v>1784</v>
+      </c>
+    </row>
+    <row r="3070" spans="1:7">
+      <c r="F3070" t="s">
+        <v>3189</v>
+      </c>
+      <c r="G3070">
+        <v>1785</v>
+      </c>
+    </row>
+    <row r="3071" spans="1:7">
+      <c r="F3071" s="27" t="s">
+        <v>3190</v>
+      </c>
+      <c r="G3071">
+        <v>1786</v>
+      </c>
+    </row>
+    <row r="3072" spans="1:7">
+      <c r="F3072" t="s">
+        <v>2443</v>
+      </c>
+      <c r="G3072">
+        <v>1787</v>
+      </c>
+    </row>
+    <row r="3073" spans="6:7">
+      <c r="F3073" t="s">
+        <v>2444</v>
+      </c>
+      <c r="G3073">
+        <v>1788</v>
+      </c>
+    </row>
+    <row r="3074" spans="6:7">
+      <c r="F3074" t="s">
+        <v>3155</v>
+      </c>
+      <c r="G3074">
+        <v>1789</v>
+      </c>
+    </row>
+    <row r="3075" spans="6:7">
+      <c r="F3075" t="s">
+        <v>3191</v>
+      </c>
+      <c r="G3075">
+        <v>1790</v>
+      </c>
+    </row>
+    <row r="3076" spans="6:7">
+      <c r="F3076" t="s">
+        <v>3187</v>
+      </c>
+      <c r="G3076">
+        <v>1791</v>
+      </c>
+    </row>
+    <row r="3077" spans="6:7">
+      <c r="F3077" t="s">
+        <v>3158</v>
+      </c>
+      <c r="G3077">
+        <v>1792</v>
+      </c>
+    </row>
+    <row r="3078" spans="6:7">
+      <c r="F3078" s="27" t="s">
+        <v>3192</v>
+      </c>
+      <c r="G3078">
+        <v>1793</v>
+      </c>
+    </row>
+    <row r="3079" spans="6:7">
+      <c r="F3079" s="27" t="s">
+        <v>3193</v>
+      </c>
+      <c r="G3079">
+        <v>1794</v>
+      </c>
+    </row>
+    <row r="3080" spans="6:7">
+      <c r="F3080" t="s">
+        <v>2443</v>
+      </c>
+      <c r="G3080">
+        <v>1795</v>
+      </c>
+    </row>
+    <row r="3081" spans="6:7">
+      <c r="F3081" t="s">
+        <v>2444</v>
+      </c>
+      <c r="G3081">
+        <v>1796</v>
+      </c>
+    </row>
+    <row r="3082" spans="6:7">
+      <c r="F3082" t="s">
+        <v>3155</v>
+      </c>
+      <c r="G3082">
+        <v>1797</v>
+      </c>
+    </row>
+    <row r="3083" spans="6:7">
+      <c r="F3083" t="s">
+        <v>3194</v>
+      </c>
+      <c r="G3083">
+        <v>1798</v>
+      </c>
+    </row>
+    <row r="3084" spans="6:7">
+      <c r="F3084" t="s">
+        <v>3195</v>
+      </c>
+      <c r="G3084">
+        <v>1799</v>
+      </c>
+    </row>
+    <row r="3085" spans="6:7">
+      <c r="F3085" t="s">
+        <v>3158</v>
+      </c>
+      <c r="G3085">
+        <v>1800</v>
+      </c>
+    </row>
+    <row r="3086" spans="6:7">
+      <c r="F3086" s="27" t="s">
+        <v>3196</v>
+      </c>
+      <c r="G3086">
+        <v>1801</v>
+      </c>
+    </row>
+    <row r="3087" spans="6:7">
+      <c r="F3087" s="27" t="s">
+        <v>3197</v>
+      </c>
+      <c r="G3087">
+        <v>1802</v>
+      </c>
+    </row>
+    <row r="3088" spans="6:7">
+      <c r="F3088" t="s">
+        <v>3198</v>
+      </c>
+      <c r="G3088">
+        <v>1803</v>
+      </c>
+    </row>
+    <row r="3089" spans="6:7">
+      <c r="F3089" t="s">
+        <v>3154</v>
+      </c>
+      <c r="G3089">
+        <v>1804</v>
+      </c>
+    </row>
+    <row r="3090" spans="6:7">
+      <c r="F3090" t="s">
+        <v>2443</v>
+      </c>
+      <c r="G3090">
+        <v>1805</v>
+      </c>
+    </row>
+    <row r="3091" spans="6:7">
+      <c r="F3091" t="s">
+        <v>2444</v>
+      </c>
+      <c r="G3091">
+        <v>1806</v>
+      </c>
+    </row>
+    <row r="3092" spans="6:7">
+      <c r="F3092" t="s">
+        <v>3155</v>
+      </c>
+      <c r="G3092">
+        <v>1807</v>
+      </c>
+    </row>
+    <row r="3093" spans="6:7">
+      <c r="F3093" t="s">
+        <v>3199</v>
+      </c>
+      <c r="G3093">
+        <v>1808</v>
+      </c>
+    </row>
+    <row r="3094" spans="6:7">
+      <c r="F3094" t="s">
+        <v>3200</v>
+      </c>
+      <c r="G3094">
+        <v>1809</v>
+      </c>
+    </row>
+    <row r="3095" spans="6:7">
+      <c r="F3095" t="s">
+        <v>3158</v>
+      </c>
+      <c r="G3095">
+        <v>1810</v>
+      </c>
+    </row>
+    <row r="3096" spans="6:7">
+      <c r="F3096" t="s">
+        <v>3201</v>
+      </c>
+      <c r="G3096">
+        <v>1811</v>
+      </c>
+    </row>
+    <row r="3097" spans="6:7">
+      <c r="F3097" t="s">
+        <v>2453</v>
+      </c>
+      <c r="G3097">
+        <v>1812</v>
+      </c>
+    </row>
+    <row r="3098" spans="6:7">
+      <c r="F3098" t="s">
+        <v>2443</v>
+      </c>
+      <c r="G3098">
+        <v>1813</v>
+      </c>
+    </row>
+    <row r="3099" spans="6:7">
+      <c r="F3099" t="s">
+        <v>3160</v>
+      </c>
+      <c r="G3099">
+        <v>1814</v>
+      </c>
+    </row>
+    <row r="3100" spans="6:7">
+      <c r="F3100" t="s">
+        <v>3155</v>
+      </c>
+      <c r="G3100">
+        <v>1815</v>
+      </c>
+    </row>
+    <row r="3101" spans="6:7">
+      <c r="F3101" t="s">
+        <v>3202</v>
+      </c>
+      <c r="G3101">
+        <v>1816</v>
+      </c>
+    </row>
+    <row r="3102" spans="6:7">
+      <c r="F3102" s="27" t="s">
+        <v>3203</v>
+      </c>
+      <c r="G3102">
+        <v>1817</v>
+      </c>
+    </row>
+    <row r="3103" spans="6:7">
+      <c r="F3103" s="27" t="s">
+        <v>3204</v>
+      </c>
+      <c r="G3103">
+        <v>1818</v>
+      </c>
+    </row>
+    <row r="3104" spans="6:7">
+      <c r="F3104" t="s">
+        <v>3205</v>
+      </c>
+      <c r="G3104">
+        <v>1819</v>
+      </c>
+    </row>
+    <row r="3105" spans="6:7">
+      <c r="F3105" t="s">
+        <v>3154</v>
+      </c>
+      <c r="G3105">
+        <v>1820</v>
+      </c>
+    </row>
+    <row r="3106" spans="6:7">
+      <c r="F3106" t="s">
+        <v>2443</v>
+      </c>
+      <c r="G3106">
+        <v>1821</v>
+      </c>
+    </row>
+    <row r="3107" spans="6:7">
+      <c r="F3107" t="s">
+        <v>3160</v>
+      </c>
+      <c r="G3107">
+        <v>1822</v>
+      </c>
+    </row>
+    <row r="3108" spans="6:7">
+      <c r="F3108" t="s">
+        <v>3155</v>
+      </c>
+      <c r="G3108">
+        <v>1823</v>
+      </c>
+    </row>
+    <row r="3109" spans="6:7">
+      <c r="F3109" t="s">
+        <v>3206</v>
+      </c>
+      <c r="G3109">
+        <v>1824</v>
+      </c>
+    </row>
   </sheetData>
-  <sortState ref="A2257:L2321">
-    <sortCondition ref="A2257:A2321"/>
+  <sortState ref="A2844:B2889">
+    <sortCondition ref="A2844:A2889"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -35145,8 +38453,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A827A58D-C8A4-4858-A89B-E853C083564F}">
   <dimension ref="A1:N32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E10" workbookViewId="0">
-      <selection activeCell="O26" sqref="O26"/>
+    <sheetView topLeftCell="C2" workbookViewId="0">
+      <selection activeCell="H25" sqref="H25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
@@ -35479,6 +38787,9 @@
       <c r="E11" s="31" t="s">
         <v>2896</v>
       </c>
+      <c r="N11" t="s">
+        <v>2977</v>
+      </c>
     </row>
     <row r="12" spans="1:14" ht="21">
       <c r="A12" s="21" t="s">
@@ -35496,6 +38807,9 @@
       <c r="E12" s="31" t="s">
         <v>2955</v>
       </c>
+      <c r="N12" t="s">
+        <v>2978</v>
+      </c>
     </row>
     <row r="13" spans="1:14" ht="21">
       <c r="A13" s="34" t="s">
@@ -35513,6 +38827,9 @@
       <c r="E13" s="31" t="s">
         <v>2956</v>
       </c>
+      <c r="N13" t="s">
+        <v>2979</v>
+      </c>
     </row>
     <row r="14" spans="1:14" ht="21">
       <c r="A14" s="34" t="s">
@@ -35563,6 +38880,10 @@
         <f>VLOOKUP(G15,prev,1,FALSE)</f>
         <v>#N/A</v>
       </c>
+      <c r="N15" t="str">
+        <f>"| "&amp;F15&amp;" | "&amp;G15&amp;" | "&amp;H15&amp;" | "&amp;I15&amp;" |"</f>
+        <v>| zero/1.0/ | 380886__morganpurkis__doom-shotgun-2017.wav | https://freesound.org/s/380886/ | morganpurkis |</v>
+      </c>
     </row>
     <row r="16" spans="1:14" ht="21">
       <c r="A16" s="21" t="s">
@@ -35596,8 +38917,12 @@
         <f>VLOOKUP(G16,prev,1,FALSE)</f>
         <v>#N/A</v>
       </c>
-    </row>
-    <row r="17" spans="1:13" ht="21">
+      <c r="N16" t="str">
+        <f t="shared" ref="N16:N32" si="0">"| "&amp;F16&amp;" | "&amp;G16&amp;" | "&amp;H16&amp;" | "&amp;I16&amp;" |"</f>
+        <v>| zero/1.0/ | 500418__dj-somar__intro-reverso-craver-microbrute.wav | https://freesound.org/s/500418/ | DJ_SoMaR |</v>
+      </c>
+    </row>
+    <row r="17" spans="1:14" ht="21">
       <c r="A17" s="34" t="s">
         <v>2880</v>
       </c>
@@ -35629,8 +38954,12 @@
         <f>VLOOKUP(G17,prev,1,FALSE)</f>
         <v>#N/A</v>
       </c>
-    </row>
-    <row r="18" spans="1:13" ht="21">
+      <c r="N17" t="str">
+        <f t="shared" si="0"/>
+        <v>| by/3.0/ | 272068__ichbinjager__shotgun-action.wav | https://freesound.org/s/272068/ | IchBinJager |</v>
+      </c>
+    </row>
+    <row r="18" spans="1:14" ht="21">
       <c r="A18" s="21" t="s">
         <v>2880</v>
       </c>
@@ -35662,8 +38991,12 @@
         <f>VLOOKUP(G18,prev,1,FALSE)</f>
         <v>#N/A</v>
       </c>
-    </row>
-    <row r="19" spans="1:13" ht="21">
+      <c r="N18" t="str">
+        <f t="shared" si="0"/>
+        <v>| by/3.0/ | 431117__inspectorj__door-front-opening-a.wav | https://freesound.org/s/431117/ | inspectorj |</v>
+      </c>
+    </row>
+    <row r="19" spans="1:14" ht="21">
       <c r="A19" s="21" t="s">
         <v>2880</v>
       </c>
@@ -35695,8 +39028,12 @@
         <f>VLOOKUP(G19,prev,1,FALSE)</f>
         <v>#N/A</v>
       </c>
-    </row>
-    <row r="20" spans="1:13" ht="21">
+      <c r="N19" t="str">
+        <f t="shared" si="0"/>
+        <v>| zero/1.0/ | 404068__swordofkings128__backyard-gate-open.wav | https://freesound.org/s/404068/ | swordofkings128 |</v>
+      </c>
+    </row>
+    <row r="20" spans="1:14" ht="21">
       <c r="A20" s="21" t="s">
         <v>2880</v>
       </c>
@@ -35728,8 +39065,12 @@
         <f>VLOOKUP(G20,prev,1,FALSE)</f>
         <v>#N/A</v>
       </c>
-    </row>
-    <row r="21" spans="1:13" ht="21">
+      <c r="N20" t="str">
+        <f t="shared" si="0"/>
+        <v>| by/3.0/ | 96964__gabisaraceni__porta-abrindo-5.wav | https://freesound.org/s/96964/ | gabisaraceni |</v>
+      </c>
+    </row>
+    <row r="21" spans="1:14" ht="21">
       <c r="A21" s="21" t="s">
         <v>2880</v>
       </c>
@@ -35761,8 +39102,12 @@
         <f>VLOOKUP(G21,prev,1,FALSE)</f>
         <v>#N/A</v>
       </c>
-    </row>
-    <row r="22" spans="1:13" ht="21">
+      <c r="N21" t="str">
+        <f t="shared" si="0"/>
+        <v>| by/3.0/ | 275537__wjoojoo__contact-mic-on-satellite-dish04.wav | https://freesound.org/s/275537/ | wjoojoo |</v>
+      </c>
+    </row>
+    <row r="22" spans="1:14" ht="21">
       <c r="A22" s="34" t="s">
         <v>2880</v>
       </c>
@@ -35794,8 +39139,12 @@
         <f>VLOOKUP(G22,prev,1,FALSE)</f>
         <v>#N/A</v>
       </c>
-    </row>
-    <row r="23" spans="1:13" ht="21">
+      <c r="N22" t="str">
+        <f t="shared" si="0"/>
+        <v>| zero/1.0/ | 352852__josepharaoh99__game-style-laser-beam.wav | https://freesound.org/s/352852/ | josepharaoh99 |</v>
+      </c>
+    </row>
+    <row r="23" spans="1:14" ht="21">
       <c r="A23" s="34" t="s">
         <v>2882</v>
       </c>
@@ -35827,8 +39176,12 @@
         <f>VLOOKUP(G23,prev,1,FALSE)</f>
         <v>#N/A</v>
       </c>
-    </row>
-    <row r="24" spans="1:13" ht="21">
+      <c r="N23" t="str">
+        <f t="shared" si="0"/>
+        <v>| by/3.0/ | 417363__xcreenplay__boing-massive-kick.wav | https://freesound.org/s/417363/ | xcreenplay |</v>
+      </c>
+    </row>
+    <row r="24" spans="1:14" ht="21">
       <c r="A24" s="34" t="s">
         <v>2882</v>
       </c>
@@ -35860,8 +39213,12 @@
         <f>VLOOKUP(G24,prev,1,FALSE)</f>
         <v>#N/A</v>
       </c>
-    </row>
-    <row r="25" spans="1:13" ht="21">
+      <c r="N24" t="str">
+        <f t="shared" si="0"/>
+        <v>| by/3.0/ | 221875__hero-of-the-winds__spring-boing.wav | https://freesound.org/s/221875/ | hero-of-the-winds |</v>
+      </c>
+    </row>
+    <row r="25" spans="1:14" ht="21">
       <c r="A25" s="21" t="s">
         <v>2882</v>
       </c>
@@ -35883,7 +39240,7 @@
       <c r="G25" s="21" t="s">
         <v>2878</v>
       </c>
-      <c r="H25" t="s">
+      <c r="H25" s="32" t="s">
         <v>2970</v>
       </c>
       <c r="I25" s="31" t="s">
@@ -35893,8 +39250,12 @@
         <f>VLOOKUP(G25,prev,1,FALSE)</f>
         <v>#N/A</v>
       </c>
-    </row>
-    <row r="26" spans="1:13" ht="21">
+      <c r="N25" t="str">
+        <f t="shared" si="0"/>
+        <v>| by/3.0/ | 240297__jalastram__abstract-guitar-sfx-003.wav | https://freesound.org/s/240297/ | jalastram |</v>
+      </c>
+    </row>
+    <row r="26" spans="1:14" ht="21">
       <c r="F26" s="39" t="s">
         <v>2889</v>
       </c>
@@ -35911,8 +39272,12 @@
         <f>VLOOKUP(G26,prev,1,FALSE)</f>
         <v>#N/A</v>
       </c>
-    </row>
-    <row r="27" spans="1:13" ht="21">
+      <c r="N26" t="str">
+        <f t="shared" si="0"/>
+        <v>| zero/1.0/ | 383760__deleted-user-7146007__laboratory-mad-scientist-science-fiction-sci-fi.wav | https://freesound.org/s/383760/ | deleted-user-7146007 |</v>
+      </c>
+    </row>
+    <row r="27" spans="1:14" ht="21">
       <c r="F27" s="41" t="s">
         <v>2897</v>
       </c>
@@ -35929,8 +39294,12 @@
         <f>VLOOKUP(G27,prev,1,FALSE)</f>
         <v>#N/A</v>
       </c>
-    </row>
-    <row r="28" spans="1:13" ht="21">
+      <c r="N27" t="str">
+        <f t="shared" si="0"/>
+        <v>| by/3.0/ | 417131__cuddlenucks__science-fiction-noise-3.wav | https://freesound.org/s/417131/ | cuddlenucks |</v>
+      </c>
+    </row>
+    <row r="28" spans="1:14" ht="21">
       <c r="F28" s="39" t="s">
         <v>2889</v>
       </c>
@@ -35948,8 +39317,12 @@
         <v>#N/A</v>
       </c>
       <c r="M28" s="32"/>
-    </row>
-    <row r="29" spans="1:13" ht="21">
+      <c r="N28" t="str">
+        <f t="shared" si="0"/>
+        <v>| zero/1.0/ | 170136__lazr2012__machinery-bo.flac | https://freesound.org/s/170136/ | lazr2012 |</v>
+      </c>
+    </row>
+    <row r="29" spans="1:14" ht="21">
       <c r="F29" s="39" t="s">
         <v>2897</v>
       </c>
@@ -35966,8 +39339,12 @@
         <f>VLOOKUP(G29,prev,1,FALSE)</f>
         <v>#N/A</v>
       </c>
-    </row>
-    <row r="30" spans="1:13" ht="21">
+      <c r="N29" t="str">
+        <f t="shared" si="0"/>
+        <v>| by/3.0/ | 169292__lazr2012__haywirefusionator.ogg | https://freesound.org/s/169292/ | lazr2012 |</v>
+      </c>
+    </row>
+    <row r="30" spans="1:14" ht="21">
       <c r="F30" s="31" t="s">
         <v>2909</v>
       </c>
@@ -35984,8 +39361,12 @@
         <f>VLOOKUP(G30,prev,1,FALSE)</f>
         <v>#N/A</v>
       </c>
-    </row>
-    <row r="31" spans="1:13" ht="21">
+      <c r="N30" t="str">
+        <f t="shared" si="0"/>
+        <v>| by-nc/3.0/ | 165483__timbre__glitch-voice-ep-mp3.mp3 | https://freesound.org/s/165483/ | timbre |</v>
+      </c>
+    </row>
+    <row r="31" spans="1:14" ht="21">
       <c r="F31" s="39" t="s">
         <v>2889</v>
       </c>
@@ -36002,8 +39383,12 @@
         <f>VLOOKUP(G31,prev,1,FALSE)</f>
         <v>#N/A</v>
       </c>
-    </row>
-    <row r="32" spans="1:13" ht="21">
+      <c r="N31" t="str">
+        <f t="shared" si="0"/>
+        <v>| zero/1.0/ | 162814__timgormly__spaceship-4.aiff | https://freesound.org/s/162814/ | timgormly |</v>
+      </c>
+    </row>
+    <row r="32" spans="1:14" ht="21">
       <c r="F32" s="39" t="s">
         <v>2909</v>
       </c>
@@ -36019,6 +39404,10 @@
       <c r="L32" t="e">
         <f>VLOOKUP(G32,prev,1,FALSE)</f>
         <v>#N/A</v>
+      </c>
+      <c r="N32" t="str">
+        <f t="shared" si="0"/>
+        <v>| by-nc/3.0/ | 91296__timbre__bwaang-2-reverb.mp3 | https://freesound.org/s/91296/ | timbre |</v>
       </c>
     </row>
   </sheetData>
@@ -36041,7 +39430,9 @@
     <hyperlink ref="H19:H20" r:id="rId13" display="https://freesound.org/s//" xr:uid="{5FB99E8B-AEFC-6A45-851E-E3C683DC5AC1}"/>
     <hyperlink ref="H19" r:id="rId14" xr:uid="{E2EACC90-D2ED-AF4A-9302-ADD31B56C321}"/>
     <hyperlink ref="H20" r:id="rId15" xr:uid="{13F37B0F-8A53-0B4F-8FE7-132D2186D638}"/>
+    <hyperlink ref="H25" r:id="rId16" xr:uid="{FA55BAC7-078A-8944-9FB5-42D7B041E218}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
fix bug in clockwise down the drain
</commit_message>
<xml_diff>
--- a/RBG_arduino/StateTable_minimal.xlsx
+++ b/RBG_arduino/StateTable_minimal.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/markdolson/GitHub-Mark-MDO47/RubberBandGun/RBG_arduino/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5BE4743-124D-AD48-91B6-391A517549F7}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7D3CC22-F369-5040-9540-2F0C62766DCA}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15540" activeTab="2" xr2:uid="{CCADFEE4-B0E1-4363-9617-1683960BED03}"/>
+    <workbookView xWindow="-40" yWindow="480" windowWidth="25600" windowHeight="15540" activeTab="2" xr2:uid="{CCADFEE4-B0E1-4363-9617-1683960BED03}"/>
   </bookViews>
   <sheets>
     <sheet name="StateTable" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
     <sheet name="Sounds" sheetId="5" r:id="rId5"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">debugging!$A$2982:$B$3064</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">debugging!$A$3077:$B$3113</definedName>
     <definedName name="prev">Sounds!$N$2:$N$9</definedName>
     <definedName name="yxcmd">'YX5200 info'!$A$2:$C$44</definedName>
   </definedNames>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4290" uniqueCount="3207">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4339" uniqueCount="3247">
   <si>
     <t>trigOnly</t>
   </si>
@@ -9468,6 +9468,9 @@
     <t>2289:DEBUG loop() - nowVinputRBG 0x240 loopCount 609</t>
   </si>
   <si>
+    <t>18:DEBUG loop() - nowVinputRBG 0x240 loopCount 1</t>
+  </si>
+  <si>
     <t>re-organize timing; sometimes sound doesn't start right. 40 msec delay for state; up to 100 msec delay for busy</t>
   </si>
   <si>
@@ -9889,13 +9892,130 @@
   </si>
   <si>
     <t>DEBUG RBG_processStateTable() - tmpVinputRBG 0x40 from row 7 foundInputRow 8 loopCount 9090</t>
+  </si>
+  <si>
+    <t>11: RBG_startEffectSound ln 608 EFCT num 40 final num 41 loopCount 0</t>
+  </si>
+  <si>
+    <t>12: RBG_startEffectSound ln 638 waited for AUDIO_BUSY (msec) 10</t>
+  </si>
+  <si>
+    <t>745:DEBUG loop() - nowVinputRBG 0x40 loopCount 122</t>
+  </si>
+  <si>
+    <t>757:DEBUG RBG_processStateTable() - tmpVinputRBG 0x40 from row 0 foundInputRow 1 loopCount 122</t>
+  </si>
+  <si>
+    <t>779:DEBUG RBG_processStateTable() - tmpVinputRBG 0x40 from row 1 foundInputRow 5 loopCount 125</t>
+  </si>
+  <si>
+    <t>780: RBG_startEffectSound ln 608 EFCT num 102 final num 102 loopCount 125</t>
+  </si>
+  <si>
+    <t>781: RBG_startEffectSound ln 638 waited for AUDIO_BUSY (msec) 10</t>
+  </si>
+  <si>
+    <t>787:DEBUG loop() - nowVinputRBG 0x240 loopCount 126</t>
+  </si>
+  <si>
+    <t>932:DEBUG loop() - nowVinputRBG 0x260 loopCount 138</t>
+  </si>
+  <si>
+    <t>946:DEBUG RBG_processStateTable() - tmpVinputRBG 0x260 from row 5 foundInputRow 7 loopCount 138</t>
+  </si>
+  <si>
+    <t>947: RBG_startEffectSound ln 608 EFCT num 0 final num 1 loopCount 139</t>
+  </si>
+  <si>
+    <t>948: RBG_startEffectSound ln 638 waited for AUDIO_BUSY (msec) 0</t>
+  </si>
+  <si>
+    <t>954:DEBUG loop() - nowVinputRBG 0x60 loopCount 140</t>
+  </si>
+  <si>
+    <t>966:DEBUG RBG_processStateTable() - tmpVinputRBG 0x60 from row 7 foundInputRow 8 loopCount 140</t>
+  </si>
+  <si>
+    <t>967:DEBUG loop() - nowVinputRBG 0x260 loopCount 141</t>
+  </si>
+  <si>
+    <t>972:DEBUG loop() - nowVinputRBG 0x240 loopCount 142</t>
+  </si>
+  <si>
+    <t>984:DEBUG RBG_processStateTable() - tmpVinputRBG 0x240 from row 8 foundInputRow 9 loopCount 142</t>
+  </si>
+  <si>
+    <t>985: RBG_startEffectSound ln 608 EFCT num 10 final num 11 loopCount 143</t>
+  </si>
+  <si>
+    <t>986: RBG_startEffectSound ln 638 waited for AUDIO_BUSY (msec) 0</t>
+  </si>
+  <si>
+    <t>1226:DEBUG loop() - nowVinputRBG 0x260 loopCount 184</t>
+  </si>
+  <si>
+    <t>1251:DEBUG loop() - nowVinputRBG 0x240 loopCount 188</t>
+  </si>
+  <si>
+    <t>1312:DEBUG loop() - nowVinputRBG 0x260 loopCount 198</t>
+  </si>
+  <si>
+    <t>1337:DEBUG loop() - nowVinputRBG 0x240 loopCount 202</t>
+  </si>
+  <si>
+    <t>1368:DEBUG loop() - nowVinputRBG 0x40 loopCount 258</t>
+  </si>
+  <si>
+    <t>1374:DEBUG RBG_processStateTable() - tmpVinputRBG 0x40 from row 9 foundInputRow 10 loopCount 258</t>
+  </si>
+  <si>
+    <t>1384:DEBUG RBG_processStateTable() - tmpVinputRBG 0x40 from row 10 foundInputRow 1 loopCount 260</t>
+  </si>
+  <si>
+    <t>1394:DEBUG RBG_processStateTable() - tmpVinputRBG 0x40 from row 1 foundInputRow 5 loopCount 262</t>
+  </si>
+  <si>
+    <t>1395: RBG_startEffectSound ln 608 EFCT num 102 final num 102 loopCount 263</t>
+  </si>
+  <si>
+    <t>1396: RBG_startEffectSound ln 638 waited for AUDIO_BUSY (msec) 10</t>
+  </si>
+  <si>
+    <t>1402:DEBUG loop() - nowVinputRBG 0x240 loopCount 263</t>
+  </si>
+  <si>
+    <t>1403:DEBUG loop() - nowVinputRBG 0x40 loopCount 1059</t>
+  </si>
+  <si>
+    <t>1408: RBG_startEffectSound ln 608 EFCT num 102 final num 102 loopCount 1059</t>
+  </si>
+  <si>
+    <t>1409: RBG_startEffectSound ln 638 waited for AUDIO_BUSY (msec) 0</t>
+  </si>
+  <si>
+    <t>1410:DEBUG loop() - nowVinputRBG 0x240 loopCount 1059</t>
+  </si>
+  <si>
+    <t>13: RBG_startEffectLED ln 552 EFCT num 40 final LED num 41 loopCount 0</t>
+  </si>
+  <si>
+    <t>782: RBG_startEffectLED ln 552 EFCT num 102 final LED num 102 loopCount 125</t>
+  </si>
+  <si>
+    <t>949: RBG_startEffectLED ln 552 EFCT num 0 final LED num 1 loopCount 139</t>
+  </si>
+  <si>
+    <t>987: RBG_startEffectLED ln 552 EFCT num 10 final LED num 11 loopCount 143</t>
+  </si>
+  <si>
+    <t>1397: RBG_startEffectLED ln 552 EFCT num 102 final LED num 102 loopCount 263</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="19">
+  <fonts count="20">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -10029,6 +10149,13 @@
       <color rgb="FF24292E"/>
       <name val="Helvetica"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFC00000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="12">
@@ -10181,7 +10308,7 @@
     <xf numFmtId="0" fontId="11" fillId="9" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="46">
+  <cellXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -10227,6 +10354,7 @@
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="7"/>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="0" xfId="5" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="5" borderId="4" xfId="4" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="6" borderId="4" xfId="5" applyBorder="1"/>
@@ -10244,6 +10372,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="11" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="19" fillId="6" borderId="3" xfId="5" applyFont="1"/>
   </cellXfs>
   <cellStyles count="8">
     <cellStyle name="Bad" xfId="2" builtinId="27"/>
@@ -11121,10 +11251,10 @@
       <c r="J24" s="9"/>
     </row>
     <row r="25" spans="1:14" s="28" customFormat="1">
-      <c r="F25" s="42"/>
-      <c r="G25" s="42"/>
-      <c r="H25" s="42"/>
-      <c r="I25" s="42"/>
+      <c r="F25" s="43"/>
+      <c r="G25" s="43"/>
+      <c r="H25" s="43"/>
+      <c r="I25" s="43"/>
     </row>
     <row r="26" spans="1:14" ht="16">
       <c r="A26" s="9" t="s">
@@ -11381,10 +11511,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F57F550E-21B4-4ED7-B7FF-211D228584A7}">
-  <dimension ref="A1:L3109"/>
+  <dimension ref="A1:L3118"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B2988" workbookViewId="0">
-      <selection activeCell="E3008" sqref="E3008"/>
+    <sheetView tabSelected="1" topLeftCell="A3078" workbookViewId="0">
+      <selection activeCell="B3081" sqref="B3081"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
@@ -34148,15 +34278,15 @@
       </c>
     </row>
     <row r="2945" spans="1:2" ht="16">
-      <c r="A2945" s="43">
+      <c r="A2945" s="44">
         <v>10</v>
       </c>
-      <c r="B2945" s="44" t="s">
+      <c r="B2945" s="45" t="s">
         <v>2980</v>
       </c>
     </row>
     <row r="2946" spans="1:2" ht="16">
-      <c r="A2946" s="43">
+      <c r="A2946" s="44">
         <v>11</v>
       </c>
       <c r="B2946" s="16" t="s">
@@ -34164,15 +34294,15 @@
       </c>
     </row>
     <row r="2947" spans="1:2" ht="16">
-      <c r="A2947" s="43">
+      <c r="A2947" s="44">
         <v>12</v>
       </c>
-      <c r="B2947" s="43" t="s">
+      <c r="B2947" s="44" t="s">
         <v>3015</v>
       </c>
     </row>
     <row r="2948" spans="1:2" ht="16">
-      <c r="A2948" s="43">
+      <c r="A2948" s="44">
         <v>30</v>
       </c>
       <c r="B2948" s="12" t="s">
@@ -34180,15 +34310,15 @@
       </c>
     </row>
     <row r="2949" spans="1:2" ht="16">
-      <c r="A2949" s="43">
+      <c r="A2949" s="44">
         <v>31</v>
       </c>
-      <c r="B2949" s="44" t="s">
+      <c r="B2949" s="45" t="s">
         <v>2981</v>
       </c>
     </row>
     <row r="2950" spans="1:2" ht="16">
-      <c r="A2950" s="43">
+      <c r="A2950" s="44">
         <v>53</v>
       </c>
       <c r="B2950" s="12" t="s">
@@ -34196,7 +34326,7 @@
       </c>
     </row>
     <row r="2951" spans="1:2" ht="16">
-      <c r="A2951" s="43">
+      <c r="A2951" s="44">
         <v>54</v>
       </c>
       <c r="B2951" s="16" t="s">
@@ -34204,15 +34334,15 @@
       </c>
     </row>
     <row r="2952" spans="1:2" ht="16">
-      <c r="A2952" s="43">
+      <c r="A2952" s="44">
         <v>61</v>
       </c>
-      <c r="B2952" s="44" t="s">
+      <c r="B2952" s="45" t="s">
         <v>2982</v>
       </c>
     </row>
     <row r="2953" spans="1:2" ht="16">
-      <c r="A2953" s="43">
+      <c r="A2953" s="44">
         <v>78</v>
       </c>
       <c r="B2953" s="16" t="s">
@@ -34220,23 +34350,23 @@
       </c>
     </row>
     <row r="2954" spans="1:2" ht="16">
-      <c r="A2954" s="43">
+      <c r="A2954" s="44">
         <v>79</v>
       </c>
-      <c r="B2954" s="44" t="s">
+      <c r="B2954" s="45" t="s">
         <v>2983</v>
       </c>
     </row>
     <row r="2955" spans="1:2" ht="16">
-      <c r="A2955" s="43">
+      <c r="A2955" s="44">
         <v>1976</v>
       </c>
-      <c r="B2955" s="44" t="s">
+      <c r="B2955" s="45" t="s">
         <v>3049</v>
       </c>
     </row>
     <row r="2956" spans="1:2" ht="16">
-      <c r="A2956" s="43">
+      <c r="A2956" s="44">
         <v>1990</v>
       </c>
       <c r="B2956" s="12" t="s">
@@ -34244,7 +34374,7 @@
       </c>
     </row>
     <row r="2957" spans="1:2" ht="16">
-      <c r="A2957" s="43">
+      <c r="A2957" s="44">
         <v>1991</v>
       </c>
       <c r="B2957" s="16" t="s">
@@ -34252,15 +34382,15 @@
       </c>
     </row>
     <row r="2958" spans="1:2" ht="16">
-      <c r="A2958" s="43">
+      <c r="A2958" s="44">
         <v>1998</v>
       </c>
-      <c r="B2958" s="44" t="s">
+      <c r="B2958" s="45" t="s">
         <v>3052</v>
       </c>
     </row>
     <row r="2959" spans="1:2" ht="16">
-      <c r="A2959" s="43">
+      <c r="A2959" s="44">
         <v>2010</v>
       </c>
       <c r="B2959" s="12" t="s">
@@ -34268,15 +34398,15 @@
       </c>
     </row>
     <row r="2960" spans="1:2" ht="16">
-      <c r="A2960" s="43">
+      <c r="A2960" s="44">
         <v>2011</v>
       </c>
-      <c r="B2960" s="44" t="s">
+      <c r="B2960" s="45" t="s">
         <v>3054</v>
       </c>
     </row>
     <row r="2961" spans="1:2" ht="16">
-      <c r="A2961" s="43">
+      <c r="A2961" s="44">
         <v>2027</v>
       </c>
       <c r="B2961" s="12" t="s">
@@ -34284,7 +34414,7 @@
       </c>
     </row>
     <row r="2962" spans="1:2" ht="16">
-      <c r="A2962" s="43">
+      <c r="A2962" s="44">
         <v>2028</v>
       </c>
       <c r="B2962" s="16" t="s">
@@ -34292,31 +34422,31 @@
       </c>
     </row>
     <row r="2963" spans="1:2" ht="16">
-      <c r="A2963" s="43">
+      <c r="A2963" s="44">
         <v>2203</v>
       </c>
-      <c r="B2963" s="44" t="s">
+      <c r="B2963" s="45" t="s">
         <v>3057</v>
       </c>
     </row>
     <row r="2964" spans="1:2" ht="16">
-      <c r="A2964" s="43">
+      <c r="A2964" s="44">
         <v>2228</v>
       </c>
-      <c r="B2964" s="44" t="s">
+      <c r="B2964" s="45" t="s">
         <v>3058</v>
       </c>
     </row>
     <row r="2965" spans="1:2" ht="16">
-      <c r="A2965" s="43">
+      <c r="A2965" s="44">
         <v>2253</v>
       </c>
-      <c r="B2965" s="44" t="s">
+      <c r="B2965" s="45" t="s">
         <v>3059</v>
       </c>
     </row>
     <row r="2966" spans="1:2" ht="16">
-      <c r="A2966" s="43">
+      <c r="A2966" s="44">
         <v>2259</v>
       </c>
       <c r="B2966" s="12" t="s">
@@ -34324,7 +34454,7 @@
       </c>
     </row>
     <row r="2967" spans="1:2" ht="16">
-      <c r="A2967" s="43">
+      <c r="A2967" s="44">
         <v>2269</v>
       </c>
       <c r="B2967" s="12" t="s">
@@ -34332,7 +34462,7 @@
       </c>
     </row>
     <row r="2968" spans="1:2" ht="16">
-      <c r="A2968" s="43">
+      <c r="A2968" s="44">
         <v>2279</v>
       </c>
       <c r="B2968" s="12" t="s">
@@ -34340,7 +34470,7 @@
       </c>
     </row>
     <row r="2969" spans="1:2" ht="16">
-      <c r="A2969" s="43">
+      <c r="A2969" s="44">
         <v>2280</v>
       </c>
       <c r="B2969" s="16" t="s">
@@ -34348,25 +34478,25 @@
       </c>
     </row>
     <row r="2970" spans="1:2" ht="16">
-      <c r="A2970" s="43">
+      <c r="A2970" s="44">
         <v>2281</v>
       </c>
-      <c r="B2970" s="43" t="s">
+      <c r="B2970" s="44" t="s">
         <v>3064</v>
       </c>
     </row>
     <row r="2971" spans="1:2" ht="16">
-      <c r="A2971" s="43">
+      <c r="A2971" s="44">
         <v>2289</v>
       </c>
-      <c r="B2971" s="44" t="s">
+      <c r="B2971" s="45" t="s">
         <v>3065</v>
       </c>
     </row>
     <row r="2973" spans="1:2" ht="16" thickBot="1"/>
     <row r="2974" spans="1:2" ht="17" thickTop="1" thickBot="1">
       <c r="B2974" s="1" t="s">
-        <v>3066</v>
+        <v>3067</v>
       </c>
     </row>
     <row r="2975" spans="1:2" ht="16" thickTop="1"/>
@@ -34419,7 +34549,7 @@
         <v>3014</v>
       </c>
       <c r="C2984" t="s">
-        <v>3147</v>
+        <v>3148</v>
       </c>
     </row>
     <row r="2985" spans="1:4">
@@ -34427,7 +34557,7 @@
         <v>12</v>
       </c>
       <c r="B2985" t="s">
-        <v>3067</v>
+        <v>3068</v>
       </c>
     </row>
     <row r="2986" spans="1:4">
@@ -34435,7 +34565,7 @@
         <v>19</v>
       </c>
       <c r="B2986" s="27" t="s">
-        <v>3068</v>
+        <v>3069</v>
       </c>
     </row>
     <row r="2987" spans="1:4">
@@ -34443,10 +34573,10 @@
         <v>752</v>
       </c>
       <c r="B2987" s="27" t="s">
-        <v>3069</v>
+        <v>3070</v>
       </c>
       <c r="C2987" t="s">
-        <v>3147</v>
+        <v>3148</v>
       </c>
     </row>
     <row r="2988" spans="1:4">
@@ -34454,7 +34584,7 @@
         <v>764</v>
       </c>
       <c r="B2988" s="12" t="s">
-        <v>3070</v>
+        <v>3071</v>
       </c>
       <c r="D2988" t="s">
         <v>2672</v>
@@ -34465,7 +34595,7 @@
         <v>786</v>
       </c>
       <c r="B2989" s="12" t="s">
-        <v>3071</v>
+        <v>3072</v>
       </c>
       <c r="D2989" t="s">
         <v>2674</v>
@@ -34476,10 +34606,10 @@
         <v>787</v>
       </c>
       <c r="B2990" s="16" t="s">
-        <v>3072</v>
+        <v>3073</v>
       </c>
       <c r="C2990" t="s">
-        <v>3147</v>
+        <v>3148</v>
       </c>
     </row>
     <row r="2991" spans="1:4">
@@ -34487,7 +34617,7 @@
         <v>788</v>
       </c>
       <c r="B2991" t="s">
-        <v>3073</v>
+        <v>3074</v>
       </c>
     </row>
     <row r="2992" spans="1:4">
@@ -34495,7 +34625,7 @@
         <v>795</v>
       </c>
       <c r="B2992" s="27" t="s">
-        <v>3074</v>
+        <v>3075</v>
       </c>
     </row>
     <row r="2993" spans="1:7">
@@ -34503,13 +34633,13 @@
         <v>1708</v>
       </c>
       <c r="B2993" s="27" t="s">
-        <v>3075</v>
+        <v>3076</v>
       </c>
       <c r="E2993" t="s">
-        <v>3149</v>
+        <v>3150</v>
       </c>
       <c r="F2993" s="27" t="s">
-        <v>3152</v>
+        <v>3153</v>
       </c>
       <c r="G2993">
         <v>1708</v>
@@ -34520,16 +34650,16 @@
         <v>1714</v>
       </c>
       <c r="B2994" s="12" t="s">
-        <v>3076</v>
+        <v>3077</v>
       </c>
       <c r="D2994" t="s">
         <v>2675</v>
       </c>
       <c r="E2994" t="s">
-        <v>3149</v>
+        <v>3150</v>
       </c>
       <c r="F2994" t="s">
-        <v>3153</v>
+        <v>3154</v>
       </c>
       <c r="G2994">
         <v>1709</v>
@@ -34540,16 +34670,16 @@
         <v>1715</v>
       </c>
       <c r="B2995" s="16" t="s">
-        <v>3077</v>
+        <v>3078</v>
       </c>
       <c r="C2995" s="4" t="s">
-        <v>3148</v>
+        <v>3149</v>
       </c>
       <c r="E2995" t="s">
-        <v>3149</v>
+        <v>3150</v>
       </c>
       <c r="F2995" t="s">
-        <v>3154</v>
+        <v>3155</v>
       </c>
       <c r="G2995">
         <v>1710</v>
@@ -34560,10 +34690,10 @@
         <v>1716</v>
       </c>
       <c r="B2996" t="s">
-        <v>3078</v>
+        <v>3079</v>
       </c>
       <c r="E2996" t="s">
-        <v>3149</v>
+        <v>3150</v>
       </c>
       <c r="F2996" t="s">
         <v>2443</v>
@@ -34577,13 +34707,13 @@
         <v>1723</v>
       </c>
       <c r="B2997" s="27" t="s">
-        <v>3079</v>
+        <v>3080</v>
       </c>
       <c r="C2997" s="4" t="s">
-        <v>3148</v>
+        <v>3149</v>
       </c>
       <c r="E2997" t="s">
-        <v>3149</v>
+        <v>3150</v>
       </c>
       <c r="F2997" t="s">
         <v>2444</v>
@@ -34597,16 +34727,16 @@
         <v>1729</v>
       </c>
       <c r="B2998" s="12" t="s">
-        <v>3080</v>
+        <v>3081</v>
       </c>
       <c r="D2998" t="s">
         <v>2676</v>
       </c>
       <c r="E2998" t="s">
-        <v>3149</v>
+        <v>3150</v>
       </c>
       <c r="F2998" t="s">
-        <v>3155</v>
+        <v>3156</v>
       </c>
       <c r="G2998">
         <v>1713</v>
@@ -34617,13 +34747,13 @@
         <v>1730</v>
       </c>
       <c r="B2999" s="27" t="s">
-        <v>3081</v>
+        <v>3082</v>
       </c>
       <c r="E2999" t="s">
-        <v>3149</v>
+        <v>3150</v>
       </c>
       <c r="F2999" t="s">
-        <v>3156</v>
+        <v>3157</v>
       </c>
       <c r="G2999">
         <v>1714</v>
@@ -34634,13 +34764,13 @@
         <v>1735</v>
       </c>
       <c r="B3000" s="27" t="s">
-        <v>3082</v>
+        <v>3083</v>
       </c>
       <c r="E3000" t="s">
-        <v>3149</v>
+        <v>3150</v>
       </c>
       <c r="F3000" s="16" t="s">
-        <v>3157</v>
+        <v>3158</v>
       </c>
       <c r="G3000">
         <v>1715</v>
@@ -34651,16 +34781,16 @@
         <v>1741</v>
       </c>
       <c r="B3001" s="12" t="s">
-        <v>3083</v>
+        <v>3084</v>
       </c>
       <c r="D3001" t="s">
         <v>2677</v>
       </c>
       <c r="E3001" t="s">
-        <v>3149</v>
+        <v>3150</v>
       </c>
       <c r="F3001" t="s">
-        <v>3158</v>
+        <v>3159</v>
       </c>
       <c r="G3001">
         <v>1716</v>
@@ -34671,16 +34801,16 @@
         <v>1742</v>
       </c>
       <c r="B3002" s="16" t="s">
-        <v>3084</v>
+        <v>3085</v>
       </c>
       <c r="C3002" s="4" t="s">
-        <v>3148</v>
+        <v>3149</v>
       </c>
       <c r="E3002" t="s">
-        <v>3149</v>
+        <v>3150</v>
       </c>
       <c r="F3002" t="s">
-        <v>3159</v>
+        <v>3160</v>
       </c>
       <c r="G3002">
         <v>1717</v>
@@ -34691,10 +34821,10 @@
         <v>1743</v>
       </c>
       <c r="B3003" t="s">
-        <v>3085</v>
+        <v>3086</v>
       </c>
       <c r="E3003" t="s">
-        <v>3149</v>
+        <v>3150</v>
       </c>
       <c r="F3003" t="s">
         <v>2453</v>
@@ -34708,13 +34838,13 @@
         <v>1750</v>
       </c>
       <c r="B3004" s="27" t="s">
-        <v>3086</v>
+        <v>3087</v>
       </c>
       <c r="C3004" s="4" t="s">
-        <v>3148</v>
+        <v>3149</v>
       </c>
       <c r="E3004" t="s">
-        <v>3151</v>
+        <v>3152</v>
       </c>
       <c r="F3004" t="s">
         <v>2443</v>
@@ -34728,13 +34858,13 @@
         <v>1756</v>
       </c>
       <c r="B3005" s="12" t="s">
-        <v>3087</v>
+        <v>3088</v>
       </c>
       <c r="D3005" t="s">
         <v>2678</v>
       </c>
       <c r="F3005" t="s">
-        <v>3160</v>
+        <v>3161</v>
       </c>
       <c r="G3005">
         <v>1720</v>
@@ -34745,13 +34875,13 @@
         <v>1757</v>
       </c>
       <c r="B3006" s="27" t="s">
-        <v>3088</v>
+        <v>3089</v>
       </c>
       <c r="C3006" s="4" t="s">
-        <v>3148</v>
+        <v>3149</v>
       </c>
       <c r="F3006" t="s">
-        <v>3155</v>
+        <v>3156</v>
       </c>
       <c r="G3006">
         <v>1721</v>
@@ -34762,13 +34892,13 @@
         <v>1767</v>
       </c>
       <c r="B3007" s="12" t="s">
-        <v>3089</v>
+        <v>3090</v>
       </c>
       <c r="D3007" t="s">
         <v>2672</v>
       </c>
       <c r="F3007" t="s">
-        <v>3161</v>
+        <v>3162</v>
       </c>
       <c r="G3007">
         <v>1722</v>
@@ -34779,13 +34909,13 @@
         <v>1777</v>
       </c>
       <c r="B3008" s="12" t="s">
-        <v>3090</v>
+        <v>3091</v>
       </c>
       <c r="D3008" t="s">
         <v>2674</v>
       </c>
       <c r="F3008" s="27" t="s">
-        <v>3162</v>
+        <v>3163</v>
       </c>
       <c r="G3008" s="4">
         <v>1723</v>
@@ -34796,10 +34926,10 @@
         <v>1778</v>
       </c>
       <c r="B3009" s="16" t="s">
-        <v>3091</v>
+        <v>3092</v>
       </c>
       <c r="F3009" t="s">
-        <v>3163</v>
+        <v>3164</v>
       </c>
       <c r="G3009">
         <v>1724</v>
@@ -34810,10 +34940,10 @@
         <v>1779</v>
       </c>
       <c r="B3010" t="s">
-        <v>3092</v>
+        <v>3093</v>
       </c>
       <c r="F3010" t="s">
-        <v>3154</v>
+        <v>3155</v>
       </c>
       <c r="G3010">
         <v>1725</v>
@@ -34824,10 +34954,10 @@
         <v>1786</v>
       </c>
       <c r="B3011" s="27" t="s">
-        <v>3093</v>
+        <v>3094</v>
       </c>
       <c r="C3011" s="4" t="s">
-        <v>3148</v>
+        <v>3149</v>
       </c>
       <c r="F3011" t="s">
         <v>2443</v>
@@ -34841,10 +34971,10 @@
         <v>1791</v>
       </c>
       <c r="B3012" s="16" t="s">
-        <v>3094</v>
+        <v>3095</v>
       </c>
       <c r="F3012" t="s">
-        <v>3160</v>
+        <v>3161</v>
       </c>
       <c r="G3012">
         <v>1727</v>
@@ -34855,10 +34985,10 @@
         <v>1792</v>
       </c>
       <c r="B3013" t="s">
-        <v>3095</v>
+        <v>3096</v>
       </c>
       <c r="F3013" t="s">
-        <v>3155</v>
+        <v>3156</v>
       </c>
       <c r="G3013">
         <v>1728</v>
@@ -34869,10 +34999,10 @@
         <v>1793</v>
       </c>
       <c r="B3014" s="27" t="s">
-        <v>3096</v>
+        <v>3097</v>
       </c>
       <c r="F3014" t="s">
-        <v>3164</v>
+        <v>3165</v>
       </c>
       <c r="G3014">
         <v>1729</v>
@@ -34883,10 +35013,10 @@
         <v>1794</v>
       </c>
       <c r="B3015" s="27" t="s">
-        <v>3097</v>
+        <v>3098</v>
       </c>
       <c r="F3015" s="27" t="s">
-        <v>3165</v>
+        <v>3166</v>
       </c>
       <c r="G3015">
         <v>1730</v>
@@ -34897,7 +35027,7 @@
         <v>1799</v>
       </c>
       <c r="B3016" s="16" t="s">
-        <v>3098</v>
+        <v>3099</v>
       </c>
       <c r="F3016" t="s">
         <v>2443</v>
@@ -34911,10 +35041,10 @@
         <v>1800</v>
       </c>
       <c r="B3017" t="s">
-        <v>3099</v>
+        <v>3100</v>
       </c>
       <c r="F3017" t="s">
-        <v>3166</v>
+        <v>3167</v>
       </c>
       <c r="G3017">
         <v>1732</v>
@@ -34925,10 +35055,10 @@
         <v>1801</v>
       </c>
       <c r="B3018" s="27" t="s">
-        <v>3100</v>
+        <v>3101</v>
       </c>
       <c r="F3018" t="s">
-        <v>3155</v>
+        <v>3156</v>
       </c>
       <c r="G3018">
         <v>1733</v>
@@ -34939,13 +35069,13 @@
         <v>1802</v>
       </c>
       <c r="B3019" s="27" t="s">
-        <v>3101</v>
+        <v>3102</v>
       </c>
       <c r="E3019" t="s">
-        <v>3149</v>
+        <v>3150</v>
       </c>
       <c r="F3019" t="s">
-        <v>3167</v>
+        <v>3168</v>
       </c>
       <c r="G3019">
         <v>1734</v>
@@ -34956,16 +35086,16 @@
         <v>1808</v>
       </c>
       <c r="B3020" s="12" t="s">
-        <v>3102</v>
+        <v>3103</v>
       </c>
       <c r="D3020" t="s">
         <v>2675</v>
       </c>
       <c r="E3020" t="s">
-        <v>3149</v>
+        <v>3150</v>
       </c>
       <c r="F3020" s="27" t="s">
-        <v>3168</v>
+        <v>3169</v>
       </c>
       <c r="G3020">
         <v>1735</v>
@@ -34976,13 +35106,13 @@
         <v>1809</v>
       </c>
       <c r="B3021" s="16" t="s">
-        <v>3103</v>
+        <v>3104</v>
       </c>
       <c r="E3021" t="s">
-        <v>3149</v>
+        <v>3150</v>
       </c>
       <c r="F3021" t="s">
-        <v>3169</v>
+        <v>3170</v>
       </c>
       <c r="G3021">
         <v>1736</v>
@@ -34993,13 +35123,13 @@
         <v>1810</v>
       </c>
       <c r="B3022" t="s">
-        <v>3104</v>
+        <v>3105</v>
       </c>
       <c r="E3022" t="s">
-        <v>3149</v>
+        <v>3150</v>
       </c>
       <c r="F3022" t="s">
-        <v>3154</v>
+        <v>3155</v>
       </c>
       <c r="G3022">
         <v>1737</v>
@@ -35010,12 +35140,12 @@
         <v>1817</v>
       </c>
       <c r="B3023" s="27" t="s">
-        <v>3105</v>
+        <v>3106</v>
       </c>
       <c r="E3023" t="s">
-        <v>3150</v>
-      </c>
-      <c r="F3023" s="45" t="s">
+        <v>3151</v>
+      </c>
+      <c r="F3023" s="46" t="s">
         <v>2443</v>
       </c>
       <c r="G3023">
@@ -35027,10 +35157,10 @@
         <v>1818</v>
       </c>
       <c r="B3024" s="27" t="s">
-        <v>3106</v>
+        <v>3107</v>
       </c>
       <c r="F3024" t="s">
-        <v>3166</v>
+        <v>3167</v>
       </c>
       <c r="G3024">
         <v>1739</v>
@@ -35041,13 +35171,13 @@
         <v>1824</v>
       </c>
       <c r="B3025" s="12" t="s">
-        <v>3107</v>
+        <v>3108</v>
       </c>
       <c r="D3025" t="s">
         <v>2676</v>
       </c>
       <c r="F3025" t="s">
-        <v>3155</v>
+        <v>3156</v>
       </c>
       <c r="G3025">
         <v>1740</v>
@@ -35058,13 +35188,13 @@
         <v>1834</v>
       </c>
       <c r="B3026" s="12" t="s">
-        <v>3108</v>
+        <v>3109</v>
       </c>
       <c r="D3026" t="s">
         <v>2677</v>
       </c>
       <c r="F3026" t="s">
-        <v>3170</v>
+        <v>3171</v>
       </c>
       <c r="G3026">
         <v>1741</v>
@@ -35075,10 +35205,10 @@
         <v>1835</v>
       </c>
       <c r="B3027" s="16" t="s">
-        <v>3109</v>
+        <v>3110</v>
       </c>
       <c r="F3027" s="16" t="s">
-        <v>3171</v>
+        <v>3172</v>
       </c>
       <c r="G3027">
         <v>1742</v>
@@ -35089,10 +35219,10 @@
         <v>1836</v>
       </c>
       <c r="B3028" t="s">
-        <v>3110</v>
+        <v>3111</v>
       </c>
       <c r="F3028" t="s">
-        <v>3158</v>
+        <v>3159</v>
       </c>
       <c r="G3028">
         <v>1743</v>
@@ -35103,10 +35233,10 @@
         <v>1843</v>
       </c>
       <c r="B3029" s="27" t="s">
-        <v>3111</v>
+        <v>3112</v>
       </c>
       <c r="F3029" t="s">
-        <v>3172</v>
+        <v>3173</v>
       </c>
       <c r="G3029">
         <v>1744</v>
@@ -35117,7 +35247,7 @@
         <v>1844</v>
       </c>
       <c r="B3030" s="27" t="s">
-        <v>3112</v>
+        <v>3113</v>
       </c>
       <c r="F3030" t="s">
         <v>2453</v>
@@ -35131,7 +35261,7 @@
         <v>1850</v>
       </c>
       <c r="B3031" s="12" t="s">
-        <v>3113</v>
+        <v>3114</v>
       </c>
       <c r="D3031" t="s">
         <v>2678</v>
@@ -35148,13 +35278,13 @@
         <v>1860</v>
       </c>
       <c r="B3032" s="12" t="s">
-        <v>3114</v>
+        <v>3115</v>
       </c>
       <c r="D3032" t="s">
         <v>2672</v>
       </c>
       <c r="F3032" t="s">
-        <v>3173</v>
+        <v>3174</v>
       </c>
       <c r="G3032">
         <v>1747</v>
@@ -35165,13 +35295,13 @@
         <v>1870</v>
       </c>
       <c r="B3033" s="12" t="s">
-        <v>3115</v>
+        <v>3116</v>
       </c>
       <c r="D3033" t="s">
         <v>2674</v>
       </c>
       <c r="F3033" t="s">
-        <v>3155</v>
+        <v>3156</v>
       </c>
       <c r="G3033">
         <v>1748</v>
@@ -35182,10 +35312,10 @@
         <v>1871</v>
       </c>
       <c r="B3034" s="16" t="s">
-        <v>3116</v>
+        <v>3117</v>
       </c>
       <c r="F3034" t="s">
-        <v>3174</v>
+        <v>3175</v>
       </c>
       <c r="G3034">
         <v>1749</v>
@@ -35196,10 +35326,10 @@
         <v>1872</v>
       </c>
       <c r="B3035" t="s">
-        <v>3117</v>
+        <v>3118</v>
       </c>
       <c r="F3035" s="27" t="s">
-        <v>3175</v>
+        <v>3176</v>
       </c>
       <c r="G3035">
         <v>1750</v>
@@ -35210,10 +35340,10 @@
         <v>1879</v>
       </c>
       <c r="B3036" s="27" t="s">
-        <v>3118</v>
+        <v>3119</v>
       </c>
       <c r="F3036" t="s">
-        <v>3176</v>
+        <v>3177</v>
       </c>
       <c r="G3036">
         <v>1751</v>
@@ -35224,10 +35354,10 @@
         <v>1880</v>
       </c>
       <c r="B3037" s="27" t="s">
-        <v>3119</v>
+        <v>3120</v>
       </c>
       <c r="F3037" t="s">
-        <v>3154</v>
+        <v>3155</v>
       </c>
       <c r="G3037">
         <v>1752</v>
@@ -35238,7 +35368,7 @@
         <v>1886</v>
       </c>
       <c r="B3038" s="12" t="s">
-        <v>3120</v>
+        <v>3121</v>
       </c>
       <c r="D3038" t="s">
         <v>2679</v>
@@ -35255,10 +35385,10 @@
         <v>1887</v>
       </c>
       <c r="B3039" s="16" t="s">
-        <v>3121</v>
+        <v>3122</v>
       </c>
       <c r="F3039" t="s">
-        <v>3173</v>
+        <v>3174</v>
       </c>
       <c r="G3039">
         <v>1754</v>
@@ -35269,10 +35399,10 @@
         <v>1888</v>
       </c>
       <c r="B3040" t="s">
-        <v>3122</v>
+        <v>3123</v>
       </c>
       <c r="F3040" t="s">
-        <v>3155</v>
+        <v>3156</v>
       </c>
       <c r="G3040">
         <v>1755</v>
@@ -35283,10 +35413,10 @@
         <v>1895</v>
       </c>
       <c r="B3041" s="27" t="s">
-        <v>3123</v>
+        <v>3124</v>
       </c>
       <c r="F3041" t="s">
-        <v>3177</v>
+        <v>3178</v>
       </c>
       <c r="G3041">
         <v>1756</v>
@@ -35297,13 +35427,13 @@
         <v>1901</v>
       </c>
       <c r="B3042" s="12" t="s">
-        <v>3124</v>
+        <v>3125</v>
       </c>
       <c r="D3042" t="s">
         <v>2672</v>
       </c>
       <c r="F3042" s="27" t="s">
-        <v>3178</v>
+        <v>3179</v>
       </c>
       <c r="G3042">
         <v>1757</v>
@@ -35314,7 +35444,7 @@
         <v>1902</v>
       </c>
       <c r="B3043" s="27" t="s">
-        <v>3125</v>
+        <v>3126</v>
       </c>
       <c r="F3043" t="s">
         <v>2443</v>
@@ -35328,13 +35458,13 @@
         <v>1912</v>
       </c>
       <c r="B3044" s="12" t="s">
-        <v>3126</v>
+        <v>3127</v>
       </c>
       <c r="D3044" t="s">
         <v>2673</v>
       </c>
       <c r="F3044" t="s">
-        <v>3179</v>
+        <v>3180</v>
       </c>
       <c r="G3044">
         <v>1759</v>
@@ -35345,10 +35475,10 @@
         <v>1913</v>
       </c>
       <c r="B3045" s="16" t="s">
-        <v>3127</v>
+        <v>3128</v>
       </c>
       <c r="F3045" t="s">
-        <v>3155</v>
+        <v>3156</v>
       </c>
       <c r="G3045">
         <v>1760</v>
@@ -35359,10 +35489,10 @@
         <v>1914</v>
       </c>
       <c r="B3046" t="s">
-        <v>3128</v>
+        <v>3129</v>
       </c>
       <c r="F3046" t="s">
-        <v>3180</v>
+        <v>3181</v>
       </c>
       <c r="G3046">
         <v>1761</v>
@@ -35373,10 +35503,10 @@
         <v>1921</v>
       </c>
       <c r="B3047" s="27" t="s">
-        <v>3129</v>
+        <v>3130</v>
       </c>
       <c r="F3047" t="s">
-        <v>3181</v>
+        <v>3182</v>
       </c>
       <c r="G3047">
         <v>1762</v>
@@ -35387,10 +35517,10 @@
         <v>1926</v>
       </c>
       <c r="B3048" s="16" t="s">
-        <v>3130</v>
+        <v>3131</v>
       </c>
       <c r="F3048" t="s">
-        <v>3154</v>
+        <v>3155</v>
       </c>
       <c r="G3048">
         <v>1763</v>
@@ -35401,7 +35531,7 @@
         <v>1927</v>
       </c>
       <c r="B3049" t="s">
-        <v>3131</v>
+        <v>3132</v>
       </c>
       <c r="F3049" t="s">
         <v>2443</v>
@@ -35415,10 +35545,10 @@
         <v>1928</v>
       </c>
       <c r="B3050" s="27" t="s">
-        <v>3132</v>
+        <v>3133</v>
       </c>
       <c r="F3050" t="s">
-        <v>3179</v>
+        <v>3180</v>
       </c>
       <c r="G3050">
         <v>1765</v>
@@ -35429,10 +35559,10 @@
         <v>1929</v>
       </c>
       <c r="B3051" s="27" t="s">
-        <v>3133</v>
+        <v>3134</v>
       </c>
       <c r="F3051" t="s">
-        <v>3155</v>
+        <v>3156</v>
       </c>
       <c r="G3051">
         <v>1766</v>
@@ -35443,13 +35573,13 @@
         <v>1935</v>
       </c>
       <c r="B3052" s="12" t="s">
-        <v>3134</v>
+        <v>3135</v>
       </c>
       <c r="D3052" t="s">
         <v>2725</v>
       </c>
       <c r="F3052" t="s">
-        <v>3182</v>
+        <v>3183</v>
       </c>
       <c r="G3052">
         <v>1767</v>
@@ -35460,7 +35590,7 @@
         <v>1936</v>
       </c>
       <c r="B3053" s="16" t="s">
-        <v>3135</v>
+        <v>3136</v>
       </c>
       <c r="F3053" t="s">
         <v>2443</v>
@@ -35474,10 +35604,10 @@
         <v>1937</v>
       </c>
       <c r="B3054" t="s">
-        <v>3136</v>
+        <v>3137</v>
       </c>
       <c r="F3054" t="s">
-        <v>3183</v>
+        <v>3184</v>
       </c>
       <c r="G3054">
         <v>1769</v>
@@ -35488,10 +35618,10 @@
         <v>1944</v>
       </c>
       <c r="B3055" s="27" t="s">
-        <v>3137</v>
+        <v>3138</v>
       </c>
       <c r="F3055" t="s">
-        <v>3155</v>
+        <v>3156</v>
       </c>
       <c r="G3055">
         <v>1770</v>
@@ -35502,13 +35632,13 @@
         <v>1950</v>
       </c>
       <c r="B3056" s="12" t="s">
-        <v>3138</v>
+        <v>3139</v>
       </c>
       <c r="D3056" t="s">
         <v>2672</v>
       </c>
       <c r="F3056" t="s">
-        <v>3184</v>
+        <v>3185</v>
       </c>
       <c r="G3056">
         <v>1771</v>
@@ -35519,10 +35649,10 @@
         <v>1951</v>
       </c>
       <c r="B3057" s="27" t="s">
-        <v>3139</v>
+        <v>3140</v>
       </c>
       <c r="F3057" t="s">
-        <v>3185</v>
+        <v>3186</v>
       </c>
       <c r="G3057">
         <v>1772</v>
@@ -35533,13 +35663,13 @@
         <v>1961</v>
       </c>
       <c r="B3058" s="12" t="s">
-        <v>3140</v>
+        <v>3141</v>
       </c>
       <c r="D3058" t="s">
         <v>2674</v>
       </c>
       <c r="F3058" t="s">
-        <v>3154</v>
+        <v>3155</v>
       </c>
       <c r="G3058">
         <v>1773</v>
@@ -35550,7 +35680,7 @@
         <v>1962</v>
       </c>
       <c r="B3059" s="16" t="s">
-        <v>3141</v>
+        <v>3142</v>
       </c>
       <c r="F3059" t="s">
         <v>2443</v>
@@ -35564,10 +35694,10 @@
         <v>1963</v>
       </c>
       <c r="B3060" t="s">
-        <v>3142</v>
+        <v>3143</v>
       </c>
       <c r="F3060" t="s">
-        <v>3183</v>
+        <v>3184</v>
       </c>
       <c r="G3060">
         <v>1775</v>
@@ -35578,10 +35708,10 @@
         <v>1970</v>
       </c>
       <c r="B3061" s="27" t="s">
-        <v>3143</v>
+        <v>3144</v>
       </c>
       <c r="F3061" t="s">
-        <v>3155</v>
+        <v>3156</v>
       </c>
       <c r="G3061">
         <v>1776</v>
@@ -35592,10 +35722,10 @@
         <v>1975</v>
       </c>
       <c r="B3062" s="16" t="s">
-        <v>3144</v>
+        <v>3145</v>
       </c>
       <c r="F3062" t="s">
-        <v>3186</v>
+        <v>3187</v>
       </c>
       <c r="G3062">
         <v>1777</v>
@@ -35606,10 +35736,10 @@
         <v>1976</v>
       </c>
       <c r="B3063" t="s">
-        <v>3145</v>
+        <v>3146</v>
       </c>
       <c r="F3063" s="16" t="s">
-        <v>3187</v>
+        <v>3188</v>
       </c>
       <c r="G3063">
         <v>1778</v>
@@ -35620,10 +35750,10 @@
         <v>1977</v>
       </c>
       <c r="B3064" s="27" t="s">
-        <v>3146</v>
+        <v>3147</v>
       </c>
       <c r="F3064" t="s">
-        <v>3158</v>
+        <v>3159</v>
       </c>
       <c r="G3064">
         <v>1779</v>
@@ -35631,7 +35761,7 @@
     </row>
     <row r="3065" spans="1:7">
       <c r="F3065" t="s">
-        <v>3188</v>
+        <v>3189</v>
       </c>
       <c r="G3065">
         <v>1780</v>
@@ -35653,7 +35783,7 @@
         <v>1782</v>
       </c>
     </row>
-    <row r="3068" spans="1:7">
+    <row r="3068" spans="1:7" ht="16" thickBot="1">
       <c r="F3068" t="s">
         <v>2444</v>
       </c>
@@ -35661,31 +35791,40 @@
         <v>1783</v>
       </c>
     </row>
-    <row r="3069" spans="1:7">
+    <row r="3069" spans="1:7" ht="17" thickTop="1" thickBot="1">
+      <c r="B3069" s="1" t="s">
+        <v>3067</v>
+      </c>
       <c r="F3069" t="s">
-        <v>3155</v>
+        <v>3156</v>
       </c>
       <c r="G3069">
         <v>1784</v>
       </c>
     </row>
-    <row r="3070" spans="1:7">
+    <row r="3070" spans="1:7" ht="16" thickTop="1">
       <c r="F3070" t="s">
-        <v>3189</v>
+        <v>3190</v>
       </c>
       <c r="G3070">
         <v>1785</v>
       </c>
     </row>
     <row r="3071" spans="1:7">
+      <c r="B3071" t="s">
+        <v>127</v>
+      </c>
       <c r="F3071" s="27" t="s">
-        <v>3190</v>
+        <v>3191</v>
       </c>
       <c r="G3071">
         <v>1786</v>
       </c>
     </row>
     <row r="3072" spans="1:7">
+      <c r="B3072" t="s">
+        <v>128</v>
+      </c>
       <c r="F3072" t="s">
         <v>2443</v>
       </c>
@@ -35693,7 +35832,10 @@
         <v>1787</v>
       </c>
     </row>
-    <row r="3073" spans="6:7">
+    <row r="3073" spans="1:7">
+      <c r="B3073" t="s">
+        <v>911</v>
+      </c>
       <c r="F3073" t="s">
         <v>2444</v>
       </c>
@@ -35701,55 +35843,85 @@
         <v>1788</v>
       </c>
     </row>
-    <row r="3074" spans="6:7">
+    <row r="3074" spans="1:7">
+      <c r="B3074" t="s">
+        <v>912</v>
+      </c>
       <c r="F3074" t="s">
-        <v>3155</v>
+        <v>3156</v>
       </c>
       <c r="G3074">
         <v>1789</v>
       </c>
     </row>
-    <row r="3075" spans="6:7">
+    <row r="3075" spans="1:7">
+      <c r="B3075" t="s">
+        <v>2821</v>
+      </c>
       <c r="F3075" t="s">
-        <v>3191</v>
+        <v>3192</v>
       </c>
       <c r="G3075">
         <v>1790</v>
       </c>
     </row>
-    <row r="3076" spans="6:7">
+    <row r="3076" spans="1:7">
       <c r="F3076" t="s">
-        <v>3187</v>
+        <v>3188</v>
       </c>
       <c r="G3076">
         <v>1791</v>
       </c>
     </row>
-    <row r="3077" spans="6:7">
+    <row r="3077" spans="1:7">
+      <c r="A3077" t="s">
+        <v>2081</v>
+      </c>
+      <c r="B3077" t="s">
+        <v>615</v>
+      </c>
       <c r="F3077" t="s">
-        <v>3158</v>
+        <v>3159</v>
       </c>
       <c r="G3077">
         <v>1792</v>
       </c>
     </row>
-    <row r="3078" spans="6:7">
+    <row r="3078" spans="1:7">
+      <c r="A3078">
+        <v>10</v>
+      </c>
+      <c r="B3078" s="27" t="s">
+        <v>2980</v>
+      </c>
       <c r="F3078" s="27" t="s">
-        <v>3192</v>
+        <v>3193</v>
       </c>
       <c r="G3078">
         <v>1793</v>
       </c>
     </row>
-    <row r="3079" spans="6:7">
+    <row r="3079" spans="1:7">
+      <c r="A3079">
+        <v>11</v>
+      </c>
+      <c r="B3079" s="16" t="s">
+        <v>3208</v>
+      </c>
       <c r="F3079" s="27" t="s">
-        <v>3193</v>
+        <v>3194</v>
       </c>
       <c r="G3079">
         <v>1794</v>
       </c>
     </row>
-    <row r="3080" spans="6:7">
+    <row r="3080" spans="1:7">
+      <c r="A3080">
+        <v>12</v>
+      </c>
+      <c r="B3080" t="s">
+        <v>3209</v>
+      </c>
       <c r="F3080" t="s">
         <v>2443</v>
       </c>
@@ -35757,7 +35929,13 @@
         <v>1795</v>
       </c>
     </row>
-    <row r="3081" spans="6:7">
+    <row r="3081" spans="1:7">
+      <c r="A3081">
+        <v>13</v>
+      </c>
+      <c r="B3081" s="48" t="s">
+        <v>3242</v>
+      </c>
       <c r="F3081" t="s">
         <v>2444</v>
       </c>
@@ -35765,71 +35943,125 @@
         <v>1796</v>
       </c>
     </row>
-    <row r="3082" spans="6:7">
+    <row r="3082" spans="1:7">
+      <c r="A3082">
+        <v>18</v>
+      </c>
+      <c r="B3082" s="27" t="s">
+        <v>3066</v>
+      </c>
       <c r="F3082" t="s">
-        <v>3155</v>
+        <v>3156</v>
       </c>
       <c r="G3082">
         <v>1797</v>
       </c>
     </row>
-    <row r="3083" spans="6:7">
+    <row r="3083" spans="1:7">
+      <c r="A3083">
+        <v>745</v>
+      </c>
+      <c r="B3083" s="27" t="s">
+        <v>3210</v>
+      </c>
       <c r="F3083" t="s">
-        <v>3194</v>
+        <v>3195</v>
       </c>
       <c r="G3083">
         <v>1798</v>
       </c>
     </row>
-    <row r="3084" spans="6:7">
+    <row r="3084" spans="1:7">
+      <c r="A3084">
+        <v>757</v>
+      </c>
+      <c r="B3084" s="12" t="s">
+        <v>3211</v>
+      </c>
       <c r="F3084" t="s">
-        <v>3195</v>
+        <v>3196</v>
       </c>
       <c r="G3084">
         <v>1799</v>
       </c>
     </row>
-    <row r="3085" spans="6:7">
+    <row r="3085" spans="1:7">
+      <c r="A3085">
+        <v>779</v>
+      </c>
+      <c r="B3085" s="17" t="s">
+        <v>3212</v>
+      </c>
       <c r="F3085" t="s">
-        <v>3158</v>
+        <v>3159</v>
       </c>
       <c r="G3085">
         <v>1800</v>
       </c>
     </row>
-    <row r="3086" spans="6:7">
+    <row r="3086" spans="1:7">
+      <c r="A3086">
+        <v>780</v>
+      </c>
+      <c r="B3086" s="33" t="s">
+        <v>3213</v>
+      </c>
       <c r="F3086" s="27" t="s">
-        <v>3196</v>
+        <v>3197</v>
       </c>
       <c r="G3086">
         <v>1801</v>
       </c>
     </row>
-    <row r="3087" spans="6:7">
+    <row r="3087" spans="1:7">
+      <c r="A3087">
+        <v>781</v>
+      </c>
+      <c r="B3087" t="s">
+        <v>3214</v>
+      </c>
       <c r="F3087" s="27" t="s">
-        <v>3197</v>
+        <v>3198</v>
       </c>
       <c r="G3087">
         <v>1802</v>
       </c>
     </row>
-    <row r="3088" spans="6:7">
+    <row r="3088" spans="1:7">
+      <c r="A3088">
+        <v>782</v>
+      </c>
+      <c r="B3088" s="48" t="s">
+        <v>3243</v>
+      </c>
       <c r="F3088" t="s">
-        <v>3198</v>
+        <v>3199</v>
       </c>
       <c r="G3088">
         <v>1803</v>
       </c>
     </row>
-    <row r="3089" spans="6:7">
+    <row r="3089" spans="1:7">
+      <c r="A3089">
+        <v>787</v>
+      </c>
+      <c r="B3089" s="27" t="s">
+        <v>3215</v>
+      </c>
       <c r="F3089" t="s">
-        <v>3154</v>
+        <v>3155</v>
       </c>
       <c r="G3089">
         <v>1804</v>
       </c>
     </row>
-    <row r="3090" spans="6:7">
+    <row r="3090" spans="1:7">
+      <c r="A3090">
+        <v>932</v>
+      </c>
+      <c r="B3090" s="47" t="s">
+        <v>3216</v>
+      </c>
       <c r="F3090" t="s">
         <v>2443</v>
       </c>
@@ -35837,7 +36069,13 @@
         <v>1805</v>
       </c>
     </row>
-    <row r="3091" spans="6:7">
+    <row r="3091" spans="1:7">
+      <c r="A3091">
+        <v>946</v>
+      </c>
+      <c r="B3091" s="12" t="s">
+        <v>3217</v>
+      </c>
       <c r="F3091" t="s">
         <v>2444</v>
       </c>
@@ -35845,47 +36083,83 @@
         <v>1806</v>
       </c>
     </row>
-    <row r="3092" spans="6:7">
+    <row r="3092" spans="1:7">
+      <c r="A3092">
+        <v>947</v>
+      </c>
+      <c r="B3092" s="33" t="s">
+        <v>3218</v>
+      </c>
       <c r="F3092" t="s">
-        <v>3155</v>
+        <v>3156</v>
       </c>
       <c r="G3092">
         <v>1807</v>
       </c>
     </row>
-    <row r="3093" spans="6:7">
+    <row r="3093" spans="1:7">
+      <c r="A3093">
+        <v>948</v>
+      </c>
+      <c r="B3093" t="s">
+        <v>3219</v>
+      </c>
       <c r="F3093" t="s">
-        <v>3199</v>
+        <v>3200</v>
       </c>
       <c r="G3093">
         <v>1808</v>
       </c>
     </row>
-    <row r="3094" spans="6:7">
+    <row r="3094" spans="1:7">
+      <c r="A3094">
+        <v>949</v>
+      </c>
+      <c r="B3094" s="48" t="s">
+        <v>3244</v>
+      </c>
       <c r="F3094" t="s">
-        <v>3200</v>
+        <v>3201</v>
       </c>
       <c r="G3094">
         <v>1809</v>
       </c>
     </row>
-    <row r="3095" spans="6:7">
+    <row r="3095" spans="1:7">
+      <c r="A3095">
+        <v>954</v>
+      </c>
+      <c r="B3095" s="27" t="s">
+        <v>3220</v>
+      </c>
       <c r="F3095" t="s">
-        <v>3158</v>
+        <v>3159</v>
       </c>
       <c r="G3095">
         <v>1810</v>
       </c>
     </row>
-    <row r="3096" spans="6:7">
+    <row r="3096" spans="1:7">
+      <c r="A3096">
+        <v>966</v>
+      </c>
+      <c r="B3096" s="12" t="s">
+        <v>3221</v>
+      </c>
       <c r="F3096" t="s">
-        <v>3201</v>
+        <v>3202</v>
       </c>
       <c r="G3096">
         <v>1811</v>
       </c>
     </row>
-    <row r="3097" spans="6:7">
+    <row r="3097" spans="1:7">
+      <c r="A3097">
+        <v>967</v>
+      </c>
+      <c r="B3097" s="47" t="s">
+        <v>3222</v>
+      </c>
       <c r="F3097" t="s">
         <v>2453</v>
       </c>
@@ -35893,7 +36167,13 @@
         <v>1812</v>
       </c>
     </row>
-    <row r="3098" spans="6:7">
+    <row r="3098" spans="1:7">
+      <c r="A3098">
+        <v>972</v>
+      </c>
+      <c r="B3098" s="27" t="s">
+        <v>3223</v>
+      </c>
       <c r="F3098" t="s">
         <v>2443</v>
       </c>
@@ -35901,63 +36181,111 @@
         <v>1813</v>
       </c>
     </row>
-    <row r="3099" spans="6:7">
+    <row r="3099" spans="1:7">
+      <c r="A3099">
+        <v>984</v>
+      </c>
+      <c r="B3099" s="12" t="s">
+        <v>3224</v>
+      </c>
       <c r="F3099" t="s">
-        <v>3160</v>
+        <v>3161</v>
       </c>
       <c r="G3099">
         <v>1814</v>
       </c>
     </row>
-    <row r="3100" spans="6:7">
+    <row r="3100" spans="1:7">
+      <c r="A3100">
+        <v>985</v>
+      </c>
+      <c r="B3100" s="33" t="s">
+        <v>3225</v>
+      </c>
       <c r="F3100" t="s">
-        <v>3155</v>
+        <v>3156</v>
       </c>
       <c r="G3100">
         <v>1815</v>
       </c>
     </row>
-    <row r="3101" spans="6:7">
+    <row r="3101" spans="1:7">
+      <c r="A3101">
+        <v>986</v>
+      </c>
+      <c r="B3101" t="s">
+        <v>3226</v>
+      </c>
       <c r="F3101" t="s">
-        <v>3202</v>
+        <v>3203</v>
       </c>
       <c r="G3101">
         <v>1816</v>
       </c>
     </row>
-    <row r="3102" spans="6:7">
+    <row r="3102" spans="1:7">
+      <c r="A3102">
+        <v>987</v>
+      </c>
+      <c r="B3102" s="48" t="s">
+        <v>3245</v>
+      </c>
       <c r="F3102" s="27" t="s">
-        <v>3203</v>
+        <v>3204</v>
       </c>
       <c r="G3102">
         <v>1817</v>
       </c>
     </row>
-    <row r="3103" spans="6:7">
+    <row r="3103" spans="1:7">
+      <c r="A3103">
+        <v>1226</v>
+      </c>
+      <c r="B3103" s="27" t="s">
+        <v>3227</v>
+      </c>
       <c r="F3103" s="27" t="s">
-        <v>3204</v>
+        <v>3205</v>
       </c>
       <c r="G3103">
         <v>1818</v>
       </c>
     </row>
-    <row r="3104" spans="6:7">
+    <row r="3104" spans="1:7">
+      <c r="A3104">
+        <v>1251</v>
+      </c>
+      <c r="B3104" s="27" t="s">
+        <v>3228</v>
+      </c>
       <c r="F3104" t="s">
-        <v>3205</v>
+        <v>3206</v>
       </c>
       <c r="G3104">
         <v>1819</v>
       </c>
     </row>
-    <row r="3105" spans="6:7">
+    <row r="3105" spans="1:7">
+      <c r="A3105">
+        <v>1312</v>
+      </c>
+      <c r="B3105" s="27" t="s">
+        <v>3229</v>
+      </c>
       <c r="F3105" t="s">
-        <v>3154</v>
+        <v>3155</v>
       </c>
       <c r="G3105">
         <v>1820</v>
       </c>
     </row>
-    <row r="3106" spans="6:7">
+    <row r="3106" spans="1:7">
+      <c r="A3106">
+        <v>1337</v>
+      </c>
+      <c r="B3106" s="27" t="s">
+        <v>3230</v>
+      </c>
       <c r="F3106" t="s">
         <v>2443</v>
       </c>
@@ -35965,33 +36293,123 @@
         <v>1821</v>
       </c>
     </row>
-    <row r="3107" spans="6:7">
+    <row r="3107" spans="1:7">
+      <c r="A3107">
+        <v>1368</v>
+      </c>
+      <c r="B3107" s="47" t="s">
+        <v>3231</v>
+      </c>
       <c r="F3107" t="s">
-        <v>3160</v>
+        <v>3161</v>
       </c>
       <c r="G3107">
         <v>1822</v>
       </c>
     </row>
-    <row r="3108" spans="6:7">
+    <row r="3108" spans="1:7">
+      <c r="A3108">
+        <v>1374</v>
+      </c>
+      <c r="B3108" s="12" t="s">
+        <v>3232</v>
+      </c>
       <c r="F3108" t="s">
-        <v>3155</v>
+        <v>3156</v>
       </c>
       <c r="G3108">
         <v>1823</v>
       </c>
     </row>
-    <row r="3109" spans="6:7">
+    <row r="3109" spans="1:7">
+      <c r="A3109">
+        <v>1384</v>
+      </c>
+      <c r="B3109" s="12" t="s">
+        <v>3233</v>
+      </c>
       <c r="F3109" t="s">
-        <v>3206</v>
+        <v>3207</v>
       </c>
       <c r="G3109">
         <v>1824</v>
       </c>
     </row>
+    <row r="3110" spans="1:7">
+      <c r="A3110">
+        <v>1394</v>
+      </c>
+      <c r="B3110" s="12" t="s">
+        <v>3234</v>
+      </c>
+    </row>
+    <row r="3111" spans="1:7">
+      <c r="A3111">
+        <v>1395</v>
+      </c>
+      <c r="B3111" s="16" t="s">
+        <v>3235</v>
+      </c>
+    </row>
+    <row r="3112" spans="1:7">
+      <c r="A3112">
+        <v>1396</v>
+      </c>
+      <c r="B3112" t="s">
+        <v>3236</v>
+      </c>
+    </row>
+    <row r="3113" spans="1:7">
+      <c r="A3113">
+        <v>1397</v>
+      </c>
+      <c r="B3113" s="48" t="s">
+        <v>3246</v>
+      </c>
+    </row>
+    <row r="3114" spans="1:7">
+      <c r="A3114">
+        <v>1402</v>
+      </c>
+      <c r="B3114" s="27" t="s">
+        <v>3237</v>
+      </c>
+    </row>
+    <row r="3115" spans="1:7">
+      <c r="A3115">
+        <v>1403</v>
+      </c>
+      <c r="B3115" s="27" t="s">
+        <v>3238</v>
+      </c>
+    </row>
+    <row r="3116" spans="1:7">
+      <c r="A3116">
+        <v>1408</v>
+      </c>
+      <c r="B3116" s="33" t="s">
+        <v>3239</v>
+      </c>
+    </row>
+    <row r="3117" spans="1:7">
+      <c r="A3117">
+        <v>1409</v>
+      </c>
+      <c r="B3117" t="s">
+        <v>3240</v>
+      </c>
+    </row>
+    <row r="3118" spans="1:7">
+      <c r="A3118">
+        <v>1410</v>
+      </c>
+      <c r="B3118" s="27" t="s">
+        <v>3241</v>
+      </c>
+    </row>
   </sheetData>
-  <sortState ref="A2844:B2889">
-    <sortCondition ref="A2844:A2889"/>
+  <sortState ref="A3078:B3118">
+    <sortCondition ref="A3078:A3118"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -38470,13 +38888,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="23" thickTop="1" thickBot="1">
-      <c r="A1" s="33" t="s">
+      <c r="A1" s="34" t="s">
         <v>2926</v>
       </c>
-      <c r="B1" s="33" t="s">
+      <c r="B1" s="34" t="s">
         <v>2886</v>
       </c>
-      <c r="C1" s="33" t="s">
+      <c r="C1" s="34" t="s">
         <v>617</v>
       </c>
       <c r="D1" s="1" t="s">
@@ -38508,7 +38926,7 @@
       <c r="C2" s="21" t="s">
         <v>2922</v>
       </c>
-      <c r="D2" s="39" t="s">
+      <c r="D2" s="40" t="s">
         <v>2889</v>
       </c>
       <c r="E2" s="31" t="s">
@@ -38531,16 +38949,16 @@
       </c>
     </row>
     <row r="3" spans="1:14" ht="21">
-      <c r="A3" s="34" t="s">
+      <c r="A3" s="35" t="s">
         <v>2923</v>
       </c>
-      <c r="B3" s="37" t="s">
+      <c r="B3" s="38" t="s">
         <v>2932</v>
       </c>
-      <c r="C3" s="38" t="s">
+      <c r="C3" s="39" t="s">
         <v>2931</v>
       </c>
-      <c r="D3" s="39" t="s">
+      <c r="D3" s="40" t="s">
         <v>2889</v>
       </c>
       <c r="E3" s="31" t="s">
@@ -38563,16 +38981,16 @@
       </c>
     </row>
     <row r="4" spans="1:14" ht="21">
-      <c r="A4" s="34" t="s">
+      <c r="A4" s="35" t="s">
         <v>2923</v>
       </c>
-      <c r="B4" s="37" t="s">
+      <c r="B4" s="38" t="s">
         <v>2936</v>
       </c>
-      <c r="C4" s="38" t="s">
+      <c r="C4" s="39" t="s">
         <v>2937</v>
       </c>
-      <c r="D4" s="39" t="s">
+      <c r="D4" s="40" t="s">
         <v>2897</v>
       </c>
       <c r="E4" s="31" t="s">
@@ -38595,16 +39013,16 @@
       </c>
     </row>
     <row r="5" spans="1:14" ht="21">
-      <c r="A5" s="34" t="s">
+      <c r="A5" s="35" t="s">
         <v>2923</v>
       </c>
-      <c r="B5" s="37" t="s">
+      <c r="B5" s="38" t="s">
         <v>2939</v>
       </c>
-      <c r="C5" s="38" t="s">
+      <c r="C5" s="39" t="s">
         <v>2950</v>
       </c>
-      <c r="D5" s="39" t="s">
+      <c r="D5" s="40" t="s">
         <v>2897</v>
       </c>
       <c r="E5" s="31" t="s">
@@ -38627,16 +39045,16 @@
       </c>
     </row>
     <row r="6" spans="1:14" ht="21">
-      <c r="A6" s="34" t="s">
+      <c r="A6" s="35" t="s">
         <v>2923</v>
       </c>
-      <c r="B6" s="40" t="s">
+      <c r="B6" s="41" t="s">
         <v>2941</v>
       </c>
       <c r="C6" s="21" t="s">
         <v>2948</v>
       </c>
-      <c r="D6" s="39" t="s">
+      <c r="D6" s="40" t="s">
         <v>2889</v>
       </c>
       <c r="E6" s="31" t="s">
@@ -38659,16 +39077,16 @@
       </c>
     </row>
     <row r="7" spans="1:14" ht="21">
-      <c r="A7" s="34" t="s">
+      <c r="A7" s="35" t="s">
         <v>2923</v>
       </c>
-      <c r="B7" s="37" t="s">
+      <c r="B7" s="38" t="s">
         <v>2943</v>
       </c>
       <c r="C7" s="21" t="s">
         <v>2949</v>
       </c>
-      <c r="D7" s="39" t="s">
+      <c r="D7" s="40" t="s">
         <v>2897</v>
       </c>
       <c r="E7" s="31" t="s">
@@ -38694,13 +39112,13 @@
       <c r="A8" s="21" t="s">
         <v>2881</v>
       </c>
-      <c r="B8" s="36" t="s">
+      <c r="B8" s="37" t="s">
         <v>2876</v>
       </c>
       <c r="C8" s="21" t="s">
         <v>2877</v>
       </c>
-      <c r="D8" s="39" t="s">
+      <c r="D8" s="40" t="s">
         <v>2897</v>
       </c>
       <c r="E8" s="31" t="s">
@@ -38723,16 +39141,16 @@
       </c>
     </row>
     <row r="9" spans="1:14" ht="21">
-      <c r="A9" s="34" t="s">
+      <c r="A9" s="35" t="s">
         <v>2881</v>
       </c>
-      <c r="B9" s="36" t="s">
+      <c r="B9" s="37" t="s">
         <v>2874</v>
       </c>
       <c r="C9" s="21" t="s">
         <v>2875</v>
       </c>
-      <c r="D9" s="39" t="s">
+      <c r="D9" s="40" t="s">
         <v>2889</v>
       </c>
       <c r="E9" s="31" t="s">
@@ -38758,13 +39176,13 @@
       <c r="A10" s="21" t="s">
         <v>2881</v>
       </c>
-      <c r="B10" s="36" t="s">
+      <c r="B10" s="37" t="s">
         <v>2866</v>
       </c>
       <c r="C10" s="21" t="s">
         <v>2867</v>
       </c>
-      <c r="D10" s="39" t="s">
+      <c r="D10" s="40" t="s">
         <v>2897</v>
       </c>
       <c r="E10" s="31" t="s">
@@ -38781,7 +39199,7 @@
       <c r="C11" s="21" t="s">
         <v>2922</v>
       </c>
-      <c r="D11" s="39" t="s">
+      <c r="D11" s="40" t="s">
         <v>2889</v>
       </c>
       <c r="E11" s="31" t="s">
@@ -38795,13 +39213,13 @@
       <c r="A12" s="21" t="s">
         <v>2880</v>
       </c>
-      <c r="B12" s="36" t="s">
+      <c r="B12" s="37" t="s">
         <v>2883</v>
       </c>
       <c r="C12" s="21" t="s">
         <v>2884</v>
       </c>
-      <c r="D12" s="39" t="s">
+      <c r="D12" s="40" t="s">
         <v>2897</v>
       </c>
       <c r="E12" s="31" t="s">
@@ -38812,16 +39230,16 @@
       </c>
     </row>
     <row r="13" spans="1:14" ht="21">
-      <c r="A13" s="34" t="s">
+      <c r="A13" s="35" t="s">
         <v>2880</v>
       </c>
-      <c r="B13" s="36" t="s">
+      <c r="B13" s="37" t="s">
         <v>2878</v>
       </c>
       <c r="C13" s="21" t="s">
         <v>2879</v>
       </c>
-      <c r="D13" s="39" t="s">
+      <c r="D13" s="40" t="s">
         <v>2897</v>
       </c>
       <c r="E13" s="31" t="s">
@@ -38832,16 +39250,16 @@
       </c>
     </row>
     <row r="14" spans="1:14" ht="21">
-      <c r="A14" s="34" t="s">
+      <c r="A14" s="35" t="s">
         <v>2880</v>
       </c>
-      <c r="B14" s="36" t="s">
+      <c r="B14" s="37" t="s">
         <v>2870</v>
       </c>
       <c r="C14" s="21" t="s">
         <v>2871</v>
       </c>
-      <c r="D14" s="39" t="s">
+      <c r="D14" s="40" t="s">
         <v>2889</v>
       </c>
       <c r="E14" s="31" t="s">
@@ -38852,13 +39270,13 @@
       <c r="A15" s="21" t="s">
         <v>2880</v>
       </c>
-      <c r="B15" s="36" t="s">
+      <c r="B15" s="37" t="s">
         <v>2868</v>
       </c>
       <c r="C15" s="21" t="s">
         <v>2869</v>
       </c>
-      <c r="D15" s="41" t="s">
+      <c r="D15" s="42" t="s">
         <v>2897</v>
       </c>
       <c r="E15" s="31" t="s">
@@ -38889,13 +39307,13 @@
       <c r="A16" s="21" t="s">
         <v>2880</v>
       </c>
-      <c r="B16" s="35" t="s">
+      <c r="B16" s="36" t="s">
         <v>2898</v>
       </c>
       <c r="C16" s="21" t="s">
         <v>2913</v>
       </c>
-      <c r="D16" s="39" t="s">
+      <c r="D16" s="40" t="s">
         <v>2897</v>
       </c>
       <c r="E16" s="31" t="s">
@@ -38923,16 +39341,16 @@
       </c>
     </row>
     <row r="17" spans="1:14" ht="21">
-      <c r="A17" s="34" t="s">
+      <c r="A17" s="35" t="s">
         <v>2880</v>
       </c>
-      <c r="B17" s="36" t="s">
+      <c r="B17" s="37" t="s">
         <v>2914</v>
       </c>
       <c r="C17" s="21" t="s">
         <v>2915</v>
       </c>
-      <c r="D17" s="39" t="s">
+      <c r="D17" s="40" t="s">
         <v>2889</v>
       </c>
       <c r="E17" s="31" t="s">
@@ -38963,13 +39381,13 @@
       <c r="A18" s="21" t="s">
         <v>2880</v>
       </c>
-      <c r="B18" s="36" t="s">
+      <c r="B18" s="37" t="s">
         <v>2917</v>
       </c>
       <c r="C18" s="21" t="s">
         <v>2916</v>
       </c>
-      <c r="D18" s="39" t="s">
+      <c r="D18" s="40" t="s">
         <v>2897</v>
       </c>
       <c r="E18" s="31" t="s">
@@ -39000,7 +39418,7 @@
       <c r="A19" s="21" t="s">
         <v>2880</v>
       </c>
-      <c r="B19" s="36" t="s">
+      <c r="B19" s="37" t="s">
         <v>2919</v>
       </c>
       <c r="C19" s="21" t="s">
@@ -39037,13 +39455,13 @@
       <c r="A20" s="21" t="s">
         <v>2880</v>
       </c>
-      <c r="B20" s="36" t="s">
+      <c r="B20" s="37" t="s">
         <v>2921</v>
       </c>
       <c r="C20" s="21" t="s">
         <v>2920</v>
       </c>
-      <c r="D20" s="39" t="s">
+      <c r="D20" s="40" t="s">
         <v>2889</v>
       </c>
       <c r="E20" s="31" t="s">
@@ -39074,19 +39492,19 @@
       <c r="A21" s="21" t="s">
         <v>2880</v>
       </c>
-      <c r="B21" s="36" t="s">
+      <c r="B21" s="37" t="s">
         <v>2924</v>
       </c>
       <c r="C21" s="21" t="s">
         <v>2925</v>
       </c>
-      <c r="D21" s="39" t="s">
+      <c r="D21" s="40" t="s">
         <v>2909</v>
       </c>
       <c r="E21" s="31" t="s">
         <v>2963</v>
       </c>
-      <c r="F21" s="39" t="s">
+      <c r="F21" s="40" t="s">
         <v>2897</v>
       </c>
       <c r="G21" s="21" t="s">
@@ -39108,22 +39526,22 @@
       </c>
     </row>
     <row r="22" spans="1:14" ht="21">
-      <c r="A22" s="34" t="s">
+      <c r="A22" s="35" t="s">
         <v>2880</v>
       </c>
-      <c r="B22" s="37" t="s">
+      <c r="B22" s="38" t="s">
         <v>2927</v>
       </c>
-      <c r="C22" s="38" t="s">
+      <c r="C22" s="39" t="s">
         <v>2928</v>
       </c>
-      <c r="D22" s="39" t="s">
+      <c r="D22" s="40" t="s">
         <v>2889</v>
       </c>
       <c r="E22" s="31" t="s">
         <v>2929</v>
       </c>
-      <c r="F22" s="39" t="s">
+      <c r="F22" s="40" t="s">
         <v>2889</v>
       </c>
       <c r="G22" s="21" t="s">
@@ -39145,22 +39563,22 @@
       </c>
     </row>
     <row r="23" spans="1:14" ht="21">
-      <c r="A23" s="34" t="s">
+      <c r="A23" s="35" t="s">
         <v>2882</v>
       </c>
-      <c r="B23" s="35" t="s">
+      <c r="B23" s="36" t="s">
         <v>2872</v>
       </c>
       <c r="C23" s="21" t="s">
         <v>2873</v>
       </c>
-      <c r="D23" s="39" t="s">
+      <c r="D23" s="40" t="s">
         <v>2897</v>
       </c>
       <c r="E23" s="31" t="s">
         <v>2908</v>
       </c>
-      <c r="F23" s="39" t="s">
+      <c r="F23" s="40" t="s">
         <v>2897</v>
       </c>
       <c r="G23" s="21" t="s">
@@ -39182,22 +39600,22 @@
       </c>
     </row>
     <row r="24" spans="1:14" ht="21">
-      <c r="A24" s="34" t="s">
+      <c r="A24" s="35" t="s">
         <v>2882</v>
       </c>
-      <c r="B24" s="35" t="s">
+      <c r="B24" s="36" t="s">
         <v>2862</v>
       </c>
       <c r="C24" s="21" t="s">
         <v>2863</v>
       </c>
-      <c r="D24" s="39" t="s">
+      <c r="D24" s="40" t="s">
         <v>2889</v>
       </c>
       <c r="E24" s="31" t="s">
         <v>2952</v>
       </c>
-      <c r="F24" s="39" t="s">
+      <c r="F24" s="40" t="s">
         <v>2897</v>
       </c>
       <c r="G24" s="21" t="s">
@@ -39222,19 +39640,19 @@
       <c r="A25" s="21" t="s">
         <v>2882</v>
       </c>
-      <c r="B25" s="35" t="s">
+      <c r="B25" s="36" t="s">
         <v>2864</v>
       </c>
       <c r="C25" s="21" t="s">
         <v>2865</v>
       </c>
-      <c r="D25" s="39" t="s">
+      <c r="D25" s="40" t="s">
         <v>2889</v>
       </c>
       <c r="E25" s="31" t="s">
         <v>2953</v>
       </c>
-      <c r="F25" s="39" t="s">
+      <c r="F25" s="40" t="s">
         <v>2897</v>
       </c>
       <c r="G25" s="21" t="s">
@@ -39256,7 +39674,7 @@
       </c>
     </row>
     <row r="26" spans="1:14" ht="21">
-      <c r="F26" s="39" t="s">
+      <c r="F26" s="40" t="s">
         <v>2889</v>
       </c>
       <c r="G26" s="21" t="s">
@@ -39278,7 +39696,7 @@
       </c>
     </row>
     <row r="27" spans="1:14" ht="21">
-      <c r="F27" s="41" t="s">
+      <c r="F27" s="42" t="s">
         <v>2897</v>
       </c>
       <c r="G27" s="21" t="s">
@@ -39300,7 +39718,7 @@
       </c>
     </row>
     <row r="28" spans="1:14" ht="21">
-      <c r="F28" s="39" t="s">
+      <c r="F28" s="40" t="s">
         <v>2889</v>
       </c>
       <c r="G28" s="21" t="s">
@@ -39323,7 +39741,7 @@
       </c>
     </row>
     <row r="29" spans="1:14" ht="21">
-      <c r="F29" s="39" t="s">
+      <c r="F29" s="40" t="s">
         <v>2897</v>
       </c>
       <c r="G29" s="21" t="s">
@@ -39367,7 +39785,7 @@
       </c>
     </row>
     <row r="31" spans="1:14" ht="21">
-      <c r="F31" s="39" t="s">
+      <c r="F31" s="40" t="s">
         <v>2889</v>
       </c>
       <c r="G31" s="21" t="s">
@@ -39389,7 +39807,7 @@
       </c>
     </row>
     <row r="32" spans="1:14" ht="21">
-      <c r="F32" s="39" t="s">
+      <c r="F32" s="40" t="s">
         <v>2909</v>
       </c>
       <c r="G32" s="21" t="s">

</xml_diff>

<commit_message>
still an issue with clockwise doing down the drain
</commit_message>
<xml_diff>
--- a/RBG_arduino/StateTable_minimal.xlsx
+++ b/RBG_arduino/StateTable_minimal.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/markdolson/GitHub-Mark-MDO47/RubberBandGun/RBG_arduino/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7D3CC22-F369-5040-9540-2F0C62766DCA}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FCFE5D8C-D357-2D48-9AA5-3FB04C7EEC96}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-40" yWindow="480" windowWidth="25600" windowHeight="15540" activeTab="2" xr2:uid="{CCADFEE4-B0E1-4363-9617-1683960BED03}"/>
+    <workbookView xWindow="-40" yWindow="480" windowWidth="25600" windowHeight="15540" xr2:uid="{CCADFEE4-B0E1-4363-9617-1683960BED03}"/>
   </bookViews>
   <sheets>
     <sheet name="StateTable" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4339" uniqueCount="3247">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4349" uniqueCount="3248">
   <si>
     <t>trigOnly</t>
   </si>
@@ -10009,6 +10009,9 @@
   </si>
   <si>
     <t>1397: RBG_startEffectLED ln 552 EFCT num 102 final LED num 102 loopCount 263</t>
+  </si>
+  <si>
+    <t>#define mROW_POWERON 0  // first address in myStateTable[]</t>
   </si>
 </sst>
 </file>
@@ -10695,11 +10698,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{90E8DFC6-94F4-4A82-A874-2F16F2CF0145}">
-  <dimension ref="A1:R28"/>
+  <dimension ref="A1:S28"/>
   <sheetViews>
-    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I28" sqref="I28"/>
+      <selection pane="bottomLeft" activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
@@ -10713,16 +10716,17 @@
     <col min="8" max="8" width="20" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="16" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="23.5" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="8" customWidth="1"/>
-    <col min="12" max="12" width="19.33203125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="16" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="16" customWidth="1"/>
-    <col min="15" max="15" width="8.5" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="20" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="12.83203125" customWidth="1"/>
+    <col min="11" max="11" width="23.5" customWidth="1"/>
+    <col min="12" max="12" width="8" customWidth="1"/>
+    <col min="13" max="13" width="19.33203125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="16" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="16" customWidth="1"/>
+    <col min="16" max="16" width="8.5" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="20" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="12.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" ht="17" thickTop="1" thickBot="1">
+    <row r="1" spans="1:19" ht="17" thickTop="1" thickBot="1">
       <c r="A1" s="4" t="s">
         <v>8</v>
       </c>
@@ -10753,27 +10757,28 @@
       <c r="J1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="L1" s="5" t="s">
+      <c r="K1" s="1"/>
+      <c r="M1" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="M1" s="5" t="s">
+      <c r="N1" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="N1" s="6"/>
-      <c r="O1" s="5" t="s">
+      <c r="O1" s="6"/>
+      <c r="P1" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="P1" s="5" t="s">
+      <c r="Q1" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="R1" t="s">
         <v>7</v>
       </c>
-      <c r="R1" s="8" t="s">
+      <c r="S1" s="8" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="2" spans="1:18" ht="49" thickTop="1">
+    <row r="2" spans="1:19" ht="49" thickTop="1">
       <c r="A2" s="10" t="s">
         <v>54</v>
       </c>
@@ -10796,23 +10801,26 @@
       <c r="J2" s="9" t="s">
         <v>65</v>
       </c>
-      <c r="L2" t="s">
+      <c r="K2" s="9" t="s">
+        <v>3247</v>
+      </c>
+      <c r="M2" t="s">
         <v>9</v>
       </c>
-      <c r="M2" t="s">
+      <c r="N2" t="s">
         <v>21</v>
       </c>
-      <c r="O2" t="s">
+      <c r="P2" t="s">
         <v>43</v>
       </c>
-      <c r="P2" t="s">
+      <c r="Q2" t="s">
         <v>51</v>
       </c>
-      <c r="R2" t="s">
+      <c r="S2" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="3" spans="1:18">
+    <row r="3" spans="1:19">
       <c r="A3" s="9"/>
       <c r="B3" s="9"/>
       <c r="C3" s="9"/>
@@ -10823,23 +10831,23 @@
       <c r="H3" s="9"/>
       <c r="I3" s="9"/>
       <c r="J3" s="9"/>
-      <c r="L3" t="s">
+      <c r="M3" t="s">
         <v>10</v>
       </c>
-      <c r="M3" t="s">
+      <c r="N3" t="s">
         <v>22</v>
       </c>
-      <c r="O3" t="s">
+      <c r="P3" t="s">
         <v>47</v>
       </c>
-      <c r="P3" t="s">
+      <c r="Q3" t="s">
         <v>50</v>
       </c>
-      <c r="R3" t="s">
+      <c r="S3" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="4" spans="1:18">
+    <row r="4" spans="1:19">
       <c r="A4" s="9"/>
       <c r="B4" s="9" t="s">
         <v>2741</v>
@@ -10858,26 +10866,29 @@
         <v>2558</v>
       </c>
       <c r="J4" s="9"/>
-      <c r="L4" t="s">
+      <c r="K4" s="9" t="s">
+        <v>2672</v>
+      </c>
+      <c r="M4" t="s">
         <v>11</v>
       </c>
-      <c r="M4" t="s">
+      <c r="N4" t="s">
         <v>23</v>
       </c>
-      <c r="O4" t="s">
+      <c r="P4" t="s">
         <v>44</v>
       </c>
-      <c r="P4" t="s">
+      <c r="Q4" t="s">
         <v>52</v>
       </c>
-      <c r="Q4" t="s">
+      <c r="R4" t="s">
         <v>32</v>
       </c>
-      <c r="R4" t="s">
+      <c r="S4" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="5" spans="1:18">
+    <row r="5" spans="1:19">
       <c r="A5" s="9"/>
       <c r="B5" s="9" t="s">
         <v>2741</v>
@@ -10896,17 +10907,17 @@
         <v>2557</v>
       </c>
       <c r="J5" s="9"/>
-      <c r="L5" t="s">
+      <c r="M5" t="s">
         <v>12</v>
       </c>
-      <c r="M5" t="s">
+      <c r="N5" t="s">
         <v>24</v>
       </c>
-      <c r="O5" t="s">
+      <c r="P5" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="6" spans="1:18">
+    <row r="6" spans="1:19">
       <c r="A6" s="9"/>
       <c r="B6" s="9"/>
       <c r="C6" s="9" t="s">
@@ -10919,20 +10930,23 @@
       <c r="H6" s="9"/>
       <c r="I6" s="9"/>
       <c r="J6" s="9"/>
-      <c r="L6" t="s">
+      <c r="K6" s="9" t="s">
+        <v>2673</v>
+      </c>
+      <c r="M6" t="s">
         <v>13</v>
       </c>
-      <c r="M6" t="s">
+      <c r="N6" t="s">
         <v>25</v>
       </c>
-      <c r="O6" t="s">
+      <c r="P6" t="s">
         <v>46</v>
       </c>
-      <c r="P6" t="s">
+      <c r="Q6" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="7" spans="1:18" ht="16">
+    <row r="7" spans="1:19" ht="16">
       <c r="A7" s="9"/>
       <c r="B7" s="10" t="s">
         <v>61</v>
@@ -10955,17 +10969,17 @@
         <v>77</v>
       </c>
       <c r="J7" s="9"/>
-      <c r="L7" t="s">
+      <c r="M7" t="s">
         <v>14</v>
       </c>
-      <c r="M7" t="s">
+      <c r="N7" t="s">
         <v>26</v>
       </c>
-      <c r="O7" t="s">
+      <c r="P7" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="8" spans="1:18" ht="16">
+    <row r="8" spans="1:19" ht="16">
       <c r="A8" s="9"/>
       <c r="B8" s="9" t="s">
         <v>61</v>
@@ -10988,17 +11002,17 @@
         <v>68</v>
       </c>
       <c r="J8" s="9"/>
-      <c r="L8" t="s">
+      <c r="M8" t="s">
         <v>15</v>
       </c>
-      <c r="M8" t="s">
+      <c r="N8" t="s">
         <v>27</v>
       </c>
-      <c r="O8" t="s">
+      <c r="P8" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="9" spans="1:18">
+    <row r="9" spans="1:19">
       <c r="A9" s="9"/>
       <c r="B9" s="9"/>
       <c r="C9" s="9" t="s">
@@ -11011,17 +11025,17 @@
       <c r="H9" s="9"/>
       <c r="I9" s="9"/>
       <c r="J9" s="9"/>
-      <c r="L9" s="2" t="s">
+      <c r="M9" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="M9" t="s">
+      <c r="N9" t="s">
         <v>28</v>
       </c>
-      <c r="O9" t="s">
+      <c r="P9" t="s">
         <v>2559</v>
       </c>
     </row>
-    <row r="10" spans="1:18" ht="16">
+    <row r="10" spans="1:19" ht="16">
       <c r="A10" s="9"/>
       <c r="B10" s="10" t="s">
         <v>61</v>
@@ -11044,17 +11058,20 @@
         <v>77</v>
       </c>
       <c r="J10" s="9"/>
-      <c r="L10" s="2" t="s">
+      <c r="K10" s="9" t="s">
+        <v>2674</v>
+      </c>
+      <c r="M10" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="M10" t="s">
+      <c r="N10" t="s">
         <v>29</v>
       </c>
-      <c r="O10" t="s">
+      <c r="P10" t="s">
         <v>2560</v>
       </c>
     </row>
-    <row r="11" spans="1:18" ht="16">
+    <row r="11" spans="1:19" ht="16">
       <c r="A11" s="9"/>
       <c r="B11" s="9" t="s">
         <v>61</v>
@@ -11077,14 +11094,14 @@
         <v>67</v>
       </c>
       <c r="J11" s="9"/>
-      <c r="L11" t="s">
+      <c r="M11" t="s">
         <v>18</v>
       </c>
-      <c r="M11" t="s">
+      <c r="N11" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="12" spans="1:18">
+    <row r="12" spans="1:19">
       <c r="A12" s="9"/>
       <c r="B12" s="9"/>
       <c r="C12" s="9"/>
@@ -11095,14 +11112,14 @@
       <c r="H12" s="9"/>
       <c r="I12" s="9"/>
       <c r="J12" s="9"/>
-      <c r="L12" s="4" t="s">
+      <c r="M12" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="M12" s="4" t="s">
+      <c r="N12" s="4" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="13" spans="1:18">
+    <row r="13" spans="1:19">
       <c r="A13" s="9"/>
       <c r="B13" s="9"/>
       <c r="C13" s="9"/>
@@ -11114,7 +11131,7 @@
       <c r="I13" s="9"/>
       <c r="J13" s="9"/>
     </row>
-    <row r="14" spans="1:18">
+    <row r="14" spans="1:19">
       <c r="A14" t="s">
         <v>80</v>
       </c>
@@ -11133,11 +11150,14 @@
       <c r="J14" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="15" spans="1:18">
+      <c r="K14" s="9" t="s">
+        <v>2675</v>
+      </c>
+    </row>
+    <row r="15" spans="1:19">
       <c r="C15" s="9"/>
     </row>
-    <row r="16" spans="1:18" ht="48">
+    <row r="16" spans="1:19" ht="48">
       <c r="A16" t="s">
         <v>73</v>
       </c>
@@ -11150,12 +11170,15 @@
       <c r="J16" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="17" spans="1:14">
+      <c r="K16" s="9" t="s">
+        <v>2676</v>
+      </c>
+    </row>
+    <row r="17" spans="1:15">
       <c r="B17" s="10"/>
       <c r="C17" s="9"/>
     </row>
-    <row r="18" spans="1:14">
+    <row r="18" spans="1:15">
       <c r="A18" t="s">
         <v>76</v>
       </c>
@@ -11174,15 +11197,18 @@
       <c r="J18" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="19" spans="1:14">
+      <c r="K18" s="9" t="s">
+        <v>2677</v>
+      </c>
+    </row>
+    <row r="19" spans="1:15">
       <c r="B19" s="10"/>
       <c r="C19" s="9"/>
     </row>
-    <row r="20" spans="1:14">
+    <row r="20" spans="1:15">
       <c r="C20" s="9"/>
     </row>
-    <row r="21" spans="1:14" ht="48">
+    <row r="21" spans="1:15" ht="48">
       <c r="A21" t="s">
         <v>74</v>
       </c>
@@ -11197,12 +11223,15 @@
       <c r="J21" s="9" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="22" spans="1:14">
+      <c r="K21" s="9" t="s">
+        <v>2678</v>
+      </c>
+    </row>
+    <row r="22" spans="1:15">
       <c r="B22" s="10"/>
       <c r="D22" s="3"/>
     </row>
-    <row r="23" spans="1:14" ht="16">
+    <row r="23" spans="1:15" ht="16">
       <c r="A23" t="s">
         <v>62</v>
       </c>
@@ -11225,8 +11254,11 @@
       <c r="J23" s="9" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="24" spans="1:14" ht="16">
+      <c r="K23" s="9" t="s">
+        <v>2679</v>
+      </c>
+    </row>
+    <row r="24" spans="1:15" ht="16">
       <c r="A24" s="9"/>
       <c r="B24" s="9" t="s">
         <v>2738</v>
@@ -11250,13 +11282,13 @@
       </c>
       <c r="J24" s="9"/>
     </row>
-    <row r="25" spans="1:14" s="28" customFormat="1">
+    <row r="25" spans="1:15" s="28" customFormat="1">
       <c r="F25" s="43"/>
       <c r="G25" s="43"/>
       <c r="H25" s="43"/>
       <c r="I25" s="43"/>
     </row>
-    <row r="26" spans="1:14" ht="16">
+    <row r="26" spans="1:15" ht="16">
       <c r="A26" s="9" t="s">
         <v>63</v>
       </c>
@@ -11275,8 +11307,11 @@
       <c r="J26" s="9" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="27" spans="1:14" ht="16">
+      <c r="K26" s="9" t="s">
+        <v>2725</v>
+      </c>
+    </row>
+    <row r="27" spans="1:15" ht="16">
       <c r="B27" s="9" t="s">
         <v>2738</v>
       </c>
@@ -11296,7 +11331,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="28" spans="1:14" ht="16">
+    <row r="28" spans="1:15" ht="16">
       <c r="B28" s="9" t="s">
         <v>2738</v>
       </c>
@@ -11315,11 +11350,11 @@
       <c r="I28" s="9" t="s">
         <v>77</v>
       </c>
-      <c r="N28" s="7"/>
+      <c r="O28" s="7"/>
     </row>
   </sheetData>
-  <sortState ref="R3:R67">
-    <sortCondition ref="R3:R67"/>
+  <sortState ref="S3:S67">
+    <sortCondition ref="S3:S67"/>
   </sortState>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -11513,8 +11548,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F57F550E-21B4-4ED7-B7FF-211D228584A7}">
   <dimension ref="A1:L3118"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3078" workbookViewId="0">
-      <selection activeCell="B3081" sqref="B3081"/>
+    <sheetView topLeftCell="A3076" workbookViewId="0">
+      <selection activeCell="B3069" sqref="B3069"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>

</xml_diff>

<commit_message>
rework the LED routines; after a while reaches one that doesn't move
</commit_message>
<xml_diff>
--- a/RBG_arduino/StateTable_minimal.xlsx
+++ b/RBG_arduino/StateTable_minimal.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/markdolson/GitHub-Mark-MDO47/RubberBandGun/RBG_arduino/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B9FDDF8-03C4-C546-BAD0-BFA48E775C89}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D4AE5E1-523C-3F48-AD42-364A754E9E86}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-40" yWindow="480" windowWidth="25600" windowHeight="15540" activeTab="1" xr2:uid="{CCADFEE4-B0E1-4363-9617-1683960BED03}"/>
+    <workbookView xWindow="-40" yWindow="480" windowWidth="25600" windowHeight="15540" activeTab="2" xr2:uid="{CCADFEE4-B0E1-4363-9617-1683960BED03}"/>
   </bookViews>
   <sheets>
     <sheet name="StateTable" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
     <sheet name="Sounds" sheetId="5" r:id="rId5"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">debugging!$A$3129:$B$3157</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">debugging!$A$3223:$B$3273</definedName>
     <definedName name="mROW">StateTable!$V$2:$X$21</definedName>
     <definedName name="prev">Sounds!$N$2:$N$9</definedName>
     <definedName name="yxcmd">'YX5200 info'!$A$2:$C$44</definedName>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4472" uniqueCount="3344">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4530" uniqueCount="3395">
   <si>
     <t>trigOnly</t>
   </si>
@@ -10301,6 +10301,159 @@
   </si>
   <si>
     <t>if it is a block of input selections, make all the rows for different behaviors have the same mROW_* name</t>
+  </si>
+  <si>
+    <t>rework the LED routines</t>
+  </si>
+  <si>
+    <t>DEBUG loop() - nowVinputRBG 0x40 loopCount 1081</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> RBG_waitForInput mINP_LOCK thisReturn 3 loopCount 1121</t>
+  </si>
+  <si>
+    <t>DEBUG loop() - nowVinputRBG 0x240 loopCount 1201</t>
+  </si>
+  <si>
+    <t>DEBUG loop() - nowVinputRBG 0x2240 loopCount 1241</t>
+  </si>
+  <si>
+    <t>DEBUG loop() - nowVinputRBG 0x40 loopCount 6127</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> RBG_waitForInput mSPCL_EFCT_ONETIME thisReturn 5 loopCount 6127</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> RBG_waitForInput mINP_LOCK thisReturn 9 loopCount 6207</t>
+  </si>
+  <si>
+    <t>DEBUG loop() - nowVinputRBG 0x240 loopCount 6287</t>
+  </si>
+  <si>
+    <t>DEBUG loop() - nowVinputRBG 0x2240 loopCount 6327</t>
+  </si>
+  <si>
+    <t>DEBUG loop() - nowVinputRBG 0x2260 loopCount 19336</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> RBG_waitForInput mINP_TRIG mINP_BANY thisReturn 11 loopCount 19336</t>
+  </si>
+  <si>
+    <t>DEBUG loop() - nowVinputRBG 0x2240 loopCount 19507</t>
+  </si>
+  <si>
+    <t>DEBUG loop() - nowVinputRBG 0x40 loopCount 39606</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> RBG_waitForInput mSPCL_EFCT_ONETIME thisReturn 12 loopCount 39606</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> RBG_waitForInput mSPCL_HANDLER thisReturn 13 loopCount 39686</t>
+  </si>
+  <si>
+    <t>DEBUG loop() - nowVinputRBG 0x240 loopCount 39931</t>
+  </si>
+  <si>
+    <t>DEBUG loop() - nowVinputRBG 0x2240 loopCount 39971</t>
+  </si>
+  <si>
+    <t>DEBUG loop() - nowVinputRBG 0x40 loopCount 43773</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> RBG_waitForInput mSPCL_EFCT_ONETIME thisReturn 14 loopCount 43773</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> RBG_waitForInput mSPCL_HANDLER thisReturn 5 loopCount 43853</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> RBG_waitForInput mINP_LOCK thisReturn 9 loopCount 43933</t>
+  </si>
+  <si>
+    <t>DEBUG loop() - nowVinputRBG 0x240 loopCount 44013</t>
+  </si>
+  <si>
+    <t>DEBUG loop() - nowVinputRBG 0x2240 loopCount 44053</t>
+  </si>
+  <si>
+    <t>DEBUG loop() - nowVinputRBG 0x40 loopCount 63953</t>
+  </si>
+  <si>
+    <t>DEBUG loop() - nowVinputRBG 0x2240 loopCount 63994</t>
+  </si>
+  <si>
+    <t>DEBUG loop() - nowVinputRBG 0x40 loopCount 83928</t>
+  </si>
+  <si>
+    <t>DEBUG loop() - nowVinputRBG 0x2240 loopCount 83969</t>
+  </si>
+  <si>
+    <t>DEBUG loop() - nowVinputRBG 0x2280 loopCount 89133</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> RBG_waitForInput mINP_OPEN thisReturn 15 loopCount 89133</t>
+  </si>
+  <si>
+    <t>DEBUG loop() - nowVinputRBG 0x2240 loopCount 92431</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> RBG_waitForInput mINP_LOCK thisReturn 17 loopCount 92431</t>
+  </si>
+  <si>
+    <t>DEBUG loop() - nowVinputRBG 0x40 loopCount 97805</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> RBG_waitForInput mSPCL_EFCT_ONETIME thisReturn 5 loopCount 97805</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> RBG_waitForInput mINP_LOCK thisReturn 9 loopCount 97885</t>
+  </si>
+  <si>
+    <t>DEBUG loop() - nowVinputRBG 0x240 loopCount 97965</t>
+  </si>
+  <si>
+    <t>DEBUG loop() - nowVinputRBG 0x2240 loopCount 98005</t>
+  </si>
+  <si>
+    <t>DEBUG loop() - nowVinputRBG 0x2260 loopCount 104535</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> RBG_waitForInput mINP_TRIG mINP_BANY thisReturn 11 loopCount 104535</t>
+  </si>
+  <si>
+    <t>DEBUG loop() - nowVinputRBG 0x2240 loopCount 104785</t>
+  </si>
+  <si>
+    <t>DEBUG loop() - nowVinputRBG 0x40 loopCount 124760</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> RBG_waitForInput mSPCL_EFCT_ONETIME thisReturn 12 loopCount 124760</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> RBG_waitForInput mSPCL_HANDLER thisReturn 13 loopCount 124840</t>
+  </si>
+  <si>
+    <t>DEBUG loop() - nowVinputRBG 0x240 loopCount 125084</t>
+  </si>
+  <si>
+    <t>DEBUG loop() - nowVinputRBG 0x2240 loopCount 125124</t>
+  </si>
+  <si>
+    <t>DEBUG loop() - nowVinputRBG 0x40 loopCount 128925</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> RBG_waitForInput mSPCL_EFCT_ONETIME thisReturn 14 loopCount 128925</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> RBG_waitForInput mSPCL_HANDLER thisReturn 5 loopCount 129005</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> RBG_waitForInput mINP_LOCK thisReturn 9 loopCount 129085</t>
+  </si>
+  <si>
+    <t>DEBUG loop() - nowVinputRBG 0x240 loopCount 129165</t>
+  </si>
+  <si>
+    <t>DEBUG loop() - nowVinputRBG 0x2240 loopCount 129205</t>
   </si>
 </sst>
 </file>
@@ -11999,7 +12152,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0B3F56F7-7110-4AD7-8B0D-AA537E4015D5}">
   <dimension ref="A1:H45"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
@@ -12188,10 +12341,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F57F550E-21B4-4ED7-B7FF-211D228584A7}">
-  <dimension ref="A1:M3212"/>
+  <dimension ref="A1:M3273"/>
   <sheetViews>
-    <sheetView topLeftCell="A3168" workbookViewId="0">
-      <selection activeCell="B3190" sqref="B3190"/>
+    <sheetView tabSelected="1" topLeftCell="A3242" workbookViewId="0">
+      <selection activeCell="B3238" sqref="B3238"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
@@ -38229,7 +38382,298 @@
         <v>4.1000000000000002E-2</v>
       </c>
     </row>
+    <row r="3214" spans="2:4" ht="16" thickBot="1"/>
+    <row r="3215" spans="2:4" ht="17" thickTop="1" thickBot="1">
+      <c r="B3215" s="1" t="s">
+        <v>3344</v>
+      </c>
+    </row>
+    <row r="3216" spans="2:4" ht="16" thickTop="1"/>
+    <row r="3217" spans="1:2">
+      <c r="B3217" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="3218" spans="1:2">
+      <c r="B3218" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="3219" spans="1:2">
+      <c r="B3219" t="s">
+        <v>904</v>
+      </c>
+    </row>
+    <row r="3220" spans="1:2">
+      <c r="B3220" t="s">
+        <v>905</v>
+      </c>
+    </row>
+    <row r="3221" spans="1:2">
+      <c r="B3221" t="s">
+        <v>2814</v>
+      </c>
+    </row>
+    <row r="3223" spans="1:2">
+      <c r="A3223" t="s">
+        <v>2074</v>
+      </c>
+      <c r="B3223" t="s">
+        <v>3274</v>
+      </c>
+    </row>
+    <row r="3224" spans="1:2">
+      <c r="B3224" s="24" t="s">
+        <v>3345</v>
+      </c>
+    </row>
+    <row r="3225" spans="1:2">
+      <c r="B3225" t="s">
+        <v>3346</v>
+      </c>
+    </row>
+    <row r="3226" spans="1:2">
+      <c r="B3226" s="24" t="s">
+        <v>3347</v>
+      </c>
+    </row>
+    <row r="3227" spans="1:2">
+      <c r="B3227" s="24" t="s">
+        <v>3348</v>
+      </c>
+    </row>
+    <row r="3228" spans="1:2">
+      <c r="B3228" s="24" t="s">
+        <v>3349</v>
+      </c>
+    </row>
+    <row r="3229" spans="1:2">
+      <c r="B3229" t="s">
+        <v>3350</v>
+      </c>
+    </row>
+    <row r="3230" spans="1:2">
+      <c r="B3230" t="s">
+        <v>3351</v>
+      </c>
+    </row>
+    <row r="3231" spans="1:2">
+      <c r="B3231" s="24" t="s">
+        <v>3352</v>
+      </c>
+    </row>
+    <row r="3232" spans="1:2">
+      <c r="B3232" s="24" t="s">
+        <v>3353</v>
+      </c>
+    </row>
+    <row r="3233" spans="2:2">
+      <c r="B3233" s="24" t="s">
+        <v>3354</v>
+      </c>
+    </row>
+    <row r="3234" spans="2:2">
+      <c r="B3234" t="s">
+        <v>3355</v>
+      </c>
+    </row>
+    <row r="3235" spans="2:2">
+      <c r="B3235" s="24" t="s">
+        <v>3356</v>
+      </c>
+    </row>
+    <row r="3236" spans="2:2">
+      <c r="B3236" s="24" t="s">
+        <v>3357</v>
+      </c>
+    </row>
+    <row r="3237" spans="2:2">
+      <c r="B3237" t="s">
+        <v>3358</v>
+      </c>
+    </row>
+    <row r="3238" spans="2:2">
+      <c r="B3238" t="s">
+        <v>3359</v>
+      </c>
+    </row>
+    <row r="3239" spans="2:2">
+      <c r="B3239" s="24" t="s">
+        <v>3360</v>
+      </c>
+    </row>
+    <row r="3240" spans="2:2">
+      <c r="B3240" s="24" t="s">
+        <v>3361</v>
+      </c>
+    </row>
+    <row r="3241" spans="2:2">
+      <c r="B3241" s="24" t="s">
+        <v>3362</v>
+      </c>
+    </row>
+    <row r="3242" spans="2:2">
+      <c r="B3242" t="s">
+        <v>3363</v>
+      </c>
+    </row>
+    <row r="3243" spans="2:2">
+      <c r="B3243" t="s">
+        <v>3364</v>
+      </c>
+    </row>
+    <row r="3244" spans="2:2">
+      <c r="B3244" t="s">
+        <v>3365</v>
+      </c>
+    </row>
+    <row r="3245" spans="2:2">
+      <c r="B3245" s="24" t="s">
+        <v>3366</v>
+      </c>
+    </row>
+    <row r="3246" spans="2:2">
+      <c r="B3246" s="24" t="s">
+        <v>3367</v>
+      </c>
+    </row>
+    <row r="3247" spans="2:2">
+      <c r="B3247" s="24" t="s">
+        <v>3368</v>
+      </c>
+    </row>
+    <row r="3248" spans="2:2">
+      <c r="B3248" s="24" t="s">
+        <v>3369</v>
+      </c>
+    </row>
+    <row r="3249" spans="2:2">
+      <c r="B3249" s="24" t="s">
+        <v>3370</v>
+      </c>
+    </row>
+    <row r="3250" spans="2:2">
+      <c r="B3250" s="24" t="s">
+        <v>3371</v>
+      </c>
+    </row>
+    <row r="3251" spans="2:2">
+      <c r="B3251" s="24" t="s">
+        <v>3372</v>
+      </c>
+    </row>
+    <row r="3252" spans="2:2">
+      <c r="B3252" t="s">
+        <v>3373</v>
+      </c>
+    </row>
+    <row r="3253" spans="2:2">
+      <c r="B3253" s="24" t="s">
+        <v>3374</v>
+      </c>
+    </row>
+    <row r="3254" spans="2:2">
+      <c r="B3254" t="s">
+        <v>3375</v>
+      </c>
+    </row>
+    <row r="3255" spans="2:2">
+      <c r="B3255" s="24" t="s">
+        <v>3376</v>
+      </c>
+    </row>
+    <row r="3256" spans="2:2">
+      <c r="B3256" t="s">
+        <v>3377</v>
+      </c>
+    </row>
+    <row r="3257" spans="2:2">
+      <c r="B3257" t="s">
+        <v>3378</v>
+      </c>
+    </row>
+    <row r="3258" spans="2:2">
+      <c r="B3258" s="24" t="s">
+        <v>3379</v>
+      </c>
+    </row>
+    <row r="3259" spans="2:2">
+      <c r="B3259" s="24" t="s">
+        <v>3380</v>
+      </c>
+    </row>
+    <row r="3260" spans="2:2">
+      <c r="B3260" s="24" t="s">
+        <v>3381</v>
+      </c>
+    </row>
+    <row r="3261" spans="2:2">
+      <c r="B3261" t="s">
+        <v>3382</v>
+      </c>
+    </row>
+    <row r="3262" spans="2:2">
+      <c r="B3262" s="24" t="s">
+        <v>3383</v>
+      </c>
+    </row>
+    <row r="3263" spans="2:2">
+      <c r="B3263" s="24" t="s">
+        <v>3384</v>
+      </c>
+    </row>
+    <row r="3264" spans="2:2">
+      <c r="B3264" t="s">
+        <v>3385</v>
+      </c>
+    </row>
+    <row r="3265" spans="2:2">
+      <c r="B3265" t="s">
+        <v>3386</v>
+      </c>
+    </row>
+    <row r="3266" spans="2:2">
+      <c r="B3266" s="24" t="s">
+        <v>3387</v>
+      </c>
+    </row>
+    <row r="3267" spans="2:2">
+      <c r="B3267" s="24" t="s">
+        <v>3388</v>
+      </c>
+    </row>
+    <row r="3268" spans="2:2">
+      <c r="B3268" s="24" t="s">
+        <v>3389</v>
+      </c>
+    </row>
+    <row r="3269" spans="2:2">
+      <c r="B3269" t="s">
+        <v>3390</v>
+      </c>
+    </row>
+    <row r="3270" spans="2:2">
+      <c r="B3270" t="s">
+        <v>3391</v>
+      </c>
+    </row>
+    <row r="3271" spans="2:2">
+      <c r="B3271" t="s">
+        <v>3392</v>
+      </c>
+    </row>
+    <row r="3272" spans="2:2">
+      <c r="B3272" s="24" t="s">
+        <v>3393</v>
+      </c>
+    </row>
+    <row r="3273" spans="2:2">
+      <c r="B3273" s="24" t="s">
+        <v>3394</v>
+      </c>
+    </row>
   </sheetData>
+  <autoFilter ref="A3223:B3273" xr:uid="{D8398E87-10B4-0F4C-AD8E-D59C955E36B3}"/>
   <sortState ref="A3078:B3118">
     <sortCondition ref="A3078:A3118"/>
   </sortState>

</xml_diff>

<commit_message>
more sounds and some new definitions
</commit_message>
<xml_diff>
--- a/RBG_arduino/StateTable_minimal.xlsx
+++ b/RBG_arduino/StateTable_minimal.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub-Mark-MDO47\RubberBandGun\RBG_arduino\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC1D72CB-CB53-4590-9FAA-0501B6A84C44}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4751DD00-6927-4450-BCEF-F7C7A212B802}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21840" xr2:uid="{CCADFEE4-B0E1-4363-9617-1683960BED03}"/>
   </bookViews>
@@ -21,8 +21,9 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">debugging!$A$3223:$B$3273</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">Sounds!$A$1:$H$44</definedName>
     <definedName name="mROW">StateTable!$V$2:$X$21</definedName>
-    <definedName name="prev">Sounds!$AK$2:$AK$16</definedName>
+    <definedName name="prev">Sounds!$AK$2:$AK$18</definedName>
     <definedName name="yxcmd">'YX5200 info'!$A$2:$C$44</definedName>
   </definedNames>
   <calcPr calcId="181029"/>
@@ -41,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4836" uniqueCount="3489">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4870" uniqueCount="3498">
   <si>
     <t>trigOnly</t>
   </si>
@@ -10504,21 +10505,9 @@
     <t>local</t>
   </si>
   <si>
-    <t>0041_FOOF.mp3</t>
-  </si>
-  <si>
     <t>PowerOn</t>
   </si>
   <si>
-    <t>my combination windup; max license is by/3.0/</t>
-  </si>
-  <si>
-    <t>My FOOF announcement; license is by/3.0/</t>
-  </si>
-  <si>
-    <t>0005_Gravitational-Waves-from-a-Neutron-Star-Merger-Produced-a-Signal-Detected-by-LIGO_2019-12-13.mp3</t>
-  </si>
-  <si>
     <t>lock/load open shoot</t>
   </si>
   <si>
@@ -10651,9 +10640,6 @@
     <t>Sorry, not yet implemented</t>
   </si>
   <si>
-    <t>mEFCT_CONFIGURE+2</t>
-  </si>
-  <si>
     <t>mADDR_CFGSND</t>
   </si>
   <si>
@@ -10687,9 +10673,6 @@
     <t>mSPCL_HANDLER | mSPCL_HANDLER_CFG2EEPROM | mSPCL_EFCT_NONE</t>
   </si>
   <si>
-    <t>mEFCT_UNIQ+2</t>
-  </si>
-  <si>
     <t>0102_uniqSorryNotYetImplemented.wav</t>
   </si>
   <si>
@@ -10699,33 +10682,15 @@
     <t>Welcome to RBG configuration: choose YELLOW for sounds, GREEN for lights, BLACK for other; then also press trigger. To go back, press trigger all by itself.</t>
   </si>
   <si>
-    <t>0062_cfg_introToConfig.wav</t>
-  </si>
-  <si>
-    <t>mEFCT_CONFIGURE+3</t>
-  </si>
-  <si>
     <t>Press just trigger to cycle through sound choices, trigger + any color to choose the sound.</t>
   </si>
   <si>
-    <t>0063_cfg_configSndInstruct.wav</t>
-  </si>
-  <si>
     <t>0064_cfg_configLEDInstruct.wav</t>
   </si>
   <si>
     <t>0065_cfg_configOtherInstruct.wav</t>
   </si>
   <si>
-    <t>0017_PewPewPew.wav</t>
-  </si>
-  <si>
-    <t>mdo47 recording of Pew Pew Pew</t>
-  </si>
-  <si>
-    <t>mdo47 recording of "Welcome to RBG configuration: choose YELLOW for sounds, GREEN for lights, BLACK for other; then also press trigger. To go back, press trigger all by itself."</t>
-  </si>
-  <si>
     <t>mdo47 recording of "Press just trigger to cycle through sound choices, trigger + any color to choose the sound."</t>
   </si>
   <si>
@@ -10742,6 +10707,69 @@
   </si>
   <si>
     <t>(7&lt;&lt;mSHIFT_EFCT_CFGMAXVAL) | mEFCT_SHOOT</t>
+  </si>
+  <si>
+    <t>mdo47 recording of FOOF announcement; license is by/3.0/</t>
+  </si>
+  <si>
+    <t>mdo47 combination windup; max license is by/3.0/</t>
+  </si>
+  <si>
+    <t>0005__mdo47__Gravitational-Waves-from-a-Neutron-Star-Merger-Produced-a-Signal-Detected-by-LIGO_mdo47.wav</t>
+  </si>
+  <si>
+    <t>0041__mdo47__lFOOF_Darling.wav</t>
+  </si>
+  <si>
+    <t>0042__mdo47__mFOOF.wav</t>
+  </si>
+  <si>
+    <t>0062__mdo47__cfg_introToConfig.wav</t>
+  </si>
+  <si>
+    <t>0063__mdo47__cfg_configSndInstruct.wav</t>
+  </si>
+  <si>
+    <t>0018__mdo47_mPewPewPew.wav</t>
+  </si>
+  <si>
+    <t>0017__mdo47_lPewPewPew.wav</t>
+  </si>
+  <si>
+    <t>0019__mdo47__iPewPewPew.wav</t>
+  </si>
+  <si>
+    <t>mdo47 "L" recording of Pew Pew Pew</t>
+  </si>
+  <si>
+    <t>mdo47 "M" recording of Pew Pew Pew</t>
+  </si>
+  <si>
+    <t>mdo47 "I" recording of Pew Pew Pew</t>
+  </si>
+  <si>
+    <t>Mnemonic</t>
+  </si>
+  <si>
+    <t>mEFCT_CFG_INTRO</t>
+  </si>
+  <si>
+    <t>mEFCT_UNIQ_SILENCE</t>
+  </si>
+  <si>
+    <t>mEFCT_UNIQ_NOT_IMPL</t>
+  </si>
+  <si>
+    <t>mEFCT_CFG_SND_INSTR</t>
+  </si>
+  <si>
+    <t>mEFCT_CFG_LED_INSTR</t>
+  </si>
+  <si>
+    <t>mEFCT_CFG_OTHR_INSTR</t>
+  </si>
+  <si>
+    <t>mdo47 recording of "Welcome to RBG configuration! Your call is important to us. Choose YELLOW for sounds, GREEN for lights, BLACK for other; then also press trigger. To go back, press trigger all by itself."</t>
   </si>
 </sst>
 </file>
@@ -11116,7 +11144,7 @@
     <xf numFmtId="0" fontId="11" fillId="9" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="76">
+  <cellXfs count="80">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -11251,6 +11279,18 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="3" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -11577,8 +11617,8 @@
   <dimension ref="A1:AB68"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A26" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G56" sqref="G56"/>
+      <pane ySplit="1" topLeftCell="A15" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D57" sqref="D57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
@@ -11804,12 +11844,12 @@
         <v>52</v>
       </c>
       <c r="F6" t="s">
-        <v>3450</v>
+        <v>3446</v>
       </c>
       <c r="G6" s="9"/>
       <c r="H6" s="9"/>
       <c r="I6" t="s">
-        <v>3449</v>
+        <v>3445</v>
       </c>
       <c r="J6" s="9"/>
       <c r="K6" s="9" t="str">
@@ -12017,12 +12057,12 @@
         <v>52</v>
       </c>
       <c r="F13" t="s">
-        <v>3450</v>
+        <v>3446</v>
       </c>
       <c r="G13" s="9"/>
       <c r="H13" s="9"/>
       <c r="I13" t="s">
-        <v>3449</v>
+        <v>3445</v>
       </c>
       <c r="J13" s="9"/>
       <c r="K13" s="9" t="str">
@@ -12175,10 +12215,10 @@
         <v>2550</v>
       </c>
       <c r="D19" s="47" t="s">
-        <v>3435</v>
+        <v>3431</v>
       </c>
       <c r="E19" s="47" t="s">
-        <v>3435</v>
+        <v>3431</v>
       </c>
       <c r="F19" s="37" t="s">
         <v>0</v>
@@ -12203,10 +12243,10 @@
         <v>2550</v>
       </c>
       <c r="D20" s="47" t="s">
-        <v>3435</v>
+        <v>3431</v>
       </c>
       <c r="E20" s="47" t="s">
-        <v>3435</v>
+        <v>3431</v>
       </c>
       <c r="F20" s="37" t="s">
         <v>4</v>
@@ -12249,10 +12289,10 @@
         <v>2549</v>
       </c>
       <c r="D22" s="47" t="s">
-        <v>3435</v>
+        <v>3431</v>
       </c>
       <c r="E22" s="47" t="s">
-        <v>3435</v>
+        <v>3431</v>
       </c>
       <c r="F22" s="37" t="s">
         <v>0</v>
@@ -12281,10 +12321,10 @@
         <v>2549</v>
       </c>
       <c r="D23" s="47" t="s">
-        <v>3435</v>
+        <v>3431</v>
       </c>
       <c r="E23" s="47" t="s">
-        <v>3435</v>
+        <v>3431</v>
       </c>
       <c r="F23" s="37" t="s">
         <v>3</v>
@@ -12639,19 +12679,19 @@
     </row>
     <row r="45" spans="1:15" ht="120">
       <c r="A45" s="63" t="s">
-        <v>3473</v>
+        <v>3467</v>
       </c>
       <c r="B45" s="9" t="s">
         <v>2730</v>
       </c>
       <c r="C45" s="9" t="s">
-        <v>3449</v>
+        <v>3445</v>
       </c>
       <c r="D45" s="3" t="s">
-        <v>3458</v>
+        <v>3491</v>
       </c>
       <c r="E45" s="47" t="s">
-        <v>3456</v>
+        <v>3452</v>
       </c>
       <c r="F45" s="9" t="s">
         <v>0</v>
@@ -12670,19 +12710,19 @@
         <v>2730</v>
       </c>
       <c r="C46" s="11" t="s">
-        <v>3449</v>
+        <v>3445</v>
       </c>
       <c r="D46" s="3" t="s">
-        <v>3458</v>
+        <v>3491</v>
       </c>
       <c r="E46" s="47" t="s">
+        <v>3452</v>
+      </c>
+      <c r="F46" t="s">
+        <v>3447</v>
+      </c>
+      <c r="I46" s="75" t="s">
         <v>3456</v>
-      </c>
-      <c r="F46" t="s">
-        <v>3451</v>
-      </c>
-      <c r="I46" s="75" t="s">
-        <v>3461</v>
       </c>
       <c r="K46" s="9" t="e">
         <f>IF(LEN(C46),VLOOKUP(C46,mROW,3,FALSE),"")</f>
@@ -12695,19 +12735,19 @@
         <v>2730</v>
       </c>
       <c r="C47" s="11" t="s">
+        <v>3445</v>
+      </c>
+      <c r="D47" s="3" t="s">
+        <v>3491</v>
+      </c>
+      <c r="E47" s="47" t="s">
+        <v>3452</v>
+      </c>
+      <c r="F47" t="s">
+        <v>3448</v>
+      </c>
+      <c r="I47" t="s">
         <v>3449</v>
-      </c>
-      <c r="D47" s="3" t="s">
-        <v>3458</v>
-      </c>
-      <c r="E47" s="47" t="s">
-        <v>3456</v>
-      </c>
-      <c r="F47" t="s">
-        <v>3452</v>
-      </c>
-      <c r="I47" t="s">
-        <v>3453</v>
       </c>
       <c r="K47" s="9" t="e">
         <f>IF(LEN(C47),VLOOKUP(C47,mROW,3,FALSE),"")</f>
@@ -12720,19 +12760,19 @@
         <v>2730</v>
       </c>
       <c r="C48" s="11" t="s">
-        <v>3449</v>
+        <v>3445</v>
       </c>
       <c r="D48" s="3" t="s">
-        <v>3458</v>
+        <v>3491</v>
       </c>
       <c r="E48" s="47" t="s">
-        <v>3456</v>
+        <v>3452</v>
       </c>
       <c r="F48" t="s">
-        <v>3454</v>
+        <v>3450</v>
       </c>
       <c r="I48" t="s">
-        <v>3455</v>
+        <v>3451</v>
       </c>
       <c r="K48" s="9" t="e">
         <f>IF(LEN(C48),VLOOKUP(C48,mROW,3,FALSE),"")</f>
@@ -12757,22 +12797,22 @@
     </row>
     <row r="51" spans="1:11" ht="30">
       <c r="A51" s="63" t="s">
-        <v>3457</v>
+        <v>3453</v>
       </c>
       <c r="B51" s="9" t="s">
         <v>2730</v>
       </c>
       <c r="C51" t="s">
-        <v>3453</v>
+        <v>3449</v>
       </c>
       <c r="D51" s="3" t="s">
-        <v>3470</v>
+        <v>3493</v>
       </c>
       <c r="E51" s="47" t="s">
-        <v>3456</v>
+        <v>3452</v>
       </c>
       <c r="J51" s="9" t="s">
-        <v>3449</v>
+        <v>3445</v>
       </c>
       <c r="K51" s="9" t="e">
         <f>IF(LEN(C51),VLOOKUP(C51,mROW,3,FALSE),"")</f>
@@ -12788,22 +12828,22 @@
     </row>
     <row r="53" spans="1:11" ht="30">
       <c r="A53" s="63" t="s">
-        <v>3457</v>
+        <v>3453</v>
       </c>
       <c r="B53" s="9" t="s">
         <v>2730</v>
       </c>
       <c r="C53" t="s">
-        <v>3455</v>
+        <v>3451</v>
       </c>
       <c r="D53" s="3" t="s">
-        <v>3470</v>
+        <v>3493</v>
       </c>
       <c r="E53" s="47" t="s">
-        <v>3456</v>
+        <v>3452</v>
       </c>
       <c r="J53" s="9" t="s">
-        <v>3449</v>
+        <v>3445</v>
       </c>
       <c r="K53" s="9" t="e">
         <f>IF(LEN(C53),VLOOKUP(C53,mROW,3,FALSE),"")</f>
@@ -12819,26 +12859,26 @@
     </row>
     <row r="55" spans="1:11" ht="45">
       <c r="A55" s="63" t="s">
-        <v>3463</v>
+        <v>3458</v>
       </c>
       <c r="B55" s="10" t="s">
-        <v>3467</v>
+        <v>3462</v>
       </c>
       <c r="C55" s="9" t="s">
-        <v>3461</v>
+        <v>3456</v>
       </c>
       <c r="D55" s="9"/>
       <c r="E55" s="9"/>
       <c r="F55" s="9"/>
       <c r="G55" s="10" t="s">
-        <v>3488</v>
+        <v>3476</v>
       </c>
       <c r="H55" s="9" t="s">
-        <v>3459</v>
+        <v>3454</v>
       </c>
       <c r="I55" s="9"/>
       <c r="J55" s="9" t="s">
-        <v>3462</v>
+        <v>3457</v>
       </c>
       <c r="K55" s="9" t="e">
         <f>IF(LEN(C55),VLOOKUP(C55,mROW,3,FALSE),"")</f>
@@ -12854,19 +12894,19 @@
     </row>
     <row r="57" spans="1:11" ht="75">
       <c r="A57" s="63" t="s">
-        <v>3476</v>
+        <v>3468</v>
       </c>
       <c r="B57" s="9" t="s">
         <v>2730</v>
       </c>
       <c r="C57" s="9" t="s">
-        <v>3462</v>
+        <v>3457</v>
       </c>
       <c r="D57" s="3" t="s">
-        <v>3475</v>
+        <v>3494</v>
       </c>
       <c r="E57" s="47" t="s">
-        <v>3456</v>
+        <v>3452</v>
       </c>
       <c r="F57" s="9" t="s">
         <v>0</v>
@@ -12874,7 +12914,7 @@
       <c r="G57" s="9"/>
       <c r="H57" s="9"/>
       <c r="I57" s="9" t="s">
-        <v>3460</v>
+        <v>3455</v>
       </c>
       <c r="J57" s="9"/>
       <c r="K57" s="9" t="e">
@@ -12890,16 +12930,16 @@
     </row>
     <row r="59" spans="1:11">
       <c r="B59" t="s">
-        <v>3464</v>
+        <v>3459</v>
       </c>
       <c r="C59" s="9" t="s">
-        <v>3460</v>
+        <v>3455</v>
       </c>
       <c r="F59" s="9" t="s">
         <v>0</v>
       </c>
       <c r="I59" s="9" t="s">
-        <v>3465</v>
+        <v>3460</v>
       </c>
       <c r="K59" s="9" t="e">
         <f>IF(LEN(C59),VLOOKUP(C59,mROW,3,FALSE),"")</f>
@@ -12908,16 +12948,16 @@
     </row>
     <row r="60" spans="1:11">
       <c r="B60" t="s">
-        <v>3464</v>
+        <v>3459</v>
       </c>
       <c r="C60" s="12" t="s">
-        <v>3460</v>
+        <v>3455</v>
       </c>
       <c r="F60" s="9" t="s">
-        <v>3450</v>
+        <v>3446</v>
       </c>
       <c r="I60" s="9" t="s">
-        <v>3466</v>
+        <v>3461</v>
       </c>
       <c r="K60" s="9" t="e">
         <f>IF(LEN(C60),VLOOKUP(C60,mROW,3,FALSE),"")</f>
@@ -12932,13 +12972,13 @@
     </row>
     <row r="62" spans="1:11" ht="45">
       <c r="B62" s="10" t="s">
-        <v>3468</v>
+        <v>3463</v>
       </c>
       <c r="C62" s="9" t="s">
-        <v>3465</v>
+        <v>3460</v>
       </c>
       <c r="J62" s="9" t="s">
-        <v>3460</v>
+        <v>3455</v>
       </c>
       <c r="K62" s="9" t="e">
         <f>IF(LEN(C62),VLOOKUP(C62,mROW,3,FALSE),"")</f>
@@ -12953,13 +12993,13 @@
     </row>
     <row r="64" spans="1:11" ht="45">
       <c r="B64" s="10" t="s">
-        <v>3469</v>
+        <v>3464</v>
       </c>
       <c r="C64" s="9" t="s">
-        <v>3466</v>
+        <v>3461</v>
       </c>
       <c r="J64" s="9" t="s">
-        <v>3449</v>
+        <v>3445</v>
       </c>
       <c r="K64" s="9" t="e">
         <f>IF(LEN(C64),VLOOKUP(C64,mROW,3,FALSE),"")</f>
@@ -39527,7 +39567,7 @@
     <row r="3276" spans="2:2" ht="15.75" thickBot="1"/>
     <row r="3277" spans="2:2" ht="16.5" thickTop="1" thickBot="1">
       <c r="B3277" s="1" t="s">
-        <v>3436</v>
+        <v>3432</v>
       </c>
     </row>
     <row r="3278" spans="2:2" ht="15.75" thickTop="1"/>
@@ -39570,7 +39610,7 @@
         <v>43</v>
       </c>
       <c r="B3286" t="s">
-        <v>3437</v>
+        <v>3433</v>
       </c>
     </row>
     <row r="3287" spans="1:2">
@@ -39579,7 +39619,7 @@
         <v>871</v>
       </c>
       <c r="B3287" t="s">
-        <v>3438</v>
+        <v>3434</v>
       </c>
     </row>
     <row r="3288" spans="1:2">
@@ -39588,7 +39628,7 @@
         <v>3109</v>
       </c>
       <c r="B3288" t="s">
-        <v>3439</v>
+        <v>3435</v>
       </c>
     </row>
     <row r="3289" spans="1:2">
@@ -39597,7 +39637,7 @@
         <v>3225</v>
       </c>
       <c r="B3289" t="s">
-        <v>3440</v>
+        <v>3436</v>
       </c>
     </row>
     <row r="3290" spans="1:2">
@@ -39606,7 +39646,7 @@
         <v>3320</v>
       </c>
       <c r="B3290" t="s">
-        <v>3441</v>
+        <v>3437</v>
       </c>
     </row>
     <row r="3291" spans="1:2">
@@ -39615,7 +39655,7 @@
         <v>3611</v>
       </c>
       <c r="B3291" t="s">
-        <v>3442</v>
+        <v>3438</v>
       </c>
     </row>
     <row r="3292" spans="1:2">
@@ -39624,7 +39664,7 @@
         <v>3727</v>
       </c>
       <c r="B3292" t="s">
-        <v>3443</v>
+        <v>3439</v>
       </c>
     </row>
     <row r="3293" spans="1:2">
@@ -39633,7 +39673,7 @@
         <v>3822</v>
       </c>
       <c r="B3293" t="s">
-        <v>3444</v>
+        <v>3440</v>
       </c>
     </row>
     <row r="3294" spans="1:2">
@@ -39642,7 +39682,7 @@
         <v>4150</v>
       </c>
       <c r="B3294" t="s">
-        <v>3445</v>
+        <v>3441</v>
       </c>
     </row>
     <row r="3295" spans="1:2">
@@ -39651,7 +39691,7 @@
         <v>4219</v>
       </c>
       <c r="B3295" t="s">
-        <v>3446</v>
+        <v>3442</v>
       </c>
     </row>
     <row r="3296" spans="1:2">
@@ -39660,7 +39700,7 @@
         <v>4271</v>
       </c>
       <c r="B3296" t="s">
-        <v>3447</v>
+        <v>3443</v>
       </c>
     </row>
     <row r="3297" spans="1:2">
@@ -39669,7 +39709,7 @@
         <v>4340</v>
       </c>
       <c r="B3297" t="s">
-        <v>3448</v>
+        <v>3444</v>
       </c>
     </row>
   </sheetData>
@@ -42134,10 +42174,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A827A58D-C8A4-4858-A89B-E853C083564F}">
-  <dimension ref="A1:AK101"/>
+  <dimension ref="A1:AK106"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+    <sheetView topLeftCell="A16" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C39" sqref="C39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
@@ -42181,7 +42221,9 @@
       <c r="H1" s="64" t="s">
         <v>2878</v>
       </c>
-      <c r="I1" s="28"/>
+      <c r="I1" s="27" t="s">
+        <v>3490</v>
+      </c>
     </row>
     <row r="2" spans="1:37" ht="20.25">
       <c r="A2" s="65" t="s">
@@ -42208,7 +42250,7 @@
       <c r="H2" s="69" t="s">
         <v>2898</v>
       </c>
-      <c r="I2" s="28"/>
+      <c r="I2" s="27"/>
       <c r="AK2" s="28"/>
     </row>
     <row r="3" spans="1:37" ht="30">
@@ -42236,7 +42278,7 @@
       <c r="H3" s="69" t="s">
         <v>2883</v>
       </c>
-      <c r="I3" s="28"/>
+      <c r="I3" s="27"/>
       <c r="AK3" s="28"/>
     </row>
     <row r="4" spans="1:37" ht="20.25">
@@ -42292,10 +42334,10 @@
       <c r="H5" s="69" t="s">
         <v>2881</v>
       </c>
-      <c r="I5" s="28"/>
+      <c r="I5" s="27"/>
       <c r="AK5" s="28"/>
     </row>
-    <row r="6" spans="1:37" ht="20.25">
+    <row r="6" spans="1:37" ht="30">
       <c r="A6" s="70" t="s">
         <v>2874</v>
       </c>
@@ -42303,10 +42345,10 @@
         <v>5</v>
       </c>
       <c r="C6" s="65" t="s">
-        <v>3413</v>
+        <v>3479</v>
       </c>
       <c r="D6" s="67" t="s">
-        <v>3411</v>
+        <v>3478</v>
       </c>
       <c r="E6" s="67" t="s">
         <v>2874</v>
@@ -42320,7 +42362,7 @@
       <c r="H6" s="70" t="s">
         <v>3408</v>
       </c>
-      <c r="I6" s="28"/>
+      <c r="I6" s="27"/>
       <c r="AK6" s="28"/>
     </row>
     <row r="7" spans="1:37" ht="30">
@@ -42348,7 +42390,7 @@
       <c r="H7" s="69" t="s">
         <v>2951</v>
       </c>
-      <c r="I7" s="28"/>
+      <c r="I7" s="27"/>
       <c r="AK7" s="28"/>
     </row>
     <row r="8" spans="1:37" ht="21" thickBot="1">
@@ -42376,7 +42418,6 @@
       <c r="H8" s="69" t="s">
         <v>2952</v>
       </c>
-      <c r="I8" s="28"/>
       <c r="AK8" s="28"/>
     </row>
     <row r="9" spans="1:37" ht="21.75" thickTop="1" thickBot="1">
@@ -42502,10 +42543,10 @@
         <v>2885</v>
       </c>
       <c r="D13" s="67" t="s">
-        <v>3415</v>
+        <v>3411</v>
       </c>
       <c r="E13" s="70" t="s">
-        <v>3414</v>
+        <v>3410</v>
       </c>
       <c r="F13" s="68" t="s">
         <v>2880</v>
@@ -42522,20 +42563,20 @@
       <c r="A14" s="70" t="s">
         <v>2873</v>
       </c>
-      <c r="B14">
+      <c r="B14" s="19">
         <v>17</v>
       </c>
-      <c r="C14" s="66" t="s">
-        <v>3480</v>
+      <c r="C14" s="65" t="s">
+        <v>3485</v>
       </c>
       <c r="D14" s="67" t="s">
-        <v>3481</v>
+        <v>3487</v>
       </c>
       <c r="E14" s="70" t="s">
         <v>2873</v>
       </c>
       <c r="F14" s="68" t="s">
-        <v>2880</v>
+        <v>2888</v>
       </c>
       <c r="G14" s="72" t="s">
         <v>3407</v>
@@ -42546,73 +42587,71 @@
       <c r="I14" s="28"/>
     </row>
     <row r="15" spans="1:37" ht="20.25">
-      <c r="A15" s="65" t="s">
-        <v>3</v>
-      </c>
-      <c r="B15" s="65">
-        <v>21</v>
-      </c>
-      <c r="C15" s="73" t="s">
-        <v>2925</v>
-      </c>
-      <c r="D15" s="71" t="s">
-        <v>2936</v>
+      <c r="A15" s="70" t="s">
+        <v>2873</v>
+      </c>
+      <c r="B15" s="19">
+        <v>18</v>
+      </c>
+      <c r="C15" s="65" t="s">
+        <v>3484</v>
+      </c>
+      <c r="D15" s="67" t="s">
+        <v>3488</v>
       </c>
       <c r="E15" s="70" t="s">
-        <v>3405</v>
+        <v>2873</v>
       </c>
       <c r="F15" s="68" t="s">
         <v>2888</v>
       </c>
-      <c r="G15" s="68" t="s">
-        <v>2926</v>
-      </c>
-      <c r="H15" s="69" t="s">
-        <v>2931</v>
+      <c r="G15" s="72" t="s">
+        <v>3407</v>
+      </c>
+      <c r="H15" s="70" t="s">
+        <v>3408</v>
       </c>
       <c r="I15" s="28"/>
-      <c r="AK15" s="28"/>
     </row>
     <row r="16" spans="1:37" ht="20.25">
-      <c r="A16" s="65" t="s">
-        <v>3</v>
-      </c>
-      <c r="B16" s="65">
-        <v>22</v>
-      </c>
-      <c r="C16" s="73" t="s">
-        <v>2927</v>
+      <c r="A16" s="70" t="s">
+        <v>2873</v>
+      </c>
+      <c r="B16" s="19">
+        <v>19</v>
+      </c>
+      <c r="C16" s="65" t="s">
+        <v>3486</v>
       </c>
       <c r="D16" s="67" t="s">
-        <v>2934</v>
+        <v>3489</v>
       </c>
       <c r="E16" s="70" t="s">
-        <v>3405</v>
+        <v>2873</v>
       </c>
       <c r="F16" s="68" t="s">
-        <v>2880</v>
-      </c>
-      <c r="G16" s="68" t="s">
-        <v>2928</v>
-      </c>
-      <c r="H16" s="69" t="s">
-        <v>2932</v>
+        <v>2888</v>
+      </c>
+      <c r="G16" s="72" t="s">
+        <v>3407</v>
+      </c>
+      <c r="H16" s="70" t="s">
+        <v>3408</v>
       </c>
       <c r="I16" s="28"/>
-      <c r="AK16" s="28"/>
     </row>
     <row r="17" spans="1:37" ht="20.25">
       <c r="A17" s="65" t="s">
         <v>3</v>
       </c>
       <c r="B17" s="65">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C17" s="73" t="s">
-        <v>2922</v>
+        <v>2925</v>
       </c>
       <c r="D17" s="71" t="s">
-        <v>2923</v>
+        <v>2936</v>
       </c>
       <c r="E17" s="70" t="s">
         <v>3405</v>
@@ -42621,10 +42660,10 @@
         <v>2888</v>
       </c>
       <c r="G17" s="68" t="s">
-        <v>2921</v>
+        <v>2926</v>
       </c>
       <c r="H17" s="69" t="s">
-        <v>2924</v>
+        <v>2931</v>
       </c>
       <c r="I17" s="28"/>
       <c r="AK17" s="28"/>
@@ -42634,121 +42673,123 @@
         <v>3</v>
       </c>
       <c r="B18" s="65">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C18" s="73" t="s">
-        <v>2929</v>
+        <v>2927</v>
       </c>
       <c r="D18" s="67" t="s">
-        <v>2935</v>
+        <v>2934</v>
       </c>
       <c r="E18" s="70" t="s">
         <v>3405</v>
       </c>
       <c r="F18" s="68" t="s">
+        <v>2880</v>
+      </c>
+      <c r="G18" s="68" t="s">
+        <v>2928</v>
+      </c>
+      <c r="H18" s="69" t="s">
+        <v>2932</v>
+      </c>
+      <c r="I18" s="28"/>
+      <c r="AK18" s="28"/>
+    </row>
+    <row r="19" spans="1:37" ht="20.25">
+      <c r="A19" s="65" t="s">
+        <v>3</v>
+      </c>
+      <c r="B19" s="65">
+        <v>23</v>
+      </c>
+      <c r="C19" s="73" t="s">
+        <v>2922</v>
+      </c>
+      <c r="D19" s="71" t="s">
+        <v>2923</v>
+      </c>
+      <c r="E19" s="70" t="s">
+        <v>3405</v>
+      </c>
+      <c r="F19" s="68" t="s">
         <v>2888</v>
       </c>
-      <c r="G18" s="68" t="s">
-        <v>2930</v>
-      </c>
-      <c r="H18" s="69" t="s">
-        <v>2933</v>
-      </c>
-      <c r="I18" s="28"/>
-    </row>
-    <row r="19" spans="1:37" ht="30">
-      <c r="A19" s="70" t="s">
-        <v>3</v>
-      </c>
-      <c r="B19" s="64">
-        <v>25</v>
-      </c>
-      <c r="C19" s="66" t="s">
-        <v>2885</v>
-      </c>
-      <c r="D19" s="67" t="s">
-        <v>2910</v>
-      </c>
-      <c r="E19" s="70" t="s">
-        <v>3414</v>
-      </c>
-      <c r="F19" s="68" t="s">
-        <v>2880</v>
-      </c>
       <c r="G19" s="68" t="s">
-        <v>2887</v>
+        <v>2921</v>
       </c>
       <c r="H19" s="69" t="s">
-        <v>2886</v>
+        <v>2924</v>
       </c>
       <c r="I19" s="28"/>
+      <c r="AK19" s="28"/>
     </row>
     <row r="20" spans="1:37" ht="20.25">
       <c r="A20" s="65" t="s">
         <v>3</v>
       </c>
       <c r="B20" s="65">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C20" s="73" t="s">
-        <v>2918</v>
-      </c>
-      <c r="D20" s="71" t="s">
-        <v>2917</v>
+        <v>2929</v>
+      </c>
+      <c r="D20" s="67" t="s">
+        <v>2935</v>
       </c>
       <c r="E20" s="70" t="s">
         <v>3405</v>
       </c>
       <c r="F20" s="68" t="s">
+        <v>2888</v>
+      </c>
+      <c r="G20" s="68" t="s">
+        <v>2930</v>
+      </c>
+      <c r="H20" s="69" t="s">
+        <v>2933</v>
+      </c>
+      <c r="I20" s="28"/>
+    </row>
+    <row r="21" spans="1:37" ht="30">
+      <c r="A21" s="70" t="s">
+        <v>3</v>
+      </c>
+      <c r="B21" s="64">
+        <v>25</v>
+      </c>
+      <c r="C21" s="66" t="s">
+        <v>2885</v>
+      </c>
+      <c r="D21" s="67" t="s">
+        <v>2910</v>
+      </c>
+      <c r="E21" s="70" t="s">
+        <v>3410</v>
+      </c>
+      <c r="F21" s="68" t="s">
         <v>2880</v>
       </c>
-      <c r="G20" s="68" t="s">
-        <v>2916</v>
-      </c>
-      <c r="H20" s="69" t="s">
-        <v>2919</v>
-      </c>
-      <c r="I20" s="28"/>
-    </row>
-    <row r="21" spans="1:37" ht="20.25">
-      <c r="A21" s="65" t="s">
-        <v>2911</v>
-      </c>
-      <c r="B21" s="65">
-        <v>31</v>
-      </c>
-      <c r="C21" s="73" t="s">
-        <v>2925</v>
-      </c>
-      <c r="D21" s="71" t="s">
-        <v>2936</v>
-      </c>
-      <c r="E21" s="70" t="s">
-        <v>3405</v>
-      </c>
-      <c r="F21" s="68" t="s">
-        <v>2888</v>
-      </c>
       <c r="G21" s="68" t="s">
-        <v>2926</v>
+        <v>2887</v>
       </c>
       <c r="H21" s="69" t="s">
-        <v>2931</v>
+        <v>2886</v>
       </c>
       <c r="I21" s="28"/>
     </row>
     <row r="22" spans="1:37" ht="20.25">
       <c r="A22" s="65" t="s">
-        <v>2911</v>
+        <v>3</v>
       </c>
       <c r="B22" s="65">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="C22" s="73" t="s">
-        <v>2927</v>
-      </c>
-      <c r="D22" s="67" t="s">
-        <v>2934</v>
+        <v>2918</v>
+      </c>
+      <c r="D22" s="71" t="s">
+        <v>2917</v>
       </c>
       <c r="E22" s="70" t="s">
         <v>3405</v>
@@ -42757,10 +42798,10 @@
         <v>2880</v>
       </c>
       <c r="G22" s="68" t="s">
-        <v>2928</v>
+        <v>2916</v>
       </c>
       <c r="H22" s="69" t="s">
-        <v>2932</v>
+        <v>2919</v>
       </c>
       <c r="I22" s="28"/>
     </row>
@@ -42769,13 +42810,13 @@
         <v>2911</v>
       </c>
       <c r="B23" s="65">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C23" s="73" t="s">
-        <v>2922</v>
+        <v>2925</v>
       </c>
       <c r="D23" s="71" t="s">
-        <v>2923</v>
+        <v>2936</v>
       </c>
       <c r="E23" s="70" t="s">
         <v>3405</v>
@@ -42784,10 +42825,10 @@
         <v>2888</v>
       </c>
       <c r="G23" s="68" t="s">
-        <v>2921</v>
+        <v>2926</v>
       </c>
       <c r="H23" s="69" t="s">
-        <v>2924</v>
+        <v>2931</v>
       </c>
       <c r="I23" s="28"/>
     </row>
@@ -42796,52 +42837,52 @@
         <v>2911</v>
       </c>
       <c r="B24" s="65">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C24" s="73" t="s">
-        <v>2929</v>
+        <v>2927</v>
       </c>
       <c r="D24" s="67" t="s">
-        <v>2935</v>
+        <v>2934</v>
       </c>
       <c r="E24" s="70" t="s">
         <v>3405</v>
       </c>
       <c r="F24" s="68" t="s">
+        <v>2880</v>
+      </c>
+      <c r="G24" s="68" t="s">
+        <v>2928</v>
+      </c>
+      <c r="H24" s="69" t="s">
+        <v>2932</v>
+      </c>
+      <c r="I24" s="28"/>
+    </row>
+    <row r="25" spans="1:37" ht="20.25">
+      <c r="A25" s="65" t="s">
+        <v>2911</v>
+      </c>
+      <c r="B25" s="65">
+        <v>33</v>
+      </c>
+      <c r="C25" s="73" t="s">
+        <v>2922</v>
+      </c>
+      <c r="D25" s="71" t="s">
+        <v>2923</v>
+      </c>
+      <c r="E25" s="70" t="s">
+        <v>3405</v>
+      </c>
+      <c r="F25" s="68" t="s">
         <v>2888</v>
       </c>
-      <c r="G24" s="68" t="s">
-        <v>2930</v>
-      </c>
-      <c r="H24" s="69" t="s">
-        <v>2933</v>
-      </c>
-      <c r="I24" s="28"/>
-    </row>
-    <row r="25" spans="1:37" ht="30">
-      <c r="A25" s="70" t="s">
-        <v>2911</v>
-      </c>
-      <c r="B25" s="64">
-        <v>35</v>
-      </c>
-      <c r="C25" s="66" t="s">
-        <v>2885</v>
-      </c>
-      <c r="D25" s="67" t="s">
-        <v>2910</v>
-      </c>
-      <c r="E25" s="70" t="s">
-        <v>3414</v>
-      </c>
-      <c r="F25" s="68" t="s">
-        <v>2880</v>
-      </c>
       <c r="G25" s="68" t="s">
-        <v>2887</v>
+        <v>2921</v>
       </c>
       <c r="H25" s="69" t="s">
-        <v>2886</v>
+        <v>2924</v>
       </c>
       <c r="I25" s="28"/>
     </row>
@@ -42850,256 +42891,256 @@
         <v>2911</v>
       </c>
       <c r="B26" s="65">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C26" s="73" t="s">
-        <v>2918</v>
-      </c>
-      <c r="D26" s="71" t="s">
-        <v>2917</v>
+        <v>2929</v>
+      </c>
+      <c r="D26" s="67" t="s">
+        <v>2935</v>
       </c>
       <c r="E26" s="70" t="s">
         <v>3405</v>
       </c>
       <c r="F26" s="68" t="s">
-        <v>2880</v>
+        <v>2888</v>
       </c>
       <c r="G26" s="68" t="s">
-        <v>2916</v>
+        <v>2930</v>
       </c>
       <c r="H26" s="69" t="s">
-        <v>2919</v>
+        <v>2933</v>
       </c>
       <c r="I26" s="28"/>
     </row>
-    <row r="27" spans="1:37" ht="20.25">
-      <c r="A27" s="65" t="s">
-        <v>3410</v>
-      </c>
-      <c r="B27" s="65">
-        <v>41</v>
-      </c>
-      <c r="C27" s="65" t="s">
-        <v>3409</v>
-      </c>
-      <c r="D27" s="71" t="s">
-        <v>3412</v>
+    <row r="27" spans="1:37" ht="30">
+      <c r="A27" s="70" t="s">
+        <v>2911</v>
+      </c>
+      <c r="B27" s="64">
+        <v>35</v>
+      </c>
+      <c r="C27" s="66" t="s">
+        <v>2885</v>
+      </c>
+      <c r="D27" s="67" t="s">
+        <v>2910</v>
       </c>
       <c r="E27" s="70" t="s">
         <v>3410</v>
       </c>
       <c r="F27" s="68" t="s">
-        <v>2888</v>
-      </c>
-      <c r="G27" s="72" t="s">
-        <v>3407</v>
-      </c>
-      <c r="H27" s="70" t="s">
-        <v>3408</v>
+        <v>2880</v>
+      </c>
+      <c r="G27" s="68" t="s">
+        <v>2887</v>
+      </c>
+      <c r="H27" s="69" t="s">
+        <v>2886</v>
       </c>
       <c r="I27" s="28"/>
     </row>
     <row r="28" spans="1:37" ht="20.25">
       <c r="A28" s="65" t="s">
-        <v>2872</v>
+        <v>2911</v>
       </c>
       <c r="B28" s="65">
-        <v>51</v>
+        <v>36</v>
       </c>
       <c r="C28" s="73" t="s">
-        <v>2870</v>
-      </c>
-      <c r="D28" s="67" t="s">
-        <v>2871</v>
-      </c>
-      <c r="E28" s="67" t="s">
-        <v>2872</v>
+        <v>2918</v>
+      </c>
+      <c r="D28" s="71" t="s">
+        <v>2917</v>
+      </c>
+      <c r="E28" s="70" t="s">
+        <v>3405</v>
       </c>
       <c r="F28" s="68" t="s">
+        <v>2880</v>
+      </c>
+      <c r="G28" s="68" t="s">
+        <v>2916</v>
+      </c>
+      <c r="H28" s="69" t="s">
+        <v>2919</v>
+      </c>
+      <c r="I28" s="28"/>
+    </row>
+    <row r="29" spans="1:37" ht="30">
+      <c r="A29" s="70" t="s">
+        <v>3409</v>
+      </c>
+      <c r="B29" s="19">
+        <v>41</v>
+      </c>
+      <c r="C29" s="65" t="s">
+        <v>3480</v>
+      </c>
+      <c r="D29" s="71" t="s">
+        <v>3477</v>
+      </c>
+      <c r="E29" s="70" t="s">
+        <v>3409</v>
+      </c>
+      <c r="F29" s="68" t="s">
         <v>2888</v>
       </c>
-      <c r="G28" s="68" t="s">
-        <v>2941</v>
-      </c>
-      <c r="H28" s="69" t="s">
-        <v>2955</v>
-      </c>
-      <c r="I28" s="28"/>
-    </row>
-    <row r="29" spans="1:37" ht="20.25">
-      <c r="A29" s="65" t="s">
-        <v>2872</v>
-      </c>
-      <c r="B29" s="65">
-        <v>52</v>
-      </c>
-      <c r="C29" s="73" t="s">
-        <v>2862</v>
-      </c>
-      <c r="D29" s="67" t="s">
-        <v>2863</v>
-      </c>
-      <c r="E29" s="67" t="s">
-        <v>2872</v>
-      </c>
-      <c r="F29" s="68" t="s">
-        <v>2880</v>
-      </c>
-      <c r="G29" s="68" t="s">
-        <v>2944</v>
-      </c>
-      <c r="H29" s="69" t="s">
-        <v>2950</v>
+      <c r="G29" s="72" t="s">
+        <v>3407</v>
+      </c>
+      <c r="H29" s="70" t="s">
+        <v>3408</v>
       </c>
       <c r="I29" s="28"/>
     </row>
     <row r="30" spans="1:37" ht="30">
-      <c r="A30" s="65" t="s">
-        <v>2872</v>
-      </c>
-      <c r="B30" s="65">
-        <v>53</v>
-      </c>
-      <c r="C30" s="73" t="s">
-        <v>2904</v>
-      </c>
-      <c r="D30" s="67" t="s">
-        <v>3399</v>
-      </c>
-      <c r="E30" s="67" t="s">
-        <v>2872</v>
+      <c r="A30" s="70" t="s">
+        <v>3409</v>
+      </c>
+      <c r="B30" s="19">
+        <v>41</v>
+      </c>
+      <c r="C30" s="65" t="s">
+        <v>3481</v>
+      </c>
+      <c r="D30" s="71" t="s">
+        <v>3477</v>
+      </c>
+      <c r="E30" s="70" t="s">
+        <v>3409</v>
       </c>
       <c r="F30" s="68" t="s">
-        <v>2880</v>
-      </c>
-      <c r="G30" s="68" t="s">
-        <v>2947</v>
-      </c>
-      <c r="H30" s="69" t="s">
-        <v>2957</v>
+        <v>2888</v>
+      </c>
+      <c r="G30" s="72" t="s">
+        <v>3407</v>
+      </c>
+      <c r="H30" s="70" t="s">
+        <v>3408</v>
       </c>
       <c r="I30" s="28"/>
     </row>
-    <row r="31" spans="1:37" ht="30">
+    <row r="31" spans="1:37" ht="20.25">
       <c r="A31" s="65" t="s">
         <v>2872</v>
       </c>
-      <c r="B31" s="64">
-        <v>54</v>
+      <c r="B31" s="65">
+        <v>51</v>
       </c>
       <c r="C31" s="73" t="s">
-        <v>2914</v>
-      </c>
-      <c r="D31" s="71" t="s">
-        <v>3401</v>
-      </c>
-      <c r="E31" s="71" t="s">
+        <v>2870</v>
+      </c>
+      <c r="D31" s="67" t="s">
+        <v>2871</v>
+      </c>
+      <c r="E31" s="67" t="s">
         <v>2872</v>
       </c>
       <c r="F31" s="68" t="s">
-        <v>2880</v>
+        <v>2888</v>
       </c>
       <c r="G31" s="68" t="s">
-        <v>2915</v>
+        <v>2941</v>
       </c>
       <c r="H31" s="69" t="s">
-        <v>2920</v>
+        <v>2955</v>
       </c>
       <c r="I31" s="28"/>
     </row>
-    <row r="32" spans="1:37" ht="30">
-      <c r="A32" s="70" t="s">
+    <row r="32" spans="1:37" ht="20.25">
+      <c r="A32" s="65" t="s">
         <v>2872</v>
       </c>
-      <c r="B32" s="9">
-        <v>55</v>
+      <c r="B32" s="65">
+        <v>52</v>
       </c>
       <c r="C32" s="73" t="s">
-        <v>2906</v>
+        <v>2862</v>
       </c>
       <c r="D32" s="67" t="s">
-        <v>2905</v>
+        <v>2863</v>
       </c>
       <c r="E32" s="67" t="s">
         <v>2872</v>
       </c>
       <c r="F32" s="68" t="s">
-        <v>2888</v>
+        <v>2880</v>
       </c>
       <c r="G32" s="68" t="s">
+        <v>2944</v>
+      </c>
+      <c r="H32" s="69" t="s">
+        <v>2950</v>
+      </c>
+      <c r="I32" s="28"/>
+    </row>
+    <row r="33" spans="1:11" ht="30">
+      <c r="A33" s="65" t="s">
+        <v>2872</v>
+      </c>
+      <c r="B33" s="65">
+        <v>53</v>
+      </c>
+      <c r="C33" s="73" t="s">
+        <v>2904</v>
+      </c>
+      <c r="D33" s="67" t="s">
+        <v>3399</v>
+      </c>
+      <c r="E33" s="67" t="s">
+        <v>2872</v>
+      </c>
+      <c r="F33" s="68" t="s">
+        <v>2880</v>
+      </c>
+      <c r="G33" s="68" t="s">
         <v>2947</v>
       </c>
-      <c r="H32" s="69" t="s">
-        <v>2958</v>
-      </c>
-      <c r="I32" s="28"/>
-    </row>
-    <row r="33" spans="1:18" ht="20.25">
-      <c r="A33" s="70" t="s">
+      <c r="H33" s="69" t="s">
+        <v>2957</v>
+      </c>
+      <c r="I33" s="28"/>
+    </row>
+    <row r="34" spans="1:11" ht="30">
+      <c r="A34" s="65" t="s">
         <v>2872</v>
       </c>
-      <c r="B33" s="64">
-        <v>56</v>
-      </c>
-      <c r="C33" s="66" t="s">
-        <v>2892</v>
-      </c>
-      <c r="D33" s="71" t="s">
-        <v>3387</v>
-      </c>
-      <c r="E33" s="71" t="s">
-        <v>3406</v>
-      </c>
-      <c r="F33" s="68" t="s">
-        <v>2888</v>
-      </c>
-      <c r="G33" s="68" t="s">
-        <v>2894</v>
-      </c>
-      <c r="H33" s="69" t="s">
-        <v>2893</v>
-      </c>
-      <c r="I33" s="28"/>
-    </row>
-    <row r="34" spans="1:18" ht="30">
-      <c r="A34" s="70" t="s">
+      <c r="B34" s="64">
+        <v>54</v>
+      </c>
+      <c r="C34" s="73" t="s">
+        <v>2914</v>
+      </c>
+      <c r="D34" s="71" t="s">
+        <v>3401</v>
+      </c>
+      <c r="E34" s="71" t="s">
         <v>2872</v>
       </c>
-      <c r="B34" s="64">
-        <v>57</v>
-      </c>
-      <c r="C34" s="73" t="s">
-        <v>2860</v>
-      </c>
-      <c r="D34" s="67" t="s">
-        <v>2861</v>
-      </c>
-      <c r="E34" s="67" t="s">
-        <v>2872</v>
-      </c>
       <c r="F34" s="68" t="s">
-        <v>2888</v>
+        <v>2880</v>
       </c>
       <c r="G34" s="68" t="s">
-        <v>2945</v>
+        <v>2915</v>
       </c>
       <c r="H34" s="69" t="s">
-        <v>2956</v>
+        <v>2920</v>
       </c>
       <c r="I34" s="28"/>
     </row>
-    <row r="35" spans="1:18" ht="30">
+    <row r="35" spans="1:11" ht="30">
       <c r="A35" s="70" t="s">
         <v>2872</v>
       </c>
-      <c r="B35" s="64">
-        <v>58</v>
+      <c r="B35" s="9">
+        <v>55</v>
       </c>
       <c r="C35" s="73" t="s">
-        <v>2875</v>
+        <v>2906</v>
       </c>
       <c r="D35" s="67" t="s">
-        <v>3403</v>
+        <v>2905</v>
       </c>
       <c r="E35" s="67" t="s">
         <v>2872</v>
@@ -43108,122 +43149,140 @@
         <v>2888</v>
       </c>
       <c r="G35" s="68" t="s">
+        <v>2947</v>
+      </c>
+      <c r="H35" s="69" t="s">
+        <v>2958</v>
+      </c>
+      <c r="I35" s="28"/>
+    </row>
+    <row r="36" spans="1:11" ht="20.25">
+      <c r="A36" s="70" t="s">
+        <v>2872</v>
+      </c>
+      <c r="B36" s="64">
+        <v>56</v>
+      </c>
+      <c r="C36" s="66" t="s">
+        <v>2892</v>
+      </c>
+      <c r="D36" s="71" t="s">
+        <v>3387</v>
+      </c>
+      <c r="E36" s="71" t="s">
+        <v>3406</v>
+      </c>
+      <c r="F36" s="68" t="s">
+        <v>2888</v>
+      </c>
+      <c r="G36" s="68" t="s">
+        <v>2894</v>
+      </c>
+      <c r="H36" s="69" t="s">
+        <v>2893</v>
+      </c>
+      <c r="I36" s="28"/>
+    </row>
+    <row r="37" spans="1:11" ht="30">
+      <c r="A37" s="70" t="s">
+        <v>2872</v>
+      </c>
+      <c r="B37" s="64">
+        <v>57</v>
+      </c>
+      <c r="C37" s="73" t="s">
+        <v>2860</v>
+      </c>
+      <c r="D37" s="67" t="s">
+        <v>2861</v>
+      </c>
+      <c r="E37" s="67" t="s">
+        <v>2872</v>
+      </c>
+      <c r="F37" s="68" t="s">
+        <v>2888</v>
+      </c>
+      <c r="G37" s="68" t="s">
+        <v>2945</v>
+      </c>
+      <c r="H37" s="69" t="s">
+        <v>2956</v>
+      </c>
+      <c r="I37" s="28"/>
+    </row>
+    <row r="38" spans="1:11" ht="30">
+      <c r="A38" s="70" t="s">
+        <v>2872</v>
+      </c>
+      <c r="B38" s="64">
+        <v>58</v>
+      </c>
+      <c r="C38" s="73" t="s">
+        <v>2875</v>
+      </c>
+      <c r="D38" s="67" t="s">
+        <v>3403</v>
+      </c>
+      <c r="E38" s="67" t="s">
+        <v>2872</v>
+      </c>
+      <c r="F38" s="68" t="s">
+        <v>2888</v>
+      </c>
+      <c r="G38" s="68" t="s">
         <v>2940</v>
       </c>
-      <c r="H35" s="69" t="s">
+      <c r="H38" s="69" t="s">
         <v>2954</v>
       </c>
     </row>
-    <row r="36" spans="1:18" ht="60">
-      <c r="A36" s="70" t="s">
-        <v>3472</v>
-      </c>
-      <c r="B36" s="70">
+    <row r="39" spans="1:11" ht="75">
+      <c r="A39" s="70" t="s">
+        <v>3466</v>
+      </c>
+      <c r="B39" s="70">
         <v>62</v>
       </c>
-      <c r="C36" s="73" t="s">
-        <v>3474</v>
-      </c>
-      <c r="D36" s="67" t="s">
+      <c r="C39" s="65" t="s">
         <v>3482</v>
       </c>
-      <c r="E36" s="67" t="s">
-        <v>3472</v>
-      </c>
-      <c r="F36" s="68" t="s">
-        <v>2880</v>
-      </c>
-      <c r="G36" s="72" t="s">
+      <c r="D39" s="67" t="s">
+        <v>3497</v>
+      </c>
+      <c r="E39" s="67" t="s">
+        <v>3466</v>
+      </c>
+      <c r="F39" s="68" t="s">
+        <v>2888</v>
+      </c>
+      <c r="G39" s="72" t="s">
         <v>3407</v>
       </c>
-      <c r="H36" s="70" t="s">
+      <c r="H39" s="70" t="s">
         <v>3408</v>
       </c>
-    </row>
-    <row r="37" spans="1:18" ht="45">
-      <c r="A37" s="70" t="s">
-        <v>3472</v>
-      </c>
-      <c r="B37" s="70">
+      <c r="I39" s="27" t="s">
+        <v>3491</v>
+      </c>
+    </row>
+    <row r="40" spans="1:11" ht="45">
+      <c r="A40" s="70" t="s">
+        <v>3466</v>
+      </c>
+      <c r="B40" s="70">
         <v>63</v>
       </c>
-      <c r="C37" s="73" t="s">
-        <v>3477</v>
-      </c>
-      <c r="D37" s="67" t="s">
+      <c r="C40" s="65" t="s">
         <v>3483</v>
       </c>
-      <c r="E37" s="67" t="s">
-        <v>3472</v>
-      </c>
-      <c r="F37" s="68" t="s">
-        <v>2880</v>
-      </c>
-      <c r="G37" s="72" t="s">
-        <v>3407</v>
-      </c>
-      <c r="H37" s="70" t="s">
-        <v>3408</v>
-      </c>
-    </row>
-    <row r="38" spans="1:18" ht="45">
-      <c r="A38" s="70" t="s">
-        <v>3472</v>
-      </c>
-      <c r="B38" s="70">
-        <v>64</v>
-      </c>
-      <c r="C38" s="73" t="s">
-        <v>3478</v>
-      </c>
-      <c r="D38" s="67" t="s">
-        <v>3484</v>
-      </c>
-      <c r="E38" s="70" t="s">
-        <v>3472</v>
-      </c>
-      <c r="F38" s="68"/>
-      <c r="G38" s="72"/>
-      <c r="H38" s="70"/>
-    </row>
-    <row r="39" spans="1:18" ht="45">
-      <c r="A39" s="70" t="s">
-        <v>3472</v>
-      </c>
-      <c r="B39" s="70">
-        <v>65</v>
-      </c>
-      <c r="C39" s="73" t="s">
-        <v>3479</v>
-      </c>
-      <c r="D39" s="67" t="s">
-        <v>3485</v>
-      </c>
-      <c r="E39" s="70" t="s">
-        <v>3472</v>
-      </c>
-      <c r="F39" s="68"/>
-      <c r="G39" s="72"/>
-      <c r="H39" s="70"/>
-    </row>
-    <row r="40" spans="1:18" ht="15.75" customHeight="1">
-      <c r="A40" s="71" t="s">
-        <v>3417</v>
-      </c>
-      <c r="B40" s="64">
-        <v>101</v>
-      </c>
-      <c r="C40" s="73" t="s">
-        <v>3416</v>
-      </c>
-      <c r="D40" s="71" t="s">
-        <v>3486</v>
-      </c>
-      <c r="E40" s="71" t="s">
-        <v>3417</v>
+      <c r="D40" s="67" t="s">
+        <v>3471</v>
+      </c>
+      <c r="E40" s="67" t="s">
+        <v>3466</v>
       </c>
       <c r="F40" s="68" t="s">
-        <v>2880</v>
+        <v>2888</v>
       </c>
       <c r="G40" s="72" t="s">
         <v>3407</v>
@@ -43231,25 +43290,28 @@
       <c r="H40" s="70" t="s">
         <v>3408</v>
       </c>
-    </row>
-    <row r="41" spans="1:18" ht="20.25">
-      <c r="A41" s="71" t="s">
-        <v>3417</v>
+      <c r="I40" s="27" t="s">
+        <v>3494</v>
+      </c>
+    </row>
+    <row r="41" spans="1:11" ht="45">
+      <c r="A41" s="70" t="s">
+        <v>3466</v>
       </c>
       <c r="B41" s="70">
-        <v>102</v>
-      </c>
-      <c r="C41" s="73" t="s">
-        <v>3471</v>
-      </c>
-      <c r="D41" s="71" t="s">
-        <v>3487</v>
-      </c>
-      <c r="E41" s="71" t="s">
-        <v>3417</v>
+        <v>64</v>
+      </c>
+      <c r="C41" s="65" t="s">
+        <v>3469</v>
+      </c>
+      <c r="D41" s="67" t="s">
+        <v>3472</v>
+      </c>
+      <c r="E41" s="70" t="s">
+        <v>3466</v>
       </c>
       <c r="F41" s="68" t="s">
-        <v>2880</v>
+        <v>2888</v>
       </c>
       <c r="G41" s="72" t="s">
         <v>3407</v>
@@ -43257,195 +43319,260 @@
       <c r="H41" s="70" t="s">
         <v>3408</v>
       </c>
-    </row>
-    <row r="42" spans="1:18">
-      <c r="K42" t="s">
+      <c r="I41" s="27" t="s">
+        <v>3495</v>
+      </c>
+    </row>
+    <row r="42" spans="1:11" ht="45">
+      <c r="A42" s="70" t="s">
+        <v>3466</v>
+      </c>
+      <c r="B42" s="70">
+        <v>65</v>
+      </c>
+      <c r="C42" s="65" t="s">
+        <v>3470</v>
+      </c>
+      <c r="D42" s="67" t="s">
+        <v>3473</v>
+      </c>
+      <c r="E42" s="70" t="s">
+        <v>3466</v>
+      </c>
+      <c r="F42" s="68" t="s">
+        <v>2888</v>
+      </c>
+      <c r="G42" s="72" t="s">
+        <v>3407</v>
+      </c>
+      <c r="H42" s="70" t="s">
+        <v>3408</v>
+      </c>
+      <c r="I42" s="27" t="s">
+        <v>3496</v>
+      </c>
+    </row>
+    <row r="43" spans="1:11" ht="15.75" customHeight="1">
+      <c r="A43" s="71" t="s">
+        <v>3413</v>
+      </c>
+      <c r="B43" s="70">
+        <v>101</v>
+      </c>
+      <c r="C43" s="65" t="s">
+        <v>3412</v>
+      </c>
+      <c r="D43" s="71" t="s">
+        <v>3474</v>
+      </c>
+      <c r="E43" s="71" t="s">
+        <v>3413</v>
+      </c>
+      <c r="F43" s="68" t="s">
+        <v>2888</v>
+      </c>
+      <c r="G43" s="72" t="s">
+        <v>3407</v>
+      </c>
+      <c r="H43" s="70" t="s">
+        <v>3408</v>
+      </c>
+      <c r="I43" s="27" t="s">
+        <v>3492</v>
+      </c>
+    </row>
+    <row r="44" spans="1:11" ht="20.25">
+      <c r="A44" s="71" t="s">
+        <v>3413</v>
+      </c>
+      <c r="B44" s="70">
+        <v>102</v>
+      </c>
+      <c r="C44" s="65" t="s">
+        <v>3465</v>
+      </c>
+      <c r="D44" s="71" t="s">
+        <v>3475</v>
+      </c>
+      <c r="E44" s="71" t="s">
+        <v>3413</v>
+      </c>
+      <c r="F44" s="68" t="s">
+        <v>2888</v>
+      </c>
+      <c r="G44" s="72" t="s">
+        <v>3407</v>
+      </c>
+      <c r="H44" s="70" t="s">
+        <v>3408</v>
+      </c>
+      <c r="I44" s="27" t="s">
+        <v>3493</v>
+      </c>
+    </row>
+    <row r="45" spans="1:11" ht="20.25">
+      <c r="E45" s="76"/>
+      <c r="F45" s="78"/>
+      <c r="G45" s="79"/>
+      <c r="H45" s="77"/>
+      <c r="I45" s="27"/>
+    </row>
+    <row r="46" spans="1:11" ht="20.25">
+      <c r="E46" s="76"/>
+      <c r="F46" s="78"/>
+      <c r="G46" s="79"/>
+      <c r="H46" s="77"/>
+      <c r="I46" s="27"/>
+    </row>
+    <row r="47" spans="1:11">
+      <c r="K47" t="s">
         <v>3391</v>
       </c>
     </row>
-    <row r="43" spans="1:18">
-      <c r="K43" t="s">
+    <row r="48" spans="1:11">
+      <c r="K48" t="s">
         <v>3392</v>
       </c>
     </row>
-    <row r="44" spans="1:18">
-      <c r="K44" t="s">
+    <row r="49" spans="1:18">
+      <c r="K49" t="s">
         <v>3393</v>
       </c>
     </row>
-    <row r="45" spans="1:18">
-      <c r="K45" t="s">
+    <row r="50" spans="1:18">
+      <c r="K50" t="s">
         <v>3394</v>
       </c>
     </row>
-    <row r="46" spans="1:18">
-      <c r="K46" t="s">
+    <row r="51" spans="1:18">
+      <c r="K51" t="s">
         <v>3395</v>
       </c>
     </row>
-    <row r="47" spans="1:18">
-      <c r="K47" t="s">
+    <row r="52" spans="1:18">
+      <c r="K52" t="s">
         <v>3396</v>
       </c>
     </row>
-    <row r="48" spans="1:18">
-      <c r="K48" t="s">
+    <row r="53" spans="1:18">
+      <c r="K53" t="s">
         <v>3397</v>
       </c>
-      <c r="R48" t="s">
+      <c r="R53" t="s">
         <v>2962</v>
       </c>
     </row>
-    <row r="49" spans="1:18" ht="20.25">
-      <c r="A49" s="56" t="s">
+    <row r="54" spans="1:18" ht="20.25">
+      <c r="A54" s="56" t="s">
         <v>2874</v>
       </c>
-      <c r="B49" s="19"/>
-      <c r="C49" s="35" t="s">
+      <c r="B54" s="19"/>
+      <c r="C54" s="35" t="s">
         <v>2901</v>
       </c>
-      <c r="D49" s="34" t="s">
+      <c r="D54" s="34" t="s">
         <v>3388</v>
       </c>
-      <c r="E49" s="34" t="s">
+      <c r="E54" s="34" t="s">
         <v>2874</v>
       </c>
-      <c r="F49" s="35" t="s">
+      <c r="F54" s="35" t="s">
         <v>2900</v>
       </c>
-      <c r="G49" s="35" t="s">
+      <c r="G54" s="35" t="s">
         <v>2903</v>
       </c>
-      <c r="H49" s="53" t="s">
+      <c r="H54" s="53" t="s">
         <v>2902</v>
       </c>
-      <c r="K49" t="s">
+      <c r="K54" t="s">
         <v>3398</v>
       </c>
-      <c r="R49" t="s">
+      <c r="R54" t="s">
         <v>2963</v>
       </c>
     </row>
-    <row r="50" spans="1:18" ht="20.25">
-      <c r="A50" s="56" t="s">
+    <row r="55" spans="1:18" ht="20.25">
+      <c r="A55" s="56" t="s">
         <v>2874</v>
       </c>
-      <c r="B50" s="19"/>
-      <c r="C50" s="55" t="s">
+      <c r="B55" s="19"/>
+      <c r="C55" s="55" t="s">
         <v>2889</v>
       </c>
-      <c r="D50" s="34" t="s">
+      <c r="D55" s="34" t="s">
         <v>3388</v>
       </c>
-      <c r="E50" s="34" t="s">
+      <c r="E55" s="34" t="s">
         <v>2874</v>
       </c>
-      <c r="F50" s="35" t="s">
+      <c r="F55" s="35" t="s">
         <v>2888</v>
       </c>
-      <c r="G50" s="35" t="s">
+      <c r="G55" s="35" t="s">
         <v>2891</v>
       </c>
-      <c r="H50" s="53" t="s">
+      <c r="H55" s="53" t="s">
         <v>2890</v>
       </c>
-      <c r="R50" t="s">
+      <c r="R55" t="s">
         <v>2964</v>
       </c>
     </row>
-    <row r="51" spans="1:18" ht="30.75">
-      <c r="A51" s="19" t="s">
+    <row r="56" spans="1:18" ht="30.75">
+      <c r="A56" s="19" t="s">
         <v>2872</v>
       </c>
-      <c r="B51" s="19">
+      <c r="B56" s="19">
         <v>57</v>
       </c>
-      <c r="C51" s="33" t="s">
+      <c r="C56" s="33" t="s">
         <v>2909</v>
       </c>
-      <c r="D51" s="54" t="s">
+      <c r="D56" s="54" t="s">
         <v>3400</v>
       </c>
-      <c r="E51" s="19" t="s">
+      <c r="E56" s="19" t="s">
         <v>2872</v>
       </c>
-      <c r="F51" s="35" t="s">
+      <c r="F56" s="35" t="s">
         <v>2880</v>
       </c>
-      <c r="G51" s="35" t="s">
+      <c r="G56" s="35" t="s">
         <v>2949</v>
       </c>
-      <c r="H51" s="19" t="s">
+      <c r="H56" s="19" t="s">
         <v>2960</v>
       </c>
     </row>
-    <row r="52" spans="1:18" ht="20.25">
-      <c r="A52" s="19" t="s">
+    <row r="57" spans="1:18" ht="20.25">
+      <c r="A57" s="19" t="s">
         <v>2872</v>
       </c>
-      <c r="B52" s="31">
+      <c r="B57" s="31">
         <v>58</v>
       </c>
-      <c r="C52" s="33" t="s">
+      <c r="C57" s="33" t="s">
         <v>2908</v>
       </c>
-      <c r="D52" s="54" t="s">
+      <c r="D57" s="54" t="s">
         <v>2907</v>
       </c>
-      <c r="E52" s="19" t="s">
+      <c r="E57" s="19" t="s">
         <v>2872</v>
       </c>
-      <c r="F52" s="35" t="s">
+      <c r="F57" s="35" t="s">
         <v>2900</v>
       </c>
-      <c r="G52" s="35" t="s">
+      <c r="G57" s="35" t="s">
         <v>2948</v>
       </c>
-      <c r="H52" s="19" t="s">
+      <c r="H57" s="19" t="s">
         <v>2959</v>
       </c>
     </row>
-    <row r="53" spans="1:18" ht="20.25">
-      <c r="A53" s="6"/>
-      <c r="D53" s="57"/>
-      <c r="E53" s="6"/>
-      <c r="F53" s="36"/>
-      <c r="G53" s="36"/>
-      <c r="H53" s="6"/>
-    </row>
-    <row r="54" spans="1:18" ht="20.25">
-      <c r="A54" s="6"/>
-      <c r="D54" s="57"/>
-      <c r="E54" s="6"/>
-      <c r="F54" s="36"/>
-      <c r="G54" s="36"/>
-      <c r="H54" s="6"/>
-    </row>
-    <row r="55" spans="1:18" ht="20.25">
-      <c r="A55" s="6"/>
-      <c r="D55" s="57"/>
-      <c r="E55" s="6"/>
-      <c r="F55" s="36"/>
-      <c r="G55" s="36"/>
-      <c r="H55" s="6"/>
-    </row>
-    <row r="56" spans="1:18" ht="20.25">
-      <c r="A56" s="6"/>
-      <c r="D56" s="57"/>
-      <c r="E56" s="6"/>
-      <c r="F56" s="36"/>
-      <c r="G56" s="36"/>
-      <c r="H56" s="6"/>
-    </row>
-    <row r="57" spans="1:18" ht="20.25">
-      <c r="A57" s="6"/>
-      <c r="D57" s="57"/>
-      <c r="E57" s="6"/>
-      <c r="F57" s="36"/>
-      <c r="G57" s="36"/>
-      <c r="H57" s="6"/>
-    </row>
     <row r="58" spans="1:18" ht="20.25">
+      <c r="A58" s="6"/>
       <c r="D58" s="57"/>
       <c r="E58" s="6"/>
       <c r="F58" s="36"/>
@@ -43453,6 +43580,7 @@
       <c r="H58" s="6"/>
     </row>
     <row r="59" spans="1:18" ht="20.25">
+      <c r="A59" s="6"/>
       <c r="D59" s="57"/>
       <c r="E59" s="6"/>
       <c r="F59" s="36"/>
@@ -43460,6 +43588,7 @@
       <c r="H59" s="6"/>
     </row>
     <row r="60" spans="1:18" ht="20.25">
+      <c r="A60" s="6"/>
       <c r="D60" s="57"/>
       <c r="E60" s="6"/>
       <c r="F60" s="36"/>
@@ -43467,9 +43596,7 @@
       <c r="H60" s="6"/>
     </row>
     <row r="61" spans="1:18" ht="20.25">
-      <c r="A61" s="6" t="s">
-        <v>3418</v>
-      </c>
+      <c r="A61" s="6"/>
       <c r="D61" s="57"/>
       <c r="E61" s="6"/>
       <c r="F61" s="36"/>
@@ -43477,9 +43604,7 @@
       <c r="H61" s="6"/>
     </row>
     <row r="62" spans="1:18" ht="20.25">
-      <c r="A62" t="s">
-        <v>3432</v>
-      </c>
+      <c r="A62" s="6"/>
       <c r="D62" s="57"/>
       <c r="E62" s="6"/>
       <c r="F62" s="36"/>
@@ -43487,9 +43612,6 @@
       <c r="H62" s="6"/>
     </row>
     <row r="63" spans="1:18" ht="20.25">
-      <c r="A63" t="s">
-        <v>3433</v>
-      </c>
       <c r="D63" s="57"/>
       <c r="E63" s="6"/>
       <c r="F63" s="36"/>
@@ -43497,9 +43619,6 @@
       <c r="H63" s="6"/>
     </row>
     <row r="64" spans="1:18" ht="20.25">
-      <c r="A64" t="s">
-        <v>3420</v>
-      </c>
       <c r="D64" s="57"/>
       <c r="E64" s="6"/>
       <c r="F64" s="36"/>
@@ -43507,758 +43626,806 @@
       <c r="H64" s="6"/>
     </row>
     <row r="65" spans="1:18" ht="20.25">
-      <c r="A65" s="6" t="str">
-        <f>"&lt;tr&gt;&lt;td&gt;&lt;b&gt;"&amp;J65&amp;"&lt;/b&gt;&lt;/td&gt;&lt;td&gt;&lt;b&gt;"&amp;K65&amp;"&lt;/b&gt;&lt;/td&gt;&lt;td&gt;&lt;b&gt;"&amp;L65&amp;"&lt;/b&gt;&lt;/td&gt;&lt;td&gt;&lt;b&gt;"&amp;M65&amp;"&lt;/b&gt;&lt;/td&gt;"</f>
-        <v>&lt;tr&gt;&lt;td&gt;&lt;b&gt;Tag&lt;/b&gt;&lt;/td&gt;&lt;td&gt;&lt;b&gt;File Name&lt;/b&gt;&lt;/td&gt;&lt;td&gt;&lt;b&gt;URL&lt;/b&gt;&lt;/td&gt;&lt;td&gt;&lt;b&gt;Who&lt;/b&gt;&lt;/td&gt;</v>
-      </c>
-      <c r="J65" s="27" t="s">
-        <v>2876</v>
-      </c>
-      <c r="K65" s="27" t="s">
-        <v>2877</v>
-      </c>
-      <c r="L65" s="27" t="s">
-        <v>2878</v>
-      </c>
-      <c r="M65" s="27" t="s">
-        <v>2879</v>
-      </c>
+      <c r="D65" s="57"/>
+      <c r="E65" s="6"/>
+      <c r="F65" s="36"/>
+      <c r="G65" s="36"/>
+      <c r="H65" s="6"/>
     </row>
     <row r="66" spans="1:18" ht="20.25">
-      <c r="A66" s="6" t="str">
-        <f>"&lt;tr&gt;&lt;td&gt;"&amp;J66&amp;"&lt;/td&gt;&lt;td&gt;"&amp;K66&amp;"&lt;/td&gt;&lt;td&gt;"&amp;L66&amp;"&lt;/td&gt;&lt;td&gt;"&amp;M66&amp;"&lt;/td&gt;"</f>
-        <v>&lt;tr&gt;&lt;td&gt;N/A&lt;/td&gt;&lt;td&gt;GW170817-template.wav&lt;/td&gt;&lt;td&gt;https://www.gw-openscience.org/audiogwtc1/&lt;/td&gt;&lt;td&gt;LIGO detectors&lt;/td&gt;</v>
-      </c>
-      <c r="J66" s="27" t="s">
+      <c r="A66" s="6" t="s">
+        <v>3414</v>
+      </c>
+      <c r="D66" s="57"/>
+      <c r="E66" s="6"/>
+      <c r="F66" s="36"/>
+      <c r="G66" s="36"/>
+      <c r="H66" s="6"/>
+    </row>
+    <row r="67" spans="1:18" ht="20.25">
+      <c r="A67" t="s">
         <v>3428</v>
       </c>
-      <c r="K66" s="27" t="s">
-        <v>3431</v>
-      </c>
-      <c r="L66" s="29" t="s">
+      <c r="D67" s="57"/>
+      <c r="E67" s="6"/>
+      <c r="F67" s="36"/>
+      <c r="G67" s="36"/>
+      <c r="H67" s="6"/>
+    </row>
+    <row r="68" spans="1:18" ht="20.25">
+      <c r="A68" t="s">
         <v>3429</v>
       </c>
-      <c r="M66" s="27" t="s">
-        <v>3430</v>
-      </c>
-    </row>
-    <row r="67" spans="1:18" ht="20.25">
-      <c r="A67" s="6" t="str">
-        <f>"&lt;tr&gt;&lt;td&gt;"&amp;J67&amp;"&lt;/td&gt;&lt;td&gt;"&amp;K67&amp;"&lt;/td&gt;&lt;td&gt;"&amp;L67&amp;"&lt;/td&gt;&lt;td&gt;"&amp;M67&amp;"&lt;/td&gt;"</f>
-        <v>&lt;tr&gt;&lt;td&gt;zero/1.0/&lt;/td&gt;&lt;td&gt;145209__lensflare8642__shotgun-sounds.mp3&lt;/td&gt;&lt;td&gt;https://freesound.org/s/145209/&lt;/td&gt;&lt;td&gt;lensflare8642&lt;/td&gt;</v>
-      </c>
-      <c r="J67" s="15" t="s">
-        <v>2880</v>
-      </c>
-      <c r="K67" s="27" t="s">
-        <v>2885</v>
-      </c>
-      <c r="L67" s="29" t="s">
-        <v>2886</v>
-      </c>
-      <c r="M67" s="28" t="s">
-        <v>2887</v>
-      </c>
-      <c r="R67" t="str">
-        <f>"| "&amp;J67&amp;" | "&amp;K67&amp;" | "&amp;L67&amp;" | "&amp;M67&amp;" |"</f>
-        <v>| zero/1.0/ | 145209__lensflare8642__shotgun-sounds.mp3 | https://freesound.org/s/145209/ | lensflare8642 |</v>
-      </c>
-    </row>
-    <row r="68" spans="1:18" ht="20.25">
-      <c r="A68" s="6" t="str">
-        <f>"&lt;tr&gt;&lt;td&gt;"&amp;J68&amp;"&lt;/td&gt;&lt;td&gt;"&amp;K68&amp;"&lt;/td&gt;&lt;td&gt;"&amp;L68&amp;"&lt;/td&gt;&lt;td&gt;"&amp;M68&amp;"&lt;/td&gt;"</f>
-        <v>&lt;tr&gt;&lt;td&gt;zero/1.0/&lt;/td&gt;&lt;td&gt;162814__timgormly__spaceship-4.aiff&lt;/td&gt;&lt;td&gt;https://freesound.org/s/162814/&lt;/td&gt;&lt;td&gt;timgormly&lt;/td&gt;</v>
-      </c>
-      <c r="J68" s="52" t="s">
-        <v>2880</v>
-      </c>
-      <c r="K68" s="6" t="s">
-        <v>2909</v>
-      </c>
-      <c r="L68" t="s">
-        <v>2960</v>
-      </c>
-      <c r="M68" s="28" t="s">
-        <v>2949</v>
-      </c>
-      <c r="R68" t="str">
-        <f>"| "&amp;J68&amp;" | "&amp;K68&amp;" | "&amp;L68&amp;" | "&amp;M68&amp;" |"</f>
-        <v>| zero/1.0/ | 162814__timgormly__spaceship-4.aiff | https://freesound.org/s/162814/ | timgormly |</v>
-      </c>
+      <c r="D68" s="57"/>
+      <c r="E68" s="6"/>
+      <c r="F68" s="36"/>
+      <c r="G68" s="36"/>
+      <c r="H68" s="6"/>
     </row>
     <row r="69" spans="1:18" ht="20.25">
-      <c r="A69" s="6" t="str">
-        <f>"&lt;tr&gt;&lt;td&gt;"&amp;J69&amp;"&lt;/td&gt;&lt;td&gt;"&amp;K69&amp;"&lt;/td&gt;&lt;td&gt;"&amp;L69&amp;"&lt;/td&gt;&lt;td&gt;"&amp;M69&amp;"&lt;/td&gt;"</f>
-        <v>&lt;tr&gt;&lt;td&gt;by-nc/3.0/&lt;/td&gt;&lt;td&gt;165483__timbre__glitch-voice-ep-mp3.mp3&lt;/td&gt;&lt;td&gt;https://freesound.org/s/165483/&lt;/td&gt;&lt;td&gt;timbre&lt;/td&gt;</v>
-      </c>
-      <c r="J69" s="52" t="s">
-        <v>2900</v>
-      </c>
-      <c r="K69" s="6" t="s">
-        <v>2908</v>
-      </c>
-      <c r="L69" t="s">
-        <v>2959</v>
-      </c>
-      <c r="M69" s="28" t="s">
-        <v>2948</v>
-      </c>
-      <c r="R69" t="str">
-        <f>"| "&amp;J69&amp;" | "&amp;K69&amp;" | "&amp;L69&amp;" | "&amp;M69&amp;" |"</f>
-        <v>| by-nc/3.0/ | 165483__timbre__glitch-voice-ep-mp3.mp3 | https://freesound.org/s/165483/ | timbre |</v>
-      </c>
+      <c r="A69" t="s">
+        <v>3416</v>
+      </c>
+      <c r="D69" s="57"/>
+      <c r="E69" s="6"/>
+      <c r="F69" s="36"/>
+      <c r="G69" s="36"/>
+      <c r="H69" s="6"/>
     </row>
     <row r="70" spans="1:18" ht="20.25">
       <c r="A70" s="6" t="str">
-        <f>"&lt;tr&gt;&lt;td&gt;"&amp;J70&amp;"&lt;/td&gt;&lt;td&gt;"&amp;K70&amp;"&lt;/td&gt;&lt;td&gt;"&amp;L70&amp;"&lt;/td&gt;&lt;td&gt;"&amp;M70&amp;"&lt;/td&gt;"</f>
-        <v>&lt;tr&gt;&lt;td&gt;by/3.0/&lt;/td&gt;&lt;td&gt;169292__lazr2012__haywirefusionator.ogg&lt;/td&gt;&lt;td&gt;https://freesound.org/s/169292/&lt;/td&gt;&lt;td&gt;lazr2012&lt;/td&gt;</v>
-      </c>
-      <c r="J70" s="52" t="s">
-        <v>2888</v>
-      </c>
-      <c r="K70" s="6" t="s">
-        <v>2906</v>
-      </c>
-      <c r="L70" t="s">
-        <v>2958</v>
-      </c>
-      <c r="M70" s="28" t="s">
-        <v>2947</v>
-      </c>
-      <c r="R70" t="str">
-        <f>"| "&amp;J70&amp;" | "&amp;K70&amp;" | "&amp;L70&amp;" | "&amp;M70&amp;" |"</f>
-        <v>| by/3.0/ | 169292__lazr2012__haywirefusionator.ogg | https://freesound.org/s/169292/ | lazr2012 |</v>
+        <f>"&lt;tr&gt;&lt;td&gt;&lt;b&gt;"&amp;J70&amp;"&lt;/b&gt;&lt;/td&gt;&lt;td&gt;&lt;b&gt;"&amp;K70&amp;"&lt;/b&gt;&lt;/td&gt;&lt;td&gt;&lt;b&gt;"&amp;L70&amp;"&lt;/b&gt;&lt;/td&gt;&lt;td&gt;&lt;b&gt;"&amp;M70&amp;"&lt;/b&gt;&lt;/td&gt;"</f>
+        <v>&lt;tr&gt;&lt;td&gt;&lt;b&gt;Tag&lt;/b&gt;&lt;/td&gt;&lt;td&gt;&lt;b&gt;File Name&lt;/b&gt;&lt;/td&gt;&lt;td&gt;&lt;b&gt;URL&lt;/b&gt;&lt;/td&gt;&lt;td&gt;&lt;b&gt;Who&lt;/b&gt;&lt;/td&gt;</v>
+      </c>
+      <c r="J70" s="27" t="s">
+        <v>2876</v>
+      </c>
+      <c r="K70" s="27" t="s">
+        <v>2877</v>
+      </c>
+      <c r="L70" s="27" t="s">
+        <v>2878</v>
+      </c>
+      <c r="M70" s="27" t="s">
+        <v>2879</v>
       </c>
     </row>
     <row r="71" spans="1:18" ht="20.25">
       <c r="A71" s="6" t="str">
         <f>"&lt;tr&gt;&lt;td&gt;"&amp;J71&amp;"&lt;/td&gt;&lt;td&gt;"&amp;K71&amp;"&lt;/td&gt;&lt;td&gt;"&amp;L71&amp;"&lt;/td&gt;&lt;td&gt;"&amp;M71&amp;"&lt;/td&gt;"</f>
-        <v>&lt;tr&gt;&lt;td&gt;zero/1.0/&lt;/td&gt;&lt;td&gt;170136__lazr2012__machinery-bo.flac&lt;/td&gt;&lt;td&gt;https://freesound.org/s/170136/&lt;/td&gt;&lt;td&gt;lazr2012&lt;/td&gt;</v>
-      </c>
-      <c r="J71" s="52" t="s">
-        <v>2880</v>
-      </c>
-      <c r="K71" s="6" t="s">
-        <v>2904</v>
-      </c>
-      <c r="L71" t="s">
-        <v>2957</v>
-      </c>
-      <c r="M71" s="28" t="s">
-        <v>2947</v>
-      </c>
-      <c r="Q71" s="29"/>
-      <c r="R71" t="str">
-        <f>"| "&amp;J71&amp;" | "&amp;K71&amp;" | "&amp;L71&amp;" | "&amp;M71&amp;" |"</f>
-        <v>| zero/1.0/ | 170136__lazr2012__machinery-bo.flac | https://freesound.org/s/170136/ | lazr2012 |</v>
+        <v>&lt;tr&gt;&lt;td&gt;N/A&lt;/td&gt;&lt;td&gt;GW170817-template.wav&lt;/td&gt;&lt;td&gt;https://www.gw-openscience.org/audiogwtc1/&lt;/td&gt;&lt;td&gt;LIGO detectors&lt;/td&gt;</v>
+      </c>
+      <c r="J71" s="27" t="s">
+        <v>3424</v>
+      </c>
+      <c r="K71" s="27" t="s">
+        <v>3427</v>
+      </c>
+      <c r="L71" s="29" t="s">
+        <v>3425</v>
+      </c>
+      <c r="M71" s="27" t="s">
+        <v>3426</v>
       </c>
     </row>
     <row r="72" spans="1:18" ht="20.25">
       <c r="A72" s="6" t="str">
         <f>"&lt;tr&gt;&lt;td&gt;"&amp;J72&amp;"&lt;/td&gt;&lt;td&gt;"&amp;K72&amp;"&lt;/td&gt;&lt;td&gt;"&amp;L72&amp;"&lt;/td&gt;&lt;td&gt;"&amp;M72&amp;"&lt;/td&gt;"</f>
-        <v>&lt;tr&gt;&lt;td&gt;by-nc/3.0/&lt;/td&gt;&lt;td&gt;179281__timbre__boingy-sweep.flac&lt;/td&gt;&lt;td&gt;https://freesound.org/s/179281/&lt;/td&gt;&lt;td&gt;Timbre&lt;/td&gt;</v>
+        <v>&lt;tr&gt;&lt;td&gt;zero/1.0/&lt;/td&gt;&lt;td&gt;145209__lensflare8642__shotgun-sounds.mp3&lt;/td&gt;&lt;td&gt;https://freesound.org/s/145209/&lt;/td&gt;&lt;td&gt;lensflare8642&lt;/td&gt;</v>
       </c>
       <c r="J72" s="15" t="s">
-        <v>2900</v>
-      </c>
-      <c r="K72" s="4" t="s">
-        <v>2901</v>
+        <v>2880</v>
+      </c>
+      <c r="K72" s="27" t="s">
+        <v>2885</v>
       </c>
       <c r="L72" s="29" t="s">
-        <v>2902</v>
+        <v>2886</v>
       </c>
       <c r="M72" s="28" t="s">
-        <v>2903</v>
+        <v>2887</v>
       </c>
       <c r="R72" t="str">
-        <f t="shared" ref="R72:R73" si="0">"| "&amp;J72&amp;" | "&amp;K72&amp;" | "&amp;L72&amp;" | "&amp;M72&amp;" |"</f>
-        <v>| by-nc/3.0/ | 179281__timbre__boingy-sweep.flac | https://freesound.org/s/179281/ | Timbre |</v>
+        <f>"| "&amp;J72&amp;" | "&amp;K72&amp;" | "&amp;L72&amp;" | "&amp;M72&amp;" |"</f>
+        <v>| zero/1.0/ | 145209__lensflare8642__shotgun-sounds.mp3 | https://freesound.org/s/145209/ | lensflare8642 |</v>
       </c>
     </row>
     <row r="73" spans="1:18" ht="20.25">
       <c r="A73" s="6" t="str">
         <f>"&lt;tr&gt;&lt;td&gt;"&amp;J73&amp;"&lt;/td&gt;&lt;td&gt;"&amp;K73&amp;"&lt;/td&gt;&lt;td&gt;"&amp;L73&amp;"&lt;/td&gt;&lt;td&gt;"&amp;M73&amp;"&lt;/td&gt;"</f>
-        <v>&lt;tr&gt;&lt;td&gt;by/3.0/&lt;/td&gt;&lt;td&gt;216096__richerlandtv__u-f-o.mp3&lt;/td&gt;&lt;td&gt;https://freesound.org/s/216096/&lt;/td&gt;&lt;td&gt;RICHERlandTV&lt;/td&gt;</v>
-      </c>
-      <c r="J73" s="15" t="s">
-        <v>2888</v>
-      </c>
-      <c r="K73" s="4" t="s">
-        <v>2889</v>
-      </c>
-      <c r="L73" s="29" t="s">
-        <v>2890</v>
+        <v>&lt;tr&gt;&lt;td&gt;zero/1.0/&lt;/td&gt;&lt;td&gt;162814__timgormly__spaceship-4.aiff&lt;/td&gt;&lt;td&gt;https://freesound.org/s/162814/&lt;/td&gt;&lt;td&gt;timgormly&lt;/td&gt;</v>
+      </c>
+      <c r="J73" s="52" t="s">
+        <v>2880</v>
+      </c>
+      <c r="K73" s="6" t="s">
+        <v>2909</v>
+      </c>
+      <c r="L73" t="s">
+        <v>2960</v>
       </c>
       <c r="M73" s="28" t="s">
-        <v>2891</v>
+        <v>2949</v>
       </c>
       <c r="R73" t="str">
-        <f t="shared" si="0"/>
-        <v>| by/3.0/ | 216096__richerlandtv__u-f-o.mp3 | https://freesound.org/s/216096/ | RICHERlandTV |</v>
+        <f>"| "&amp;J73&amp;" | "&amp;K73&amp;" | "&amp;L73&amp;" | "&amp;M73&amp;" |"</f>
+        <v>| zero/1.0/ | 162814__timgormly__spaceship-4.aiff | https://freesound.org/s/162814/ | timgormly |</v>
       </c>
     </row>
     <row r="74" spans="1:18" ht="20.25">
       <c r="A74" s="6" t="str">
         <f>"&lt;tr&gt;&lt;td&gt;"&amp;J74&amp;"&lt;/td&gt;&lt;td&gt;"&amp;K74&amp;"&lt;/td&gt;&lt;td&gt;"&amp;L74&amp;"&lt;/td&gt;&lt;td&gt;"&amp;M74&amp;"&lt;/td&gt;"</f>
-        <v>&lt;tr&gt;&lt;td&gt;by/3.0/&lt;/td&gt;&lt;td&gt;221875__hero-of-the-winds__spring-boing.wav&lt;/td&gt;&lt;td&gt;https://freesound.org/s/221875/&lt;/td&gt;&lt;td&gt;hero-of-the-winds&lt;/td&gt;</v>
+        <v>&lt;tr&gt;&lt;td&gt;by-nc/3.0/&lt;/td&gt;&lt;td&gt;165483__timbre__glitch-voice-ep-mp3.mp3&lt;/td&gt;&lt;td&gt;https://freesound.org/s/165483/&lt;/td&gt;&lt;td&gt;timbre&lt;/td&gt;</v>
       </c>
       <c r="J74" s="52" t="s">
-        <v>2888</v>
+        <v>2900</v>
       </c>
       <c r="K74" s="6" t="s">
-        <v>2875</v>
+        <v>2908</v>
       </c>
       <c r="L74" t="s">
-        <v>2954</v>
+        <v>2959</v>
       </c>
       <c r="M74" s="28" t="s">
-        <v>2940</v>
+        <v>2948</v>
       </c>
       <c r="R74" t="str">
         <f>"| "&amp;J74&amp;" | "&amp;K74&amp;" | "&amp;L74&amp;" | "&amp;M74&amp;" |"</f>
-        <v>| by/3.0/ | 221875__hero-of-the-winds__spring-boing.wav | https://freesound.org/s/221875/ | hero-of-the-winds |</v>
+        <v>| by-nc/3.0/ | 165483__timbre__glitch-voice-ep-mp3.mp3 | https://freesound.org/s/165483/ | timbre |</v>
       </c>
     </row>
     <row r="75" spans="1:18" ht="20.25">
       <c r="A75" s="6" t="str">
         <f>"&lt;tr&gt;&lt;td&gt;"&amp;J75&amp;"&lt;/td&gt;&lt;td&gt;"&amp;K75&amp;"&lt;/td&gt;&lt;td&gt;"&amp;L75&amp;"&lt;/td&gt;&lt;td&gt;"&amp;M75&amp;"&lt;/td&gt;"</f>
-        <v>&lt;tr&gt;&lt;td&gt;by/3.0/&lt;/td&gt;&lt;td&gt;240297__jalastram__abstract-guitar-sfx-003.wav&lt;/td&gt;&lt;td&gt;https://freesound.org/s/240297/&lt;/td&gt;&lt;td&gt;jalastram&lt;/td&gt;</v>
-      </c>
-      <c r="J75" s="36" t="s">
+        <v>&lt;tr&gt;&lt;td&gt;by/3.0/&lt;/td&gt;&lt;td&gt;169292__lazr2012__haywirefusionator.ogg&lt;/td&gt;&lt;td&gt;https://freesound.org/s/169292/&lt;/td&gt;&lt;td&gt;lazr2012&lt;/td&gt;</v>
+      </c>
+      <c r="J75" s="52" t="s">
         <v>2888</v>
       </c>
       <c r="K75" s="6" t="s">
-        <v>2870</v>
-      </c>
-      <c r="L75" s="29" t="s">
-        <v>2955</v>
+        <v>2906</v>
+      </c>
+      <c r="L75" t="s">
+        <v>2958</v>
       </c>
       <c r="M75" s="28" t="s">
-        <v>2941</v>
+        <v>2947</v>
       </c>
       <c r="R75" t="str">
         <f>"| "&amp;J75&amp;" | "&amp;K75&amp;" | "&amp;L75&amp;" | "&amp;M75&amp;" |"</f>
-        <v>| by/3.0/ | 240297__jalastram__abstract-guitar-sfx-003.wav | https://freesound.org/s/240297/ | jalastram |</v>
+        <v>| by/3.0/ | 169292__lazr2012__haywirefusionator.ogg | https://freesound.org/s/169292/ | lazr2012 |</v>
       </c>
     </row>
     <row r="76" spans="1:18" ht="20.25">
       <c r="A76" s="6" t="str">
         <f>"&lt;tr&gt;&lt;td&gt;"&amp;J76&amp;"&lt;/td&gt;&lt;td&gt;"&amp;K76&amp;"&lt;/td&gt;&lt;td&gt;"&amp;L76&amp;"&lt;/td&gt;&lt;td&gt;"&amp;M76&amp;"&lt;/td&gt;"</f>
-        <v>&lt;tr&gt;&lt;td&gt;by/3.0/&lt;/td&gt;&lt;td&gt;272068__ichbinjager__shotgun-action.wav&lt;/td&gt;&lt;td&gt;https://freesound.org/s/272068/&lt;/td&gt;&lt;td&gt;IchBinJager&lt;/td&gt;</v>
-      </c>
-      <c r="J76" s="28" t="s">
-        <v>2888</v>
-      </c>
-      <c r="K76" t="s">
-        <v>2922</v>
-      </c>
-      <c r="L76" s="29" t="s">
-        <v>2924</v>
+        <v>&lt;tr&gt;&lt;td&gt;zero/1.0/&lt;/td&gt;&lt;td&gt;170136__lazr2012__machinery-bo.flac&lt;/td&gt;&lt;td&gt;https://freesound.org/s/170136/&lt;/td&gt;&lt;td&gt;lazr2012&lt;/td&gt;</v>
+      </c>
+      <c r="J76" s="52" t="s">
+        <v>2880</v>
+      </c>
+      <c r="K76" s="6" t="s">
+        <v>2904</v>
+      </c>
+      <c r="L76" t="s">
+        <v>2957</v>
       </c>
       <c r="M76" s="28" t="s">
-        <v>2921</v>
-      </c>
+        <v>2947</v>
+      </c>
+      <c r="Q76" s="29"/>
       <c r="R76" t="str">
         <f>"| "&amp;J76&amp;" | "&amp;K76&amp;" | "&amp;L76&amp;" | "&amp;M76&amp;" |"</f>
-        <v>| by/3.0/ | 272068__ichbinjager__shotgun-action.wav | https://freesound.org/s/272068/ | IchBinJager |</v>
+        <v>| zero/1.0/ | 170136__lazr2012__machinery-bo.flac | https://freesound.org/s/170136/ | lazr2012 |</v>
       </c>
     </row>
     <row r="77" spans="1:18" ht="20.25">
       <c r="A77" s="6" t="str">
         <f>"&lt;tr&gt;&lt;td&gt;"&amp;J77&amp;"&lt;/td&gt;&lt;td&gt;"&amp;K77&amp;"&lt;/td&gt;&lt;td&gt;"&amp;L77&amp;"&lt;/td&gt;&lt;td&gt;"&amp;M77&amp;"&lt;/td&gt;"</f>
-        <v>&lt;tr&gt;&lt;td&gt;by/3.0/&lt;/td&gt;&lt;td&gt;275537__wjoojoo__contact-mic-on-satellite-dish04.wav&lt;/td&gt;&lt;td&gt;https://freesound.org/s/275537/&lt;/td&gt;&lt;td&gt;wjoojoo&lt;/td&gt;</v>
-      </c>
-      <c r="J77" s="36" t="s">
-        <v>2888</v>
-      </c>
-      <c r="K77" s="6" t="s">
-        <v>2868</v>
-      </c>
-      <c r="L77" t="s">
-        <v>2951</v>
+        <v>&lt;tr&gt;&lt;td&gt;by-nc/3.0/&lt;/td&gt;&lt;td&gt;179281__timbre__boingy-sweep.flac&lt;/td&gt;&lt;td&gt;https://freesound.org/s/179281/&lt;/td&gt;&lt;td&gt;Timbre&lt;/td&gt;</v>
+      </c>
+      <c r="J77" s="15" t="s">
+        <v>2900</v>
+      </c>
+      <c r="K77" s="4" t="s">
+        <v>2901</v>
+      </c>
+      <c r="L77" s="29" t="s">
+        <v>2902</v>
       </c>
       <c r="M77" s="28" t="s">
-        <v>2942</v>
+        <v>2903</v>
       </c>
       <c r="R77" t="str">
-        <f>"| "&amp;J77&amp;" | "&amp;K77&amp;" | "&amp;L77&amp;" | "&amp;M77&amp;" |"</f>
-        <v>| by/3.0/ | 275537__wjoojoo__contact-mic-on-satellite-dish04.wav | https://freesound.org/s/275537/ | wjoojoo |</v>
+        <f t="shared" ref="R77:R78" si="0">"| "&amp;J77&amp;" | "&amp;K77&amp;" | "&amp;L77&amp;" | "&amp;M77&amp;" |"</f>
+        <v>| by-nc/3.0/ | 179281__timbre__boingy-sweep.flac | https://freesound.org/s/179281/ | Timbre |</v>
       </c>
     </row>
     <row r="78" spans="1:18" ht="20.25">
       <c r="A78" s="6" t="str">
         <f>"&lt;tr&gt;&lt;td&gt;"&amp;J78&amp;"&lt;/td&gt;&lt;td&gt;"&amp;K78&amp;"&lt;/td&gt;&lt;td&gt;"&amp;L78&amp;"&lt;/td&gt;&lt;td&gt;"&amp;M78&amp;"&lt;/td&gt;"</f>
-        <v>&lt;tr&gt;&lt;td&gt;zero/1.0/&lt;/td&gt;&lt;td&gt;352852__josepharaoh99__game-style-laser-beam.wav&lt;/td&gt;&lt;td&gt;https://freesound.org/s/352852/&lt;/td&gt;&lt;td&gt;josepharaoh99&lt;/td&gt;</v>
-      </c>
-      <c r="J78" s="36" t="s">
-        <v>2880</v>
-      </c>
-      <c r="K78" s="6" t="s">
-        <v>2866</v>
-      </c>
-      <c r="L78" t="s">
-        <v>2952</v>
+        <v>&lt;tr&gt;&lt;td&gt;by/3.0/&lt;/td&gt;&lt;td&gt;216096__richerlandtv__u-f-o.mp3&lt;/td&gt;&lt;td&gt;https://freesound.org/s/216096/&lt;/td&gt;&lt;td&gt;RICHERlandTV&lt;/td&gt;</v>
+      </c>
+      <c r="J78" s="15" t="s">
+        <v>2888</v>
+      </c>
+      <c r="K78" s="4" t="s">
+        <v>2889</v>
+      </c>
+      <c r="L78" s="29" t="s">
+        <v>2890</v>
       </c>
       <c r="M78" s="28" t="s">
-        <v>2943</v>
+        <v>2891</v>
       </c>
       <c r="R78" t="str">
-        <f>"| "&amp;J78&amp;" | "&amp;K78&amp;" | "&amp;L78&amp;" | "&amp;M78&amp;" |"</f>
-        <v>| zero/1.0/ | 352852__josepharaoh99__game-style-laser-beam.wav | https://freesound.org/s/352852/ | josepharaoh99 |</v>
+        <f t="shared" si="0"/>
+        <v>| by/3.0/ | 216096__richerlandtv__u-f-o.mp3 | https://freesound.org/s/216096/ | RICHERlandTV |</v>
       </c>
     </row>
     <row r="79" spans="1:18" ht="20.25">
       <c r="A79" s="6" t="str">
         <f>"&lt;tr&gt;&lt;td&gt;"&amp;J79&amp;"&lt;/td&gt;&lt;td&gt;"&amp;K79&amp;"&lt;/td&gt;&lt;td&gt;"&amp;L79&amp;"&lt;/td&gt;&lt;td&gt;"&amp;M79&amp;"&lt;/td&gt;"</f>
-        <v>&lt;tr&gt;&lt;td&gt;zero/1.0/&lt;/td&gt;&lt;td&gt;380886__morganpurkis__doom-shotgun-2017.wav&lt;/td&gt;&lt;td&gt;https://freesound.org/s/380886/&lt;/td&gt;&lt;td&gt;morganpurkis&lt;/td&gt;</v>
-      </c>
-      <c r="J79" s="28" t="s">
-        <v>2880</v>
-      </c>
-      <c r="K79" t="s">
-        <v>2918</v>
-      </c>
-      <c r="L79" s="29" t="s">
-        <v>2919</v>
+        <v>&lt;tr&gt;&lt;td&gt;by/3.0/&lt;/td&gt;&lt;td&gt;221875__hero-of-the-winds__spring-boing.wav&lt;/td&gt;&lt;td&gt;https://freesound.org/s/221875/&lt;/td&gt;&lt;td&gt;hero-of-the-winds&lt;/td&gt;</v>
+      </c>
+      <c r="J79" s="52" t="s">
+        <v>2888</v>
+      </c>
+      <c r="K79" s="6" t="s">
+        <v>2875</v>
+      </c>
+      <c r="L79" t="s">
+        <v>2954</v>
       </c>
       <c r="M79" s="28" t="s">
-        <v>2916</v>
+        <v>2940</v>
       </c>
       <c r="R79" t="str">
         <f>"| "&amp;J79&amp;" | "&amp;K79&amp;" | "&amp;L79&amp;" | "&amp;M79&amp;" |"</f>
-        <v>| zero/1.0/ | 380886__morganpurkis__doom-shotgun-2017.wav | https://freesound.org/s/380886/ | morganpurkis |</v>
+        <v>| by/3.0/ | 221875__hero-of-the-winds__spring-boing.wav | https://freesound.org/s/221875/ | hero-of-the-winds |</v>
       </c>
     </row>
     <row r="80" spans="1:18" ht="20.25">
       <c r="A80" s="6" t="str">
         <f>"&lt;tr&gt;&lt;td&gt;"&amp;J80&amp;"&lt;/td&gt;&lt;td&gt;"&amp;K80&amp;"&lt;/td&gt;&lt;td&gt;"&amp;L80&amp;"&lt;/td&gt;&lt;td&gt;"&amp;M80&amp;"&lt;/td&gt;"</f>
-        <v>&lt;tr&gt;&lt;td&gt;by/3.0/&lt;/td&gt;&lt;td&gt;383205__spiceprogram__loading-sound.wav&lt;/td&gt;&lt;td&gt;https://freesound.org/s/383205/&lt;/td&gt;&lt;td&gt;SpiceProgram&lt;/td&gt;</v>
-      </c>
-      <c r="J80" s="30" t="s">
+        <v>&lt;tr&gt;&lt;td&gt;by/3.0/&lt;/td&gt;&lt;td&gt;240297__jalastram__abstract-guitar-sfx-003.wav&lt;/td&gt;&lt;td&gt;https://freesound.org/s/240297/&lt;/td&gt;&lt;td&gt;jalastram&lt;/td&gt;</v>
+      </c>
+      <c r="J80" s="36" t="s">
         <v>2888</v>
       </c>
-      <c r="K80" s="28" t="s">
-        <v>2864</v>
+      <c r="K80" s="6" t="s">
+        <v>2870</v>
       </c>
       <c r="L80" s="29" t="s">
-        <v>2898</v>
+        <v>2955</v>
       </c>
       <c r="M80" s="28" t="s">
-        <v>2899</v>
+        <v>2941</v>
       </c>
       <c r="R80" t="str">
         <f>"| "&amp;J80&amp;" | "&amp;K80&amp;" | "&amp;L80&amp;" | "&amp;M80&amp;" |"</f>
-        <v>| by/3.0/ | 383205__spiceprogram__loading-sound.wav | https://freesound.org/s/383205/ | SpiceProgram |</v>
+        <v>| by/3.0/ | 240297__jalastram__abstract-guitar-sfx-003.wav | https://freesound.org/s/240297/ | jalastram |</v>
       </c>
     </row>
     <row r="81" spans="1:18" ht="20.25">
       <c r="A81" s="6" t="str">
         <f>"&lt;tr&gt;&lt;td&gt;"&amp;J81&amp;"&lt;/td&gt;&lt;td&gt;"&amp;K81&amp;"&lt;/td&gt;&lt;td&gt;"&amp;L81&amp;"&lt;/td&gt;&lt;td&gt;"&amp;M81&amp;"&lt;/td&gt;"</f>
-        <v>&lt;tr&gt;&lt;td&gt;zero/1.0/&lt;/td&gt;&lt;td&gt;383760__deleted-user-7146007__laboratory-mad-scientist-science-fiction-sci-fi.wav&lt;/td&gt;&lt;td&gt;https://freesound.org/s/383760/&lt;/td&gt;&lt;td&gt;deleted-user-7146007&lt;/td&gt;</v>
-      </c>
-      <c r="J81" s="35" t="s">
-        <v>2880</v>
-      </c>
-      <c r="K81" s="19" t="s">
-        <v>2862</v>
-      </c>
-      <c r="L81" t="s">
-        <v>2950</v>
+        <v>&lt;tr&gt;&lt;td&gt;by/3.0/&lt;/td&gt;&lt;td&gt;272068__ichbinjager__shotgun-action.wav&lt;/td&gt;&lt;td&gt;https://freesound.org/s/272068/&lt;/td&gt;&lt;td&gt;IchBinJager&lt;/td&gt;</v>
+      </c>
+      <c r="J81" s="28" t="s">
+        <v>2888</v>
+      </c>
+      <c r="K81" t="s">
+        <v>2922</v>
+      </c>
+      <c r="L81" s="29" t="s">
+        <v>2924</v>
       </c>
       <c r="M81" s="28" t="s">
-        <v>2944</v>
+        <v>2921</v>
       </c>
       <c r="R81" t="str">
         <f>"| "&amp;J81&amp;" | "&amp;K81&amp;" | "&amp;L81&amp;" | "&amp;M81&amp;" |"</f>
-        <v>| zero/1.0/ | 383760__deleted-user-7146007__laboratory-mad-scientist-science-fiction-sci-fi.wav | https://freesound.org/s/383760/ | deleted-user-7146007 |</v>
+        <v>| by/3.0/ | 272068__ichbinjager__shotgun-action.wav | https://freesound.org/s/272068/ | IchBinJager |</v>
       </c>
     </row>
     <row r="82" spans="1:18" ht="20.25">
       <c r="A82" s="6" t="str">
         <f>"&lt;tr&gt;&lt;td&gt;"&amp;J82&amp;"&lt;/td&gt;&lt;td&gt;"&amp;K82&amp;"&lt;/td&gt;&lt;td&gt;"&amp;L82&amp;"&lt;/td&gt;&lt;td&gt;"&amp;M82&amp;"&lt;/td&gt;"</f>
-        <v>&lt;tr&gt;&lt;td&gt;zero/1.0/&lt;/td&gt;&lt;td&gt;397254__screamstudio__loading.wav&lt;/td&gt;&lt;td&gt;https://freesound.org/s/397254/&lt;/td&gt;&lt;td&gt;ScreamStudio&lt;/td&gt;</v>
-      </c>
-      <c r="J82" s="32" t="s">
-        <v>2880</v>
-      </c>
-      <c r="K82" s="35" t="s">
-        <v>2854</v>
-      </c>
-      <c r="L82" s="29" t="s">
-        <v>2883</v>
+        <v>&lt;tr&gt;&lt;td&gt;by/3.0/&lt;/td&gt;&lt;td&gt;275537__wjoojoo__contact-mic-on-satellite-dish04.wav&lt;/td&gt;&lt;td&gt;https://freesound.org/s/275537/&lt;/td&gt;&lt;td&gt;wjoojoo&lt;/td&gt;</v>
+      </c>
+      <c r="J82" s="36" t="s">
+        <v>2888</v>
+      </c>
+      <c r="K82" s="6" t="s">
+        <v>2868</v>
+      </c>
+      <c r="L82" t="s">
+        <v>2951</v>
       </c>
       <c r="M82" s="28" t="s">
-        <v>2884</v>
+        <v>2942</v>
       </c>
       <c r="R82" t="str">
         <f>"| "&amp;J82&amp;" | "&amp;K82&amp;" | "&amp;L82&amp;" | "&amp;M82&amp;" |"</f>
-        <v>| zero/1.0/ | 397254__screamstudio__loading.wav | https://freesound.org/s/397254/ | ScreamStudio |</v>
+        <v>| by/3.0/ | 275537__wjoojoo__contact-mic-on-satellite-dish04.wav | https://freesound.org/s/275537/ | wjoojoo |</v>
       </c>
     </row>
     <row r="83" spans="1:18" ht="20.25">
       <c r="A83" s="6" t="str">
         <f>"&lt;tr&gt;&lt;td&gt;"&amp;J83&amp;"&lt;/td&gt;&lt;td&gt;"&amp;K83&amp;"&lt;/td&gt;&lt;td&gt;"&amp;L83&amp;"&lt;/td&gt;&lt;td&gt;"&amp;M83&amp;"&lt;/td&gt;"</f>
-        <v>&lt;tr&gt;&lt;td&gt;zero/1.0/&lt;/td&gt;&lt;td&gt;404068__swordofkings128__backyard-gate-open.wav&lt;/td&gt;&lt;td&gt;https://freesound.org/s/404068/&lt;/td&gt;&lt;td&gt;swordofkings128&lt;/td&gt;</v>
-      </c>
-      <c r="J83" s="35" t="s">
+        <v>&lt;tr&gt;&lt;td&gt;zero/1.0/&lt;/td&gt;&lt;td&gt;352852__josepharaoh99__game-style-laser-beam.wav&lt;/td&gt;&lt;td&gt;https://freesound.org/s/352852/&lt;/td&gt;&lt;td&gt;josepharaoh99&lt;/td&gt;</v>
+      </c>
+      <c r="J83" s="36" t="s">
         <v>2880</v>
       </c>
-      <c r="K83" s="19" t="s">
-        <v>2927</v>
-      </c>
-      <c r="L83" s="29" t="s">
-        <v>2932</v>
+      <c r="K83" s="6" t="s">
+        <v>2866</v>
+      </c>
+      <c r="L83" t="s">
+        <v>2952</v>
       </c>
       <c r="M83" s="28" t="s">
-        <v>2928</v>
+        <v>2943</v>
       </c>
       <c r="R83" t="str">
         <f>"| "&amp;J83&amp;" | "&amp;K83&amp;" | "&amp;L83&amp;" | "&amp;M83&amp;" |"</f>
-        <v>| zero/1.0/ | 404068__swordofkings128__backyard-gate-open.wav | https://freesound.org/s/404068/ | swordofkings128 |</v>
+        <v>| zero/1.0/ | 352852__josepharaoh99__game-style-laser-beam.wav | https://freesound.org/s/352852/ | josepharaoh99 |</v>
       </c>
     </row>
     <row r="84" spans="1:18" ht="20.25">
       <c r="A84" s="6" t="str">
         <f>"&lt;tr&gt;&lt;td&gt;"&amp;J84&amp;"&lt;/td&gt;&lt;td&gt;"&amp;K84&amp;"&lt;/td&gt;&lt;td&gt;"&amp;L84&amp;"&lt;/td&gt;&lt;td&gt;"&amp;M84&amp;"&lt;/td&gt;"</f>
-        <v>&lt;tr&gt;&lt;td&gt;zero/1.0/&lt;/td&gt;&lt;td&gt;407052__sojan__power-charge.flac&lt;/td&gt;&lt;td&gt;https://freesound.org/s/193610/&lt;/td&gt;&lt;td&gt;crashoverride61088&lt;/td&gt;</v>
-      </c>
-      <c r="J84" s="32" t="s">
+        <v>&lt;tr&gt;&lt;td&gt;zero/1.0/&lt;/td&gt;&lt;td&gt;380886__morganpurkis__doom-shotgun-2017.wav&lt;/td&gt;&lt;td&gt;https://freesound.org/s/380886/&lt;/td&gt;&lt;td&gt;morganpurkis&lt;/td&gt;</v>
+      </c>
+      <c r="J84" s="28" t="s">
         <v>2880</v>
       </c>
-      <c r="K84" s="35" t="s">
-        <v>2856</v>
+      <c r="K84" t="s">
+        <v>2918</v>
       </c>
       <c r="L84" s="29" t="s">
-        <v>2881</v>
+        <v>2919</v>
       </c>
       <c r="M84" s="28" t="s">
-        <v>2882</v>
+        <v>2916</v>
       </c>
       <c r="R84" t="str">
         <f>"| "&amp;J84&amp;" | "&amp;K84&amp;" | "&amp;L84&amp;" | "&amp;M84&amp;" |"</f>
-        <v>| zero/1.0/ | 407052__sojan__power-charge.flac | https://freesound.org/s/193610/ | crashoverride61088 |</v>
+        <v>| zero/1.0/ | 380886__morganpurkis__doom-shotgun-2017.wav | https://freesound.org/s/380886/ | morganpurkis |</v>
       </c>
     </row>
     <row r="85" spans="1:18" ht="20.25">
       <c r="A85" s="6" t="str">
         <f>"&lt;tr&gt;&lt;td&gt;"&amp;J85&amp;"&lt;/td&gt;&lt;td&gt;"&amp;K85&amp;"&lt;/td&gt;&lt;td&gt;"&amp;L85&amp;"&lt;/td&gt;&lt;td&gt;"&amp;M85&amp;"&lt;/td&gt;"</f>
-        <v>&lt;tr&gt;&lt;td&gt;by/3.0/&lt;/td&gt;&lt;td&gt;417131__cuddlenucks__science-fiction-noise-3.wav&lt;/td&gt;&lt;td&gt;https://freesound.org/s/417131/&lt;/td&gt;&lt;td&gt;cuddlenucks&lt;/td&gt;</v>
-      </c>
-      <c r="J85" s="35" t="s">
+        <v>&lt;tr&gt;&lt;td&gt;by/3.0/&lt;/td&gt;&lt;td&gt;383205__spiceprogram__loading-sound.wav&lt;/td&gt;&lt;td&gt;https://freesound.org/s/383205/&lt;/td&gt;&lt;td&gt;SpiceProgram&lt;/td&gt;</v>
+      </c>
+      <c r="J85" s="30" t="s">
         <v>2888</v>
       </c>
-      <c r="K85" s="19" t="s">
-        <v>2860</v>
-      </c>
-      <c r="L85" t="s">
-        <v>2956</v>
+      <c r="K85" s="28" t="s">
+        <v>2864</v>
+      </c>
+      <c r="L85" s="29" t="s">
+        <v>2898</v>
       </c>
       <c r="M85" s="28" t="s">
-        <v>2945</v>
+        <v>2899</v>
       </c>
       <c r="R85" t="str">
         <f>"| "&amp;J85&amp;" | "&amp;K85&amp;" | "&amp;L85&amp;" | "&amp;M85&amp;" |"</f>
-        <v>| by/3.0/ | 417131__cuddlenucks__science-fiction-noise-3.wav | https://freesound.org/s/417131/ | cuddlenucks |</v>
+        <v>| by/3.0/ | 383205__spiceprogram__loading-sound.wav | https://freesound.org/s/383205/ | SpiceProgram |</v>
       </c>
     </row>
     <row r="86" spans="1:18" ht="20.25">
       <c r="A86" s="6" t="str">
         <f>"&lt;tr&gt;&lt;td&gt;"&amp;J86&amp;"&lt;/td&gt;&lt;td&gt;"&amp;K86&amp;"&lt;/td&gt;&lt;td&gt;"&amp;L86&amp;"&lt;/td&gt;&lt;td&gt;"&amp;M86&amp;"&lt;/td&gt;"</f>
-        <v>&lt;tr&gt;&lt;td&gt;by/3.0/&lt;/td&gt;&lt;td&gt;417363__xcreenplay__boing-massive-kick.wav&lt;/td&gt;&lt;td&gt;https://freesound.org/s/417363/&lt;/td&gt;&lt;td&gt;xcreenplay&lt;/td&gt;</v>
+        <v>&lt;tr&gt;&lt;td&gt;zero/1.0/&lt;/td&gt;&lt;td&gt;383760__deleted-user-7146007__laboratory-mad-scientist-science-fiction-sci-fi.wav&lt;/td&gt;&lt;td&gt;https://freesound.org/s/383760/&lt;/td&gt;&lt;td&gt;deleted-user-7146007&lt;/td&gt;</v>
       </c>
       <c r="J86" s="35" t="s">
-        <v>2888</v>
+        <v>2880</v>
       </c>
       <c r="K86" s="19" t="s">
-        <v>2858</v>
+        <v>2862</v>
       </c>
       <c r="L86" t="s">
-        <v>2953</v>
+        <v>2950</v>
       </c>
       <c r="M86" s="28" t="s">
-        <v>2946</v>
+        <v>2944</v>
       </c>
       <c r="R86" t="str">
         <f>"| "&amp;J86&amp;" | "&amp;K86&amp;" | "&amp;L86&amp;" | "&amp;M86&amp;" |"</f>
-        <v>| by/3.0/ | 417363__xcreenplay__boing-massive-kick.wav | https://freesound.org/s/417363/ | xcreenplay |</v>
+        <v>| zero/1.0/ | 383760__deleted-user-7146007__laboratory-mad-scientist-science-fiction-sci-fi.wav | https://freesound.org/s/383760/ | deleted-user-7146007 |</v>
       </c>
     </row>
     <row r="87" spans="1:18" ht="20.25">
       <c r="A87" s="6" t="str">
         <f>"&lt;tr&gt;&lt;td&gt;"&amp;J87&amp;"&lt;/td&gt;&lt;td&gt;"&amp;K87&amp;"&lt;/td&gt;&lt;td&gt;"&amp;L87&amp;"&lt;/td&gt;&lt;td&gt;"&amp;M87&amp;"&lt;/td&gt;"</f>
-        <v>&lt;tr&gt;&lt;td&gt;by/3.0/&lt;/td&gt;&lt;td&gt;431117__inspectorj__door-front-opening-a.wav&lt;/td&gt;&lt;td&gt;https://freesound.org/s/431117/&lt;/td&gt;&lt;td&gt;inspectorj&lt;/td&gt;</v>
-      </c>
-      <c r="J87" s="28" t="s">
-        <v>2888</v>
-      </c>
-      <c r="K87" s="19" t="s">
-        <v>2925</v>
+        <v>&lt;tr&gt;&lt;td&gt;zero/1.0/&lt;/td&gt;&lt;td&gt;397254__screamstudio__loading.wav&lt;/td&gt;&lt;td&gt;https://freesound.org/s/397254/&lt;/td&gt;&lt;td&gt;ScreamStudio&lt;/td&gt;</v>
+      </c>
+      <c r="J87" s="32" t="s">
+        <v>2880</v>
+      </c>
+      <c r="K87" s="35" t="s">
+        <v>2854</v>
       </c>
       <c r="L87" s="29" t="s">
-        <v>2931</v>
+        <v>2883</v>
       </c>
       <c r="M87" s="28" t="s">
-        <v>2926</v>
+        <v>2884</v>
       </c>
       <c r="R87" t="str">
         <f>"| "&amp;J87&amp;" | "&amp;K87&amp;" | "&amp;L87&amp;" | "&amp;M87&amp;" |"</f>
-        <v>| by/3.0/ | 431117__inspectorj__door-front-opening-a.wav | https://freesound.org/s/431117/ | inspectorj |</v>
+        <v>| zero/1.0/ | 397254__screamstudio__loading.wav | https://freesound.org/s/397254/ | ScreamStudio |</v>
       </c>
     </row>
     <row r="88" spans="1:18" ht="20.25">
       <c r="A88" s="6" t="str">
         <f>"&lt;tr&gt;&lt;td&gt;"&amp;J88&amp;"&lt;/td&gt;&lt;td&gt;"&amp;K88&amp;"&lt;/td&gt;&lt;td&gt;"&amp;L88&amp;"&lt;/td&gt;&lt;td&gt;"&amp;M88&amp;"&lt;/td&gt;"</f>
-        <v>&lt;tr&gt;&lt;td&gt;zero/1.0/&lt;/td&gt;&lt;td&gt;500418__dj-somar__intro-reverso-craver-microbrute.wav&lt;/td&gt;&lt;td&gt;https://freesound.org/s/500418/&lt;/td&gt;&lt;td&gt;DJ_SoMaR&lt;/td&gt;</v>
+        <v>&lt;tr&gt;&lt;td&gt;zero/1.0/&lt;/td&gt;&lt;td&gt;404068__swordofkings128__backyard-gate-open.wav&lt;/td&gt;&lt;td&gt;https://freesound.org/s/404068/&lt;/td&gt;&lt;td&gt;swordofkings128&lt;/td&gt;</v>
       </c>
       <c r="J88" s="35" t="s">
         <v>2880</v>
       </c>
       <c r="K88" s="19" t="s">
-        <v>2914</v>
+        <v>2927</v>
       </c>
       <c r="L88" s="29" t="s">
-        <v>2920</v>
+        <v>2932</v>
       </c>
       <c r="M88" s="28" t="s">
-        <v>2915</v>
+        <v>2928</v>
       </c>
       <c r="R88" t="str">
         <f>"| "&amp;J88&amp;" | "&amp;K88&amp;" | "&amp;L88&amp;" | "&amp;M88&amp;" |"</f>
-        <v>| zero/1.0/ | 500418__dj-somar__intro-reverso-craver-microbrute.wav | https://freesound.org/s/500418/ | DJ_SoMaR |</v>
+        <v>| zero/1.0/ | 404068__swordofkings128__backyard-gate-open.wav | https://freesound.org/s/404068/ | swordofkings128 |</v>
       </c>
     </row>
     <row r="89" spans="1:18" ht="20.25">
       <c r="A89" s="6" t="str">
         <f>"&lt;tr&gt;&lt;td&gt;"&amp;J89&amp;"&lt;/td&gt;&lt;td&gt;"&amp;K89&amp;"&lt;/td&gt;&lt;td&gt;"&amp;L89&amp;"&lt;/td&gt;&lt;td&gt;"&amp;M89&amp;"&lt;/td&gt;"</f>
-        <v>&lt;tr&gt;&lt;td&gt;by/3.0/&lt;/td&gt;&lt;td&gt;7967__cfork__boing-raw.aiff&lt;/td&gt;&lt;td&gt;https://freesound.org/s/7967/&lt;/td&gt;&lt;td&gt;cfork&lt;/td&gt;</v>
+        <v>&lt;tr&gt;&lt;td&gt;zero/1.0/&lt;/td&gt;&lt;td&gt;407052__sojan__power-charge.flac&lt;/td&gt;&lt;td&gt;https://freesound.org/s/193610/&lt;/td&gt;&lt;td&gt;crashoverride61088&lt;/td&gt;</v>
       </c>
       <c r="J89" s="32" t="s">
-        <v>2888</v>
+        <v>2880</v>
       </c>
       <c r="K89" s="35" t="s">
-        <v>2895</v>
+        <v>2856</v>
       </c>
       <c r="L89" s="29" t="s">
-        <v>2896</v>
+        <v>2881</v>
       </c>
       <c r="M89" s="28" t="s">
-        <v>2897</v>
+        <v>2882</v>
       </c>
       <c r="R89" t="str">
         <f>"| "&amp;J89&amp;" | "&amp;K89&amp;" | "&amp;L89&amp;" | "&amp;M89&amp;" |"</f>
-        <v>| by/3.0/ | 7967__cfork__boing-raw.aiff | https://freesound.org/s/7967/ | cfork |</v>
+        <v>| zero/1.0/ | 407052__sojan__power-charge.flac | https://freesound.org/s/193610/ | crashoverride61088 |</v>
       </c>
     </row>
     <row r="90" spans="1:18" ht="20.25">
       <c r="A90" s="6" t="str">
         <f>"&lt;tr&gt;&lt;td&gt;"&amp;J90&amp;"&lt;/td&gt;&lt;td&gt;"&amp;K90&amp;"&lt;/td&gt;&lt;td&gt;"&amp;L90&amp;"&lt;/td&gt;&lt;td&gt;"&amp;M90&amp;"&lt;/td&gt;"</f>
-        <v>&lt;tr&gt;&lt;td&gt;by/3.0/&lt;/td&gt;&lt;td&gt;88635__uair01__bicycle-picture-in-spectrum.wav&lt;/td&gt;&lt;td&gt;https://freesound.org/s/88635/&lt;/td&gt;&lt;td&gt;uair01&lt;/td&gt;</v>
-      </c>
-      <c r="J90" s="30" t="s">
+        <v>&lt;tr&gt;&lt;td&gt;by/3.0/&lt;/td&gt;&lt;td&gt;417131__cuddlenucks__science-fiction-noise-3.wav&lt;/td&gt;&lt;td&gt;https://freesound.org/s/417131/&lt;/td&gt;&lt;td&gt;cuddlenucks&lt;/td&gt;</v>
+      </c>
+      <c r="J90" s="35" t="s">
         <v>2888</v>
       </c>
-      <c r="K90" s="35" t="s">
-        <v>2892</v>
-      </c>
-      <c r="L90" s="29" t="s">
-        <v>2893</v>
+      <c r="K90" s="19" t="s">
+        <v>2860</v>
+      </c>
+      <c r="L90" t="s">
+        <v>2956</v>
       </c>
       <c r="M90" s="28" t="s">
-        <v>2894</v>
+        <v>2945</v>
       </c>
       <c r="R90" t="str">
         <f>"| "&amp;J90&amp;" | "&amp;K90&amp;" | "&amp;L90&amp;" | "&amp;M90&amp;" |"</f>
-        <v>| by/3.0/ | 88635__uair01__bicycle-picture-in-spectrum.wav | https://freesound.org/s/88635/ | uair01 |</v>
+        <v>| by/3.0/ | 417131__cuddlenucks__science-fiction-noise-3.wav | https://freesound.org/s/417131/ | cuddlenucks |</v>
       </c>
     </row>
     <row r="91" spans="1:18" ht="20.25">
       <c r="A91" s="6" t="str">
         <f>"&lt;tr&gt;&lt;td&gt;"&amp;J91&amp;"&lt;/td&gt;&lt;td&gt;"&amp;K91&amp;"&lt;/td&gt;&lt;td&gt;"&amp;L91&amp;"&lt;/td&gt;&lt;td&gt;"&amp;M91&amp;"&lt;/td&gt;"</f>
-        <v>&lt;tr&gt;&lt;td&gt;by-nc/3.0/&lt;/td&gt;&lt;td&gt;91296__timbre__bwaang-2-reverb.mp3&lt;/td&gt;&lt;td&gt;https://freesound.org/s/91296/&lt;/td&gt;&lt;td&gt;timbre&lt;/td&gt;</v>
+        <v>&lt;tr&gt;&lt;td&gt;by/3.0/&lt;/td&gt;&lt;td&gt;417363__xcreenplay__boing-massive-kick.wav&lt;/td&gt;&lt;td&gt;https://freesound.org/s/417363/&lt;/td&gt;&lt;td&gt;xcreenplay&lt;/td&gt;</v>
       </c>
       <c r="J91" s="35" t="s">
-        <v>2900</v>
+        <v>2888</v>
       </c>
       <c r="K91" s="19" t="s">
-        <v>2912</v>
+        <v>2858</v>
       </c>
       <c r="L91" t="s">
-        <v>2961</v>
+        <v>2953</v>
       </c>
       <c r="M91" s="28" t="s">
-        <v>2948</v>
+        <v>2946</v>
       </c>
       <c r="R91" t="str">
         <f>"| "&amp;J91&amp;" | "&amp;K91&amp;" | "&amp;L91&amp;" | "&amp;M91&amp;" |"</f>
-        <v>| by-nc/3.0/ | 91296__timbre__bwaang-2-reverb.mp3 | https://freesound.org/s/91296/ | timbre |</v>
+        <v>| by/3.0/ | 417363__xcreenplay__boing-massive-kick.wav | https://freesound.org/s/417363/ | xcreenplay |</v>
       </c>
     </row>
     <row r="92" spans="1:18" ht="20.25">
       <c r="A92" s="6" t="str">
         <f>"&lt;tr&gt;&lt;td&gt;"&amp;J92&amp;"&lt;/td&gt;&lt;td&gt;"&amp;K92&amp;"&lt;/td&gt;&lt;td&gt;"&amp;L92&amp;"&lt;/td&gt;&lt;td&gt;"&amp;M92&amp;"&lt;/td&gt;"</f>
-        <v>&lt;tr&gt;&lt;td&gt;by/3.0/&lt;/td&gt;&lt;td&gt;96964__gabisaraceni__porta-abrindo-5.wav&lt;/td&gt;&lt;td&gt;https://freesound.org/s/96964/&lt;/td&gt;&lt;td&gt;gabisaraceni&lt;/td&gt;</v>
-      </c>
-      <c r="J92" s="35" t="s">
+        <v>&lt;tr&gt;&lt;td&gt;by/3.0/&lt;/td&gt;&lt;td&gt;431117__inspectorj__door-front-opening-a.wav&lt;/td&gt;&lt;td&gt;https://freesound.org/s/431117/&lt;/td&gt;&lt;td&gt;inspectorj&lt;/td&gt;</v>
+      </c>
+      <c r="J92" s="28" t="s">
         <v>2888</v>
       </c>
       <c r="K92" s="19" t="s">
-        <v>2929</v>
+        <v>2925</v>
       </c>
       <c r="L92" s="29" t="s">
-        <v>2933</v>
+        <v>2931</v>
       </c>
       <c r="M92" s="28" t="s">
-        <v>2930</v>
+        <v>2926</v>
       </c>
       <c r="R92" t="str">
         <f>"| "&amp;J92&amp;" | "&amp;K92&amp;" | "&amp;L92&amp;" | "&amp;M92&amp;" |"</f>
+        <v>| by/3.0/ | 431117__inspectorj__door-front-opening-a.wav | https://freesound.org/s/431117/ | inspectorj |</v>
+      </c>
+    </row>
+    <row r="93" spans="1:18" ht="20.25">
+      <c r="A93" s="6" t="str">
+        <f>"&lt;tr&gt;&lt;td&gt;"&amp;J93&amp;"&lt;/td&gt;&lt;td&gt;"&amp;K93&amp;"&lt;/td&gt;&lt;td&gt;"&amp;L93&amp;"&lt;/td&gt;&lt;td&gt;"&amp;M93&amp;"&lt;/td&gt;"</f>
+        <v>&lt;tr&gt;&lt;td&gt;zero/1.0/&lt;/td&gt;&lt;td&gt;500418__dj-somar__intro-reverso-craver-microbrute.wav&lt;/td&gt;&lt;td&gt;https://freesound.org/s/500418/&lt;/td&gt;&lt;td&gt;DJ_SoMaR&lt;/td&gt;</v>
+      </c>
+      <c r="J93" s="35" t="s">
+        <v>2880</v>
+      </c>
+      <c r="K93" s="19" t="s">
+        <v>2914</v>
+      </c>
+      <c r="L93" s="29" t="s">
+        <v>2920</v>
+      </c>
+      <c r="M93" s="28" t="s">
+        <v>2915</v>
+      </c>
+      <c r="R93" t="str">
+        <f>"| "&amp;J93&amp;" | "&amp;K93&amp;" | "&amp;L93&amp;" | "&amp;M93&amp;" |"</f>
+        <v>| zero/1.0/ | 500418__dj-somar__intro-reverso-craver-microbrute.wav | https://freesound.org/s/500418/ | DJ_SoMaR |</v>
+      </c>
+    </row>
+    <row r="94" spans="1:18" ht="20.25">
+      <c r="A94" s="6" t="str">
+        <f>"&lt;tr&gt;&lt;td&gt;"&amp;J94&amp;"&lt;/td&gt;&lt;td&gt;"&amp;K94&amp;"&lt;/td&gt;&lt;td&gt;"&amp;L94&amp;"&lt;/td&gt;&lt;td&gt;"&amp;M94&amp;"&lt;/td&gt;"</f>
+        <v>&lt;tr&gt;&lt;td&gt;by/3.0/&lt;/td&gt;&lt;td&gt;7967__cfork__boing-raw.aiff&lt;/td&gt;&lt;td&gt;https://freesound.org/s/7967/&lt;/td&gt;&lt;td&gt;cfork&lt;/td&gt;</v>
+      </c>
+      <c r="J94" s="32" t="s">
+        <v>2888</v>
+      </c>
+      <c r="K94" s="35" t="s">
+        <v>2895</v>
+      </c>
+      <c r="L94" s="29" t="s">
+        <v>2896</v>
+      </c>
+      <c r="M94" s="28" t="s">
+        <v>2897</v>
+      </c>
+      <c r="R94" t="str">
+        <f>"| "&amp;J94&amp;" | "&amp;K94&amp;" | "&amp;L94&amp;" | "&amp;M94&amp;" |"</f>
+        <v>| by/3.0/ | 7967__cfork__boing-raw.aiff | https://freesound.org/s/7967/ | cfork |</v>
+      </c>
+    </row>
+    <row r="95" spans="1:18" ht="20.25">
+      <c r="A95" s="6" t="str">
+        <f>"&lt;tr&gt;&lt;td&gt;"&amp;J95&amp;"&lt;/td&gt;&lt;td&gt;"&amp;K95&amp;"&lt;/td&gt;&lt;td&gt;"&amp;L95&amp;"&lt;/td&gt;&lt;td&gt;"&amp;M95&amp;"&lt;/td&gt;"</f>
+        <v>&lt;tr&gt;&lt;td&gt;by/3.0/&lt;/td&gt;&lt;td&gt;88635__uair01__bicycle-picture-in-spectrum.wav&lt;/td&gt;&lt;td&gt;https://freesound.org/s/88635/&lt;/td&gt;&lt;td&gt;uair01&lt;/td&gt;</v>
+      </c>
+      <c r="J95" s="30" t="s">
+        <v>2888</v>
+      </c>
+      <c r="K95" s="35" t="s">
+        <v>2892</v>
+      </c>
+      <c r="L95" s="29" t="s">
+        <v>2893</v>
+      </c>
+      <c r="M95" s="28" t="s">
+        <v>2894</v>
+      </c>
+      <c r="R95" t="str">
+        <f>"| "&amp;J95&amp;" | "&amp;K95&amp;" | "&amp;L95&amp;" | "&amp;M95&amp;" |"</f>
+        <v>| by/3.0/ | 88635__uair01__bicycle-picture-in-spectrum.wav | https://freesound.org/s/88635/ | uair01 |</v>
+      </c>
+    </row>
+    <row r="96" spans="1:18" ht="20.25">
+      <c r="A96" s="6" t="str">
+        <f>"&lt;tr&gt;&lt;td&gt;"&amp;J96&amp;"&lt;/td&gt;&lt;td&gt;"&amp;K96&amp;"&lt;/td&gt;&lt;td&gt;"&amp;L96&amp;"&lt;/td&gt;&lt;td&gt;"&amp;M96&amp;"&lt;/td&gt;"</f>
+        <v>&lt;tr&gt;&lt;td&gt;by-nc/3.0/&lt;/td&gt;&lt;td&gt;91296__timbre__bwaang-2-reverb.mp3&lt;/td&gt;&lt;td&gt;https://freesound.org/s/91296/&lt;/td&gt;&lt;td&gt;timbre&lt;/td&gt;</v>
+      </c>
+      <c r="J96" s="35" t="s">
+        <v>2900</v>
+      </c>
+      <c r="K96" s="19" t="s">
+        <v>2912</v>
+      </c>
+      <c r="L96" t="s">
+        <v>2961</v>
+      </c>
+      <c r="M96" s="28" t="s">
+        <v>2948</v>
+      </c>
+      <c r="R96" t="str">
+        <f>"| "&amp;J96&amp;" | "&amp;K96&amp;" | "&amp;L96&amp;" | "&amp;M96&amp;" |"</f>
+        <v>| by-nc/3.0/ | 91296__timbre__bwaang-2-reverb.mp3 | https://freesound.org/s/91296/ | timbre |</v>
+      </c>
+    </row>
+    <row r="97" spans="1:18" ht="20.25">
+      <c r="A97" s="6" t="str">
+        <f>"&lt;tr&gt;&lt;td&gt;"&amp;J97&amp;"&lt;/td&gt;&lt;td&gt;"&amp;K97&amp;"&lt;/td&gt;&lt;td&gt;"&amp;L97&amp;"&lt;/td&gt;&lt;td&gt;"&amp;M97&amp;"&lt;/td&gt;"</f>
+        <v>&lt;tr&gt;&lt;td&gt;by/3.0/&lt;/td&gt;&lt;td&gt;96964__gabisaraceni__porta-abrindo-5.wav&lt;/td&gt;&lt;td&gt;https://freesound.org/s/96964/&lt;/td&gt;&lt;td&gt;gabisaraceni&lt;/td&gt;</v>
+      </c>
+      <c r="J97" s="35" t="s">
+        <v>2888</v>
+      </c>
+      <c r="K97" s="19" t="s">
+        <v>2929</v>
+      </c>
+      <c r="L97" s="29" t="s">
+        <v>2933</v>
+      </c>
+      <c r="M97" s="28" t="s">
+        <v>2930</v>
+      </c>
+      <c r="R97" t="str">
+        <f>"| "&amp;J97&amp;" | "&amp;K97&amp;" | "&amp;L97&amp;" | "&amp;M97&amp;" |"</f>
         <v>| by/3.0/ | 96964__gabisaraceni__porta-abrindo-5.wav | https://freesound.org/s/96964/ | gabisaraceni |</v>
       </c>
     </row>
-    <row r="93" spans="1:18">
-      <c r="A93" s="6" t="s">
+    <row r="98" spans="1:18">
+      <c r="A98" s="6" t="s">
+        <v>3415</v>
+      </c>
+    </row>
+    <row r="99" spans="1:18">
+      <c r="A99" t="s">
+        <v>3430</v>
+      </c>
+    </row>
+    <row r="100" spans="1:18">
+      <c r="A100" s="6" t="s">
+        <v>3414</v>
+      </c>
+    </row>
+    <row r="101" spans="1:18" ht="15.75" thickBot="1">
+      <c r="A101" t="s">
+        <v>3416</v>
+      </c>
+    </row>
+    <row r="102" spans="1:18" ht="18" thickBot="1">
+      <c r="A102" s="6" t="str">
+        <f>"&lt;tr&gt;&lt;td&gt;&lt;b&gt;"&amp;J102&amp;"&lt;/b&gt;&lt;/td&gt;&lt;td&gt;&lt;b&gt;"&amp;K102&amp;"&lt;/b&gt;&lt;/td&gt;&lt;td&gt;&lt;b&gt;"&amp;L102&amp;"&lt;/b&gt;&lt;/td&gt;"</f>
+        <v>&lt;tr&gt;&lt;td&gt;&lt;b&gt;Tag&lt;/b&gt;&lt;/td&gt;&lt;td&gt;&lt;b&gt;Name&lt;/b&gt;&lt;/td&gt;&lt;td&gt;&lt;b&gt;URL&lt;/b&gt;&lt;/td&gt;</v>
+      </c>
+      <c r="J102" s="58" t="s">
+        <v>2876</v>
+      </c>
+      <c r="K102" s="58" t="s">
+        <v>3417</v>
+      </c>
+      <c r="L102" s="58" t="s">
+        <v>2878</v>
+      </c>
+    </row>
+    <row r="103" spans="1:18" ht="45.75" thickBot="1">
+      <c r="A103" s="6" t="str">
+        <f>"&lt;tr&gt;&lt;td&gt;"&amp;J103&amp;"&lt;/td&gt;&lt;td&gt;"&amp;K103&amp;"&lt;/td&gt;&lt;td&gt;"&amp;L103&amp;"&lt;/td&gt;"</f>
+        <v>&lt;tr&gt;&lt;td&gt;zero/1.0/&lt;/td&gt;&lt;td&gt;Creative Commons 0 License&lt;/td&gt;&lt;td&gt;https://creativecommons.org/publicdomain/zero/1.0/&lt;/td&gt;</v>
+      </c>
+      <c r="J103" s="59" t="s">
+        <v>2880</v>
+      </c>
+      <c r="K103" s="59" t="s">
+        <v>3418</v>
+      </c>
+      <c r="L103" s="60" t="s">
         <v>3419</v>
       </c>
     </row>
-    <row r="94" spans="1:18">
-      <c r="A94" t="s">
-        <v>3434</v>
-      </c>
-    </row>
-    <row r="95" spans="1:18">
-      <c r="A95" s="6" t="s">
-        <v>3418</v>
-      </c>
-    </row>
-    <row r="96" spans="1:18" ht="15.75" thickBot="1">
-      <c r="A96" t="s">
+    <row r="104" spans="1:18" ht="30.75" thickBot="1">
+      <c r="A104" s="6" t="str">
+        <f>"&lt;tr&gt;&lt;td&gt;"&amp;J104&amp;"&lt;/td&gt;&lt;td&gt;"&amp;K104&amp;"&lt;/td&gt;&lt;td&gt;"&amp;L104&amp;"&lt;/td&gt;"</f>
+        <v>&lt;tr&gt;&lt;td&gt;by/3.0/&lt;/td&gt;&lt;td&gt;Creative Commons Attribution License&lt;/td&gt;&lt;td&gt;https://creativecommons.org/licenses/by/3.0/&lt;/td&gt;</v>
+      </c>
+      <c r="J104" s="61" t="s">
+        <v>2888</v>
+      </c>
+      <c r="K104" s="61" t="s">
         <v>3420</v>
       </c>
-    </row>
-    <row r="97" spans="1:12" ht="18" thickBot="1">
-      <c r="A97" s="6" t="str">
-        <f>"&lt;tr&gt;&lt;td&gt;&lt;b&gt;"&amp;J97&amp;"&lt;/b&gt;&lt;/td&gt;&lt;td&gt;&lt;b&gt;"&amp;K97&amp;"&lt;/b&gt;&lt;/td&gt;&lt;td&gt;&lt;b&gt;"&amp;L97&amp;"&lt;/b&gt;&lt;/td&gt;"</f>
-        <v>&lt;tr&gt;&lt;td&gt;&lt;b&gt;Tag&lt;/b&gt;&lt;/td&gt;&lt;td&gt;&lt;b&gt;Name&lt;/b&gt;&lt;/td&gt;&lt;td&gt;&lt;b&gt;URL&lt;/b&gt;&lt;/td&gt;</v>
-      </c>
-      <c r="J97" s="58" t="s">
-        <v>2876</v>
-      </c>
-      <c r="K97" s="58" t="s">
+      <c r="L104" s="62" t="s">
         <v>3421</v>
       </c>
-      <c r="L97" s="58" t="s">
-        <v>2878</v>
-      </c>
-    </row>
-    <row r="98" spans="1:12" ht="45.75" thickBot="1">
-      <c r="A98" s="6" t="str">
-        <f>"&lt;tr&gt;&lt;td&gt;"&amp;J98&amp;"&lt;/td&gt;&lt;td&gt;"&amp;K98&amp;"&lt;/td&gt;&lt;td&gt;"&amp;L98&amp;"&lt;/td&gt;"</f>
-        <v>&lt;tr&gt;&lt;td&gt;zero/1.0/&lt;/td&gt;&lt;td&gt;Creative Commons 0 License&lt;/td&gt;&lt;td&gt;https://creativecommons.org/publicdomain/zero/1.0/&lt;/td&gt;</v>
-      </c>
-      <c r="J98" s="59" t="s">
-        <v>2880</v>
-      </c>
-      <c r="K98" s="59" t="s">
+    </row>
+    <row r="105" spans="1:18" ht="30.75" thickBot="1">
+      <c r="A105" s="6" t="str">
+        <f>"&lt;tr&gt;&lt;td&gt;"&amp;J105&amp;"&lt;/td&gt;&lt;td&gt;"&amp;K105&amp;"&lt;/td&gt;&lt;td&gt;"&amp;L105&amp;"&lt;/td&gt;"</f>
+        <v>&lt;tr&gt;&lt;td&gt;by-nc/3.0/&lt;/td&gt;&lt;td&gt;Creative Commons Attribution Noncommercial License&lt;/td&gt;&lt;td&gt;https://creativecommons.org/licenses/by-nc/3.0/&lt;/td&gt;</v>
+      </c>
+      <c r="J105" s="59" t="s">
+        <v>2900</v>
+      </c>
+      <c r="K105" s="59" t="s">
         <v>3422</v>
       </c>
-      <c r="L98" s="60" t="s">
+      <c r="L105" s="60" t="s">
         <v>3423</v>
       </c>
     </row>
-    <row r="99" spans="1:12" ht="30.75" thickBot="1">
-      <c r="A99" s="6" t="str">
-        <f>"&lt;tr&gt;&lt;td&gt;"&amp;J99&amp;"&lt;/td&gt;&lt;td&gt;"&amp;K99&amp;"&lt;/td&gt;&lt;td&gt;"&amp;L99&amp;"&lt;/td&gt;"</f>
-        <v>&lt;tr&gt;&lt;td&gt;by/3.0/&lt;/td&gt;&lt;td&gt;Creative Commons Attribution License&lt;/td&gt;&lt;td&gt;https://creativecommons.org/licenses/by/3.0/&lt;/td&gt;</v>
-      </c>
-      <c r="J99" s="61" t="s">
-        <v>2888</v>
-      </c>
-      <c r="K99" s="61" t="s">
-        <v>3424</v>
-      </c>
-      <c r="L99" s="62" t="s">
-        <v>3425</v>
-      </c>
-    </row>
-    <row r="100" spans="1:12" ht="30.75" thickBot="1">
-      <c r="A100" s="6" t="str">
-        <f>"&lt;tr&gt;&lt;td&gt;"&amp;J100&amp;"&lt;/td&gt;&lt;td&gt;"&amp;K100&amp;"&lt;/td&gt;&lt;td&gt;"&amp;L100&amp;"&lt;/td&gt;"</f>
-        <v>&lt;tr&gt;&lt;td&gt;by-nc/3.0/&lt;/td&gt;&lt;td&gt;Creative Commons Attribution Noncommercial License&lt;/td&gt;&lt;td&gt;https://creativecommons.org/licenses/by-nc/3.0/&lt;/td&gt;</v>
-      </c>
-      <c r="J100" s="59" t="s">
-        <v>2900</v>
-      </c>
-      <c r="K100" s="59" t="s">
-        <v>3426</v>
-      </c>
-      <c r="L100" s="60" t="s">
-        <v>3427</v>
-      </c>
-    </row>
-    <row r="101" spans="1:12">
-      <c r="A101" s="6" t="s">
-        <v>3419</v>
+    <row r="106" spans="1:18">
+      <c r="A106" s="6" t="s">
+        <v>3415</v>
       </c>
     </row>
   </sheetData>
-  <sortState ref="A68:D75">
-    <sortCondition descending="1" ref="A68:A75"/>
-    <sortCondition ref="B68:B75"/>
+  <autoFilter ref="A1:H44" xr:uid="{D49867B0-9605-4DAD-A171-997D81FF01DA}"/>
+  <sortState ref="A73:D80">
+    <sortCondition descending="1" ref="A73:A80"/>
+    <sortCondition ref="B73:B80"/>
   </sortState>
   <hyperlinks>
-    <hyperlink ref="L84" r:id="rId1" xr:uid="{0389BFEF-2278-1C4C-AFFD-40911D54BA38}"/>
-    <hyperlink ref="L82" r:id="rId2" xr:uid="{6DC6DCC3-96F7-244A-A515-6ACC236B66A6}"/>
-    <hyperlink ref="L67" r:id="rId3" xr:uid="{CCE745AF-D2B8-1E45-81C2-27CEF6C5B2AF}"/>
-    <hyperlink ref="L73" r:id="rId4" xr:uid="{FC7F966A-1EC2-DE4A-875D-CA9E5FD25210}"/>
-    <hyperlink ref="L90" r:id="rId5" xr:uid="{0DB3DAF8-4FD8-5441-A5EE-FDB2E3108255}"/>
-    <hyperlink ref="L89" r:id="rId6" xr:uid="{6722E195-E4EF-1D49-A046-EFE49EC89CB6}"/>
-    <hyperlink ref="L80" r:id="rId7" xr:uid="{35EA502B-43EE-5648-92D3-03388141605B}"/>
-    <hyperlink ref="L72" r:id="rId8" xr:uid="{F628B53D-420C-0844-AF06-3CBF155582C6}"/>
-    <hyperlink ref="L79" r:id="rId9" xr:uid="{FA1B324F-1513-1343-9CCE-E23AFD154FFD}"/>
-    <hyperlink ref="L88" r:id="rId10" xr:uid="{C5AA4A87-0C8F-9A4C-974F-82A19E89F99C}"/>
-    <hyperlink ref="L76" r:id="rId11" xr:uid="{E1112DD8-8BE8-BD47-9002-F00DDA38363C}"/>
-    <hyperlink ref="L87" r:id="rId12" xr:uid="{4D774EC1-CC16-C24F-88F2-E9E20B8A8FC0}"/>
-    <hyperlink ref="L79:L80" r:id="rId13" display="https://freesound.org/s//" xr:uid="{5FB99E8B-AEFC-6A45-851E-E3C683DC5AC1}"/>
-    <hyperlink ref="L83" r:id="rId14" xr:uid="{E2EACC90-D2ED-AF4A-9302-ADD31B56C321}"/>
-    <hyperlink ref="L92" r:id="rId15" xr:uid="{13F37B0F-8A53-0B4F-8FE7-132D2186D638}"/>
-    <hyperlink ref="L75" r:id="rId16" xr:uid="{FA55BAC7-078A-8944-9FB5-42D7B041E218}"/>
-    <hyperlink ref="H25" r:id="rId17" xr:uid="{4419FB35-315D-4DE4-9E5C-9B20E33A87FF}"/>
-    <hyperlink ref="H20" r:id="rId18" xr:uid="{0ABC5FB6-8ADD-42B9-BF56-61A08BCA415C}"/>
-    <hyperlink ref="H23" r:id="rId19" xr:uid="{189EA614-1A03-48EB-A1CB-FFAA9A4096B3}"/>
-    <hyperlink ref="H15" r:id="rId20" xr:uid="{E08EAADE-B534-4F10-8046-41A89DE60AED}"/>
-    <hyperlink ref="H22" r:id="rId21" xr:uid="{1C69CE9F-8A0A-46D7-8D36-88F69F179169}"/>
+    <hyperlink ref="L89" r:id="rId1" xr:uid="{0389BFEF-2278-1C4C-AFFD-40911D54BA38}"/>
+    <hyperlink ref="L87" r:id="rId2" xr:uid="{6DC6DCC3-96F7-244A-A515-6ACC236B66A6}"/>
+    <hyperlink ref="L72" r:id="rId3" xr:uid="{CCE745AF-D2B8-1E45-81C2-27CEF6C5B2AF}"/>
+    <hyperlink ref="L78" r:id="rId4" xr:uid="{FC7F966A-1EC2-DE4A-875D-CA9E5FD25210}"/>
+    <hyperlink ref="L95" r:id="rId5" xr:uid="{0DB3DAF8-4FD8-5441-A5EE-FDB2E3108255}"/>
+    <hyperlink ref="L94" r:id="rId6" xr:uid="{6722E195-E4EF-1D49-A046-EFE49EC89CB6}"/>
+    <hyperlink ref="L85" r:id="rId7" xr:uid="{35EA502B-43EE-5648-92D3-03388141605B}"/>
+    <hyperlink ref="L77" r:id="rId8" xr:uid="{F628B53D-420C-0844-AF06-3CBF155582C6}"/>
+    <hyperlink ref="L84" r:id="rId9" xr:uid="{FA1B324F-1513-1343-9CCE-E23AFD154FFD}"/>
+    <hyperlink ref="L93" r:id="rId10" xr:uid="{C5AA4A87-0C8F-9A4C-974F-82A19E89F99C}"/>
+    <hyperlink ref="L81" r:id="rId11" xr:uid="{E1112DD8-8BE8-BD47-9002-F00DDA38363C}"/>
+    <hyperlink ref="L92" r:id="rId12" xr:uid="{4D774EC1-CC16-C24F-88F2-E9E20B8A8FC0}"/>
+    <hyperlink ref="L84:L85" r:id="rId13" display="https://freesound.org/s//" xr:uid="{5FB99E8B-AEFC-6A45-851E-E3C683DC5AC1}"/>
+    <hyperlink ref="L88" r:id="rId14" xr:uid="{E2EACC90-D2ED-AF4A-9302-ADD31B56C321}"/>
+    <hyperlink ref="L97" r:id="rId15" xr:uid="{13F37B0F-8A53-0B4F-8FE7-132D2186D638}"/>
+    <hyperlink ref="L80" r:id="rId16" xr:uid="{FA55BAC7-078A-8944-9FB5-42D7B041E218}"/>
+    <hyperlink ref="H27" r:id="rId17" xr:uid="{4419FB35-315D-4DE4-9E5C-9B20E33A87FF}"/>
+    <hyperlink ref="H22" r:id="rId18" xr:uid="{0ABC5FB6-8ADD-42B9-BF56-61A08BCA415C}"/>
+    <hyperlink ref="H25" r:id="rId19" xr:uid="{189EA614-1A03-48EB-A1CB-FFAA9A4096B3}"/>
+    <hyperlink ref="H17" r:id="rId20" xr:uid="{E08EAADE-B534-4F10-8046-41A89DE60AED}"/>
+    <hyperlink ref="H24" r:id="rId21" xr:uid="{1C69CE9F-8A0A-46D7-8D36-88F69F179169}"/>
     <hyperlink ref="H11" r:id="rId22" xr:uid="{98ABC161-AB9D-4F60-87BE-749E4E4F50E4}"/>
     <hyperlink ref="H9" r:id="rId23" xr:uid="{DBFADD8C-4C9E-493D-9424-41720C23C9D3}"/>
-    <hyperlink ref="H35" r:id="rId24" xr:uid="{C1B31281-1033-4BC4-9D4B-CC2023FF56DB}"/>
-    <hyperlink ref="H28" r:id="rId25" xr:uid="{233967F1-D44D-4DD7-8621-DB03C700D78B}"/>
-    <hyperlink ref="H29" r:id="rId26" xr:uid="{668B5A5D-33C3-48F3-B29D-78E17C45647B}"/>
-    <hyperlink ref="H34" r:id="rId27" xr:uid="{358F58C7-5E85-4805-BCE6-BEBC9EFC5590}"/>
-    <hyperlink ref="H30" r:id="rId28" xr:uid="{9857E7A2-3B5E-4C6F-BE6B-75B1942BF2F1}"/>
-    <hyperlink ref="H32" r:id="rId29" xr:uid="{7817D13B-66BE-451C-A663-245A7D32FB4E}"/>
+    <hyperlink ref="H38" r:id="rId24" xr:uid="{C1B31281-1033-4BC4-9D4B-CC2023FF56DB}"/>
+    <hyperlink ref="H31" r:id="rId25" xr:uid="{233967F1-D44D-4DD7-8621-DB03C700D78B}"/>
+    <hyperlink ref="H32" r:id="rId26" xr:uid="{668B5A5D-33C3-48F3-B29D-78E17C45647B}"/>
+    <hyperlink ref="H37" r:id="rId27" xr:uid="{358F58C7-5E85-4805-BCE6-BEBC9EFC5590}"/>
+    <hyperlink ref="H33" r:id="rId28" xr:uid="{9857E7A2-3B5E-4C6F-BE6B-75B1942BF2F1}"/>
+    <hyperlink ref="H35" r:id="rId29" xr:uid="{7817D13B-66BE-451C-A663-245A7D32FB4E}"/>
     <hyperlink ref="H12" r:id="rId30" xr:uid="{7C24BB00-1AF3-4126-B137-A49F7832B368}"/>
-    <hyperlink ref="H31" r:id="rId31" xr:uid="{093D12FF-CE66-488E-919F-B618F1024F05}"/>
-    <hyperlink ref="H33" r:id="rId32" xr:uid="{99E100BC-474F-4957-8AB6-A17E6091CEA4}"/>
+    <hyperlink ref="H34" r:id="rId31" xr:uid="{093D12FF-CE66-488E-919F-B618F1024F05}"/>
+    <hyperlink ref="H36" r:id="rId32" xr:uid="{99E100BC-474F-4957-8AB6-A17E6091CEA4}"/>
     <hyperlink ref="H2" r:id="rId33" xr:uid="{25C6586F-F991-4DAC-AEAE-61EB9CF85AF5}"/>
     <hyperlink ref="H3" r:id="rId34" xr:uid="{3FD4754B-D29F-42BF-9347-AEB60E71BDB1}"/>
     <hyperlink ref="H5" r:id="rId35" xr:uid="{6D41BF09-100E-4896-BD25-6704EAC36A60}"/>
     <hyperlink ref="H4" r:id="rId36" xr:uid="{2DD3B0DC-A175-4C8A-841B-658057AE051F}"/>
-    <hyperlink ref="H16" r:id="rId37" xr:uid="{33C6D4A0-BD27-430A-9E84-AE82A539480A}"/>
-    <hyperlink ref="H18" r:id="rId38" xr:uid="{8E6DDEF9-D8C3-4DA8-A4AD-2596F9F0C140}"/>
-    <hyperlink ref="H19" r:id="rId39" xr:uid="{58DE9C77-4D8A-49B7-B8ED-B830856345DB}"/>
+    <hyperlink ref="H18" r:id="rId37" xr:uid="{33C6D4A0-BD27-430A-9E84-AE82A539480A}"/>
+    <hyperlink ref="H20" r:id="rId38" xr:uid="{8E6DDEF9-D8C3-4DA8-A4AD-2596F9F0C140}"/>
+    <hyperlink ref="H21" r:id="rId39" xr:uid="{58DE9C77-4D8A-49B7-B8ED-B830856345DB}"/>
     <hyperlink ref="H10" r:id="rId40" xr:uid="{F25DAD37-A019-474B-A9A2-BCA497746C14}"/>
-    <hyperlink ref="H17" r:id="rId41" xr:uid="{63C79250-783C-452C-9453-FFE824D74709}"/>
-    <hyperlink ref="H26" r:id="rId42" xr:uid="{9A5F93C5-437C-488C-B3D7-22BAEE17A695}"/>
-    <hyperlink ref="H24" r:id="rId43" xr:uid="{5BFD487A-D636-4DDD-B229-99F5CBDC0BE1}"/>
-    <hyperlink ref="H21" r:id="rId44" xr:uid="{46A4F8EE-A89B-4A07-8D5D-E50FDDE0611E}"/>
-    <hyperlink ref="H49" r:id="rId45" xr:uid="{5B231739-C8F4-4D4E-B946-7A383ECBBB35}"/>
-    <hyperlink ref="H50" r:id="rId46" xr:uid="{6D8EAE93-D71D-4499-8388-86B77E8848FB}"/>
+    <hyperlink ref="H19" r:id="rId41" xr:uid="{63C79250-783C-452C-9453-FFE824D74709}"/>
+    <hyperlink ref="H28" r:id="rId42" xr:uid="{9A5F93C5-437C-488C-B3D7-22BAEE17A695}"/>
+    <hyperlink ref="H26" r:id="rId43" xr:uid="{5BFD487A-D636-4DDD-B229-99F5CBDC0BE1}"/>
+    <hyperlink ref="H23" r:id="rId44" xr:uid="{46A4F8EE-A89B-4A07-8D5D-E50FDDE0611E}"/>
+    <hyperlink ref="H54" r:id="rId45" xr:uid="{5B231739-C8F4-4D4E-B946-7A383ECBBB35}"/>
+    <hyperlink ref="H55" r:id="rId46" xr:uid="{6D8EAE93-D71D-4499-8388-86B77E8848FB}"/>
     <hyperlink ref="H8" r:id="rId47" xr:uid="{2AE693E7-7449-4538-80A8-30A52F2A22F5}"/>
     <hyperlink ref="H7" r:id="rId48" xr:uid="{2FE1FB4D-693E-4830-8337-658393F68B92}"/>
     <hyperlink ref="H13" r:id="rId49" xr:uid="{DE9970E0-9BDB-45D1-93FA-3F6E016EDFDA}"/>
-    <hyperlink ref="L98" r:id="rId50" xr:uid="{643921F6-79ED-48CE-BC1D-7689B067914F}"/>
-    <hyperlink ref="L99" r:id="rId51" xr:uid="{5EB50EDD-6F80-49BD-9E94-C3F33E3E21E7}"/>
-    <hyperlink ref="L100" r:id="rId52" xr:uid="{3C3C642F-1CE9-4D06-A8F2-3D9A9371558D}"/>
-    <hyperlink ref="L66" r:id="rId53" xr:uid="{EAAF1456-48F9-4E52-8F61-7A6218C1AD87}"/>
+    <hyperlink ref="L103" r:id="rId50" xr:uid="{643921F6-79ED-48CE-BC1D-7689B067914F}"/>
+    <hyperlink ref="L104" r:id="rId51" xr:uid="{5EB50EDD-6F80-49BD-9E94-C3F33E3E21E7}"/>
+    <hyperlink ref="L105" r:id="rId52" xr:uid="{3C3C642F-1CE9-4D06-A8F2-3D9A9371558D}"/>
+    <hyperlink ref="L71" r:id="rId53" xr:uid="{EAAF1456-48F9-4E52-8F61-7A6218C1AD87}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId54"/>

</xml_diff>

<commit_message>
get rid of mEFCT_CONFIGURE as an EEPROM-configurable item; use mEFCT_UNIQ
</commit_message>
<xml_diff>
--- a/RBG_arduino/StateTable_minimal.xlsx
+++ b/RBG_arduino/StateTable_minimal.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub-Mark-MDO47\RubberBandGun\RBG_arduino\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97F90589-31E4-4BD5-8F70-32856E650EB7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8AB1741-964A-48DE-B7DE-4D1A8C840849}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21840" xr2:uid="{CCADFEE4-B0E1-4363-9617-1683960BED03}"/>
   </bookViews>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4886" uniqueCount="3506">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4886" uniqueCount="3507">
   <si>
     <t>trigOnly</t>
   </si>
@@ -10601,9 +10601,6 @@
     <t>mCFG_OTHER</t>
   </si>
   <si>
-    <t>mEFCT_CONFIGURE</t>
-  </si>
-  <si>
     <t>Sorry, not yet implemented</t>
   </si>
   <si>
@@ -10794,6 +10791,12 @@
   </si>
   <si>
     <t>#define mCFG_SOUND_CHOICE 33</t>
+  </si>
+  <si>
+    <t>mEFCT_UNIQ_INTRO</t>
+  </si>
+  <si>
+    <t>mEFCT_UNIQ_SND_INSTR</t>
   </si>
 </sst>
 </file>
@@ -11647,8 +11650,8 @@
   <dimension ref="A1:AB68"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A33" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B59" sqref="B59"/>
+      <pane ySplit="1" topLeftCell="A35" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D62" sqref="D62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
@@ -11770,7 +11773,7 @@
         <v>26</v>
       </c>
       <c r="X2" s="2" t="s">
-        <v>3499</v>
+        <v>3498</v>
       </c>
       <c r="AB2" s="25"/>
     </row>
@@ -11804,7 +11807,7 @@
         <v>27</v>
       </c>
       <c r="X3" s="2" t="s">
-        <v>3500</v>
+        <v>3499</v>
       </c>
     </row>
     <row r="4" spans="1:28">
@@ -11813,13 +11816,13 @@
         <v/>
       </c>
       <c r="V4" t="s">
-        <v>3450</v>
+        <v>3449</v>
       </c>
       <c r="W4">
         <v>33</v>
       </c>
       <c r="X4" s="2" t="s">
-        <v>3505</v>
+        <v>3504</v>
       </c>
     </row>
     <row r="5" spans="1:28" ht="45">
@@ -11850,13 +11853,13 @@
         <v>#define mROW_PWRON_OPEN 2</v>
       </c>
       <c r="V5" t="s">
-        <v>3444</v>
+        <v>3443</v>
       </c>
       <c r="W5">
         <v>30</v>
       </c>
       <c r="X5" s="2" t="s">
-        <v>3503</v>
+        <v>3502</v>
       </c>
     </row>
     <row r="6" spans="1:28">
@@ -11887,13 +11890,13 @@
         <v>#define mROW_PWRON_OPEN 2</v>
       </c>
       <c r="V6" t="s">
-        <v>3446</v>
+        <v>3445</v>
       </c>
       <c r="W6">
         <v>29</v>
       </c>
       <c r="X6" s="2" t="s">
-        <v>3502</v>
+        <v>3501</v>
       </c>
       <c r="AB6" s="25"/>
     </row>
@@ -11903,13 +11906,13 @@
         <v/>
       </c>
       <c r="V7" t="s">
-        <v>3449</v>
+        <v>3448</v>
       </c>
       <c r="W7">
         <v>32</v>
       </c>
       <c r="X7" s="2" t="s">
-        <v>3504</v>
+        <v>3503</v>
       </c>
     </row>
     <row r="8" spans="1:28">
@@ -11918,13 +11921,13 @@
         <v/>
       </c>
       <c r="V8" t="s">
-        <v>3445</v>
+        <v>3444</v>
       </c>
       <c r="W8">
         <v>28</v>
       </c>
       <c r="X8" s="2" t="s">
-        <v>3501</v>
+        <v>3500</v>
       </c>
     </row>
     <row r="9" spans="1:28">
@@ -11939,7 +11942,7 @@
         <v>19</v>
       </c>
       <c r="X9" s="2" t="s">
-        <v>3497</v>
+        <v>3496</v>
       </c>
     </row>
     <row r="10" spans="1:28" s="25" customFormat="1">
@@ -11972,7 +11975,7 @@
         <v>7</v>
       </c>
       <c r="X10" s="2" t="s">
-        <v>3489</v>
+        <v>3488</v>
       </c>
       <c r="AB10"/>
     </row>
@@ -12019,7 +12022,7 @@
         <v>11</v>
       </c>
       <c r="X11" s="2" t="s">
-        <v>3491</v>
+        <v>3490</v>
       </c>
       <c r="AB11"/>
     </row>
@@ -12069,7 +12072,7 @@
         <v>9</v>
       </c>
       <c r="X12" s="2" t="s">
-        <v>3490</v>
+        <v>3489</v>
       </c>
     </row>
     <row r="13" spans="1:28" s="25" customFormat="1">
@@ -12115,7 +12118,7 @@
         <v>22</v>
       </c>
       <c r="X13" s="2" t="s">
-        <v>3498</v>
+        <v>3497</v>
       </c>
       <c r="AB13"/>
     </row>
@@ -12136,7 +12139,7 @@
         <v>17</v>
       </c>
       <c r="X14" s="2" t="s">
-        <v>3496</v>
+        <v>3495</v>
       </c>
     </row>
     <row r="15" spans="1:28" s="25" customFormat="1">
@@ -12198,7 +12201,7 @@
         <v>4</v>
       </c>
       <c r="X16" s="2" t="s">
-        <v>3488</v>
+        <v>3487</v>
       </c>
     </row>
     <row r="17" spans="1:26" s="25" customFormat="1">
@@ -12272,7 +12275,7 @@
         <v>14</v>
       </c>
       <c r="X18" s="2" t="s">
-        <v>3493</v>
+        <v>3492</v>
       </c>
       <c r="Y18"/>
       <c r="Z18"/>
@@ -12288,7 +12291,7 @@
       <c r="D19" s="47" t="s">
         <v>3420</v>
       </c>
-      <c r="E19" s="47" t="s">
+      <c r="E19" s="81" t="s">
         <v>3420</v>
       </c>
       <c r="F19" s="37" t="s">
@@ -12311,7 +12314,7 @@
         <v>15</v>
       </c>
       <c r="X19" s="2" t="s">
-        <v>3494</v>
+        <v>3493</v>
       </c>
     </row>
     <row r="20" spans="1:26">
@@ -12325,7 +12328,7 @@
       <c r="D20" s="47" t="s">
         <v>3420</v>
       </c>
-      <c r="E20" s="47" t="s">
+      <c r="E20" s="81" t="s">
         <v>3420</v>
       </c>
       <c r="F20" s="37" t="s">
@@ -12348,7 +12351,7 @@
         <v>16</v>
       </c>
       <c r="X20" s="2" t="s">
-        <v>3495</v>
+        <v>3494</v>
       </c>
     </row>
     <row r="21" spans="1:26">
@@ -12358,7 +12361,7 @@
         <v>60</v>
       </c>
       <c r="D21" s="37"/>
-      <c r="E21" s="37"/>
+      <c r="E21" s="76"/>
       <c r="F21" s="37"/>
       <c r="G21" s="37"/>
       <c r="H21" s="37"/>
@@ -12375,7 +12378,7 @@
         <v>13</v>
       </c>
       <c r="X21" s="2" t="s">
-        <v>3492</v>
+        <v>3491</v>
       </c>
     </row>
     <row r="22" spans="1:26">
@@ -12389,7 +12392,7 @@
       <c r="D22" s="47" t="s">
         <v>3420</v>
       </c>
-      <c r="E22" s="47" t="s">
+      <c r="E22" s="81" t="s">
         <v>3420</v>
       </c>
       <c r="F22" s="37" t="s">
@@ -12419,7 +12422,7 @@
       <c r="D23" s="47" t="s">
         <v>3420</v>
       </c>
-      <c r="E23" s="47" t="s">
+      <c r="E23" s="81" t="s">
         <v>3420</v>
       </c>
       <c r="F23" s="37" t="s">
@@ -12597,7 +12600,7 @@
     </row>
     <row r="33" spans="1:24" ht="45">
       <c r="A33" s="63" t="s">
-        <v>3487</v>
+        <v>3486</v>
       </c>
       <c r="B33" s="10" t="s">
         <v>2731</v>
@@ -12805,7 +12808,7 @@
     </row>
     <row r="45" spans="1:24" ht="120">
       <c r="A45" s="63" t="s">
-        <v>3456</v>
+        <v>3455</v>
       </c>
       <c r="B45" s="9" t="s">
         <v>2729</v>
@@ -12814,10 +12817,10 @@
         <v>3434</v>
       </c>
       <c r="D45" s="3" t="s">
-        <v>3480</v>
+        <v>3505</v>
       </c>
       <c r="E45" s="81" t="s">
-        <v>3441</v>
+        <v>3420</v>
       </c>
       <c r="F45" s="9" t="s">
         <v>0</v>
@@ -12839,16 +12842,16 @@
         <v>3434</v>
       </c>
       <c r="D46" s="3" t="s">
-        <v>3480</v>
+        <v>3505</v>
       </c>
       <c r="E46" s="81" t="s">
-        <v>3441</v>
+        <v>3420</v>
       </c>
       <c r="F46" t="s">
         <v>3436</v>
       </c>
       <c r="I46" s="75" t="s">
-        <v>3445</v>
+        <v>3444</v>
       </c>
       <c r="K46" s="9" t="str">
         <f>IF(LEN(C46),VLOOKUP(C46,mROW,3,FALSE),"")</f>
@@ -12865,10 +12868,10 @@
         <v>3434</v>
       </c>
       <c r="D47" s="3" t="s">
-        <v>3480</v>
+        <v>3505</v>
       </c>
       <c r="E47" s="81" t="s">
-        <v>3441</v>
+        <v>3420</v>
       </c>
       <c r="F47" t="s">
         <v>3437</v>
@@ -12890,10 +12893,10 @@
         <v>3434</v>
       </c>
       <c r="D48" s="3" t="s">
-        <v>3480</v>
+        <v>3505</v>
       </c>
       <c r="E48" s="81" t="s">
-        <v>3441</v>
+        <v>3420</v>
       </c>
       <c r="F48" t="s">
         <v>3439</v>
@@ -12927,7 +12930,7 @@
     </row>
     <row r="51" spans="1:22" ht="30">
       <c r="A51" s="63" t="s">
-        <v>3442</v>
+        <v>3441</v>
       </c>
       <c r="B51" s="9" t="s">
         <v>2729</v>
@@ -12936,10 +12939,10 @@
         <v>3438</v>
       </c>
       <c r="D51" s="3" t="s">
-        <v>3482</v>
+        <v>3481</v>
       </c>
       <c r="E51" s="81" t="s">
-        <v>3441</v>
+        <v>3420</v>
       </c>
       <c r="J51" s="9" t="s">
         <v>3434</v>
@@ -12959,7 +12962,7 @@
     </row>
     <row r="53" spans="1:22" ht="30">
       <c r="A53" s="63" t="s">
-        <v>3442</v>
+        <v>3441</v>
       </c>
       <c r="B53" s="9" t="s">
         <v>2729</v>
@@ -12968,10 +12971,10 @@
         <v>3440</v>
       </c>
       <c r="D53" s="3" t="s">
-        <v>3482</v>
+        <v>3481</v>
       </c>
       <c r="E53" s="81" t="s">
-        <v>3441</v>
+        <v>3420</v>
       </c>
       <c r="J53" s="9" t="s">
         <v>3434</v>
@@ -12991,26 +12994,26 @@
     </row>
     <row r="55" spans="1:22" ht="45">
       <c r="A55" s="63" t="s">
-        <v>3447</v>
+        <v>3446</v>
       </c>
       <c r="B55" s="10" t="s">
-        <v>3451</v>
+        <v>3450</v>
       </c>
       <c r="C55" s="9" t="s">
-        <v>3445</v>
+        <v>3444</v>
       </c>
       <c r="D55" s="9"/>
       <c r="E55" s="76"/>
       <c r="F55" s="9"/>
       <c r="G55" s="10" t="s">
-        <v>3465</v>
+        <v>3464</v>
       </c>
       <c r="H55" s="9" t="s">
-        <v>3443</v>
+        <v>3442</v>
       </c>
       <c r="I55" s="9"/>
       <c r="J55" s="9" t="s">
-        <v>3446</v>
+        <v>3445</v>
       </c>
       <c r="K55" s="9" t="str">
         <f>IF(LEN(C55),VLOOKUP(C55,mROW,3,FALSE),"")</f>
@@ -13028,19 +13031,19 @@
     </row>
     <row r="57" spans="1:22" ht="75">
       <c r="A57" s="63" t="s">
-        <v>3457</v>
+        <v>3456</v>
       </c>
       <c r="B57" s="9" t="s">
         <v>2729</v>
       </c>
       <c r="C57" s="9" t="s">
-        <v>3446</v>
+        <v>3445</v>
       </c>
       <c r="D57" s="3" t="s">
-        <v>3483</v>
+        <v>3506</v>
       </c>
       <c r="E57" s="81" t="s">
-        <v>3441</v>
+        <v>3420</v>
       </c>
       <c r="F57" s="9" t="s">
         <v>0</v>
@@ -13048,7 +13051,7 @@
       <c r="G57" s="9"/>
       <c r="H57" s="9"/>
       <c r="I57" s="9" t="s">
-        <v>3444</v>
+        <v>3443</v>
       </c>
       <c r="J57" s="9"/>
       <c r="K57" s="9" t="str">
@@ -13064,16 +13067,16 @@
     </row>
     <row r="59" spans="1:22">
       <c r="B59" t="s">
-        <v>3448</v>
+        <v>3447</v>
       </c>
       <c r="C59" s="9" t="s">
-        <v>3444</v>
+        <v>3443</v>
       </c>
       <c r="F59" s="9" t="s">
         <v>0</v>
       </c>
       <c r="I59" s="9" t="s">
-        <v>3449</v>
+        <v>3448</v>
       </c>
       <c r="K59" s="9" t="str">
         <f>IF(LEN(C59),VLOOKUP(C59,mROW,3,FALSE),"")</f>
@@ -13082,16 +13085,16 @@
     </row>
     <row r="60" spans="1:22">
       <c r="B60" t="s">
-        <v>3448</v>
+        <v>3447</v>
       </c>
       <c r="C60" s="12" t="s">
-        <v>3444</v>
+        <v>3443</v>
       </c>
       <c r="F60" s="9" t="s">
         <v>3435</v>
       </c>
       <c r="I60" s="9" t="s">
-        <v>3450</v>
+        <v>3449</v>
       </c>
       <c r="K60" s="9" t="str">
         <f>IF(LEN(C60),VLOOKUP(C60,mROW,3,FALSE),"")</f>
@@ -13106,13 +13109,13 @@
     </row>
     <row r="62" spans="1:22" ht="45">
       <c r="B62" s="10" t="s">
-        <v>3452</v>
+        <v>3451</v>
       </c>
       <c r="C62" s="9" t="s">
-        <v>3449</v>
+        <v>3448</v>
       </c>
       <c r="J62" s="9" t="s">
-        <v>3444</v>
+        <v>3443</v>
       </c>
       <c r="K62" s="9" t="str">
         <f>IF(LEN(C62),VLOOKUP(C62,mROW,3,FALSE),"")</f>
@@ -13127,10 +13130,10 @@
     </row>
     <row r="64" spans="1:22" ht="45">
       <c r="B64" s="10" t="s">
-        <v>3453</v>
+        <v>3452</v>
       </c>
       <c r="C64" s="9" t="s">
-        <v>3450</v>
+        <v>3449</v>
       </c>
       <c r="J64" s="9" t="s">
         <v>3434</v>
@@ -42356,7 +42359,7 @@
         <v>2877</v>
       </c>
       <c r="I1" s="27" t="s">
-        <v>3479</v>
+        <v>3478</v>
       </c>
     </row>
     <row r="2" spans="1:37" ht="20.25">
@@ -42479,10 +42482,10 @@
         <v>5</v>
       </c>
       <c r="C6" s="65" t="s">
-        <v>3468</v>
+        <v>3467</v>
       </c>
       <c r="D6" s="67" t="s">
-        <v>3467</v>
+        <v>3466</v>
       </c>
       <c r="E6" s="67" t="s">
         <v>2873</v>
@@ -42701,10 +42704,10 @@
         <v>17</v>
       </c>
       <c r="C14" s="65" t="s">
-        <v>3474</v>
+        <v>3473</v>
       </c>
       <c r="D14" s="67" t="s">
-        <v>3476</v>
+        <v>3475</v>
       </c>
       <c r="E14" s="70" t="s">
         <v>2872</v>
@@ -42728,10 +42731,10 @@
         <v>18</v>
       </c>
       <c r="C15" s="65" t="s">
-        <v>3473</v>
+        <v>3472</v>
       </c>
       <c r="D15" s="67" t="s">
-        <v>3477</v>
+        <v>3476</v>
       </c>
       <c r="E15" s="70" t="s">
         <v>2872</v>
@@ -42755,10 +42758,10 @@
         <v>19</v>
       </c>
       <c r="C16" s="65" t="s">
-        <v>3475</v>
+        <v>3474</v>
       </c>
       <c r="D16" s="67" t="s">
-        <v>3478</v>
+        <v>3477</v>
       </c>
       <c r="E16" s="70" t="s">
         <v>2872</v>
@@ -43109,10 +43112,10 @@
         <v>41</v>
       </c>
       <c r="C29" s="65" t="s">
-        <v>3469</v>
+        <v>3468</v>
       </c>
       <c r="D29" s="71" t="s">
-        <v>3466</v>
+        <v>3465</v>
       </c>
       <c r="E29" s="70" t="s">
         <v>3398</v>
@@ -43136,10 +43139,10 @@
         <v>41</v>
       </c>
       <c r="C30" s="65" t="s">
-        <v>3470</v>
+        <v>3469</v>
       </c>
       <c r="D30" s="71" t="s">
-        <v>3466</v>
+        <v>3465</v>
       </c>
       <c r="E30" s="70" t="s">
         <v>3398</v>
@@ -43372,19 +43375,19 @@
     </row>
     <row r="39" spans="1:11" ht="75">
       <c r="A39" s="70" t="s">
-        <v>3455</v>
+        <v>3454</v>
       </c>
       <c r="B39" s="70">
         <v>62</v>
       </c>
       <c r="C39" s="65" t="s">
-        <v>3471</v>
+        <v>3470</v>
       </c>
       <c r="D39" s="67" t="s">
-        <v>3486</v>
+        <v>3485</v>
       </c>
       <c r="E39" s="67" t="s">
-        <v>3455</v>
+        <v>3454</v>
       </c>
       <c r="F39" s="68" t="s">
         <v>2887</v>
@@ -43396,24 +43399,24 @@
         <v>3397</v>
       </c>
       <c r="I39" s="27" t="s">
-        <v>3480</v>
+        <v>3479</v>
       </c>
     </row>
     <row r="40" spans="1:11" ht="45">
       <c r="A40" s="70" t="s">
-        <v>3455</v>
+        <v>3454</v>
       </c>
       <c r="B40" s="70">
         <v>63</v>
       </c>
       <c r="C40" s="65" t="s">
-        <v>3472</v>
+        <v>3471</v>
       </c>
       <c r="D40" s="67" t="s">
-        <v>3460</v>
+        <v>3459</v>
       </c>
       <c r="E40" s="67" t="s">
-        <v>3455</v>
+        <v>3454</v>
       </c>
       <c r="F40" s="68" t="s">
         <v>2887</v>
@@ -43425,24 +43428,24 @@
         <v>3397</v>
       </c>
       <c r="I40" s="27" t="s">
-        <v>3483</v>
+        <v>3482</v>
       </c>
     </row>
     <row r="41" spans="1:11" ht="45">
       <c r="A41" s="70" t="s">
-        <v>3455</v>
+        <v>3454</v>
       </c>
       <c r="B41" s="70">
         <v>64</v>
       </c>
       <c r="C41" s="65" t="s">
-        <v>3458</v>
+        <v>3457</v>
       </c>
       <c r="D41" s="67" t="s">
-        <v>3461</v>
+        <v>3460</v>
       </c>
       <c r="E41" s="70" t="s">
-        <v>3455</v>
+        <v>3454</v>
       </c>
       <c r="F41" s="68" t="s">
         <v>2887</v>
@@ -43454,24 +43457,24 @@
         <v>3397</v>
       </c>
       <c r="I41" s="27" t="s">
-        <v>3484</v>
+        <v>3483</v>
       </c>
     </row>
     <row r="42" spans="1:11" ht="45">
       <c r="A42" s="70" t="s">
-        <v>3455</v>
+        <v>3454</v>
       </c>
       <c r="B42" s="70">
         <v>65</v>
       </c>
       <c r="C42" s="65" t="s">
-        <v>3459</v>
+        <v>3458</v>
       </c>
       <c r="D42" s="67" t="s">
-        <v>3462</v>
+        <v>3461</v>
       </c>
       <c r="E42" s="70" t="s">
-        <v>3455</v>
+        <v>3454</v>
       </c>
       <c r="F42" s="68" t="s">
         <v>2887</v>
@@ -43483,7 +43486,7 @@
         <v>3397</v>
       </c>
       <c r="I42" s="27" t="s">
-        <v>3485</v>
+        <v>3484</v>
       </c>
     </row>
     <row r="43" spans="1:11" ht="15.75" customHeight="1">
@@ -43497,7 +43500,7 @@
         <v>3401</v>
       </c>
       <c r="D43" s="71" t="s">
-        <v>3463</v>
+        <v>3462</v>
       </c>
       <c r="E43" s="71" t="s">
         <v>3402</v>
@@ -43512,7 +43515,7 @@
         <v>3397</v>
       </c>
       <c r="I43" s="27" t="s">
-        <v>3481</v>
+        <v>3480</v>
       </c>
     </row>
     <row r="44" spans="1:11" ht="20.25">
@@ -43523,10 +43526,10 @@
         <v>102</v>
       </c>
       <c r="C44" s="65" t="s">
-        <v>3454</v>
+        <v>3453</v>
       </c>
       <c r="D44" s="71" t="s">
-        <v>3464</v>
+        <v>3463</v>
       </c>
       <c r="E44" s="71" t="s">
         <v>3402</v>
@@ -43541,7 +43544,7 @@
         <v>3397</v>
       </c>
       <c r="I44" s="27" t="s">
-        <v>3482</v>
+        <v>3481</v>
       </c>
     </row>
     <row r="45" spans="1:11" ht="20.25">

</xml_diff>

<commit_message>
plan for complete config loops
</commit_message>
<xml_diff>
--- a/RBG_arduino/StateTable_minimal.xlsx
+++ b/RBG_arduino/StateTable_minimal.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub-Mark-MDO47\RubberBandGun\RBG_arduino\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C0D93F2-5E73-4477-B3F9-E4CEC0A46869}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E08772AD-AD62-48F7-ADAC-D23754D05F58}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21840" xr2:uid="{CCADFEE4-B0E1-4363-9617-1683960BED03}"/>
   </bookViews>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5505" uniqueCount="4010">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5586" uniqueCount="4050">
   <si>
     <t>trigOnly</t>
   </si>
@@ -12807,6 +12807,126 @@
   </si>
   <si>
     <t>mdo47 recording of "Welcome to RBG configuration! Your call is important to us. Press color button first then trigger: YELLOW for sounds, GREEN for lights, BLACK for other. To go back, press trigger all by itself."</t>
+  </si>
+  <si>
+    <t>store EEPROM</t>
+  </si>
+  <si>
+    <t>choose effect category sound, LED, other</t>
+  </si>
+  <si>
+    <t>choose effect type (number group: shooting, open, close, etc.</t>
+  </si>
+  <si>
+    <t>store RAM (already have place for this but mechanism changes)</t>
+  </si>
+  <si>
+    <t>cycle through effects of type</t>
+  </si>
+  <si>
+    <t>change CFGSTORE ?</t>
+  </si>
+  <si>
+    <t>we have this</t>
+  </si>
+  <si>
+    <t>this is CFGNEXT loop</t>
+  </si>
+  <si>
+    <t>1 - need to re-establish CONFIG as EEPROM category so can say choose sound, choose LED pattern, etc.</t>
+  </si>
+  <si>
+    <t>add CFGNEXT capability for category</t>
+  </si>
+  <si>
+    <t>this changes numbers of everything past 60</t>
+  </si>
+  <si>
+    <t>mBITCFG_SOUND</t>
+  </si>
+  <si>
+    <t>mBITCFG_NUMBER</t>
+  </si>
+  <si>
+    <t>mSPCL_HANDLER_CFG2CATEGORY</t>
+  </si>
+  <si>
+    <t>mCFG_CATEGORY_NEXT</t>
+  </si>
+  <si>
+    <t>mCFG_CATEGORY_LOOPSTART</t>
+  </si>
+  <si>
+    <t>mEFCT_UNIQ_SND_CATEGORY</t>
+  </si>
+  <si>
+    <t>mCFG_CATEGORY_LOOP</t>
+  </si>
+  <si>
+    <t>mCFG_CATEGORY_CHOICE</t>
+  </si>
+  <si>
+    <t>mSPCL_HANDLER | mSPCL_HANDLER_CFG2CATEGORY | mSPCL_EFCT_NONE</t>
+  </si>
+  <si>
+    <t>mCFG_TYPE</t>
+  </si>
+  <si>
+    <t>CFGSTORE needs to know the loop count</t>
+  </si>
+  <si>
+    <t>mCFG_CATEGORY</t>
+  </si>
+  <si>
+    <t>mADDR_CFG_CATEGORY</t>
+  </si>
+  <si>
+    <t>mADDR_CFG_TYPE</t>
+  </si>
+  <si>
+    <t>mCFG_TYPE_LOOPSTART</t>
+  </si>
+  <si>
+    <t>mEFCT_UNIQ_SND_TYPE</t>
+  </si>
+  <si>
+    <t>mCFG_TYPE_LOOP</t>
+  </si>
+  <si>
+    <t>mCFG_TYPE_NEXT</t>
+  </si>
+  <si>
+    <t>mCFG_TYPE_CHOICE</t>
+  </si>
+  <si>
+    <t>mSPCL_HANDLER | mSPCL_HANDLER_CFG2TYPE | mSPCL_EFCT_NONE</t>
+  </si>
+  <si>
+    <t>CFGSTORE needs to know the loop count GIVEN the category</t>
+  </si>
+  <si>
+    <t>mCFG_EFFECT</t>
+  </si>
+  <si>
+    <t>mADDR_CFG_EFFECT</t>
+  </si>
+  <si>
+    <t>mCFG_EFFECT_LOOPSTART</t>
+  </si>
+  <si>
+    <t>mEFCT_UNIQ_SND_EFFECT</t>
+  </si>
+  <si>
+    <t>mCFG_EFFECT_LOOP</t>
+  </si>
+  <si>
+    <t>mCFG_EFFECT_NEXT</t>
+  </si>
+  <si>
+    <t>mCFG_EFFECT_CHOICE</t>
+  </si>
+  <si>
+    <t>CFGSTORE needs to know the loop count GIVEN the category AND the type</t>
   </si>
 </sst>
 </file>
@@ -13229,7 +13349,7 @@
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="24" fillId="12" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="85">
+  <cellXfs count="86">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -13389,6 +13509,9 @@
     </xf>
     <xf numFmtId="0" fontId="24" fillId="12" borderId="3" xfId="8"/>
     <xf numFmtId="0" fontId="31" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="2" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="9">
     <cellStyle name="Bad" xfId="2" builtinId="27"/>
@@ -13716,17 +13839,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{90E8DFC6-94F4-4A82-A874-2F16F2CF0145}">
-  <dimension ref="A1:AB84"/>
+  <dimension ref="A1:AB129"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A33" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E56" sqref="E56"/>
+      <pane ySplit="1" topLeftCell="A94" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D115" sqref="D115"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="22.85546875" customWidth="1"/>
-    <col min="2" max="2" width="28.7109375" customWidth="1"/>
+    <col min="2" max="2" width="30.7109375" customWidth="1"/>
     <col min="3" max="3" width="25.140625" bestFit="1" customWidth="1"/>
     <col min="4" max="5" width="42.42578125" customWidth="1"/>
     <col min="6" max="6" width="10" bestFit="1" customWidth="1"/>
@@ -15409,39 +15532,15 @@
       </c>
     </row>
     <row r="60" spans="1:24">
-      <c r="B60" t="s">
-        <v>3413</v>
-      </c>
-      <c r="C60" s="9" t="s">
-        <v>3409</v>
-      </c>
-      <c r="F60" s="9" t="s">
-        <v>0</v>
-      </c>
-      <c r="I60" s="9" t="s">
-        <v>3414</v>
-      </c>
-      <c r="K60" s="9" t="str">
-        <f>IF(LEN(C60),VLOOKUP(C60,mROW,3,FALSE),"")</f>
-        <v>#define mCFG_SOUND_LOOP 32</v>
+      <c r="K60" s="9" t="e">
+        <f>IF(LEN(C100),VLOOKUP(C100,mROW,3,FALSE),"")</f>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="61" spans="1:24">
-      <c r="B61" t="s">
-        <v>3413</v>
-      </c>
-      <c r="C61" s="12" t="s">
-        <v>3409</v>
-      </c>
-      <c r="F61" s="63" t="s">
-        <v>3583</v>
-      </c>
-      <c r="I61" s="9" t="s">
-        <v>3415</v>
-      </c>
-      <c r="K61" s="9" t="str">
-        <f>IF(LEN(C61),VLOOKUP(C61,mROW,3,FALSE),"")</f>
-        <v>#define mCFG_SOUND_LOOP 32</v>
+      <c r="K61" s="9" t="e">
+        <f>IF(LEN(C101),VLOOKUP(C101,mROW,3,FALSE),"")</f>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="62" spans="1:24">
@@ -15661,8 +15760,365 @@
         <v>mdo47 recording of "Effect type WAITING-FOR-TRIGGER. Trigger alone for next type."</v>
       </c>
     </row>
-    <row r="84" spans="6:6">
+    <row r="82" spans="2:12">
+      <c r="D82" s="10" t="s">
+        <v>4011</v>
+      </c>
+      <c r="E82" s="10" t="s">
+        <v>4010</v>
+      </c>
+      <c r="G82" s="13" t="s">
+        <v>4019</v>
+      </c>
+    </row>
+    <row r="83" spans="2:12" ht="30">
+      <c r="D83" s="10" t="s">
+        <v>4012</v>
+      </c>
+      <c r="E83" s="10" t="s">
+        <v>4013</v>
+      </c>
+      <c r="G83" s="13" t="s">
+        <v>4015</v>
+      </c>
+    </row>
+    <row r="84" spans="2:12">
+      <c r="D84" s="10" t="s">
+        <v>4014</v>
+      </c>
+      <c r="E84" s="10" t="s">
+        <v>4016</v>
+      </c>
       <c r="F84" s="63"/>
+      <c r="G84" t="s">
+        <v>4017</v>
+      </c>
+    </row>
+    <row r="85" spans="2:12">
+      <c r="D85" s="10"/>
+      <c r="E85" s="10"/>
+    </row>
+    <row r="86" spans="2:12">
+      <c r="D86" s="10"/>
+      <c r="E86" s="10"/>
+    </row>
+    <row r="87" spans="2:12" ht="45">
+      <c r="D87" s="10" t="s">
+        <v>4018</v>
+      </c>
+      <c r="E87" s="10" t="s">
+        <v>4020</v>
+      </c>
+    </row>
+    <row r="88" spans="2:12">
+      <c r="D88" s="10"/>
+      <c r="E88" s="10"/>
+    </row>
+    <row r="89" spans="2:12">
+      <c r="D89" s="10"/>
+      <c r="E89" s="10"/>
+    </row>
+    <row r="90" spans="2:12">
+      <c r="D90" s="10"/>
+      <c r="E90" s="10"/>
+      <c r="J90" t="s">
+        <v>4021</v>
+      </c>
+      <c r="K90" t="s">
+        <v>4023</v>
+      </c>
+    </row>
+    <row r="91" spans="2:12">
+      <c r="D91" s="10"/>
+      <c r="E91" s="10"/>
+      <c r="J91" t="s">
+        <v>4022</v>
+      </c>
+    </row>
+    <row r="96" spans="2:12" ht="45">
+      <c r="B96" s="10" t="s">
+        <v>3416</v>
+      </c>
+      <c r="C96" s="9" t="s">
+        <v>4032</v>
+      </c>
+      <c r="D96" s="9"/>
+      <c r="E96" s="76"/>
+      <c r="F96" s="9"/>
+      <c r="G96" s="85">
+        <v>0</v>
+      </c>
+      <c r="H96" s="75" t="s">
+        <v>4033</v>
+      </c>
+      <c r="J96" s="9" t="s">
+        <v>4025</v>
+      </c>
+      <c r="L96" s="13" t="s">
+        <v>4031</v>
+      </c>
+    </row>
+    <row r="98" spans="2:12">
+      <c r="B98" s="82" t="s">
+        <v>35</v>
+      </c>
+      <c r="C98" s="9" t="s">
+        <v>4025</v>
+      </c>
+      <c r="D98" s="3" t="s">
+        <v>4026</v>
+      </c>
+      <c r="E98" s="81" t="s">
+        <v>3400</v>
+      </c>
+      <c r="F98" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="G98" s="9"/>
+      <c r="H98" s="9"/>
+      <c r="I98" s="9" t="s">
+        <v>4027</v>
+      </c>
+    </row>
+    <row r="100" spans="2:12">
+      <c r="B100" t="s">
+        <v>3413</v>
+      </c>
+      <c r="C100" s="9" t="s">
+        <v>4027</v>
+      </c>
+      <c r="F100" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="I100" s="9" t="s">
+        <v>4024</v>
+      </c>
+    </row>
+    <row r="101" spans="2:12">
+      <c r="B101" t="s">
+        <v>3413</v>
+      </c>
+      <c r="C101" s="12" t="s">
+        <v>4027</v>
+      </c>
+      <c r="F101" s="63" t="s">
+        <v>3583</v>
+      </c>
+      <c r="I101" s="9" t="s">
+        <v>4028</v>
+      </c>
+    </row>
+    <row r="103" spans="2:12" ht="45">
+      <c r="B103" s="10" t="s">
+        <v>3417</v>
+      </c>
+      <c r="C103" s="9" t="s">
+        <v>4024</v>
+      </c>
+      <c r="J103" s="9" t="s">
+        <v>4024</v>
+      </c>
+    </row>
+    <row r="105" spans="2:12" ht="45">
+      <c r="B105" s="10" t="s">
+        <v>4029</v>
+      </c>
+      <c r="C105" s="9" t="s">
+        <v>4028</v>
+      </c>
+      <c r="J105" s="9" t="s">
+        <v>4030</v>
+      </c>
+    </row>
+    <row r="108" spans="2:12" ht="45">
+      <c r="B108" s="10" t="s">
+        <v>3416</v>
+      </c>
+      <c r="C108" s="9" t="s">
+        <v>4030</v>
+      </c>
+      <c r="D108" s="9"/>
+      <c r="E108" s="76"/>
+      <c r="F108" s="9"/>
+      <c r="G108" s="85">
+        <v>0</v>
+      </c>
+      <c r="H108" s="75" t="s">
+        <v>4034</v>
+      </c>
+      <c r="J108" s="9" t="s">
+        <v>4035</v>
+      </c>
+      <c r="L108" s="13" t="s">
+        <v>4041</v>
+      </c>
+    </row>
+    <row r="110" spans="2:12">
+      <c r="B110" s="82" t="s">
+        <v>35</v>
+      </c>
+      <c r="C110" s="9" t="s">
+        <v>4035</v>
+      </c>
+      <c r="D110" s="3" t="s">
+        <v>4036</v>
+      </c>
+      <c r="E110" s="81" t="s">
+        <v>3400</v>
+      </c>
+      <c r="F110" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="G110" s="9"/>
+      <c r="H110" s="9"/>
+      <c r="I110" s="9" t="s">
+        <v>4037</v>
+      </c>
+    </row>
+    <row r="112" spans="2:12">
+      <c r="B112" t="s">
+        <v>3413</v>
+      </c>
+      <c r="C112" s="9" t="s">
+        <v>4037</v>
+      </c>
+      <c r="F112" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="I112" s="9" t="s">
+        <v>4038</v>
+      </c>
+    </row>
+    <row r="113" spans="2:12">
+      <c r="B113" t="s">
+        <v>3413</v>
+      </c>
+      <c r="C113" s="12" t="s">
+        <v>4037</v>
+      </c>
+      <c r="F113" s="63" t="s">
+        <v>3583</v>
+      </c>
+      <c r="I113" s="9" t="s">
+        <v>4039</v>
+      </c>
+    </row>
+    <row r="115" spans="2:12" ht="45">
+      <c r="B115" s="10" t="s">
+        <v>3417</v>
+      </c>
+      <c r="C115" s="9" t="s">
+        <v>4038</v>
+      </c>
+      <c r="J115" s="9" t="s">
+        <v>4038</v>
+      </c>
+    </row>
+    <row r="117" spans="2:12" ht="45">
+      <c r="B117" s="10" t="s">
+        <v>4040</v>
+      </c>
+      <c r="C117" s="9" t="s">
+        <v>4039</v>
+      </c>
+      <c r="J117" s="9" t="s">
+        <v>4030</v>
+      </c>
+    </row>
+    <row r="120" spans="2:12" ht="45">
+      <c r="B120" s="10" t="s">
+        <v>3416</v>
+      </c>
+      <c r="C120" s="9" t="s">
+        <v>4042</v>
+      </c>
+      <c r="D120" s="9"/>
+      <c r="E120" s="76"/>
+      <c r="F120" s="9"/>
+      <c r="G120" s="85">
+        <v>0</v>
+      </c>
+      <c r="H120" s="75" t="s">
+        <v>4043</v>
+      </c>
+      <c r="J120" s="9" t="s">
+        <v>4044</v>
+      </c>
+      <c r="L120" s="13" t="s">
+        <v>4049</v>
+      </c>
+    </row>
+    <row r="122" spans="2:12">
+      <c r="B122" s="82" t="s">
+        <v>35</v>
+      </c>
+      <c r="C122" s="9" t="s">
+        <v>4044</v>
+      </c>
+      <c r="D122" s="3" t="s">
+        <v>4045</v>
+      </c>
+      <c r="E122" s="81" t="s">
+        <v>3400</v>
+      </c>
+      <c r="F122" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="G122" s="9"/>
+      <c r="H122" s="9"/>
+      <c r="I122" s="9" t="s">
+        <v>4046</v>
+      </c>
+    </row>
+    <row r="124" spans="2:12">
+      <c r="B124" t="s">
+        <v>3413</v>
+      </c>
+      <c r="C124" s="9" t="s">
+        <v>4046</v>
+      </c>
+      <c r="F124" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="I124" s="9" t="s">
+        <v>4047</v>
+      </c>
+    </row>
+    <row r="125" spans="2:12">
+      <c r="B125" t="s">
+        <v>3413</v>
+      </c>
+      <c r="C125" s="12" t="s">
+        <v>4046</v>
+      </c>
+      <c r="F125" s="63" t="s">
+        <v>3583</v>
+      </c>
+      <c r="I125" s="9" t="s">
+        <v>4048</v>
+      </c>
+    </row>
+    <row r="127" spans="2:12" ht="45">
+      <c r="B127" s="10" t="s">
+        <v>3417</v>
+      </c>
+      <c r="C127" s="9" t="s">
+        <v>4047</v>
+      </c>
+      <c r="J127" s="9" t="s">
+        <v>4047</v>
+      </c>
+    </row>
+    <row r="129" spans="2:10" ht="45">
+      <c r="B129" s="10" t="s">
+        <v>3418</v>
+      </c>
+      <c r="C129" s="9" t="s">
+        <v>4048</v>
+      </c>
+      <c r="J129" s="9" t="s">
+        <v>4042</v>
+      </c>
     </row>
   </sheetData>
   <autoFilter ref="A1:K69" xr:uid="{51E2FD16-9FD1-4BB3-809D-A325584B4921}"/>
@@ -48707,8 +49163,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A827A58D-C8A4-4858-A89B-E853C083564F}">
   <dimension ref="A1:AK114"/>
   <sheetViews>
-    <sheetView topLeftCell="G27" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D41" sqref="D41"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
@@ -48979,7 +49435,7 @@
       <c r="I9" s="27"/>
       <c r="AK9" s="28"/>
     </row>
-    <row r="10" spans="1:37" ht="30.75" thickTop="1">
+    <row r="10" spans="1:37" ht="31.5" thickTop="1" thickBot="1">
       <c r="A10" s="70" t="s">
         <v>2852</v>
       </c>
@@ -49007,11 +49463,11 @@
       <c r="I10" s="28"/>
       <c r="AK10" s="28"/>
     </row>
-    <row r="11" spans="1:37" ht="30">
+    <row r="11" spans="1:37" ht="31.5" thickTop="1" thickBot="1">
       <c r="A11" s="70" t="s">
         <v>2852</v>
       </c>
-      <c r="B11" s="70">
+      <c r="B11" s="74">
         <v>14</v>
       </c>
       <c r="C11" s="73" t="s">
@@ -49035,7 +49491,7 @@
       <c r="I11" s="28"/>
       <c r="AK11" s="28"/>
     </row>
-    <row r="12" spans="1:37" ht="20.25">
+    <row r="12" spans="1:37" ht="21" thickTop="1">
       <c r="A12" s="70" t="s">
         <v>2852</v>
       </c>

</xml_diff>

<commit_message>
moved myStateTable into FLASH (PROGMEM)
</commit_message>
<xml_diff>
--- a/RBG_arduino/StateTable_minimal.xlsx
+++ b/RBG_arduino/StateTable_minimal.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub-Mark-MDO47\RubberBandGun\RBG_arduino\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F81698A4-0407-4C98-978D-791AAE421B7B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6BA1E677-F1FC-4657-9459-4C9FEB99DCDB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21840" activeTab="5" xr2:uid="{CCADFEE4-B0E1-4363-9617-1683960BED03}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21840" xr2:uid="{CCADFEE4-B0E1-4363-9617-1683960BED03}"/>
   </bookViews>
   <sheets>
     <sheet name="StateTable" sheetId="1" r:id="rId1"/>
@@ -13894,9 +13894,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{90E8DFC6-94F4-4A82-A874-2F16F2CF0145}">
   <dimension ref="A1:AB86"/>
   <sheetViews>
-    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A38" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A43" sqref="A43"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A41" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C54" sqref="C54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
@@ -49469,7 +49469,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A827A58D-C8A4-4858-A89B-E853C083564F}">
   <dimension ref="A1:AK168"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView topLeftCell="A37" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="L54" sqref="L54:L56"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
add the 2save variables and some new config sounds
</commit_message>
<xml_diff>
--- a/RBG_arduino/StateTable_minimal.xlsx
+++ b/RBG_arduino/StateTable_minimal.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub-Mark-MDO47\RubberBandGun\RBG_arduino\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C95F63A-B5B3-479B-BC4F-8E5AB51BCD07}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E11FF4F-A0F5-45AB-98A0-7FCFA9C5498B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21840" xr2:uid="{CCADFEE4-B0E1-4363-9617-1683960BED03}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21840" activeTab="5" xr2:uid="{CCADFEE4-B0E1-4363-9617-1683960BED03}"/>
   </bookViews>
   <sheets>
     <sheet name="StateTable" sheetId="1" r:id="rId1"/>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5682" uniqueCount="4071">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5685" uniqueCount="4074">
   <si>
     <t>trigOnly</t>
   </si>
@@ -12921,9 +12921,6 @@
     <t>trigBlue</t>
   </si>
   <si>
-    <t>Welcome to RBG configuration! Your call is important to us. To go forward to next step or to cycle through choices, always press trigger by itself. To go back, press trigger plus Yellow, Green or Black button. To exit configuration, press trigger plus Blue button.</t>
-  </si>
-  <si>
     <t>Now choose when the effect happens: this list includes when powering-on, when shooting, etc. As always press trigger by itself to go forward to next step  or to cycle through choices. To select a choice, press trigger plus any combination of Yellow, Green or Black button. To exit configuration, press trigger plus Blue button.</t>
   </si>
   <si>
@@ -12933,18 +12930,12 @@
     <t>Now choose the effect itself. This list cycles through the effects one by one. As always press trigger by itself to go forward to next step  or to cycle through choices. To select a choice, press trigger plus any combination of Yellow, Green or Black button. To exit configuration, press trigger plus Blue button.</t>
   </si>
   <si>
-    <t>mdo47 recording of "Now choose which effect category: sounds or LED patterns. As always press trigger by itself to go forward to next step or to cycle through choices To select a choice, press trigger plus any combination of Yellow, Green or Black button. To exit configuration, press trigger plus Blue button."</t>
-  </si>
-  <si>
     <t>mdo47 recording of "Now choose when the effect happens. This list includes when powering-on, when shooting, etc. As always press trigger by itself to go forward to next step  or to cycle through choices. To select a choice, press trigger plus any combination of Yellow, Green or Black button. To exit configuration, press trigger plus Blue button."</t>
   </si>
   <si>
     <t>mdo47 recording of "Now choose the effect itself. This list cycles through the effects one by one. As always press trigger by itself to go forward to next step  or to cycle through choices. To select a choice, press trigger plus any combination of Yellow, Green or Black button. To exit configuration, press trigger plus Blue button."</t>
   </si>
   <si>
-    <t>mdo47 recording of "Welcome to RBG configuration! Your call is important to us. To go forward to next step or to cycle through choices, always press trigger by itself. To go back, press trigger plus Yellow, Green or Black button. To exit configuration, press trigger plus Blue button."</t>
-  </si>
-  <si>
     <t>#define mROW_CFG_MENU 24</t>
   </si>
   <si>
@@ -12991,6 +12982,24 @@
   </si>
   <si>
     <t>#define mROW_CFG_EFFECT_CHOICE 49</t>
+  </si>
+  <si>
+    <t>mdo47 recording of "Now choose which effect category: sounds or LED patterns. As always press trigger by itself to go forward to next step or to cycle through choices. To select a choice, press trigger plus any combination of Yellow, Green or Black button. To exit configuration, press trigger plus Blue button."</t>
+  </si>
+  <si>
+    <t>Welcome to RBG configuration! Your call is important to us. Press trigger by itself to go forward to next step or to cycle through choices To select a choice, press trigger plus any combination of Yellow, Green or Black button. To exit configuration, press trigger plus Blue button.</t>
+  </si>
+  <si>
+    <t>mdo47 recording of "Welcome to FOOF RBG configuration! Your call is important to us. Press trigger by itself to go forward to next step or to cycle through choices To select a choice, press trigger plus any combination of Yellow, Green or Black button. To exit configuration, press trigger plus Blue button."</t>
+  </si>
+  <si>
+    <t>0063__mdo47__cfg_configCategInstruct.wav</t>
+  </si>
+  <si>
+    <t>0064__mdo47__cfg_configWhenInstruct.wav</t>
+  </si>
+  <si>
+    <t>0065__mdo47__cfg_configEffectInstruct.wav</t>
   </si>
 </sst>
 </file>
@@ -13484,7 +13493,6 @@
     <xf numFmtId="0" fontId="23" fillId="3" borderId="0" xfId="2" applyFont="1"/>
     <xf numFmtId="165" fontId="4" fillId="3" borderId="0" xfId="2" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="4" xfId="3" applyBorder="1"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="4" xfId="7" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -13584,6 +13592,9 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="4" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="4" xfId="3" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -13915,9 +13926,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{90E8DFC6-94F4-4A82-A874-2F16F2CF0145}">
   <dimension ref="A1:AB93"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="O43" sqref="O43"/>
+    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A32" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B43" sqref="B43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
@@ -14033,7 +14044,7 @@
         <v>27</v>
       </c>
       <c r="X2" s="2" t="s">
-        <v>4056</v>
+        <v>4053</v>
       </c>
       <c r="AB2" s="25"/>
     </row>
@@ -14067,7 +14078,7 @@
         <v>35</v>
       </c>
       <c r="X3" s="2" t="s">
-        <v>4060</v>
+        <v>4057</v>
       </c>
     </row>
     <row r="4" spans="1:28">
@@ -14082,7 +14093,7 @@
         <v>31</v>
       </c>
       <c r="X4" s="2" t="s">
-        <v>4058</v>
+        <v>4055</v>
       </c>
     </row>
     <row r="5" spans="1:28" ht="45">
@@ -14112,7 +14123,7 @@
         <f>IF(LEN(C5),VLOOKUP(C5,mROW,3,FALSE),"")</f>
         <v>#define mROW_PWRON_OPEN 2</v>
       </c>
-      <c r="M5" s="64" t="s">
+      <c r="M5" s="63" t="s">
         <v>3565</v>
       </c>
       <c r="V5" t="s">
@@ -14122,7 +14133,7 @@
         <v>28</v>
       </c>
       <c r="X5" s="2" t="s">
-        <v>4057</v>
+        <v>4054</v>
       </c>
     </row>
     <row r="6" spans="1:28">
@@ -14139,7 +14150,7 @@
       <c r="E6" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="F6" s="64" t="s">
+      <c r="F6" s="63" t="s">
         <v>4042</v>
       </c>
       <c r="G6" s="9"/>
@@ -14152,7 +14163,7 @@
         <f>IF(LEN(C6),VLOOKUP(C6,mROW,3,FALSE),"")</f>
         <v>#define mROW_PWRON_OPEN 2</v>
       </c>
-      <c r="M6" s="64" t="s">
+      <c r="M6" s="63" t="s">
         <v>3566</v>
       </c>
       <c r="V6" t="s">
@@ -14162,7 +14173,7 @@
         <v>34</v>
       </c>
       <c r="X6" s="2" t="s">
-        <v>4059</v>
+        <v>4056</v>
       </c>
       <c r="AB6" s="25"/>
     </row>
@@ -14171,7 +14182,7 @@
         <f>IF(LEN(C7),VLOOKUP(C7,mROW,3,FALSE),"")</f>
         <v/>
       </c>
-      <c r="M7" s="64" t="s">
+      <c r="M7" s="63" t="s">
         <v>3567</v>
       </c>
       <c r="V7" t="s">
@@ -14181,7 +14192,7 @@
         <v>44</v>
       </c>
       <c r="X7" s="2" t="s">
-        <v>4066</v>
+        <v>4063</v>
       </c>
     </row>
     <row r="8" spans="1:28">
@@ -14189,7 +14200,7 @@
         <f>IF(LEN(C8),VLOOKUP(C8,mROW,3,FALSE),"")</f>
         <v/>
       </c>
-      <c r="M8" s="64" t="s">
+      <c r="M8" s="63" t="s">
         <v>3568</v>
       </c>
       <c r="V8" t="s">
@@ -14199,7 +14210,7 @@
         <v>49</v>
       </c>
       <c r="X8" s="2" t="s">
-        <v>4070</v>
+        <v>4067</v>
       </c>
     </row>
     <row r="9" spans="1:28">
@@ -14207,7 +14218,7 @@
         <f>IF(LEN(C9),VLOOKUP(C9,mROW,3,FALSE),"")</f>
         <v/>
       </c>
-      <c r="M9" s="64" t="s">
+      <c r="M9" s="63" t="s">
         <v>3569</v>
       </c>
       <c r="V9" t="s">
@@ -14217,7 +14228,7 @@
         <v>46</v>
       </c>
       <c r="X9" s="2" t="s">
-        <v>4068</v>
+        <v>4065</v>
       </c>
     </row>
     <row r="10" spans="1:28" s="25" customFormat="1">
@@ -14225,7 +14236,7 @@
         <f>IF(LEN(C10),VLOOKUP(C10,mROW,3,FALSE),"")</f>
         <v/>
       </c>
-      <c r="M10" s="64" t="s">
+      <c r="M10" s="63" t="s">
         <v>3570</v>
       </c>
       <c r="P10" s="25" t="s">
@@ -14247,7 +14258,7 @@
         <v>45</v>
       </c>
       <c r="X10" s="2" t="s">
-        <v>4067</v>
+        <v>4064</v>
       </c>
       <c r="AB10"/>
     </row>
@@ -14278,7 +14289,7 @@
         <f>IF(LEN(C11),VLOOKUP(C11,mROW,3,FALSE),"")</f>
         <v>#define mROW_PWRON_LOCKED 4</v>
       </c>
-      <c r="M11" s="64" t="s">
+      <c r="M11" s="63" t="s">
         <v>3571</v>
       </c>
       <c r="P11" s="25" t="s">
@@ -14291,7 +14302,7 @@
         <v>48</v>
       </c>
       <c r="X11" s="2" t="s">
-        <v>4069</v>
+        <v>4066</v>
       </c>
       <c r="AB11"/>
     </row>
@@ -14322,7 +14333,7 @@
         <f>IF(LEN(C12),VLOOKUP(C12,mROW,3,FALSE),"")</f>
         <v>#define mROW_PWRON_LOCKED 4</v>
       </c>
-      <c r="M12" s="64" t="s">
+      <c r="M12" s="63" t="s">
         <v>3572</v>
       </c>
       <c r="P12" s="25" t="s">
@@ -14338,7 +14349,7 @@
         <v>24</v>
       </c>
       <c r="X12" s="2" t="s">
-        <v>4055</v>
+        <v>4052</v>
       </c>
     </row>
     <row r="13" spans="1:28" s="25" customFormat="1">
@@ -14355,7 +14366,7 @@
       <c r="E13" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="F13" s="64" t="s">
+      <c r="F13" s="63" t="s">
         <v>4042</v>
       </c>
       <c r="G13" s="9"/>
@@ -14368,7 +14379,7 @@
         <f>IF(LEN(C13),VLOOKUP(C13,mROW,3,FALSE),"")</f>
         <v>#define mROW_PWRON_LOCKED 4</v>
       </c>
-      <c r="M13" s="64" t="s">
+      <c r="M13" s="63" t="s">
         <v>3573</v>
       </c>
       <c r="P13" s="25" t="s">
@@ -14381,7 +14392,7 @@
         <v>36</v>
       </c>
       <c r="X13" s="2" t="s">
-        <v>4061</v>
+        <v>4058</v>
       </c>
       <c r="AB13"/>
     </row>
@@ -14396,7 +14407,7 @@
         <v>43</v>
       </c>
       <c r="X14" s="2" t="s">
-        <v>4065</v>
+        <v>4062</v>
       </c>
     </row>
     <row r="15" spans="1:28" s="25" customFormat="1">
@@ -14412,12 +14423,12 @@
         <v>40</v>
       </c>
       <c r="X15" s="2" t="s">
-        <v>4063</v>
+        <v>4060</v>
       </c>
     </row>
     <row r="16" spans="1:28" s="25" customFormat="1">
       <c r="A16" s="37"/>
-      <c r="B16" s="77" t="s">
+      <c r="B16" s="76" t="s">
         <v>2712</v>
       </c>
       <c r="C16" s="37" t="s">
@@ -14448,12 +14459,12 @@
         <v>37</v>
       </c>
       <c r="X16" s="2" t="s">
-        <v>4062</v>
+        <v>4059</v>
       </c>
     </row>
     <row r="17" spans="1:26" s="25" customFormat="1">
       <c r="A17" s="37"/>
-      <c r="B17" s="77" t="s">
+      <c r="B17" s="76" t="s">
         <v>2712</v>
       </c>
       <c r="C17" s="48" t="s">
@@ -14481,14 +14492,14 @@
         <v>42</v>
       </c>
       <c r="X17" s="2" t="s">
-        <v>4064</v>
+        <v>4061</v>
       </c>
       <c r="Y17"/>
       <c r="Z17"/>
     </row>
     <row r="18" spans="1:26" s="25" customFormat="1">
       <c r="A18" s="37"/>
-      <c r="B18" s="77"/>
+      <c r="B18" s="76"/>
       <c r="C18" s="37" t="s">
         <v>40</v>
       </c>
@@ -14519,7 +14530,7 @@
     </row>
     <row r="19" spans="1:26">
       <c r="A19" s="37"/>
-      <c r="B19" s="83" t="s">
+      <c r="B19" s="82" t="s">
         <v>35</v>
       </c>
       <c r="C19" s="37" t="s">
@@ -14528,7 +14539,7 @@
       <c r="D19" s="47" t="s">
         <v>3401</v>
       </c>
-      <c r="E19" s="82" t="s">
+      <c r="E19" s="81" t="s">
         <v>3401</v>
       </c>
       <c r="F19" s="37" t="s">
@@ -14556,7 +14567,7 @@
     </row>
     <row r="20" spans="1:26">
       <c r="A20" s="37"/>
-      <c r="B20" s="77" t="s">
+      <c r="B20" s="76" t="s">
         <v>35</v>
       </c>
       <c r="C20" s="48" t="s">
@@ -14565,7 +14576,7 @@
       <c r="D20" s="47" t="s">
         <v>3401</v>
       </c>
-      <c r="E20" s="82" t="s">
+      <c r="E20" s="81" t="s">
         <v>3401</v>
       </c>
       <c r="F20" s="37" t="s">
@@ -14593,7 +14604,7 @@
     </row>
     <row r="21" spans="1:26">
       <c r="A21" s="37"/>
-      <c r="B21" s="77" t="s">
+      <c r="B21" s="76" t="s">
         <v>35</v>
       </c>
       <c r="C21" s="48" t="s">
@@ -14602,10 +14613,10 @@
       <c r="D21" s="47" t="s">
         <v>3401</v>
       </c>
-      <c r="E21" s="82" t="s">
+      <c r="E21" s="81" t="s">
         <v>3401</v>
       </c>
-      <c r="F21" s="64" t="s">
+      <c r="F21" s="63" t="s">
         <v>4042</v>
       </c>
       <c r="G21" s="37"/>
@@ -14630,12 +14641,12 @@
     </row>
     <row r="22" spans="1:26">
       <c r="A22" s="37"/>
-      <c r="B22" s="77"/>
+      <c r="B22" s="76"/>
       <c r="C22" s="37" t="s">
         <v>40</v>
       </c>
       <c r="D22" s="37"/>
-      <c r="E22" s="77"/>
+      <c r="E22" s="76"/>
       <c r="F22" s="37"/>
       <c r="G22" s="37"/>
       <c r="H22" s="37"/>
@@ -14658,7 +14669,7 @@
     </row>
     <row r="23" spans="1:26">
       <c r="A23" s="37"/>
-      <c r="B23" s="83" t="s">
+      <c r="B23" s="82" t="s">
         <v>35</v>
       </c>
       <c r="C23" s="37" t="s">
@@ -14667,7 +14678,7 @@
       <c r="D23" s="47" t="s">
         <v>3401</v>
       </c>
-      <c r="E23" s="82" t="s">
+      <c r="E23" s="81" t="s">
         <v>3401</v>
       </c>
       <c r="F23" s="37" t="s">
@@ -14695,7 +14706,7 @@
     </row>
     <row r="24" spans="1:26">
       <c r="A24" s="37"/>
-      <c r="B24" s="77" t="s">
+      <c r="B24" s="76" t="s">
         <v>35</v>
       </c>
       <c r="C24" s="48" t="s">
@@ -14704,7 +14715,7 @@
       <c r="D24" s="47" t="s">
         <v>3401</v>
       </c>
-      <c r="E24" s="82" t="s">
+      <c r="E24" s="81" t="s">
         <v>3401</v>
       </c>
       <c r="F24" s="37" t="s">
@@ -14733,7 +14744,7 @@
     </row>
     <row r="25" spans="1:26">
       <c r="A25" s="37"/>
-      <c r="B25" s="77" t="s">
+      <c r="B25" s="76" t="s">
         <v>35</v>
       </c>
       <c r="C25" s="48" t="s">
@@ -14742,10 +14753,10 @@
       <c r="D25" s="47" t="s">
         <v>3401</v>
       </c>
-      <c r="E25" s="82" t="s">
+      <c r="E25" s="81" t="s">
         <v>3401</v>
       </c>
-      <c r="F25" s="64" t="s">
+      <c r="F25" s="63" t="s">
         <v>4042</v>
       </c>
       <c r="G25" s="37"/>
@@ -14795,7 +14806,7 @@
       <c r="Y26" s="25"/>
     </row>
     <row r="27" spans="1:26">
-      <c r="A27" s="63" t="s">
+      <c r="A27" s="62" t="s">
         <v>52</v>
       </c>
       <c r="B27" t="s">
@@ -14830,7 +14841,7 @@
       <c r="Y27" s="25"/>
     </row>
     <row r="28" spans="1:26">
-      <c r="A28" s="63"/>
+      <c r="A28" s="62"/>
       <c r="C28" s="9"/>
       <c r="I28" s="9"/>
       <c r="J28" s="9"/>
@@ -14849,7 +14860,7 @@
       </c>
     </row>
     <row r="29" spans="1:26" ht="45">
-      <c r="A29" s="63" t="s">
+      <c r="A29" s="62" t="s">
         <v>47</v>
       </c>
       <c r="B29" s="10" t="s">
@@ -14878,7 +14889,7 @@
       <c r="Y29" s="25"/>
     </row>
     <row r="30" spans="1:26">
-      <c r="A30" s="63"/>
+      <c r="A30" s="62"/>
       <c r="B30" s="10"/>
       <c r="C30" s="9"/>
       <c r="I30" s="9"/>
@@ -14890,7 +14901,7 @@
       <c r="X30" s="2"/>
     </row>
     <row r="31" spans="1:26" s="25" customFormat="1">
-      <c r="A31" s="63" t="s">
+      <c r="A31" s="62" t="s">
         <v>49</v>
       </c>
       <c r="B31" s="9" t="s">
@@ -14923,7 +14934,7 @@
       <c r="Y31"/>
     </row>
     <row r="32" spans="1:26">
-      <c r="A32" s="63"/>
+      <c r="A32" s="62"/>
       <c r="B32" s="10"/>
       <c r="C32" s="9"/>
       <c r="I32" s="9"/>
@@ -14937,7 +14948,7 @@
       <c r="X32" s="2"/>
     </row>
     <row r="33" spans="1:24">
-      <c r="A33" s="63"/>
+      <c r="A33" s="62"/>
       <c r="C33" s="9"/>
       <c r="I33" s="9"/>
       <c r="J33" s="9"/>
@@ -14949,7 +14960,7 @@
       <c r="X33" s="2"/>
     </row>
     <row r="34" spans="1:24" ht="45">
-      <c r="A34" s="63" t="s">
+      <c r="A34" s="62" t="s">
         <v>3438</v>
       </c>
       <c r="B34" s="10" t="s">
@@ -14972,7 +14983,7 @@
       <c r="X34" s="2"/>
     </row>
     <row r="35" spans="1:24">
-      <c r="A35" s="63"/>
+      <c r="A35" s="62"/>
       <c r="B35" s="10"/>
       <c r="D35" s="3"/>
       <c r="I35" s="9"/>
@@ -14983,7 +14994,7 @@
       </c>
     </row>
     <row r="36" spans="1:24">
-      <c r="A36" s="63" t="s">
+      <c r="A36" s="62" t="s">
         <v>36</v>
       </c>
       <c r="B36" s="9" t="s">
@@ -15011,7 +15022,7 @@
       </c>
     </row>
     <row r="37" spans="1:24">
-      <c r="A37" s="63"/>
+      <c r="A37" s="62"/>
       <c r="B37" s="9" t="s">
         <v>2709</v>
       </c>
@@ -15039,7 +15050,7 @@
       </c>
     </row>
     <row r="38" spans="1:24">
-      <c r="A38" s="63"/>
+      <c r="A38" s="62"/>
       <c r="B38" s="25"/>
       <c r="C38" s="25"/>
       <c r="D38" s="25"/>
@@ -15055,7 +15066,7 @@
       </c>
     </row>
     <row r="39" spans="1:24" ht="30">
-      <c r="A39" s="63" t="s">
+      <c r="A39" s="62" t="s">
         <v>37</v>
       </c>
       <c r="B39" s="9" t="s">
@@ -15080,7 +15091,7 @@
       </c>
     </row>
     <row r="40" spans="1:24">
-      <c r="A40" s="63"/>
+      <c r="A40" s="62"/>
       <c r="B40" s="9" t="s">
         <v>2709</v>
       </c>
@@ -15139,11 +15150,11 @@
       <c r="J42" s="9"/>
       <c r="K42" s="9"/>
     </row>
-    <row r="43" spans="1:24" ht="180">
-      <c r="A43" s="87" t="s">
-        <v>4047</v>
-      </c>
-      <c r="B43" s="83" t="s">
+    <row r="43" spans="1:24" ht="195">
+      <c r="A43" s="86" t="s">
+        <v>4069</v>
+      </c>
+      <c r="B43" s="82" t="s">
         <v>35</v>
       </c>
       <c r="C43" s="9" t="s">
@@ -15152,7 +15163,7 @@
       <c r="D43" s="3" t="s">
         <v>3443</v>
       </c>
-      <c r="E43" s="82" t="s">
+      <c r="E43" s="81" t="s">
         <v>3401</v>
       </c>
       <c r="F43" s="9" t="s">
@@ -15169,8 +15180,8 @@
       <c r="O43" s="37"/>
     </row>
     <row r="44" spans="1:24">
-      <c r="A44" s="63"/>
-      <c r="B44" s="83" t="s">
+      <c r="A44" s="62"/>
+      <c r="B44" s="82" t="s">
         <v>35</v>
       </c>
       <c r="C44" s="11" t="s">
@@ -15179,10 +15190,10 @@
       <c r="D44" s="3" t="s">
         <v>3443</v>
       </c>
-      <c r="E44" s="82" t="s">
+      <c r="E44" s="81" t="s">
         <v>3401</v>
       </c>
-      <c r="F44" s="64" t="s">
+      <c r="F44" s="63" t="s">
         <v>3574</v>
       </c>
       <c r="I44" s="9" t="s">
@@ -15195,7 +15206,7 @@
       </c>
     </row>
     <row r="45" spans="1:24">
-      <c r="B45" s="83" t="s">
+      <c r="B45" s="82" t="s">
         <v>35</v>
       </c>
       <c r="C45" s="12" t="s">
@@ -15204,13 +15215,13 @@
       <c r="D45" s="3" t="s">
         <v>3443</v>
       </c>
-      <c r="E45" s="82" t="s">
+      <c r="E45" s="81" t="s">
         <v>3401</v>
       </c>
-      <c r="F45" s="64" t="s">
+      <c r="F45" s="63" t="s">
         <v>4046</v>
       </c>
-      <c r="I45" s="77" t="s">
+      <c r="I45" s="76" t="s">
         <v>39</v>
       </c>
       <c r="J45" s="9"/>
@@ -15243,12 +15254,12 @@
         <v>4038</v>
       </c>
       <c r="D48" s="9"/>
-      <c r="E48" s="77"/>
+      <c r="E48" s="76"/>
       <c r="F48" s="9"/>
-      <c r="G48" s="86">
+      <c r="G48" s="85">
         <v>0</v>
       </c>
-      <c r="H48" s="76" t="s">
+      <c r="H48" s="75" t="s">
         <v>4014</v>
       </c>
       <c r="I48" s="9"/>
@@ -15269,10 +15280,10 @@
       </c>
     </row>
     <row r="50" spans="1:11" ht="210">
-      <c r="A50" s="88" t="s">
-        <v>4049</v>
-      </c>
-      <c r="B50" s="83" t="s">
+      <c r="A50" s="87" t="s">
+        <v>4048</v>
+      </c>
+      <c r="B50" s="82" t="s">
         <v>35</v>
       </c>
       <c r="C50" s="9" t="s">
@@ -15281,7 +15292,7 @@
       <c r="D50" s="3" t="s">
         <v>4043</v>
       </c>
-      <c r="E50" s="82" t="s">
+      <c r="E50" s="81" t="s">
         <v>3401</v>
       </c>
       <c r="F50" s="9" t="s">
@@ -15299,7 +15310,7 @@
       </c>
     </row>
     <row r="51" spans="1:11">
-      <c r="B51" s="83" t="s">
+      <c r="B51" s="82" t="s">
         <v>35</v>
       </c>
       <c r="C51" s="12" t="s">
@@ -15308,10 +15319,10 @@
       <c r="D51" s="3" t="s">
         <v>4043</v>
       </c>
-      <c r="E51" s="82" t="s">
+      <c r="E51" s="81" t="s">
         <v>3401</v>
       </c>
-      <c r="F51" s="64" t="s">
+      <c r="F51" s="63" t="s">
         <v>3574</v>
       </c>
       <c r="G51" s="9"/>
@@ -15326,7 +15337,7 @@
       </c>
     </row>
     <row r="52" spans="1:11">
-      <c r="B52" s="83" t="s">
+      <c r="B52" s="82" t="s">
         <v>35</v>
       </c>
       <c r="C52" s="12" t="s">
@@ -15335,13 +15346,13 @@
       <c r="D52" s="3" t="s">
         <v>4043</v>
       </c>
-      <c r="E52" s="82" t="s">
+      <c r="E52" s="81" t="s">
         <v>3401</v>
       </c>
-      <c r="F52" s="64" t="s">
+      <c r="F52" s="63" t="s">
         <v>4046</v>
       </c>
-      <c r="I52" s="77" t="s">
+      <c r="I52" s="76" t="s">
         <v>39</v>
       </c>
       <c r="J52" s="9"/>
@@ -15384,7 +15395,7 @@
       <c r="C55" s="12" t="s">
         <v>4025</v>
       </c>
-      <c r="F55" s="64" t="s">
+      <c r="F55" s="63" t="s">
         <v>3574</v>
       </c>
       <c r="I55" s="9" t="s">
@@ -15404,11 +15415,11 @@
         <v>4025</v>
       </c>
       <c r="D56" s="3"/>
-      <c r="E56" s="82"/>
-      <c r="F56" s="64" t="s">
+      <c r="E56" s="81"/>
+      <c r="F56" s="63" t="s">
         <v>4046</v>
       </c>
-      <c r="I56" s="77" t="s">
+      <c r="I56" s="76" t="s">
         <v>39</v>
       </c>
       <c r="J56" s="9"/>
@@ -15487,12 +15498,12 @@
         <v>4028</v>
       </c>
       <c r="D63" s="9"/>
-      <c r="E63" s="77"/>
+      <c r="E63" s="76"/>
       <c r="F63" s="9"/>
-      <c r="G63" s="86">
+      <c r="G63" s="85">
         <v>0</v>
       </c>
-      <c r="H63" s="76" t="s">
+      <c r="H63" s="75" t="s">
         <v>4015</v>
       </c>
       <c r="J63" s="9" t="s">
@@ -15510,10 +15521,10 @@
       </c>
     </row>
     <row r="65" spans="1:24" ht="225">
-      <c r="A65" s="88" t="s">
-        <v>4048</v>
-      </c>
-      <c r="B65" s="83" t="s">
+      <c r="A65" s="87" t="s">
+        <v>4047</v>
+      </c>
+      <c r="B65" s="82" t="s">
         <v>35</v>
       </c>
       <c r="C65" s="9" t="s">
@@ -15522,7 +15533,7 @@
       <c r="D65" s="3" t="s">
         <v>4044</v>
       </c>
-      <c r="E65" s="82" t="s">
+      <c r="E65" s="81" t="s">
         <v>3401</v>
       </c>
       <c r="F65" s="9" t="s">
@@ -15539,7 +15550,7 @@
       </c>
     </row>
     <row r="66" spans="1:24">
-      <c r="B66" s="83" t="s">
+      <c r="B66" s="82" t="s">
         <v>35</v>
       </c>
       <c r="C66" s="12" t="s">
@@ -15548,7 +15559,7 @@
       <c r="D66" s="3" t="s">
         <v>4044</v>
       </c>
-      <c r="E66" s="82" t="s">
+      <c r="E66" s="81" t="s">
         <v>3401</v>
       </c>
       <c r="F66" s="9"/>
@@ -15572,7 +15583,7 @@
       </c>
     </row>
     <row r="67" spans="1:24">
-      <c r="B67" s="83" t="s">
+      <c r="B67" s="82" t="s">
         <v>35</v>
       </c>
       <c r="C67" s="12" t="s">
@@ -15581,7 +15592,7 @@
       <c r="D67" s="3" t="s">
         <v>4044</v>
       </c>
-      <c r="E67" s="82" t="s">
+      <c r="E67" s="81" t="s">
         <v>3401</v>
       </c>
       <c r="F67" s="9"/>
@@ -15657,7 +15668,7 @@
       <c r="C70" s="12" t="s">
         <v>4030</v>
       </c>
-      <c r="F70" s="64" t="s">
+      <c r="F70" s="63" t="s">
         <v>3574</v>
       </c>
       <c r="I70" s="9" t="s">
@@ -15800,8 +15811,8 @@
       </c>
     </row>
     <row r="77" spans="1:24" ht="210">
-      <c r="A77" s="88" t="s">
-        <v>4050</v>
+      <c r="A77" s="87" t="s">
+        <v>4049</v>
       </c>
       <c r="B77" s="10" t="s">
         <v>4040</v>
@@ -15810,12 +15821,12 @@
         <v>4037</v>
       </c>
       <c r="D77" s="9"/>
-      <c r="E77" s="77"/>
+      <c r="E77" s="76"/>
       <c r="F77" s="9"/>
-      <c r="G77" s="86">
+      <c r="G77" s="85">
         <v>0</v>
       </c>
-      <c r="H77" s="76" t="s">
+      <c r="H77" s="75" t="s">
         <v>4016</v>
       </c>
       <c r="J77" s="9" t="s">
@@ -15851,11 +15862,11 @@
         <v>24</v>
       </c>
       <c r="X78" t="s">
-        <v>4055</v>
+        <v>4052</v>
       </c>
     </row>
     <row r="79" spans="1:24">
-      <c r="B79" s="83" t="s">
+      <c r="B79" s="82" t="s">
         <v>35</v>
       </c>
       <c r="C79" s="9" t="s">
@@ -15864,7 +15875,7 @@
       <c r="D79" s="3" t="s">
         <v>4045</v>
       </c>
-      <c r="E79" s="82" t="s">
+      <c r="E79" s="81" t="s">
         <v>3401</v>
       </c>
       <c r="F79" s="9" t="s">
@@ -15888,7 +15899,7 @@
         <v>27</v>
       </c>
       <c r="X79" t="s">
-        <v>4056</v>
+        <v>4053</v>
       </c>
     </row>
     <row r="80" spans="1:24">
@@ -15905,7 +15916,7 @@
         <v>28</v>
       </c>
       <c r="X80" t="s">
-        <v>4057</v>
+        <v>4054</v>
       </c>
     </row>
     <row r="81" spans="2:24">
@@ -15934,7 +15945,7 @@
         <v>31</v>
       </c>
       <c r="X81" t="s">
-        <v>4058</v>
+        <v>4055</v>
       </c>
     </row>
     <row r="82" spans="2:24">
@@ -15944,7 +15955,7 @@
       <c r="C82" s="12" t="s">
         <v>4034</v>
       </c>
-      <c r="F82" s="64" t="s">
+      <c r="F82" s="63" t="s">
         <v>3574</v>
       </c>
       <c r="I82" s="9" t="s">
@@ -15963,7 +15974,7 @@
         <v>34</v>
       </c>
       <c r="X82" t="s">
-        <v>4059</v>
+        <v>4056</v>
       </c>
     </row>
     <row r="83" spans="2:24">
@@ -15980,7 +15991,7 @@
         <v>35</v>
       </c>
       <c r="X83" t="s">
-        <v>4060</v>
+        <v>4057</v>
       </c>
     </row>
     <row r="84" spans="2:24" ht="45">
@@ -16006,7 +16017,7 @@
         <v>36</v>
       </c>
       <c r="X84" t="s">
-        <v>4061</v>
+        <v>4058</v>
       </c>
     </row>
     <row r="85" spans="2:24">
@@ -16023,7 +16034,7 @@
         <v>37</v>
       </c>
       <c r="X85" t="s">
-        <v>4062</v>
+        <v>4059</v>
       </c>
     </row>
     <row r="86" spans="2:24" ht="45">
@@ -16049,7 +16060,7 @@
         <v>40</v>
       </c>
       <c r="X86" t="s">
-        <v>4063</v>
+        <v>4060</v>
       </c>
     </row>
     <row r="87" spans="2:24">
@@ -16062,7 +16073,7 @@
         <v>42</v>
       </c>
       <c r="X87" t="s">
-        <v>4064</v>
+        <v>4061</v>
       </c>
     </row>
     <row r="88" spans="2:24">
@@ -16075,7 +16086,7 @@
         <v>43</v>
       </c>
       <c r="X88" t="s">
-        <v>4065</v>
+        <v>4062</v>
       </c>
     </row>
     <row r="89" spans="2:24">
@@ -16088,7 +16099,7 @@
         <v>44</v>
       </c>
       <c r="X89" t="s">
-        <v>4066</v>
+        <v>4063</v>
       </c>
     </row>
     <row r="90" spans="2:24">
@@ -16101,7 +16112,7 @@
         <v>45</v>
       </c>
       <c r="X90" t="s">
-        <v>4067</v>
+        <v>4064</v>
       </c>
     </row>
     <row r="91" spans="2:24">
@@ -16114,7 +16125,7 @@
         <v>46</v>
       </c>
       <c r="X91" t="s">
-        <v>4068</v>
+        <v>4065</v>
       </c>
     </row>
     <row r="92" spans="2:24">
@@ -16127,7 +16138,7 @@
         <v>48</v>
       </c>
       <c r="X92" t="s">
-        <v>4069</v>
+        <v>4066</v>
       </c>
     </row>
     <row r="93" spans="2:24">
@@ -16140,7 +16151,7 @@
         <v>49</v>
       </c>
       <c r="X93" t="s">
-        <v>4070</v>
+        <v>4067</v>
       </c>
     </row>
   </sheetData>
@@ -16199,10 +16210,10 @@
       </c>
     </row>
     <row r="3" spans="1:24" ht="135">
-      <c r="A3" s="63" t="s">
+      <c r="A3" s="62" t="s">
         <v>3958</v>
       </c>
-      <c r="B3" s="83" t="s">
+      <c r="B3" s="82" t="s">
         <v>35</v>
       </c>
       <c r="C3" s="9" t="s">
@@ -16211,7 +16222,7 @@
       <c r="D3" s="3" t="s">
         <v>3443</v>
       </c>
-      <c r="E3" s="82" t="s">
+      <c r="E3" s="81" t="s">
         <v>3401</v>
       </c>
       <c r="F3" s="9" t="s">
@@ -16237,8 +16248,8 @@
       </c>
     </row>
     <row r="4" spans="1:24">
-      <c r="A4" s="63"/>
-      <c r="B4" s="83" t="s">
+      <c r="A4" s="62"/>
+      <c r="B4" s="82" t="s">
         <v>35</v>
       </c>
       <c r="C4" s="11" t="s">
@@ -16247,13 +16258,13 @@
       <c r="D4" s="3" t="s">
         <v>3443</v>
       </c>
-      <c r="E4" s="82" t="s">
+      <c r="E4" s="81" t="s">
         <v>3401</v>
       </c>
       <c r="F4" t="s">
         <v>3403</v>
       </c>
-      <c r="I4" s="76" t="s">
+      <c r="I4" s="75" t="s">
         <v>4019</v>
       </c>
       <c r="K4" s="9" t="e">
@@ -16273,8 +16284,8 @@
       </c>
     </row>
     <row r="5" spans="1:24">
-      <c r="A5" s="63"/>
-      <c r="B5" s="83" t="s">
+      <c r="A5" s="62"/>
+      <c r="B5" s="82" t="s">
         <v>35</v>
       </c>
       <c r="C5" s="11" t="s">
@@ -16283,7 +16294,7 @@
       <c r="D5" s="3" t="s">
         <v>3443</v>
       </c>
-      <c r="E5" s="82" t="s">
+      <c r="E5" s="81" t="s">
         <v>3401</v>
       </c>
       <c r="F5" t="s">
@@ -16309,8 +16320,8 @@
       </c>
     </row>
     <row r="6" spans="1:24">
-      <c r="A6" s="63"/>
-      <c r="B6" s="83" t="s">
+      <c r="A6" s="62"/>
+      <c r="B6" s="82" t="s">
         <v>35</v>
       </c>
       <c r="C6" s="11" t="s">
@@ -16319,7 +16330,7 @@
       <c r="D6" s="3" t="s">
         <v>3443</v>
       </c>
-      <c r="E6" s="82" t="s">
+      <c r="E6" s="81" t="s">
         <v>3401</v>
       </c>
       <c r="F6" t="s">
@@ -16345,7 +16356,7 @@
       </c>
     </row>
     <row r="7" spans="1:24">
-      <c r="A7" s="63"/>
+      <c r="A7" s="62"/>
       <c r="D7" s="3"/>
       <c r="E7" s="2"/>
       <c r="K7" s="9" t="str">
@@ -16365,7 +16376,7 @@
       </c>
     </row>
     <row r="8" spans="1:24">
-      <c r="A8" s="63"/>
+      <c r="A8" s="62"/>
       <c r="D8" s="3"/>
       <c r="E8" s="2"/>
       <c r="K8" s="9" t="str">
@@ -16385,7 +16396,7 @@
       </c>
     </row>
     <row r="9" spans="1:24" ht="30">
-      <c r="A9" s="63" t="s">
+      <c r="A9" s="62" t="s">
         <v>3406</v>
       </c>
       <c r="B9" s="9" t="s">
@@ -16397,7 +16408,7 @@
       <c r="D9" s="3" t="s">
         <v>3437</v>
       </c>
-      <c r="E9" s="82" t="s">
+      <c r="E9" s="81" t="s">
         <v>3401</v>
       </c>
       <c r="J9" s="9" t="s">
@@ -16420,7 +16431,7 @@
       </c>
     </row>
     <row r="10" spans="1:24">
-      <c r="A10" s="63"/>
+      <c r="A10" s="62"/>
       <c r="C10" s="9"/>
       <c r="E10" s="2"/>
       <c r="K10" s="9" t="str">
@@ -16440,7 +16451,7 @@
       </c>
     </row>
     <row r="11" spans="1:24" ht="30">
-      <c r="A11" s="63" t="s">
+      <c r="A11" s="62" t="s">
         <v>3406</v>
       </c>
       <c r="B11" s="9" t="s">
@@ -16452,7 +16463,7 @@
       <c r="D11" s="3" t="s">
         <v>3437</v>
       </c>
-      <c r="E11" s="82" t="s">
+      <c r="E11" s="81" t="s">
         <v>3401</v>
       </c>
       <c r="J11" s="9" t="s">
@@ -16475,7 +16486,7 @@
       </c>
     </row>
     <row r="12" spans="1:24">
-      <c r="A12" s="63"/>
+      <c r="A12" s="62"/>
       <c r="C12" s="9"/>
       <c r="E12" s="2"/>
       <c r="K12" s="9" t="str">
@@ -16495,7 +16506,7 @@
       </c>
     </row>
     <row r="13" spans="1:24" ht="45">
-      <c r="A13" s="63" t="s">
+      <c r="A13" s="62" t="s">
         <v>3411</v>
       </c>
       <c r="B13" s="10" t="s">
@@ -16505,7 +16516,7 @@
         <v>4019</v>
       </c>
       <c r="D13" s="9"/>
-      <c r="E13" s="77"/>
+      <c r="E13" s="76"/>
       <c r="F13" s="9"/>
       <c r="G13" s="10" t="s">
         <v>3957</v>
@@ -16534,7 +16545,7 @@
       </c>
     </row>
     <row r="14" spans="1:24">
-      <c r="A14" s="63"/>
+      <c r="A14" s="62"/>
       <c r="E14" s="2"/>
       <c r="K14" s="9" t="str">
         <f>IF(LEN(C14),VLOOKUP(C14,mROW,3,FALSE),"")</f>
@@ -16553,10 +16564,10 @@
       </c>
     </row>
     <row r="15" spans="1:24" ht="75">
-      <c r="A15" s="63" t="s">
+      <c r="A15" s="62" t="s">
         <v>3418</v>
       </c>
-      <c r="B15" s="83" t="s">
+      <c r="B15" s="82" t="s">
         <v>35</v>
       </c>
       <c r="C15" s="9" t="s">
@@ -16565,7 +16576,7 @@
       <c r="D15" s="3" t="s">
         <v>3444</v>
       </c>
-      <c r="E15" s="82" t="s">
+      <c r="E15" s="81" t="s">
         <v>3401</v>
       </c>
       <c r="F15" s="9" t="s">
@@ -16655,7 +16666,7 @@
       </c>
     </row>
     <row r="25" spans="1:11" ht="75">
-      <c r="A25" s="63" t="s">
+      <c r="A25" s="62" t="s">
         <v>3964</v>
       </c>
       <c r="B25">
@@ -16674,7 +16685,7 @@
       </c>
     </row>
     <row r="26" spans="1:11" ht="45">
-      <c r="A26" s="63" t="s">
+      <c r="A26" s="62" t="s">
         <v>3991</v>
       </c>
       <c r="B26">
@@ -16696,7 +16707,7 @@
       </c>
     </row>
     <row r="27" spans="1:11" ht="30">
-      <c r="A27" s="63" t="s">
+      <c r="A27" s="62" t="s">
         <v>3992</v>
       </c>
       <c r="B27">
@@ -16718,7 +16729,7 @@
       </c>
     </row>
     <row r="28" spans="1:11" ht="45">
-      <c r="A28" s="63" t="s">
+      <c r="A28" s="62" t="s">
         <v>3993</v>
       </c>
       <c r="B28">
@@ -16740,7 +16751,7 @@
       </c>
     </row>
     <row r="29" spans="1:11" ht="45">
-      <c r="A29" s="63" t="s">
+      <c r="A29" s="62" t="s">
         <v>3994</v>
       </c>
       <c r="B29">
@@ -16762,7 +16773,7 @@
       </c>
     </row>
     <row r="30" spans="1:11" ht="45">
-      <c r="A30" s="63" t="s">
+      <c r="A30" s="62" t="s">
         <v>3995</v>
       </c>
       <c r="B30">
@@ -16784,7 +16795,7 @@
       </c>
     </row>
     <row r="31" spans="1:11" ht="45">
-      <c r="A31" s="63" t="s">
+      <c r="A31" s="62" t="s">
         <v>3996</v>
       </c>
       <c r="B31">
@@ -16846,7 +16857,7 @@
       <c r="E40" s="10" t="s">
         <v>4006</v>
       </c>
-      <c r="F40" s="64"/>
+      <c r="F40" s="63"/>
       <c r="G40" t="s">
         <v>4007</v>
       </c>
@@ -43607,7 +43618,7 @@
       <c r="A3304">
         <v>1733</v>
       </c>
-      <c r="B3304" s="84" t="s">
+      <c r="B3304" s="83" t="s">
         <v>3553</v>
       </c>
     </row>
@@ -43746,7 +43757,7 @@
       <c r="A3321">
         <v>4842</v>
       </c>
-      <c r="B3321" s="84" t="s">
+      <c r="B3321" s="83" t="s">
         <v>3555</v>
       </c>
     </row>
@@ -43883,7 +43894,7 @@
       <c r="A3337">
         <v>5039</v>
       </c>
-      <c r="B3337" s="84" t="s">
+      <c r="B3337" s="83" t="s">
         <v>3559</v>
       </c>
     </row>
@@ -44010,7 +44021,7 @@
       <c r="A3351">
         <v>5251</v>
       </c>
-      <c r="B3351" s="84" t="s">
+      <c r="B3351" s="83" t="s">
         <v>3561</v>
       </c>
     </row>
@@ -44080,7 +44091,7 @@
       <c r="A3359">
         <v>5421</v>
       </c>
-      <c r="B3359" s="84" t="s">
+      <c r="B3359" s="83" t="s">
         <v>3562</v>
       </c>
     </row>
@@ -44201,7 +44212,7 @@
       <c r="A3373">
         <v>5609</v>
       </c>
-      <c r="B3373" s="84" t="s">
+      <c r="B3373" s="83" t="s">
         <v>3544</v>
       </c>
     </row>
@@ -44265,7 +44276,7 @@
       <c r="A3381">
         <v>5741</v>
       </c>
-      <c r="B3381" s="84" t="s">
+      <c r="B3381" s="83" t="s">
         <v>3548</v>
       </c>
     </row>
@@ -49930,8 +49941,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A827A58D-C8A4-4858-A89B-E853C083564F}">
   <dimension ref="A1:AK168"/>
   <sheetViews>
-    <sheetView topLeftCell="A37" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="L54" sqref="L54:L56"/>
+    <sheetView tabSelected="1" topLeftCell="A37" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C56" sqref="C56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
@@ -49951,28 +49962,28 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:37" ht="20.25">
-      <c r="A1" s="65" t="s">
+      <c r="A1" s="64" t="s">
         <v>2892</v>
       </c>
-      <c r="B1" s="65" t="s">
+      <c r="B1" s="64" t="s">
         <v>3360</v>
       </c>
-      <c r="C1" s="65" t="s">
+      <c r="C1" s="64" t="s">
         <v>2856</v>
       </c>
-      <c r="D1" s="65" t="s">
+      <c r="D1" s="64" t="s">
         <v>588</v>
       </c>
-      <c r="E1" s="65" t="s">
+      <c r="E1" s="64" t="s">
         <v>3374</v>
       </c>
-      <c r="F1" s="65" t="s">
+      <c r="F1" s="64" t="s">
         <v>2916</v>
       </c>
-      <c r="G1" s="65" t="s">
+      <c r="G1" s="64" t="s">
         <v>2858</v>
       </c>
-      <c r="H1" s="65" t="s">
+      <c r="H1" s="64" t="s">
         <v>2857</v>
       </c>
       <c r="I1" s="27" t="s">
@@ -49980,824 +49991,824 @@
       </c>
     </row>
     <row r="2" spans="1:37" ht="20.25">
-      <c r="A2" s="66" t="s">
+      <c r="A2" s="65" t="s">
         <v>2853</v>
       </c>
-      <c r="B2" s="65">
+      <c r="B2" s="64">
         <v>1</v>
       </c>
-      <c r="C2" s="67" t="s">
+      <c r="C2" s="66" t="s">
         <v>2843</v>
       </c>
-      <c r="D2" s="68" t="s">
+      <c r="D2" s="67" t="s">
         <v>2844</v>
       </c>
-      <c r="E2" s="68" t="s">
+      <c r="E2" s="67" t="s">
         <v>2853</v>
       </c>
-      <c r="F2" s="69" t="s">
+      <c r="F2" s="68" t="s">
         <v>2867</v>
       </c>
-      <c r="G2" s="69" t="s">
+      <c r="G2" s="68" t="s">
         <v>2878</v>
       </c>
-      <c r="H2" s="70" t="s">
+      <c r="H2" s="69" t="s">
         <v>2877</v>
       </c>
       <c r="I2" s="27"/>
       <c r="AK2" s="28"/>
     </row>
     <row r="3" spans="1:37" ht="30">
-      <c r="A3" s="66" t="s">
+      <c r="A3" s="65" t="s">
         <v>2853</v>
       </c>
-      <c r="B3" s="66">
+      <c r="B3" s="65">
         <v>2</v>
       </c>
-      <c r="C3" s="67" t="s">
+      <c r="C3" s="66" t="s">
         <v>2833</v>
       </c>
-      <c r="D3" s="68" t="s">
+      <c r="D3" s="67" t="s">
         <v>2834</v>
       </c>
-      <c r="E3" s="68" t="s">
+      <c r="E3" s="67" t="s">
         <v>2853</v>
       </c>
-      <c r="F3" s="69" t="s">
+      <c r="F3" s="68" t="s">
         <v>2859</v>
       </c>
-      <c r="G3" s="69" t="s">
+      <c r="G3" s="68" t="s">
         <v>2917</v>
       </c>
-      <c r="H3" s="70" t="s">
+      <c r="H3" s="69" t="s">
         <v>2862</v>
       </c>
       <c r="I3" s="27"/>
       <c r="AK3" s="28"/>
     </row>
     <row r="4" spans="1:37" ht="20.25">
-      <c r="A4" s="71" t="s">
+      <c r="A4" s="70" t="s">
         <v>2853</v>
       </c>
-      <c r="B4" s="65">
+      <c r="B4" s="64">
         <v>3</v>
       </c>
-      <c r="C4" s="67" t="s">
+      <c r="C4" s="66" t="s">
         <v>2871</v>
       </c>
-      <c r="D4" s="72" t="s">
+      <c r="D4" s="71" t="s">
         <v>3357</v>
       </c>
-      <c r="E4" s="72" t="s">
+      <c r="E4" s="71" t="s">
         <v>3376</v>
       </c>
-      <c r="F4" s="69" t="s">
+      <c r="F4" s="68" t="s">
         <v>2867</v>
       </c>
-      <c r="G4" s="69" t="s">
+      <c r="G4" s="68" t="s">
         <v>2873</v>
       </c>
-      <c r="H4" s="70" t="s">
+      <c r="H4" s="69" t="s">
         <v>2872</v>
       </c>
       <c r="I4" s="27"/>
       <c r="AK4" s="28"/>
     </row>
     <row r="5" spans="1:37" ht="20.25">
-      <c r="A5" s="71" t="s">
+      <c r="A5" s="70" t="s">
         <v>2853</v>
       </c>
-      <c r="B5" s="71">
+      <c r="B5" s="70">
         <v>4</v>
       </c>
-      <c r="C5" s="67" t="s">
+      <c r="C5" s="66" t="s">
         <v>2835</v>
       </c>
-      <c r="D5" s="68" t="s">
+      <c r="D5" s="67" t="s">
         <v>2836</v>
       </c>
-      <c r="E5" s="68" t="s">
+      <c r="E5" s="67" t="s">
         <v>2853</v>
       </c>
-      <c r="F5" s="69" t="s">
+      <c r="F5" s="68" t="s">
         <v>2859</v>
       </c>
-      <c r="G5" s="69" t="s">
+      <c r="G5" s="68" t="s">
         <v>2918</v>
       </c>
-      <c r="H5" s="70" t="s">
+      <c r="H5" s="69" t="s">
         <v>2860</v>
       </c>
       <c r="I5" s="27"/>
       <c r="AK5" s="28"/>
     </row>
     <row r="6" spans="1:37" ht="30">
-      <c r="A6" s="71" t="s">
+      <c r="A6" s="70" t="s">
         <v>2853</v>
       </c>
-      <c r="B6" s="71">
+      <c r="B6" s="70">
         <v>5</v>
       </c>
-      <c r="C6" s="66" t="s">
+      <c r="C6" s="65" t="s">
         <v>3424</v>
       </c>
-      <c r="D6" s="68" t="s">
+      <c r="D6" s="67" t="s">
         <v>3423</v>
       </c>
-      <c r="E6" s="68" t="s">
+      <c r="E6" s="67" t="s">
         <v>2853</v>
       </c>
-      <c r="F6" s="69" t="s">
+      <c r="F6" s="68" t="s">
         <v>2867</v>
       </c>
-      <c r="G6" s="73" t="s">
+      <c r="G6" s="72" t="s">
         <v>3377</v>
       </c>
-      <c r="H6" s="71" t="s">
+      <c r="H6" s="70" t="s">
         <v>3378</v>
       </c>
       <c r="I6" s="27"/>
       <c r="AK6" s="28"/>
     </row>
     <row r="7" spans="1:37" ht="30">
-      <c r="A7" s="71" t="s">
+      <c r="A7" s="70" t="s">
         <v>2853</v>
       </c>
-      <c r="B7" s="65">
+      <c r="B7" s="64">
         <v>6</v>
       </c>
-      <c r="C7" s="74" t="s">
+      <c r="C7" s="73" t="s">
         <v>2847</v>
       </c>
-      <c r="D7" s="68" t="s">
+      <c r="D7" s="67" t="s">
         <v>2848</v>
       </c>
-      <c r="E7" s="68" t="s">
+      <c r="E7" s="67" t="s">
         <v>2852</v>
       </c>
-      <c r="F7" s="69" t="s">
+      <c r="F7" s="68" t="s">
         <v>2867</v>
       </c>
-      <c r="G7" s="69" t="s">
+      <c r="G7" s="68" t="s">
         <v>2921</v>
       </c>
-      <c r="H7" s="70" t="s">
+      <c r="H7" s="69" t="s">
         <v>2930</v>
       </c>
       <c r="I7" s="27"/>
       <c r="AK7" s="28"/>
     </row>
     <row r="8" spans="1:37" ht="21" thickBot="1">
-      <c r="A8" s="66" t="s">
+      <c r="A8" s="65" t="s">
         <v>2852</v>
       </c>
-      <c r="B8" s="66">
+      <c r="B8" s="65">
         <v>11</v>
       </c>
-      <c r="C8" s="74" t="s">
+      <c r="C8" s="73" t="s">
         <v>2845</v>
       </c>
-      <c r="D8" s="68" t="s">
+      <c r="D8" s="67" t="s">
         <v>2846</v>
       </c>
-      <c r="E8" s="68" t="s">
+      <c r="E8" s="67" t="s">
         <v>2852</v>
       </c>
-      <c r="F8" s="69" t="s">
+      <c r="F8" s="68" t="s">
         <v>2859</v>
       </c>
-      <c r="G8" s="69" t="s">
+      <c r="G8" s="68" t="s">
         <v>2922</v>
       </c>
-      <c r="H8" s="70" t="s">
+      <c r="H8" s="69" t="s">
         <v>2931</v>
       </c>
       <c r="AK8" s="28"/>
     </row>
     <row r="9" spans="1:37" ht="21.75" thickTop="1" thickBot="1">
-      <c r="A9" s="66" t="s">
+      <c r="A9" s="65" t="s">
         <v>2852</v>
       </c>
-      <c r="B9" s="75">
+      <c r="B9" s="74">
         <v>12</v>
       </c>
-      <c r="C9" s="67" t="s">
+      <c r="C9" s="66" t="s">
         <v>2874</v>
       </c>
-      <c r="D9" s="72" t="s">
+      <c r="D9" s="71" t="s">
         <v>3359</v>
       </c>
-      <c r="E9" s="72" t="s">
+      <c r="E9" s="71" t="s">
         <v>2852</v>
       </c>
-      <c r="F9" s="69" t="s">
+      <c r="F9" s="68" t="s">
         <v>2867</v>
       </c>
-      <c r="G9" s="69" t="s">
+      <c r="G9" s="68" t="s">
         <v>2876</v>
       </c>
-      <c r="H9" s="70" t="s">
+      <c r="H9" s="69" t="s">
         <v>2875</v>
       </c>
       <c r="I9" s="27"/>
       <c r="AK9" s="28"/>
     </row>
     <row r="10" spans="1:37" ht="31.5" thickTop="1" thickBot="1">
-      <c r="A10" s="71" t="s">
+      <c r="A10" s="70" t="s">
         <v>2852</v>
       </c>
-      <c r="B10" s="65">
+      <c r="B10" s="64">
         <v>13</v>
       </c>
-      <c r="C10" s="74" t="s">
+      <c r="C10" s="73" t="s">
         <v>2847</v>
       </c>
-      <c r="D10" s="68" t="s">
+      <c r="D10" s="67" t="s">
         <v>2848</v>
       </c>
-      <c r="E10" s="68" t="s">
+      <c r="E10" s="67" t="s">
         <v>2852</v>
       </c>
-      <c r="F10" s="69" t="s">
+      <c r="F10" s="68" t="s">
         <v>2867</v>
       </c>
-      <c r="G10" s="69" t="s">
+      <c r="G10" s="68" t="s">
         <v>2921</v>
       </c>
-      <c r="H10" s="70" t="s">
+      <c r="H10" s="69" t="s">
         <v>2930</v>
       </c>
       <c r="I10" s="28"/>
       <c r="AK10" s="28"/>
     </row>
     <row r="11" spans="1:37" ht="31.5" thickTop="1" thickBot="1">
-      <c r="A11" s="71" t="s">
+      <c r="A11" s="70" t="s">
         <v>2852</v>
       </c>
-      <c r="B11" s="75">
+      <c r="B11" s="74">
         <v>14</v>
       </c>
-      <c r="C11" s="74" t="s">
+      <c r="C11" s="73" t="s">
         <v>2837</v>
       </c>
-      <c r="D11" s="68" t="s">
+      <c r="D11" s="67" t="s">
         <v>2838</v>
       </c>
-      <c r="E11" s="68" t="s">
+      <c r="E11" s="67" t="s">
         <v>2852</v>
       </c>
-      <c r="F11" s="69" t="s">
+      <c r="F11" s="68" t="s">
         <v>2867</v>
       </c>
-      <c r="G11" s="69" t="s">
+      <c r="G11" s="68" t="s">
         <v>2925</v>
       </c>
-      <c r="H11" s="70" t="s">
+      <c r="H11" s="69" t="s">
         <v>2932</v>
       </c>
       <c r="I11" s="28"/>
       <c r="AK11" s="28"/>
     </row>
     <row r="12" spans="1:37" ht="21" thickTop="1">
-      <c r="A12" s="71" t="s">
+      <c r="A12" s="70" t="s">
         <v>2852</v>
       </c>
-      <c r="B12" s="65">
+      <c r="B12" s="64">
         <v>15</v>
       </c>
-      <c r="C12" s="74" t="s">
+      <c r="C12" s="73" t="s">
         <v>2891</v>
       </c>
-      <c r="D12" s="68" t="s">
+      <c r="D12" s="67" t="s">
         <v>3372</v>
       </c>
-      <c r="E12" s="71" t="s">
+      <c r="E12" s="70" t="s">
         <v>2852</v>
       </c>
-      <c r="F12" s="69" t="s">
+      <c r="F12" s="68" t="s">
         <v>2879</v>
       </c>
-      <c r="G12" s="69" t="s">
+      <c r="G12" s="68" t="s">
         <v>2927</v>
       </c>
-      <c r="H12" s="70" t="s">
+      <c r="H12" s="69" t="s">
         <v>2940</v>
       </c>
       <c r="I12" s="28"/>
       <c r="AK12" s="28"/>
     </row>
     <row r="13" spans="1:37" ht="30">
-      <c r="A13" s="71" t="s">
+      <c r="A13" s="70" t="s">
         <v>2852</v>
       </c>
-      <c r="B13" s="65">
+      <c r="B13" s="64">
         <v>16</v>
       </c>
-      <c r="C13" s="67" t="s">
+      <c r="C13" s="66" t="s">
         <v>2864</v>
       </c>
-      <c r="D13" s="68" t="s">
+      <c r="D13" s="67" t="s">
         <v>3381</v>
       </c>
-      <c r="E13" s="71" t="s">
+      <c r="E13" s="70" t="s">
         <v>3380</v>
       </c>
-      <c r="F13" s="69" t="s">
+      <c r="F13" s="68" t="s">
         <v>2859</v>
       </c>
-      <c r="G13" s="69" t="s">
+      <c r="G13" s="68" t="s">
         <v>2866</v>
       </c>
-      <c r="H13" s="70" t="s">
+      <c r="H13" s="69" t="s">
         <v>2865</v>
       </c>
       <c r="I13" s="28"/>
     </row>
     <row r="14" spans="1:37" ht="20.25">
-      <c r="A14" s="71" t="s">
+      <c r="A14" s="70" t="s">
         <v>2852</v>
       </c>
       <c r="B14" s="19">
         <v>17</v>
       </c>
-      <c r="C14" s="66" t="s">
+      <c r="C14" s="65" t="s">
         <v>3430</v>
       </c>
-      <c r="D14" s="68" t="s">
+      <c r="D14" s="67" t="s">
         <v>3432</v>
       </c>
-      <c r="E14" s="71" t="s">
+      <c r="E14" s="70" t="s">
         <v>2852</v>
       </c>
-      <c r="F14" s="69" t="s">
+      <c r="F14" s="68" t="s">
         <v>2867</v>
       </c>
-      <c r="G14" s="73" t="s">
+      <c r="G14" s="72" t="s">
         <v>3377</v>
       </c>
-      <c r="H14" s="71" t="s">
+      <c r="H14" s="70" t="s">
         <v>3378</v>
       </c>
       <c r="I14" s="28"/>
     </row>
     <row r="15" spans="1:37" ht="20.25">
-      <c r="A15" s="71" t="s">
+      <c r="A15" s="70" t="s">
         <v>2852</v>
       </c>
       <c r="B15" s="19">
         <v>18</v>
       </c>
-      <c r="C15" s="66" t="s">
+      <c r="C15" s="65" t="s">
         <v>3429</v>
       </c>
-      <c r="D15" s="68" t="s">
+      <c r="D15" s="67" t="s">
         <v>3433</v>
       </c>
-      <c r="E15" s="71" t="s">
+      <c r="E15" s="70" t="s">
         <v>2852</v>
       </c>
-      <c r="F15" s="69" t="s">
+      <c r="F15" s="68" t="s">
         <v>2867</v>
       </c>
-      <c r="G15" s="73" t="s">
+      <c r="G15" s="72" t="s">
         <v>3377</v>
       </c>
-      <c r="H15" s="71" t="s">
+      <c r="H15" s="70" t="s">
         <v>3378</v>
       </c>
       <c r="I15" s="28"/>
     </row>
     <row r="16" spans="1:37" ht="20.25">
-      <c r="A16" s="71" t="s">
+      <c r="A16" s="70" t="s">
         <v>2852</v>
       </c>
       <c r="B16" s="19">
         <v>19</v>
       </c>
-      <c r="C16" s="66" t="s">
+      <c r="C16" s="65" t="s">
         <v>3431</v>
       </c>
-      <c r="D16" s="68" t="s">
+      <c r="D16" s="67" t="s">
         <v>3434</v>
       </c>
-      <c r="E16" s="71" t="s">
+      <c r="E16" s="70" t="s">
         <v>2852</v>
       </c>
-      <c r="F16" s="69" t="s">
+      <c r="F16" s="68" t="s">
         <v>2867</v>
       </c>
-      <c r="G16" s="73" t="s">
+      <c r="G16" s="72" t="s">
         <v>3377</v>
       </c>
-      <c r="H16" s="71" t="s">
+      <c r="H16" s="70" t="s">
         <v>3378</v>
       </c>
       <c r="I16" s="28"/>
     </row>
     <row r="17" spans="1:37" ht="20.25">
-      <c r="A17" s="66" t="s">
+      <c r="A17" s="65" t="s">
         <v>3</v>
       </c>
-      <c r="B17" s="66">
+      <c r="B17" s="65">
         <v>21</v>
       </c>
-      <c r="C17" s="74" t="s">
+      <c r="C17" s="73" t="s">
         <v>2904</v>
       </c>
-      <c r="D17" s="72" t="s">
+      <c r="D17" s="71" t="s">
         <v>2915</v>
       </c>
-      <c r="E17" s="71" t="s">
+      <c r="E17" s="70" t="s">
         <v>3375</v>
       </c>
-      <c r="F17" s="69" t="s">
+      <c r="F17" s="68" t="s">
         <v>2867</v>
       </c>
-      <c r="G17" s="69" t="s">
+      <c r="G17" s="68" t="s">
         <v>2905</v>
       </c>
-      <c r="H17" s="70" t="s">
+      <c r="H17" s="69" t="s">
         <v>2910</v>
       </c>
       <c r="I17" s="28"/>
       <c r="AK17" s="28"/>
     </row>
     <row r="18" spans="1:37" ht="20.25">
-      <c r="A18" s="66" t="s">
+      <c r="A18" s="65" t="s">
         <v>3</v>
       </c>
-      <c r="B18" s="66">
+      <c r="B18" s="65">
         <v>22</v>
       </c>
-      <c r="C18" s="74" t="s">
+      <c r="C18" s="73" t="s">
         <v>2906</v>
       </c>
-      <c r="D18" s="68" t="s">
+      <c r="D18" s="67" t="s">
         <v>2913</v>
       </c>
-      <c r="E18" s="71" t="s">
+      <c r="E18" s="70" t="s">
         <v>3375</v>
       </c>
-      <c r="F18" s="69" t="s">
+      <c r="F18" s="68" t="s">
         <v>2859</v>
       </c>
-      <c r="G18" s="69" t="s">
+      <c r="G18" s="68" t="s">
         <v>2907</v>
       </c>
-      <c r="H18" s="70" t="s">
+      <c r="H18" s="69" t="s">
         <v>2911</v>
       </c>
       <c r="I18" s="28"/>
       <c r="AK18" s="28"/>
     </row>
     <row r="19" spans="1:37" ht="20.25">
-      <c r="A19" s="66" t="s">
+      <c r="A19" s="65" t="s">
         <v>3</v>
       </c>
-      <c r="B19" s="66">
+      <c r="B19" s="65">
         <v>23</v>
       </c>
-      <c r="C19" s="74" t="s">
+      <c r="C19" s="73" t="s">
         <v>2901</v>
       </c>
-      <c r="D19" s="72" t="s">
+      <c r="D19" s="71" t="s">
         <v>2902</v>
       </c>
-      <c r="E19" s="71" t="s">
+      <c r="E19" s="70" t="s">
         <v>3375</v>
       </c>
-      <c r="F19" s="69" t="s">
+      <c r="F19" s="68" t="s">
         <v>2867</v>
       </c>
-      <c r="G19" s="69" t="s">
+      <c r="G19" s="68" t="s">
         <v>2900</v>
       </c>
-      <c r="H19" s="70" t="s">
+      <c r="H19" s="69" t="s">
         <v>2903</v>
       </c>
       <c r="I19" s="28"/>
       <c r="AK19" s="28"/>
     </row>
     <row r="20" spans="1:37" ht="20.25">
-      <c r="A20" s="66" t="s">
+      <c r="A20" s="65" t="s">
         <v>3</v>
       </c>
-      <c r="B20" s="66">
+      <c r="B20" s="65">
         <v>24</v>
       </c>
-      <c r="C20" s="74" t="s">
+      <c r="C20" s="73" t="s">
         <v>2908</v>
       </c>
-      <c r="D20" s="68" t="s">
+      <c r="D20" s="67" t="s">
         <v>2914</v>
       </c>
-      <c r="E20" s="71" t="s">
+      <c r="E20" s="70" t="s">
         <v>3375</v>
       </c>
-      <c r="F20" s="69" t="s">
+      <c r="F20" s="68" t="s">
         <v>2867</v>
       </c>
-      <c r="G20" s="69" t="s">
+      <c r="G20" s="68" t="s">
         <v>2909</v>
       </c>
-      <c r="H20" s="70" t="s">
+      <c r="H20" s="69" t="s">
         <v>2912</v>
       </c>
       <c r="I20" s="28"/>
     </row>
     <row r="21" spans="1:37" ht="30">
-      <c r="A21" s="71" t="s">
+      <c r="A21" s="70" t="s">
         <v>3</v>
       </c>
-      <c r="B21" s="65">
+      <c r="B21" s="64">
         <v>25</v>
       </c>
-      <c r="C21" s="67" t="s">
+      <c r="C21" s="66" t="s">
         <v>2864</v>
       </c>
-      <c r="D21" s="68" t="s">
+      <c r="D21" s="67" t="s">
         <v>2889</v>
       </c>
-      <c r="E21" s="71" t="s">
+      <c r="E21" s="70" t="s">
         <v>3380</v>
       </c>
-      <c r="F21" s="69" t="s">
+      <c r="F21" s="68" t="s">
         <v>2859</v>
       </c>
-      <c r="G21" s="69" t="s">
+      <c r="G21" s="68" t="s">
         <v>2866</v>
       </c>
-      <c r="H21" s="70" t="s">
+      <c r="H21" s="69" t="s">
         <v>2865</v>
       </c>
       <c r="I21" s="28"/>
     </row>
     <row r="22" spans="1:37" ht="20.25">
-      <c r="A22" s="66" t="s">
+      <c r="A22" s="65" t="s">
         <v>3</v>
       </c>
-      <c r="B22" s="66">
+      <c r="B22" s="65">
         <v>26</v>
       </c>
-      <c r="C22" s="74" t="s">
+      <c r="C22" s="73" t="s">
         <v>2897</v>
       </c>
-      <c r="D22" s="72" t="s">
+      <c r="D22" s="71" t="s">
         <v>2896</v>
       </c>
-      <c r="E22" s="71" t="s">
+      <c r="E22" s="70" t="s">
         <v>3375</v>
       </c>
-      <c r="F22" s="69" t="s">
+      <c r="F22" s="68" t="s">
         <v>2859</v>
       </c>
-      <c r="G22" s="69" t="s">
+      <c r="G22" s="68" t="s">
         <v>2895</v>
       </c>
-      <c r="H22" s="70" t="s">
+      <c r="H22" s="69" t="s">
         <v>2898</v>
       </c>
       <c r="I22" s="28"/>
     </row>
     <row r="23" spans="1:37" ht="20.25">
-      <c r="A23" s="66" t="s">
+      <c r="A23" s="65" t="s">
         <v>2890</v>
       </c>
-      <c r="B23" s="66">
+      <c r="B23" s="65">
         <v>31</v>
       </c>
-      <c r="C23" s="74" t="s">
+      <c r="C23" s="73" t="s">
         <v>2904</v>
       </c>
-      <c r="D23" s="72" t="s">
+      <c r="D23" s="71" t="s">
         <v>2915</v>
       </c>
-      <c r="E23" s="71" t="s">
+      <c r="E23" s="70" t="s">
         <v>3375</v>
       </c>
-      <c r="F23" s="69" t="s">
+      <c r="F23" s="68" t="s">
         <v>2867</v>
       </c>
-      <c r="G23" s="69" t="s">
+      <c r="G23" s="68" t="s">
         <v>2905</v>
       </c>
-      <c r="H23" s="70" t="s">
+      <c r="H23" s="69" t="s">
         <v>2910</v>
       </c>
       <c r="I23" s="28"/>
     </row>
     <row r="24" spans="1:37" ht="20.25">
-      <c r="A24" s="66" t="s">
+      <c r="A24" s="65" t="s">
         <v>2890</v>
       </c>
-      <c r="B24" s="66">
+      <c r="B24" s="65">
         <v>32</v>
       </c>
-      <c r="C24" s="74" t="s">
+      <c r="C24" s="73" t="s">
         <v>2906</v>
       </c>
-      <c r="D24" s="68" t="s">
+      <c r="D24" s="67" t="s">
         <v>2913</v>
       </c>
-      <c r="E24" s="71" t="s">
+      <c r="E24" s="70" t="s">
         <v>3375</v>
       </c>
-      <c r="F24" s="69" t="s">
+      <c r="F24" s="68" t="s">
         <v>2859</v>
       </c>
-      <c r="G24" s="69" t="s">
+      <c r="G24" s="68" t="s">
         <v>2907</v>
       </c>
-      <c r="H24" s="70" t="s">
+      <c r="H24" s="69" t="s">
         <v>2911</v>
       </c>
       <c r="I24" s="28"/>
     </row>
     <row r="25" spans="1:37" ht="20.25">
-      <c r="A25" s="66" t="s">
+      <c r="A25" s="65" t="s">
         <v>2890</v>
       </c>
-      <c r="B25" s="66">
+      <c r="B25" s="65">
         <v>33</v>
       </c>
-      <c r="C25" s="74" t="s">
+      <c r="C25" s="73" t="s">
         <v>2901</v>
       </c>
-      <c r="D25" s="72" t="s">
+      <c r="D25" s="71" t="s">
         <v>2902</v>
       </c>
-      <c r="E25" s="71" t="s">
+      <c r="E25" s="70" t="s">
         <v>3375</v>
       </c>
-      <c r="F25" s="69" t="s">
+      <c r="F25" s="68" t="s">
         <v>2867</v>
       </c>
-      <c r="G25" s="69" t="s">
+      <c r="G25" s="68" t="s">
         <v>2900</v>
       </c>
-      <c r="H25" s="70" t="s">
+      <c r="H25" s="69" t="s">
         <v>2903</v>
       </c>
       <c r="I25" s="28"/>
     </row>
     <row r="26" spans="1:37" ht="20.25">
-      <c r="A26" s="66" t="s">
+      <c r="A26" s="65" t="s">
         <v>2890</v>
       </c>
-      <c r="B26" s="66">
+      <c r="B26" s="65">
         <v>34</v>
       </c>
-      <c r="C26" s="74" t="s">
+      <c r="C26" s="73" t="s">
         <v>2908</v>
       </c>
-      <c r="D26" s="68" t="s">
+      <c r="D26" s="67" t="s">
         <v>2914</v>
       </c>
-      <c r="E26" s="71" t="s">
+      <c r="E26" s="70" t="s">
         <v>3375</v>
       </c>
-      <c r="F26" s="69" t="s">
+      <c r="F26" s="68" t="s">
         <v>2867</v>
       </c>
-      <c r="G26" s="69" t="s">
+      <c r="G26" s="68" t="s">
         <v>2909</v>
       </c>
-      <c r="H26" s="70" t="s">
+      <c r="H26" s="69" t="s">
         <v>2912</v>
       </c>
       <c r="I26" s="28"/>
     </row>
     <row r="27" spans="1:37" ht="30">
-      <c r="A27" s="71" t="s">
+      <c r="A27" s="70" t="s">
         <v>2890</v>
       </c>
-      <c r="B27" s="65">
+      <c r="B27" s="64">
         <v>35</v>
       </c>
-      <c r="C27" s="67" t="s">
+      <c r="C27" s="66" t="s">
         <v>2864</v>
       </c>
-      <c r="D27" s="68" t="s">
+      <c r="D27" s="67" t="s">
         <v>2889</v>
       </c>
-      <c r="E27" s="71" t="s">
+      <c r="E27" s="70" t="s">
         <v>3380</v>
       </c>
-      <c r="F27" s="69" t="s">
+      <c r="F27" s="68" t="s">
         <v>2859</v>
       </c>
-      <c r="G27" s="69" t="s">
+      <c r="G27" s="68" t="s">
         <v>2866</v>
       </c>
-      <c r="H27" s="70" t="s">
+      <c r="H27" s="69" t="s">
         <v>2865</v>
       </c>
       <c r="I27" s="28"/>
     </row>
     <row r="28" spans="1:37" ht="20.25">
-      <c r="A28" s="66" t="s">
+      <c r="A28" s="65" t="s">
         <v>2890</v>
       </c>
-      <c r="B28" s="66">
+      <c r="B28" s="65">
         <v>36</v>
       </c>
-      <c r="C28" s="74" t="s">
+      <c r="C28" s="73" t="s">
         <v>2897</v>
       </c>
-      <c r="D28" s="72" t="s">
+      <c r="D28" s="71" t="s">
         <v>2896</v>
       </c>
-      <c r="E28" s="71" t="s">
+      <c r="E28" s="70" t="s">
         <v>3375</v>
       </c>
-      <c r="F28" s="69" t="s">
+      <c r="F28" s="68" t="s">
         <v>2859</v>
       </c>
-      <c r="G28" s="69" t="s">
+      <c r="G28" s="68" t="s">
         <v>2895</v>
       </c>
-      <c r="H28" s="70" t="s">
+      <c r="H28" s="69" t="s">
         <v>2898</v>
       </c>
       <c r="I28" s="28"/>
     </row>
     <row r="29" spans="1:37" ht="30">
-      <c r="A29" s="71" t="s">
+      <c r="A29" s="70" t="s">
         <v>3379</v>
       </c>
       <c r="B29" s="19">
         <v>41</v>
       </c>
-      <c r="C29" s="66" t="s">
+      <c r="C29" s="65" t="s">
         <v>3425</v>
       </c>
-      <c r="D29" s="72" t="s">
+      <c r="D29" s="71" t="s">
         <v>3422</v>
       </c>
-      <c r="E29" s="71" t="s">
+      <c r="E29" s="70" t="s">
         <v>3379</v>
       </c>
-      <c r="F29" s="69" t="s">
+      <c r="F29" s="68" t="s">
         <v>2867</v>
       </c>
-      <c r="G29" s="73" t="s">
+      <c r="G29" s="72" t="s">
         <v>3377</v>
       </c>
-      <c r="H29" s="71" t="s">
+      <c r="H29" s="70" t="s">
         <v>3378</v>
       </c>
       <c r="I29" s="28"/>
     </row>
     <row r="30" spans="1:37" ht="30">
-      <c r="A30" s="71" t="s">
+      <c r="A30" s="70" t="s">
         <v>3379</v>
       </c>
       <c r="B30" s="19">
         <v>42</v>
       </c>
-      <c r="C30" s="66" t="s">
+      <c r="C30" s="65" t="s">
         <v>3426</v>
       </c>
-      <c r="D30" s="72" t="s">
+      <c r="D30" s="71" t="s">
         <v>3422</v>
       </c>
-      <c r="E30" s="71" t="s">
+      <c r="E30" s="70" t="s">
         <v>3379</v>
       </c>
-      <c r="F30" s="69" t="s">
+      <c r="F30" s="68" t="s">
         <v>2867</v>
       </c>
-      <c r="G30" s="73" t="s">
+      <c r="G30" s="72" t="s">
         <v>3377</v>
       </c>
-      <c r="H30" s="71" t="s">
+      <c r="H30" s="70" t="s">
         <v>3378</v>
       </c>
       <c r="I30" s="28"/>
     </row>
     <row r="31" spans="1:37" ht="30">
-      <c r="A31" s="71" t="s">
+      <c r="A31" s="70" t="s">
         <v>3379</v>
       </c>
       <c r="B31" s="19">
         <v>43</v>
       </c>
-      <c r="C31" s="66" t="s">
+      <c r="C31" s="65" t="s">
         <v>3564</v>
       </c>
-      <c r="D31" s="72" t="s">
+      <c r="D31" s="71" t="s">
         <v>3422</v>
       </c>
-      <c r="E31" s="71" t="s">
+      <c r="E31" s="70" t="s">
         <v>3379</v>
       </c>
-      <c r="F31" s="69" t="s">
+      <c r="F31" s="68" t="s">
         <v>2867</v>
       </c>
-      <c r="G31" s="73" t="s">
+      <c r="G31" s="72" t="s">
         <v>3377</v>
       </c>
-      <c r="H31" s="71" t="s">
+      <c r="H31" s="70" t="s">
         <v>3378</v>
       </c>
       <c r="I31" s="28"/>
@@ -50807,217 +50818,217 @@
       </c>
     </row>
     <row r="32" spans="1:37" ht="20.25">
-      <c r="A32" s="66" t="s">
+      <c r="A32" s="65" t="s">
         <v>2851</v>
       </c>
-      <c r="B32" s="66">
+      <c r="B32" s="65">
         <v>51</v>
       </c>
-      <c r="C32" s="74" t="s">
+      <c r="C32" s="73" t="s">
         <v>2849</v>
       </c>
-      <c r="D32" s="68" t="s">
+      <c r="D32" s="67" t="s">
         <v>2850</v>
       </c>
-      <c r="E32" s="68" t="s">
+      <c r="E32" s="67" t="s">
         <v>2851</v>
       </c>
-      <c r="F32" s="69" t="s">
+      <c r="F32" s="68" t="s">
         <v>2867</v>
       </c>
-      <c r="G32" s="69" t="s">
+      <c r="G32" s="68" t="s">
         <v>2920</v>
       </c>
-      <c r="H32" s="70" t="s">
+      <c r="H32" s="69" t="s">
         <v>2934</v>
       </c>
       <c r="I32" s="28"/>
     </row>
     <row r="33" spans="1:12" ht="20.25">
-      <c r="A33" s="66" t="s">
+      <c r="A33" s="65" t="s">
         <v>2851</v>
       </c>
-      <c r="B33" s="66">
+      <c r="B33" s="65">
         <v>52</v>
       </c>
-      <c r="C33" s="74" t="s">
+      <c r="C33" s="73" t="s">
         <v>2841</v>
       </c>
-      <c r="D33" s="68" t="s">
+      <c r="D33" s="67" t="s">
         <v>2842</v>
       </c>
-      <c r="E33" s="68" t="s">
+      <c r="E33" s="67" t="s">
         <v>2851</v>
       </c>
-      <c r="F33" s="69" t="s">
+      <c r="F33" s="68" t="s">
         <v>2859</v>
       </c>
-      <c r="G33" s="69" t="s">
+      <c r="G33" s="68" t="s">
         <v>2923</v>
       </c>
-      <c r="H33" s="70" t="s">
+      <c r="H33" s="69" t="s">
         <v>2929</v>
       </c>
       <c r="I33" s="28"/>
     </row>
     <row r="34" spans="1:12" ht="30">
-      <c r="A34" s="66" t="s">
+      <c r="A34" s="65" t="s">
         <v>2851</v>
       </c>
-      <c r="B34" s="66">
+      <c r="B34" s="65">
         <v>53</v>
       </c>
-      <c r="C34" s="74" t="s">
+      <c r="C34" s="73" t="s">
         <v>2883</v>
       </c>
-      <c r="D34" s="68" t="s">
+      <c r="D34" s="67" t="s">
         <v>3369</v>
       </c>
-      <c r="E34" s="68" t="s">
+      <c r="E34" s="67" t="s">
         <v>2851</v>
       </c>
-      <c r="F34" s="69" t="s">
+      <c r="F34" s="68" t="s">
         <v>2859</v>
       </c>
-      <c r="G34" s="69" t="s">
+      <c r="G34" s="68" t="s">
         <v>2926</v>
       </c>
-      <c r="H34" s="70" t="s">
+      <c r="H34" s="69" t="s">
         <v>2936</v>
       </c>
       <c r="I34" s="28"/>
     </row>
     <row r="35" spans="1:12" ht="30">
-      <c r="A35" s="66" t="s">
+      <c r="A35" s="65" t="s">
         <v>2851</v>
       </c>
-      <c r="B35" s="65">
+      <c r="B35" s="64">
         <v>54</v>
       </c>
-      <c r="C35" s="74" t="s">
+      <c r="C35" s="73" t="s">
         <v>2893</v>
       </c>
-      <c r="D35" s="72" t="s">
+      <c r="D35" s="71" t="s">
         <v>3371</v>
       </c>
-      <c r="E35" s="72" t="s">
+      <c r="E35" s="71" t="s">
         <v>2851</v>
       </c>
-      <c r="F35" s="69" t="s">
+      <c r="F35" s="68" t="s">
         <v>2859</v>
       </c>
-      <c r="G35" s="69" t="s">
+      <c r="G35" s="68" t="s">
         <v>2894</v>
       </c>
-      <c r="H35" s="70" t="s">
+      <c r="H35" s="69" t="s">
         <v>2899</v>
       </c>
       <c r="I35" s="28"/>
     </row>
     <row r="36" spans="1:12" ht="30">
-      <c r="A36" s="71" t="s">
+      <c r="A36" s="70" t="s">
         <v>2851</v>
       </c>
       <c r="B36" s="9">
         <v>55</v>
       </c>
-      <c r="C36" s="74" t="s">
+      <c r="C36" s="73" t="s">
         <v>2885</v>
       </c>
-      <c r="D36" s="68" t="s">
+      <c r="D36" s="67" t="s">
         <v>2884</v>
       </c>
-      <c r="E36" s="68" t="s">
+      <c r="E36" s="67" t="s">
         <v>2851</v>
       </c>
-      <c r="F36" s="69" t="s">
+      <c r="F36" s="68" t="s">
         <v>2867</v>
       </c>
-      <c r="G36" s="69" t="s">
+      <c r="G36" s="68" t="s">
         <v>2926</v>
       </c>
-      <c r="H36" s="70" t="s">
+      <c r="H36" s="69" t="s">
         <v>2937</v>
       </c>
       <c r="I36" s="28"/>
     </row>
     <row r="37" spans="1:12" ht="20.25">
-      <c r="A37" s="71" t="s">
+      <c r="A37" s="70" t="s">
         <v>2851</v>
       </c>
-      <c r="B37" s="65">
+      <c r="B37" s="64">
         <v>56</v>
       </c>
-      <c r="C37" s="67" t="s">
+      <c r="C37" s="66" t="s">
         <v>2871</v>
       </c>
-      <c r="D37" s="72" t="s">
+      <c r="D37" s="71" t="s">
         <v>3357</v>
       </c>
-      <c r="E37" s="72" t="s">
+      <c r="E37" s="71" t="s">
         <v>3376</v>
       </c>
-      <c r="F37" s="69" t="s">
+      <c r="F37" s="68" t="s">
         <v>2867</v>
       </c>
-      <c r="G37" s="69" t="s">
+      <c r="G37" s="68" t="s">
         <v>2873</v>
       </c>
-      <c r="H37" s="70" t="s">
+      <c r="H37" s="69" t="s">
         <v>2872</v>
       </c>
       <c r="I37" s="28"/>
     </row>
     <row r="38" spans="1:12" ht="30">
-      <c r="A38" s="71" t="s">
+      <c r="A38" s="70" t="s">
         <v>2851</v>
       </c>
-      <c r="B38" s="65">
+      <c r="B38" s="64">
         <v>57</v>
       </c>
-      <c r="C38" s="74" t="s">
+      <c r="C38" s="73" t="s">
         <v>2839</v>
       </c>
-      <c r="D38" s="68" t="s">
+      <c r="D38" s="67" t="s">
         <v>2840</v>
       </c>
-      <c r="E38" s="68" t="s">
+      <c r="E38" s="67" t="s">
         <v>2851</v>
       </c>
-      <c r="F38" s="69" t="s">
+      <c r="F38" s="68" t="s">
         <v>2867</v>
       </c>
-      <c r="G38" s="69" t="s">
+      <c r="G38" s="68" t="s">
         <v>2924</v>
       </c>
-      <c r="H38" s="70" t="s">
+      <c r="H38" s="69" t="s">
         <v>2935</v>
       </c>
       <c r="I38" s="28"/>
     </row>
     <row r="39" spans="1:12" ht="30">
-      <c r="A39" s="71" t="s">
+      <c r="A39" s="70" t="s">
         <v>2851</v>
       </c>
-      <c r="B39" s="65">
+      <c r="B39" s="64">
         <v>58</v>
       </c>
-      <c r="C39" s="74" t="s">
+      <c r="C39" s="73" t="s">
         <v>2854</v>
       </c>
-      <c r="D39" s="68" t="s">
+      <c r="D39" s="67" t="s">
         <v>3373</v>
       </c>
-      <c r="E39" s="68" t="s">
+      <c r="E39" s="67" t="s">
         <v>2851</v>
       </c>
-      <c r="F39" s="69" t="s">
+      <c r="F39" s="68" t="s">
         <v>2867</v>
       </c>
-      <c r="G39" s="69" t="s">
+      <c r="G39" s="68" t="s">
         <v>2919</v>
       </c>
-      <c r="H39" s="70" t="s">
+      <c r="H39" s="69" t="s">
         <v>2933</v>
       </c>
       <c r="J39">
@@ -51028,29 +51039,29 @@
         <v>3999</v>
       </c>
     </row>
-    <row r="40" spans="1:12" ht="90.75">
-      <c r="A40" s="72" t="s">
+    <row r="40" spans="1:12" ht="105.75">
+      <c r="A40" s="71" t="s">
         <v>3383</v>
       </c>
-      <c r="B40" s="71">
+      <c r="B40" s="70">
         <v>62</v>
       </c>
-      <c r="C40" s="66" t="s">
+      <c r="C40" s="65" t="s">
         <v>3427</v>
       </c>
-      <c r="D40" s="87" t="s">
-        <v>4054</v>
-      </c>
-      <c r="E40" s="72" t="s">
+      <c r="D40" s="86" t="s">
+        <v>4070</v>
+      </c>
+      <c r="E40" s="71" t="s">
         <v>3383</v>
       </c>
-      <c r="F40" s="69" t="s">
+      <c r="F40" s="68" t="s">
         <v>2867</v>
       </c>
-      <c r="G40" s="73" t="s">
+      <c r="G40" s="72" t="s">
         <v>3377</v>
       </c>
-      <c r="H40" s="71" t="s">
+      <c r="H40" s="70" t="s">
         <v>3378</v>
       </c>
       <c r="I40" s="27" t="s">
@@ -51060,34 +51071,34 @@
         <f>LEN(I40)</f>
         <v>16</v>
       </c>
-      <c r="L40" s="85" t="str">
+      <c r="L40" s="84" t="str">
         <f>"#define "&amp;I40&amp;" "&amp;REPT(" ",$J$39-J40)&amp;RIGHT(TEXT(B40,"    #"),3)&amp;" // "&amp;RIGHT(LEFT(D40,LEN(D40)-1),LEN(D40)-1-FIND("""",D40))</f>
-        <v>#define mEFCT_UNIQ_INTRO               62 // Welcome to RBG configuration! Your call is important to us. To go forward to next step or to cycle through choices, always press trigger by itself. To go back, press trigger plus Yellow, Green or Black button. To exit configuration, press trigger plus Blue button.</v>
+        <v>#define mEFCT_UNIQ_INTRO               62 // Welcome to FOOF RBG configuration! Your call is important to us. Press trigger by itself to go forward to next step or to cycle through choices To select a choice, press trigger plus any combination of Yellow, Green or Black button. To exit configuration, press trigger plus Blue button.</v>
       </c>
     </row>
     <row r="41" spans="1:12" ht="45">
-      <c r="A41" s="72" t="s">
+      <c r="A41" s="71" t="s">
         <v>3383</v>
       </c>
-      <c r="B41" s="71">
+      <c r="B41" s="70">
         <v>63</v>
       </c>
-      <c r="C41" s="89" t="s">
+      <c r="C41" s="88" t="s">
         <v>3428</v>
       </c>
-      <c r="D41" s="68" t="s">
+      <c r="D41" s="67" t="s">
         <v>3419</v>
       </c>
-      <c r="E41" s="72" t="s">
+      <c r="E41" s="71" t="s">
         <v>3383</v>
       </c>
-      <c r="F41" s="69" t="s">
+      <c r="F41" s="68" t="s">
         <v>2867</v>
       </c>
-      <c r="G41" s="73" t="s">
+      <c r="G41" s="72" t="s">
         <v>3377</v>
       </c>
-      <c r="H41" s="71" t="s">
+      <c r="H41" s="70" t="s">
         <v>3378</v>
       </c>
       <c r="I41" s="27" t="s">
@@ -51097,34 +51108,34 @@
         <f t="shared" ref="J41:J56" si="0">LEN(I41)</f>
         <v>20</v>
       </c>
-      <c r="L41" s="85" t="str">
+      <c r="L41" s="84" t="str">
         <f t="shared" ref="L41:L52" si="1">"#define "&amp;I41&amp;" "&amp;REPT(" ",$J$39-J41)&amp;RIGHT(TEXT(B41,"    #"),3)&amp;" // "&amp;RIGHT(LEFT(D41,LEN(D41)-1),LEN(D41)-1-FIND("""",D41))</f>
         <v>#define mEFCT_UNIQ_SND_INSTR           63 // Press just trigger to cycle through sound choices, trigger + any color to choose the sound.</v>
       </c>
     </row>
     <row r="42" spans="1:12" ht="45">
-      <c r="A42" s="72" t="s">
+      <c r="A42" s="71" t="s">
         <v>3383</v>
       </c>
-      <c r="B42" s="71">
+      <c r="B42" s="70">
         <v>64</v>
       </c>
-      <c r="C42" s="89" t="s">
+      <c r="C42" s="88" t="s">
         <v>3973</v>
       </c>
-      <c r="D42" s="68" t="s">
+      <c r="D42" s="67" t="s">
         <v>3420</v>
       </c>
-      <c r="E42" s="72" t="s">
+      <c r="E42" s="71" t="s">
         <v>3383</v>
       </c>
-      <c r="F42" s="69" t="s">
+      <c r="F42" s="68" t="s">
         <v>2867</v>
       </c>
-      <c r="G42" s="73" t="s">
+      <c r="G42" s="72" t="s">
         <v>3377</v>
       </c>
-      <c r="H42" s="71" t="s">
+      <c r="H42" s="70" t="s">
         <v>3378</v>
       </c>
       <c r="I42" s="27" t="s">
@@ -51134,34 +51145,34 @@
         <f t="shared" si="0"/>
         <v>20</v>
       </c>
-      <c r="L42" s="85" t="str">
+      <c r="L42" s="84" t="str">
         <f t="shared" si="1"/>
         <v>#define mEFCT_UNIQ_LED_INSTR           64 // Press just trigger to cycle through LED pattern choices, trigger + any color to choose the LED Pattern.</v>
       </c>
     </row>
     <row r="43" spans="1:12" ht="45">
-      <c r="A43" s="72" t="s">
+      <c r="A43" s="71" t="s">
         <v>3383</v>
       </c>
-      <c r="B43" s="71">
+      <c r="B43" s="70">
         <v>65</v>
       </c>
-      <c r="C43" s="89" t="s">
+      <c r="C43" s="88" t="s">
         <v>3974</v>
       </c>
-      <c r="D43" s="68" t="s">
+      <c r="D43" s="67" t="s">
         <v>3421</v>
       </c>
-      <c r="E43" s="72" t="s">
+      <c r="E43" s="71" t="s">
         <v>3383</v>
       </c>
-      <c r="F43" s="69" t="s">
+      <c r="F43" s="68" t="s">
         <v>2867</v>
       </c>
-      <c r="G43" s="73" t="s">
+      <c r="G43" s="72" t="s">
         <v>3377</v>
       </c>
-      <c r="H43" s="71" t="s">
+      <c r="H43" s="70" t="s">
         <v>3378</v>
       </c>
       <c r="I43" s="27" t="s">
@@ -51171,34 +51182,34 @@
         <f t="shared" si="0"/>
         <v>21</v>
       </c>
-      <c r="L43" s="85" t="str">
+      <c r="L43" s="84" t="str">
         <f t="shared" si="1"/>
         <v>#define mEFCT_UNIQ_OTHR_INSTR          65 // Press just trigger to cycle through a list of other choices, trigger + any color to choose the other choice.</v>
       </c>
     </row>
     <row r="44" spans="1:12" ht="45">
-      <c r="A44" s="72" t="s">
+      <c r="A44" s="71" t="s">
         <v>3383</v>
       </c>
-      <c r="B44" s="71">
+      <c r="B44" s="70">
         <v>66</v>
       </c>
-      <c r="C44" s="89" t="s">
+      <c r="C44" s="88" t="s">
         <v>3966</v>
       </c>
-      <c r="D44" s="68" t="s">
+      <c r="D44" s="67" t="s">
         <v>3975</v>
       </c>
-      <c r="E44" s="72" t="s">
+      <c r="E44" s="71" t="s">
         <v>3383</v>
       </c>
-      <c r="F44" s="69" t="s">
+      <c r="F44" s="68" t="s">
         <v>2867</v>
       </c>
-      <c r="G44" s="73" t="s">
+      <c r="G44" s="72" t="s">
         <v>3377</v>
       </c>
-      <c r="H44" s="71" t="s">
+      <c r="H44" s="70" t="s">
         <v>3378</v>
       </c>
       <c r="I44" s="27" t="s">
@@ -51208,34 +51219,34 @@
         <f t="shared" si="0"/>
         <v>29</v>
       </c>
-      <c r="L44" s="85" t="str">
+      <c r="L44" s="84" t="str">
         <f t="shared" si="1"/>
         <v>#define mEFCT_UNIQ_TYPE_CHOICES_INSTR  66 // Press just trigger to cycle through effect TYPE choices, trigger + any color to choose the effect TYPE.</v>
       </c>
     </row>
     <row r="45" spans="1:12" ht="30">
-      <c r="A45" s="72" t="s">
+      <c r="A45" s="71" t="s">
         <v>3383</v>
       </c>
-      <c r="B45" s="71">
+      <c r="B45" s="70">
         <v>71</v>
       </c>
-      <c r="C45" s="89" t="s">
+      <c r="C45" s="88" t="s">
         <v>3967</v>
       </c>
-      <c r="D45" s="68" t="s">
+      <c r="D45" s="67" t="s">
         <v>3985</v>
       </c>
-      <c r="E45" s="72" t="s">
+      <c r="E45" s="71" t="s">
         <v>3383</v>
       </c>
-      <c r="F45" s="69" t="s">
+      <c r="F45" s="68" t="s">
         <v>2867</v>
       </c>
-      <c r="G45" s="73" t="s">
+      <c r="G45" s="72" t="s">
         <v>3377</v>
       </c>
-      <c r="H45" s="71" t="s">
+      <c r="H45" s="70" t="s">
         <v>3378</v>
       </c>
       <c r="I45" s="27" t="s">
@@ -51245,34 +51256,34 @@
         <f t="shared" si="0"/>
         <v>19</v>
       </c>
-      <c r="L45" s="85" t="str">
+      <c r="L45" s="84" t="str">
         <f t="shared" si="1"/>
         <v>#define mEFCT_UNIQ_CHARGEUP            71 // Effect typeCHARGE-UP FOR SHOOTING. Trigger alone for next type.</v>
       </c>
     </row>
     <row r="46" spans="1:12" ht="30">
-      <c r="A46" s="72" t="s">
+      <c r="A46" s="71" t="s">
         <v>3383</v>
       </c>
-      <c r="B46" s="71">
+      <c r="B46" s="70">
         <v>72</v>
       </c>
-      <c r="C46" s="89" t="s">
+      <c r="C46" s="88" t="s">
         <v>3968</v>
       </c>
-      <c r="D46" s="68" t="s">
+      <c r="D46" s="67" t="s">
         <v>3986</v>
       </c>
-      <c r="E46" s="72" t="s">
+      <c r="E46" s="71" t="s">
         <v>3383</v>
       </c>
-      <c r="F46" s="69" t="s">
+      <c r="F46" s="68" t="s">
         <v>2867</v>
       </c>
-      <c r="G46" s="73" t="s">
+      <c r="G46" s="72" t="s">
         <v>3377</v>
       </c>
-      <c r="H46" s="71" t="s">
+      <c r="H46" s="70" t="s">
         <v>3378</v>
       </c>
       <c r="I46" s="27" t="s">
@@ -51282,34 +51293,34 @@
         <f t="shared" si="0"/>
         <v>19</v>
       </c>
-      <c r="L46" s="85" t="str">
+      <c r="L46" s="84" t="str">
         <f t="shared" si="1"/>
         <v>#define mEFCT_UNIQ_SHOOTING            72 // Effect type SHOOTING. Trigger alone for next type.</v>
       </c>
     </row>
     <row r="47" spans="1:12" ht="30">
-      <c r="A47" s="72" t="s">
+      <c r="A47" s="71" t="s">
         <v>3383</v>
       </c>
-      <c r="B47" s="71">
+      <c r="B47" s="70">
         <v>73</v>
       </c>
-      <c r="C47" s="89" t="s">
+      <c r="C47" s="88" t="s">
         <v>3969</v>
       </c>
-      <c r="D47" s="68" t="s">
+      <c r="D47" s="67" t="s">
         <v>3987</v>
       </c>
-      <c r="E47" s="72" t="s">
+      <c r="E47" s="71" t="s">
         <v>3383</v>
       </c>
-      <c r="F47" s="69" t="s">
+      <c r="F47" s="68" t="s">
         <v>2867</v>
       </c>
-      <c r="G47" s="73" t="s">
+      <c r="G47" s="72" t="s">
         <v>3377</v>
       </c>
-      <c r="H47" s="71" t="s">
+      <c r="H47" s="70" t="s">
         <v>3378</v>
       </c>
       <c r="I47" s="27" t="s">
@@ -51319,34 +51330,34 @@
         <f t="shared" si="0"/>
         <v>21</v>
       </c>
-      <c r="L47" s="85" t="str">
+      <c r="L47" s="84" t="str">
         <f t="shared" si="1"/>
         <v>#define mEFCT_UNIQ_OPENBARREL          73 // Effect type OPEN BARREL. Trigger alone for next type.</v>
       </c>
     </row>
     <row r="48" spans="1:12" ht="30">
-      <c r="A48" s="72" t="s">
+      <c r="A48" s="71" t="s">
         <v>3383</v>
       </c>
-      <c r="B48" s="71">
+      <c r="B48" s="70">
         <v>74</v>
       </c>
-      <c r="C48" s="89" t="s">
+      <c r="C48" s="88" t="s">
         <v>3970</v>
       </c>
-      <c r="D48" s="68" t="s">
+      <c r="D48" s="67" t="s">
         <v>3988</v>
       </c>
-      <c r="E48" s="72" t="s">
+      <c r="E48" s="71" t="s">
         <v>3383</v>
       </c>
-      <c r="F48" s="69" t="s">
+      <c r="F48" s="68" t="s">
         <v>2867</v>
       </c>
-      <c r="G48" s="73" t="s">
+      <c r="G48" s="72" t="s">
         <v>3377</v>
       </c>
-      <c r="H48" s="71" t="s">
+      <c r="H48" s="70" t="s">
         <v>3378</v>
       </c>
       <c r="I48" s="27" t="s">
@@ -51356,34 +51367,34 @@
         <f t="shared" si="0"/>
         <v>19</v>
       </c>
-      <c r="L48" s="85" t="str">
+      <c r="L48" s="84" t="str">
         <f t="shared" si="1"/>
         <v>#define mEFCT_UNIQ_LOCKLOAD            74 // Effect type LOCK-AND-LOAD. Trigger alone for next type.</v>
       </c>
     </row>
     <row r="49" spans="1:18" ht="30">
-      <c r="A49" s="72" t="s">
+      <c r="A49" s="71" t="s">
         <v>3383</v>
       </c>
-      <c r="B49" s="71">
+      <c r="B49" s="70">
         <v>75</v>
       </c>
-      <c r="C49" s="89" t="s">
+      <c r="C49" s="88" t="s">
         <v>3971</v>
       </c>
-      <c r="D49" s="68" t="s">
+      <c r="D49" s="67" t="s">
         <v>3989</v>
       </c>
-      <c r="E49" s="72" t="s">
+      <c r="E49" s="71" t="s">
         <v>3383</v>
       </c>
-      <c r="F49" s="69" t="s">
+      <c r="F49" s="68" t="s">
         <v>2867</v>
       </c>
-      <c r="G49" s="73" t="s">
+      <c r="G49" s="72" t="s">
         <v>3377</v>
       </c>
-      <c r="H49" s="71" t="s">
+      <c r="H49" s="70" t="s">
         <v>3378</v>
       </c>
       <c r="I49" s="27" t="s">
@@ -51393,34 +51404,34 @@
         <f t="shared" si="0"/>
         <v>18</v>
       </c>
-      <c r="L49" s="85" t="str">
+      <c r="L49" s="84" t="str">
         <f t="shared" si="1"/>
         <v>#define mEFCT_UNIQ_POWERON             75 // Effect type POWER-ON. Trigger alone for next type.</v>
       </c>
     </row>
     <row r="50" spans="1:18" ht="30">
-      <c r="A50" s="72" t="s">
+      <c r="A50" s="71" t="s">
         <v>3383</v>
       </c>
-      <c r="B50" s="71">
+      <c r="B50" s="70">
         <v>76</v>
       </c>
-      <c r="C50" s="89" t="s">
+      <c r="C50" s="88" t="s">
         <v>3972</v>
       </c>
-      <c r="D50" s="68" t="s">
+      <c r="D50" s="67" t="s">
         <v>3990</v>
       </c>
-      <c r="E50" s="72" t="s">
+      <c r="E50" s="71" t="s">
         <v>3383</v>
       </c>
-      <c r="F50" s="69" t="s">
+      <c r="F50" s="68" t="s">
         <v>2867</v>
       </c>
-      <c r="G50" s="73" t="s">
+      <c r="G50" s="72" t="s">
         <v>3377</v>
       </c>
-      <c r="H50" s="71" t="s">
+      <c r="H50" s="70" t="s">
         <v>3378</v>
       </c>
       <c r="I50" s="27" t="s">
@@ -51430,34 +51441,34 @@
         <f t="shared" si="0"/>
         <v>22</v>
       </c>
-      <c r="L50" s="85" t="str">
+      <c r="L50" s="84" t="str">
         <f t="shared" si="1"/>
         <v>#define mEFCT_UNIQ_WAITFORTRIG         76 // Effect type WAITING-FOR-TRIGGER. Trigger alone for next type.</v>
       </c>
     </row>
     <row r="51" spans="1:18" ht="15.75" customHeight="1">
-      <c r="A51" s="72" t="s">
+      <c r="A51" s="71" t="s">
         <v>3383</v>
       </c>
-      <c r="B51" s="71">
+      <c r="B51" s="70">
         <v>101</v>
       </c>
-      <c r="C51" s="66" t="s">
+      <c r="C51" s="65" t="s">
         <v>3382</v>
       </c>
-      <c r="D51" s="72" t="s">
+      <c r="D51" s="71" t="s">
         <v>3997</v>
       </c>
-      <c r="E51" s="72" t="s">
+      <c r="E51" s="71" t="s">
         <v>3383</v>
       </c>
-      <c r="F51" s="69" t="s">
+      <c r="F51" s="68" t="s">
         <v>2867</v>
       </c>
-      <c r="G51" s="73" t="s">
+      <c r="G51" s="72" t="s">
         <v>3377</v>
       </c>
-      <c r="H51" s="71" t="s">
+      <c r="H51" s="70" t="s">
         <v>3378</v>
       </c>
       <c r="I51" s="27" t="s">
@@ -51467,34 +51478,34 @@
         <f t="shared" si="0"/>
         <v>18</v>
       </c>
-      <c r="L51" s="85" t="str">
+      <c r="L51" s="84" t="str">
         <f t="shared" si="1"/>
         <v>#define mEFCT_UNIQ_SILENCE            101 // silence</v>
       </c>
     </row>
     <row r="52" spans="1:18" ht="20.25">
-      <c r="A52" s="72" t="s">
+      <c r="A52" s="71" t="s">
         <v>3383</v>
       </c>
-      <c r="B52" s="71">
+      <c r="B52" s="70">
         <v>102</v>
       </c>
-      <c r="C52" s="66" t="s">
+      <c r="C52" s="65" t="s">
         <v>3417</v>
       </c>
-      <c r="D52" s="72" t="s">
+      <c r="D52" s="71" t="s">
         <v>3998</v>
       </c>
-      <c r="E52" s="72" t="s">
+      <c r="E52" s="71" t="s">
         <v>3383</v>
       </c>
-      <c r="F52" s="69" t="s">
+      <c r="F52" s="68" t="s">
         <v>2867</v>
       </c>
-      <c r="G52" s="73" t="s">
+      <c r="G52" s="72" t="s">
         <v>3377</v>
       </c>
-      <c r="H52" s="71" t="s">
+      <c r="H52" s="70" t="s">
         <v>3378</v>
       </c>
       <c r="I52" s="27" t="s">
@@ -51504,39 +51515,41 @@
         <f t="shared" si="0"/>
         <v>19</v>
       </c>
-      <c r="L52" s="85" t="str">
+      <c r="L52" s="84" t="str">
         <f t="shared" si="1"/>
         <v>#define mEFCT_UNIQ_NOT_IMPL           102 // Not yet implemented</v>
       </c>
     </row>
     <row r="53" spans="1:18" ht="20.25">
-      <c r="E53" s="78"/>
-      <c r="F53" s="80"/>
-      <c r="G53" s="81"/>
-      <c r="H53" s="79"/>
+      <c r="E53" s="77"/>
+      <c r="F53" s="79"/>
+      <c r="G53" s="80"/>
+      <c r="H53" s="78"/>
       <c r="I53" s="27"/>
     </row>
     <row r="54" spans="1:18" ht="105">
-      <c r="A54" s="72" t="s">
+      <c r="A54" s="71" t="s">
         <v>3383</v>
       </c>
-      <c r="B54" s="71">
+      <c r="B54" s="70">
         <v>63</v>
       </c>
-      <c r="C54" s="52"/>
-      <c r="D54" s="88" t="s">
-        <v>4051</v>
-      </c>
-      <c r="E54" s="72" t="s">
+      <c r="C54" s="89" t="s">
+        <v>4071</v>
+      </c>
+      <c r="D54" s="87" t="s">
+        <v>4068</v>
+      </c>
+      <c r="E54" s="71" t="s">
         <v>3383</v>
       </c>
-      <c r="F54" s="69" t="s">
+      <c r="F54" s="68" t="s">
         <v>2867</v>
       </c>
-      <c r="G54" s="73" t="s">
+      <c r="G54" s="72" t="s">
         <v>3377</v>
       </c>
-      <c r="H54" s="71" t="s">
+      <c r="H54" s="70" t="s">
         <v>3378</v>
       </c>
       <c r="I54" s="3" t="s">
@@ -51546,32 +51559,34 @@
         <f t="shared" si="0"/>
         <v>23</v>
       </c>
-      <c r="L54" s="85" t="str">
-        <f t="shared" ref="L54:L56" si="2">"#define "&amp;I54&amp;" "&amp;REPT(" ",$J$39-J54)&amp;RIGHT(TEXT(B54,"    #"),3)&amp;" // "&amp;RIGHT(LEFT(D54,LEN(D54)-1),LEN(D54)-1-FIND("""",D54))</f>
-        <v>#define mEFCT_UNIQ_CFG_CATEGORY        63 // Now choose which effect category: sounds or LED patterns. As always press trigger by itself to go forward to next step or to cycle through choices To select a choice, press trigger plus any combination of Yellow, Green or Black button. To exit configuration, press trigger plus Blue button.</v>
+      <c r="L54" s="84" t="str">
+        <f>"#define "&amp;I54&amp;" "&amp;REPT(" ",$J$39-J54)&amp;RIGHT(TEXT(B54,"    #"),3)&amp;" // "&amp;RIGHT(LEFT(D54,LEN(D54)-1),LEN(D54)-1-FIND("""",D54))</f>
+        <v>#define mEFCT_UNIQ_CFG_CATEGORY        63 // Now choose which effect category: sounds or LED patterns. As always press trigger by itself to go forward to next step or to cycle through choices. To select a choice, press trigger plus any combination of Yellow, Green or Black button. To exit configuration, press trigger plus Blue button.</v>
       </c>
     </row>
     <row r="55" spans="1:18" ht="120">
-      <c r="A55" s="72" t="s">
+      <c r="A55" s="71" t="s">
         <v>3383</v>
       </c>
-      <c r="B55" s="71">
+      <c r="B55" s="70">
         <v>64</v>
       </c>
-      <c r="C55" s="52"/>
-      <c r="D55" s="88" t="s">
-        <v>4052</v>
-      </c>
-      <c r="E55" s="72" t="s">
+      <c r="C55" s="89" t="s">
+        <v>4072</v>
+      </c>
+      <c r="D55" s="87" t="s">
+        <v>4050</v>
+      </c>
+      <c r="E55" s="71" t="s">
         <v>3383</v>
       </c>
-      <c r="F55" s="69" t="s">
+      <c r="F55" s="68" t="s">
         <v>2867</v>
       </c>
-      <c r="G55" s="73" t="s">
+      <c r="G55" s="72" t="s">
         <v>3377</v>
       </c>
-      <c r="H55" s="71" t="s">
+      <c r="H55" s="70" t="s">
         <v>3378</v>
       </c>
       <c r="I55" s="3" t="s">
@@ -51581,32 +51596,34 @@
         <f t="shared" si="0"/>
         <v>19</v>
       </c>
-      <c r="L55" s="85" t="str">
-        <f t="shared" si="2"/>
+      <c r="L55" s="84" t="str">
+        <f t="shared" ref="L54:L56" si="2">"#define "&amp;I55&amp;" "&amp;REPT(" ",$J$39-J55)&amp;RIGHT(TEXT(B55,"    #"),3)&amp;" // "&amp;RIGHT(LEFT(D55,LEN(D55)-1),LEN(D55)-1-FIND("""",D55))</f>
         <v>#define mEFCT_UNIQ_CFG_TYPE            64 // Now choose when the effect happens. This list includes when powering-on, when shooting, etc. As always press trigger by itself to go forward to next step  or to cycle through choices. To select a choice, press trigger plus any combination of Yellow, Green or Black button. To exit configuration, press trigger plus Blue button.</v>
       </c>
     </row>
     <row r="56" spans="1:18" ht="120">
-      <c r="A56" s="72" t="s">
+      <c r="A56" s="71" t="s">
         <v>3383</v>
       </c>
-      <c r="B56" s="71">
+      <c r="B56" s="70">
         <v>65</v>
       </c>
-      <c r="C56" s="52"/>
-      <c r="D56" s="88" t="s">
-        <v>4053</v>
-      </c>
-      <c r="E56" s="72" t="s">
+      <c r="C56" s="89" t="s">
+        <v>4073</v>
+      </c>
+      <c r="D56" s="87" t="s">
+        <v>4051</v>
+      </c>
+      <c r="E56" s="71" t="s">
         <v>3383</v>
       </c>
-      <c r="F56" s="69" t="s">
+      <c r="F56" s="68" t="s">
         <v>2867</v>
       </c>
-      <c r="G56" s="73" t="s">
+      <c r="G56" s="72" t="s">
         <v>3377</v>
       </c>
-      <c r="H56" s="71" t="s">
+      <c r="H56" s="70" t="s">
         <v>3378</v>
       </c>
       <c r="I56" s="3" t="s">
@@ -51616,7 +51633,7 @@
         <f t="shared" si="0"/>
         <v>20</v>
       </c>
-      <c r="L56" s="85" t="str">
+      <c r="L56" s="84" t="str">
         <f t="shared" si="2"/>
         <v>#define mEFCT_UNIQ_CFG_EFECT           65 // Now choose the effect itself. This list cycles through the effects one by one. As always press trigger by itself to go forward to next step  or to cycle through choices. To select a choice, press trigger plus any combination of Yellow, Green or Black button. To exit configuration, press trigger plus Blue button.</v>
       </c>
@@ -51660,7 +51677,7 @@
       </c>
     </row>
     <row r="64" spans="1:18" ht="20.25">
-      <c r="A64" s="56" t="s">
+      <c r="A64" s="55" t="s">
         <v>2853</v>
       </c>
       <c r="B64" s="19"/>
@@ -51679,7 +51696,7 @@
       <c r="G64" s="35" t="s">
         <v>2882</v>
       </c>
-      <c r="H64" s="53" t="s">
+      <c r="H64" s="52" t="s">
         <v>2881</v>
       </c>
       <c r="K64" t="s">
@@ -51690,11 +51707,11 @@
       </c>
     </row>
     <row r="65" spans="1:18" ht="20.25">
-      <c r="A65" s="56" t="s">
+      <c r="A65" s="55" t="s">
         <v>2853</v>
       </c>
       <c r="B65" s="19"/>
-      <c r="C65" s="55" t="s">
+      <c r="C65" s="54" t="s">
         <v>2868</v>
       </c>
       <c r="D65" s="34" t="s">
@@ -51709,7 +51726,7 @@
       <c r="G65" s="35" t="s">
         <v>2870</v>
       </c>
-      <c r="H65" s="53" t="s">
+      <c r="H65" s="52" t="s">
         <v>2869</v>
       </c>
       <c r="R65" t="s">
@@ -51726,7 +51743,7 @@
       <c r="C66" s="33" t="s">
         <v>2888</v>
       </c>
-      <c r="D66" s="54" t="s">
+      <c r="D66" s="53" t="s">
         <v>3370</v>
       </c>
       <c r="E66" s="19" t="s">
@@ -51752,7 +51769,7 @@
       <c r="C67" s="33" t="s">
         <v>2887</v>
       </c>
-      <c r="D67" s="54" t="s">
+      <c r="D67" s="53" t="s">
         <v>2886</v>
       </c>
       <c r="E67" s="19" t="s">
@@ -51770,7 +51787,7 @@
     </row>
     <row r="68" spans="1:18" ht="20.25">
       <c r="A68" s="6"/>
-      <c r="D68" s="57"/>
+      <c r="D68" s="56"/>
       <c r="E68" s="6"/>
       <c r="F68" s="36"/>
       <c r="G68" s="36"/>
@@ -51778,7 +51795,7 @@
     </row>
     <row r="69" spans="1:18" ht="20.25">
       <c r="A69" s="6"/>
-      <c r="D69" s="57"/>
+      <c r="D69" s="56"/>
       <c r="E69" s="6"/>
       <c r="F69" s="36"/>
       <c r="G69" s="36"/>
@@ -51789,7 +51806,7 @@
     </row>
     <row r="70" spans="1:18" ht="20.25">
       <c r="A70" s="6"/>
-      <c r="D70" s="57"/>
+      <c r="D70" s="56"/>
       <c r="E70" s="6"/>
       <c r="F70" s="36"/>
       <c r="G70" s="36"/>
@@ -51800,7 +51817,7 @@
     </row>
     <row r="71" spans="1:18" ht="20.25">
       <c r="A71" s="6"/>
-      <c r="D71" s="57"/>
+      <c r="D71" s="56"/>
       <c r="E71" s="6"/>
       <c r="F71" s="36"/>
       <c r="G71" s="36"/>
@@ -51811,28 +51828,28 @@
     </row>
     <row r="72" spans="1:18" ht="20.25">
       <c r="A72" s="6"/>
-      <c r="D72" s="57"/>
+      <c r="D72" s="56"/>
       <c r="E72" s="6"/>
       <c r="F72" s="36"/>
       <c r="G72" s="36"/>
       <c r="H72" s="6"/>
     </row>
     <row r="73" spans="1:18" ht="20.25">
-      <c r="D73" s="57"/>
+      <c r="D73" s="56"/>
       <c r="E73" s="6"/>
       <c r="F73" s="36"/>
       <c r="G73" s="36"/>
       <c r="H73" s="6"/>
     </row>
     <row r="74" spans="1:18" ht="20.25">
-      <c r="D74" s="57"/>
+      <c r="D74" s="56"/>
       <c r="E74" s="6"/>
       <c r="F74" s="36"/>
       <c r="G74" s="36"/>
       <c r="H74" s="6"/>
     </row>
     <row r="75" spans="1:18" ht="20.25">
-      <c r="D75" s="57"/>
+      <c r="D75" s="56"/>
       <c r="E75" s="6"/>
       <c r="F75" s="36"/>
       <c r="G75" s="36"/>
@@ -51842,7 +51859,7 @@
       <c r="A76" s="6" t="s">
         <v>3384</v>
       </c>
-      <c r="D76" s="57"/>
+      <c r="D76" s="56"/>
       <c r="E76" s="6"/>
       <c r="F76" s="36"/>
       <c r="G76" s="36"/>
@@ -51852,7 +51869,7 @@
       <c r="A77" t="s">
         <v>3398</v>
       </c>
-      <c r="D77" s="57"/>
+      <c r="D77" s="56"/>
       <c r="E77" s="6"/>
       <c r="F77" s="36"/>
       <c r="G77" s="36"/>
@@ -51862,7 +51879,7 @@
       <c r="A78" t="s">
         <v>3399</v>
       </c>
-      <c r="D78" s="57"/>
+      <c r="D78" s="56"/>
       <c r="E78" s="6"/>
       <c r="F78" s="36"/>
       <c r="G78" s="36"/>
@@ -51872,7 +51889,7 @@
       <c r="A79" t="s">
         <v>3386</v>
       </c>
-      <c r="D79" s="57"/>
+      <c r="D79" s="56"/>
       <c r="E79" s="6"/>
       <c r="F79" s="36"/>
       <c r="G79" s="36"/>
@@ -52512,13 +52529,13 @@
         <f>"&lt;tr&gt;&lt;td&gt;&lt;b&gt;"&amp;J112&amp;"&lt;/b&gt;&lt;/td&gt;&lt;td&gt;&lt;b&gt;"&amp;K112&amp;"&lt;/b&gt;&lt;/td&gt;&lt;td&gt;&lt;b&gt;"&amp;L112&amp;"&lt;/b&gt;&lt;/td&gt;"</f>
         <v>&lt;tr&gt;&lt;td&gt;&lt;b&gt;Tag&lt;/b&gt;&lt;/td&gt;&lt;td&gt;&lt;b&gt;Name&lt;/b&gt;&lt;/td&gt;&lt;td&gt;&lt;b&gt;URL&lt;/b&gt;&lt;/td&gt;</v>
       </c>
-      <c r="J112" s="58" t="s">
+      <c r="J112" s="57" t="s">
         <v>2855</v>
       </c>
-      <c r="K112" s="58" t="s">
+      <c r="K112" s="57" t="s">
         <v>3387</v>
       </c>
-      <c r="L112" s="58" t="s">
+      <c r="L112" s="57" t="s">
         <v>2857</v>
       </c>
     </row>
@@ -52527,13 +52544,13 @@
         <f>"&lt;tr&gt;&lt;td&gt;"&amp;J113&amp;"&lt;/td&gt;&lt;td&gt;"&amp;K113&amp;"&lt;/td&gt;&lt;td&gt;"&amp;L113&amp;"&lt;/td&gt;"</f>
         <v>&lt;tr&gt;&lt;td&gt;zero/1.0/&lt;/td&gt;&lt;td&gt;Creative Commons 0 License&lt;/td&gt;&lt;td&gt;https://creativecommons.org/publicdomain/zero/1.0/&lt;/td&gt;</v>
       </c>
-      <c r="J113" s="59" t="s">
+      <c r="J113" s="58" t="s">
         <v>2859</v>
       </c>
-      <c r="K113" s="59" t="s">
+      <c r="K113" s="58" t="s">
         <v>3388</v>
       </c>
-      <c r="L113" s="60" t="s">
+      <c r="L113" s="59" t="s">
         <v>3389</v>
       </c>
     </row>
@@ -52542,13 +52559,13 @@
         <f>"&lt;tr&gt;&lt;td&gt;"&amp;J114&amp;"&lt;/td&gt;&lt;td&gt;"&amp;K114&amp;"&lt;/td&gt;&lt;td&gt;"&amp;L114&amp;"&lt;/td&gt;"</f>
         <v>&lt;tr&gt;&lt;td&gt;by/3.0/&lt;/td&gt;&lt;td&gt;Creative Commons Attribution License&lt;/td&gt;&lt;td&gt;https://creativecommons.org/licenses/by/3.0/&lt;/td&gt;</v>
       </c>
-      <c r="J114" s="61" t="s">
+      <c r="J114" s="60" t="s">
         <v>2867</v>
       </c>
-      <c r="K114" s="61" t="s">
+      <c r="K114" s="60" t="s">
         <v>3390</v>
       </c>
-      <c r="L114" s="62" t="s">
+      <c r="L114" s="61" t="s">
         <v>3391</v>
       </c>
     </row>
@@ -52557,13 +52574,13 @@
         <f>"&lt;tr&gt;&lt;td&gt;"&amp;J115&amp;"&lt;/td&gt;&lt;td&gt;"&amp;K115&amp;"&lt;/td&gt;&lt;td&gt;"&amp;L115&amp;"&lt;/td&gt;"</f>
         <v>&lt;tr&gt;&lt;td&gt;by-nc/3.0/&lt;/td&gt;&lt;td&gt;Creative Commons Attribution Noncommercial License&lt;/td&gt;&lt;td&gt;https://creativecommons.org/licenses/by-nc/3.0/&lt;/td&gt;</v>
       </c>
-      <c r="J115" s="59" t="s">
+      <c r="J115" s="58" t="s">
         <v>2879</v>
       </c>
-      <c r="K115" s="59" t="s">
+      <c r="K115" s="58" t="s">
         <v>3392</v>
       </c>
-      <c r="L115" s="60" t="s">
+      <c r="L115" s="59" t="s">
         <v>3393</v>
       </c>
     </row>

</xml_diff>

<commit_message>
get ready to add LingoJam.com robotic voice for power-on
</commit_message>
<xml_diff>
--- a/RBG_arduino/StateTable_minimal.xlsx
+++ b/RBG_arduino/StateTable_minimal.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22228"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22325"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub-Mark-MDO47\RubberBandGun\RBG_arduino\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C511C5BF-27C7-4BEF-8142-7F9CD4896FC6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4855E262-849B-40DA-B8E2-F7CB22009468}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21840" xr2:uid="{CCADFEE4-B0E1-4363-9617-1683960BED03}"/>
+    <workbookView xWindow="1860" yWindow="2025" windowWidth="32745" windowHeight="16875" activeTab="5" xr2:uid="{CCADFEE4-B0E1-4363-9617-1683960BED03}"/>
   </bookViews>
   <sheets>
     <sheet name="StateTable" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">debugging!$A$3889:$B$4396</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">Sounds!$A$1:$H$53</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">Sounds!$A$1:$H$54</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">StateTable!$A$1:$K$88</definedName>
     <definedName name="mROW">StateTable!$V$2:$X$30</definedName>
     <definedName name="prev">Sounds!$AK$2:$AK$18</definedName>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6560" uniqueCount="4694">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6568" uniqueCount="4700">
   <si>
     <t>trigOnly</t>
   </si>
@@ -15222,15 +15222,6 @@
     <t>mdo47 recording of "Achtung! This is the awesome FOOF Rubber Band Gun."</t>
   </si>
   <si>
-    <t>mEFCT_UNIQ_LFOOF</t>
-  </si>
-  <si>
-    <t>mEFCT_UNIQ_MFOOF</t>
-  </si>
-  <si>
-    <t>mEFCT_UNIQ_CFOOF</t>
-  </si>
-  <si>
     <t>mdo47 recording of "The effect happens during wind-up to shooting"</t>
   </si>
   <si>
@@ -15256,6 +15247,33 @@
   </si>
   <si>
     <t>mdo47 recording of "This feature is not yet implemented"</t>
+  </si>
+  <si>
+    <t>0044__LingoJam.com__FOOF.wav</t>
+  </si>
+  <si>
+    <t>https://lingojam.com/RobotVoiceGenerator</t>
+  </si>
+  <si>
+    <t>mdo47 recording of "https://lingojam.com/RobotVoiceGenerator: This is the awesome FOOF Rubber Band Gun. Be afraid."</t>
+  </si>
+  <si>
+    <t>Feel free to use the generated audio for any of your projects (commercial or personal).</t>
+  </si>
+  <si>
+    <t>LingoJam.com</t>
+  </si>
+  <si>
+    <t>mEFCT_PWRON_LFOOF</t>
+  </si>
+  <si>
+    <t>mEFCT_PWRON_MFOOF</t>
+  </si>
+  <si>
+    <t>mEFCT_PWRON_CFOOF</t>
+  </si>
+  <si>
+    <t>mEFCT_PWRON_RFOOF</t>
   </si>
 </sst>
 </file>
@@ -15708,7 +15726,7 @@
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="24" fillId="12" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="93">
+  <cellXfs count="94">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -15889,6 +15907,9 @@
     <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="6" xfId="3" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="4" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="9">
@@ -16219,7 +16240,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{90E8DFC6-94F4-4A82-A874-2F16F2CF0145}">
   <dimension ref="A1:AB93"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A69" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="J86" sqref="J86"/>
     </sheetView>
@@ -16318,7 +16339,7 @@
         <v>3246</v>
       </c>
       <c r="K2" s="9" t="str">
-        <f>IF(LEN(C2),VLOOKUP(C2,mROW,3,FALSE),"")</f>
+        <f t="shared" ref="K2:K13" si="0">IF(LEN(C2),VLOOKUP(C2,mROW,3,FALSE),"")</f>
         <v>#define mROW_POWERON 0</v>
       </c>
       <c r="P2" t="s">
@@ -16361,7 +16382,7 @@
       </c>
       <c r="J3" s="9"/>
       <c r="K3" s="9" t="str">
-        <f>IF(LEN(C3),VLOOKUP(C3,mROW,3,FALSE),"")</f>
+        <f t="shared" si="0"/>
         <v>#define mROW_POWERON 0</v>
       </c>
       <c r="V3" t="s">
@@ -16376,7 +16397,7 @@
     </row>
     <row r="4" spans="1:28">
       <c r="K4" s="9" t="str">
-        <f>IF(LEN(C4),VLOOKUP(C4,mROW,3,FALSE),"")</f>
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="V4" t="s">
@@ -16413,7 +16434,7 @@
         <v>39</v>
       </c>
       <c r="K5" s="9" t="str">
-        <f>IF(LEN(C5),VLOOKUP(C5,mROW,3,FALSE),"")</f>
+        <f t="shared" si="0"/>
         <v>#define mROW_PWRON_OPEN 2</v>
       </c>
       <c r="M5" s="63" t="s">
@@ -16453,7 +16474,7 @@
       </c>
       <c r="J6" s="9"/>
       <c r="K6" s="9" t="str">
-        <f>IF(LEN(C6),VLOOKUP(C6,mROW,3,FALSE),"")</f>
+        <f t="shared" si="0"/>
         <v>#define mROW_PWRON_OPEN 2</v>
       </c>
       <c r="M6" s="63" t="s">
@@ -16472,7 +16493,7 @@
     </row>
     <row r="7" spans="1:28">
       <c r="K7" s="9" t="str">
-        <f>IF(LEN(C7),VLOOKUP(C7,mROW,3,FALSE),"")</f>
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="M7" s="63" t="s">
@@ -16490,7 +16511,7 @@
     </row>
     <row r="8" spans="1:28">
       <c r="K8" s="9" t="str">
-        <f>IF(LEN(C8),VLOOKUP(C8,mROW,3,FALSE),"")</f>
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="M8" s="63" t="s">
@@ -16508,7 +16529,7 @@
     </row>
     <row r="9" spans="1:28">
       <c r="K9" s="9" t="str">
-        <f>IF(LEN(C9),VLOOKUP(C9,mROW,3,FALSE),"")</f>
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="M9" s="63" t="s">
@@ -16526,7 +16547,7 @@
     </row>
     <row r="10" spans="1:28" s="25" customFormat="1">
       <c r="K10" s="9" t="str">
-        <f>IF(LEN(C10),VLOOKUP(C10,mROW,3,FALSE),"")</f>
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="M10" s="63" t="s">
@@ -16579,7 +16600,7 @@
         <v>39</v>
       </c>
       <c r="K11" s="9" t="str">
-        <f>IF(LEN(C11),VLOOKUP(C11,mROW,3,FALSE),"")</f>
+        <f t="shared" si="0"/>
         <v>#define mROW_PWRON_LOCKED 4</v>
       </c>
       <c r="M11" s="63" t="s">
@@ -16623,7 +16644,7 @@
       </c>
       <c r="J12" s="9"/>
       <c r="K12" s="9" t="str">
-        <f>IF(LEN(C12),VLOOKUP(C12,mROW,3,FALSE),"")</f>
+        <f t="shared" si="0"/>
         <v>#define mROW_PWRON_LOCKED 4</v>
       </c>
       <c r="M12" s="63" t="s">
@@ -16669,7 +16690,7 @@
       </c>
       <c r="J13" s="9"/>
       <c r="K13" s="9" t="str">
-        <f>IF(LEN(C13),VLOOKUP(C13,mROW,3,FALSE),"")</f>
+        <f t="shared" si="0"/>
         <v>#define mROW_PWRON_LOCKED 4</v>
       </c>
       <c r="M13" s="63" t="s">
@@ -16739,7 +16760,7 @@
       </c>
       <c r="J16" s="37"/>
       <c r="K16" s="9" t="str">
-        <f>IF(LEN(C16),VLOOKUP(C16,mROW,3,FALSE),"")</f>
+        <f t="shared" ref="K16:K41" si="1">IF(LEN(C16),VLOOKUP(C16,mROW,3,FALSE),"")</f>
         <v>#define mROW_MENU 7</v>
       </c>
       <c r="P16" s="25" t="s">
@@ -16775,7 +16796,7 @@
       </c>
       <c r="J17" s="37"/>
       <c r="K17" s="9" t="str">
-        <f>IF(LEN(C17),VLOOKUP(C17,mROW,3,FALSE),"")</f>
+        <f t="shared" si="1"/>
         <v>#define mROW_MENU 7</v>
       </c>
       <c r="V17" t="s">
@@ -16804,7 +16825,7 @@
       <c r="I18" s="37"/>
       <c r="J18" s="37"/>
       <c r="K18" s="9" t="str">
-        <f>IF(LEN(C18),VLOOKUP(C18,mROW,3,FALSE),"")</f>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="M18"/>
@@ -16845,7 +16866,7 @@
       </c>
       <c r="J19" s="37"/>
       <c r="K19" s="9" t="str">
-        <f>IF(LEN(C19),VLOOKUP(C19,mROW,3,FALSE),"")</f>
+        <f t="shared" si="1"/>
         <v>#define mROW_MENU_OPEN 9</v>
       </c>
       <c r="V19" t="s">
@@ -16882,7 +16903,7 @@
       </c>
       <c r="J20" s="37"/>
       <c r="K20" s="9" t="str">
-        <f>IF(LEN(C20),VLOOKUP(C20,mROW,3,FALSE),"")</f>
+        <f t="shared" si="1"/>
         <v>#define mROW_MENU_OPEN 9</v>
       </c>
       <c r="V20" t="s">
@@ -16919,7 +16940,7 @@
       </c>
       <c r="J21" s="37"/>
       <c r="K21" s="9" t="str">
-        <f>IF(LEN(C21),VLOOKUP(C21,mROW,3,FALSE),"")</f>
+        <f t="shared" si="1"/>
         <v>#define mROW_MENU_CLOSED 11</v>
       </c>
       <c r="V21" t="s">
@@ -16946,7 +16967,7 @@
       <c r="I22" s="37"/>
       <c r="J22" s="37"/>
       <c r="K22" s="9" t="str">
-        <f>IF(LEN(C22),VLOOKUP(C22,mROW,3,FALSE),"")</f>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="V22" t="s">
@@ -16984,7 +17005,7 @@
       </c>
       <c r="J23" s="37"/>
       <c r="K23" s="9" t="str">
-        <f>IF(LEN(C23),VLOOKUP(C23,mROW,3,FALSE),"")</f>
+        <f t="shared" si="1"/>
         <v>#define mROW_MENU_CLOSED 11</v>
       </c>
       <c r="V23" t="s">
@@ -17021,7 +17042,7 @@
       </c>
       <c r="J24" s="37"/>
       <c r="K24" s="9" t="str">
-        <f>IF(LEN(C24),VLOOKUP(C24,mROW,3,FALSE),"")</f>
+        <f t="shared" si="1"/>
         <v>#define mROW_MENU_CLOSED 11</v>
       </c>
       <c r="V24" t="s">
@@ -17059,7 +17080,7 @@
       </c>
       <c r="J25" s="37"/>
       <c r="K25" s="9" t="str">
-        <f>IF(LEN(C25),VLOOKUP(C25,mROW,3,FALSE),"")</f>
+        <f t="shared" si="1"/>
         <v>#define mROW_MENU_CLOSED 11</v>
       </c>
       <c r="V25" t="s">
@@ -17084,7 +17105,7 @@
       <c r="I26" s="9"/>
       <c r="J26" s="9"/>
       <c r="K26" s="9" t="str">
-        <f>IF(LEN(C26),VLOOKUP(C26,mROW,3,FALSE),"")</f>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="V26" t="s">
@@ -17119,7 +17140,7 @@
         <v>43</v>
       </c>
       <c r="K27" s="9" t="str">
-        <f>IF(LEN(C27),VLOOKUP(C27,mROW,3,FALSE),"")</f>
+        <f t="shared" si="1"/>
         <v>#define mROW_WINDUP_SOUND 15</v>
       </c>
       <c r="V27" t="s">
@@ -17139,7 +17160,7 @@
       <c r="I28" s="9"/>
       <c r="J28" s="9"/>
       <c r="K28" s="9" t="str">
-        <f>IF(LEN(C28),VLOOKUP(C28,mROW,3,FALSE),"")</f>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="V28" t="s">
@@ -17167,7 +17188,7 @@
         <v>48</v>
       </c>
       <c r="K29" s="9" t="str">
-        <f>IF(LEN(C29),VLOOKUP(C29,mROW,3,FALSE),"")</f>
+        <f t="shared" si="1"/>
         <v>#define mROW_SHOOT 16</v>
       </c>
       <c r="V29" t="s">
@@ -17188,7 +17209,7 @@
       <c r="I30" s="9"/>
       <c r="J30" s="9"/>
       <c r="K30" s="9" t="str">
-        <f>IF(LEN(C30),VLOOKUP(C30,mROW,3,FALSE),"")</f>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="X30" s="2"/>
@@ -17217,7 +17238,7 @@
         <v>46</v>
       </c>
       <c r="K31" s="9" t="str">
-        <f>IF(LEN(C31),VLOOKUP(C31,mROW,3,FALSE),"")</f>
+        <f t="shared" si="1"/>
         <v>#define mROW_SHOOT_SOUND 17</v>
       </c>
       <c r="R31"/>
@@ -17233,7 +17254,7 @@
       <c r="I32" s="9"/>
       <c r="J32" s="9"/>
       <c r="K32" s="9" t="str">
-        <f>IF(LEN(C32),VLOOKUP(C32,mROW,3,FALSE),"")</f>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="V32" s="2"/>
@@ -17246,7 +17267,7 @@
       <c r="I33" s="9"/>
       <c r="J33" s="9"/>
       <c r="K33" s="9" t="str">
-        <f>IF(LEN(C33),VLOOKUP(C33,mROW,3,FALSE),"")</f>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="R33" s="2"/>
@@ -17269,7 +17290,7 @@
         <v>39</v>
       </c>
       <c r="K34" s="9" t="str">
-        <f>IF(LEN(C34),VLOOKUP(C34,mROW,3,FALSE),"")</f>
+        <f t="shared" si="1"/>
         <v>#define mROW_SOLENOID 18</v>
       </c>
       <c r="O34" s="7"/>
@@ -17282,7 +17303,7 @@
       <c r="I35" s="9"/>
       <c r="J35" s="9"/>
       <c r="K35" s="9" t="str">
-        <f>IF(LEN(C35),VLOOKUP(C35,mROW,3,FALSE),"")</f>
+        <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
@@ -17310,7 +17331,7 @@
         <v>39</v>
       </c>
       <c r="K36" s="9" t="str">
-        <f>IF(LEN(C36),VLOOKUP(C36,mROW,3,FALSE),"")</f>
+        <f t="shared" si="1"/>
         <v>#define mROW_OPNBRL 19</v>
       </c>
     </row>
@@ -17338,7 +17359,7 @@
       </c>
       <c r="J37" s="9"/>
       <c r="K37" s="9" t="str">
-        <f>IF(LEN(C37),VLOOKUP(C37,mROW,3,FALSE),"")</f>
+        <f t="shared" si="1"/>
         <v>#define mROW_OPNBRL 19</v>
       </c>
     </row>
@@ -17354,7 +17375,7 @@
       <c r="I38" s="37"/>
       <c r="J38" s="37"/>
       <c r="K38" s="9" t="str">
-        <f>IF(LEN(C38),VLOOKUP(C38,mROW,3,FALSE),"")</f>
+        <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
@@ -17379,7 +17400,7 @@
         <v>39</v>
       </c>
       <c r="K39" s="9" t="str">
-        <f>IF(LEN(C39),VLOOKUP(C39,mROW,3,FALSE),"")</f>
+        <f t="shared" si="1"/>
         <v>#define mROW_LOKLOD 21</v>
       </c>
     </row>
@@ -17405,7 +17426,7 @@
       </c>
       <c r="J40" s="9"/>
       <c r="K40" s="9" t="str">
-        <f>IF(LEN(C40),VLOOKUP(C40,mROW,3,FALSE),"")</f>
+        <f t="shared" si="1"/>
         <v>#define mROW_LOKLOD 21</v>
       </c>
     </row>
@@ -17430,7 +17451,7 @@
       </c>
       <c r="J41" s="9"/>
       <c r="K41" s="9" t="str">
-        <f>IF(LEN(C41),VLOOKUP(C41,mROW,3,FALSE),"")</f>
+        <f t="shared" si="1"/>
         <v>#define mROW_LOKLOD 21</v>
       </c>
     </row>
@@ -17467,7 +17488,7 @@
       </c>
       <c r="J43" s="9"/>
       <c r="K43" s="9" t="str">
-        <f>IF(LEN(C43),VLOOKUP(C43,mROW,3,FALSE),"")</f>
+        <f t="shared" ref="K43:K86" si="2">IF(LEN(C43),VLOOKUP(C43,mROW,3,FALSE),"")</f>
         <v>#define mROW_CFG_MENU 24</v>
       </c>
       <c r="O43" s="37"/>
@@ -17494,7 +17515,7 @@
       </c>
       <c r="J44" s="9"/>
       <c r="K44" s="9" t="str">
-        <f>IF(LEN(C44),VLOOKUP(C44,mROW,3,FALSE),"")</f>
+        <f t="shared" si="2"/>
         <v>#define mROW_CFG_MENU 24</v>
       </c>
     </row>
@@ -17519,7 +17540,7 @@
       </c>
       <c r="J45" s="9"/>
       <c r="K45" s="9" t="str">
-        <f>IF(LEN(C45),VLOOKUP(C45,mROW,3,FALSE),"")</f>
+        <f t="shared" si="2"/>
         <v>#define mROW_CFG_MENU 24</v>
       </c>
     </row>
@@ -17527,7 +17548,7 @@
       <c r="I46" s="9"/>
       <c r="J46" s="9"/>
       <c r="K46" s="9" t="str">
-        <f>IF(LEN(C46),VLOOKUP(C46,mROW,3,FALSE),"")</f>
+        <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
@@ -17535,7 +17556,7 @@
       <c r="I47" s="9"/>
       <c r="J47" s="9"/>
       <c r="K47" s="9" t="str">
-        <f>IF(LEN(C47),VLOOKUP(C47,mROW,3,FALSE),"")</f>
+        <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
@@ -17560,7 +17581,7 @@
         <v>3711</v>
       </c>
       <c r="K48" s="9" t="str">
-        <f>IF(LEN(C48),VLOOKUP(C48,mROW,3,FALSE),"")</f>
+        <f t="shared" si="2"/>
         <v>#define mROW_CFG_CATEGORY 27</v>
       </c>
     </row>
@@ -17568,7 +17589,7 @@
       <c r="I49" s="9"/>
       <c r="J49" s="9"/>
       <c r="K49" s="9" t="str">
-        <f>IF(LEN(C49),VLOOKUP(C49,mROW,3,FALSE),"")</f>
+        <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
@@ -17598,7 +17619,7 @@
       </c>
       <c r="J50" s="9"/>
       <c r="K50" s="9" t="str">
-        <f>IF(LEN(C50),VLOOKUP(C50,mROW,3,FALSE),"")</f>
+        <f t="shared" si="2"/>
         <v>#define mROW_CFG_CATEGORY_LOOPSTART 28</v>
       </c>
     </row>
@@ -17625,7 +17646,7 @@
       </c>
       <c r="J51" s="9"/>
       <c r="K51" s="9" t="str">
-        <f>IF(LEN(C51),VLOOKUP(C51,mROW,3,FALSE),"")</f>
+        <f t="shared" si="2"/>
         <v>#define mROW_CFG_CATEGORY_LOOPSTART 28</v>
       </c>
     </row>
@@ -17650,7 +17671,7 @@
       </c>
       <c r="J52" s="9"/>
       <c r="K52" s="9" t="str">
-        <f>IF(LEN(C52),VLOOKUP(C52,mROW,3,FALSE),"")</f>
+        <f t="shared" si="2"/>
         <v>#define mROW_CFG_CATEGORY_LOOPSTART 28</v>
       </c>
     </row>
@@ -17658,7 +17679,7 @@
       <c r="I53" s="9"/>
       <c r="J53" s="9"/>
       <c r="K53" s="9" t="str">
-        <f>IF(LEN(C53),VLOOKUP(C53,mROW,3,FALSE),"")</f>
+        <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
@@ -17677,7 +17698,7 @@
       </c>
       <c r="J54" s="9"/>
       <c r="K54" s="9" t="str">
-        <f>IF(LEN(C54),VLOOKUP(C54,mROW,3,FALSE),"")</f>
+        <f t="shared" si="2"/>
         <v>#define mROW_CFG_CATEGORY_LOOP 31</v>
       </c>
     </row>
@@ -17696,7 +17717,7 @@
       </c>
       <c r="J55" s="9"/>
       <c r="K55" s="9" t="str">
-        <f>IF(LEN(C55),VLOOKUP(C55,mROW,3,FALSE),"")</f>
+        <f t="shared" si="2"/>
         <v>#define mROW_CFG_CATEGORY_LOOP 31</v>
       </c>
     </row>
@@ -17717,7 +17738,7 @@
       </c>
       <c r="J56" s="9"/>
       <c r="K56" s="9" t="str">
-        <f>IF(LEN(C56),VLOOKUP(C56,mROW,3,FALSE),"")</f>
+        <f t="shared" si="2"/>
         <v>#define mROW_CFG_CATEGORY_LOOP 31</v>
       </c>
     </row>
@@ -17725,7 +17746,7 @@
       <c r="I57" s="9"/>
       <c r="J57" s="9"/>
       <c r="K57" s="9" t="str">
-        <f>IF(LEN(C57),VLOOKUP(C57,mROW,3,FALSE),"")</f>
+        <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
@@ -17741,7 +17762,7 @@
         <v>3712</v>
       </c>
       <c r="K58" s="9" t="str">
-        <f>IF(LEN(C58),VLOOKUP(C58,mROW,3,FALSE),"")</f>
+        <f t="shared" si="2"/>
         <v>#define mROW_CFG_CATEGORY_NEXT 34</v>
       </c>
     </row>
@@ -17749,7 +17770,7 @@
       <c r="I59" s="9"/>
       <c r="J59" s="9"/>
       <c r="K59" s="9" t="str">
-        <f>IF(LEN(C59),VLOOKUP(C59,mROW,3,FALSE),"")</f>
+        <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
@@ -17765,7 +17786,7 @@
         <v>3715</v>
       </c>
       <c r="K60" s="9" t="str">
-        <f>IF(LEN(C60),VLOOKUP(C60,mROW,3,FALSE),"")</f>
+        <f t="shared" si="2"/>
         <v>#define mROW_CFG_CATEGORY_CHOICE 35</v>
       </c>
     </row>
@@ -17773,13 +17794,13 @@
       <c r="I61" s="9"/>
       <c r="J61" s="9"/>
       <c r="K61" s="9" t="str">
-        <f>IF(LEN(C61),VLOOKUP(C61,mROW,3,FALSE),"")</f>
+        <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
     <row r="62" spans="1:11">
       <c r="K62" s="9" t="str">
-        <f>IF(LEN(C62),VLOOKUP(C62,mROW,3,FALSE),"")</f>
+        <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
@@ -17803,17 +17824,17 @@
         <v>3716</v>
       </c>
       <c r="K63" s="9" t="str">
-        <f>IF(LEN(C63),VLOOKUP(C63,mROW,3,FALSE),"")</f>
+        <f t="shared" si="2"/>
         <v>#define mROW_CFG_TYPE 36</v>
       </c>
     </row>
     <row r="64" spans="1:11">
       <c r="K64" s="9" t="str">
-        <f>IF(LEN(C64),VLOOKUP(C64,mROW,3,FALSE),"")</f>
+        <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
-    <row r="65" spans="1:24" ht="240">
+    <row r="65" spans="1:24" ht="225">
       <c r="A65" s="83" t="s">
         <v>3734</v>
       </c>
@@ -17838,7 +17859,7 @@
         <v>3717</v>
       </c>
       <c r="K65" s="9" t="str">
-        <f>IF(LEN(C65),VLOOKUP(C65,mROW,3,FALSE),"")</f>
+        <f t="shared" si="2"/>
         <v>#define mROW_CFG_TYPE_LOOPSTART 37</v>
       </c>
     </row>
@@ -17860,7 +17881,7 @@
       <c r="H66" s="9"/>
       <c r="I66" s="9"/>
       <c r="K66" s="9" t="str">
-        <f>IF(LEN(C66),VLOOKUP(C66,mROW,3,FALSE),"")</f>
+        <f t="shared" si="2"/>
         <v>#define mROW_CFG_TYPE_LOOPSTART 37</v>
       </c>
       <c r="V66" t="str">
@@ -17893,15 +17914,15 @@
       <c r="H67" s="9"/>
       <c r="I67" s="9"/>
       <c r="K67" s="9" t="str">
-        <f>IF(LEN(C67),VLOOKUP(C67,mROW,3,FALSE),"")</f>
+        <f t="shared" si="2"/>
         <v>#define mROW_CFG_TYPE_LOOPSTART 37</v>
       </c>
       <c r="V67" t="str">
-        <f t="shared" ref="V67:V93" si="0">MID(X67,9,FIND(" ",X67,9)-9)</f>
+        <f t="shared" ref="V67:V93" si="3">MID(X67,9,FIND(" ",X67,9)-9)</f>
         <v>mROW_PWRON_OPEN</v>
       </c>
       <c r="W67">
-        <f t="shared" ref="W67:W93" si="1">0+MID(X67,10+LEN(V67),2)</f>
+        <f t="shared" ref="W67:W93" si="4">0+MID(X67,10+LEN(V67),2)</f>
         <v>2</v>
       </c>
       <c r="X67" s="15" t="s">
@@ -17910,15 +17931,15 @@
     </row>
     <row r="68" spans="1:24">
       <c r="K68" s="9" t="str">
-        <f>IF(LEN(C68),VLOOKUP(C68,mROW,3,FALSE),"")</f>
+        <f t="shared" si="2"/>
         <v/>
       </c>
       <c r="V68" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>mROW_PWRON_LOCKED</v>
       </c>
       <c r="W68">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>4</v>
       </c>
       <c r="X68" s="15" t="s">
@@ -17939,15 +17960,15 @@
         <v>3718</v>
       </c>
       <c r="K69" s="9" t="str">
-        <f>IF(LEN(C69),VLOOKUP(C69,mROW,3,FALSE),"")</f>
+        <f t="shared" si="2"/>
         <v>#define mROW_CFG_TYPE_LOOP 40</v>
       </c>
       <c r="V69" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>mROW_MENU</v>
       </c>
       <c r="W69">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>7</v>
       </c>
       <c r="X69" s="15" t="s">
@@ -17968,15 +17989,15 @@
         <v>3719</v>
       </c>
       <c r="K70" s="9" t="str">
-        <f>IF(LEN(C70),VLOOKUP(C70,mROW,3,FALSE),"")</f>
+        <f t="shared" si="2"/>
         <v>#define mROW_CFG_TYPE_LOOP 40</v>
       </c>
       <c r="V70" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>mROW_MENU_OPEN</v>
       </c>
       <c r="W70">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>9</v>
       </c>
       <c r="X70" s="15" t="s">
@@ -17985,15 +18006,15 @@
     </row>
     <row r="71" spans="1:24">
       <c r="K71" s="9" t="str">
-        <f>IF(LEN(C71),VLOOKUP(C71,mROW,3,FALSE),"")</f>
+        <f t="shared" si="2"/>
         <v/>
       </c>
       <c r="V71" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>mROW_MENU_CLOSED</v>
       </c>
       <c r="W71">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>11</v>
       </c>
       <c r="X71" s="15" t="s">
@@ -18011,15 +18032,15 @@
         <v>3717</v>
       </c>
       <c r="K72" s="9" t="str">
-        <f>IF(LEN(C72),VLOOKUP(C72,mROW,3,FALSE),"")</f>
+        <f t="shared" si="2"/>
         <v>#define mROW_CFG_TYPE_NEXT 42</v>
       </c>
       <c r="V72" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>mROW_WINDUP_SOUND</v>
       </c>
       <c r="W72">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>15</v>
       </c>
       <c r="X72" s="15" t="s">
@@ -18028,15 +18049,15 @@
     </row>
     <row r="73" spans="1:24">
       <c r="K73" s="9" t="str">
-        <f>IF(LEN(C73),VLOOKUP(C73,mROW,3,FALSE),"")</f>
+        <f t="shared" si="2"/>
         <v/>
       </c>
       <c r="V73" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>mROW_SHOOT</v>
       </c>
       <c r="W73">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>16</v>
       </c>
       <c r="X73" s="15" t="s">
@@ -18054,15 +18075,15 @@
         <v>3724</v>
       </c>
       <c r="K74" s="9" t="str">
-        <f>IF(LEN(C74),VLOOKUP(C74,mROW,3,FALSE),"")</f>
+        <f t="shared" si="2"/>
         <v>#define mROW_CFG_TYPE_CHOICE 43</v>
       </c>
       <c r="V74" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>mROW_SHOOT_SOUND</v>
       </c>
       <c r="W74">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>17</v>
       </c>
       <c r="X74" s="15" t="s">
@@ -18071,15 +18092,15 @@
     </row>
     <row r="75" spans="1:24">
       <c r="K75" s="9" t="str">
-        <f>IF(LEN(C75),VLOOKUP(C75,mROW,3,FALSE),"")</f>
+        <f t="shared" si="2"/>
         <v/>
       </c>
       <c r="V75" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>mROW_SOLENOID</v>
       </c>
       <c r="W75">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>18</v>
       </c>
       <c r="X75" s="15" t="s">
@@ -18088,15 +18109,15 @@
     </row>
     <row r="76" spans="1:24">
       <c r="K76" s="9" t="str">
-        <f>IF(LEN(C76),VLOOKUP(C76,mROW,3,FALSE),"")</f>
+        <f t="shared" si="2"/>
         <v/>
       </c>
       <c r="V76" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>mROW_OPNBRL</v>
       </c>
       <c r="W76">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>19</v>
       </c>
       <c r="X76" s="15" t="s">
@@ -18126,15 +18147,15 @@
         <v>3720</v>
       </c>
       <c r="K77" s="9" t="str">
-        <f>IF(LEN(C77),VLOOKUP(C77,mROW,3,FALSE),"")</f>
+        <f t="shared" si="2"/>
         <v>#define mROW_CFG_EFFECT 44</v>
       </c>
       <c r="V77" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>mROW_LOKLOD</v>
       </c>
       <c r="W77">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>21</v>
       </c>
       <c r="X77" s="15" t="s">
@@ -18143,15 +18164,15 @@
     </row>
     <row r="78" spans="1:24">
       <c r="K78" s="9" t="str">
-        <f>IF(LEN(C78),VLOOKUP(C78,mROW,3,FALSE),"")</f>
+        <f t="shared" si="2"/>
         <v/>
       </c>
       <c r="V78" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>mROW_CFG_MENU</v>
       </c>
       <c r="W78">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>24</v>
       </c>
       <c r="X78" t="s">
@@ -18180,15 +18201,15 @@
         <v>3721</v>
       </c>
       <c r="K79" s="9" t="str">
-        <f>IF(LEN(C79),VLOOKUP(C79,mROW,3,FALSE),"")</f>
+        <f t="shared" si="2"/>
         <v>#define mROW_CFG_EFFECT_LOOPSTART 45</v>
       </c>
       <c r="V79" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>mROW_CFG_CATEGORY</v>
       </c>
       <c r="W79">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>27</v>
       </c>
       <c r="X79" t="s">
@@ -18197,15 +18218,15 @@
     </row>
     <row r="80" spans="1:24">
       <c r="K80" s="9" t="str">
-        <f>IF(LEN(C80),VLOOKUP(C80,mROW,3,FALSE),"")</f>
+        <f t="shared" si="2"/>
         <v/>
       </c>
       <c r="V80" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>mROW_CFG_CATEGORY_LOOPSTART</v>
       </c>
       <c r="W80">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>28</v>
       </c>
       <c r="X80" t="s">
@@ -18226,15 +18247,15 @@
         <v>3722</v>
       </c>
       <c r="K81" s="9" t="str">
-        <f>IF(LEN(C81),VLOOKUP(C81,mROW,3,FALSE),"")</f>
+        <f t="shared" si="2"/>
         <v>#define mROW_CFG_EFFECT_LOOP 46</v>
       </c>
       <c r="V81" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>mROW_CFG_CATEGORY_LOOP</v>
       </c>
       <c r="W81">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>31</v>
       </c>
       <c r="X81" t="s">
@@ -18255,15 +18276,15 @@
         <v>3723</v>
       </c>
       <c r="K82" s="9" t="str">
-        <f>IF(LEN(C82),VLOOKUP(C82,mROW,3,FALSE),"")</f>
+        <f t="shared" si="2"/>
         <v>#define mROW_CFG_EFFECT_LOOP 46</v>
       </c>
       <c r="V82" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>mROW_CFG_CATEGORY_NEXT</v>
       </c>
       <c r="W82">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>34</v>
       </c>
       <c r="X82" t="s">
@@ -18272,15 +18293,15 @@
     </row>
     <row r="83" spans="2:24">
       <c r="K83" s="9" t="str">
-        <f>IF(LEN(C83),VLOOKUP(C83,mROW,3,FALSE),"")</f>
+        <f t="shared" si="2"/>
         <v/>
       </c>
       <c r="V83" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>mROW_CFG_CATEGORY_CHOICE</v>
       </c>
       <c r="W83">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>35</v>
       </c>
       <c r="X83" t="s">
@@ -18298,15 +18319,15 @@
         <v>3721</v>
       </c>
       <c r="K84" s="9" t="str">
-        <f>IF(LEN(C84),VLOOKUP(C84,mROW,3,FALSE),"")</f>
+        <f t="shared" si="2"/>
         <v>#define mROW_CFG_EFFECT_NEXT 48</v>
       </c>
       <c r="V84" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>mROW_CFG_TYPE</v>
       </c>
       <c r="W84">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>36</v>
       </c>
       <c r="X84" t="s">
@@ -18315,15 +18336,15 @@
     </row>
     <row r="85" spans="2:24">
       <c r="K85" s="9" t="str">
-        <f>IF(LEN(C85),VLOOKUP(C85,mROW,3,FALSE),"")</f>
+        <f t="shared" si="2"/>
         <v/>
       </c>
       <c r="V85" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>mROW_CFG_TYPE_LOOPSTART</v>
       </c>
       <c r="W85">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>37</v>
       </c>
       <c r="X85" t="s">
@@ -18341,15 +18362,15 @@
         <v>3716</v>
       </c>
       <c r="K86" s="9" t="str">
-        <f>IF(LEN(C86),VLOOKUP(C86,mROW,3,FALSE),"")</f>
+        <f t="shared" si="2"/>
         <v>#define mROW_CFG_EFFECT_CHOICE 49</v>
       </c>
       <c r="V86" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>mROW_CFG_TYPE_LOOP</v>
       </c>
       <c r="W86">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>40</v>
       </c>
       <c r="X86" t="s">
@@ -18358,11 +18379,11 @@
     </row>
     <row r="87" spans="2:24">
       <c r="V87" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>mROW_CFG_TYPE_NEXT</v>
       </c>
       <c r="W87">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>42</v>
       </c>
       <c r="X87" t="s">
@@ -18371,11 +18392,11 @@
     </row>
     <row r="88" spans="2:24">
       <c r="V88" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>mROW_CFG_TYPE_CHOICE</v>
       </c>
       <c r="W88">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>43</v>
       </c>
       <c r="X88" t="s">
@@ -18384,11 +18405,11 @@
     </row>
     <row r="89" spans="2:24">
       <c r="V89" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>mROW_CFG_EFFECT</v>
       </c>
       <c r="W89">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>44</v>
       </c>
       <c r="X89" t="s">
@@ -18397,11 +18418,11 @@
     </row>
     <row r="90" spans="2:24">
       <c r="V90" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>mROW_CFG_EFFECT_LOOPSTART</v>
       </c>
       <c r="W90">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>45</v>
       </c>
       <c r="X90" t="s">
@@ -18410,11 +18431,11 @@
     </row>
     <row r="91" spans="2:24">
       <c r="V91" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>mROW_CFG_EFFECT_LOOP</v>
       </c>
       <c r="W91">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>46</v>
       </c>
       <c r="X91" t="s">
@@ -18423,11 +18444,11 @@
     </row>
     <row r="92" spans="2:24">
       <c r="V92" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>mROW_CFG_EFFECT_NEXT</v>
       </c>
       <c r="W92">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>48</v>
       </c>
       <c r="X92" t="s">
@@ -18436,11 +18457,11 @@
     </row>
     <row r="93" spans="2:24">
       <c r="V93" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>mROW_CFG_EFFECT_CHOICE</v>
       </c>
       <c r="W93">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>49</v>
       </c>
       <c r="X93" t="s">
@@ -18470,15 +18491,15 @@
   <sheetData>
     <row r="1" spans="1:24">
       <c r="K1" s="9" t="str">
-        <f>IF(LEN(C1),VLOOKUP(C1,mROW,3,FALSE),"")</f>
+        <f t="shared" ref="K1:K16" si="0">IF(LEN(C1),VLOOKUP(C1,mROW,3,FALSE),"")</f>
         <v/>
       </c>
       <c r="V1" t="str">
-        <f>MID(X1,9,FIND(" ",X1,9)-9)</f>
+        <f t="shared" ref="V1:V14" si="1">MID(X1,9,FIND(" ",X1,9)-9)</f>
         <v>mROW_MENU</v>
       </c>
       <c r="W1">
-        <f>0+MID(X1,10+LEN(V1),2)</f>
+        <f t="shared" ref="W1:W14" si="2">0+MID(X1,10+LEN(V1),2)</f>
         <v>7</v>
       </c>
       <c r="X1" s="15" t="s">
@@ -18487,22 +18508,22 @@
     </row>
     <row r="2" spans="1:24">
       <c r="K2" s="9" t="str">
-        <f>IF(LEN(C2),VLOOKUP(C2,mROW,3,FALSE),"")</f>
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="V2" t="str">
-        <f>MID(X2,9,FIND(" ",X2,9)-9)</f>
+        <f t="shared" si="1"/>
         <v>mROW_MENU</v>
       </c>
       <c r="W2">
-        <f>0+MID(X2,10+LEN(V2),2)</f>
+        <f t="shared" si="2"/>
         <v>7</v>
       </c>
       <c r="X2" s="15" t="s">
         <v>3435</v>
       </c>
     </row>
-    <row r="3" spans="1:24" ht="135">
+    <row r="3" spans="1:24" ht="405">
       <c r="A3" s="62" t="s">
         <v>3671</v>
       </c>
@@ -18525,22 +18546,22 @@
         <v>39</v>
       </c>
       <c r="K3" s="9" t="e">
-        <f>IF(LEN(C3),VLOOKUP(C3,mROW,3,FALSE),"")</f>
+        <f t="shared" si="0"/>
         <v>#N/A</v>
       </c>
       <c r="V3" t="str">
-        <f>MID(X3,9,FIND(" ",X3,9)-9)</f>
+        <f t="shared" si="1"/>
         <v>mROW_MENU_CLOSED</v>
       </c>
       <c r="W3">
-        <f>0+MID(X3,10+LEN(V3),2)</f>
+        <f t="shared" si="2"/>
         <v>11</v>
       </c>
       <c r="X3" s="15" t="s">
         <v>3437</v>
       </c>
     </row>
-    <row r="4" spans="1:24">
+    <row r="4" spans="1:24" ht="45">
       <c r="A4" s="62"/>
       <c r="B4" s="78" t="s">
         <v>35</v>
@@ -18561,22 +18582,22 @@
         <v>3706</v>
       </c>
       <c r="K4" s="9" t="e">
-        <f>IF(LEN(C4),VLOOKUP(C4,mROW,3,FALSE),"")</f>
+        <f t="shared" si="0"/>
         <v>#N/A</v>
       </c>
       <c r="V4" t="str">
-        <f>MID(X4,9,FIND(" ",X4,9)-9)</f>
+        <f t="shared" si="1"/>
         <v>mROW_MENU_OPEN</v>
       </c>
       <c r="W4">
-        <f>0+MID(X4,10+LEN(V4),2)</f>
+        <f t="shared" si="2"/>
         <v>9</v>
       </c>
       <c r="X4" s="15" t="s">
         <v>3436</v>
       </c>
     </row>
-    <row r="5" spans="1:24">
+    <row r="5" spans="1:24" ht="45">
       <c r="A5" s="62"/>
       <c r="B5" s="78" t="s">
         <v>35</v>
@@ -18597,22 +18618,22 @@
         <v>3704</v>
       </c>
       <c r="K5" s="9" t="e">
-        <f>IF(LEN(C5),VLOOKUP(C5,mROW,3,FALSE),"")</f>
+        <f t="shared" si="0"/>
         <v>#N/A</v>
       </c>
       <c r="V5" t="str">
-        <f>MID(X5,9,FIND(" ",X5,9)-9)</f>
+        <f t="shared" si="1"/>
         <v>mROW_MENUCFG</v>
       </c>
       <c r="W5">
-        <f>0+MID(X5,10+LEN(V5),2)</f>
+        <f t="shared" si="2"/>
         <v>24</v>
       </c>
       <c r="X5" s="15" t="s">
         <v>3447</v>
       </c>
     </row>
-    <row r="6" spans="1:24">
+    <row r="6" spans="1:24" ht="45">
       <c r="A6" s="62"/>
       <c r="B6" s="78" t="s">
         <v>35</v>
@@ -18633,15 +18654,15 @@
         <v>3705</v>
       </c>
       <c r="K6" s="9" t="e">
-        <f>IF(LEN(C6),VLOOKUP(C6,mROW,3,FALSE),"")</f>
+        <f t="shared" si="0"/>
         <v>#N/A</v>
       </c>
       <c r="V6" t="str">
-        <f>MID(X6,9,FIND(" ",X6,9)-9)</f>
+        <f t="shared" si="1"/>
         <v>mROW_MENUCFG</v>
       </c>
       <c r="W6">
-        <f>0+MID(X6,10+LEN(V6),2)</f>
+        <f t="shared" si="2"/>
         <v>24</v>
       </c>
       <c r="X6" s="15" t="s">
@@ -18653,15 +18674,15 @@
       <c r="D7" s="3"/>
       <c r="E7" s="2"/>
       <c r="K7" s="9" t="str">
-        <f>IF(LEN(C7),VLOOKUP(C7,mROW,3,FALSE),"")</f>
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="V7" t="str">
-        <f>MID(X7,9,FIND(" ",X7,9)-9)</f>
+        <f t="shared" si="1"/>
         <v>mROW_OPNBRL</v>
       </c>
       <c r="W7">
-        <f>0+MID(X7,10+LEN(V7),2)</f>
+        <f t="shared" si="2"/>
         <v>19</v>
       </c>
       <c r="X7" s="15" t="s">
@@ -18673,22 +18694,22 @@
       <c r="D8" s="3"/>
       <c r="E8" s="2"/>
       <c r="K8" s="9" t="str">
-        <f>IF(LEN(C8),VLOOKUP(C8,mROW,3,FALSE),"")</f>
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="V8" t="str">
-        <f>MID(X8,9,FIND(" ",X8,9)-9)</f>
+        <f t="shared" si="1"/>
         <v>mROW_POWERON</v>
       </c>
       <c r="W8">
-        <f>0+MID(X8,10+LEN(V8),2)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="X8" s="15" t="s">
         <v>3211</v>
       </c>
     </row>
-    <row r="9" spans="1:24" ht="30">
+    <row r="9" spans="1:24" ht="60">
       <c r="A9" s="62" t="s">
         <v>3406</v>
       </c>
@@ -18708,15 +18729,15 @@
         <v>3402</v>
       </c>
       <c r="K9" s="9" t="e">
-        <f>IF(LEN(C9),VLOOKUP(C9,mROW,3,FALSE),"")</f>
+        <f t="shared" si="0"/>
         <v>#N/A</v>
       </c>
       <c r="V9" t="str">
-        <f>MID(X9,9,FIND(" ",X9,9)-9)</f>
+        <f t="shared" si="1"/>
         <v>mROW_PWRON_LOCKED</v>
       </c>
       <c r="W9">
-        <f>0+MID(X9,10+LEN(V9),2)</f>
+        <f t="shared" si="2"/>
         <v>4</v>
       </c>
       <c r="X9" s="15" t="s">
@@ -18728,22 +18749,22 @@
       <c r="C10" s="9"/>
       <c r="E10" s="2"/>
       <c r="K10" s="9" t="str">
-        <f>IF(LEN(C10),VLOOKUP(C10,mROW,3,FALSE),"")</f>
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="V10" t="str">
-        <f>MID(X10,9,FIND(" ",X10,9)-9)</f>
+        <f t="shared" si="1"/>
         <v>mROW_PWRON_OPEN</v>
       </c>
       <c r="W10">
-        <f>0+MID(X10,10+LEN(V10),2)</f>
+        <f t="shared" si="2"/>
         <v>2</v>
       </c>
       <c r="X10" s="15" t="s">
         <v>3248</v>
       </c>
     </row>
-    <row r="11" spans="1:24" ht="30">
+    <row r="11" spans="1:24" ht="60">
       <c r="A11" s="62" t="s">
         <v>3406</v>
       </c>
@@ -18763,15 +18784,15 @@
         <v>3402</v>
       </c>
       <c r="K11" s="9" t="e">
-        <f>IF(LEN(C11),VLOOKUP(C11,mROW,3,FALSE),"")</f>
+        <f t="shared" si="0"/>
         <v>#N/A</v>
       </c>
       <c r="V11" t="str">
-        <f>MID(X11,9,FIND(" ",X11,9)-9)</f>
+        <f t="shared" si="1"/>
         <v>mROW_SHOOT</v>
       </c>
       <c r="W11">
-        <f>0+MID(X11,10+LEN(V11),2)</f>
+        <f t="shared" si="2"/>
         <v>16</v>
       </c>
       <c r="X11" s="15" t="s">
@@ -18783,22 +18804,22 @@
       <c r="C12" s="9"/>
       <c r="E12" s="2"/>
       <c r="K12" s="9" t="str">
-        <f>IF(LEN(C12),VLOOKUP(C12,mROW,3,FALSE),"")</f>
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="V12" t="str">
-        <f>MID(X12,9,FIND(" ",X12,9)-9)</f>
+        <f t="shared" si="1"/>
         <v>mROW_SHOOT_SOUND</v>
       </c>
       <c r="W12">
-        <f>0+MID(X12,10+LEN(V12),2)</f>
+        <f t="shared" si="2"/>
         <v>17</v>
       </c>
       <c r="X12" s="15" t="s">
         <v>3443</v>
       </c>
     </row>
-    <row r="13" spans="1:24" ht="45">
+    <row r="13" spans="1:24" ht="150">
       <c r="A13" s="62" t="s">
         <v>3411</v>
       </c>
@@ -18822,15 +18843,15 @@
         <v>3707</v>
       </c>
       <c r="K13" s="9" t="e">
-        <f>IF(LEN(C13),VLOOKUP(C13,mROW,3,FALSE),"")</f>
+        <f t="shared" si="0"/>
         <v>#N/A</v>
       </c>
       <c r="V13" t="str">
-        <f>MID(X13,9,FIND(" ",X13,9)-9)</f>
+        <f t="shared" si="1"/>
         <v>mROW_SOLENOID</v>
       </c>
       <c r="W13">
-        <f>0+MID(X13,10+LEN(V13),2)</f>
+        <f t="shared" si="2"/>
         <v>18</v>
       </c>
       <c r="X13" s="15" t="s">
@@ -18841,22 +18862,22 @@
       <c r="A14" s="62"/>
       <c r="E14" s="2"/>
       <c r="K14" s="9" t="str">
-        <f>IF(LEN(C14),VLOOKUP(C14,mROW,3,FALSE),"")</f>
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="V14" t="str">
-        <f>MID(X14,9,FIND(" ",X14,9)-9)</f>
+        <f t="shared" si="1"/>
         <v>mROW_WINDUP_SOUND</v>
       </c>
       <c r="W14">
-        <f>0+MID(X14,10+LEN(V14),2)</f>
+        <f t="shared" si="2"/>
         <v>15</v>
       </c>
       <c r="X14" s="15" t="s">
         <v>3441</v>
       </c>
     </row>
-    <row r="15" spans="1:24" ht="75">
+    <row r="15" spans="1:24" ht="195">
       <c r="A15" s="62" t="s">
         <v>3418</v>
       </c>
@@ -18882,13 +18903,13 @@
       </c>
       <c r="J15" s="9"/>
       <c r="K15" s="9" t="e">
-        <f>IF(LEN(C15),VLOOKUP(C15,mROW,3,FALSE),"")</f>
+        <f t="shared" si="0"/>
         <v>#N/A</v>
       </c>
     </row>
     <row r="16" spans="1:24">
       <c r="K16" s="9" t="str">
-        <f>IF(LEN(C16),VLOOKUP(C16,mROW,3,FALSE),"")</f>
+        <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
@@ -18906,11 +18927,11 @@
     </row>
     <row r="19" spans="1:11">
       <c r="K19" s="9" t="str">
-        <f>IF(LEN(C19),VLOOKUP(C19,mROW,3,FALSE),"")</f>
+        <f t="shared" ref="K19:K24" si="3">IF(LEN(C19),VLOOKUP(C19,mROW,3,FALSE),"")</f>
         <v/>
       </c>
     </row>
-    <row r="20" spans="1:11" ht="45">
+    <row r="20" spans="1:11" ht="150">
       <c r="B20" s="10" t="s">
         <v>3415</v>
       </c>
@@ -18921,17 +18942,17 @@
         <v>3710</v>
       </c>
       <c r="K20" s="9" t="e">
-        <f>IF(LEN(C20),VLOOKUP(C20,mROW,3,FALSE),"")</f>
+        <f t="shared" si="3"/>
         <v>#N/A</v>
       </c>
     </row>
     <row r="21" spans="1:11">
       <c r="K21" s="9" t="str">
-        <f>IF(LEN(C21),VLOOKUP(C21,mROW,3,FALSE),"")</f>
+        <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
-    <row r="22" spans="1:11" ht="45">
+    <row r="22" spans="1:11" ht="150">
       <c r="B22" s="10" t="s">
         <v>3416</v>
       </c>
@@ -18942,23 +18963,23 @@
         <v>3402</v>
       </c>
       <c r="K22" s="9" t="e">
-        <f>IF(LEN(C22),VLOOKUP(C22,mROW,3,FALSE),"")</f>
+        <f t="shared" si="3"/>
         <v>#N/A</v>
       </c>
     </row>
     <row r="23" spans="1:11">
       <c r="K23" s="9" t="str">
-        <f>IF(LEN(C23),VLOOKUP(C23,mROW,3,FALSE),"")</f>
+        <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
     <row r="24" spans="1:11">
       <c r="K24" s="9" t="str">
-        <f>IF(LEN(C24),VLOOKUP(C24,mROW,3,FALSE),"")</f>
+        <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
-    <row r="25" spans="1:11" ht="75">
+    <row r="25" spans="1:11" ht="225">
       <c r="A25" s="62" t="s">
         <v>3677</v>
       </c>
@@ -18969,15 +18990,15 @@
         <v>3672</v>
       </c>
       <c r="E25" t="str">
-        <f>TEXT(B25,"0000")&amp;"__mdo47__"&amp;D25&amp;".wav"</f>
+        <f t="shared" ref="E25:E31" si="4">TEXT(B25,"0000")&amp;"__mdo47__"&amp;D25&amp;".wav"</f>
         <v>0066__mdo47__TypeChoices.wav</v>
       </c>
       <c r="G25" t="str">
-        <f>"mdo47 recording of """&amp;A25&amp;""""</f>
+        <f t="shared" ref="G25:G31" si="5">"mdo47 recording of """&amp;A25&amp;""""</f>
         <v>mdo47 recording of "Press just trigger to cycle through effect TYPE choices, trigger + any color to choose the effect TYPE."</v>
       </c>
     </row>
-    <row r="26" spans="1:11" ht="45">
+    <row r="26" spans="1:11" ht="150">
       <c r="A26" s="62" t="s">
         <v>3679</v>
       </c>
@@ -18991,15 +19012,15 @@
         <v>3678</v>
       </c>
       <c r="E26" t="str">
-        <f>TEXT(B26,"0000")&amp;"__mdo47__"&amp;D26&amp;".wav"</f>
+        <f t="shared" si="4"/>
         <v>0071__mdo47__ChargeUpForShooting.wav</v>
       </c>
       <c r="G26" t="str">
-        <f>"mdo47 recording of """&amp;A26&amp;""""</f>
+        <f t="shared" si="5"/>
         <v>mdo47 recording of "Effect type CHARGE-UP FOR SHOOTING. Trigger alone for next type."</v>
       </c>
     </row>
-    <row r="27" spans="1:11" ht="30">
+    <row r="27" spans="1:11" ht="120">
       <c r="A27" s="62" t="s">
         <v>3680</v>
       </c>
@@ -19013,15 +19034,15 @@
         <v>3673</v>
       </c>
       <c r="E27" t="str">
-        <f>TEXT(B27,"0000")&amp;"__mdo47__"&amp;D27&amp;".wav"</f>
+        <f t="shared" si="4"/>
         <v>0072__mdo47__Shoot.wav</v>
       </c>
       <c r="G27" t="str">
-        <f>"mdo47 recording of """&amp;A27&amp;""""</f>
+        <f t="shared" si="5"/>
         <v>mdo47 recording of "Effect type SHOOTING. Trigger alone for next type."</v>
       </c>
     </row>
-    <row r="28" spans="1:11" ht="45">
+    <row r="28" spans="1:11" ht="120">
       <c r="A28" s="62" t="s">
         <v>3681</v>
       </c>
@@ -19035,15 +19056,15 @@
         <v>3674</v>
       </c>
       <c r="E28" t="str">
-        <f>TEXT(B28,"0000")&amp;"__mdo47__"&amp;D28&amp;".wav"</f>
+        <f t="shared" si="4"/>
         <v>0073__mdo47__OpenBarrel.wav</v>
       </c>
       <c r="G28" t="str">
-        <f>"mdo47 recording of """&amp;A28&amp;""""</f>
+        <f t="shared" si="5"/>
         <v>mdo47 recording of "Effect type OPEN BARREL. Trigger alone for next type."</v>
       </c>
     </row>
-    <row r="29" spans="1:11" ht="45">
+    <row r="29" spans="1:11" ht="135">
       <c r="A29" s="62" t="s">
         <v>3682</v>
       </c>
@@ -19057,15 +19078,15 @@
         <v>3675</v>
       </c>
       <c r="E29" t="str">
-        <f>TEXT(B29,"0000")&amp;"__mdo47__"&amp;D29&amp;".wav"</f>
+        <f t="shared" si="4"/>
         <v>0074__mdo47__LockAndLoad.wav</v>
       </c>
       <c r="G29" t="str">
-        <f>"mdo47 recording of """&amp;A29&amp;""""</f>
+        <f t="shared" si="5"/>
         <v>mdo47 recording of "Effect type LOCK-AND-LOAD. Trigger alone for next type."</v>
       </c>
     </row>
-    <row r="30" spans="1:11" ht="45">
+    <row r="30" spans="1:11" ht="120">
       <c r="A30" s="62" t="s">
         <v>3683</v>
       </c>
@@ -19079,15 +19100,15 @@
         <v>3379</v>
       </c>
       <c r="E30" t="str">
-        <f>TEXT(B30,"0000")&amp;"__mdo47__"&amp;D30&amp;".wav"</f>
+        <f t="shared" si="4"/>
         <v>0075__mdo47__PowerOn.wav</v>
       </c>
       <c r="G30" t="str">
-        <f>"mdo47 recording of """&amp;A30&amp;""""</f>
+        <f t="shared" si="5"/>
         <v>mdo47 recording of "Effect type POWER-ON. Trigger alone for next type."</v>
       </c>
     </row>
-    <row r="31" spans="1:11" ht="45">
+    <row r="31" spans="1:11" ht="135">
       <c r="A31" s="62" t="s">
         <v>3684</v>
       </c>
@@ -19101,11 +19122,11 @@
         <v>3676</v>
       </c>
       <c r="E31" t="str">
-        <f>TEXT(B31,"0000")&amp;"__mdo47__"&amp;D31&amp;".wav"</f>
+        <f t="shared" si="4"/>
         <v>0076__mdo47__WaitingForTrigger.wav</v>
       </c>
       <c r="G31" t="str">
-        <f>"mdo47 recording of """&amp;A31&amp;""""</f>
+        <f t="shared" si="5"/>
         <v>mdo47 recording of "Effect type WAITING-FOR-TRIGGER. Trigger alone for next type."</v>
       </c>
     </row>
@@ -19121,7 +19142,7 @@
         <v/>
       </c>
     </row>
-    <row r="38" spans="4:11">
+    <row r="38" spans="4:11" ht="90">
       <c r="D38" s="10" t="s">
         <v>3688</v>
       </c>
@@ -19132,7 +19153,7 @@
         <v>3696</v>
       </c>
     </row>
-    <row r="39" spans="4:11" ht="30">
+    <row r="39" spans="4:11" ht="135">
       <c r="D39" s="10" t="s">
         <v>3689</v>
       </c>
@@ -19143,7 +19164,7 @@
         <v>3692</v>
       </c>
     </row>
-    <row r="40" spans="4:11">
+    <row r="40" spans="4:11" ht="60">
       <c r="D40" s="10" t="s">
         <v>3691</v>
       </c>
@@ -19163,7 +19184,7 @@
       <c r="D42" s="10"/>
       <c r="E42" s="10"/>
     </row>
-    <row r="43" spans="4:11" ht="45">
+    <row r="43" spans="4:11" ht="225">
       <c r="D43" s="10" t="s">
         <v>3695</v>
       </c>
@@ -41021,7 +41042,7 @@
     </row>
     <row r="2774" spans="1:2">
       <c r="A2774">
-        <f t="shared" ref="A2774:A2805" si="11">0+LEFT(B2774,FIND(":",B2774)-1)</f>
+        <f t="shared" ref="A2774:A2781" si="11">0+LEFT(B2774,FIND(":",B2774)-1)</f>
         <v>12670</v>
       </c>
       <c r="B2774" s="11" t="s">
@@ -57927,10 +57948,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A827A58D-C8A4-4858-A89B-E853C083564F}">
-  <dimension ref="A1:AK169"/>
+  <dimension ref="A1:AK170"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C40" sqref="C40"/>
+    <sheetView tabSelected="1" topLeftCell="D22" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="I30" sqref="I30:I32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
@@ -58746,15 +58767,15 @@
         <v>3378</v>
       </c>
       <c r="I29" s="27" t="s">
-        <v>4682</v>
+        <v>4696</v>
       </c>
       <c r="J29">
         <f t="shared" ref="J29:J31" si="0">LEN(I29)</f>
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="L29" s="80" t="str">
-        <f t="shared" ref="L29:L31" si="1">"#define "&amp;I29&amp;" "&amp;REPT(" ",$J$39-J29)&amp;RIGHT(TEXT(B29,"    #"),3)&amp;" // "&amp;RIGHT(LEFT(D29,LEN(D29)-1),LEN(D29)-1-FIND("""",D29))</f>
-        <v>#define mEFCT_UNIQ_LFOOF                41 // This is the awesome FOOF Rubber Band Gun, darling.</v>
+        <f t="shared" ref="L29:L31" si="1">"#define "&amp;I29&amp;" "&amp;REPT(" ",$J$40-J29)&amp;RIGHT(TEXT(B29,"    #"),3)&amp;" // "&amp;RIGHT(LEFT(D29,LEN(D29)-1),LEN(D29)-1-FIND("""",D29))</f>
+        <v>#define mEFCT_PWRON_LFOOF               41 // This is the awesome FOOF Rubber Band Gun, darling.</v>
       </c>
     </row>
     <row r="30" spans="1:37" ht="30">
@@ -58783,15 +58804,15 @@
         <v>3378</v>
       </c>
       <c r="I30" s="27" t="s">
-        <v>4683</v>
+        <v>4697</v>
       </c>
       <c r="J30">
         <f t="shared" si="0"/>
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="L30" s="80" t="str">
         <f t="shared" si="1"/>
-        <v>#define mEFCT_UNIQ_MFOOF                42 // This is the awesome FOOF Rubber Band Gun.</v>
+        <v>#define mEFCT_PWRON_MFOOF               42 // This is the awesome FOOF Rubber Band Gun.</v>
       </c>
     </row>
     <row r="31" spans="1:37" ht="30">
@@ -58820,87 +58841,98 @@
         <v>3378</v>
       </c>
       <c r="I31" s="27" t="s">
-        <v>4684</v>
+        <v>4698</v>
       </c>
       <c r="J31">
         <f t="shared" si="0"/>
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="L31" s="80" t="str">
         <f t="shared" si="1"/>
-        <v>#define mEFCT_UNIQ_CFOOF                43 // Achtung! This is the awesome FOOF Rubber Band Gun.</v>
+        <v>#define mEFCT_PWRON_CFOOF               43 // Achtung! This is the awesome FOOF Rubber Band Gun.</v>
       </c>
       <c r="P31" t="str">
-        <f>REPT(" ",J39-J40)</f>
+        <f>REPT(" ",J40-J41)</f>
         <v xml:space="preserve">              </v>
       </c>
     </row>
-    <row r="32" spans="1:37" ht="20.25">
-      <c r="A32" s="65" t="s">
-        <v>2851</v>
-      </c>
-      <c r="B32" s="65">
-        <v>51</v>
-      </c>
-      <c r="C32" s="73" t="s">
-        <v>2849</v>
-      </c>
-      <c r="D32" s="67" t="s">
-        <v>2850</v>
-      </c>
-      <c r="E32" s="67" t="s">
-        <v>2851</v>
-      </c>
-      <c r="F32" s="68" t="s">
-        <v>2867</v>
-      </c>
-      <c r="G32" s="68" t="s">
-        <v>2920</v>
-      </c>
-      <c r="H32" s="69" t="s">
-        <v>2934</v>
-      </c>
-      <c r="I32" s="28"/>
+    <row r="32" spans="1:37" ht="60">
+      <c r="A32" s="70" t="s">
+        <v>3379</v>
+      </c>
+      <c r="B32" s="19">
+        <v>44</v>
+      </c>
+      <c r="C32" s="65" t="s">
+        <v>4691</v>
+      </c>
+      <c r="D32" s="71" t="s">
+        <v>4693</v>
+      </c>
+      <c r="E32" s="70" t="s">
+        <v>3379</v>
+      </c>
+      <c r="F32" s="93" t="s">
+        <v>4694</v>
+      </c>
+      <c r="G32" s="93" t="s">
+        <v>4695</v>
+      </c>
+      <c r="H32" s="93" t="s">
+        <v>4692</v>
+      </c>
+      <c r="I32" s="27" t="s">
+        <v>4699</v>
+      </c>
+      <c r="J32">
+        <f t="shared" ref="J32" si="2">LEN(I32)</f>
+        <v>17</v>
+      </c>
+      <c r="L32" s="80" t="str">
+        <f t="shared" ref="L32" si="3">"#define "&amp;I32&amp;" "&amp;REPT(" ",$J$40-J32)&amp;RIGHT(TEXT(B32,"    #"),3)&amp;" // "&amp;RIGHT(LEFT(D32,LEN(D32)-1),LEN(D32)-1-FIND("""",D32))</f>
+        <v>#define mEFCT_PWRON_RFOOF               44 // https://lingojam.com/RobotVoiceGenerator: This is the awesome FOOF Rubber Band Gun. Be afraid.</v>
+      </c>
+      <c r="N32" s="29"/>
     </row>
     <row r="33" spans="1:12" ht="20.25">
       <c r="A33" s="65" t="s">
         <v>2851</v>
       </c>
       <c r="B33" s="65">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C33" s="73" t="s">
-        <v>2841</v>
+        <v>2849</v>
       </c>
       <c r="D33" s="67" t="s">
-        <v>2842</v>
+        <v>2850</v>
       </c>
       <c r="E33" s="67" t="s">
         <v>2851</v>
       </c>
       <c r="F33" s="68" t="s">
-        <v>2859</v>
+        <v>2867</v>
       </c>
       <c r="G33" s="68" t="s">
-        <v>2923</v>
+        <v>2920</v>
       </c>
       <c r="H33" s="69" t="s">
-        <v>2929</v>
+        <v>2934</v>
       </c>
       <c r="I33" s="28"/>
     </row>
-    <row r="34" spans="1:12" ht="30">
+    <row r="34" spans="1:12" ht="20.25">
       <c r="A34" s="65" t="s">
         <v>2851</v>
       </c>
       <c r="B34" s="65">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C34" s="73" t="s">
-        <v>2883</v>
+        <v>2841</v>
       </c>
       <c r="D34" s="67" t="s">
-        <v>3369</v>
+        <v>2842</v>
       </c>
       <c r="E34" s="67" t="s">
         <v>2851</v>
@@ -58909,10 +58941,10 @@
         <v>2859</v>
       </c>
       <c r="G34" s="68" t="s">
-        <v>2926</v>
+        <v>2923</v>
       </c>
       <c r="H34" s="69" t="s">
-        <v>2936</v>
+        <v>2929</v>
       </c>
       <c r="I34" s="28"/>
     </row>
@@ -58920,107 +58952,107 @@
       <c r="A35" s="65" t="s">
         <v>2851</v>
       </c>
-      <c r="B35" s="64">
-        <v>54</v>
+      <c r="B35" s="65">
+        <v>53</v>
       </c>
       <c r="C35" s="73" t="s">
-        <v>2893</v>
-      </c>
-      <c r="D35" s="71" t="s">
-        <v>3371</v>
-      </c>
-      <c r="E35" s="71" t="s">
+        <v>2883</v>
+      </c>
+      <c r="D35" s="67" t="s">
+        <v>3369</v>
+      </c>
+      <c r="E35" s="67" t="s">
         <v>2851</v>
       </c>
       <c r="F35" s="68" t="s">
         <v>2859</v>
       </c>
       <c r="G35" s="68" t="s">
+        <v>2926</v>
+      </c>
+      <c r="H35" s="69" t="s">
+        <v>2936</v>
+      </c>
+      <c r="I35" s="28"/>
+    </row>
+    <row r="36" spans="1:12" ht="30">
+      <c r="A36" s="65" t="s">
+        <v>2851</v>
+      </c>
+      <c r="B36" s="64">
+        <v>54</v>
+      </c>
+      <c r="C36" s="73" t="s">
+        <v>2893</v>
+      </c>
+      <c r="D36" s="71" t="s">
+        <v>3371</v>
+      </c>
+      <c r="E36" s="71" t="s">
+        <v>2851</v>
+      </c>
+      <c r="F36" s="68" t="s">
+        <v>2859</v>
+      </c>
+      <c r="G36" s="68" t="s">
         <v>2894</v>
       </c>
-      <c r="H35" s="69" t="s">
+      <c r="H36" s="69" t="s">
         <v>2899</v>
       </c>
-      <c r="I35" s="28"/>
-    </row>
-    <row r="36" spans="1:12" ht="30">
-      <c r="A36" s="70" t="s">
-        <v>2851</v>
-      </c>
-      <c r="B36" s="9">
-        <v>55</v>
-      </c>
-      <c r="C36" s="73" t="s">
-        <v>2885</v>
-      </c>
-      <c r="D36" s="67" t="s">
-        <v>2884</v>
-      </c>
-      <c r="E36" s="67" t="s">
-        <v>2851</v>
-      </c>
-      <c r="F36" s="68" t="s">
-        <v>2867</v>
-      </c>
-      <c r="G36" s="68" t="s">
-        <v>2926</v>
-      </c>
-      <c r="H36" s="69" t="s">
-        <v>2937</v>
-      </c>
       <c r="I36" s="28"/>
     </row>
-    <row r="37" spans="1:12" ht="20.25">
+    <row r="37" spans="1:12" ht="30">
       <c r="A37" s="70" t="s">
         <v>2851</v>
       </c>
-      <c r="B37" s="64">
-        <v>56</v>
-      </c>
-      <c r="C37" s="66" t="s">
-        <v>2871</v>
-      </c>
-      <c r="D37" s="71" t="s">
-        <v>3357</v>
-      </c>
-      <c r="E37" s="71" t="s">
-        <v>3376</v>
+      <c r="B37" s="9">
+        <v>55</v>
+      </c>
+      <c r="C37" s="73" t="s">
+        <v>2885</v>
+      </c>
+      <c r="D37" s="67" t="s">
+        <v>2884</v>
+      </c>
+      <c r="E37" s="67" t="s">
+        <v>2851</v>
       </c>
       <c r="F37" s="68" t="s">
         <v>2867</v>
       </c>
       <c r="G37" s="68" t="s">
-        <v>2873</v>
+        <v>2926</v>
       </c>
       <c r="H37" s="69" t="s">
-        <v>2872</v>
+        <v>2937</v>
       </c>
       <c r="I37" s="28"/>
     </row>
-    <row r="38" spans="1:12" ht="30">
+    <row r="38" spans="1:12" ht="20.25">
       <c r="A38" s="70" t="s">
         <v>2851</v>
       </c>
       <c r="B38" s="64">
-        <v>57</v>
-      </c>
-      <c r="C38" s="73" t="s">
-        <v>2839</v>
-      </c>
-      <c r="D38" s="67" t="s">
-        <v>2840</v>
-      </c>
-      <c r="E38" s="67" t="s">
-        <v>2851</v>
+        <v>56</v>
+      </c>
+      <c r="C38" s="66" t="s">
+        <v>2871</v>
+      </c>
+      <c r="D38" s="71" t="s">
+        <v>3357</v>
+      </c>
+      <c r="E38" s="71" t="s">
+        <v>3376</v>
       </c>
       <c r="F38" s="68" t="s">
         <v>2867</v>
       </c>
       <c r="G38" s="68" t="s">
-        <v>2924</v>
+        <v>2873</v>
       </c>
       <c r="H38" s="69" t="s">
-        <v>2935</v>
+        <v>2872</v>
       </c>
       <c r="I38" s="28"/>
     </row>
@@ -59029,13 +59061,13 @@
         <v>2851</v>
       </c>
       <c r="B39" s="64">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C39" s="73" t="s">
-        <v>2854</v>
+        <v>2839</v>
       </c>
       <c r="D39" s="67" t="s">
-        <v>3373</v>
+        <v>2840</v>
       </c>
       <c r="E39" s="67" t="s">
         <v>2851</v>
@@ -59044,54 +59076,44 @@
         <v>2867</v>
       </c>
       <c r="G39" s="68" t="s">
-        <v>2919</v>
+        <v>2924</v>
       </c>
       <c r="H39" s="69" t="s">
-        <v>2933</v>
-      </c>
-      <c r="J39">
-        <f>MAX(J40:J57)</f>
-        <v>30</v>
-      </c>
-      <c r="K39" t="s">
-        <v>3686</v>
-      </c>
-    </row>
-    <row r="40" spans="1:12" ht="120">
-      <c r="A40" s="71" t="s">
-        <v>3383</v>
-      </c>
-      <c r="B40" s="70">
-        <v>62</v>
-      </c>
-      <c r="C40" s="65" t="s">
-        <v>3423</v>
-      </c>
-      <c r="D40" s="10" t="s">
-        <v>4674</v>
-      </c>
-      <c r="E40" s="71" t="s">
-        <v>3383</v>
+        <v>2935</v>
+      </c>
+      <c r="I39" s="28"/>
+    </row>
+    <row r="40" spans="1:12" ht="30">
+      <c r="A40" s="70" t="s">
+        <v>2851</v>
+      </c>
+      <c r="B40" s="64">
+        <v>58</v>
+      </c>
+      <c r="C40" s="73" t="s">
+        <v>2854</v>
+      </c>
+      <c r="D40" s="67" t="s">
+        <v>3373</v>
+      </c>
+      <c r="E40" s="67" t="s">
+        <v>2851</v>
       </c>
       <c r="F40" s="68" t="s">
         <v>2867</v>
       </c>
-      <c r="G40" s="72" t="s">
-        <v>3377</v>
-      </c>
-      <c r="H40" s="70" t="s">
-        <v>3378</v>
-      </c>
-      <c r="I40" s="27" t="s">
-        <v>3438</v>
+      <c r="G40" s="68" t="s">
+        <v>2919</v>
+      </c>
+      <c r="H40" s="69" t="s">
+        <v>2933</v>
       </c>
       <c r="J40">
-        <f>LEN(I40)</f>
-        <v>16</v>
-      </c>
-      <c r="L40" s="80" t="str">
-        <f>"#define "&amp;I40&amp;" "&amp;REPT(" ",$J$39-J40)&amp;RIGHT(TEXT(B40,"    #"),3)&amp;" // "&amp;RIGHT(LEFT(D40,LEN(D40)-1),LEN(D40)-1-FIND("""",D40))</f>
-        <v>#define mEFCT_UNIQ_INTRO                62 // Welcome to the FOOF Rubber Band Gun configuration! Your call is important to us. Press trigger by itself to go forward to next step or to cycle through choices. To select a choice, first hold down any combination of Yellow, Green or Black button then press trigger. To exit configuration, hold down Blue button then press trigger.</v>
+        <f>MAX(J41:J58)</f>
+        <v>30</v>
+      </c>
+      <c r="K40" t="s">
+        <v>3686</v>
       </c>
     </row>
     <row r="41" spans="1:12" ht="120">
@@ -59099,13 +59121,13 @@
         <v>3383</v>
       </c>
       <c r="B41" s="70">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C41" s="65" t="s">
-        <v>3754</v>
+        <v>3423</v>
       </c>
       <c r="D41" s="10" t="s">
-        <v>4673</v>
+        <v>4674</v>
       </c>
       <c r="E41" s="71" t="s">
         <v>3383</v>
@@ -59120,15 +59142,15 @@
         <v>3378</v>
       </c>
       <c r="I41" s="27" t="s">
-        <v>3730</v>
+        <v>3438</v>
       </c>
       <c r="J41">
-        <f t="shared" ref="J41:J43" si="2">LEN(I41)</f>
-        <v>23</v>
+        <f>LEN(I41)</f>
+        <v>16</v>
       </c>
       <c r="L41" s="80" t="str">
-        <f t="shared" ref="L41:L44" si="3">"#define "&amp;I41&amp;" "&amp;REPT(" ",$J$39-J41)&amp;RIGHT(TEXT(B41,"    #"),3)&amp;" // "&amp;RIGHT(LEFT(D41,LEN(D41)-1),LEN(D41)-1-FIND("""",D41))</f>
-        <v>#define mEFCT_UNIQ_CFG_CATEGORY         63 // Now choose which effect category: sounds or LED patterns. As always, press trigger by itself to go forward to next step or to cycle through choices. To select a choice, first hold down any combination of Yellow, Green or Black button then press trigger. To exit configuration, hold down Blue button then press trigger.</v>
+        <f>"#define "&amp;I41&amp;" "&amp;REPT(" ",$J$40-J41)&amp;RIGHT(TEXT(B41,"    #"),3)&amp;" // "&amp;RIGHT(LEFT(D41,LEN(D41)-1),LEN(D41)-1-FIND("""",D41))</f>
+        <v>#define mEFCT_UNIQ_INTRO                62 // Welcome to the FOOF Rubber Band Gun configuration! Your call is important to us. Press trigger by itself to go forward to next step or to cycle through choices. To select a choice, first hold down any combination of Yellow, Green or Black button then press trigger. To exit configuration, hold down Blue button then press trigger.</v>
       </c>
     </row>
     <row r="42" spans="1:12" ht="120">
@@ -59136,13 +59158,13 @@
         <v>3383</v>
       </c>
       <c r="B42" s="70">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C42" s="65" t="s">
-        <v>3755</v>
+        <v>3754</v>
       </c>
       <c r="D42" s="10" t="s">
-        <v>4672</v>
+        <v>4673</v>
       </c>
       <c r="E42" s="71" t="s">
         <v>3383</v>
@@ -59157,15 +59179,15 @@
         <v>3378</v>
       </c>
       <c r="I42" s="27" t="s">
-        <v>3731</v>
+        <v>3730</v>
       </c>
       <c r="J42">
-        <f t="shared" si="2"/>
-        <v>19</v>
+        <f t="shared" ref="J42:J44" si="4">LEN(I42)</f>
+        <v>23</v>
       </c>
       <c r="L42" s="80" t="str">
-        <f t="shared" si="3"/>
-        <v>#define mEFCT_UNIQ_CFG_TYPE             64 // Now choose when the effect happens. This list includes when powering-on, when shooting, etc. As always, press trigger by itself to go forward to next step or to cycle through choices. To select a choice, first hold down any combination of Yellow, Green or Black button then press trigger. To exit configuration, hold down Blue button then press trigger.</v>
+        <f t="shared" ref="L42:L45" si="5">"#define "&amp;I42&amp;" "&amp;REPT(" ",$J$40-J42)&amp;RIGHT(TEXT(B42,"    #"),3)&amp;" // "&amp;RIGHT(LEFT(D42,LEN(D42)-1),LEN(D42)-1-FIND("""",D42))</f>
+        <v>#define mEFCT_UNIQ_CFG_CATEGORY         63 // Now choose which effect category: sounds or LED patterns. As always, press trigger by itself to go forward to next step or to cycle through choices. To select a choice, first hold down any combination of Yellow, Green or Black button then press trigger. To exit configuration, hold down Blue button then press trigger.</v>
       </c>
     </row>
     <row r="43" spans="1:12" ht="120">
@@ -59173,13 +59195,13 @@
         <v>3383</v>
       </c>
       <c r="B43" s="70">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C43" s="65" t="s">
-        <v>3756</v>
+        <v>3755</v>
       </c>
       <c r="D43" s="10" t="s">
-        <v>4671</v>
+        <v>4672</v>
       </c>
       <c r="E43" s="71" t="s">
         <v>3383</v>
@@ -59194,29 +59216,29 @@
         <v>3378</v>
       </c>
       <c r="I43" s="27" t="s">
-        <v>3732</v>
+        <v>3731</v>
       </c>
       <c r="J43">
-        <f t="shared" si="2"/>
-        <v>20</v>
+        <f t="shared" si="4"/>
+        <v>19</v>
       </c>
       <c r="L43" s="80" t="str">
-        <f t="shared" si="3"/>
-        <v>#define mEFCT_UNIQ_CFG_EFECT            65 // Now choose the effect itself. This list cycles through the effects one by one. As always, press trigger by itself to go forward to next step or to cycle through choices. To select a choice, first hold down any combination of Yellow, Green or Black button then press trigger. To exit configuration, hold down Blue button then press trigger.</v>
-      </c>
-    </row>
-    <row r="44" spans="1:12" ht="30">
+        <f t="shared" si="5"/>
+        <v>#define mEFCT_UNIQ_CFG_TYPE             64 // Now choose when the effect happens. This list includes when powering-on, when shooting, etc. As always, press trigger by itself to go forward to next step or to cycle through choices. To select a choice, first hold down any combination of Yellow, Green or Black button then press trigger. To exit configuration, hold down Blue button then press trigger.</v>
+      </c>
+    </row>
+    <row r="44" spans="1:12" ht="120">
       <c r="A44" s="71" t="s">
         <v>3383</v>
       </c>
       <c r="B44" s="70">
-        <v>71</v>
+        <v>65</v>
       </c>
       <c r="C44" s="65" t="s">
-        <v>3766</v>
+        <v>3756</v>
       </c>
       <c r="D44" s="10" t="s">
-        <v>4685</v>
+        <v>4671</v>
       </c>
       <c r="E44" s="71" t="s">
         <v>3383</v>
@@ -59231,15 +59253,15 @@
         <v>3378</v>
       </c>
       <c r="I44" s="27" t="s">
-        <v>3761</v>
+        <v>3732</v>
       </c>
       <c r="J44">
-        <f>LEN(I44)</f>
-        <v>29</v>
+        <f t="shared" si="4"/>
+        <v>20</v>
       </c>
       <c r="L44" s="80" t="str">
-        <f t="shared" si="3"/>
-        <v>#define mEFCT_UNIQ_CFG_WINDUP_DESCRIP   71 // The effect happens during wind-up to shooting</v>
+        <f t="shared" si="5"/>
+        <v>#define mEFCT_UNIQ_CFG_EFECT            65 // Now choose the effect itself. This list cycles through the effects one by one. As always, press trigger by itself to go forward to next step or to cycle through choices. To select a choice, first hold down any combination of Yellow, Green or Black button then press trigger. To exit configuration, hold down Blue button then press trigger.</v>
       </c>
     </row>
     <row r="45" spans="1:12" ht="30">
@@ -59247,13 +59269,13 @@
         <v>3383</v>
       </c>
       <c r="B45" s="70">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C45" s="65" t="s">
-        <v>3767</v>
+        <v>3766</v>
       </c>
       <c r="D45" s="10" t="s">
-        <v>4686</v>
+        <v>4682</v>
       </c>
       <c r="E45" s="71" t="s">
         <v>3383</v>
@@ -59268,89 +59290,89 @@
         <v>3378</v>
       </c>
       <c r="I45" s="27" t="s">
+        <v>3761</v>
+      </c>
+      <c r="J45">
+        <f>LEN(I45)</f>
+        <v>29</v>
+      </c>
+      <c r="L45" s="80" t="str">
+        <f t="shared" si="5"/>
+        <v>#define mEFCT_UNIQ_CFG_WINDUP_DESCRIP   71 // The effect happens during wind-up to shooting</v>
+      </c>
+    </row>
+    <row r="46" spans="1:12" ht="30">
+      <c r="A46" s="71" t="s">
+        <v>3383</v>
+      </c>
+      <c r="B46" s="70">
+        <v>72</v>
+      </c>
+      <c r="C46" s="65" t="s">
+        <v>3767</v>
+      </c>
+      <c r="D46" s="10" t="s">
+        <v>4683</v>
+      </c>
+      <c r="E46" s="71" t="s">
+        <v>3383</v>
+      </c>
+      <c r="F46" s="68" t="s">
+        <v>2867</v>
+      </c>
+      <c r="G46" s="72" t="s">
+        <v>3377</v>
+      </c>
+      <c r="H46" s="70" t="s">
+        <v>3378</v>
+      </c>
+      <c r="I46" s="27" t="s">
         <v>3760</v>
       </c>
-      <c r="J45">
-        <f t="shared" ref="J45:J51" si="4">LEN(I45)</f>
+      <c r="J46">
+        <f t="shared" ref="J46:J52" si="6">LEN(I46)</f>
         <v>28</v>
       </c>
-      <c r="L45" s="80" t="str">
-        <f t="shared" ref="L45:L49" si="5">"#define "&amp;I45&amp;" "&amp;REPT(" ",$J$39-J45)&amp;RIGHT(TEXT(B45,"    #"),3)&amp;" // "&amp;RIGHT(LEFT(D45,LEN(D45)-1),LEN(D45)-1-FIND("""",D45))</f>
+      <c r="L46" s="80" t="str">
+        <f t="shared" ref="L46:L50" si="7">"#define "&amp;I46&amp;" "&amp;REPT(" ",$J$40-J46)&amp;RIGHT(TEXT(B46,"    #"),3)&amp;" // "&amp;RIGHT(LEFT(D46,LEN(D46)-1),LEN(D46)-1-FIND("""",D46))</f>
         <v>#define mEFCT_UNIQ_CFG_SHOOT_DESCRIP    72 // The effect happens during shooting itself</v>
       </c>
     </row>
-    <row r="46" spans="1:12" ht="30">
-      <c r="A46" s="86" t="s">
+    <row r="47" spans="1:12" ht="30">
+      <c r="A47" s="86" t="s">
         <v>3383</v>
       </c>
-      <c r="B46" s="87">
+      <c r="B47" s="87">
         <v>73</v>
       </c>
-      <c r="C46" s="88" t="s">
+      <c r="C47" s="88" t="s">
         <v>3768</v>
       </c>
-      <c r="D46" s="10" t="s">
-        <v>4687</v>
-      </c>
-      <c r="E46" s="86" t="s">
+      <c r="D47" s="10" t="s">
+        <v>4684</v>
+      </c>
+      <c r="E47" s="86" t="s">
         <v>3383</v>
       </c>
-      <c r="F46" s="89" t="s">
+      <c r="F47" s="89" t="s">
         <v>2867</v>
       </c>
-      <c r="G46" s="90" t="s">
+      <c r="G47" s="90" t="s">
         <v>3377</v>
       </c>
-      <c r="H46" s="87" t="s">
+      <c r="H47" s="87" t="s">
         <v>3378</v>
       </c>
-      <c r="I46" s="27" t="s">
+      <c r="I47" s="27" t="s">
         <v>3762</v>
       </c>
-      <c r="J46">
-        <f t="shared" si="4"/>
+      <c r="J47">
+        <f t="shared" si="6"/>
         <v>27</v>
       </c>
-      <c r="L46" s="80" t="str">
-        <f t="shared" si="5"/>
+      <c r="L47" s="80" t="str">
+        <f t="shared" si="7"/>
         <v>#define mEFCT_UNIQ_CFG_OPEN_DESCRIP     73 // The effect happens during opening of the barrel</v>
-      </c>
-    </row>
-    <row r="47" spans="1:12" ht="30">
-      <c r="A47" s="71" t="s">
-        <v>3383</v>
-      </c>
-      <c r="B47" s="70">
-        <v>74</v>
-      </c>
-      <c r="C47" s="65" t="s">
-        <v>3769</v>
-      </c>
-      <c r="D47" s="67" t="s">
-        <v>4688</v>
-      </c>
-      <c r="E47" s="71" t="s">
-        <v>3383</v>
-      </c>
-      <c r="F47" s="68" t="s">
-        <v>2867</v>
-      </c>
-      <c r="G47" s="72" t="s">
-        <v>3377</v>
-      </c>
-      <c r="H47" s="70" t="s">
-        <v>3378</v>
-      </c>
-      <c r="I47" s="27" t="s">
-        <v>3763</v>
-      </c>
-      <c r="J47">
-        <f t="shared" si="4"/>
-        <v>28</v>
-      </c>
-      <c r="L47" s="80" t="str">
-        <f t="shared" si="5"/>
-        <v>#define mEFCT_UNIQ_CFG_LKLOD_DESCRIP    74 // The effect happens during lock-and-load of the barrel</v>
       </c>
     </row>
     <row r="48" spans="1:12" ht="30">
@@ -59358,13 +59380,13 @@
         <v>3383</v>
       </c>
       <c r="B48" s="70">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C48" s="65" t="s">
-        <v>3770</v>
+        <v>3769</v>
       </c>
       <c r="D48" s="67" t="s">
-        <v>4689</v>
+        <v>4685</v>
       </c>
       <c r="E48" s="71" t="s">
         <v>3383</v>
@@ -59379,29 +59401,29 @@
         <v>3378</v>
       </c>
       <c r="I48" s="27" t="s">
-        <v>3764</v>
+        <v>3763</v>
       </c>
       <c r="J48">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>28</v>
       </c>
       <c r="L48" s="80" t="str">
-        <f t="shared" si="5"/>
-        <v>#define mEFCT_UNIQ_CFG_PWRON_DESCRIP    75 // The effect happens during initial power-on</v>
-      </c>
-    </row>
-    <row r="49" spans="1:18" ht="30">
+        <f t="shared" si="7"/>
+        <v>#define mEFCT_UNIQ_CFG_LKLOD_DESCRIP    74 // The effect happens during lock-and-load of the barrel</v>
+      </c>
+    </row>
+    <row r="49" spans="1:12" ht="30">
       <c r="A49" s="71" t="s">
         <v>3383</v>
       </c>
       <c r="B49" s="70">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C49" s="65" t="s">
-        <v>3771</v>
+        <v>3770</v>
       </c>
       <c r="D49" s="67" t="s">
-        <v>4690</v>
+        <v>4686</v>
       </c>
       <c r="E49" s="71" t="s">
         <v>3383</v>
@@ -59416,29 +59438,29 @@
         <v>3378</v>
       </c>
       <c r="I49" s="27" t="s">
-        <v>3765</v>
+        <v>3764</v>
       </c>
       <c r="J49">
-        <f t="shared" si="4"/>
-        <v>27</v>
+        <f t="shared" si="6"/>
+        <v>28</v>
       </c>
       <c r="L49" s="80" t="str">
-        <f t="shared" si="5"/>
-        <v>#define mEFCT_UNIQ_CFG_WAIT_DESCRIP     76 // The effect happens when waiting to shoot</v>
-      </c>
-    </row>
-    <row r="50" spans="1:18" ht="20.25">
+        <f t="shared" si="7"/>
+        <v>#define mEFCT_UNIQ_CFG_PWRON_DESCRIP    75 // The effect happens during initial power-on</v>
+      </c>
+    </row>
+    <row r="50" spans="1:12" ht="30">
       <c r="A50" s="71" t="s">
         <v>3383</v>
       </c>
       <c r="B50" s="70">
-        <v>81</v>
-      </c>
-      <c r="C50" s="85" t="s">
-        <v>4143</v>
+        <v>76</v>
+      </c>
+      <c r="C50" s="65" t="s">
+        <v>3771</v>
       </c>
       <c r="D50" s="67" t="s">
-        <v>4691</v>
+        <v>4687</v>
       </c>
       <c r="E50" s="71" t="s">
         <v>3383</v>
@@ -59453,29 +59475,29 @@
         <v>3378</v>
       </c>
       <c r="I50" s="27" t="s">
-        <v>4141</v>
+        <v>3765</v>
       </c>
       <c r="J50">
-        <f t="shared" si="4"/>
-        <v>29</v>
+        <f t="shared" si="6"/>
+        <v>27</v>
       </c>
       <c r="L50" s="80" t="str">
-        <f t="shared" ref="L50:L51" si="6">"#define "&amp;I50&amp;" "&amp;REPT(" ",$J$39-J50)&amp;RIGHT(TEXT(B50,"    #"),3)&amp;" // "&amp;RIGHT(LEFT(D50,LEN(D50)-1),LEN(D50)-1-FIND("""",D50))</f>
-        <v>#define mEFCT_UNIQ_CFG_SOUNDS_DESCRIP   81 // The effect is SOUNDS</v>
-      </c>
-    </row>
-    <row r="51" spans="1:18" ht="20.25">
+        <f t="shared" si="7"/>
+        <v>#define mEFCT_UNIQ_CFG_WAIT_DESCRIP     76 // The effect happens when waiting to shoot</v>
+      </c>
+    </row>
+    <row r="51" spans="1:12" ht="20.25">
       <c r="A51" s="71" t="s">
         <v>3383</v>
       </c>
       <c r="B51" s="70">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C51" s="85" t="s">
-        <v>4144</v>
+        <v>4143</v>
       </c>
       <c r="D51" s="67" t="s">
-        <v>4692</v>
+        <v>4688</v>
       </c>
       <c r="E51" s="71" t="s">
         <v>3383</v>
@@ -59490,29 +59512,29 @@
         <v>3378</v>
       </c>
       <c r="I51" s="27" t="s">
-        <v>4142</v>
+        <v>4141</v>
       </c>
       <c r="J51">
-        <f t="shared" si="4"/>
-        <v>30</v>
+        <f t="shared" si="6"/>
+        <v>29</v>
       </c>
       <c r="L51" s="80" t="str">
-        <f t="shared" si="6"/>
-        <v>#define mEFCT_UNIQ_CFG_LEDPTRN_DESCRIP  82 // The effect is LED PATTERNS</v>
-      </c>
-    </row>
-    <row r="52" spans="1:18" ht="15.75" customHeight="1">
+        <f t="shared" ref="L51:L52" si="8">"#define "&amp;I51&amp;" "&amp;REPT(" ",$J$40-J51)&amp;RIGHT(TEXT(B51,"    #"),3)&amp;" // "&amp;RIGHT(LEFT(D51,LEN(D51)-1),LEN(D51)-1-FIND("""",D51))</f>
+        <v>#define mEFCT_UNIQ_CFG_SOUNDS_DESCRIP   81 // The effect is SOUNDS</v>
+      </c>
+    </row>
+    <row r="52" spans="1:12" ht="20.25">
       <c r="A52" s="71" t="s">
         <v>3383</v>
       </c>
       <c r="B52" s="70">
-        <v>101</v>
-      </c>
-      <c r="C52" s="65" t="s">
-        <v>3382</v>
-      </c>
-      <c r="D52" s="71" t="s">
-        <v>3685</v>
+        <v>82</v>
+      </c>
+      <c r="C52" s="85" t="s">
+        <v>4144</v>
+      </c>
+      <c r="D52" s="67" t="s">
+        <v>4689</v>
       </c>
       <c r="E52" s="71" t="s">
         <v>3383</v>
@@ -59527,29 +59549,29 @@
         <v>3378</v>
       </c>
       <c r="I52" s="27" t="s">
-        <v>3431</v>
+        <v>4142</v>
       </c>
       <c r="J52">
-        <f t="shared" ref="J52:J57" si="7">LEN(I52)</f>
-        <v>18</v>
+        <f t="shared" si="6"/>
+        <v>30</v>
       </c>
       <c r="L52" s="80" t="str">
-        <f t="shared" ref="L52:L53" si="8">"#define "&amp;I52&amp;" "&amp;REPT(" ",$J$39-J52)&amp;RIGHT(TEXT(B52,"    #"),3)&amp;" // "&amp;RIGHT(LEFT(D52,LEN(D52)-1),LEN(D52)-1-FIND("""",D52))</f>
-        <v>#define mEFCT_UNIQ_SILENCE             101 // silence</v>
-      </c>
-    </row>
-    <row r="53" spans="1:18" ht="30">
+        <f t="shared" si="8"/>
+        <v>#define mEFCT_UNIQ_CFG_LEDPTRN_DESCRIP  82 // The effect is LED PATTERNS</v>
+      </c>
+    </row>
+    <row r="53" spans="1:12" ht="15.75" customHeight="1">
       <c r="A53" s="71" t="s">
         <v>3383</v>
       </c>
       <c r="B53" s="70">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C53" s="65" t="s">
-        <v>3417</v>
+        <v>3382</v>
       </c>
       <c r="D53" s="71" t="s">
-        <v>4693</v>
+        <v>3685</v>
       </c>
       <c r="E53" s="71" t="s">
         <v>3383</v>
@@ -59564,77 +59586,77 @@
         <v>3378</v>
       </c>
       <c r="I53" s="27" t="s">
+        <v>3431</v>
+      </c>
+      <c r="J53">
+        <f t="shared" ref="J53:J58" si="9">LEN(I53)</f>
+        <v>18</v>
+      </c>
+      <c r="L53" s="80" t="str">
+        <f t="shared" ref="L53:L54" si="10">"#define "&amp;I53&amp;" "&amp;REPT(" ",$J$40-J53)&amp;RIGHT(TEXT(B53,"    #"),3)&amp;" // "&amp;RIGHT(LEFT(D53,LEN(D53)-1),LEN(D53)-1-FIND("""",D53))</f>
+        <v>#define mEFCT_UNIQ_SILENCE             101 // silence</v>
+      </c>
+    </row>
+    <row r="54" spans="1:12" ht="30">
+      <c r="A54" s="71" t="s">
+        <v>3383</v>
+      </c>
+      <c r="B54" s="70">
+        <v>102</v>
+      </c>
+      <c r="C54" s="65" t="s">
+        <v>3417</v>
+      </c>
+      <c r="D54" s="71" t="s">
+        <v>4690</v>
+      </c>
+      <c r="E54" s="71" t="s">
+        <v>3383</v>
+      </c>
+      <c r="F54" s="68" t="s">
+        <v>2867</v>
+      </c>
+      <c r="G54" s="72" t="s">
+        <v>3377</v>
+      </c>
+      <c r="H54" s="70" t="s">
+        <v>3378</v>
+      </c>
+      <c r="I54" s="27" t="s">
         <v>3432</v>
       </c>
-      <c r="J53">
-        <f t="shared" si="7"/>
+      <c r="J54">
+        <f t="shared" si="9"/>
         <v>19</v>
       </c>
-      <c r="L53" s="80" t="str">
-        <f t="shared" si="8"/>
+      <c r="L54" s="80" t="str">
+        <f t="shared" si="10"/>
         <v>#define mEFCT_UNIQ_NOT_IMPL            102 // This feature is not yet implemented</v>
       </c>
     </row>
-    <row r="54" spans="1:18" ht="20.25">
-      <c r="A54" s="19"/>
-      <c r="B54" s="19"/>
-      <c r="C54" s="19"/>
-      <c r="D54" s="19"/>
-      <c r="E54" s="71"/>
-      <c r="F54" s="68"/>
-      <c r="G54" s="72"/>
-      <c r="H54" s="70"/>
-      <c r="I54" s="27"/>
-    </row>
-    <row r="55" spans="1:18" ht="120.75">
-      <c r="A55" s="71" t="s">
-        <v>3383</v>
-      </c>
-      <c r="B55" s="70">
-        <v>63</v>
-      </c>
-      <c r="C55" s="84" t="s">
-        <v>3754</v>
-      </c>
-      <c r="D55" s="83" t="s">
-        <v>3757</v>
-      </c>
-      <c r="E55" s="71" t="s">
-        <v>3383</v>
-      </c>
-      <c r="F55" s="68" t="s">
-        <v>2867</v>
-      </c>
-      <c r="G55" s="72" t="s">
-        <v>3377</v>
-      </c>
-      <c r="H55" s="70" t="s">
-        <v>3378</v>
-      </c>
-      <c r="I55" s="27" t="s">
-        <v>3730</v>
-      </c>
-      <c r="J55">
-        <f t="shared" si="7"/>
-        <v>23</v>
-      </c>
-      <c r="L55" s="80" t="str">
-        <f t="shared" ref="L55:L57" si="9">"#define "&amp;I55&amp;" "&amp;REPT(" ",$J$39-J55)&amp;RIGHT(TEXT(B55,"    #"),3)&amp;" // "&amp;RIGHT(LEFT(D55,LEN(D55)-1),LEN(D55)-1-FIND("""",D55))</f>
-        <v>#define mEFCT_UNIQ_CFG_CATEGORY         63 // Now choose which effect category: sounds or LED patterns. As always, press trigger by itself to go forward to next step or to cycle through choices. To select a choice, first hold down any combination of Yellow, Green or Black button then press trigger. To exit configuration, hold down Blue button thenpress trigger.</v>
-      </c>
-    </row>
-    <row r="56" spans="1:18" ht="120.75">
+    <row r="55" spans="1:12" ht="20.25">
+      <c r="A55" s="19"/>
+      <c r="B55" s="19"/>
+      <c r="C55" s="19"/>
+      <c r="D55" s="19"/>
+      <c r="E55" s="71"/>
+      <c r="F55" s="68"/>
+      <c r="G55" s="72"/>
+      <c r="H55" s="70"/>
+      <c r="I55" s="27"/>
+    </row>
+    <row r="56" spans="1:12" ht="120.75">
       <c r="A56" s="71" t="s">
         <v>3383</v>
       </c>
       <c r="B56" s="70">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C56" s="84" t="s">
-        <v>3755</v>
+        <v>3754</v>
       </c>
       <c r="D56" s="83" t="s">
-        <v>3759</v>
+        <v>3757</v>
       </c>
       <c r="E56" s="71" t="s">
         <v>3383</v>
@@ -59649,29 +59671,29 @@
         <v>3378</v>
       </c>
       <c r="I56" s="27" t="s">
-        <v>3731</v>
+        <v>3730</v>
       </c>
       <c r="J56">
-        <f t="shared" si="7"/>
-        <v>19</v>
+        <f t="shared" si="9"/>
+        <v>23</v>
       </c>
       <c r="L56" s="80" t="str">
-        <f t="shared" si="9"/>
-        <v>#define mEFCT_UNIQ_CFG_TYPE             64 // Now choose when the effect happens. This list includes when powering-on, when shooting, etc. As always, press trigger by itself to go forward to next step or to cycle through choices. To select a choice, first hold down any combination of Yellow, Green or Black button then press trigger. To exit configuration, hold down Blue button thenpress trigger.</v>
-      </c>
-    </row>
-    <row r="57" spans="1:18" ht="120.75">
+        <f t="shared" ref="L56:L58" si="11">"#define "&amp;I56&amp;" "&amp;REPT(" ",$J$40-J56)&amp;RIGHT(TEXT(B56,"    #"),3)&amp;" // "&amp;RIGHT(LEFT(D56,LEN(D56)-1),LEN(D56)-1-FIND("""",D56))</f>
+        <v>#define mEFCT_UNIQ_CFG_CATEGORY         63 // Now choose which effect category: sounds or LED patterns. As always, press trigger by itself to go forward to next step or to cycle through choices. To select a choice, first hold down any combination of Yellow, Green or Black button then press trigger. To exit configuration, hold down Blue button thenpress trigger.</v>
+      </c>
+    </row>
+    <row r="57" spans="1:12" ht="120.75">
       <c r="A57" s="71" t="s">
         <v>3383</v>
       </c>
       <c r="B57" s="70">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C57" s="84" t="s">
-        <v>3756</v>
+        <v>3755</v>
       </c>
       <c r="D57" s="83" t="s">
-        <v>3758</v>
+        <v>3759</v>
       </c>
       <c r="E57" s="71" t="s">
         <v>3383</v>
@@ -59686,135 +59708,147 @@
         <v>3378</v>
       </c>
       <c r="I57" s="27" t="s">
+        <v>3731</v>
+      </c>
+      <c r="J57">
+        <f t="shared" si="9"/>
+        <v>19</v>
+      </c>
+      <c r="L57" s="80" t="str">
+        <f t="shared" si="11"/>
+        <v>#define mEFCT_UNIQ_CFG_TYPE             64 // Now choose when the effect happens. This list includes when powering-on, when shooting, etc. As always, press trigger by itself to go forward to next step or to cycle through choices. To select a choice, first hold down any combination of Yellow, Green or Black button then press trigger. To exit configuration, hold down Blue button thenpress trigger.</v>
+      </c>
+    </row>
+    <row r="58" spans="1:12" ht="120.75">
+      <c r="A58" s="71" t="s">
+        <v>3383</v>
+      </c>
+      <c r="B58" s="70">
+        <v>65</v>
+      </c>
+      <c r="C58" s="84" t="s">
+        <v>3756</v>
+      </c>
+      <c r="D58" s="83" t="s">
+        <v>3758</v>
+      </c>
+      <c r="E58" s="71" t="s">
+        <v>3383</v>
+      </c>
+      <c r="F58" s="68" t="s">
+        <v>2867</v>
+      </c>
+      <c r="G58" s="72" t="s">
+        <v>3377</v>
+      </c>
+      <c r="H58" s="70" t="s">
+        <v>3378</v>
+      </c>
+      <c r="I58" s="27" t="s">
         <v>3732</v>
       </c>
-      <c r="J57">
-        <f t="shared" si="7"/>
+      <c r="J58">
+        <f t="shared" si="9"/>
         <v>20</v>
       </c>
-      <c r="L57" s="80" t="str">
-        <f t="shared" si="9"/>
+      <c r="L58" s="80" t="str">
+        <f t="shared" si="11"/>
         <v>#define mEFCT_UNIQ_CFG_EFECT            65 // Now choose the effect itself. This list cycles through the effects one by one. As always, press trigger by itself to go forward to next step or to cycle through choices. To select a choice, first hold down any combination of Yellow, Green or Black button then press trigger. To exit configuration, hold down Blue button thenpress trigger.</v>
       </c>
     </row>
-    <row r="58" spans="1:18">
-      <c r="A58" s="92" t="s">
+    <row r="59" spans="1:12">
+      <c r="A59" s="92" t="s">
         <v>4678</v>
       </c>
-      <c r="B58" s="92" t="s">
+      <c r="B59" s="92" t="s">
         <v>4678</v>
       </c>
-      <c r="C58" s="92" t="s">
+      <c r="C59" s="92" t="s">
         <v>4678</v>
       </c>
-      <c r="D58" s="92" t="s">
+      <c r="D59" s="92" t="s">
         <v>4678</v>
       </c>
-      <c r="E58" s="92" t="s">
+      <c r="E59" s="92" t="s">
         <v>4678</v>
       </c>
-      <c r="F58" s="92" t="s">
+      <c r="F59" s="92" t="s">
         <v>4678</v>
       </c>
-      <c r="G58" s="92" t="s">
+      <c r="G59" s="92" t="s">
         <v>4678</v>
       </c>
-      <c r="H58" s="92" t="s">
+      <c r="H59" s="92" t="s">
         <v>4678</v>
       </c>
-      <c r="I58" s="92" t="s">
+      <c r="I59" s="92" t="s">
         <v>4678</v>
       </c>
     </row>
-    <row r="59" spans="1:18">
-      <c r="K59" t="s">
+    <row r="60" spans="1:12">
+      <c r="K60" t="s">
         <v>3361</v>
       </c>
     </row>
-    <row r="60" spans="1:18">
-      <c r="K60" t="s">
+    <row r="61" spans="1:12">
+      <c r="K61" t="s">
         <v>3362</v>
       </c>
     </row>
-    <row r="61" spans="1:18">
-      <c r="K61" t="s">
+    <row r="62" spans="1:12">
+      <c r="K62" t="s">
         <v>3363</v>
       </c>
     </row>
-    <row r="62" spans="1:18">
-      <c r="K62" t="s">
+    <row r="63" spans="1:12">
+      <c r="K63" t="s">
         <v>3364</v>
       </c>
     </row>
-    <row r="63" spans="1:18">
-      <c r="K63" t="s">
+    <row r="64" spans="1:12">
+      <c r="K64" t="s">
         <v>3365</v>
-      </c>
-    </row>
-    <row r="64" spans="1:18">
-      <c r="K64" t="s">
-        <v>3366</v>
-      </c>
-      <c r="R64" t="s">
-        <v>2941</v>
       </c>
     </row>
     <row r="65" spans="1:18">
       <c r="K65" t="s">
-        <v>3367</v>
+        <v>3366</v>
       </c>
       <c r="R65" t="s">
-        <v>2942</v>
+        <v>2941</v>
       </c>
     </row>
     <row r="66" spans="1:18">
       <c r="K66" t="s">
+        <v>3367</v>
+      </c>
+      <c r="R66" t="s">
+        <v>2942</v>
+      </c>
+    </row>
+    <row r="67" spans="1:18">
+      <c r="K67" t="s">
         <v>3368</v>
       </c>
-      <c r="R66" t="s">
+      <c r="R67" t="s">
         <v>2943</v>
       </c>
     </row>
-    <row r="69" spans="1:18" ht="20.25">
-      <c r="A69" s="6"/>
-      <c r="D69" s="56"/>
-      <c r="E69" s="6"/>
-      <c r="F69" s="36"/>
-      <c r="G69" s="36"/>
-      <c r="H69" s="6"/>
-    </row>
     <row r="70" spans="1:18" ht="20.25">
-      <c r="A70" s="55" t="s">
-        <v>2853</v>
-      </c>
-      <c r="B70" s="19"/>
-      <c r="C70" s="35" t="s">
-        <v>2880</v>
-      </c>
-      <c r="D70" s="34" t="s">
-        <v>3358</v>
-      </c>
-      <c r="E70" s="34" t="s">
-        <v>2853</v>
-      </c>
-      <c r="F70" s="35" t="s">
-        <v>2879</v>
-      </c>
-      <c r="G70" s="35" t="s">
-        <v>2882</v>
-      </c>
-      <c r="H70" s="52" t="s">
-        <v>2881</v>
-      </c>
-      <c r="I70" s="3"/>
+      <c r="A70" s="6"/>
+      <c r="D70" s="56"/>
+      <c r="E70" s="6"/>
+      <c r="F70" s="36"/>
+      <c r="G70" s="36"/>
+      <c r="H70" s="6"/>
     </row>
     <row r="71" spans="1:18" ht="20.25">
       <c r="A71" s="55" t="s">
         <v>2853</v>
       </c>
       <c r="B71" s="19"/>
-      <c r="C71" s="54" t="s">
-        <v>2868</v>
+      <c r="C71" s="35" t="s">
+        <v>2880</v>
       </c>
       <c r="D71" s="34" t="s">
         <v>3358</v>
@@ -59823,75 +59857,93 @@
         <v>2853</v>
       </c>
       <c r="F71" s="35" t="s">
+        <v>2879</v>
+      </c>
+      <c r="G71" s="35" t="s">
+        <v>2882</v>
+      </c>
+      <c r="H71" s="52" t="s">
+        <v>2881</v>
+      </c>
+      <c r="I71" s="3"/>
+    </row>
+    <row r="72" spans="1:18" ht="20.25">
+      <c r="A72" s="55" t="s">
+        <v>2853</v>
+      </c>
+      <c r="B72" s="19"/>
+      <c r="C72" s="54" t="s">
+        <v>2868</v>
+      </c>
+      <c r="D72" s="34" t="s">
+        <v>3358</v>
+      </c>
+      <c r="E72" s="34" t="s">
+        <v>2853</v>
+      </c>
+      <c r="F72" s="35" t="s">
         <v>2867</v>
       </c>
-      <c r="G71" s="35" t="s">
+      <c r="G72" s="35" t="s">
         <v>2870</v>
       </c>
-      <c r="H71" s="52" t="s">
+      <c r="H72" s="52" t="s">
         <v>2869</v>
       </c>
-      <c r="I71" s="3"/>
-    </row>
-    <row r="72" spans="1:18" ht="30.75">
-      <c r="A72" s="19" t="s">
-        <v>2851</v>
-      </c>
-      <c r="B72" s="19">
-        <v>57</v>
-      </c>
-      <c r="C72" s="33" t="s">
-        <v>2888</v>
-      </c>
-      <c r="D72" s="53" t="s">
-        <v>3370</v>
-      </c>
-      <c r="E72" s="19" t="s">
-        <v>2851</v>
-      </c>
-      <c r="F72" s="35" t="s">
-        <v>2859</v>
-      </c>
-      <c r="G72" s="35" t="s">
-        <v>2928</v>
-      </c>
-      <c r="H72" s="19" t="s">
-        <v>2939</v>
-      </c>
       <c r="I72" s="3"/>
     </row>
-    <row r="73" spans="1:18" ht="20.25">
+    <row r="73" spans="1:18" ht="30.75">
       <c r="A73" s="19" t="s">
         <v>2851</v>
       </c>
-      <c r="B73" s="31">
-        <v>58</v>
+      <c r="B73" s="19">
+        <v>57</v>
       </c>
       <c r="C73" s="33" t="s">
-        <v>2887</v>
+        <v>2888</v>
       </c>
       <c r="D73" s="53" t="s">
-        <v>2886</v>
+        <v>3370</v>
       </c>
       <c r="E73" s="19" t="s">
         <v>2851</v>
       </c>
       <c r="F73" s="35" t="s">
+        <v>2859</v>
+      </c>
+      <c r="G73" s="35" t="s">
+        <v>2928</v>
+      </c>
+      <c r="H73" s="19" t="s">
+        <v>2939</v>
+      </c>
+      <c r="I73" s="3"/>
+    </row>
+    <row r="74" spans="1:18" ht="20.25">
+      <c r="A74" s="19" t="s">
+        <v>2851</v>
+      </c>
+      <c r="B74" s="31">
+        <v>58</v>
+      </c>
+      <c r="C74" s="33" t="s">
+        <v>2887</v>
+      </c>
+      <c r="D74" s="53" t="s">
+        <v>2886</v>
+      </c>
+      <c r="E74" s="19" t="s">
+        <v>2851</v>
+      </c>
+      <c r="F74" s="35" t="s">
         <v>2879</v>
       </c>
-      <c r="G73" s="35" t="s">
+      <c r="G74" s="35" t="s">
         <v>2927</v>
       </c>
-      <c r="H73" s="19" t="s">
+      <c r="H74" s="19" t="s">
         <v>2938</v>
       </c>
-    </row>
-    <row r="74" spans="1:18" ht="20.25">
-      <c r="D74" s="56"/>
-      <c r="E74" s="6"/>
-      <c r="F74" s="36"/>
-      <c r="G74" s="36"/>
-      <c r="H74" s="6"/>
     </row>
     <row r="75" spans="1:18" ht="20.25">
       <c r="D75" s="56"/>
@@ -59908,9 +59960,6 @@
       <c r="H76" s="6"/>
     </row>
     <row r="77" spans="1:18" ht="20.25">
-      <c r="A77" s="6" t="s">
-        <v>3384</v>
-      </c>
       <c r="D77" s="56"/>
       <c r="E77" s="6"/>
       <c r="F77" s="36"/>
@@ -59918,8 +59967,8 @@
       <c r="H77" s="6"/>
     </row>
     <row r="78" spans="1:18" ht="20.25">
-      <c r="A78" t="s">
-        <v>3398</v>
+      <c r="A78" s="6" t="s">
+        <v>3384</v>
       </c>
       <c r="D78" s="56"/>
       <c r="E78" s="6"/>
@@ -59929,7 +59978,7 @@
     </row>
     <row r="79" spans="1:18" ht="20.25">
       <c r="A79" t="s">
-        <v>3399</v>
+        <v>3398</v>
       </c>
       <c r="D79" s="56"/>
       <c r="E79" s="6"/>
@@ -59939,7 +59988,7 @@
     </row>
     <row r="80" spans="1:18" ht="20.25">
       <c r="A80" t="s">
-        <v>3386</v>
+        <v>3399</v>
       </c>
       <c r="D80" s="56"/>
       <c r="E80" s="6"/>
@@ -59948,738 +59997,748 @@
       <c r="H80" s="6"/>
     </row>
     <row r="81" spans="1:18" ht="20.25">
-      <c r="A81" s="6" t="str">
-        <f>"&lt;tr&gt;&lt;td&gt;&lt;b&gt;"&amp;J81&amp;"&lt;/b&gt;&lt;/td&gt;&lt;td&gt;&lt;b&gt;"&amp;K81&amp;"&lt;/b&gt;&lt;/td&gt;&lt;td&gt;&lt;b&gt;"&amp;L81&amp;"&lt;/b&gt;&lt;/td&gt;&lt;td&gt;&lt;b&gt;"&amp;M81&amp;"&lt;/b&gt;&lt;/td&gt;"</f>
-        <v>&lt;tr&gt;&lt;td&gt;&lt;b&gt;Tag&lt;/b&gt;&lt;/td&gt;&lt;td&gt;&lt;b&gt;File Name&lt;/b&gt;&lt;/td&gt;&lt;td&gt;&lt;b&gt;URL&lt;/b&gt;&lt;/td&gt;&lt;td&gt;&lt;b&gt;Who&lt;/b&gt;&lt;/td&gt;</v>
-      </c>
-      <c r="J81" s="27" t="s">
-        <v>2855</v>
-      </c>
-      <c r="K81" s="27" t="s">
-        <v>2856</v>
-      </c>
-      <c r="L81" s="27" t="s">
-        <v>2857</v>
-      </c>
-      <c r="M81" s="27" t="s">
-        <v>2858</v>
-      </c>
+      <c r="A81" t="s">
+        <v>3386</v>
+      </c>
+      <c r="D81" s="56"/>
+      <c r="E81" s="6"/>
+      <c r="F81" s="36"/>
+      <c r="G81" s="36"/>
+      <c r="H81" s="6"/>
     </row>
     <row r="82" spans="1:18" ht="20.25">
       <c r="A82" s="6" t="str">
-        <f>"&lt;tr&gt;&lt;td&gt;"&amp;J82&amp;"&lt;/td&gt;&lt;td&gt;"&amp;K82&amp;"&lt;/td&gt;&lt;td&gt;"&amp;L82&amp;"&lt;/td&gt;&lt;td&gt;"&amp;M82&amp;"&lt;/td&gt;"</f>
-        <v>&lt;tr&gt;&lt;td&gt;N/A&lt;/td&gt;&lt;td&gt;GW170817-template.wav&lt;/td&gt;&lt;td&gt;https://www.gw-openscience.org/audiogwtc1/&lt;/td&gt;&lt;td&gt;LIGO detectors&lt;/td&gt;</v>
+        <f>"&lt;tr&gt;&lt;td&gt;&lt;b&gt;"&amp;J82&amp;"&lt;/b&gt;&lt;/td&gt;&lt;td&gt;&lt;b&gt;"&amp;K82&amp;"&lt;/b&gt;&lt;/td&gt;&lt;td&gt;&lt;b&gt;"&amp;L82&amp;"&lt;/b&gt;&lt;/td&gt;&lt;td&gt;&lt;b&gt;"&amp;M82&amp;"&lt;/b&gt;&lt;/td&gt;"</f>
+        <v>&lt;tr&gt;&lt;td&gt;&lt;b&gt;Tag&lt;/b&gt;&lt;/td&gt;&lt;td&gt;&lt;b&gt;File Name&lt;/b&gt;&lt;/td&gt;&lt;td&gt;&lt;b&gt;URL&lt;/b&gt;&lt;/td&gt;&lt;td&gt;&lt;b&gt;Who&lt;/b&gt;&lt;/td&gt;</v>
       </c>
       <c r="J82" s="27" t="s">
-        <v>3394</v>
+        <v>2855</v>
       </c>
       <c r="K82" s="27" t="s">
-        <v>3397</v>
-      </c>
-      <c r="L82" s="29" t="s">
-        <v>3395</v>
+        <v>2856</v>
+      </c>
+      <c r="L82" s="27" t="s">
+        <v>2857</v>
       </c>
       <c r="M82" s="27" t="s">
-        <v>3396</v>
+        <v>2858</v>
       </c>
     </row>
     <row r="83" spans="1:18" ht="20.25">
       <c r="A83" s="6" t="str">
-        <f>"&lt;tr&gt;&lt;td&gt;"&amp;J83&amp;"&lt;/td&gt;&lt;td&gt;"&amp;K83&amp;"&lt;/td&gt;&lt;td&gt;"&amp;L83&amp;"&lt;/td&gt;&lt;td&gt;"&amp;M83&amp;"&lt;/td&gt;"</f>
-        <v>&lt;tr&gt;&lt;td&gt;zero/1.0/&lt;/td&gt;&lt;td&gt;145209__lensflare8642__shotgun-sounds.mp3&lt;/td&gt;&lt;td&gt;https://freesound.org/s/145209/&lt;/td&gt;&lt;td&gt;lensflare8642&lt;/td&gt;</v>
-      </c>
-      <c r="J83" s="15" t="s">
-        <v>2859</v>
+        <f t="shared" ref="A83:A109" si="12">"&lt;tr&gt;&lt;td&gt;"&amp;J83&amp;"&lt;/td&gt;&lt;td&gt;"&amp;K83&amp;"&lt;/td&gt;&lt;td&gt;"&amp;L83&amp;"&lt;/td&gt;&lt;td&gt;"&amp;M83&amp;"&lt;/td&gt;"</f>
+        <v>&lt;tr&gt;&lt;td&gt;N/A&lt;/td&gt;&lt;td&gt;GW170817-template.wav&lt;/td&gt;&lt;td&gt;https://www.gw-openscience.org/audiogwtc1/&lt;/td&gt;&lt;td&gt;LIGO detectors&lt;/td&gt;</v>
+      </c>
+      <c r="J83" s="27" t="s">
+        <v>3394</v>
       </c>
       <c r="K83" s="27" t="s">
-        <v>2864</v>
+        <v>3397</v>
       </c>
       <c r="L83" s="29" t="s">
-        <v>2865</v>
-      </c>
-      <c r="M83" s="28" t="s">
-        <v>2866</v>
-      </c>
-      <c r="R83" t="str">
-        <f>"| "&amp;J83&amp;" | "&amp;K83&amp;" | "&amp;L83&amp;" | "&amp;M83&amp;" |"</f>
-        <v>| zero/1.0/ | 145209__lensflare8642__shotgun-sounds.mp3 | https://freesound.org/s/145209/ | lensflare8642 |</v>
+        <v>3395</v>
+      </c>
+      <c r="M83" s="27" t="s">
+        <v>3396</v>
       </c>
     </row>
     <row r="84" spans="1:18" ht="20.25">
       <c r="A84" s="6" t="str">
-        <f>"&lt;tr&gt;&lt;td&gt;"&amp;J84&amp;"&lt;/td&gt;&lt;td&gt;"&amp;K84&amp;"&lt;/td&gt;&lt;td&gt;"&amp;L84&amp;"&lt;/td&gt;&lt;td&gt;"&amp;M84&amp;"&lt;/td&gt;"</f>
-        <v>&lt;tr&gt;&lt;td&gt;zero/1.0/&lt;/td&gt;&lt;td&gt;162814__timgormly__spaceship-4.aiff&lt;/td&gt;&lt;td&gt;https://freesound.org/s/162814/&lt;/td&gt;&lt;td&gt;timgormly&lt;/td&gt;</v>
-      </c>
-      <c r="J84" s="51" t="s">
+        <f t="shared" si="12"/>
+        <v>&lt;tr&gt;&lt;td&gt;zero/1.0/&lt;/td&gt;&lt;td&gt;145209__lensflare8642__shotgun-sounds.mp3&lt;/td&gt;&lt;td&gt;https://freesound.org/s/145209/&lt;/td&gt;&lt;td&gt;lensflare8642&lt;/td&gt;</v>
+      </c>
+      <c r="J84" s="15" t="s">
         <v>2859</v>
       </c>
-      <c r="K84" s="6" t="s">
-        <v>2888</v>
-      </c>
-      <c r="L84" t="s">
-        <v>2939</v>
+      <c r="K84" s="27" t="s">
+        <v>2864</v>
+      </c>
+      <c r="L84" s="29" t="s">
+        <v>2865</v>
       </c>
       <c r="M84" s="28" t="s">
-        <v>2928</v>
+        <v>2866</v>
       </c>
       <c r="R84" t="str">
         <f>"| "&amp;J84&amp;" | "&amp;K84&amp;" | "&amp;L84&amp;" | "&amp;M84&amp;" |"</f>
-        <v>| zero/1.0/ | 162814__timgormly__spaceship-4.aiff | https://freesound.org/s/162814/ | timgormly |</v>
+        <v>| zero/1.0/ | 145209__lensflare8642__shotgun-sounds.mp3 | https://freesound.org/s/145209/ | lensflare8642 |</v>
       </c>
     </row>
     <row r="85" spans="1:18" ht="20.25">
       <c r="A85" s="6" t="str">
-        <f>"&lt;tr&gt;&lt;td&gt;"&amp;J85&amp;"&lt;/td&gt;&lt;td&gt;"&amp;K85&amp;"&lt;/td&gt;&lt;td&gt;"&amp;L85&amp;"&lt;/td&gt;&lt;td&gt;"&amp;M85&amp;"&lt;/td&gt;"</f>
-        <v>&lt;tr&gt;&lt;td&gt;by-nc/3.0/&lt;/td&gt;&lt;td&gt;165483__timbre__glitch-voice-ep-mp3.mp3&lt;/td&gt;&lt;td&gt;https://freesound.org/s/165483/&lt;/td&gt;&lt;td&gt;timbre&lt;/td&gt;</v>
+        <f t="shared" si="12"/>
+        <v>&lt;tr&gt;&lt;td&gt;zero/1.0/&lt;/td&gt;&lt;td&gt;162814__timgormly__spaceship-4.aiff&lt;/td&gt;&lt;td&gt;https://freesound.org/s/162814/&lt;/td&gt;&lt;td&gt;timgormly&lt;/td&gt;</v>
       </c>
       <c r="J85" s="51" t="s">
-        <v>2879</v>
+        <v>2859</v>
       </c>
       <c r="K85" s="6" t="s">
-        <v>2887</v>
+        <v>2888</v>
       </c>
       <c r="L85" t="s">
-        <v>2938</v>
+        <v>2939</v>
       </c>
       <c r="M85" s="28" t="s">
-        <v>2927</v>
+        <v>2928</v>
       </c>
       <c r="R85" t="str">
         <f>"| "&amp;J85&amp;" | "&amp;K85&amp;" | "&amp;L85&amp;" | "&amp;M85&amp;" |"</f>
-        <v>| by-nc/3.0/ | 165483__timbre__glitch-voice-ep-mp3.mp3 | https://freesound.org/s/165483/ | timbre |</v>
+        <v>| zero/1.0/ | 162814__timgormly__spaceship-4.aiff | https://freesound.org/s/162814/ | timgormly |</v>
       </c>
     </row>
     <row r="86" spans="1:18" ht="20.25">
       <c r="A86" s="6" t="str">
-        <f>"&lt;tr&gt;&lt;td&gt;"&amp;J86&amp;"&lt;/td&gt;&lt;td&gt;"&amp;K86&amp;"&lt;/td&gt;&lt;td&gt;"&amp;L86&amp;"&lt;/td&gt;&lt;td&gt;"&amp;M86&amp;"&lt;/td&gt;"</f>
-        <v>&lt;tr&gt;&lt;td&gt;by/3.0/&lt;/td&gt;&lt;td&gt;169292__lazr2012__haywirefusionator.ogg&lt;/td&gt;&lt;td&gt;https://freesound.org/s/169292/&lt;/td&gt;&lt;td&gt;lazr2012&lt;/td&gt;</v>
+        <f t="shared" si="12"/>
+        <v>&lt;tr&gt;&lt;td&gt;by-nc/3.0/&lt;/td&gt;&lt;td&gt;165483__timbre__glitch-voice-ep-mp3.mp3&lt;/td&gt;&lt;td&gt;https://freesound.org/s/165483/&lt;/td&gt;&lt;td&gt;timbre&lt;/td&gt;</v>
       </c>
       <c r="J86" s="51" t="s">
-        <v>2867</v>
+        <v>2879</v>
       </c>
       <c r="K86" s="6" t="s">
-        <v>2885</v>
+        <v>2887</v>
       </c>
       <c r="L86" t="s">
-        <v>2937</v>
+        <v>2938</v>
       </c>
       <c r="M86" s="28" t="s">
-        <v>2926</v>
+        <v>2927</v>
       </c>
       <c r="R86" t="str">
         <f>"| "&amp;J86&amp;" | "&amp;K86&amp;" | "&amp;L86&amp;" | "&amp;M86&amp;" |"</f>
-        <v>| by/3.0/ | 169292__lazr2012__haywirefusionator.ogg | https://freesound.org/s/169292/ | lazr2012 |</v>
+        <v>| by-nc/3.0/ | 165483__timbre__glitch-voice-ep-mp3.mp3 | https://freesound.org/s/165483/ | timbre |</v>
       </c>
     </row>
     <row r="87" spans="1:18" ht="20.25">
       <c r="A87" s="6" t="str">
-        <f>"&lt;tr&gt;&lt;td&gt;"&amp;J87&amp;"&lt;/td&gt;&lt;td&gt;"&amp;K87&amp;"&lt;/td&gt;&lt;td&gt;"&amp;L87&amp;"&lt;/td&gt;&lt;td&gt;"&amp;M87&amp;"&lt;/td&gt;"</f>
-        <v>&lt;tr&gt;&lt;td&gt;zero/1.0/&lt;/td&gt;&lt;td&gt;170136__lazr2012__machinery-bo.flac&lt;/td&gt;&lt;td&gt;https://freesound.org/s/170136/&lt;/td&gt;&lt;td&gt;lazr2012&lt;/td&gt;</v>
+        <f t="shared" si="12"/>
+        <v>&lt;tr&gt;&lt;td&gt;by/3.0/&lt;/td&gt;&lt;td&gt;169292__lazr2012__haywirefusionator.ogg&lt;/td&gt;&lt;td&gt;https://freesound.org/s/169292/&lt;/td&gt;&lt;td&gt;lazr2012&lt;/td&gt;</v>
       </c>
       <c r="J87" s="51" t="s">
-        <v>2859</v>
+        <v>2867</v>
       </c>
       <c r="K87" s="6" t="s">
-        <v>2883</v>
+        <v>2885</v>
       </c>
       <c r="L87" t="s">
-        <v>2936</v>
+        <v>2937</v>
       </c>
       <c r="M87" s="28" t="s">
         <v>2926</v>
       </c>
-      <c r="Q87" s="29"/>
       <c r="R87" t="str">
         <f>"| "&amp;J87&amp;" | "&amp;K87&amp;" | "&amp;L87&amp;" | "&amp;M87&amp;" |"</f>
-        <v>| zero/1.0/ | 170136__lazr2012__machinery-bo.flac | https://freesound.org/s/170136/ | lazr2012 |</v>
+        <v>| by/3.0/ | 169292__lazr2012__haywirefusionator.ogg | https://freesound.org/s/169292/ | lazr2012 |</v>
       </c>
     </row>
     <row r="88" spans="1:18" ht="20.25">
       <c r="A88" s="6" t="str">
-        <f>"&lt;tr&gt;&lt;td&gt;"&amp;J88&amp;"&lt;/td&gt;&lt;td&gt;"&amp;K88&amp;"&lt;/td&gt;&lt;td&gt;"&amp;L88&amp;"&lt;/td&gt;&lt;td&gt;"&amp;M88&amp;"&lt;/td&gt;"</f>
-        <v>&lt;tr&gt;&lt;td&gt;by-nc/3.0/&lt;/td&gt;&lt;td&gt;179281__timbre__boingy-sweep.flac&lt;/td&gt;&lt;td&gt;https://freesound.org/s/179281/&lt;/td&gt;&lt;td&gt;Timbre&lt;/td&gt;</v>
-      </c>
-      <c r="J88" s="15" t="s">
-        <v>2879</v>
-      </c>
-      <c r="K88" s="4" t="s">
-        <v>2880</v>
-      </c>
-      <c r="L88" s="29" t="s">
-        <v>2881</v>
+        <f t="shared" si="12"/>
+        <v>&lt;tr&gt;&lt;td&gt;zero/1.0/&lt;/td&gt;&lt;td&gt;170136__lazr2012__machinery-bo.flac&lt;/td&gt;&lt;td&gt;https://freesound.org/s/170136/&lt;/td&gt;&lt;td&gt;lazr2012&lt;/td&gt;</v>
+      </c>
+      <c r="J88" s="51" t="s">
+        <v>2859</v>
+      </c>
+      <c r="K88" s="6" t="s">
+        <v>2883</v>
+      </c>
+      <c r="L88" t="s">
+        <v>2936</v>
       </c>
       <c r="M88" s="28" t="s">
-        <v>2882</v>
-      </c>
+        <v>2926</v>
+      </c>
+      <c r="Q88" s="29"/>
       <c r="R88" t="str">
-        <f t="shared" ref="R88:R89" si="10">"| "&amp;J88&amp;" | "&amp;K88&amp;" | "&amp;L88&amp;" | "&amp;M88&amp;" |"</f>
-        <v>| by-nc/3.0/ | 179281__timbre__boingy-sweep.flac | https://freesound.org/s/179281/ | Timbre |</v>
+        <f>"| "&amp;J88&amp;" | "&amp;K88&amp;" | "&amp;L88&amp;" | "&amp;M88&amp;" |"</f>
+        <v>| zero/1.0/ | 170136__lazr2012__machinery-bo.flac | https://freesound.org/s/170136/ | lazr2012 |</v>
       </c>
     </row>
     <row r="89" spans="1:18" ht="20.25">
       <c r="A89" s="6" t="str">
-        <f>"&lt;tr&gt;&lt;td&gt;"&amp;J89&amp;"&lt;/td&gt;&lt;td&gt;"&amp;K89&amp;"&lt;/td&gt;&lt;td&gt;"&amp;L89&amp;"&lt;/td&gt;&lt;td&gt;"&amp;M89&amp;"&lt;/td&gt;"</f>
-        <v>&lt;tr&gt;&lt;td&gt;by/3.0/&lt;/td&gt;&lt;td&gt;216096__richerlandtv__u-f-o.mp3&lt;/td&gt;&lt;td&gt;https://freesound.org/s/216096/&lt;/td&gt;&lt;td&gt;RICHERlandTV&lt;/td&gt;</v>
+        <f t="shared" si="12"/>
+        <v>&lt;tr&gt;&lt;td&gt;by-nc/3.0/&lt;/td&gt;&lt;td&gt;179281__timbre__boingy-sweep.flac&lt;/td&gt;&lt;td&gt;https://freesound.org/s/179281/&lt;/td&gt;&lt;td&gt;Timbre&lt;/td&gt;</v>
       </c>
       <c r="J89" s="15" t="s">
-        <v>2867</v>
+        <v>2879</v>
       </c>
       <c r="K89" s="4" t="s">
-        <v>2868</v>
+        <v>2880</v>
       </c>
       <c r="L89" s="29" t="s">
-        <v>2869</v>
+        <v>2881</v>
       </c>
       <c r="M89" s="28" t="s">
-        <v>2870</v>
+        <v>2882</v>
       </c>
       <c r="R89" t="str">
-        <f t="shared" si="10"/>
-        <v>| by/3.0/ | 216096__richerlandtv__u-f-o.mp3 | https://freesound.org/s/216096/ | RICHERlandTV |</v>
+        <f t="shared" ref="R89:R90" si="13">"| "&amp;J89&amp;" | "&amp;K89&amp;" | "&amp;L89&amp;" | "&amp;M89&amp;" |"</f>
+        <v>| by-nc/3.0/ | 179281__timbre__boingy-sweep.flac | https://freesound.org/s/179281/ | Timbre |</v>
       </c>
     </row>
     <row r="90" spans="1:18" ht="20.25">
       <c r="A90" s="6" t="str">
-        <f>"&lt;tr&gt;&lt;td&gt;"&amp;J90&amp;"&lt;/td&gt;&lt;td&gt;"&amp;K90&amp;"&lt;/td&gt;&lt;td&gt;"&amp;L90&amp;"&lt;/td&gt;&lt;td&gt;"&amp;M90&amp;"&lt;/td&gt;"</f>
-        <v>&lt;tr&gt;&lt;td&gt;by/3.0/&lt;/td&gt;&lt;td&gt;221875__hero-of-the-winds__spring-boing.wav&lt;/td&gt;&lt;td&gt;https://freesound.org/s/221875/&lt;/td&gt;&lt;td&gt;hero-of-the-winds&lt;/td&gt;</v>
-      </c>
-      <c r="J90" s="51" t="s">
+        <f t="shared" si="12"/>
+        <v>&lt;tr&gt;&lt;td&gt;by/3.0/&lt;/td&gt;&lt;td&gt;216096__richerlandtv__u-f-o.mp3&lt;/td&gt;&lt;td&gt;https://freesound.org/s/216096/&lt;/td&gt;&lt;td&gt;RICHERlandTV&lt;/td&gt;</v>
+      </c>
+      <c r="J90" s="15" t="s">
         <v>2867</v>
       </c>
-      <c r="K90" s="6" t="s">
-        <v>2854</v>
-      </c>
-      <c r="L90" t="s">
-        <v>2933</v>
+      <c r="K90" s="4" t="s">
+        <v>2868</v>
+      </c>
+      <c r="L90" s="29" t="s">
+        <v>2869</v>
       </c>
       <c r="M90" s="28" t="s">
-        <v>2919</v>
+        <v>2870</v>
       </c>
       <c r="R90" t="str">
-        <f>"| "&amp;J90&amp;" | "&amp;K90&amp;" | "&amp;L90&amp;" | "&amp;M90&amp;" |"</f>
-        <v>| by/3.0/ | 221875__hero-of-the-winds__spring-boing.wav | https://freesound.org/s/221875/ | hero-of-the-winds |</v>
+        <f t="shared" si="13"/>
+        <v>| by/3.0/ | 216096__richerlandtv__u-f-o.mp3 | https://freesound.org/s/216096/ | RICHERlandTV |</v>
       </c>
     </row>
     <row r="91" spans="1:18" ht="20.25">
       <c r="A91" s="6" t="str">
-        <f>"&lt;tr&gt;&lt;td&gt;"&amp;J91&amp;"&lt;/td&gt;&lt;td&gt;"&amp;K91&amp;"&lt;/td&gt;&lt;td&gt;"&amp;L91&amp;"&lt;/td&gt;&lt;td&gt;"&amp;M91&amp;"&lt;/td&gt;"</f>
-        <v>&lt;tr&gt;&lt;td&gt;by/3.0/&lt;/td&gt;&lt;td&gt;240297__jalastram__abstract-guitar-sfx-003.wav&lt;/td&gt;&lt;td&gt;https://freesound.org/s/240297/&lt;/td&gt;&lt;td&gt;jalastram&lt;/td&gt;</v>
-      </c>
-      <c r="J91" s="36" t="s">
+        <f t="shared" si="12"/>
+        <v>&lt;tr&gt;&lt;td&gt;by/3.0/&lt;/td&gt;&lt;td&gt;221875__hero-of-the-winds__spring-boing.wav&lt;/td&gt;&lt;td&gt;https://freesound.org/s/221875/&lt;/td&gt;&lt;td&gt;hero-of-the-winds&lt;/td&gt;</v>
+      </c>
+      <c r="J91" s="51" t="s">
         <v>2867</v>
       </c>
       <c r="K91" s="6" t="s">
-        <v>2849</v>
-      </c>
-      <c r="L91" s="29" t="s">
-        <v>2934</v>
+        <v>2854</v>
+      </c>
+      <c r="L91" t="s">
+        <v>2933</v>
       </c>
       <c r="M91" s="28" t="s">
-        <v>2920</v>
+        <v>2919</v>
       </c>
       <c r="R91" t="str">
-        <f>"| "&amp;J91&amp;" | "&amp;K91&amp;" | "&amp;L91&amp;" | "&amp;M91&amp;" |"</f>
-        <v>| by/3.0/ | 240297__jalastram__abstract-guitar-sfx-003.wav | https://freesound.org/s/240297/ | jalastram |</v>
+        <f t="shared" ref="R91:R109" si="14">"| "&amp;J91&amp;" | "&amp;K91&amp;" | "&amp;L91&amp;" | "&amp;M91&amp;" |"</f>
+        <v>| by/3.0/ | 221875__hero-of-the-winds__spring-boing.wav | https://freesound.org/s/221875/ | hero-of-the-winds |</v>
       </c>
     </row>
     <row r="92" spans="1:18" ht="20.25">
       <c r="A92" s="6" t="str">
-        <f>"&lt;tr&gt;&lt;td&gt;"&amp;J92&amp;"&lt;/td&gt;&lt;td&gt;"&amp;K92&amp;"&lt;/td&gt;&lt;td&gt;"&amp;L92&amp;"&lt;/td&gt;&lt;td&gt;"&amp;M92&amp;"&lt;/td&gt;"</f>
-        <v>&lt;tr&gt;&lt;td&gt;by/3.0/&lt;/td&gt;&lt;td&gt;272068__ichbinjager__shotgun-action.wav&lt;/td&gt;&lt;td&gt;https://freesound.org/s/272068/&lt;/td&gt;&lt;td&gt;IchBinJager&lt;/td&gt;</v>
-      </c>
-      <c r="J92" s="28" t="s">
+        <f t="shared" si="12"/>
+        <v>&lt;tr&gt;&lt;td&gt;by/3.0/&lt;/td&gt;&lt;td&gt;240297__jalastram__abstract-guitar-sfx-003.wav&lt;/td&gt;&lt;td&gt;https://freesound.org/s/240297/&lt;/td&gt;&lt;td&gt;jalastram&lt;/td&gt;</v>
+      </c>
+      <c r="J92" s="36" t="s">
         <v>2867</v>
       </c>
-      <c r="K92" t="s">
-        <v>2901</v>
+      <c r="K92" s="6" t="s">
+        <v>2849</v>
       </c>
       <c r="L92" s="29" t="s">
-        <v>2903</v>
+        <v>2934</v>
       </c>
       <c r="M92" s="28" t="s">
-        <v>2900</v>
+        <v>2920</v>
       </c>
       <c r="R92" t="str">
-        <f>"| "&amp;J92&amp;" | "&amp;K92&amp;" | "&amp;L92&amp;" | "&amp;M92&amp;" |"</f>
-        <v>| by/3.0/ | 272068__ichbinjager__shotgun-action.wav | https://freesound.org/s/272068/ | IchBinJager |</v>
+        <f t="shared" si="14"/>
+        <v>| by/3.0/ | 240297__jalastram__abstract-guitar-sfx-003.wav | https://freesound.org/s/240297/ | jalastram |</v>
       </c>
     </row>
     <row r="93" spans="1:18" ht="20.25">
       <c r="A93" s="6" t="str">
-        <f>"&lt;tr&gt;&lt;td&gt;"&amp;J93&amp;"&lt;/td&gt;&lt;td&gt;"&amp;K93&amp;"&lt;/td&gt;&lt;td&gt;"&amp;L93&amp;"&lt;/td&gt;&lt;td&gt;"&amp;M93&amp;"&lt;/td&gt;"</f>
-        <v>&lt;tr&gt;&lt;td&gt;by/3.0/&lt;/td&gt;&lt;td&gt;275537__wjoojoo__contact-mic-on-satellite-dish04.wav&lt;/td&gt;&lt;td&gt;https://freesound.org/s/275537/&lt;/td&gt;&lt;td&gt;wjoojoo&lt;/td&gt;</v>
-      </c>
-      <c r="J93" s="36" t="s">
+        <f t="shared" si="12"/>
+        <v>&lt;tr&gt;&lt;td&gt;by/3.0/&lt;/td&gt;&lt;td&gt;272068__ichbinjager__shotgun-action.wav&lt;/td&gt;&lt;td&gt;https://freesound.org/s/272068/&lt;/td&gt;&lt;td&gt;IchBinJager&lt;/td&gt;</v>
+      </c>
+      <c r="J93" s="28" t="s">
         <v>2867</v>
       </c>
-      <c r="K93" s="6" t="s">
-        <v>2847</v>
-      </c>
-      <c r="L93" t="s">
-        <v>2930</v>
+      <c r="K93" t="s">
+        <v>2901</v>
+      </c>
+      <c r="L93" s="29" t="s">
+        <v>2903</v>
       </c>
       <c r="M93" s="28" t="s">
-        <v>2921</v>
+        <v>2900</v>
       </c>
       <c r="R93" t="str">
-        <f>"| "&amp;J93&amp;" | "&amp;K93&amp;" | "&amp;L93&amp;" | "&amp;M93&amp;" |"</f>
-        <v>| by/3.0/ | 275537__wjoojoo__contact-mic-on-satellite-dish04.wav | https://freesound.org/s/275537/ | wjoojoo |</v>
+        <f t="shared" si="14"/>
+        <v>| by/3.0/ | 272068__ichbinjager__shotgun-action.wav | https://freesound.org/s/272068/ | IchBinJager |</v>
       </c>
     </row>
     <row r="94" spans="1:18" ht="20.25">
       <c r="A94" s="6" t="str">
-        <f>"&lt;tr&gt;&lt;td&gt;"&amp;J94&amp;"&lt;/td&gt;&lt;td&gt;"&amp;K94&amp;"&lt;/td&gt;&lt;td&gt;"&amp;L94&amp;"&lt;/td&gt;&lt;td&gt;"&amp;M94&amp;"&lt;/td&gt;"</f>
-        <v>&lt;tr&gt;&lt;td&gt;zero/1.0/&lt;/td&gt;&lt;td&gt;352852__josepharaoh99__game-style-laser-beam.wav&lt;/td&gt;&lt;td&gt;https://freesound.org/s/352852/&lt;/td&gt;&lt;td&gt;josepharaoh99&lt;/td&gt;</v>
+        <f t="shared" si="12"/>
+        <v>&lt;tr&gt;&lt;td&gt;by/3.0/&lt;/td&gt;&lt;td&gt;275537__wjoojoo__contact-mic-on-satellite-dish04.wav&lt;/td&gt;&lt;td&gt;https://freesound.org/s/275537/&lt;/td&gt;&lt;td&gt;wjoojoo&lt;/td&gt;</v>
       </c>
       <c r="J94" s="36" t="s">
-        <v>2859</v>
+        <v>2867</v>
       </c>
       <c r="K94" s="6" t="s">
-        <v>2845</v>
+        <v>2847</v>
       </c>
       <c r="L94" t="s">
-        <v>2931</v>
+        <v>2930</v>
       </c>
       <c r="M94" s="28" t="s">
-        <v>2922</v>
+        <v>2921</v>
       </c>
       <c r="R94" t="str">
-        <f>"| "&amp;J94&amp;" | "&amp;K94&amp;" | "&amp;L94&amp;" | "&amp;M94&amp;" |"</f>
-        <v>| zero/1.0/ | 352852__josepharaoh99__game-style-laser-beam.wav | https://freesound.org/s/352852/ | josepharaoh99 |</v>
+        <f t="shared" si="14"/>
+        <v>| by/3.0/ | 275537__wjoojoo__contact-mic-on-satellite-dish04.wav | https://freesound.org/s/275537/ | wjoojoo |</v>
       </c>
     </row>
     <row r="95" spans="1:18" ht="20.25">
       <c r="A95" s="6" t="str">
-        <f>"&lt;tr&gt;&lt;td&gt;"&amp;J95&amp;"&lt;/td&gt;&lt;td&gt;"&amp;K95&amp;"&lt;/td&gt;&lt;td&gt;"&amp;L95&amp;"&lt;/td&gt;&lt;td&gt;"&amp;M95&amp;"&lt;/td&gt;"</f>
-        <v>&lt;tr&gt;&lt;td&gt;zero/1.0/&lt;/td&gt;&lt;td&gt;380886__morganpurkis__doom-shotgun-2017.wav&lt;/td&gt;&lt;td&gt;https://freesound.org/s/380886/&lt;/td&gt;&lt;td&gt;morganpurkis&lt;/td&gt;</v>
-      </c>
-      <c r="J95" s="28" t="s">
+        <f t="shared" si="12"/>
+        <v>&lt;tr&gt;&lt;td&gt;zero/1.0/&lt;/td&gt;&lt;td&gt;352852__josepharaoh99__game-style-laser-beam.wav&lt;/td&gt;&lt;td&gt;https://freesound.org/s/352852/&lt;/td&gt;&lt;td&gt;josepharaoh99&lt;/td&gt;</v>
+      </c>
+      <c r="J95" s="36" t="s">
         <v>2859</v>
       </c>
-      <c r="K95" t="s">
-        <v>2897</v>
-      </c>
-      <c r="L95" s="29" t="s">
-        <v>2898</v>
+      <c r="K95" s="6" t="s">
+        <v>2845</v>
+      </c>
+      <c r="L95" t="s">
+        <v>2931</v>
       </c>
       <c r="M95" s="28" t="s">
-        <v>2895</v>
+        <v>2922</v>
       </c>
       <c r="R95" t="str">
-        <f>"| "&amp;J95&amp;" | "&amp;K95&amp;" | "&amp;L95&amp;" | "&amp;M95&amp;" |"</f>
-        <v>| zero/1.0/ | 380886__morganpurkis__doom-shotgun-2017.wav | https://freesound.org/s/380886/ | morganpurkis |</v>
+        <f t="shared" si="14"/>
+        <v>| zero/1.0/ | 352852__josepharaoh99__game-style-laser-beam.wav | https://freesound.org/s/352852/ | josepharaoh99 |</v>
       </c>
     </row>
     <row r="96" spans="1:18" ht="20.25">
       <c r="A96" s="6" t="str">
-        <f>"&lt;tr&gt;&lt;td&gt;"&amp;J96&amp;"&lt;/td&gt;&lt;td&gt;"&amp;K96&amp;"&lt;/td&gt;&lt;td&gt;"&amp;L96&amp;"&lt;/td&gt;&lt;td&gt;"&amp;M96&amp;"&lt;/td&gt;"</f>
-        <v>&lt;tr&gt;&lt;td&gt;by/3.0/&lt;/td&gt;&lt;td&gt;383205__spiceprogram__loading-sound.wav&lt;/td&gt;&lt;td&gt;https://freesound.org/s/383205/&lt;/td&gt;&lt;td&gt;SpiceProgram&lt;/td&gt;</v>
-      </c>
-      <c r="J96" s="30" t="s">
-        <v>2867</v>
-      </c>
-      <c r="K96" s="28" t="s">
-        <v>2843</v>
+        <f t="shared" si="12"/>
+        <v>&lt;tr&gt;&lt;td&gt;zero/1.0/&lt;/td&gt;&lt;td&gt;380886__morganpurkis__doom-shotgun-2017.wav&lt;/td&gt;&lt;td&gt;https://freesound.org/s/380886/&lt;/td&gt;&lt;td&gt;morganpurkis&lt;/td&gt;</v>
+      </c>
+      <c r="J96" s="28" t="s">
+        <v>2859</v>
+      </c>
+      <c r="K96" t="s">
+        <v>2897</v>
       </c>
       <c r="L96" s="29" t="s">
-        <v>2877</v>
+        <v>2898</v>
       </c>
       <c r="M96" s="28" t="s">
-        <v>2878</v>
+        <v>2895</v>
       </c>
       <c r="R96" t="str">
-        <f>"| "&amp;J96&amp;" | "&amp;K96&amp;" | "&amp;L96&amp;" | "&amp;M96&amp;" |"</f>
-        <v>| by/3.0/ | 383205__spiceprogram__loading-sound.wav | https://freesound.org/s/383205/ | SpiceProgram |</v>
+        <f t="shared" si="14"/>
+        <v>| zero/1.0/ | 380886__morganpurkis__doom-shotgun-2017.wav | https://freesound.org/s/380886/ | morganpurkis |</v>
       </c>
     </row>
     <row r="97" spans="1:18" ht="20.25">
       <c r="A97" s="6" t="str">
-        <f>"&lt;tr&gt;&lt;td&gt;"&amp;J97&amp;"&lt;/td&gt;&lt;td&gt;"&amp;K97&amp;"&lt;/td&gt;&lt;td&gt;"&amp;L97&amp;"&lt;/td&gt;&lt;td&gt;"&amp;M97&amp;"&lt;/td&gt;"</f>
-        <v>&lt;tr&gt;&lt;td&gt;zero/1.0/&lt;/td&gt;&lt;td&gt;383760__deleted-user-7146007__laboratory-mad-scientist-science-fiction-sci-fi.wav&lt;/td&gt;&lt;td&gt;https://freesound.org/s/383760/&lt;/td&gt;&lt;td&gt;deleted-user-7146007&lt;/td&gt;</v>
-      </c>
-      <c r="J97" s="35" t="s">
-        <v>2859</v>
-      </c>
-      <c r="K97" s="19" t="s">
-        <v>2841</v>
-      </c>
-      <c r="L97" t="s">
-        <v>2929</v>
+        <f t="shared" si="12"/>
+        <v>&lt;tr&gt;&lt;td&gt;by/3.0/&lt;/td&gt;&lt;td&gt;383205__spiceprogram__loading-sound.wav&lt;/td&gt;&lt;td&gt;https://freesound.org/s/383205/&lt;/td&gt;&lt;td&gt;SpiceProgram&lt;/td&gt;</v>
+      </c>
+      <c r="J97" s="30" t="s">
+        <v>2867</v>
+      </c>
+      <c r="K97" s="28" t="s">
+        <v>2843</v>
+      </c>
+      <c r="L97" s="29" t="s">
+        <v>2877</v>
       </c>
       <c r="M97" s="28" t="s">
-        <v>2923</v>
+        <v>2878</v>
       </c>
       <c r="R97" t="str">
-        <f>"| "&amp;J97&amp;" | "&amp;K97&amp;" | "&amp;L97&amp;" | "&amp;M97&amp;" |"</f>
-        <v>| zero/1.0/ | 383760__deleted-user-7146007__laboratory-mad-scientist-science-fiction-sci-fi.wav | https://freesound.org/s/383760/ | deleted-user-7146007 |</v>
+        <f t="shared" si="14"/>
+        <v>| by/3.0/ | 383205__spiceprogram__loading-sound.wav | https://freesound.org/s/383205/ | SpiceProgram |</v>
       </c>
     </row>
     <row r="98" spans="1:18" ht="20.25">
       <c r="A98" s="6" t="str">
-        <f>"&lt;tr&gt;&lt;td&gt;"&amp;J98&amp;"&lt;/td&gt;&lt;td&gt;"&amp;K98&amp;"&lt;/td&gt;&lt;td&gt;"&amp;L98&amp;"&lt;/td&gt;&lt;td&gt;"&amp;M98&amp;"&lt;/td&gt;"</f>
-        <v>&lt;tr&gt;&lt;td&gt;zero/1.0/&lt;/td&gt;&lt;td&gt;397254__screamstudio__loading.wav&lt;/td&gt;&lt;td&gt;https://freesound.org/s/397254/&lt;/td&gt;&lt;td&gt;ScreamStudio&lt;/td&gt;</v>
-      </c>
-      <c r="J98" s="32" t="s">
+        <f t="shared" si="12"/>
+        <v>&lt;tr&gt;&lt;td&gt;zero/1.0/&lt;/td&gt;&lt;td&gt;383760__deleted-user-7146007__laboratory-mad-scientist-science-fiction-sci-fi.wav&lt;/td&gt;&lt;td&gt;https://freesound.org/s/383760/&lt;/td&gt;&lt;td&gt;deleted-user-7146007&lt;/td&gt;</v>
+      </c>
+      <c r="J98" s="35" t="s">
         <v>2859</v>
       </c>
-      <c r="K98" s="35" t="s">
-        <v>2833</v>
-      </c>
-      <c r="L98" s="29" t="s">
-        <v>2862</v>
+      <c r="K98" s="19" t="s">
+        <v>2841</v>
+      </c>
+      <c r="L98" t="s">
+        <v>2929</v>
       </c>
       <c r="M98" s="28" t="s">
-        <v>2863</v>
+        <v>2923</v>
       </c>
       <c r="R98" t="str">
-        <f>"| "&amp;J98&amp;" | "&amp;K98&amp;" | "&amp;L98&amp;" | "&amp;M98&amp;" |"</f>
-        <v>| zero/1.0/ | 397254__screamstudio__loading.wav | https://freesound.org/s/397254/ | ScreamStudio |</v>
+        <f t="shared" si="14"/>
+        <v>| zero/1.0/ | 383760__deleted-user-7146007__laboratory-mad-scientist-science-fiction-sci-fi.wav | https://freesound.org/s/383760/ | deleted-user-7146007 |</v>
       </c>
     </row>
     <row r="99" spans="1:18" ht="20.25">
       <c r="A99" s="6" t="str">
-        <f>"&lt;tr&gt;&lt;td&gt;"&amp;J99&amp;"&lt;/td&gt;&lt;td&gt;"&amp;K99&amp;"&lt;/td&gt;&lt;td&gt;"&amp;L99&amp;"&lt;/td&gt;&lt;td&gt;"&amp;M99&amp;"&lt;/td&gt;"</f>
-        <v>&lt;tr&gt;&lt;td&gt;zero/1.0/&lt;/td&gt;&lt;td&gt;404068__swordofkings128__backyard-gate-open.wav&lt;/td&gt;&lt;td&gt;https://freesound.org/s/404068/&lt;/td&gt;&lt;td&gt;swordofkings128&lt;/td&gt;</v>
-      </c>
-      <c r="J99" s="35" t="s">
+        <f t="shared" si="12"/>
+        <v>&lt;tr&gt;&lt;td&gt;zero/1.0/&lt;/td&gt;&lt;td&gt;397254__screamstudio__loading.wav&lt;/td&gt;&lt;td&gt;https://freesound.org/s/397254/&lt;/td&gt;&lt;td&gt;ScreamStudio&lt;/td&gt;</v>
+      </c>
+      <c r="J99" s="32" t="s">
         <v>2859</v>
       </c>
-      <c r="K99" s="19" t="s">
-        <v>2906</v>
+      <c r="K99" s="35" t="s">
+        <v>2833</v>
       </c>
       <c r="L99" s="29" t="s">
-        <v>2911</v>
+        <v>2862</v>
       </c>
       <c r="M99" s="28" t="s">
-        <v>2907</v>
+        <v>2863</v>
       </c>
       <c r="R99" t="str">
-        <f>"| "&amp;J99&amp;" | "&amp;K99&amp;" | "&amp;L99&amp;" | "&amp;M99&amp;" |"</f>
-        <v>| zero/1.0/ | 404068__swordofkings128__backyard-gate-open.wav | https://freesound.org/s/404068/ | swordofkings128 |</v>
+        <f t="shared" si="14"/>
+        <v>| zero/1.0/ | 397254__screamstudio__loading.wav | https://freesound.org/s/397254/ | ScreamStudio |</v>
       </c>
     </row>
     <row r="100" spans="1:18" ht="20.25">
       <c r="A100" s="6" t="str">
-        <f>"&lt;tr&gt;&lt;td&gt;"&amp;J100&amp;"&lt;/td&gt;&lt;td&gt;"&amp;K100&amp;"&lt;/td&gt;&lt;td&gt;"&amp;L100&amp;"&lt;/td&gt;&lt;td&gt;"&amp;M100&amp;"&lt;/td&gt;"</f>
-        <v>&lt;tr&gt;&lt;td&gt;zero/1.0/&lt;/td&gt;&lt;td&gt;407052__sojan__power-charge.flac&lt;/td&gt;&lt;td&gt;https://freesound.org/s/193610/&lt;/td&gt;&lt;td&gt;crashoverride61088&lt;/td&gt;</v>
-      </c>
-      <c r="J100" s="32" t="s">
+        <f t="shared" si="12"/>
+        <v>&lt;tr&gt;&lt;td&gt;zero/1.0/&lt;/td&gt;&lt;td&gt;404068__swordofkings128__backyard-gate-open.wav&lt;/td&gt;&lt;td&gt;https://freesound.org/s/404068/&lt;/td&gt;&lt;td&gt;swordofkings128&lt;/td&gt;</v>
+      </c>
+      <c r="J100" s="35" t="s">
         <v>2859</v>
       </c>
-      <c r="K100" s="35" t="s">
-        <v>2835</v>
+      <c r="K100" s="19" t="s">
+        <v>2906</v>
       </c>
       <c r="L100" s="29" t="s">
-        <v>2860</v>
+        <v>2911</v>
       </c>
       <c r="M100" s="28" t="s">
-        <v>2861</v>
+        <v>2907</v>
       </c>
       <c r="R100" t="str">
-        <f>"| "&amp;J100&amp;" | "&amp;K100&amp;" | "&amp;L100&amp;" | "&amp;M100&amp;" |"</f>
-        <v>| zero/1.0/ | 407052__sojan__power-charge.flac | https://freesound.org/s/193610/ | crashoverride61088 |</v>
+        <f t="shared" si="14"/>
+        <v>| zero/1.0/ | 404068__swordofkings128__backyard-gate-open.wav | https://freesound.org/s/404068/ | swordofkings128 |</v>
       </c>
     </row>
     <row r="101" spans="1:18" ht="20.25">
       <c r="A101" s="6" t="str">
-        <f>"&lt;tr&gt;&lt;td&gt;"&amp;J101&amp;"&lt;/td&gt;&lt;td&gt;"&amp;K101&amp;"&lt;/td&gt;&lt;td&gt;"&amp;L101&amp;"&lt;/td&gt;&lt;td&gt;"&amp;M101&amp;"&lt;/td&gt;"</f>
-        <v>&lt;tr&gt;&lt;td&gt;by/3.0/&lt;/td&gt;&lt;td&gt;417131__cuddlenucks__science-fiction-noise-3.wav&lt;/td&gt;&lt;td&gt;https://freesound.org/s/417131/&lt;/td&gt;&lt;td&gt;cuddlenucks&lt;/td&gt;</v>
-      </c>
-      <c r="J101" s="35" t="s">
-        <v>2867</v>
-      </c>
-      <c r="K101" s="19" t="s">
-        <v>2839</v>
-      </c>
-      <c r="L101" t="s">
-        <v>2935</v>
+        <f t="shared" si="12"/>
+        <v>&lt;tr&gt;&lt;td&gt;zero/1.0/&lt;/td&gt;&lt;td&gt;407052__sojan__power-charge.flac&lt;/td&gt;&lt;td&gt;https://freesound.org/s/193610/&lt;/td&gt;&lt;td&gt;crashoverride61088&lt;/td&gt;</v>
+      </c>
+      <c r="J101" s="32" t="s">
+        <v>2859</v>
+      </c>
+      <c r="K101" s="35" t="s">
+        <v>2835</v>
+      </c>
+      <c r="L101" s="29" t="s">
+        <v>2860</v>
       </c>
       <c r="M101" s="28" t="s">
-        <v>2924</v>
+        <v>2861</v>
       </c>
       <c r="R101" t="str">
-        <f>"| "&amp;J101&amp;" | "&amp;K101&amp;" | "&amp;L101&amp;" | "&amp;M101&amp;" |"</f>
-        <v>| by/3.0/ | 417131__cuddlenucks__science-fiction-noise-3.wav | https://freesound.org/s/417131/ | cuddlenucks |</v>
+        <f t="shared" si="14"/>
+        <v>| zero/1.0/ | 407052__sojan__power-charge.flac | https://freesound.org/s/193610/ | crashoverride61088 |</v>
       </c>
     </row>
     <row r="102" spans="1:18" ht="20.25">
       <c r="A102" s="6" t="str">
-        <f>"&lt;tr&gt;&lt;td&gt;"&amp;J102&amp;"&lt;/td&gt;&lt;td&gt;"&amp;K102&amp;"&lt;/td&gt;&lt;td&gt;"&amp;L102&amp;"&lt;/td&gt;&lt;td&gt;"&amp;M102&amp;"&lt;/td&gt;"</f>
-        <v>&lt;tr&gt;&lt;td&gt;by/3.0/&lt;/td&gt;&lt;td&gt;417363__xcreenplay__boing-massive-kick.wav&lt;/td&gt;&lt;td&gt;https://freesound.org/s/417363/&lt;/td&gt;&lt;td&gt;xcreenplay&lt;/td&gt;</v>
+        <f t="shared" si="12"/>
+        <v>&lt;tr&gt;&lt;td&gt;by/3.0/&lt;/td&gt;&lt;td&gt;417131__cuddlenucks__science-fiction-noise-3.wav&lt;/td&gt;&lt;td&gt;https://freesound.org/s/417131/&lt;/td&gt;&lt;td&gt;cuddlenucks&lt;/td&gt;</v>
       </c>
       <c r="J102" s="35" t="s">
         <v>2867</v>
       </c>
       <c r="K102" s="19" t="s">
-        <v>2837</v>
+        <v>2839</v>
       </c>
       <c r="L102" t="s">
-        <v>2932</v>
+        <v>2935</v>
       </c>
       <c r="M102" s="28" t="s">
-        <v>2925</v>
+        <v>2924</v>
       </c>
       <c r="R102" t="str">
-        <f>"| "&amp;J102&amp;" | "&amp;K102&amp;" | "&amp;L102&amp;" | "&amp;M102&amp;" |"</f>
-        <v>| by/3.0/ | 417363__xcreenplay__boing-massive-kick.wav | https://freesound.org/s/417363/ | xcreenplay |</v>
+        <f t="shared" si="14"/>
+        <v>| by/3.0/ | 417131__cuddlenucks__science-fiction-noise-3.wav | https://freesound.org/s/417131/ | cuddlenucks |</v>
       </c>
     </row>
     <row r="103" spans="1:18" ht="20.25">
       <c r="A103" s="6" t="str">
-        <f>"&lt;tr&gt;&lt;td&gt;"&amp;J103&amp;"&lt;/td&gt;&lt;td&gt;"&amp;K103&amp;"&lt;/td&gt;&lt;td&gt;"&amp;L103&amp;"&lt;/td&gt;&lt;td&gt;"&amp;M103&amp;"&lt;/td&gt;"</f>
-        <v>&lt;tr&gt;&lt;td&gt;by/3.0/&lt;/td&gt;&lt;td&gt;431117__inspectorj__door-front-opening-a.wav&lt;/td&gt;&lt;td&gt;https://freesound.org/s/431117/&lt;/td&gt;&lt;td&gt;inspectorj&lt;/td&gt;</v>
-      </c>
-      <c r="J103" s="28" t="s">
+        <f t="shared" si="12"/>
+        <v>&lt;tr&gt;&lt;td&gt;by/3.0/&lt;/td&gt;&lt;td&gt;417363__xcreenplay__boing-massive-kick.wav&lt;/td&gt;&lt;td&gt;https://freesound.org/s/417363/&lt;/td&gt;&lt;td&gt;xcreenplay&lt;/td&gt;</v>
+      </c>
+      <c r="J103" s="35" t="s">
         <v>2867</v>
       </c>
       <c r="K103" s="19" t="s">
-        <v>2904</v>
-      </c>
-      <c r="L103" s="29" t="s">
-        <v>2910</v>
+        <v>2837</v>
+      </c>
+      <c r="L103" t="s">
+        <v>2932</v>
       </c>
       <c r="M103" s="28" t="s">
-        <v>2905</v>
+        <v>2925</v>
       </c>
       <c r="R103" t="str">
-        <f>"| "&amp;J103&amp;" | "&amp;K103&amp;" | "&amp;L103&amp;" | "&amp;M103&amp;" |"</f>
-        <v>| by/3.0/ | 431117__inspectorj__door-front-opening-a.wav | https://freesound.org/s/431117/ | inspectorj |</v>
+        <f t="shared" si="14"/>
+        <v>| by/3.0/ | 417363__xcreenplay__boing-massive-kick.wav | https://freesound.org/s/417363/ | xcreenplay |</v>
       </c>
     </row>
     <row r="104" spans="1:18" ht="20.25">
       <c r="A104" s="6" t="str">
-        <f>"&lt;tr&gt;&lt;td&gt;"&amp;J104&amp;"&lt;/td&gt;&lt;td&gt;"&amp;K104&amp;"&lt;/td&gt;&lt;td&gt;"&amp;L104&amp;"&lt;/td&gt;&lt;td&gt;"&amp;M104&amp;"&lt;/td&gt;"</f>
-        <v>&lt;tr&gt;&lt;td&gt;zero/1.0/&lt;/td&gt;&lt;td&gt;500418__dj-somar__intro-reverso-craver-microbrute.wav&lt;/td&gt;&lt;td&gt;https://freesound.org/s/500418/&lt;/td&gt;&lt;td&gt;DJ_SoMaR&lt;/td&gt;</v>
-      </c>
-      <c r="J104" s="35" t="s">
-        <v>2859</v>
+        <f t="shared" si="12"/>
+        <v>&lt;tr&gt;&lt;td&gt;by/3.0/&lt;/td&gt;&lt;td&gt;431117__inspectorj__door-front-opening-a.wav&lt;/td&gt;&lt;td&gt;https://freesound.org/s/431117/&lt;/td&gt;&lt;td&gt;inspectorj&lt;/td&gt;</v>
+      </c>
+      <c r="J104" s="28" t="s">
+        <v>2867</v>
       </c>
       <c r="K104" s="19" t="s">
-        <v>2893</v>
+        <v>2904</v>
       </c>
       <c r="L104" s="29" t="s">
-        <v>2899</v>
+        <v>2910</v>
       </c>
       <c r="M104" s="28" t="s">
-        <v>2894</v>
+        <v>2905</v>
       </c>
       <c r="R104" t="str">
-        <f>"| "&amp;J104&amp;" | "&amp;K104&amp;" | "&amp;L104&amp;" | "&amp;M104&amp;" |"</f>
-        <v>| zero/1.0/ | 500418__dj-somar__intro-reverso-craver-microbrute.wav | https://freesound.org/s/500418/ | DJ_SoMaR |</v>
+        <f t="shared" si="14"/>
+        <v>| by/3.0/ | 431117__inspectorj__door-front-opening-a.wav | https://freesound.org/s/431117/ | inspectorj |</v>
       </c>
     </row>
     <row r="105" spans="1:18" ht="20.25">
       <c r="A105" s="6" t="str">
-        <f>"&lt;tr&gt;&lt;td&gt;"&amp;J105&amp;"&lt;/td&gt;&lt;td&gt;"&amp;K105&amp;"&lt;/td&gt;&lt;td&gt;"&amp;L105&amp;"&lt;/td&gt;&lt;td&gt;"&amp;M105&amp;"&lt;/td&gt;"</f>
-        <v>&lt;tr&gt;&lt;td&gt;by/3.0/&lt;/td&gt;&lt;td&gt;7967__cfork__boing-raw.aiff&lt;/td&gt;&lt;td&gt;https://freesound.org/s/7967/&lt;/td&gt;&lt;td&gt;cfork&lt;/td&gt;</v>
-      </c>
-      <c r="J105" s="32" t="s">
-        <v>2867</v>
-      </c>
-      <c r="K105" s="35" t="s">
-        <v>2874</v>
+        <f t="shared" si="12"/>
+        <v>&lt;tr&gt;&lt;td&gt;zero/1.0/&lt;/td&gt;&lt;td&gt;500418__dj-somar__intro-reverso-craver-microbrute.wav&lt;/td&gt;&lt;td&gt;https://freesound.org/s/500418/&lt;/td&gt;&lt;td&gt;DJ_SoMaR&lt;/td&gt;</v>
+      </c>
+      <c r="J105" s="35" t="s">
+        <v>2859</v>
+      </c>
+      <c r="K105" s="19" t="s">
+        <v>2893</v>
       </c>
       <c r="L105" s="29" t="s">
-        <v>2875</v>
+        <v>2899</v>
       </c>
       <c r="M105" s="28" t="s">
-        <v>2876</v>
+        <v>2894</v>
       </c>
       <c r="R105" t="str">
-        <f>"| "&amp;J105&amp;" | "&amp;K105&amp;" | "&amp;L105&amp;" | "&amp;M105&amp;" |"</f>
-        <v>| by/3.0/ | 7967__cfork__boing-raw.aiff | https://freesound.org/s/7967/ | cfork |</v>
+        <f t="shared" si="14"/>
+        <v>| zero/1.0/ | 500418__dj-somar__intro-reverso-craver-microbrute.wav | https://freesound.org/s/500418/ | DJ_SoMaR |</v>
       </c>
     </row>
     <row r="106" spans="1:18" ht="20.25">
       <c r="A106" s="6" t="str">
-        <f>"&lt;tr&gt;&lt;td&gt;"&amp;J106&amp;"&lt;/td&gt;&lt;td&gt;"&amp;K106&amp;"&lt;/td&gt;&lt;td&gt;"&amp;L106&amp;"&lt;/td&gt;&lt;td&gt;"&amp;M106&amp;"&lt;/td&gt;"</f>
-        <v>&lt;tr&gt;&lt;td&gt;by/3.0/&lt;/td&gt;&lt;td&gt;88635__uair01__bicycle-picture-in-spectrum.wav&lt;/td&gt;&lt;td&gt;https://freesound.org/s/88635/&lt;/td&gt;&lt;td&gt;uair01&lt;/td&gt;</v>
-      </c>
-      <c r="J106" s="30" t="s">
+        <f t="shared" si="12"/>
+        <v>&lt;tr&gt;&lt;td&gt;by/3.0/&lt;/td&gt;&lt;td&gt;7967__cfork__boing-raw.aiff&lt;/td&gt;&lt;td&gt;https://freesound.org/s/7967/&lt;/td&gt;&lt;td&gt;cfork&lt;/td&gt;</v>
+      </c>
+      <c r="J106" s="32" t="s">
         <v>2867</v>
       </c>
       <c r="K106" s="35" t="s">
-        <v>2871</v>
+        <v>2874</v>
       </c>
       <c r="L106" s="29" t="s">
-        <v>2872</v>
+        <v>2875</v>
       </c>
       <c r="M106" s="28" t="s">
-        <v>2873</v>
+        <v>2876</v>
       </c>
       <c r="R106" t="str">
-        <f>"| "&amp;J106&amp;" | "&amp;K106&amp;" | "&amp;L106&amp;" | "&amp;M106&amp;" |"</f>
-        <v>| by/3.0/ | 88635__uair01__bicycle-picture-in-spectrum.wav | https://freesound.org/s/88635/ | uair01 |</v>
+        <f t="shared" si="14"/>
+        <v>| by/3.0/ | 7967__cfork__boing-raw.aiff | https://freesound.org/s/7967/ | cfork |</v>
       </c>
     </row>
     <row r="107" spans="1:18" ht="20.25">
       <c r="A107" s="6" t="str">
-        <f>"&lt;tr&gt;&lt;td&gt;"&amp;J107&amp;"&lt;/td&gt;&lt;td&gt;"&amp;K107&amp;"&lt;/td&gt;&lt;td&gt;"&amp;L107&amp;"&lt;/td&gt;&lt;td&gt;"&amp;M107&amp;"&lt;/td&gt;"</f>
-        <v>&lt;tr&gt;&lt;td&gt;by-nc/3.0/&lt;/td&gt;&lt;td&gt;91296__timbre__bwaang-2-reverb.mp3&lt;/td&gt;&lt;td&gt;https://freesound.org/s/91296/&lt;/td&gt;&lt;td&gt;timbre&lt;/td&gt;</v>
-      </c>
-      <c r="J107" s="35" t="s">
-        <v>2879</v>
-      </c>
-      <c r="K107" s="19" t="s">
-        <v>2891</v>
-      </c>
-      <c r="L107" t="s">
-        <v>2940</v>
+        <f t="shared" si="12"/>
+        <v>&lt;tr&gt;&lt;td&gt;by/3.0/&lt;/td&gt;&lt;td&gt;88635__uair01__bicycle-picture-in-spectrum.wav&lt;/td&gt;&lt;td&gt;https://freesound.org/s/88635/&lt;/td&gt;&lt;td&gt;uair01&lt;/td&gt;</v>
+      </c>
+      <c r="J107" s="30" t="s">
+        <v>2867</v>
+      </c>
+      <c r="K107" s="35" t="s">
+        <v>2871</v>
+      </c>
+      <c r="L107" s="29" t="s">
+        <v>2872</v>
       </c>
       <c r="M107" s="28" t="s">
-        <v>2927</v>
+        <v>2873</v>
       </c>
       <c r="R107" t="str">
-        <f>"| "&amp;J107&amp;" | "&amp;K107&amp;" | "&amp;L107&amp;" | "&amp;M107&amp;" |"</f>
-        <v>| by-nc/3.0/ | 91296__timbre__bwaang-2-reverb.mp3 | https://freesound.org/s/91296/ | timbre |</v>
+        <f t="shared" si="14"/>
+        <v>| by/3.0/ | 88635__uair01__bicycle-picture-in-spectrum.wav | https://freesound.org/s/88635/ | uair01 |</v>
       </c>
     </row>
     <row r="108" spans="1:18" ht="20.25">
       <c r="A108" s="6" t="str">
-        <f>"&lt;tr&gt;&lt;td&gt;"&amp;J108&amp;"&lt;/td&gt;&lt;td&gt;"&amp;K108&amp;"&lt;/td&gt;&lt;td&gt;"&amp;L108&amp;"&lt;/td&gt;&lt;td&gt;"&amp;M108&amp;"&lt;/td&gt;"</f>
+        <f t="shared" si="12"/>
+        <v>&lt;tr&gt;&lt;td&gt;by-nc/3.0/&lt;/td&gt;&lt;td&gt;91296__timbre__bwaang-2-reverb.mp3&lt;/td&gt;&lt;td&gt;https://freesound.org/s/91296/&lt;/td&gt;&lt;td&gt;timbre&lt;/td&gt;</v>
+      </c>
+      <c r="J108" s="35" t="s">
+        <v>2879</v>
+      </c>
+      <c r="K108" s="19" t="s">
+        <v>2891</v>
+      </c>
+      <c r="L108" t="s">
+        <v>2940</v>
+      </c>
+      <c r="M108" s="28" t="s">
+        <v>2927</v>
+      </c>
+      <c r="R108" t="str">
+        <f t="shared" si="14"/>
+        <v>| by-nc/3.0/ | 91296__timbre__bwaang-2-reverb.mp3 | https://freesound.org/s/91296/ | timbre |</v>
+      </c>
+    </row>
+    <row r="109" spans="1:18" ht="20.25">
+      <c r="A109" s="6" t="str">
+        <f t="shared" si="12"/>
         <v>&lt;tr&gt;&lt;td&gt;by/3.0/&lt;/td&gt;&lt;td&gt;96964__gabisaraceni__porta-abrindo-5.wav&lt;/td&gt;&lt;td&gt;https://freesound.org/s/96964/&lt;/td&gt;&lt;td&gt;gabisaraceni&lt;/td&gt;</v>
       </c>
-      <c r="J108" s="35" t="s">
+      <c r="J109" s="35" t="s">
         <v>2867</v>
       </c>
-      <c r="K108" s="19" t="s">
+      <c r="K109" s="19" t="s">
         <v>2908</v>
       </c>
-      <c r="L108" s="29" t="s">
+      <c r="L109" s="29" t="s">
         <v>2912</v>
       </c>
-      <c r="M108" s="28" t="s">
+      <c r="M109" s="28" t="s">
         <v>2909</v>
       </c>
-      <c r="R108" t="str">
-        <f>"| "&amp;J108&amp;" | "&amp;K108&amp;" | "&amp;L108&amp;" | "&amp;M108&amp;" |"</f>
+      <c r="R109" t="str">
+        <f t="shared" si="14"/>
         <v>| by/3.0/ | 96964__gabisaraceni__porta-abrindo-5.wav | https://freesound.org/s/96964/ | gabisaraceni |</v>
       </c>
     </row>
-    <row r="109" spans="1:18">
-      <c r="A109" s="6" t="s">
+    <row r="110" spans="1:18">
+      <c r="A110" s="6" t="s">
         <v>3385</v>
       </c>
     </row>
-    <row r="110" spans="1:18">
-      <c r="A110" t="s">
+    <row r="111" spans="1:18">
+      <c r="A111" t="s">
         <v>3400</v>
       </c>
     </row>
-    <row r="111" spans="1:18">
-      <c r="A111" s="6" t="s">
+    <row r="112" spans="1:18">
+      <c r="A112" s="6" t="s">
         <v>3384</v>
       </c>
     </row>
-    <row r="112" spans="1:18" ht="15.75" thickBot="1">
-      <c r="A112" t="s">
+    <row r="113" spans="1:12" ht="15.75" thickBot="1">
+      <c r="A113" t="s">
         <v>3386</v>
       </c>
     </row>
-    <row r="113" spans="1:12" ht="18" thickBot="1">
-      <c r="A113" s="6" t="str">
-        <f>"&lt;tr&gt;&lt;td&gt;&lt;b&gt;"&amp;J113&amp;"&lt;/b&gt;&lt;/td&gt;&lt;td&gt;&lt;b&gt;"&amp;K113&amp;"&lt;/b&gt;&lt;/td&gt;&lt;td&gt;&lt;b&gt;"&amp;L113&amp;"&lt;/b&gt;&lt;/td&gt;"</f>
+    <row r="114" spans="1:12" ht="18" thickBot="1">
+      <c r="A114" s="6" t="str">
+        <f>"&lt;tr&gt;&lt;td&gt;&lt;b&gt;"&amp;J114&amp;"&lt;/b&gt;&lt;/td&gt;&lt;td&gt;&lt;b&gt;"&amp;K114&amp;"&lt;/b&gt;&lt;/td&gt;&lt;td&gt;&lt;b&gt;"&amp;L114&amp;"&lt;/b&gt;&lt;/td&gt;"</f>
         <v>&lt;tr&gt;&lt;td&gt;&lt;b&gt;Tag&lt;/b&gt;&lt;/td&gt;&lt;td&gt;&lt;b&gt;Name&lt;/b&gt;&lt;/td&gt;&lt;td&gt;&lt;b&gt;URL&lt;/b&gt;&lt;/td&gt;</v>
       </c>
-      <c r="J113" s="57" t="s">
+      <c r="J114" s="57" t="s">
         <v>2855</v>
       </c>
-      <c r="K113" s="57" t="s">
+      <c r="K114" s="57" t="s">
         <v>3387</v>
       </c>
-      <c r="L113" s="57" t="s">
+      <c r="L114" s="57" t="s">
         <v>2857</v>
       </c>
     </row>
-    <row r="114" spans="1:12" ht="45.75" thickBot="1">
-      <c r="A114" s="6" t="str">
-        <f>"&lt;tr&gt;&lt;td&gt;"&amp;J114&amp;"&lt;/td&gt;&lt;td&gt;"&amp;K114&amp;"&lt;/td&gt;&lt;td&gt;"&amp;L114&amp;"&lt;/td&gt;"</f>
-        <v>&lt;tr&gt;&lt;td&gt;zero/1.0/&lt;/td&gt;&lt;td&gt;Creative Commons 0 License&lt;/td&gt;&lt;td&gt;https://creativecommons.org/publicdomain/zero/1.0/&lt;/td&gt;</v>
-      </c>
-      <c r="J114" s="58" t="s">
-        <v>2859</v>
-      </c>
-      <c r="K114" s="58" t="s">
-        <v>3388</v>
-      </c>
-      <c r="L114" s="59" t="s">
-        <v>3389</v>
-      </c>
-    </row>
-    <row r="115" spans="1:12" ht="30.75" thickBot="1">
+    <row r="115" spans="1:12" ht="45.75" thickBot="1">
       <c r="A115" s="6" t="str">
         <f>"&lt;tr&gt;&lt;td&gt;"&amp;J115&amp;"&lt;/td&gt;&lt;td&gt;"&amp;K115&amp;"&lt;/td&gt;&lt;td&gt;"&amp;L115&amp;"&lt;/td&gt;"</f>
-        <v>&lt;tr&gt;&lt;td&gt;by/3.0/&lt;/td&gt;&lt;td&gt;Creative Commons Attribution License&lt;/td&gt;&lt;td&gt;https://creativecommons.org/licenses/by/3.0/&lt;/td&gt;</v>
-      </c>
-      <c r="J115" s="60" t="s">
-        <v>2867</v>
-      </c>
-      <c r="K115" s="60" t="s">
-        <v>3390</v>
-      </c>
-      <c r="L115" s="61" t="s">
-        <v>3391</v>
+        <v>&lt;tr&gt;&lt;td&gt;zero/1.0/&lt;/td&gt;&lt;td&gt;Creative Commons 0 License&lt;/td&gt;&lt;td&gt;https://creativecommons.org/publicdomain/zero/1.0/&lt;/td&gt;</v>
+      </c>
+      <c r="J115" s="58" t="s">
+        <v>2859</v>
+      </c>
+      <c r="K115" s="58" t="s">
+        <v>3388</v>
+      </c>
+      <c r="L115" s="59" t="s">
+        <v>3389</v>
       </c>
     </row>
     <row r="116" spans="1:12" ht="30.75" thickBot="1">
       <c r="A116" s="6" t="str">
         <f>"&lt;tr&gt;&lt;td&gt;"&amp;J116&amp;"&lt;/td&gt;&lt;td&gt;"&amp;K116&amp;"&lt;/td&gt;&lt;td&gt;"&amp;L116&amp;"&lt;/td&gt;"</f>
+        <v>&lt;tr&gt;&lt;td&gt;by/3.0/&lt;/td&gt;&lt;td&gt;Creative Commons Attribution License&lt;/td&gt;&lt;td&gt;https://creativecommons.org/licenses/by/3.0/&lt;/td&gt;</v>
+      </c>
+      <c r="J116" s="60" t="s">
+        <v>2867</v>
+      </c>
+      <c r="K116" s="60" t="s">
+        <v>3390</v>
+      </c>
+      <c r="L116" s="61" t="s">
+        <v>3391</v>
+      </c>
+    </row>
+    <row r="117" spans="1:12" ht="30.75" thickBot="1">
+      <c r="A117" s="6" t="str">
+        <f>"&lt;tr&gt;&lt;td&gt;"&amp;J117&amp;"&lt;/td&gt;&lt;td&gt;"&amp;K117&amp;"&lt;/td&gt;&lt;td&gt;"&amp;L117&amp;"&lt;/td&gt;"</f>
         <v>&lt;tr&gt;&lt;td&gt;by-nc/3.0/&lt;/td&gt;&lt;td&gt;Creative Commons Attribution Noncommercial License&lt;/td&gt;&lt;td&gt;https://creativecommons.org/licenses/by-nc/3.0/&lt;/td&gt;</v>
       </c>
-      <c r="J116" s="58" t="s">
+      <c r="J117" s="58" t="s">
         <v>2879</v>
       </c>
-      <c r="K116" s="58" t="s">
+      <c r="K117" s="58" t="s">
         <v>3392</v>
       </c>
-      <c r="L116" s="59" t="s">
+      <c r="L117" s="59" t="s">
         <v>3393</v>
       </c>
     </row>
-    <row r="117" spans="1:12">
-      <c r="A117" s="6" t="s">
+    <row r="118" spans="1:12">
+      <c r="A118" s="6" t="s">
         <v>3385</v>
       </c>
     </row>
-    <row r="125" spans="1:12">
-      <c r="C125" t="s">
+    <row r="126" spans="1:12">
+      <c r="C126" t="s">
         <v>4677</v>
       </c>
-      <c r="D125" s="29" t="s">
+      <c r="D126" s="29" t="s">
         <v>4676</v>
       </c>
-      <c r="E125" s="29" t="s">
+      <c r="E126" s="29" t="s">
         <v>4675</v>
       </c>
     </row>
-    <row r="158" spans="4:4">
-      <c r="D158" s="9"/>
-    </row>
-    <row r="169" spans="4:4">
-      <c r="D169" s="9"/>
+    <row r="159" spans="4:4">
+      <c r="D159" s="9"/>
+    </row>
+    <row r="170" spans="4:4">
+      <c r="D170" s="9"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:H53" xr:uid="{D49867B0-9605-4DAD-A171-997D81FF01DA}"/>
-  <sortState ref="D146:D170">
-    <sortCondition ref="D146:D170"/>
+  <autoFilter ref="A1:H54" xr:uid="{D49867B0-9605-4DAD-A171-997D81FF01DA}"/>
+  <sortState ref="D147:D171">
+    <sortCondition ref="D147:D171"/>
   </sortState>
   <hyperlinks>
-    <hyperlink ref="L100" r:id="rId1" xr:uid="{0389BFEF-2278-1C4C-AFFD-40911D54BA38}"/>
-    <hyperlink ref="L98" r:id="rId2" xr:uid="{6DC6DCC3-96F7-244A-A515-6ACC236B66A6}"/>
-    <hyperlink ref="L83" r:id="rId3" xr:uid="{CCE745AF-D2B8-1E45-81C2-27CEF6C5B2AF}"/>
-    <hyperlink ref="L89" r:id="rId4" xr:uid="{FC7F966A-1EC2-DE4A-875D-CA9E5FD25210}"/>
-    <hyperlink ref="L106" r:id="rId5" xr:uid="{0DB3DAF8-4FD8-5441-A5EE-FDB2E3108255}"/>
-    <hyperlink ref="L105" r:id="rId6" xr:uid="{6722E195-E4EF-1D49-A046-EFE49EC89CB6}"/>
-    <hyperlink ref="L96" r:id="rId7" xr:uid="{35EA502B-43EE-5648-92D3-03388141605B}"/>
-    <hyperlink ref="L88" r:id="rId8" xr:uid="{F628B53D-420C-0844-AF06-3CBF155582C6}"/>
-    <hyperlink ref="L95" r:id="rId9" xr:uid="{FA1B324F-1513-1343-9CCE-E23AFD154FFD}"/>
-    <hyperlink ref="L104" r:id="rId10" xr:uid="{C5AA4A87-0C8F-9A4C-974F-82A19E89F99C}"/>
-    <hyperlink ref="L92" r:id="rId11" xr:uid="{E1112DD8-8BE8-BD47-9002-F00DDA38363C}"/>
-    <hyperlink ref="L103" r:id="rId12" xr:uid="{4D774EC1-CC16-C24F-88F2-E9E20B8A8FC0}"/>
-    <hyperlink ref="L95:L96" r:id="rId13" display="https://freesound.org/s//" xr:uid="{5FB99E8B-AEFC-6A45-851E-E3C683DC5AC1}"/>
-    <hyperlink ref="L99" r:id="rId14" xr:uid="{E2EACC90-D2ED-AF4A-9302-ADD31B56C321}"/>
-    <hyperlink ref="L108" r:id="rId15" xr:uid="{13F37B0F-8A53-0B4F-8FE7-132D2186D638}"/>
-    <hyperlink ref="L91" r:id="rId16" xr:uid="{FA55BAC7-078A-8944-9FB5-42D7B041E218}"/>
+    <hyperlink ref="L101" r:id="rId1" xr:uid="{0389BFEF-2278-1C4C-AFFD-40911D54BA38}"/>
+    <hyperlink ref="L99" r:id="rId2" xr:uid="{6DC6DCC3-96F7-244A-A515-6ACC236B66A6}"/>
+    <hyperlink ref="L84" r:id="rId3" xr:uid="{CCE745AF-D2B8-1E45-81C2-27CEF6C5B2AF}"/>
+    <hyperlink ref="L90" r:id="rId4" xr:uid="{FC7F966A-1EC2-DE4A-875D-CA9E5FD25210}"/>
+    <hyperlink ref="L107" r:id="rId5" xr:uid="{0DB3DAF8-4FD8-5441-A5EE-FDB2E3108255}"/>
+    <hyperlink ref="L106" r:id="rId6" xr:uid="{6722E195-E4EF-1D49-A046-EFE49EC89CB6}"/>
+    <hyperlink ref="L97" r:id="rId7" xr:uid="{35EA502B-43EE-5648-92D3-03388141605B}"/>
+    <hyperlink ref="L89" r:id="rId8" xr:uid="{F628B53D-420C-0844-AF06-3CBF155582C6}"/>
+    <hyperlink ref="L96" r:id="rId9" xr:uid="{FA1B324F-1513-1343-9CCE-E23AFD154FFD}"/>
+    <hyperlink ref="L105" r:id="rId10" xr:uid="{C5AA4A87-0C8F-9A4C-974F-82A19E89F99C}"/>
+    <hyperlink ref="L93" r:id="rId11" xr:uid="{E1112DD8-8BE8-BD47-9002-F00DDA38363C}"/>
+    <hyperlink ref="L104" r:id="rId12" xr:uid="{4D774EC1-CC16-C24F-88F2-E9E20B8A8FC0}"/>
+    <hyperlink ref="L96:L97" r:id="rId13" display="https://freesound.org/s//" xr:uid="{5FB99E8B-AEFC-6A45-851E-E3C683DC5AC1}"/>
+    <hyperlink ref="L100" r:id="rId14" xr:uid="{E2EACC90-D2ED-AF4A-9302-ADD31B56C321}"/>
+    <hyperlink ref="L109" r:id="rId15" xr:uid="{13F37B0F-8A53-0B4F-8FE7-132D2186D638}"/>
+    <hyperlink ref="L92" r:id="rId16" xr:uid="{FA55BAC7-078A-8944-9FB5-42D7B041E218}"/>
     <hyperlink ref="H27" r:id="rId17" xr:uid="{4419FB35-315D-4DE4-9E5C-9B20E33A87FF}"/>
     <hyperlink ref="H22" r:id="rId18" xr:uid="{0ABC5FB6-8ADD-42B9-BF56-61A08BCA415C}"/>
     <hyperlink ref="H25" r:id="rId19" xr:uid="{189EA614-1A03-48EB-A1CB-FFAA9A4096B3}"/>
@@ -60687,15 +60746,15 @@
     <hyperlink ref="H24" r:id="rId21" xr:uid="{1C69CE9F-8A0A-46D7-8D36-88F69F179169}"/>
     <hyperlink ref="H11" r:id="rId22" xr:uid="{98ABC161-AB9D-4F60-87BE-749E4E4F50E4}"/>
     <hyperlink ref="H9" r:id="rId23" xr:uid="{DBFADD8C-4C9E-493D-9424-41720C23C9D3}"/>
-    <hyperlink ref="H39" r:id="rId24" xr:uid="{C1B31281-1033-4BC4-9D4B-CC2023FF56DB}"/>
-    <hyperlink ref="H32" r:id="rId25" xr:uid="{233967F1-D44D-4DD7-8621-DB03C700D78B}"/>
-    <hyperlink ref="H33" r:id="rId26" xr:uid="{668B5A5D-33C3-48F3-B29D-78E17C45647B}"/>
-    <hyperlink ref="H38" r:id="rId27" xr:uid="{358F58C7-5E85-4805-BCE6-BEBC9EFC5590}"/>
-    <hyperlink ref="H34" r:id="rId28" xr:uid="{9857E7A2-3B5E-4C6F-BE6B-75B1942BF2F1}"/>
-    <hyperlink ref="H36" r:id="rId29" xr:uid="{7817D13B-66BE-451C-A663-245A7D32FB4E}"/>
+    <hyperlink ref="H40" r:id="rId24" xr:uid="{C1B31281-1033-4BC4-9D4B-CC2023FF56DB}"/>
+    <hyperlink ref="H33" r:id="rId25" xr:uid="{233967F1-D44D-4DD7-8621-DB03C700D78B}"/>
+    <hyperlink ref="H34" r:id="rId26" xr:uid="{668B5A5D-33C3-48F3-B29D-78E17C45647B}"/>
+    <hyperlink ref="H39" r:id="rId27" xr:uid="{358F58C7-5E85-4805-BCE6-BEBC9EFC5590}"/>
+    <hyperlink ref="H35" r:id="rId28" xr:uid="{9857E7A2-3B5E-4C6F-BE6B-75B1942BF2F1}"/>
+    <hyperlink ref="H37" r:id="rId29" xr:uid="{7817D13B-66BE-451C-A663-245A7D32FB4E}"/>
     <hyperlink ref="H12" r:id="rId30" xr:uid="{7C24BB00-1AF3-4126-B137-A49F7832B368}"/>
-    <hyperlink ref="H35" r:id="rId31" xr:uid="{093D12FF-CE66-488E-919F-B618F1024F05}"/>
-    <hyperlink ref="H37" r:id="rId32" xr:uid="{99E100BC-474F-4957-8AB6-A17E6091CEA4}"/>
+    <hyperlink ref="H36" r:id="rId31" xr:uid="{093D12FF-CE66-488E-919F-B618F1024F05}"/>
+    <hyperlink ref="H38" r:id="rId32" xr:uid="{99E100BC-474F-4957-8AB6-A17E6091CEA4}"/>
     <hyperlink ref="H2" r:id="rId33" xr:uid="{25C6586F-F991-4DAC-AEAE-61EB9CF85AF5}"/>
     <hyperlink ref="H3" r:id="rId34" xr:uid="{3FD4754B-D29F-42BF-9347-AEB60E71BDB1}"/>
     <hyperlink ref="H5" r:id="rId35" xr:uid="{6D41BF09-100E-4896-BD25-6704EAC36A60}"/>
@@ -60708,17 +60767,17 @@
     <hyperlink ref="H28" r:id="rId42" xr:uid="{9A5F93C5-437C-488C-B3D7-22BAEE17A695}"/>
     <hyperlink ref="H26" r:id="rId43" xr:uid="{5BFD487A-D636-4DDD-B229-99F5CBDC0BE1}"/>
     <hyperlink ref="H23" r:id="rId44" xr:uid="{46A4F8EE-A89B-4A07-8D5D-E50FDDE0611E}"/>
-    <hyperlink ref="H70" r:id="rId45" xr:uid="{5B231739-C8F4-4D4E-B946-7A383ECBBB35}"/>
-    <hyperlink ref="H71" r:id="rId46" xr:uid="{6D8EAE93-D71D-4499-8388-86B77E8848FB}"/>
+    <hyperlink ref="H71" r:id="rId45" xr:uid="{5B231739-C8F4-4D4E-B946-7A383ECBBB35}"/>
+    <hyperlink ref="H72" r:id="rId46" xr:uid="{6D8EAE93-D71D-4499-8388-86B77E8848FB}"/>
     <hyperlink ref="H8" r:id="rId47" xr:uid="{2AE693E7-7449-4538-80A8-30A52F2A22F5}"/>
     <hyperlink ref="H7" r:id="rId48" xr:uid="{2FE1FB4D-693E-4830-8337-658393F68B92}"/>
     <hyperlink ref="H13" r:id="rId49" xr:uid="{DE9970E0-9BDB-45D1-93FA-3F6E016EDFDA}"/>
-    <hyperlink ref="L114" r:id="rId50" xr:uid="{643921F6-79ED-48CE-BC1D-7689B067914F}"/>
-    <hyperlink ref="L115" r:id="rId51" xr:uid="{5EB50EDD-6F80-49BD-9E94-C3F33E3E21E7}"/>
-    <hyperlink ref="L116" r:id="rId52" xr:uid="{3C3C642F-1CE9-4D06-A8F2-3D9A9371558D}"/>
-    <hyperlink ref="L82" r:id="rId53" xr:uid="{EAAF1456-48F9-4E52-8F61-7A6218C1AD87}"/>
-    <hyperlink ref="E125" r:id="rId54" xr:uid="{39B9B4E4-D455-4AB5-A866-4483392BA542}"/>
-    <hyperlink ref="D125" r:id="rId55" xr:uid="{53F0CD4A-267F-4EBB-A9F0-6B230EE74F90}"/>
+    <hyperlink ref="L115" r:id="rId50" xr:uid="{643921F6-79ED-48CE-BC1D-7689B067914F}"/>
+    <hyperlink ref="L116" r:id="rId51" xr:uid="{5EB50EDD-6F80-49BD-9E94-C3F33E3E21E7}"/>
+    <hyperlink ref="L117" r:id="rId52" xr:uid="{3C3C642F-1CE9-4D06-A8F2-3D9A9371558D}"/>
+    <hyperlink ref="L83" r:id="rId53" xr:uid="{EAAF1456-48F9-4E52-8F61-7A6218C1AD87}"/>
+    <hyperlink ref="E126" r:id="rId54" xr:uid="{39B9B4E4-D455-4AB5-A866-4483392BA542}"/>
+    <hyperlink ref="D126" r:id="rId55" xr:uid="{53F0CD4A-267F-4EBB-A9F0-6B230EE74F90}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId56"/>

</xml_diff>

<commit_message>
add factory reset routine
</commit_message>
<xml_diff>
--- a/RBG_arduino/StateTable_minimal.xlsx
+++ b/RBG_arduino/StateTable_minimal.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub-Mark-MDO47\RubberBandGun\RBG_arduino\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F95FBA6-B114-4521-A360-1E630132233A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77995296-BBDB-4CDF-BF34-24E453533888}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21840" activeTab="6" xr2:uid="{CCADFEE4-B0E1-4363-9617-1683960BED03}"/>
   </bookViews>
@@ -47,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7491" uniqueCount="5560">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7499" uniqueCount="5568">
   <si>
     <t>trigOnly</t>
   </si>
@@ -17019,6 +17019,30 @@
   </si>
   <si>
     <t>SKIP</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/* 0 LED PTRN */ </t>
+  </si>
+  <si>
+    <t xml:space="preserve">/* 1 LED PTRN */ </t>
+  </si>
+  <si>
+    <t xml:space="preserve">/* 2 LED PTRN */ </t>
+  </si>
+  <si>
+    <t xml:space="preserve">/* 3 LED PTRN */ </t>
+  </si>
+  <si>
+    <t xml:space="preserve">/* 0 SOUND */    </t>
+  </si>
+  <si>
+    <t xml:space="preserve">/* 1 SOUND */    </t>
+  </si>
+  <si>
+    <t xml:space="preserve">/* 2 SOUND */    </t>
+  </si>
+  <si>
+    <t xml:space="preserve">/* 3 SOUND */    </t>
   </si>
 </sst>
 </file>
@@ -65369,8 +65393,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A827A58D-C8A4-4858-A89B-E853C083564F}">
   <dimension ref="A1:AK187"/>
   <sheetViews>
-    <sheetView topLeftCell="A61" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C69" sqref="C69"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
@@ -70663,16 +70687,16 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B7BCD6B9-C154-4F9D-B8BC-4D842A94058B}">
-  <dimension ref="A1:Y14"/>
+  <dimension ref="A1:AX30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+    <sheetView tabSelected="1" topLeftCell="O1" workbookViewId="0">
+      <selection activeCell="O40" sqref="O40:P40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="2" max="2" width="9.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="3.5703125" customWidth="1"/>
     <col min="4" max="4" width="107" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="3" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="50" bestFit="1" customWidth="1"/>
@@ -70685,6 +70709,7 @@
     <col min="13" max="13" width="3" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="77.28515625" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="29.28515625" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="15.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:25" ht="16.5" thickTop="1" thickBot="1">
@@ -71099,7 +71124,7 @@
         <v>607</v>
       </c>
       <c r="E9" s="55">
-        <v>17</v>
+        <v>7</v>
       </c>
       <c r="F9" s="55" t="s">
         <v>612</v>
@@ -71130,7 +71155,7 @@
       </c>
       <c r="O9" s="55" t="str">
         <f>Y9&amp;M9&amp;" };"</f>
-        <v>/* 2 SOUND */ { 5, 17, 4, 5, 3, 2 };</v>
+        <v>/* 2 SOUND */ { 5, 7, 4, 5, 3, 2 };</v>
       </c>
       <c r="T9" t="str">
         <f>"/* "&amp;A9&amp;" "&amp;B9&amp;" */ { "</f>
@@ -71142,19 +71167,19 @@
       </c>
       <c r="V9" t="str">
         <f>U9&amp;E9&amp;", "</f>
-        <v xml:space="preserve">/* 2 SOUND */ { 5, 17, </v>
+        <v xml:space="preserve">/* 2 SOUND */ { 5, 7, </v>
       </c>
       <c r="W9" t="str">
         <f>V9&amp;G9&amp;", "</f>
-        <v xml:space="preserve">/* 2 SOUND */ { 5, 17, 4, </v>
+        <v xml:space="preserve">/* 2 SOUND */ { 5, 7, 4, </v>
       </c>
       <c r="X9" t="str">
         <f>W9&amp;I9&amp;", "</f>
-        <v xml:space="preserve">/* 2 SOUND */ { 5, 17, 4, 5, </v>
+        <v xml:space="preserve">/* 2 SOUND */ { 5, 7, 4, 5, </v>
       </c>
       <c r="Y9" t="str">
         <f>X9&amp;K9&amp;", "</f>
-        <v xml:space="preserve">/* 2 SOUND */ { 5, 17, 4, 5, 3, </v>
+        <v xml:space="preserve">/* 2 SOUND */ { 5, 7, 4, 5, 3, </v>
       </c>
     </row>
     <row r="10" spans="1:25" ht="16.5" thickTop="1" thickBot="1">
@@ -71391,6 +71416,1052 @@
       </c>
     </row>
     <row r="14" spans="1:25" ht="15.75" thickTop="1"/>
+    <row r="18" spans="16:50" ht="15.75" thickBot="1"/>
+    <row r="19" spans="16:50" ht="16.5" thickTop="1" thickBot="1">
+      <c r="P19" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q19" s="1">
+        <v>1</v>
+      </c>
+      <c r="R19" s="1">
+        <v>2</v>
+      </c>
+      <c r="S19" s="1">
+        <v>3</v>
+      </c>
+      <c r="T19" s="1">
+        <v>4</v>
+      </c>
+      <c r="U19" s="1">
+        <v>5</v>
+      </c>
+      <c r="V19" s="1">
+        <v>6</v>
+      </c>
+      <c r="W19" s="1">
+        <v>7</v>
+      </c>
+      <c r="X19" s="1">
+        <v>8</v>
+      </c>
+      <c r="Y19" s="1">
+        <v>9</v>
+      </c>
+      <c r="Z19" s="1">
+        <v>10</v>
+      </c>
+      <c r="AA19" s="1">
+        <v>11</v>
+      </c>
+      <c r="AB19" s="1">
+        <v>12</v>
+      </c>
+      <c r="AC19" s="1">
+        <v>13</v>
+      </c>
+      <c r="AD19" s="1">
+        <v>14</v>
+      </c>
+      <c r="AE19" s="1">
+        <v>15</v>
+      </c>
+      <c r="AF19" s="1">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="20" spans="16:50" ht="15.75" thickTop="1">
+      <c r="P20">
+        <v>1</v>
+      </c>
+      <c r="Q20">
+        <v>1</v>
+      </c>
+      <c r="R20">
+        <v>6</v>
+      </c>
+      <c r="S20">
+        <v>3</v>
+      </c>
+      <c r="T20">
+        <v>1</v>
+      </c>
+      <c r="U20">
+        <v>1</v>
+      </c>
+      <c r="V20">
+        <v>1</v>
+      </c>
+      <c r="W20">
+        <v>1</v>
+      </c>
+      <c r="X20">
+        <v>1</v>
+      </c>
+      <c r="Y20">
+        <v>1</v>
+      </c>
+      <c r="Z20">
+        <v>1</v>
+      </c>
+      <c r="AA20">
+        <v>1</v>
+      </c>
+      <c r="AB20">
+        <v>1</v>
+      </c>
+      <c r="AC20">
+        <v>1</v>
+      </c>
+      <c r="AD20">
+        <v>1</v>
+      </c>
+      <c r="AE20">
+        <v>25</v>
+      </c>
+      <c r="AF20">
+        <v>1</v>
+      </c>
+      <c r="AG20">
+        <f>LEN(AH20)</f>
+        <v>17</v>
+      </c>
+      <c r="AH20" t="s">
+        <v>5564</v>
+      </c>
+      <c r="AI20" t="str">
+        <f>AH20&amp;P20</f>
+        <v>/* 0 SOUND */    1</v>
+      </c>
+      <c r="AJ20" t="str">
+        <f>AI20&amp;", "&amp;Q20</f>
+        <v>/* 0 SOUND */    1, 1</v>
+      </c>
+      <c r="AK20" t="str">
+        <f t="shared" ref="AK20:BE20" si="0">AJ20&amp;", "&amp;R20</f>
+        <v>/* 0 SOUND */    1, 1, 6</v>
+      </c>
+      <c r="AL20" t="str">
+        <f t="shared" si="0"/>
+        <v>/* 0 SOUND */    1, 1, 6, 3</v>
+      </c>
+      <c r="AM20" t="str">
+        <f t="shared" si="0"/>
+        <v>/* 0 SOUND */    1, 1, 6, 3, 1</v>
+      </c>
+      <c r="AN20" t="str">
+        <f t="shared" si="0"/>
+        <v>/* 0 SOUND */    1, 1, 6, 3, 1, 1</v>
+      </c>
+      <c r="AO20" t="str">
+        <f t="shared" si="0"/>
+        <v>/* 0 SOUND */    1, 1, 6, 3, 1, 1, 1</v>
+      </c>
+      <c r="AP20" t="str">
+        <f t="shared" si="0"/>
+        <v>/* 0 SOUND */    1, 1, 6, 3, 1, 1, 1, 1</v>
+      </c>
+      <c r="AQ20" t="str">
+        <f t="shared" si="0"/>
+        <v>/* 0 SOUND */    1, 1, 6, 3, 1, 1, 1, 1, 1</v>
+      </c>
+      <c r="AR20" t="str">
+        <f t="shared" si="0"/>
+        <v>/* 0 SOUND */    1, 1, 6, 3, 1, 1, 1, 1, 1, 1</v>
+      </c>
+      <c r="AS20" t="str">
+        <f t="shared" si="0"/>
+        <v>/* 0 SOUND */    1, 1, 6, 3, 1, 1, 1, 1, 1, 1, 1</v>
+      </c>
+      <c r="AT20" t="str">
+        <f t="shared" si="0"/>
+        <v>/* 0 SOUND */    1, 1, 6, 3, 1, 1, 1, 1, 1, 1, 1, 1</v>
+      </c>
+      <c r="AU20" t="str">
+        <f t="shared" si="0"/>
+        <v>/* 0 SOUND */    1, 1, 6, 3, 1, 1, 1, 1, 1, 1, 1, 1, 1</v>
+      </c>
+      <c r="AV20" t="str">
+        <f t="shared" si="0"/>
+        <v>/* 0 SOUND */    1, 1, 6, 3, 1, 1, 1, 1, 1, 1, 1, 1, 1, 1</v>
+      </c>
+      <c r="AW20" t="str">
+        <f t="shared" si="0"/>
+        <v>/* 0 SOUND */    1, 1, 6, 3, 1, 1, 1, 1, 1, 1, 1, 1, 1, 1, 1</v>
+      </c>
+      <c r="AX20" t="str">
+        <f t="shared" si="0"/>
+        <v>/* 0 SOUND */    1, 1, 6, 3, 1, 1, 1, 1, 1, 1, 1, 1, 1, 1, 1, 25</v>
+      </c>
+    </row>
+    <row r="21" spans="16:50">
+      <c r="P21">
+        <v>3</v>
+      </c>
+      <c r="Q21">
+        <v>1</v>
+      </c>
+      <c r="R21">
+        <v>5</v>
+      </c>
+      <c r="S21">
+        <v>1</v>
+      </c>
+      <c r="T21">
+        <v>1</v>
+      </c>
+      <c r="U21">
+        <v>7</v>
+      </c>
+      <c r="V21">
+        <v>1</v>
+      </c>
+      <c r="W21">
+        <v>1</v>
+      </c>
+      <c r="X21">
+        <v>1</v>
+      </c>
+      <c r="Y21">
+        <v>1</v>
+      </c>
+      <c r="Z21">
+        <v>1</v>
+      </c>
+      <c r="AA21">
+        <v>1</v>
+      </c>
+      <c r="AB21">
+        <v>1</v>
+      </c>
+      <c r="AC21">
+        <v>1</v>
+      </c>
+      <c r="AD21">
+        <v>1</v>
+      </c>
+      <c r="AE21">
+        <v>1</v>
+      </c>
+      <c r="AF21">
+        <v>1</v>
+      </c>
+      <c r="AG21">
+        <f>LEN(AH21)</f>
+        <v>17</v>
+      </c>
+      <c r="AH21" t="s">
+        <v>5560</v>
+      </c>
+      <c r="AI21" t="str">
+        <f>AH21&amp;P21</f>
+        <v>/* 0 LED PTRN */ 3</v>
+      </c>
+      <c r="AJ21" t="str">
+        <f>AI21&amp;", "&amp;Q21</f>
+        <v>/* 0 LED PTRN */ 3, 1</v>
+      </c>
+      <c r="AK21" t="str">
+        <f t="shared" ref="AK21" si="1">AJ21&amp;", "&amp;R21</f>
+        <v>/* 0 LED PTRN */ 3, 1, 5</v>
+      </c>
+      <c r="AL21" t="str">
+        <f t="shared" ref="AL21" si="2">AK21&amp;", "&amp;S21</f>
+        <v>/* 0 LED PTRN */ 3, 1, 5, 1</v>
+      </c>
+      <c r="AM21" t="str">
+        <f t="shared" ref="AM21" si="3">AL21&amp;", "&amp;T21</f>
+        <v>/* 0 LED PTRN */ 3, 1, 5, 1, 1</v>
+      </c>
+      <c r="AN21" t="str">
+        <f t="shared" ref="AN21" si="4">AM21&amp;", "&amp;U21</f>
+        <v>/* 0 LED PTRN */ 3, 1, 5, 1, 1, 7</v>
+      </c>
+      <c r="AO21" t="str">
+        <f t="shared" ref="AO21" si="5">AN21&amp;", "&amp;V21</f>
+        <v>/* 0 LED PTRN */ 3, 1, 5, 1, 1, 7, 1</v>
+      </c>
+      <c r="AP21" t="str">
+        <f t="shared" ref="AP21" si="6">AO21&amp;", "&amp;W21</f>
+        <v>/* 0 LED PTRN */ 3, 1, 5, 1, 1, 7, 1, 1</v>
+      </c>
+      <c r="AQ21" t="str">
+        <f t="shared" ref="AQ21" si="7">AP21&amp;", "&amp;X21</f>
+        <v>/* 0 LED PTRN */ 3, 1, 5, 1, 1, 7, 1, 1, 1</v>
+      </c>
+      <c r="AR21" t="str">
+        <f t="shared" ref="AR21" si="8">AQ21&amp;", "&amp;Y21</f>
+        <v>/* 0 LED PTRN */ 3, 1, 5, 1, 1, 7, 1, 1, 1, 1</v>
+      </c>
+      <c r="AS21" t="str">
+        <f t="shared" ref="AS21" si="9">AR21&amp;", "&amp;Z21</f>
+        <v>/* 0 LED PTRN */ 3, 1, 5, 1, 1, 7, 1, 1, 1, 1, 1</v>
+      </c>
+      <c r="AT21" t="str">
+        <f t="shared" ref="AT21" si="10">AS21&amp;", "&amp;AA21</f>
+        <v>/* 0 LED PTRN */ 3, 1, 5, 1, 1, 7, 1, 1, 1, 1, 1, 1</v>
+      </c>
+      <c r="AU21" t="str">
+        <f t="shared" ref="AU21" si="11">AT21&amp;", "&amp;AB21</f>
+        <v>/* 0 LED PTRN */ 3, 1, 5, 1, 1, 7, 1, 1, 1, 1, 1, 1, 1</v>
+      </c>
+      <c r="AV21" t="str">
+        <f t="shared" ref="AV21" si="12">AU21&amp;", "&amp;AC21</f>
+        <v>/* 0 LED PTRN */ 3, 1, 5, 1, 1, 7, 1, 1, 1, 1, 1, 1, 1, 1</v>
+      </c>
+      <c r="AW21" t="str">
+        <f t="shared" ref="AW21" si="13">AV21&amp;", "&amp;AD21</f>
+        <v>/* 0 LED PTRN */ 3, 1, 5, 1, 1, 7, 1, 1, 1, 1, 1, 1, 1, 1, 1</v>
+      </c>
+      <c r="AX21" t="str">
+        <f t="shared" ref="AX21" si="14">AW21&amp;", "&amp;AE21</f>
+        <v>/* 0 LED PTRN */ 3, 1, 5, 1, 1, 7, 1, 1, 1, 1, 1, 1, 1, 1, 1, 1</v>
+      </c>
+    </row>
+    <row r="23" spans="16:50">
+      <c r="P23">
+        <v>4</v>
+      </c>
+      <c r="Q23">
+        <v>4</v>
+      </c>
+      <c r="R23">
+        <v>5</v>
+      </c>
+      <c r="S23">
+        <v>4</v>
+      </c>
+      <c r="T23">
+        <v>2</v>
+      </c>
+      <c r="U23">
+        <v>3</v>
+      </c>
+      <c r="V23">
+        <v>1</v>
+      </c>
+      <c r="W23">
+        <v>1</v>
+      </c>
+      <c r="X23">
+        <v>1</v>
+      </c>
+      <c r="Y23">
+        <v>1</v>
+      </c>
+      <c r="Z23">
+        <v>1</v>
+      </c>
+      <c r="AA23">
+        <v>1</v>
+      </c>
+      <c r="AB23">
+        <v>1</v>
+      </c>
+      <c r="AC23">
+        <v>1</v>
+      </c>
+      <c r="AD23">
+        <v>1</v>
+      </c>
+      <c r="AE23">
+        <v>25</v>
+      </c>
+      <c r="AF23">
+        <v>1</v>
+      </c>
+      <c r="AG23">
+        <f>LEN(AH23)</f>
+        <v>17</v>
+      </c>
+      <c r="AH23" t="s">
+        <v>5565</v>
+      </c>
+      <c r="AI23" t="str">
+        <f>AH23&amp;P23</f>
+        <v>/* 1 SOUND */    4</v>
+      </c>
+      <c r="AJ23" t="str">
+        <f>AI23&amp;", "&amp;Q23</f>
+        <v>/* 1 SOUND */    4, 4</v>
+      </c>
+      <c r="AK23" t="str">
+        <f t="shared" ref="AK23:AK24" si="15">AJ23&amp;", "&amp;R23</f>
+        <v>/* 1 SOUND */    4, 4, 5</v>
+      </c>
+      <c r="AL23" t="str">
+        <f t="shared" ref="AL23:AL24" si="16">AK23&amp;", "&amp;S23</f>
+        <v>/* 1 SOUND */    4, 4, 5, 4</v>
+      </c>
+      <c r="AM23" t="str">
+        <f t="shared" ref="AM23:AM24" si="17">AL23&amp;", "&amp;T23</f>
+        <v>/* 1 SOUND */    4, 4, 5, 4, 2</v>
+      </c>
+      <c r="AN23" t="str">
+        <f t="shared" ref="AN23:AN24" si="18">AM23&amp;", "&amp;U23</f>
+        <v>/* 1 SOUND */    4, 4, 5, 4, 2, 3</v>
+      </c>
+      <c r="AO23" t="str">
+        <f t="shared" ref="AO23:AO24" si="19">AN23&amp;", "&amp;V23</f>
+        <v>/* 1 SOUND */    4, 4, 5, 4, 2, 3, 1</v>
+      </c>
+      <c r="AP23" t="str">
+        <f t="shared" ref="AP23:AP24" si="20">AO23&amp;", "&amp;W23</f>
+        <v>/* 1 SOUND */    4, 4, 5, 4, 2, 3, 1, 1</v>
+      </c>
+      <c r="AQ23" t="str">
+        <f t="shared" ref="AQ23:AQ24" si="21">AP23&amp;", "&amp;X23</f>
+        <v>/* 1 SOUND */    4, 4, 5, 4, 2, 3, 1, 1, 1</v>
+      </c>
+      <c r="AR23" t="str">
+        <f t="shared" ref="AR23:AR24" si="22">AQ23&amp;", "&amp;Y23</f>
+        <v>/* 1 SOUND */    4, 4, 5, 4, 2, 3, 1, 1, 1, 1</v>
+      </c>
+      <c r="AS23" t="str">
+        <f t="shared" ref="AS23:AS24" si="23">AR23&amp;", "&amp;Z23</f>
+        <v>/* 1 SOUND */    4, 4, 5, 4, 2, 3, 1, 1, 1, 1, 1</v>
+      </c>
+      <c r="AT23" t="str">
+        <f t="shared" ref="AT23:AT24" si="24">AS23&amp;", "&amp;AA23</f>
+        <v>/* 1 SOUND */    4, 4, 5, 4, 2, 3, 1, 1, 1, 1, 1, 1</v>
+      </c>
+      <c r="AU23" t="str">
+        <f t="shared" ref="AU23:AU24" si="25">AT23&amp;", "&amp;AB23</f>
+        <v>/* 1 SOUND */    4, 4, 5, 4, 2, 3, 1, 1, 1, 1, 1, 1, 1</v>
+      </c>
+      <c r="AV23" t="str">
+        <f t="shared" ref="AV23:AV24" si="26">AU23&amp;", "&amp;AC23</f>
+        <v>/* 1 SOUND */    4, 4, 5, 4, 2, 3, 1, 1, 1, 1, 1, 1, 1, 1</v>
+      </c>
+      <c r="AW23" t="str">
+        <f t="shared" ref="AW23:AW24" si="27">AV23&amp;", "&amp;AD23</f>
+        <v>/* 1 SOUND */    4, 4, 5, 4, 2, 3, 1, 1, 1, 1, 1, 1, 1, 1, 1</v>
+      </c>
+      <c r="AX23" t="str">
+        <f t="shared" ref="AX23:AX24" si="28">AW23&amp;", "&amp;AE23</f>
+        <v>/* 1 SOUND */    4, 4, 5, 4, 2, 3, 1, 1, 1, 1, 1, 1, 1, 1, 1, 25</v>
+      </c>
+    </row>
+    <row r="24" spans="16:50">
+      <c r="P24">
+        <v>6</v>
+      </c>
+      <c r="Q24">
+        <v>2</v>
+      </c>
+      <c r="R24">
+        <v>4</v>
+      </c>
+      <c r="S24">
+        <v>6</v>
+      </c>
+      <c r="T24">
+        <v>2</v>
+      </c>
+      <c r="U24">
+        <v>6</v>
+      </c>
+      <c r="V24">
+        <v>1</v>
+      </c>
+      <c r="W24">
+        <v>1</v>
+      </c>
+      <c r="X24">
+        <v>1</v>
+      </c>
+      <c r="Y24">
+        <v>1</v>
+      </c>
+      <c r="Z24">
+        <v>1</v>
+      </c>
+      <c r="AA24">
+        <v>1</v>
+      </c>
+      <c r="AB24">
+        <v>1</v>
+      </c>
+      <c r="AC24">
+        <v>1</v>
+      </c>
+      <c r="AD24">
+        <v>1</v>
+      </c>
+      <c r="AE24">
+        <v>1</v>
+      </c>
+      <c r="AF24">
+        <v>1</v>
+      </c>
+      <c r="AG24">
+        <f>LEN(AH24)</f>
+        <v>17</v>
+      </c>
+      <c r="AH24" t="s">
+        <v>5561</v>
+      </c>
+      <c r="AI24" t="str">
+        <f>AH24&amp;P24</f>
+        <v>/* 1 LED PTRN */ 6</v>
+      </c>
+      <c r="AJ24" t="str">
+        <f>AI24&amp;", "&amp;Q24</f>
+        <v>/* 1 LED PTRN */ 6, 2</v>
+      </c>
+      <c r="AK24" t="str">
+        <f t="shared" si="15"/>
+        <v>/* 1 LED PTRN */ 6, 2, 4</v>
+      </c>
+      <c r="AL24" t="str">
+        <f t="shared" si="16"/>
+        <v>/* 1 LED PTRN */ 6, 2, 4, 6</v>
+      </c>
+      <c r="AM24" t="str">
+        <f t="shared" si="17"/>
+        <v>/* 1 LED PTRN */ 6, 2, 4, 6, 2</v>
+      </c>
+      <c r="AN24" t="str">
+        <f t="shared" si="18"/>
+        <v>/* 1 LED PTRN */ 6, 2, 4, 6, 2, 6</v>
+      </c>
+      <c r="AO24" t="str">
+        <f t="shared" si="19"/>
+        <v>/* 1 LED PTRN */ 6, 2, 4, 6, 2, 6, 1</v>
+      </c>
+      <c r="AP24" t="str">
+        <f t="shared" si="20"/>
+        <v>/* 1 LED PTRN */ 6, 2, 4, 6, 2, 6, 1, 1</v>
+      </c>
+      <c r="AQ24" t="str">
+        <f t="shared" si="21"/>
+        <v>/* 1 LED PTRN */ 6, 2, 4, 6, 2, 6, 1, 1, 1</v>
+      </c>
+      <c r="AR24" t="str">
+        <f t="shared" si="22"/>
+        <v>/* 1 LED PTRN */ 6, 2, 4, 6, 2, 6, 1, 1, 1, 1</v>
+      </c>
+      <c r="AS24" t="str">
+        <f t="shared" si="23"/>
+        <v>/* 1 LED PTRN */ 6, 2, 4, 6, 2, 6, 1, 1, 1, 1, 1</v>
+      </c>
+      <c r="AT24" t="str">
+        <f t="shared" si="24"/>
+        <v>/* 1 LED PTRN */ 6, 2, 4, 6, 2, 6, 1, 1, 1, 1, 1, 1</v>
+      </c>
+      <c r="AU24" t="str">
+        <f t="shared" si="25"/>
+        <v>/* 1 LED PTRN */ 6, 2, 4, 6, 2, 6, 1, 1, 1, 1, 1, 1, 1</v>
+      </c>
+      <c r="AV24" t="str">
+        <f t="shared" si="26"/>
+        <v>/* 1 LED PTRN */ 6, 2, 4, 6, 2, 6, 1, 1, 1, 1, 1, 1, 1, 1</v>
+      </c>
+      <c r="AW24" t="str">
+        <f t="shared" si="27"/>
+        <v>/* 1 LED PTRN */ 6, 2, 4, 6, 2, 6, 1, 1, 1, 1, 1, 1, 1, 1, 1</v>
+      </c>
+      <c r="AX24" t="str">
+        <f t="shared" si="28"/>
+        <v>/* 1 LED PTRN */ 6, 2, 4, 6, 2, 6, 1, 1, 1, 1, 1, 1, 1, 1, 1, 1</v>
+      </c>
+    </row>
+    <row r="26" spans="16:50">
+      <c r="P26">
+        <v>5</v>
+      </c>
+      <c r="Q26">
+        <v>7</v>
+      </c>
+      <c r="R26">
+        <v>4</v>
+      </c>
+      <c r="S26">
+        <v>5</v>
+      </c>
+      <c r="T26">
+        <v>3</v>
+      </c>
+      <c r="U26">
+        <v>2</v>
+      </c>
+      <c r="V26">
+        <v>1</v>
+      </c>
+      <c r="W26">
+        <v>1</v>
+      </c>
+      <c r="X26">
+        <v>1</v>
+      </c>
+      <c r="Y26">
+        <v>1</v>
+      </c>
+      <c r="Z26">
+        <v>1</v>
+      </c>
+      <c r="AA26">
+        <v>1</v>
+      </c>
+      <c r="AB26">
+        <v>1</v>
+      </c>
+      <c r="AC26">
+        <v>1</v>
+      </c>
+      <c r="AD26">
+        <v>1</v>
+      </c>
+      <c r="AE26">
+        <v>25</v>
+      </c>
+      <c r="AF26">
+        <v>1</v>
+      </c>
+      <c r="AG26">
+        <f>LEN(AH26)</f>
+        <v>17</v>
+      </c>
+      <c r="AH26" t="s">
+        <v>5566</v>
+      </c>
+      <c r="AI26" t="str">
+        <f>AH26&amp;P26</f>
+        <v>/* 2 SOUND */    5</v>
+      </c>
+      <c r="AJ26" t="str">
+        <f>AI26&amp;", "&amp;Q26</f>
+        <v>/* 2 SOUND */    5, 7</v>
+      </c>
+      <c r="AK26" t="str">
+        <f t="shared" ref="AK26:AK27" si="29">AJ26&amp;", "&amp;R26</f>
+        <v>/* 2 SOUND */    5, 7, 4</v>
+      </c>
+      <c r="AL26" t="str">
+        <f t="shared" ref="AL26:AL27" si="30">AK26&amp;", "&amp;S26</f>
+        <v>/* 2 SOUND */    5, 7, 4, 5</v>
+      </c>
+      <c r="AM26" t="str">
+        <f t="shared" ref="AM26:AM27" si="31">AL26&amp;", "&amp;T26</f>
+        <v>/* 2 SOUND */    5, 7, 4, 5, 3</v>
+      </c>
+      <c r="AN26" t="str">
+        <f t="shared" ref="AN26:AN27" si="32">AM26&amp;", "&amp;U26</f>
+        <v>/* 2 SOUND */    5, 7, 4, 5, 3, 2</v>
+      </c>
+      <c r="AO26" t="str">
+        <f t="shared" ref="AO26:AO27" si="33">AN26&amp;", "&amp;V26</f>
+        <v>/* 2 SOUND */    5, 7, 4, 5, 3, 2, 1</v>
+      </c>
+      <c r="AP26" t="str">
+        <f t="shared" ref="AP26:AP27" si="34">AO26&amp;", "&amp;W26</f>
+        <v>/* 2 SOUND */    5, 7, 4, 5, 3, 2, 1, 1</v>
+      </c>
+      <c r="AQ26" t="str">
+        <f t="shared" ref="AQ26:AQ27" si="35">AP26&amp;", "&amp;X26</f>
+        <v>/* 2 SOUND */    5, 7, 4, 5, 3, 2, 1, 1, 1</v>
+      </c>
+      <c r="AR26" t="str">
+        <f t="shared" ref="AR26:AR27" si="36">AQ26&amp;", "&amp;Y26</f>
+        <v>/* 2 SOUND */    5, 7, 4, 5, 3, 2, 1, 1, 1, 1</v>
+      </c>
+      <c r="AS26" t="str">
+        <f t="shared" ref="AS26:AS27" si="37">AR26&amp;", "&amp;Z26</f>
+        <v>/* 2 SOUND */    5, 7, 4, 5, 3, 2, 1, 1, 1, 1, 1</v>
+      </c>
+      <c r="AT26" t="str">
+        <f t="shared" ref="AT26:AT27" si="38">AS26&amp;", "&amp;AA26</f>
+        <v>/* 2 SOUND */    5, 7, 4, 5, 3, 2, 1, 1, 1, 1, 1, 1</v>
+      </c>
+      <c r="AU26" t="str">
+        <f t="shared" ref="AU26:AU27" si="39">AT26&amp;", "&amp;AB26</f>
+        <v>/* 2 SOUND */    5, 7, 4, 5, 3, 2, 1, 1, 1, 1, 1, 1, 1</v>
+      </c>
+      <c r="AV26" t="str">
+        <f t="shared" ref="AV26:AV27" si="40">AU26&amp;", "&amp;AC26</f>
+        <v>/* 2 SOUND */    5, 7, 4, 5, 3, 2, 1, 1, 1, 1, 1, 1, 1, 1</v>
+      </c>
+      <c r="AW26" t="str">
+        <f t="shared" ref="AW26:AW27" si="41">AV26&amp;", "&amp;AD26</f>
+        <v>/* 2 SOUND */    5, 7, 4, 5, 3, 2, 1, 1, 1, 1, 1, 1, 1, 1, 1</v>
+      </c>
+      <c r="AX26" t="str">
+        <f t="shared" ref="AX26:AX27" si="42">AW26&amp;", "&amp;AE26</f>
+        <v>/* 2 SOUND */    5, 7, 4, 5, 3, 2, 1, 1, 1, 1, 1, 1, 1, 1, 1, 25</v>
+      </c>
+    </row>
+    <row r="27" spans="16:50">
+      <c r="P27">
+        <v>1</v>
+      </c>
+      <c r="Q27">
+        <v>3</v>
+      </c>
+      <c r="R27">
+        <v>1</v>
+      </c>
+      <c r="S27">
+        <v>3</v>
+      </c>
+      <c r="T27">
+        <v>3</v>
+      </c>
+      <c r="U27">
+        <v>1</v>
+      </c>
+      <c r="V27">
+        <v>1</v>
+      </c>
+      <c r="W27">
+        <v>1</v>
+      </c>
+      <c r="X27">
+        <v>1</v>
+      </c>
+      <c r="Y27">
+        <v>1</v>
+      </c>
+      <c r="Z27">
+        <v>1</v>
+      </c>
+      <c r="AA27">
+        <v>1</v>
+      </c>
+      <c r="AB27">
+        <v>1</v>
+      </c>
+      <c r="AC27">
+        <v>1</v>
+      </c>
+      <c r="AD27">
+        <v>1</v>
+      </c>
+      <c r="AE27">
+        <v>1</v>
+      </c>
+      <c r="AF27">
+        <v>1</v>
+      </c>
+      <c r="AG27">
+        <f>LEN(AH27)</f>
+        <v>17</v>
+      </c>
+      <c r="AH27" t="s">
+        <v>5562</v>
+      </c>
+      <c r="AI27" t="str">
+        <f>AH27&amp;P27</f>
+        <v>/* 2 LED PTRN */ 1</v>
+      </c>
+      <c r="AJ27" t="str">
+        <f>AI27&amp;", "&amp;Q27</f>
+        <v>/* 2 LED PTRN */ 1, 3</v>
+      </c>
+      <c r="AK27" t="str">
+        <f t="shared" si="29"/>
+        <v>/* 2 LED PTRN */ 1, 3, 1</v>
+      </c>
+      <c r="AL27" t="str">
+        <f t="shared" si="30"/>
+        <v>/* 2 LED PTRN */ 1, 3, 1, 3</v>
+      </c>
+      <c r="AM27" t="str">
+        <f t="shared" si="31"/>
+        <v>/* 2 LED PTRN */ 1, 3, 1, 3, 3</v>
+      </c>
+      <c r="AN27" t="str">
+        <f t="shared" si="32"/>
+        <v>/* 2 LED PTRN */ 1, 3, 1, 3, 3, 1</v>
+      </c>
+      <c r="AO27" t="str">
+        <f t="shared" si="33"/>
+        <v>/* 2 LED PTRN */ 1, 3, 1, 3, 3, 1, 1</v>
+      </c>
+      <c r="AP27" t="str">
+        <f t="shared" si="34"/>
+        <v>/* 2 LED PTRN */ 1, 3, 1, 3, 3, 1, 1, 1</v>
+      </c>
+      <c r="AQ27" t="str">
+        <f t="shared" si="35"/>
+        <v>/* 2 LED PTRN */ 1, 3, 1, 3, 3, 1, 1, 1, 1</v>
+      </c>
+      <c r="AR27" t="str">
+        <f t="shared" si="36"/>
+        <v>/* 2 LED PTRN */ 1, 3, 1, 3, 3, 1, 1, 1, 1, 1</v>
+      </c>
+      <c r="AS27" t="str">
+        <f t="shared" si="37"/>
+        <v>/* 2 LED PTRN */ 1, 3, 1, 3, 3, 1, 1, 1, 1, 1, 1</v>
+      </c>
+      <c r="AT27" t="str">
+        <f t="shared" si="38"/>
+        <v>/* 2 LED PTRN */ 1, 3, 1, 3, 3, 1, 1, 1, 1, 1, 1, 1</v>
+      </c>
+      <c r="AU27" t="str">
+        <f t="shared" si="39"/>
+        <v>/* 2 LED PTRN */ 1, 3, 1, 3, 3, 1, 1, 1, 1, 1, 1, 1, 1</v>
+      </c>
+      <c r="AV27" t="str">
+        <f t="shared" si="40"/>
+        <v>/* 2 LED PTRN */ 1, 3, 1, 3, 3, 1, 1, 1, 1, 1, 1, 1, 1, 1</v>
+      </c>
+      <c r="AW27" t="str">
+        <f t="shared" si="41"/>
+        <v>/* 2 LED PTRN */ 1, 3, 1, 3, 3, 1, 1, 1, 1, 1, 1, 1, 1, 1, 1</v>
+      </c>
+      <c r="AX27" t="str">
+        <f t="shared" si="42"/>
+        <v>/* 2 LED PTRN */ 1, 3, 1, 3, 3, 1, 1, 1, 1, 1, 1, 1, 1, 1, 1, 1</v>
+      </c>
+    </row>
+    <row r="29" spans="16:50">
+      <c r="P29">
+        <v>3</v>
+      </c>
+      <c r="Q29">
+        <v>2</v>
+      </c>
+      <c r="R29">
+        <v>3</v>
+      </c>
+      <c r="S29">
+        <v>6</v>
+      </c>
+      <c r="T29">
+        <v>4</v>
+      </c>
+      <c r="U29">
+        <v>6</v>
+      </c>
+      <c r="V29">
+        <v>1</v>
+      </c>
+      <c r="W29">
+        <v>1</v>
+      </c>
+      <c r="X29">
+        <v>1</v>
+      </c>
+      <c r="Y29">
+        <v>1</v>
+      </c>
+      <c r="Z29">
+        <v>1</v>
+      </c>
+      <c r="AA29">
+        <v>1</v>
+      </c>
+      <c r="AB29">
+        <v>1</v>
+      </c>
+      <c r="AC29">
+        <v>1</v>
+      </c>
+      <c r="AD29">
+        <v>1</v>
+      </c>
+      <c r="AE29">
+        <v>25</v>
+      </c>
+      <c r="AF29">
+        <v>1</v>
+      </c>
+      <c r="AG29">
+        <f t="shared" ref="AG29:AG30" si="43">LEN(AH29)</f>
+        <v>17</v>
+      </c>
+      <c r="AH29" t="s">
+        <v>5567</v>
+      </c>
+      <c r="AI29" t="str">
+        <f>AH29&amp;P29</f>
+        <v>/* 3 SOUND */    3</v>
+      </c>
+      <c r="AJ29" t="str">
+        <f>AI29&amp;", "&amp;Q29</f>
+        <v>/* 3 SOUND */    3, 2</v>
+      </c>
+      <c r="AK29" t="str">
+        <f t="shared" ref="AK29:AK30" si="44">AJ29&amp;", "&amp;R29</f>
+        <v>/* 3 SOUND */    3, 2, 3</v>
+      </c>
+      <c r="AL29" t="str">
+        <f t="shared" ref="AL29:AL30" si="45">AK29&amp;", "&amp;S29</f>
+        <v>/* 3 SOUND */    3, 2, 3, 6</v>
+      </c>
+      <c r="AM29" t="str">
+        <f t="shared" ref="AM29:AM30" si="46">AL29&amp;", "&amp;T29</f>
+        <v>/* 3 SOUND */    3, 2, 3, 6, 4</v>
+      </c>
+      <c r="AN29" t="str">
+        <f t="shared" ref="AN29:AN30" si="47">AM29&amp;", "&amp;U29</f>
+        <v>/* 3 SOUND */    3, 2, 3, 6, 4, 6</v>
+      </c>
+      <c r="AO29" t="str">
+        <f t="shared" ref="AO29:AO30" si="48">AN29&amp;", "&amp;V29</f>
+        <v>/* 3 SOUND */    3, 2, 3, 6, 4, 6, 1</v>
+      </c>
+      <c r="AP29" t="str">
+        <f t="shared" ref="AP29:AP30" si="49">AO29&amp;", "&amp;W29</f>
+        <v>/* 3 SOUND */    3, 2, 3, 6, 4, 6, 1, 1</v>
+      </c>
+      <c r="AQ29" t="str">
+        <f t="shared" ref="AQ29:AQ30" si="50">AP29&amp;", "&amp;X29</f>
+        <v>/* 3 SOUND */    3, 2, 3, 6, 4, 6, 1, 1, 1</v>
+      </c>
+      <c r="AR29" t="str">
+        <f t="shared" ref="AR29:AR30" si="51">AQ29&amp;", "&amp;Y29</f>
+        <v>/* 3 SOUND */    3, 2, 3, 6, 4, 6, 1, 1, 1, 1</v>
+      </c>
+      <c r="AS29" t="str">
+        <f t="shared" ref="AS29:AS30" si="52">AR29&amp;", "&amp;Z29</f>
+        <v>/* 3 SOUND */    3, 2, 3, 6, 4, 6, 1, 1, 1, 1, 1</v>
+      </c>
+      <c r="AT29" t="str">
+        <f t="shared" ref="AT29:AT30" si="53">AS29&amp;", "&amp;AA29</f>
+        <v>/* 3 SOUND */    3, 2, 3, 6, 4, 6, 1, 1, 1, 1, 1, 1</v>
+      </c>
+      <c r="AU29" t="str">
+        <f t="shared" ref="AU29:AU30" si="54">AT29&amp;", "&amp;AB29</f>
+        <v>/* 3 SOUND */    3, 2, 3, 6, 4, 6, 1, 1, 1, 1, 1, 1, 1</v>
+      </c>
+      <c r="AV29" t="str">
+        <f t="shared" ref="AV29:AV30" si="55">AU29&amp;", "&amp;AC29</f>
+        <v>/* 3 SOUND */    3, 2, 3, 6, 4, 6, 1, 1, 1, 1, 1, 1, 1, 1</v>
+      </c>
+      <c r="AW29" t="str">
+        <f t="shared" ref="AW29:AW30" si="56">AV29&amp;", "&amp;AD29</f>
+        <v>/* 3 SOUND */    3, 2, 3, 6, 4, 6, 1, 1, 1, 1, 1, 1, 1, 1, 1</v>
+      </c>
+      <c r="AX29" t="str">
+        <f t="shared" ref="AX29:AX30" si="57">AW29&amp;", "&amp;AE29</f>
+        <v>/* 3 SOUND */    3, 2, 3, 6, 4, 6, 1, 1, 1, 1, 1, 1, 1, 1, 1, 25</v>
+      </c>
+    </row>
+    <row r="30" spans="16:50">
+      <c r="P30">
+        <v>5</v>
+      </c>
+      <c r="Q30">
+        <v>8</v>
+      </c>
+      <c r="R30">
+        <v>6</v>
+      </c>
+      <c r="S30">
+        <v>2</v>
+      </c>
+      <c r="T30">
+        <v>7</v>
+      </c>
+      <c r="U30">
+        <v>3</v>
+      </c>
+      <c r="V30">
+        <v>1</v>
+      </c>
+      <c r="W30">
+        <v>1</v>
+      </c>
+      <c r="X30">
+        <v>1</v>
+      </c>
+      <c r="Y30">
+        <v>1</v>
+      </c>
+      <c r="Z30">
+        <v>1</v>
+      </c>
+      <c r="AA30">
+        <v>1</v>
+      </c>
+      <c r="AB30">
+        <v>1</v>
+      </c>
+      <c r="AC30">
+        <v>1</v>
+      </c>
+      <c r="AD30">
+        <v>1</v>
+      </c>
+      <c r="AE30">
+        <v>1</v>
+      </c>
+      <c r="AF30">
+        <v>1</v>
+      </c>
+      <c r="AG30">
+        <f t="shared" si="43"/>
+        <v>17</v>
+      </c>
+      <c r="AH30" t="s">
+        <v>5563</v>
+      </c>
+      <c r="AI30" t="str">
+        <f>AH30&amp;P30</f>
+        <v>/* 3 LED PTRN */ 5</v>
+      </c>
+      <c r="AJ30" t="str">
+        <f>AI30&amp;", "&amp;Q30</f>
+        <v>/* 3 LED PTRN */ 5, 8</v>
+      </c>
+      <c r="AK30" t="str">
+        <f t="shared" si="44"/>
+        <v>/* 3 LED PTRN */ 5, 8, 6</v>
+      </c>
+      <c r="AL30" t="str">
+        <f t="shared" si="45"/>
+        <v>/* 3 LED PTRN */ 5, 8, 6, 2</v>
+      </c>
+      <c r="AM30" t="str">
+        <f t="shared" si="46"/>
+        <v>/* 3 LED PTRN */ 5, 8, 6, 2, 7</v>
+      </c>
+      <c r="AN30" t="str">
+        <f t="shared" si="47"/>
+        <v>/* 3 LED PTRN */ 5, 8, 6, 2, 7, 3</v>
+      </c>
+      <c r="AO30" t="str">
+        <f t="shared" si="48"/>
+        <v>/* 3 LED PTRN */ 5, 8, 6, 2, 7, 3, 1</v>
+      </c>
+      <c r="AP30" t="str">
+        <f t="shared" si="49"/>
+        <v>/* 3 LED PTRN */ 5, 8, 6, 2, 7, 3, 1, 1</v>
+      </c>
+      <c r="AQ30" t="str">
+        <f t="shared" si="50"/>
+        <v>/* 3 LED PTRN */ 5, 8, 6, 2, 7, 3, 1, 1, 1</v>
+      </c>
+      <c r="AR30" t="str">
+        <f t="shared" si="51"/>
+        <v>/* 3 LED PTRN */ 5, 8, 6, 2, 7, 3, 1, 1, 1, 1</v>
+      </c>
+      <c r="AS30" t="str">
+        <f t="shared" si="52"/>
+        <v>/* 3 LED PTRN */ 5, 8, 6, 2, 7, 3, 1, 1, 1, 1, 1</v>
+      </c>
+      <c r="AT30" t="str">
+        <f t="shared" si="53"/>
+        <v>/* 3 LED PTRN */ 5, 8, 6, 2, 7, 3, 1, 1, 1, 1, 1, 1</v>
+      </c>
+      <c r="AU30" t="str">
+        <f t="shared" si="54"/>
+        <v>/* 3 LED PTRN */ 5, 8, 6, 2, 7, 3, 1, 1, 1, 1, 1, 1, 1</v>
+      </c>
+      <c r="AV30" t="str">
+        <f t="shared" si="55"/>
+        <v>/* 3 LED PTRN */ 5, 8, 6, 2, 7, 3, 1, 1, 1, 1, 1, 1, 1, 1</v>
+      </c>
+      <c r="AW30" t="str">
+        <f t="shared" si="56"/>
+        <v>/* 3 LED PTRN */ 5, 8, 6, 2, 7, 3, 1, 1, 1, 1, 1, 1, 1, 1, 1</v>
+      </c>
+      <c r="AX30" t="str">
+        <f t="shared" si="57"/>
+        <v>/* 3 LED PTRN */ 5, 8, 6, 2, 7, 3, 1, 1, 1, 1, 1, 1, 1, 1, 1, 1</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="7">
     <mergeCell ref="O1:O2"/>

</xml_diff>

<commit_message>
update to KiCad 5.1.5 and implement RAM copy of EEPROM settings
</commit_message>
<xml_diff>
--- a/RBG_arduino/StateTable_minimal.xlsx
+++ b/RBG_arduino/StateTable_minimal.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub-Mark-MDO47\RubberBandGun\RBG_arduino\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E0B736A-C39C-4828-9126-3E1F6849E417}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{50039932-9DBD-404C-97EF-39F06FA75451}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21840" activeTab="6" xr2:uid="{CCADFEE4-B0E1-4363-9617-1683960BED03}"/>
+    <workbookView xWindow="11460" yWindow="3435" windowWidth="25965" windowHeight="16875" activeTab="7" xr2:uid="{CCADFEE4-B0E1-4363-9617-1683960BED03}"/>
   </bookViews>
   <sheets>
     <sheet name="StateTable" sheetId="1" r:id="rId1"/>
@@ -20,12 +20,14 @@
     <sheet name="Sounds" sheetId="5" r:id="rId5"/>
     <sheet name="LEDpatterns" sheetId="7" r:id="rId6"/>
     <sheet name="FactorySettings" sheetId="8" r:id="rId7"/>
+    <sheet name="NPNdriver" sheetId="9" r:id="rId8"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">debugging!$A$4959:$B$5342</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">LEDpatterns!$A$1:$M$61</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">Sounds!$A$1:$H$60</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">StateTable!$A$1:$K$168</definedName>
+    <definedName name="gain2N3904">NPNdriver!$K$20:$L$24</definedName>
     <definedName name="LEDlookup">LEDpatterns!$I$2:$J$31</definedName>
     <definedName name="mROW">StateTable!$V$2:$X$40</definedName>
     <definedName name="prev">Sounds!$AK$2:$AK$18</definedName>
@@ -47,7 +49,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8121" uniqueCount="5985">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8150" uniqueCount="6011">
   <si>
     <t>trigOnly</t>
   </si>
@@ -18295,12 +18297,162 @@
   <si>
     <t>mdo47 "I" recording of "Pew... pew-pew!"</t>
   </si>
+  <si>
+    <t>For an example, the load you are controlling requires 200mA; that's the collector current I . Further let's use a typical</t>
+  </si>
+  <si>
+    <t>transistor (such as a PN2222) that has a gain of ~100 at that collector current. Looking at the</t>
+  </si>
+  <si>
+    <t>datasheet (https://adafru.it/CoB) we see that the Base-Emitter Saturation Voltage (on page 2) is 0.6v. That will cause</t>
+  </si>
+  <si>
+    <t>the transistor to saturate. If we control this with a 3.3v microcontroller then the bias resistor needs to have 3.3v - 0.6v =</t>
+  </si>
+  <si>
+    <t>2.7v across it. With an I of 200mA and a gain of 100, we have a base current I of I /gain = 200mA/100 = 2mA. This is</t>
+  </si>
+  <si>
+    <t>within the range of a typical GPIO pin's current rating*. We will need a resistor of 2.7v/2mA = 2.7/0.002 = 1350 ohms.</t>
+  </si>
+  <si>
+    <t>1.2K ohms is a common value, and using a slightly lower bias resistor than the calculation indicates will result in a</t>
+  </si>
+  <si>
+    <t>slightly higher base-emitter current and guarantee that the transistor is saturated when the input is high.</t>
+  </si>
+  <si>
+    <t>Assume:</t>
+  </si>
+  <si>
+    <t>mA</t>
+  </si>
+  <si>
+    <t>load current</t>
+  </si>
+  <si>
+    <t>2N3904</t>
+  </si>
+  <si>
+    <t>https://www.onsemi.com/pub/Collateral/2N3903-D.PDF</t>
+  </si>
+  <si>
+    <t>https://www.onsemi.com/pub/Collateral/PN2222-D.PDF</t>
+  </si>
+  <si>
+    <t>PN2222</t>
+  </si>
+  <si>
+    <r>
+      <t>(collector current I</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>c</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>)</t>
+    </r>
+  </si>
+  <si>
+    <t>gain</t>
+  </si>
+  <si>
+    <t>Base-Emitter Saturation Voltage</t>
+  </si>
+  <si>
+    <r>
+      <t>(Base−Emitter Saturation Voltage V</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>BE(sat)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>)</t>
+    </r>
+  </si>
+  <si>
+    <t>V</t>
+  </si>
+  <si>
+    <t>operating voltage</t>
+  </si>
+  <si>
+    <r>
+      <t>(DC Current Gain h</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>FE</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>)</t>
+    </r>
+  </si>
+  <si>
+    <t>Ohms</t>
+  </si>
+  <si>
+    <t>bias resistor</t>
+  </si>
+  <si>
+    <t>draw from Arduino</t>
+  </si>
+  <si>
+    <t>2N3904 gain</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="25">
+  <numFmts count="1">
+    <numFmt numFmtId="168" formatCode="0.000"/>
+  </numFmts>
+  <fonts count="26">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -18475,6 +18627,14 @@
       <color theme="1"/>
       <name val="Courier New"/>
       <family val="3"/>
+    </font>
+    <font>
+      <vertAlign val="subscript"/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="14">
@@ -18729,7 +18889,7 @@
     <xf numFmtId="0" fontId="19" fillId="10" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="10" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="91">
+  <cellXfs count="93">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -18907,12 +19067,6 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="12" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="12" xfId="1" applyBorder="1" applyAlignment="1">
@@ -18926,6 +19080,16 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="12" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="168" fontId="19" fillId="10" borderId="3" xfId="8" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="10">
@@ -79590,7 +79754,7 @@
       <c r="A76" s="56" t="s">
         <v>583</v>
       </c>
-      <c r="B76" s="90">
+      <c r="B76" s="88">
         <v>108</v>
       </c>
       <c r="C76" s="76" t="s">
@@ -79627,7 +79791,7 @@
       <c r="A77" s="56" t="s">
         <v>583</v>
       </c>
-      <c r="B77" s="90">
+      <c r="B77" s="88">
         <v>109</v>
       </c>
       <c r="C77" s="76" t="s">
@@ -82468,7 +82632,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B7BCD6B9-C154-4F9D-B8BC-4D842A94058B}">
   <dimension ref="A1:AX30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F51" sqref="F51"/>
     </sheetView>
   </sheetViews>
@@ -82492,10 +82656,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:25" ht="16.5" thickTop="1" thickBot="1">
-      <c r="A1" s="86" t="s">
+      <c r="A1" s="84" t="s">
         <v>3965</v>
       </c>
-      <c r="B1" s="86" t="s">
+      <c r="B1" s="84" t="s">
         <v>4490</v>
       </c>
       <c r="C1" s="59">
@@ -82534,44 +82698,44 @@
       <c r="N1" s="82" t="s">
         <v>4488</v>
       </c>
-      <c r="O1" s="84" t="s">
+      <c r="O1" s="89" t="s">
         <v>4491</v>
       </c>
     </row>
     <row r="2" spans="1:25" ht="16.5" thickTop="1" thickBot="1">
-      <c r="A2" s="87"/>
+      <c r="A2" s="85"/>
       <c r="B2" s="59"/>
-      <c r="C2" s="84" t="s">
+      <c r="C2" s="89" t="s">
         <v>45</v>
       </c>
-      <c r="D2" s="84"/>
-      <c r="E2" s="84" t="s">
+      <c r="D2" s="89"/>
+      <c r="E2" s="89" t="s">
         <v>44</v>
       </c>
-      <c r="F2" s="84"/>
-      <c r="G2" s="84" t="s">
+      <c r="F2" s="89"/>
+      <c r="G2" s="89" t="s">
         <v>33</v>
       </c>
-      <c r="H2" s="84"/>
-      <c r="I2" s="84" t="s">
+      <c r="H2" s="89"/>
+      <c r="I2" s="89" t="s">
         <v>34</v>
       </c>
-      <c r="J2" s="84"/>
-      <c r="K2" s="84" t="s">
+      <c r="J2" s="89"/>
+      <c r="K2" s="89" t="s">
         <v>32</v>
       </c>
-      <c r="L2" s="84"/>
-      <c r="M2" s="84" t="s">
+      <c r="L2" s="89"/>
+      <c r="M2" s="89" t="s">
         <v>601</v>
       </c>
-      <c r="N2" s="84"/>
-      <c r="O2" s="85"/>
+      <c r="N2" s="89"/>
+      <c r="O2" s="90"/>
     </row>
     <row r="3" spans="1:25" ht="16.5" thickTop="1" thickBot="1">
       <c r="A3" s="59">
         <v>0</v>
       </c>
-      <c r="B3" s="88" t="s">
+      <c r="B3" s="86" t="s">
         <v>4489</v>
       </c>
       <c r="C3" s="55">
@@ -82643,7 +82807,7 @@
       <c r="A4" s="59">
         <v>0</v>
       </c>
-      <c r="B4" s="88" t="s">
+      <c r="B4" s="86" t="s">
         <v>4492</v>
       </c>
       <c r="C4" s="55">
@@ -82713,7 +82877,7 @@
     </row>
     <row r="5" spans="1:25" ht="5.0999999999999996" customHeight="1" thickTop="1" thickBot="1">
       <c r="A5" s="55"/>
-      <c r="B5" s="89"/>
+      <c r="B5" s="87"/>
       <c r="C5" s="55"/>
       <c r="D5" s="55"/>
       <c r="E5" s="55"/>
@@ -82732,7 +82896,7 @@
       <c r="A6" s="59">
         <v>1</v>
       </c>
-      <c r="B6" s="88" t="s">
+      <c r="B6" s="86" t="s">
         <v>4489</v>
       </c>
       <c r="C6" s="55">
@@ -82804,7 +82968,7 @@
       <c r="A7" s="59">
         <v>1</v>
       </c>
-      <c r="B7" s="88" t="s">
+      <c r="B7" s="86" t="s">
         <v>4492</v>
       </c>
       <c r="C7" s="55">
@@ -82874,7 +83038,7 @@
     </row>
     <row r="8" spans="1:25" ht="5.0999999999999996" customHeight="1" thickTop="1" thickBot="1">
       <c r="A8" s="55"/>
-      <c r="B8" s="89"/>
+      <c r="B8" s="87"/>
       <c r="C8" s="55"/>
       <c r="D8" s="55"/>
       <c r="E8" s="55"/>
@@ -82893,7 +83057,7 @@
       <c r="A9" s="59">
         <v>2</v>
       </c>
-      <c r="B9" s="88" t="s">
+      <c r="B9" s="86" t="s">
         <v>4489</v>
       </c>
       <c r="C9" s="55">
@@ -82965,7 +83129,7 @@
       <c r="A10" s="59">
         <v>2</v>
       </c>
-      <c r="B10" s="88" t="s">
+      <c r="B10" s="86" t="s">
         <v>4492</v>
       </c>
       <c r="C10" s="55">
@@ -83035,7 +83199,7 @@
     </row>
     <row r="11" spans="1:25" ht="5.0999999999999996" customHeight="1" thickTop="1" thickBot="1">
       <c r="A11" s="55"/>
-      <c r="B11" s="89"/>
+      <c r="B11" s="87"/>
       <c r="C11" s="55"/>
       <c r="D11" s="55"/>
       <c r="E11" s="55"/>
@@ -83054,7 +83218,7 @@
       <c r="A12" s="59">
         <v>3</v>
       </c>
-      <c r="B12" s="88" t="s">
+      <c r="B12" s="86" t="s">
         <v>4489</v>
       </c>
       <c r="C12" s="55">
@@ -83126,7 +83290,7 @@
       <c r="A13" s="59">
         <v>3</v>
       </c>
-      <c r="B13" s="88" t="s">
+      <c r="B13" s="86" t="s">
         <v>4492</v>
       </c>
       <c r="C13" s="55">
@@ -83317,7 +83481,7 @@
         <v>/* 0 SOUND */    1, 1</v>
       </c>
       <c r="AK20" t="str">
-        <f t="shared" ref="AK20:BE20" si="0">AJ20&amp;", "&amp;R20</f>
+        <f t="shared" ref="AK20:AX20" si="0">AJ20&amp;", "&amp;R20</f>
         <v>/* 0 SOUND */    1, 1, 6</v>
       </c>
       <c r="AL20" t="str">
@@ -84254,4 +84418,202 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8BE2C291-905D-498B-BBAE-3002C1E85A91}">
+  <dimension ref="A2:L24"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B20" sqref="B20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="2" spans="1:2">
+      <c r="A2" t="s">
+        <v>5985</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" t="s">
+        <v>5986</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4" t="s">
+        <v>5987</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
+      <c r="A5" t="s">
+        <v>5988</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
+      <c r="A6" t="s">
+        <v>5989</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2">
+      <c r="A7" t="s">
+        <v>5990</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2">
+      <c r="A8" t="s">
+        <v>5991</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2">
+      <c r="A9" t="s">
+        <v>5992</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2">
+      <c r="A13" t="s">
+        <v>5999</v>
+      </c>
+      <c r="B13" s="24" t="s">
+        <v>5998</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2">
+      <c r="A14" t="s">
+        <v>5996</v>
+      </c>
+      <c r="B14" s="24" t="s">
+        <v>5997</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2">
+      <c r="A16" t="s">
+        <v>5993</v>
+      </c>
+    </row>
+    <row r="18" spans="2:12">
+      <c r="B18" t="s">
+        <v>5996</v>
+      </c>
+    </row>
+    <row r="19" spans="2:12" ht="18">
+      <c r="B19">
+        <v>50</v>
+      </c>
+      <c r="C19" t="s">
+        <v>5994</v>
+      </c>
+      <c r="D19" t="s">
+        <v>5995</v>
+      </c>
+      <c r="F19" t="s">
+        <v>6000</v>
+      </c>
+      <c r="K19" s="92" t="s">
+        <v>6010</v>
+      </c>
+      <c r="L19" s="92"/>
+    </row>
+    <row r="20" spans="2:12" ht="18">
+      <c r="B20">
+        <f>VLOOKUP(B19,gain2N3904,2,TRUE)</f>
+        <v>60</v>
+      </c>
+      <c r="D20" t="s">
+        <v>6001</v>
+      </c>
+      <c r="F20" t="s">
+        <v>6006</v>
+      </c>
+      <c r="K20">
+        <v>0.1</v>
+      </c>
+      <c r="L20">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="21" spans="2:12" ht="18">
+      <c r="B21">
+        <v>0.85</v>
+      </c>
+      <c r="C21" t="s">
+        <v>6004</v>
+      </c>
+      <c r="D21" t="s">
+        <v>6002</v>
+      </c>
+      <c r="F21" t="s">
+        <v>6003</v>
+      </c>
+      <c r="K21">
+        <v>1</v>
+      </c>
+      <c r="L21">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="22" spans="2:12">
+      <c r="B22">
+        <v>5</v>
+      </c>
+      <c r="C22" t="s">
+        <v>6004</v>
+      </c>
+      <c r="D22" t="s">
+        <v>6005</v>
+      </c>
+      <c r="K22">
+        <v>10</v>
+      </c>
+      <c r="L22">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="23" spans="2:12">
+      <c r="B23" s="91">
+        <f>B19/B20</f>
+        <v>0.83333333333333337</v>
+      </c>
+      <c r="C23" t="s">
+        <v>5994</v>
+      </c>
+      <c r="D23" t="s">
+        <v>6009</v>
+      </c>
+      <c r="K23">
+        <v>50</v>
+      </c>
+      <c r="L23">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="24" spans="2:12">
+      <c r="B24" s="64">
+        <f>(B22-B21)/(B23/1000)</f>
+        <v>4980</v>
+      </c>
+      <c r="C24" t="s">
+        <v>6007</v>
+      </c>
+      <c r="D24" t="s">
+        <v>6008</v>
+      </c>
+      <c r="K24">
+        <v>100</v>
+      </c>
+      <c r="L24">
+        <v>30</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="K19:L19"/>
+  </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="B14" r:id="rId1" xr:uid="{48EBF1C7-8AFD-4D66-9287-83DD11BFAEB9}"/>
+    <hyperlink ref="B13" r:id="rId2" xr:uid="{D1796FDE-0C80-45EF-AE7E-88A546D83D38}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
add Cassini Saturn sound
</commit_message>
<xml_diff>
--- a/RBG_arduino/StateTable_minimal.xlsx
+++ b/RBG_arduino/StateTable_minimal.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub-Mark-MDO47\RubberBandGun\RBG_arduino\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0AF6DDA9-A92E-48F9-908E-0A6878C601EC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52A0A78D-35AD-478E-8CC7-5141C370236B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21840" xr2:uid="{CCADFEE4-B0E1-4363-9617-1683960BED03}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21840" activeTab="6" xr2:uid="{CCADFEE4-B0E1-4363-9617-1683960BED03}"/>
   </bookViews>
   <sheets>
     <sheet name="StateTable" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">debugging!$A$5359:$B$5769</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">LEDpatterns!$A$1:$M$61</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">Sounds!$A$1:$H$60</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">Sounds!$A$1:$H$61</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">StateTable!$A$1:$K$162</definedName>
     <definedName name="gain2N3904">NPNdriver!$K$20:$L$24</definedName>
     <definedName name="LEDlookup">LEDpatterns!$I$2:$J$31</definedName>
@@ -49,7 +49,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8746" uniqueCount="6450">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8753" uniqueCount="6454">
   <si>
     <t>trigOnly</t>
   </si>
@@ -19760,6 +19760,18 @@
   </si>
   <si>
     <t>Advanced menu - demo mode</t>
+  </si>
+  <si>
+    <t>SKR-03-324.wav</t>
+  </si>
+  <si>
+    <t>http://www-pw.physics.uiowa.edu/space-audio/cassini/SKR1/SKR-03-324.wav</t>
+  </si>
+  <si>
+    <t>Cassini sounds of Saturn radio waves</t>
+  </si>
+  <si>
+    <t>NASA Cassini University of Iowa</t>
   </si>
 </sst>
 </file>
@@ -20730,9 +20742,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{90E8DFC6-94F4-4A82-A874-2F16F2CF0145}">
   <dimension ref="A1:AB162"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E89" sqref="E89:E91"/>
+    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A119" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D30" sqref="D30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
@@ -76458,10 +76470,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A827A58D-C8A4-4858-A89B-E853C083564F}">
-  <dimension ref="A1:AK189"/>
+  <dimension ref="A1:AK190"/>
   <sheetViews>
-    <sheetView topLeftCell="A65" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C74" sqref="C74"/>
+    <sheetView topLeftCell="A23" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="D44" sqref="D44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
@@ -77371,7 +77383,7 @@
         <v>#define mEFCT_PWRON_CFOOF                 43 // Achtung! This is the awesome FOOF Rubber Band Gun.</v>
       </c>
       <c r="P31" t="str">
-        <f>REPT(" ",J40-J41)</f>
+        <f>REPT(" ",J40-J42)</f>
         <v xml:space="preserve">                </v>
       </c>
     </row>
@@ -77628,62 +77640,51 @@
         <v>537</v>
       </c>
       <c r="J40">
-        <f>MAX(J41:J73)</f>
+        <f>MAX(J42:J74)</f>
         <v>32</v>
       </c>
       <c r="K40" t="s">
         <v>642</v>
       </c>
     </row>
-    <row r="41" spans="1:11" ht="120">
-      <c r="A41" s="56" t="s">
-        <v>583</v>
-      </c>
-      <c r="B41" s="55">
-        <v>62</v>
-      </c>
-      <c r="C41" s="50" t="s">
-        <v>607</v>
-      </c>
-      <c r="D41" s="10" t="s">
-        <v>709</v>
-      </c>
-      <c r="E41" s="56" t="s">
-        <v>583</v>
-      </c>
-      <c r="F41" s="53" t="s">
-        <v>471</v>
+    <row r="41" spans="1:11" ht="20.25">
+      <c r="A41" s="55" t="s">
+        <v>455</v>
+      </c>
+      <c r="B41" s="49">
+        <v>59</v>
+      </c>
+      <c r="C41" s="58" t="s">
+        <v>6450</v>
+      </c>
+      <c r="D41" s="52" t="s">
+        <v>6452</v>
+      </c>
+      <c r="E41" s="52" t="s">
+        <v>455</v>
+      </c>
+      <c r="F41" s="57" t="s">
+        <v>594</v>
       </c>
       <c r="G41" s="57" t="s">
-        <v>578</v>
-      </c>
-      <c r="H41" s="55" t="s">
-        <v>579</v>
-      </c>
-      <c r="I41" s="22" t="s">
-        <v>619</v>
-      </c>
-      <c r="J41">
-        <f>LEN(I41)</f>
-        <v>16</v>
-      </c>
-      <c r="K41" s="65" t="str">
-        <f t="shared" ref="K41:K56" si="2">"#define "&amp;I41&amp;" "&amp;REPT(" ",$J$40-J41)&amp;RIGHT(TEXT(B41,"    #"),3)&amp;" // "&amp;RIGHT(LEFT(D41,LEN(D41)-1),LEN(D41)-1-FIND("""",D41))</f>
-        <v>#define mEFCT_UNIQ_INTRO                  62 // Welcome to the FOOF Rubber Band Gun configuration! Your call is important to us. Press trigger by itself to go forward to next step or to cycle through choices. To select a choice, first hold down any combination of Yellow or Green button then press trigger. To exit configuration, hold down Red button then press trigger.</v>
-      </c>
-    </row>
-    <row r="42" spans="1:11" ht="135">
+        <v>6453</v>
+      </c>
+      <c r="H41" s="54" t="s">
+        <v>6451</v>
+      </c>
+    </row>
+    <row r="42" spans="1:11" ht="120">
       <c r="A42" s="56" t="s">
         <v>583</v>
       </c>
       <c r="B42" s="55">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C42" s="50" t="s">
-        <v>670</v>
+        <v>607</v>
       </c>
       <c r="D42" s="52" t="s">
-        <v>4481</v>
+        <v>709</v>
       </c>
       <c r="E42" s="56" t="s">
         <v>583</v>
@@ -77698,52 +77699,52 @@
         <v>579</v>
       </c>
       <c r="I42" s="22" t="s">
+        <v>619</v>
+      </c>
+      <c r="J42">
+        <f>LEN(I42)</f>
+        <v>16</v>
+      </c>
+      <c r="K42" s="65" t="str">
+        <f t="shared" ref="K42:K57" si="2">"#define "&amp;I42&amp;" "&amp;REPT(" ",$J$40-J42)&amp;RIGHT(TEXT(B42,"    #"),3)&amp;" // "&amp;RIGHT(LEFT(D42,LEN(D42)-1),LEN(D42)-1-FIND("""",D42))</f>
+        <v>#define mEFCT_UNIQ_INTRO                  62 // Welcome to the FOOF Rubber Band Gun configuration! Your call is important to us. Press trigger by itself to go forward to next step or to cycle through choices. To select a choice, first hold down any combination of Yellow or Green button then press trigger. To exit configuration, hold down Red button then press trigger.</v>
+      </c>
+    </row>
+    <row r="43" spans="1:11" ht="135">
+      <c r="A43" s="56" t="s">
+        <v>583</v>
+      </c>
+      <c r="B43" s="55">
+        <v>63</v>
+      </c>
+      <c r="C43" s="50" t="s">
+        <v>670</v>
+      </c>
+      <c r="D43" s="52" t="s">
+        <v>4481</v>
+      </c>
+      <c r="E43" s="56" t="s">
+        <v>583</v>
+      </c>
+      <c r="F43" s="53" t="s">
+        <v>471</v>
+      </c>
+      <c r="G43" s="57" t="s">
+        <v>578</v>
+      </c>
+      <c r="H43" s="55" t="s">
+        <v>579</v>
+      </c>
+      <c r="I43" s="22" t="s">
         <v>662</v>
       </c>
-      <c r="J42">
-        <f t="shared" ref="J42:J44" si="3">LEN(I42)</f>
+      <c r="J43">
+        <f t="shared" ref="J43:J45" si="3">LEN(I43)</f>
         <v>23</v>
       </c>
-      <c r="K42" s="65" t="str">
+      <c r="K43" s="65" t="str">
         <f t="shared" si="2"/>
         <v>#define mEFCT_UNIQ_CFG_CATEGORY           63 // Now choose which configuration category: sound effects, LED pattern effects, configuration resets and copying, or advanced settings. As always, press trigger by itself to go forward to next step or to cycle through choices. To select a choice, first hold down any combination of Yellow or Green button then press trigger. To exit configuration, hold down Red button then press trigger.</v>
-      </c>
-    </row>
-    <row r="43" spans="1:11" ht="120">
-      <c r="A43" s="56" t="s">
-        <v>583</v>
-      </c>
-      <c r="B43" s="55">
-        <v>64</v>
-      </c>
-      <c r="C43" s="50" t="s">
-        <v>671</v>
-      </c>
-      <c r="D43" s="52" t="s">
-        <v>710</v>
-      </c>
-      <c r="E43" s="56" t="s">
-        <v>583</v>
-      </c>
-      <c r="F43" s="53" t="s">
-        <v>471</v>
-      </c>
-      <c r="G43" s="57" t="s">
-        <v>578</v>
-      </c>
-      <c r="H43" s="55" t="s">
-        <v>579</v>
-      </c>
-      <c r="I43" s="22" t="s">
-        <v>663</v>
-      </c>
-      <c r="J43">
-        <f t="shared" si="3"/>
-        <v>19</v>
-      </c>
-      <c r="K43" s="65" t="str">
-        <f t="shared" si="2"/>
-        <v>#define mEFCT_UNIQ_CFG_TYPE               64 // Now choose when the effect happens. This list includes when powering-on, when shooting, etc. As always, press trigger by itself to go forward to next step or to cycle through choices. To select a choice, first hold down any combination of Yellow or Green button then press trigger. To exit configuration, hold down Red button then press trigger.</v>
       </c>
     </row>
     <row r="44" spans="1:11" ht="120">
@@ -77751,13 +77752,13 @@
         <v>583</v>
       </c>
       <c r="B44" s="55">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C44" s="50" t="s">
-        <v>672</v>
+        <v>671</v>
       </c>
       <c r="D44" s="52" t="s">
-        <v>711</v>
+        <v>710</v>
       </c>
       <c r="E44" s="56" t="s">
         <v>583</v>
@@ -77772,29 +77773,29 @@
         <v>579</v>
       </c>
       <c r="I44" s="22" t="s">
-        <v>714</v>
+        <v>663</v>
       </c>
       <c r="J44">
         <f t="shared" si="3"/>
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="K44" s="65" t="str">
         <f t="shared" si="2"/>
-        <v>#define mEFCT_UNIQ_CFG_EFFECT             65 // Now choose the effect itself. This list cycles through the effects one by one. As always, press trigger by itself to go forward to next step or to cycle through choices. To select a choice, first hold down any combination of Yellow or Green button then press trigger. To exit configuration, hold down Red button then press trigger.</v>
-      </c>
-    </row>
-    <row r="45" spans="1:11" ht="105">
+        <v>#define mEFCT_UNIQ_CFG_TYPE               64 // Now choose when the effect happens. This list includes when powering-on, when shooting, etc. As always, press trigger by itself to go forward to next step or to cycle through choices. To select a choice, first hold down any combination of Yellow or Green button then press trigger. To exit configuration, hold down Red button then press trigger.</v>
+      </c>
+    </row>
+    <row r="45" spans="1:11" ht="120">
       <c r="A45" s="56" t="s">
         <v>583</v>
       </c>
       <c r="B45" s="55">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C45" s="50" t="s">
-        <v>4436</v>
+        <v>672</v>
       </c>
       <c r="D45" s="52" t="s">
-        <v>4434</v>
+        <v>711</v>
       </c>
       <c r="E45" s="56" t="s">
         <v>583</v>
@@ -77809,29 +77810,29 @@
         <v>579</v>
       </c>
       <c r="I45" s="22" t="s">
-        <v>4433</v>
+        <v>714</v>
       </c>
       <c r="J45">
-        <f>LEN(I45)</f>
-        <v>25</v>
+        <f t="shared" si="3"/>
+        <v>21</v>
       </c>
       <c r="K45" s="65" t="str">
         <f t="shared" si="2"/>
-        <v>#define mEFCT_UNIQ_CFG_LED2CHOOSE         66 // This is an LED pattern you can choose. As always, press trigger by itself to go forward to next step or to cycle through choices. To select a choice, first hold down any combination of Yellow or Green button then press trigger. To exit configuration, hold down Red button then press trigger.</v>
-      </c>
-    </row>
-    <row r="46" spans="1:11" ht="30">
+        <v>#define mEFCT_UNIQ_CFG_EFFECT             65 // Now choose the effect itself. This list cycles through the effects one by one. As always, press trigger by itself to go forward to next step or to cycle through choices. To select a choice, first hold down any combination of Yellow or Green button then press trigger. To exit configuration, hold down Red button then press trigger.</v>
+      </c>
+    </row>
+    <row r="46" spans="1:11" ht="105">
       <c r="A46" s="56" t="s">
         <v>583</v>
       </c>
       <c r="B46" s="55">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C46" s="50" t="s">
-        <v>4435</v>
+        <v>4436</v>
       </c>
       <c r="D46" s="52" t="s">
-        <v>4452</v>
+        <v>4434</v>
       </c>
       <c r="E46" s="56" t="s">
         <v>583</v>
@@ -77846,15 +77847,15 @@
         <v>579</v>
       </c>
       <c r="I46" s="22" t="s">
-        <v>713</v>
+        <v>4433</v>
       </c>
       <c r="J46">
-        <f t="shared" ref="J46:J48" si="4">LEN(I46)</f>
-        <v>21</v>
+        <f>LEN(I46)</f>
+        <v>25</v>
       </c>
       <c r="K46" s="65" t="str">
         <f t="shared" si="2"/>
-        <v>#define mEFCT_UNIQ_CFG_ACCEPT             67 // Your choice has been saved into the running settings.</v>
+        <v>#define mEFCT_UNIQ_CFG_LED2CHOOSE         66 // This is an LED pattern you can choose. As always, press trigger by itself to go forward to next step or to cycle through choices. To select a choice, first hold down any combination of Yellow or Green button then press trigger. To exit configuration, hold down Red button then press trigger.</v>
       </c>
     </row>
     <row r="47" spans="1:11" ht="30">
@@ -77862,13 +77863,13 @@
         <v>583</v>
       </c>
       <c r="B47" s="55">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C47" s="50" t="s">
-        <v>4453</v>
-      </c>
-      <c r="D47" s="56" t="s">
-        <v>725</v>
+        <v>4435</v>
+      </c>
+      <c r="D47" s="52" t="s">
+        <v>4452</v>
       </c>
       <c r="E47" s="56" t="s">
         <v>583</v>
@@ -77883,29 +77884,29 @@
         <v>579</v>
       </c>
       <c r="I47" s="22" t="s">
-        <v>613</v>
+        <v>713</v>
       </c>
       <c r="J47">
-        <f>LEN(I47)</f>
-        <v>19</v>
+        <f t="shared" ref="J47:J49" si="4">LEN(I47)</f>
+        <v>21</v>
       </c>
       <c r="K47" s="65" t="str">
         <f t="shared" si="2"/>
-        <v>#define mEFCT_UNIQ_NOT_IMPL               68 // This feature is not yet implemented.</v>
-      </c>
-    </row>
-    <row r="48" spans="1:11" ht="20.25">
+        <v>#define mEFCT_UNIQ_CFG_ACCEPT             67 // Your choice has been saved into the running settings.</v>
+      </c>
+    </row>
+    <row r="48" spans="1:11" ht="30">
       <c r="A48" s="56" t="s">
         <v>583</v>
       </c>
       <c r="B48" s="55">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C48" s="50" t="s">
-        <v>4454</v>
+        <v>4453</v>
       </c>
       <c r="D48" s="56" t="s">
-        <v>641</v>
+        <v>725</v>
       </c>
       <c r="E48" s="56" t="s">
         <v>583</v>
@@ -77920,52 +77921,52 @@
         <v>579</v>
       </c>
       <c r="I48" s="22" t="s">
+        <v>613</v>
+      </c>
+      <c r="J48">
+        <f>LEN(I48)</f>
+        <v>19</v>
+      </c>
+      <c r="K48" s="65" t="str">
+        <f t="shared" si="2"/>
+        <v>#define mEFCT_UNIQ_NOT_IMPL               68 // This feature is not yet implemented.</v>
+      </c>
+    </row>
+    <row r="49" spans="1:12" ht="20.25">
+      <c r="A49" s="56" t="s">
+        <v>583</v>
+      </c>
+      <c r="B49" s="55">
+        <v>69</v>
+      </c>
+      <c r="C49" s="50" t="s">
+        <v>4454</v>
+      </c>
+      <c r="D49" s="56" t="s">
+        <v>641</v>
+      </c>
+      <c r="E49" s="56" t="s">
+        <v>583</v>
+      </c>
+      <c r="F49" s="53" t="s">
+        <v>471</v>
+      </c>
+      <c r="G49" s="57" t="s">
+        <v>578</v>
+      </c>
+      <c r="H49" s="55" t="s">
+        <v>579</v>
+      </c>
+      <c r="I49" s="22" t="s">
         <v>612</v>
       </c>
-      <c r="J48">
+      <c r="J49">
         <f t="shared" si="4"/>
         <v>18</v>
       </c>
-      <c r="K48" s="65" t="str">
+      <c r="K49" s="65" t="str">
         <f t="shared" si="2"/>
         <v>#define mEFCT_UNIQ_SILENCE                69 // silence</v>
-      </c>
-    </row>
-    <row r="49" spans="1:12" ht="30">
-      <c r="A49" s="56" t="s">
-        <v>583</v>
-      </c>
-      <c r="B49" s="55">
-        <v>71</v>
-      </c>
-      <c r="C49" s="50" t="s">
-        <v>679</v>
-      </c>
-      <c r="D49" s="10" t="s">
-        <v>719</v>
-      </c>
-      <c r="E49" s="56" t="s">
-        <v>583</v>
-      </c>
-      <c r="F49" s="53" t="s">
-        <v>471</v>
-      </c>
-      <c r="G49" s="57" t="s">
-        <v>578</v>
-      </c>
-      <c r="H49" s="55" t="s">
-        <v>579</v>
-      </c>
-      <c r="I49" s="22" t="s">
-        <v>674</v>
-      </c>
-      <c r="J49">
-        <f>LEN(I49)</f>
-        <v>29</v>
-      </c>
-      <c r="K49" s="65" t="str">
-        <f t="shared" si="2"/>
-        <v>#define mEFCT_UNIQ_CFG_WINDUP_DESCRIP     71 // The effect happens during wind-up to shooting.</v>
       </c>
     </row>
     <row r="50" spans="1:12" ht="30">
@@ -77973,13 +77974,13 @@
         <v>583</v>
       </c>
       <c r="B50" s="55">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C50" s="50" t="s">
-        <v>680</v>
+        <v>679</v>
       </c>
       <c r="D50" s="10" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="E50" s="56" t="s">
         <v>583</v>
@@ -77994,89 +77995,89 @@
         <v>579</v>
       </c>
       <c r="I50" s="22" t="s">
-        <v>673</v>
+        <v>674</v>
       </c>
       <c r="J50">
-        <f t="shared" ref="J50:J74" si="5">LEN(I50)</f>
-        <v>28</v>
+        <f>LEN(I50)</f>
+        <v>29</v>
       </c>
       <c r="K50" s="65" t="str">
         <f t="shared" si="2"/>
+        <v>#define mEFCT_UNIQ_CFG_WINDUP_DESCRIP     71 // The effect happens during wind-up to shooting.</v>
+      </c>
+    </row>
+    <row r="51" spans="1:12" ht="30">
+      <c r="A51" s="56" t="s">
+        <v>583</v>
+      </c>
+      <c r="B51" s="55">
+        <v>72</v>
+      </c>
+      <c r="C51" s="50" t="s">
+        <v>680</v>
+      </c>
+      <c r="D51" s="10" t="s">
+        <v>720</v>
+      </c>
+      <c r="E51" s="56" t="s">
+        <v>583</v>
+      </c>
+      <c r="F51" s="53" t="s">
+        <v>471</v>
+      </c>
+      <c r="G51" s="57" t="s">
+        <v>578</v>
+      </c>
+      <c r="H51" s="55" t="s">
+        <v>579</v>
+      </c>
+      <c r="I51" s="22" t="s">
+        <v>673</v>
+      </c>
+      <c r="J51">
+        <f t="shared" ref="J51:J75" si="5">LEN(I51)</f>
+        <v>28</v>
+      </c>
+      <c r="K51" s="65" t="str">
+        <f t="shared" si="2"/>
         <v>#define mEFCT_UNIQ_CFG_SHOOT_DESCRIP      72 // The effect happens during shooting itself.</v>
       </c>
     </row>
-    <row r="51" spans="1:12" ht="30">
-      <c r="A51" s="69" t="s">
+    <row r="52" spans="1:12" ht="30">
+      <c r="A52" s="69" t="s">
         <v>583</v>
       </c>
-      <c r="B51" s="70">
+      <c r="B52" s="70">
         <v>73</v>
       </c>
-      <c r="C51" s="71" t="s">
+      <c r="C52" s="71" t="s">
         <v>681</v>
       </c>
-      <c r="D51" s="10" t="s">
+      <c r="D52" s="10" t="s">
         <v>721</v>
       </c>
-      <c r="E51" s="69" t="s">
+      <c r="E52" s="69" t="s">
         <v>583</v>
       </c>
-      <c r="F51" s="72" t="s">
+      <c r="F52" s="72" t="s">
         <v>471</v>
       </c>
-      <c r="G51" s="73" t="s">
+      <c r="G52" s="73" t="s">
         <v>578</v>
       </c>
-      <c r="H51" s="70" t="s">
+      <c r="H52" s="70" t="s">
         <v>579</v>
       </c>
-      <c r="I51" s="22" t="s">
+      <c r="I52" s="22" t="s">
         <v>675</v>
       </c>
-      <c r="J51">
+      <c r="J52">
         <f t="shared" si="5"/>
         <v>27</v>
       </c>
-      <c r="K51" s="65" t="str">
+      <c r="K52" s="65" t="str">
         <f t="shared" si="2"/>
         <v>#define mEFCT_UNIQ_CFG_OPEN_DESCRIP       73 // The effect happens during opening of the barrel.</v>
-      </c>
-    </row>
-    <row r="52" spans="1:12" ht="30">
-      <c r="A52" s="56" t="s">
-        <v>583</v>
-      </c>
-      <c r="B52" s="55">
-        <v>74</v>
-      </c>
-      <c r="C52" s="50" t="s">
-        <v>682</v>
-      </c>
-      <c r="D52" s="52" t="s">
-        <v>722</v>
-      </c>
-      <c r="E52" s="56" t="s">
-        <v>583</v>
-      </c>
-      <c r="F52" s="53" t="s">
-        <v>471</v>
-      </c>
-      <c r="G52" s="57" t="s">
-        <v>578</v>
-      </c>
-      <c r="H52" s="55" t="s">
-        <v>579</v>
-      </c>
-      <c r="I52" s="22" t="s">
-        <v>676</v>
-      </c>
-      <c r="J52">
-        <f t="shared" si="5"/>
-        <v>28</v>
-      </c>
-      <c r="K52" s="65" t="str">
-        <f t="shared" si="2"/>
-        <v>#define mEFCT_UNIQ_CFG_LKLOD_DESCRIP      74 // The effect happens during lock-and-load of the barrel.</v>
       </c>
     </row>
     <row r="53" spans="1:12" ht="30">
@@ -78084,13 +78085,13 @@
         <v>583</v>
       </c>
       <c r="B53" s="55">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C53" s="50" t="s">
-        <v>683</v>
+        <v>682</v>
       </c>
       <c r="D53" s="52" t="s">
-        <v>723</v>
+        <v>722</v>
       </c>
       <c r="E53" s="56" t="s">
         <v>583</v>
@@ -78105,7 +78106,7 @@
         <v>579</v>
       </c>
       <c r="I53" s="22" t="s">
-        <v>677</v>
+        <v>676</v>
       </c>
       <c r="J53">
         <f t="shared" si="5"/>
@@ -78113,7 +78114,7 @@
       </c>
       <c r="K53" s="65" t="str">
         <f t="shared" si="2"/>
-        <v>#define mEFCT_UNIQ_CFG_PWRON_DESCRIP      75 // The effect happens during initial power-on.</v>
+        <v>#define mEFCT_UNIQ_CFG_LKLOD_DESCRIP      74 // The effect happens during lock-and-load of the barrel.</v>
       </c>
     </row>
     <row r="54" spans="1:12" ht="30">
@@ -78121,13 +78122,13 @@
         <v>583</v>
       </c>
       <c r="B54" s="55">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C54" s="50" t="s">
-        <v>684</v>
+        <v>683</v>
       </c>
       <c r="D54" s="52" t="s">
-        <v>724</v>
+        <v>723</v>
       </c>
       <c r="E54" s="56" t="s">
         <v>583</v>
@@ -78142,29 +78143,29 @@
         <v>579</v>
       </c>
       <c r="I54" s="22" t="s">
-        <v>678</v>
+        <v>677</v>
       </c>
       <c r="J54">
         <f t="shared" si="5"/>
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="K54" s="65" t="str">
         <f t="shared" si="2"/>
-        <v>#define mEFCT_UNIQ_CFG_WAIT_DESCRIP       76 // The effect happens when waiting to shoot.</v>
-      </c>
-    </row>
-    <row r="55" spans="1:12" ht="20.25">
+        <v>#define mEFCT_UNIQ_CFG_PWRON_DESCRIP      75 // The effect happens during initial power-on.</v>
+      </c>
+    </row>
+    <row r="55" spans="1:12" ht="30">
       <c r="A55" s="56" t="s">
         <v>583</v>
       </c>
       <c r="B55" s="55">
-        <v>81</v>
-      </c>
-      <c r="C55" s="75" t="s">
-        <v>689</v>
+        <v>76</v>
+      </c>
+      <c r="C55" s="50" t="s">
+        <v>684</v>
       </c>
       <c r="D55" s="52" t="s">
-        <v>4475</v>
+        <v>724</v>
       </c>
       <c r="E55" s="56" t="s">
         <v>583</v>
@@ -78179,29 +78180,29 @@
         <v>579</v>
       </c>
       <c r="I55" s="22" t="s">
-        <v>687</v>
+        <v>678</v>
       </c>
       <c r="J55">
         <f t="shared" si="5"/>
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="K55" s="65" t="str">
         <f t="shared" si="2"/>
-        <v>#define mEFCT_UNIQ_CFG_SOUNDS_DESCRIP     81 // The category is SOUNDS.</v>
-      </c>
-    </row>
-    <row r="56" spans="1:12" ht="30">
+        <v>#define mEFCT_UNIQ_CFG_WAIT_DESCRIP       76 // The effect happens when waiting to shoot.</v>
+      </c>
+    </row>
+    <row r="56" spans="1:12" ht="20.25">
       <c r="A56" s="56" t="s">
         <v>583</v>
       </c>
       <c r="B56" s="55">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C56" s="75" t="s">
-        <v>690</v>
+        <v>689</v>
       </c>
       <c r="D56" s="52" t="s">
-        <v>4476</v>
+        <v>4475</v>
       </c>
       <c r="E56" s="56" t="s">
         <v>583</v>
@@ -78216,15 +78217,15 @@
         <v>579</v>
       </c>
       <c r="I56" s="22" t="s">
-        <v>688</v>
+        <v>687</v>
       </c>
       <c r="J56">
         <f t="shared" si="5"/>
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="K56" s="65" t="str">
         <f t="shared" si="2"/>
-        <v>#define mEFCT_UNIQ_CFG_LEDPTRN_DESCRIP    82 // The category is L. E. D. PATTERNS.</v>
+        <v>#define mEFCT_UNIQ_CFG_SOUNDS_DESCRIP     81 // The category is SOUNDS.</v>
       </c>
     </row>
     <row r="57" spans="1:12" ht="30">
@@ -78232,13 +78233,13 @@
         <v>583</v>
       </c>
       <c r="B57" s="55">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C57" s="75" t="s">
-        <v>4479</v>
+        <v>690</v>
       </c>
       <c r="D57" s="52" t="s">
-        <v>4477</v>
+        <v>4476</v>
       </c>
       <c r="E57" s="56" t="s">
         <v>583</v>
@@ -78253,15 +78254,15 @@
         <v>579</v>
       </c>
       <c r="I57" s="22" t="s">
-        <v>4473</v>
+        <v>688</v>
       </c>
       <c r="J57">
-        <f t="shared" ref="J57:J58" si="6">LEN(I57)</f>
+        <f t="shared" si="5"/>
         <v>30</v>
       </c>
       <c r="K57" s="65" t="str">
-        <f t="shared" ref="K57:K58" si="7">"#define "&amp;I57&amp;" "&amp;REPT(" ",$J$40-J57)&amp;RIGHT(TEXT(B57,"    #"),3)&amp;" // "&amp;RIGHT(LEFT(D57,LEN(D57)-1),LEN(D57)-1-FIND("""",D57))</f>
-        <v>#define mEFCT_UNIQ_CFG_CPY_RST_DESCRIP    83 // The category is configuration resets and copying.</v>
+        <f t="shared" si="2"/>
+        <v>#define mEFCT_UNIQ_CFG_LEDPTRN_DESCRIP    82 // The category is L. E. D. PATTERNS.</v>
       </c>
     </row>
     <row r="58" spans="1:12" ht="30">
@@ -78269,13 +78270,13 @@
         <v>583</v>
       </c>
       <c r="B58" s="55">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C58" s="75" t="s">
-        <v>4480</v>
+        <v>4479</v>
       </c>
       <c r="D58" s="52" t="s">
-        <v>4478</v>
+        <v>4477</v>
       </c>
       <c r="E58" s="56" t="s">
         <v>583</v>
@@ -78290,15 +78291,15 @@
         <v>579</v>
       </c>
       <c r="I58" s="22" t="s">
-        <v>4474</v>
+        <v>4473</v>
       </c>
       <c r="J58">
-        <f t="shared" si="6"/>
-        <v>31</v>
+        <f t="shared" ref="J58:J59" si="6">LEN(I58)</f>
+        <v>30</v>
       </c>
       <c r="K58" s="65" t="str">
-        <f t="shared" si="7"/>
-        <v>#define mEFCT_UNIQ_CFG_ADVANCED_DESCRIP   84 // The category is advanced settings.</v>
+        <f t="shared" ref="K58:K59" si="7">"#define "&amp;I58&amp;" "&amp;REPT(" ",$J$40-J58)&amp;RIGHT(TEXT(B58,"    #"),3)&amp;" // "&amp;RIGHT(LEFT(D58,LEN(D58)-1),LEN(D58)-1-FIND("""",D58))</f>
+        <v>#define mEFCT_UNIQ_CFG_CPY_RST_DESCRIP    83 // The category is configuration resets and copying.</v>
       </c>
     </row>
     <row r="59" spans="1:12" ht="30">
@@ -78306,13 +78307,13 @@
         <v>583</v>
       </c>
       <c r="B59" s="55">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="C59" s="75" t="s">
-        <v>5527</v>
+        <v>4480</v>
       </c>
       <c r="D59" s="52" t="s">
-        <v>4466</v>
+        <v>4478</v>
       </c>
       <c r="E59" s="56" t="s">
         <v>583</v>
@@ -78326,32 +78327,30 @@
       <c r="H59" s="55" t="s">
         <v>579</v>
       </c>
-      <c r="I59" s="22" t="str">
-        <f>SUBSTITUTE("mEFCT_UNIQ_CFG_"&amp;UPPER(MID(C59,FIND("cfg",C59)+4,999)),".WAV","")</f>
-        <v>mEFCT_UNIQ_CFG_ENTER_PASSWORD</v>
+      <c r="I59" s="22" t="s">
+        <v>4474</v>
       </c>
       <c r="J59">
-        <f>LEN(I59)</f>
-        <v>29</v>
+        <f t="shared" si="6"/>
+        <v>31</v>
       </c>
       <c r="K59" s="65" t="str">
-        <f>"#define "&amp;I59&amp;" "&amp;REPT(" ",$J$40-J59)&amp;RIGHT(TEXT(B59,"    #"),3)&amp;" // "&amp;RIGHT(LEFT(D59,LEN(D59)-1),LEN(D59)-1-FIND("""",D59))</f>
-        <v>#define mEFCT_UNIQ_CFG_ENTER_PASSWORD     86 // Please state password loudly, then press trigger.</v>
-      </c>
-      <c r="L59" s="65"/>
-    </row>
-    <row r="60" spans="1:12" ht="45">
+        <f t="shared" si="7"/>
+        <v>#define mEFCT_UNIQ_CFG_ADVANCED_DESCRIP   84 // The category is advanced settings.</v>
+      </c>
+    </row>
+    <row r="60" spans="1:12" ht="30">
       <c r="A60" s="56" t="s">
         <v>583</v>
       </c>
       <c r="B60" s="55">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C60" s="75" t="s">
-        <v>5528</v>
+        <v>5527</v>
       </c>
       <c r="D60" s="52" t="s">
-        <v>4467</v>
+        <v>4466</v>
       </c>
       <c r="E60" s="56" t="s">
         <v>583</v>
@@ -78367,15 +78366,15 @@
       </c>
       <c r="I60" s="22" t="str">
         <f>SUBSTITUTE("mEFCT_UNIQ_CFG_"&amp;UPPER(MID(C60,FIND("cfg",C60)+4,999)),".WAV","")</f>
-        <v>mEFCT_UNIQ_CFG_ENTER_DANCE</v>
+        <v>mEFCT_UNIQ_CFG_ENTER_PASSWORD</v>
       </c>
       <c r="J60">
-        <f t="shared" ref="J60:J61" si="8">LEN(I60)</f>
-        <v>26</v>
+        <f>LEN(I60)</f>
+        <v>29</v>
       </c>
       <c r="K60" s="65" t="str">
-        <f t="shared" ref="K60:K61" si="9">"#define "&amp;I60&amp;" "&amp;REPT(" ",$J$40-J60)&amp;RIGHT(TEXT(B60,"    #"),3)&amp;" // "&amp;RIGHT(LEFT(D60,LEN(D60)-1),LEN(D60)-1-FIND("""",D60))</f>
-        <v>#define mEFCT_UNIQ_CFG_ENTER_DANCE        87 // I could not understand your password, please enter password by interpretive dance, then press trigger.</v>
+        <f>"#define "&amp;I60&amp;" "&amp;REPT(" ",$J$40-J60)&amp;RIGHT(TEXT(B60,"    #"),3)&amp;" // "&amp;RIGHT(LEFT(D60,LEN(D60)-1),LEN(D60)-1-FIND("""",D60))</f>
+        <v>#define mEFCT_UNIQ_CFG_ENTER_PASSWORD     86 // Please state password loudly, then press trigger.</v>
       </c>
       <c r="L60" s="65"/>
     </row>
@@ -78384,13 +78383,13 @@
         <v>583</v>
       </c>
       <c r="B61" s="55">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C61" s="75" t="s">
-        <v>5529</v>
+        <v>5528</v>
       </c>
       <c r="D61" s="52" t="s">
-        <v>4468</v>
+        <v>4467</v>
       </c>
       <c r="E61" s="56" t="s">
         <v>583</v>
@@ -78406,66 +78405,68 @@
       </c>
       <c r="I61" s="22" t="str">
         <f>SUBSTITUTE("mEFCT_UNIQ_CFG_"&amp;UPPER(MID(C61,FIND("cfg",C61)+4,999)),".WAV","")</f>
+        <v>mEFCT_UNIQ_CFG_ENTER_DANCE</v>
+      </c>
+      <c r="J61">
+        <f t="shared" ref="J61:J62" si="8">LEN(I61)</f>
+        <v>26</v>
+      </c>
+      <c r="K61" s="65" t="str">
+        <f t="shared" ref="K61:K62" si="9">"#define "&amp;I61&amp;" "&amp;REPT(" ",$J$40-J61)&amp;RIGHT(TEXT(B61,"    #"),3)&amp;" // "&amp;RIGHT(LEFT(D61,LEN(D61)-1),LEN(D61)-1-FIND("""",D61))</f>
+        <v>#define mEFCT_UNIQ_CFG_ENTER_DANCE        87 // I could not understand your password, please enter password by interpretive dance, then press trigger.</v>
+      </c>
+      <c r="L61" s="65"/>
+    </row>
+    <row r="62" spans="1:12" ht="45">
+      <c r="A62" s="56" t="s">
+        <v>583</v>
+      </c>
+      <c r="B62" s="55">
+        <v>88</v>
+      </c>
+      <c r="C62" s="75" t="s">
+        <v>5529</v>
+      </c>
+      <c r="D62" s="52" t="s">
+        <v>4468</v>
+      </c>
+      <c r="E62" s="56" t="s">
+        <v>583</v>
+      </c>
+      <c r="F62" s="53" t="s">
+        <v>471</v>
+      </c>
+      <c r="G62" s="57" t="s">
+        <v>578</v>
+      </c>
+      <c r="H62" s="55" t="s">
+        <v>579</v>
+      </c>
+      <c r="I62" s="22" t="str">
+        <f>SUBSTITUTE("mEFCT_UNIQ_CFG_"&amp;UPPER(MID(C62,FIND("cfg",C62)+4,999)),".WAV","")</f>
         <v>mEFCT_UNIQ_CFG_SORRY_NO_PASSWORD</v>
       </c>
-      <c r="J61">
+      <c r="J62">
         <f t="shared" si="8"/>
         <v>32</v>
       </c>
-      <c r="K61" s="65" t="str">
+      <c r="K62" s="65" t="str">
         <f t="shared" si="9"/>
         <v>#define mEFCT_UNIQ_CFG_SORRY_NO_PASSWORD  88 // Sorry, I don't have a password, but you dance very well. Please press trigger.</v>
       </c>
     </row>
-    <row r="62" spans="1:12" ht="285">
-      <c r="A62" s="56" t="s">
-        <v>583</v>
-      </c>
-      <c r="B62" s="55">
-        <v>89</v>
-      </c>
-      <c r="C62" s="75" t="s">
-        <v>4472</v>
-      </c>
-      <c r="D62" s="52" t="s">
-        <v>6037</v>
-      </c>
-      <c r="E62" s="56" t="s">
-        <v>583</v>
-      </c>
-      <c r="F62" s="53" t="s">
-        <v>471</v>
-      </c>
-      <c r="G62" s="57" t="s">
-        <v>578</v>
-      </c>
-      <c r="H62" s="55" t="s">
-        <v>579</v>
-      </c>
-      <c r="I62" s="22" t="s">
-        <v>4471</v>
-      </c>
-      <c r="J62">
-        <f t="shared" ref="J62" si="10">LEN(I62)</f>
-        <v>22</v>
-      </c>
-      <c r="K62" s="65" t="str">
-        <f t="shared" ref="K62:K74" si="11">"#define "&amp;I62&amp;" "&amp;REPT(" ",$J$40-J62)&amp;RIGHT(TEXT(B62,"    #"),3)&amp;" // "&amp;RIGHT(LEFT(D62,LEN(D62)-1),LEN(D62)-1-FIND("""",D62))</f>
-        <v>#define mEFCT_UNIQ_CFG_CREDITS            89 // The FOOF Science Fiction Rubber Band Gun was originally conceived by Mark and Keith. The hardware implementation was designed and built by Jim. The software and most of the sounds were generated by Mark. Some build information is at Git Hub dot Com slash Mark Dash Em Dee Oh Forty Seven dot Com slash Rubber Band Gun. Some sounds are recordings of Mark's family. Many of the Sci Fi sounds are transmogrified versions of Creative Commons sounds stored on Free Sound dot Org. Other Sci Fi sounds originated from El Eye Gee Oh gravity wave detections of stellar events found at Gee Double You Dash Open Science dot Org slash Audio Gee Double You Tee See One. The robotic voice sounds were generated using the eSpeak text to speech program found on eSpeak dot Source Forge dot net. See the Git Hub page for more attributions.</v>
-      </c>
-    </row>
-    <row r="63" spans="1:12" ht="45">
+    <row r="63" spans="1:12" ht="285">
       <c r="A63" s="56" t="s">
         <v>583</v>
       </c>
       <c r="B63" s="55">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="C63" s="75" t="s">
-        <v>4455</v>
+        <v>4472</v>
       </c>
       <c r="D63" s="52" t="s">
-        <v>5544</v>
+        <v>6037</v>
       </c>
       <c r="E63" s="56" t="s">
         <v>583</v>
@@ -78479,17 +78480,16 @@
       <c r="H63" s="55" t="s">
         <v>579</v>
       </c>
-      <c r="I63" s="22" t="str">
-        <f>SUBSTITUTE("mEFCT_UNIQ_CFG_"&amp;UPPER(MID(C63,FIND("cfg",C63)+4,999)),".WAV","")</f>
-        <v>mEFCT_UNIQ_CFG_MGMT_01</v>
+      <c r="I63" s="22" t="s">
+        <v>4471</v>
       </c>
       <c r="J63">
-        <f t="shared" si="5"/>
+        <f t="shared" ref="J63" si="10">LEN(I63)</f>
         <v>22</v>
       </c>
       <c r="K63" s="65" t="str">
-        <f t="shared" si="11"/>
-        <v>#define mEFCT_UNIQ_CFG_MGMT_01            91 // Erase the running setting only and reset the running setting to the factory settings.</v>
+        <f t="shared" ref="K63:K75" si="11">"#define "&amp;I63&amp;" "&amp;REPT(" ",$J$40-J63)&amp;RIGHT(TEXT(B63,"    #"),3)&amp;" // "&amp;RIGHT(LEFT(D63,LEN(D63)-1),LEN(D63)-1-FIND("""",D63))</f>
+        <v>#define mEFCT_UNIQ_CFG_CREDITS            89 // The FOOF Science Fiction Rubber Band Gun was originally conceived by Mark and Keith. The hardware implementation was designed and built by Jim. The software and most of the sounds were generated by Mark. Some build information is at Git Hub dot Com slash Mark Dash Em Dee Oh Forty Seven dot Com slash Rubber Band Gun. Some sounds are recordings of Mark's family. Many of the Sci Fi sounds are transmogrified versions of Creative Commons sounds stored on Free Sound dot Org. Other Sci Fi sounds originated from El Eye Gee Oh gravity wave detections of stellar events found at Gee Double You Dash Open Science dot Org slash Audio Gee Double You Tee See One. The robotic voice sounds were generated using the eSpeak text to speech program found on eSpeak dot Source Forge dot net. See the Git Hub page for more attributions.</v>
       </c>
     </row>
     <row r="64" spans="1:12" ht="45">
@@ -78497,13 +78497,13 @@
         <v>583</v>
       </c>
       <c r="B64" s="55">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C64" s="75" t="s">
-        <v>4456</v>
+        <v>4455</v>
       </c>
       <c r="D64" s="52" t="s">
-        <v>5545</v>
+        <v>5544</v>
       </c>
       <c r="E64" s="56" t="s">
         <v>583</v>
@@ -78518,8 +78518,8 @@
         <v>579</v>
       </c>
       <c r="I64" s="22" t="str">
-        <f t="shared" ref="I64:I74" si="12">SUBSTITUTE("mEFCT_UNIQ_CFG_"&amp;UPPER(MID(C64,FIND("cfg",C64)+4,999)),".WAV","")</f>
-        <v>mEFCT_UNIQ_CFG_MGMT_02</v>
+        <f>SUBSTITUTE("mEFCT_UNIQ_CFG_"&amp;UPPER(MID(C64,FIND("cfg",C64)+4,999)),".WAV","")</f>
+        <v>mEFCT_UNIQ_CFG_MGMT_01</v>
       </c>
       <c r="J64">
         <f t="shared" si="5"/>
@@ -78527,7 +78527,7 @@
       </c>
       <c r="K64" s="65" t="str">
         <f t="shared" si="11"/>
-        <v>#define mEFCT_UNIQ_CFG_MGMT_02            92 // Erase the running setting and erase all saved auxilliary settings and reset to the factory settings.</v>
+        <v>#define mEFCT_UNIQ_CFG_MGMT_01            91 // Erase the running setting only and reset the running setting to the factory settings.</v>
       </c>
     </row>
     <row r="65" spans="1:11" ht="45">
@@ -78535,13 +78535,13 @@
         <v>583</v>
       </c>
       <c r="B65" s="55">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C65" s="75" t="s">
-        <v>4457</v>
+        <v>4456</v>
       </c>
       <c r="D65" s="52" t="s">
-        <v>5546</v>
+        <v>5545</v>
       </c>
       <c r="E65" s="56" t="s">
         <v>583</v>
@@ -78556,8 +78556,8 @@
         <v>579</v>
       </c>
       <c r="I65" s="22" t="str">
-        <f t="shared" si="12"/>
-        <v>mEFCT_UNIQ_CFG_MGMT_03</v>
+        <f t="shared" ref="I65:I75" si="12">SUBSTITUTE("mEFCT_UNIQ_CFG_"&amp;UPPER(MID(C65,FIND("cfg",C65)+4,999)),".WAV","")</f>
+        <v>mEFCT_UNIQ_CFG_MGMT_02</v>
       </c>
       <c r="J65">
         <f t="shared" si="5"/>
@@ -78565,7 +78565,7 @@
       </c>
       <c r="K65" s="65" t="str">
         <f t="shared" si="11"/>
-        <v>#define mEFCT_UNIQ_CFG_MGMT_03            93 // Copy the running setting and overwrite into saved auxilliary setting number one.</v>
+        <v>#define mEFCT_UNIQ_CFG_MGMT_02            92 // Erase the running setting and erase all saved auxilliary settings and reset to the factory settings.</v>
       </c>
     </row>
     <row r="66" spans="1:11" ht="45">
@@ -78573,13 +78573,13 @@
         <v>583</v>
       </c>
       <c r="B66" s="55">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C66" s="75" t="s">
-        <v>4458</v>
+        <v>4457</v>
       </c>
       <c r="D66" s="52" t="s">
-        <v>5547</v>
+        <v>5546</v>
       </c>
       <c r="E66" s="56" t="s">
         <v>583</v>
@@ -78595,7 +78595,7 @@
       </c>
       <c r="I66" s="22" t="str">
         <f t="shared" si="12"/>
-        <v>mEFCT_UNIQ_CFG_MGMT_04</v>
+        <v>mEFCT_UNIQ_CFG_MGMT_03</v>
       </c>
       <c r="J66">
         <f t="shared" si="5"/>
@@ -78603,7 +78603,7 @@
       </c>
       <c r="K66" s="65" t="str">
         <f t="shared" si="11"/>
-        <v>#define mEFCT_UNIQ_CFG_MGMT_04            94 // Copy the running setting and overwrite into saved auxilliary setting number two.</v>
+        <v>#define mEFCT_UNIQ_CFG_MGMT_03            93 // Copy the running setting and overwrite into saved auxilliary setting number one.</v>
       </c>
     </row>
     <row r="67" spans="1:11" ht="45">
@@ -78611,13 +78611,13 @@
         <v>583</v>
       </c>
       <c r="B67" s="55">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C67" s="75" t="s">
-        <v>4459</v>
+        <v>4458</v>
       </c>
       <c r="D67" s="52" t="s">
-        <v>5548</v>
+        <v>5547</v>
       </c>
       <c r="E67" s="56" t="s">
         <v>583</v>
@@ -78633,7 +78633,7 @@
       </c>
       <c r="I67" s="22" t="str">
         <f t="shared" si="12"/>
-        <v>mEFCT_UNIQ_CFG_MGMT_05</v>
+        <v>mEFCT_UNIQ_CFG_MGMT_04</v>
       </c>
       <c r="J67">
         <f t="shared" si="5"/>
@@ -78641,7 +78641,7 @@
       </c>
       <c r="K67" s="65" t="str">
         <f t="shared" si="11"/>
-        <v>#define mEFCT_UNIQ_CFG_MGMT_05            95 // Copy the running setting and overwrite into saved auxilliary setting number three.</v>
+        <v>#define mEFCT_UNIQ_CFG_MGMT_04            94 // Copy the running setting and overwrite into saved auxilliary setting number two.</v>
       </c>
     </row>
     <row r="68" spans="1:11" ht="45">
@@ -78649,13 +78649,13 @@
         <v>583</v>
       </c>
       <c r="B68" s="55">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C68" s="75" t="s">
-        <v>4460</v>
+        <v>4459</v>
       </c>
       <c r="D68" s="52" t="s">
-        <v>5549</v>
+        <v>5548</v>
       </c>
       <c r="E68" s="56" t="s">
         <v>583</v>
@@ -78671,7 +78671,7 @@
       </c>
       <c r="I68" s="22" t="str">
         <f t="shared" si="12"/>
-        <v>mEFCT_UNIQ_CFG_MGMT_06</v>
+        <v>mEFCT_UNIQ_CFG_MGMT_05</v>
       </c>
       <c r="J68">
         <f t="shared" si="5"/>
@@ -78679,7 +78679,7 @@
       </c>
       <c r="K68" s="65" t="str">
         <f t="shared" si="11"/>
-        <v>#define mEFCT_UNIQ_CFG_MGMT_06            96 // Copy the saved auxilliary setting number one and overwrite into the running setting.</v>
+        <v>#define mEFCT_UNIQ_CFG_MGMT_05            95 // Copy the running setting and overwrite into saved auxilliary setting number three.</v>
       </c>
     </row>
     <row r="69" spans="1:11" ht="45">
@@ -78687,13 +78687,13 @@
         <v>583</v>
       </c>
       <c r="B69" s="55">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C69" s="75" t="s">
-        <v>4461</v>
+        <v>4460</v>
       </c>
       <c r="D69" s="52" t="s">
-        <v>5550</v>
+        <v>5549</v>
       </c>
       <c r="E69" s="56" t="s">
         <v>583</v>
@@ -78709,7 +78709,7 @@
       </c>
       <c r="I69" s="22" t="str">
         <f t="shared" si="12"/>
-        <v>mEFCT_UNIQ_CFG_MGMT_07</v>
+        <v>mEFCT_UNIQ_CFG_MGMT_06</v>
       </c>
       <c r="J69">
         <f t="shared" si="5"/>
@@ -78717,7 +78717,7 @@
       </c>
       <c r="K69" s="65" t="str">
         <f t="shared" si="11"/>
-        <v>#define mEFCT_UNIQ_CFG_MGMT_07            97 // Copy the saved auxilliary setting number two and overwrite into the running setting.</v>
+        <v>#define mEFCT_UNIQ_CFG_MGMT_06            96 // Copy the saved auxilliary setting number one and overwrite into the running setting.</v>
       </c>
     </row>
     <row r="70" spans="1:11" ht="45">
@@ -78725,13 +78725,13 @@
         <v>583</v>
       </c>
       <c r="B70" s="55">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C70" s="75" t="s">
-        <v>4462</v>
+        <v>4461</v>
       </c>
       <c r="D70" s="52" t="s">
-        <v>5551</v>
+        <v>5550</v>
       </c>
       <c r="E70" s="56" t="s">
         <v>583</v>
@@ -78747,7 +78747,7 @@
       </c>
       <c r="I70" s="22" t="str">
         <f t="shared" si="12"/>
-        <v>mEFCT_UNIQ_CFG_MGMT_08</v>
+        <v>mEFCT_UNIQ_CFG_MGMT_07</v>
       </c>
       <c r="J70">
         <f t="shared" si="5"/>
@@ -78755,21 +78755,21 @@
       </c>
       <c r="K70" s="65" t="str">
         <f t="shared" si="11"/>
-        <v>#define mEFCT_UNIQ_CFG_MGMT_08            98 // Copy the saved auxilliary setting number three and overwrite into the running setting.</v>
-      </c>
-    </row>
-    <row r="71" spans="1:11" ht="120">
+        <v>#define mEFCT_UNIQ_CFG_MGMT_07            97 // Copy the saved auxilliary setting number two and overwrite into the running setting.</v>
+      </c>
+    </row>
+    <row r="71" spans="1:11" ht="45">
       <c r="A71" s="56" t="s">
         <v>583</v>
       </c>
       <c r="B71" s="55">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="C71" s="75" t="s">
-        <v>4463</v>
+        <v>4462</v>
       </c>
       <c r="D71" s="52" t="s">
-        <v>6018</v>
+        <v>5551</v>
       </c>
       <c r="E71" s="56" t="s">
         <v>583</v>
@@ -78785,15 +78785,15 @@
       </c>
       <c r="I71" s="22" t="str">
         <f t="shared" si="12"/>
-        <v>mEFCT_UNIQ_CFG_ADVANCED_01</v>
+        <v>mEFCT_UNIQ_CFG_MGMT_08</v>
       </c>
       <c r="J71">
         <f t="shared" si="5"/>
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="K71" s="65" t="str">
         <f t="shared" si="11"/>
-        <v>#define mEFCT_UNIQ_CFG_ADVANCED_01       101 // Demo mode: Switch through the saved configurations each time you shoot. Power cycle to exit demo mode. As always, press trigger by itself to go forward to next step or to cycle through choices. To select a choice, first hold down any combination of Yellow or Green button then press trigger. To exit configuration, hold down Red button then press trigger.</v>
+        <v>#define mEFCT_UNIQ_CFG_MGMT_08            98 // Copy the saved auxilliary setting number three and overwrite into the running setting.</v>
       </c>
     </row>
     <row r="72" spans="1:11" ht="120">
@@ -78801,13 +78801,13 @@
         <v>583</v>
       </c>
       <c r="B72" s="55">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C72" s="75" t="s">
-        <v>4464</v>
+        <v>4463</v>
       </c>
       <c r="D72" s="52" t="s">
-        <v>4469</v>
+        <v>6018</v>
       </c>
       <c r="E72" s="56" t="s">
         <v>583</v>
@@ -78823,7 +78823,7 @@
       </c>
       <c r="I72" s="22" t="str">
         <f t="shared" si="12"/>
-        <v>mEFCT_UNIQ_CFG_ADVANCED_02</v>
+        <v>mEFCT_UNIQ_CFG_ADVANCED_01</v>
       </c>
       <c r="J72">
         <f t="shared" si="5"/>
@@ -78831,21 +78831,21 @@
       </c>
       <c r="K72" s="65" t="str">
         <f t="shared" si="11"/>
-        <v>#define mEFCT_UNIQ_CFG_ADVANCED_02       102 // Enable time travel and teleportation capabilities (requires password). As always, press trigger by itself to go forward to next step or to cycle through choices. To select a choice, first hold down any combination of Yellow or Green button then press trigger. To exit configuration, hold down Red button then press trigger.</v>
-      </c>
-    </row>
-    <row r="73" spans="1:11" ht="105">
+        <v>#define mEFCT_UNIQ_CFG_ADVANCED_01       101 // Demo mode: Switch through the saved configurations each time you shoot. Power cycle to exit demo mode. As always, press trigger by itself to go forward to next step or to cycle through choices. To select a choice, first hold down any combination of Yellow or Green button then press trigger. To exit configuration, hold down Red button then press trigger.</v>
+      </c>
+    </row>
+    <row r="73" spans="1:11" ht="120">
       <c r="A73" s="56" t="s">
         <v>583</v>
       </c>
       <c r="B73" s="55">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C73" s="75" t="s">
-        <v>4465</v>
+        <v>4464</v>
       </c>
       <c r="D73" s="52" t="s">
-        <v>4470</v>
+        <v>4469</v>
       </c>
       <c r="E73" s="56" t="s">
         <v>583</v>
@@ -78861,7 +78861,7 @@
       </c>
       <c r="I73" s="22" t="str">
         <f t="shared" si="12"/>
-        <v>mEFCT_UNIQ_CFG_ADVANCED_03</v>
+        <v>mEFCT_UNIQ_CFG_ADVANCED_02</v>
       </c>
       <c r="J73">
         <f t="shared" si="5"/>
@@ -78869,21 +78869,21 @@
       </c>
       <c r="K73" s="65" t="str">
         <f t="shared" si="11"/>
-        <v>#define mEFCT_UNIQ_CFG_ADVANCED_03       103 // Hear Rubber Band Gun credits. As always, press trigger by itself to go forward to next step or to cycle through choices. To select a choice, first hold down any combination of Yellow or Green button then press trigger. To exit configuration, hold down Red button then press trigger.</v>
-      </c>
-    </row>
-    <row r="74" spans="1:11" ht="135">
+        <v>#define mEFCT_UNIQ_CFG_ADVANCED_02       102 // Enable time travel and teleportation capabilities (requires password). As always, press trigger by itself to go forward to next step or to cycle through choices. To select a choice, first hold down any combination of Yellow or Green button then press trigger. To exit configuration, hold down Red button then press trigger.</v>
+      </c>
+    </row>
+    <row r="74" spans="1:11" ht="105">
       <c r="A74" s="56" t="s">
         <v>583</v>
       </c>
       <c r="B74" s="55">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="C74" s="75" t="s">
-        <v>6034</v>
+        <v>4465</v>
       </c>
       <c r="D74" s="52" t="s">
-        <v>6035</v>
+        <v>4470</v>
       </c>
       <c r="E74" s="56" t="s">
         <v>583</v>
@@ -78899,29 +78899,29 @@
       </c>
       <c r="I74" s="22" t="str">
         <f t="shared" si="12"/>
-        <v>mEFCT_UNIQ_CFG_ADVANCED</v>
+        <v>mEFCT_UNIQ_CFG_ADVANCED_03</v>
       </c>
       <c r="J74">
         <f t="shared" si="5"/>
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="K74" s="65" t="str">
         <f t="shared" si="11"/>
-        <v>#define mEFCT_UNIQ_CFG_ADVANCED          106 // Now choose which ADVANCED configuration category: Demo Mode, Time Travel and Teleportation, or Credits. As always, press trigger by itself to go forward to next step or to cycle through choices. To select a choice, first hold down any combination of Yellow or Green button then press trigger. To exit configuration, hold down Red button then press trigger.</v>
-      </c>
-    </row>
-    <row r="75" spans="1:11" ht="30">
+        <v>#define mEFCT_UNIQ_CFG_ADVANCED_03       103 // Hear Rubber Band Gun credits. As always, press trigger by itself to go forward to next step or to cycle through choices. To select a choice, first hold down any combination of Yellow or Green button then press trigger. To exit configuration, hold down Red button then press trigger.</v>
+      </c>
+    </row>
+    <row r="75" spans="1:11" ht="135">
       <c r="A75" s="56" t="s">
         <v>583</v>
       </c>
       <c r="B75" s="55">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C75" s="75" t="s">
-        <v>6024</v>
+        <v>6034</v>
       </c>
       <c r="D75" s="52" t="s">
-        <v>6025</v>
+        <v>6035</v>
       </c>
       <c r="E75" s="56" t="s">
         <v>583</v>
@@ -78936,30 +78936,30 @@
         <v>579</v>
       </c>
       <c r="I75" s="22" t="str">
-        <f t="shared" ref="I75" si="13">SUBSTITUTE("mEFCT_UNIQ_CFG_"&amp;UPPER(MID(C75,FIND("cfg",C75)+4,999)),".WAV","")</f>
-        <v>mEFCT_UNIQ_CFG_DEMO_STARTED</v>
+        <f t="shared" si="12"/>
+        <v>mEFCT_UNIQ_CFG_ADVANCED</v>
       </c>
       <c r="J75">
-        <f t="shared" ref="J75" si="14">LEN(I75)</f>
-        <v>27</v>
+        <f t="shared" si="5"/>
+        <v>23</v>
       </c>
       <c r="K75" s="65" t="str">
-        <f t="shared" ref="K75" si="15">"#define "&amp;I75&amp;" "&amp;REPT(" ",$J$40-J75)&amp;RIGHT(TEXT(B75,"    #"),3)&amp;" // "&amp;RIGHT(LEFT(D75,LEN(D75)-1),LEN(D75)-1-FIND("""",D75))</f>
-        <v>#define mEFCT_UNIQ_CFG_DEMO_STARTED      107 // Demo mode started. Power cycle to exit demo mode.</v>
-      </c>
-    </row>
-    <row r="76" spans="1:11" ht="135">
+        <f t="shared" si="11"/>
+        <v>#define mEFCT_UNIQ_CFG_ADVANCED          106 // Now choose which ADVANCED configuration category: Demo Mode, Time Travel and Teleportation, or Credits. As always, press trigger by itself to go forward to next step or to cycle through choices. To select a choice, first hold down any combination of Yellow or Green button then press trigger. To exit configuration, hold down Red button then press trigger.</v>
+      </c>
+    </row>
+    <row r="76" spans="1:11" ht="30">
       <c r="A76" s="56" t="s">
         <v>583</v>
       </c>
       <c r="B76" s="55">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C76" s="75" t="s">
-        <v>5541</v>
+        <v>6024</v>
       </c>
       <c r="D76" s="52" t="s">
-        <v>5538</v>
+        <v>6025</v>
       </c>
       <c r="E76" s="56" t="s">
         <v>583</v>
@@ -78973,172 +78973,186 @@
       <c r="H76" s="55" t="s">
         <v>579</v>
       </c>
-      <c r="I76" s="22" t="s">
+      <c r="I76" s="22" t="str">
+        <f t="shared" ref="I76" si="13">SUBSTITUTE("mEFCT_UNIQ_CFG_"&amp;UPPER(MID(C76,FIND("cfg",C76)+4,999)),".WAV","")</f>
+        <v>mEFCT_UNIQ_CFG_DEMO_STARTED</v>
+      </c>
+      <c r="J76">
+        <f t="shared" ref="J76" si="14">LEN(I76)</f>
+        <v>27</v>
+      </c>
+      <c r="K76" s="65" t="str">
+        <f t="shared" ref="K76" si="15">"#define "&amp;I76&amp;" "&amp;REPT(" ",$J$40-J76)&amp;RIGHT(TEXT(B76,"    #"),3)&amp;" // "&amp;RIGHT(LEFT(D76,LEN(D76)-1),LEN(D76)-1-FIND("""",D76))</f>
+        <v>#define mEFCT_UNIQ_CFG_DEMO_STARTED      107 // Demo mode started. Power cycle to exit demo mode.</v>
+      </c>
+    </row>
+    <row r="77" spans="1:11" ht="135">
+      <c r="A77" s="56" t="s">
+        <v>583</v>
+      </c>
+      <c r="B77" s="55">
+        <v>108</v>
+      </c>
+      <c r="C77" s="75" t="s">
+        <v>5541</v>
+      </c>
+      <c r="D77" s="52" t="s">
+        <v>5538</v>
+      </c>
+      <c r="E77" s="56" t="s">
+        <v>583</v>
+      </c>
+      <c r="F77" s="53" t="s">
+        <v>471</v>
+      </c>
+      <c r="G77" s="57" t="s">
+        <v>578</v>
+      </c>
+      <c r="H77" s="55" t="s">
+        <v>579</v>
+      </c>
+      <c r="I77" s="22" t="s">
         <v>5537</v>
       </c>
-      <c r="J76">
-        <f t="shared" ref="J76:J77" si="16">LEN(I76)</f>
+      <c r="J77">
+        <f t="shared" ref="J77:J78" si="16">LEN(I77)</f>
         <v>22</v>
       </c>
-      <c r="K76" s="65" t="str">
-        <f t="shared" ref="K76:K77" si="17">"#define "&amp;I76&amp;" "&amp;REPT(" ",$J$40-J76)&amp;RIGHT(TEXT(B76,"    #"),3)&amp;" // "&amp;RIGHT(LEFT(D76,LEN(D76)-1),LEN(D76)-1-FIND("""",D76))</f>
+      <c r="K77" s="65" t="str">
+        <f t="shared" ref="K77:K78" si="17">"#define "&amp;I77&amp;" "&amp;REPT(" ",$J$40-J77)&amp;RIGHT(TEXT(B77,"    #"),3)&amp;" // "&amp;RIGHT(LEFT(D77,LEN(D77)-1),LEN(D77)-1-FIND("""",D77))</f>
         <v>#define mEFCT_UNIQ_CFG_CPY_RST           108 // Now choose the, factory reset, or, configuration, copy, option. This list cycles through the options one by one. As always, press trigger by itself to go forward to next step or to cycle through choices. To select a choice, first hold down any combination of Yellow or Green button then press trigger. To exit configuration, hold down Red button then press trigger.</v>
       </c>
     </row>
-    <row r="77" spans="1:11" ht="45">
-      <c r="A77" s="69" t="s">
+    <row r="78" spans="1:11" ht="45">
+      <c r="A78" s="69" t="s">
         <v>583</v>
       </c>
-      <c r="B77" s="70">
+      <c r="B78" s="70">
         <v>109</v>
       </c>
-      <c r="C77" s="92" t="s">
+      <c r="C78" s="92" t="s">
         <v>5542</v>
       </c>
-      <c r="D77" s="93" t="s">
+      <c r="D78" s="93" t="s">
         <v>5539</v>
       </c>
-      <c r="E77" s="69" t="s">
+      <c r="E78" s="69" t="s">
         <v>583</v>
       </c>
-      <c r="F77" s="72" t="s">
+      <c r="F78" s="72" t="s">
         <v>471</v>
       </c>
-      <c r="G77" s="73" t="s">
+      <c r="G78" s="73" t="s">
         <v>578</v>
       </c>
-      <c r="H77" s="70" t="s">
+      <c r="H78" s="70" t="s">
         <v>579</v>
       </c>
-      <c r="I77" s="22" t="s">
+      <c r="I78" s="22" t="s">
         <v>5540</v>
       </c>
-      <c r="J77">
+      <c r="J78">
         <f t="shared" si="16"/>
         <v>29</v>
       </c>
-      <c r="K77" s="65" t="str">
+      <c r="K78" s="65" t="str">
         <f t="shared" si="17"/>
         <v>#define mEFCT_UNIQ_CFG_CPY_RST_ACCEPT    109 // Your, factory reset, or, configuration copy, option, has been accepted. Rebooting.</v>
       </c>
     </row>
-    <row r="78" spans="1:11">
-      <c r="A78" s="91" t="s">
+    <row r="79" spans="1:11">
+      <c r="A79" s="91" t="s">
         <v>694</v>
       </c>
-      <c r="B78" s="91" t="s">
+      <c r="B79" s="91" t="s">
         <v>694</v>
       </c>
-      <c r="C78" s="91" t="s">
+      <c r="C79" s="91" t="s">
         <v>694</v>
       </c>
-      <c r="D78" s="91" t="s">
+      <c r="D79" s="91" t="s">
         <v>694</v>
       </c>
-      <c r="E78" s="91" t="s">
+      <c r="E79" s="91" t="s">
         <v>694</v>
       </c>
-      <c r="F78" s="91" t="s">
+      <c r="F79" s="91" t="s">
         <v>694</v>
       </c>
-      <c r="G78" s="91" t="s">
+      <c r="G79" s="91" t="s">
         <v>694</v>
       </c>
-      <c r="H78" s="91" t="s">
+      <c r="H79" s="91" t="s">
         <v>694</v>
       </c>
-      <c r="I78" s="91" t="s">
+      <c r="I79" s="91" t="s">
         <v>694</v>
-      </c>
-    </row>
-    <row r="79" spans="1:11">
-      <c r="K79" t="s">
-        <v>562</v>
       </c>
     </row>
     <row r="80" spans="1:11">
       <c r="K80" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
     </row>
     <row r="81" spans="1:18">
       <c r="K81" t="s">
-        <v>564</v>
+        <v>563</v>
       </c>
     </row>
     <row r="82" spans="1:18">
       <c r="K82" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
     </row>
     <row r="83" spans="1:18">
       <c r="K83" t="s">
-        <v>566</v>
+        <v>565</v>
       </c>
     </row>
     <row r="84" spans="1:18">
       <c r="K84" t="s">
-        <v>567</v>
-      </c>
-      <c r="R84" t="s">
-        <v>545</v>
+        <v>566</v>
       </c>
     </row>
     <row r="85" spans="1:18">
       <c r="K85" t="s">
-        <v>568</v>
+        <v>567</v>
       </c>
       <c r="R85" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
     </row>
     <row r="86" spans="1:18">
       <c r="K86" t="s">
+        <v>568</v>
+      </c>
+      <c r="R86" t="s">
+        <v>546</v>
+      </c>
+    </row>
+    <row r="87" spans="1:18">
+      <c r="K87" t="s">
         <v>569</v>
       </c>
-      <c r="R86" t="s">
+      <c r="R87" t="s">
         <v>547</v>
       </c>
     </row>
-    <row r="89" spans="1:18" ht="20.25">
-      <c r="A89" s="6"/>
-      <c r="D89" s="41"/>
-      <c r="E89" s="6"/>
-      <c r="F89" s="31"/>
-      <c r="G89" s="31"/>
-      <c r="H89" s="6"/>
-    </row>
     <row r="90" spans="1:18" ht="20.25">
-      <c r="A90" s="40" t="s">
-        <v>457</v>
-      </c>
-      <c r="B90" s="17"/>
-      <c r="C90" s="30" t="s">
-        <v>484</v>
-      </c>
-      <c r="D90" s="29" t="s">
-        <v>559</v>
-      </c>
-      <c r="E90" s="29" t="s">
-        <v>457</v>
-      </c>
-      <c r="F90" s="30" t="s">
-        <v>483</v>
-      </c>
-      <c r="G90" s="30" t="s">
-        <v>486</v>
-      </c>
-      <c r="H90" s="37" t="s">
-        <v>485</v>
-      </c>
+      <c r="A90" s="6"/>
+      <c r="D90" s="41"/>
+      <c r="E90" s="6"/>
+      <c r="F90" s="31"/>
+      <c r="G90" s="31"/>
+      <c r="H90" s="6"/>
     </row>
     <row r="91" spans="1:18" ht="20.25">
       <c r="A91" s="40" t="s">
         <v>457</v>
       </c>
       <c r="B91" s="17"/>
-      <c r="C91" s="39" t="s">
-        <v>472</v>
+      <c r="C91" s="30" t="s">
+        <v>484</v>
       </c>
       <c r="D91" s="29" t="s">
         <v>559</v>
@@ -79147,73 +79161,90 @@
         <v>457</v>
       </c>
       <c r="F91" s="30" t="s">
+        <v>483</v>
+      </c>
+      <c r="G91" s="30" t="s">
+        <v>486</v>
+      </c>
+      <c r="H91" s="37" t="s">
+        <v>485</v>
+      </c>
+    </row>
+    <row r="92" spans="1:18" ht="20.25">
+      <c r="A92" s="40" t="s">
+        <v>457</v>
+      </c>
+      <c r="B92" s="17"/>
+      <c r="C92" s="39" t="s">
+        <v>472</v>
+      </c>
+      <c r="D92" s="29" t="s">
+        <v>559</v>
+      </c>
+      <c r="E92" s="29" t="s">
+        <v>457</v>
+      </c>
+      <c r="F92" s="30" t="s">
         <v>471</v>
       </c>
-      <c r="G91" s="30" t="s">
+      <c r="G92" s="30" t="s">
         <v>474</v>
       </c>
-      <c r="H91" s="37" t="s">
+      <c r="H92" s="37" t="s">
         <v>473</v>
       </c>
     </row>
-    <row r="92" spans="1:18" ht="30.75">
-      <c r="A92" s="17" t="s">
-        <v>455</v>
-      </c>
-      <c r="B92" s="17">
-        <v>57</v>
-      </c>
-      <c r="C92" s="28" t="s">
-        <v>492</v>
-      </c>
-      <c r="D92" s="38" t="s">
-        <v>571</v>
-      </c>
-      <c r="E92" s="17" t="s">
-        <v>455</v>
-      </c>
-      <c r="F92" s="30" t="s">
-        <v>463</v>
-      </c>
-      <c r="G92" s="30" t="s">
-        <v>532</v>
-      </c>
-      <c r="H92" s="17" t="s">
-        <v>543</v>
-      </c>
-    </row>
-    <row r="93" spans="1:18" ht="20.25">
+    <row r="93" spans="1:18" ht="30.75">
       <c r="A93" s="17" t="s">
         <v>455</v>
       </c>
-      <c r="B93" s="26">
-        <v>58</v>
+      <c r="B93" s="17">
+        <v>57</v>
       </c>
       <c r="C93" s="28" t="s">
-        <v>491</v>
+        <v>492</v>
       </c>
       <c r="D93" s="38" t="s">
-        <v>490</v>
+        <v>571</v>
       </c>
       <c r="E93" s="17" t="s">
         <v>455</v>
       </c>
       <c r="F93" s="30" t="s">
+        <v>463</v>
+      </c>
+      <c r="G93" s="30" t="s">
+        <v>532</v>
+      </c>
+      <c r="H93" s="17" t="s">
+        <v>543</v>
+      </c>
+    </row>
+    <row r="94" spans="1:18" ht="20.25">
+      <c r="A94" s="17" t="s">
+        <v>455</v>
+      </c>
+      <c r="B94" s="26">
+        <v>58</v>
+      </c>
+      <c r="C94" s="28" t="s">
+        <v>491</v>
+      </c>
+      <c r="D94" s="38" t="s">
+        <v>490</v>
+      </c>
+      <c r="E94" s="17" t="s">
+        <v>455</v>
+      </c>
+      <c r="F94" s="30" t="s">
         <v>483</v>
       </c>
-      <c r="G93" s="30" t="s">
+      <c r="G94" s="30" t="s">
         <v>531</v>
       </c>
-      <c r="H93" s="17" t="s">
+      <c r="H94" s="17" t="s">
         <v>542</v>
       </c>
-    </row>
-    <row r="94" spans="1:18" ht="20.25">
-      <c r="D94" s="41"/>
-      <c r="E94" s="6"/>
-      <c r="F94" s="31"/>
-      <c r="G94" s="31"/>
-      <c r="H94" s="6"/>
     </row>
     <row r="95" spans="1:18" ht="20.25">
       <c r="D95" s="41"/>
@@ -79230,9 +79261,6 @@
       <c r="H96" s="6"/>
     </row>
     <row r="97" spans="1:18" ht="20.25">
-      <c r="A97" s="6" t="s">
-        <v>584</v>
-      </c>
       <c r="D97" s="41"/>
       <c r="E97" s="6"/>
       <c r="F97" s="31"/>
@@ -79240,8 +79268,8 @@
       <c r="H97" s="6"/>
     </row>
     <row r="98" spans="1:18" ht="20.25">
-      <c r="A98" t="s">
-        <v>598</v>
+      <c r="A98" s="6" t="s">
+        <v>584</v>
       </c>
       <c r="D98" s="41"/>
       <c r="E98" s="6"/>
@@ -79251,7 +79279,7 @@
     </row>
     <row r="99" spans="1:18" ht="20.25">
       <c r="A99" t="s">
-        <v>599</v>
+        <v>598</v>
       </c>
       <c r="D99" s="41"/>
       <c r="E99" s="6"/>
@@ -79261,7 +79289,7 @@
     </row>
     <row r="100" spans="1:18" ht="20.25">
       <c r="A100" t="s">
-        <v>586</v>
+        <v>599</v>
       </c>
       <c r="D100" s="41"/>
       <c r="E100" s="6"/>
@@ -79270,859 +79298,869 @@
       <c r="H100" s="6"/>
     </row>
     <row r="101" spans="1:18" ht="20.25">
-      <c r="A101" s="6" t="str">
-        <f>"&lt;tr&gt;&lt;td&gt;&lt;b&gt;"&amp;J101&amp;"&lt;/b&gt;&lt;/td&gt;&lt;td&gt;&lt;b&gt;"&amp;K101&amp;"&lt;/b&gt;&lt;/td&gt;&lt;td&gt;&lt;b&gt;"&amp;L101&amp;"&lt;/b&gt;&lt;/td&gt;&lt;td&gt;&lt;b&gt;"&amp;M101&amp;"&lt;/b&gt;&lt;/td&gt;"</f>
-        <v>&lt;tr&gt;&lt;td&gt;&lt;b&gt;Tag&lt;/b&gt;&lt;/td&gt;&lt;td&gt;&lt;b&gt;File Name&lt;/b&gt;&lt;/td&gt;&lt;td&gt;&lt;b&gt;URL&lt;/b&gt;&lt;/td&gt;&lt;td&gt;&lt;b&gt;Who&lt;/b&gt;&lt;/td&gt;</v>
-      </c>
-      <c r="J101" s="22" t="s">
-        <v>459</v>
-      </c>
-      <c r="K101" s="22" t="s">
-        <v>460</v>
-      </c>
-      <c r="L101" s="22" t="s">
-        <v>461</v>
-      </c>
-      <c r="M101" s="22" t="s">
-        <v>462</v>
-      </c>
+      <c r="A101" t="s">
+        <v>586</v>
+      </c>
+      <c r="D101" s="41"/>
+      <c r="E101" s="6"/>
+      <c r="F101" s="31"/>
+      <c r="G101" s="31"/>
+      <c r="H101" s="6"/>
     </row>
     <row r="102" spans="1:18" ht="20.25">
       <c r="A102" s="6" t="str">
-        <f t="shared" ref="A102:A128" si="18">"&lt;tr&gt;&lt;td&gt;"&amp;J102&amp;"&lt;/td&gt;&lt;td&gt;"&amp;K102&amp;"&lt;/td&gt;&lt;td&gt;"&amp;L102&amp;"&lt;/td&gt;&lt;td&gt;"&amp;M102&amp;"&lt;/td&gt;"</f>
-        <v>&lt;tr&gt;&lt;td&gt;N/A&lt;/td&gt;&lt;td&gt;GW170817-template.wav&lt;/td&gt;&lt;td&gt;https://www.gw-openscience.org/audiogwtc1/&lt;/td&gt;&lt;td&gt;LIGO detectors&lt;/td&gt;</v>
+        <f>"&lt;tr&gt;&lt;td&gt;&lt;b&gt;"&amp;J102&amp;"&lt;/b&gt;&lt;/td&gt;&lt;td&gt;&lt;b&gt;"&amp;K102&amp;"&lt;/b&gt;&lt;/td&gt;&lt;td&gt;&lt;b&gt;"&amp;L102&amp;"&lt;/b&gt;&lt;/td&gt;&lt;td&gt;&lt;b&gt;"&amp;M102&amp;"&lt;/b&gt;&lt;/td&gt;"</f>
+        <v>&lt;tr&gt;&lt;td&gt;&lt;b&gt;Tag&lt;/b&gt;&lt;/td&gt;&lt;td&gt;&lt;b&gt;File Name&lt;/b&gt;&lt;/td&gt;&lt;td&gt;&lt;b&gt;URL&lt;/b&gt;&lt;/td&gt;&lt;td&gt;&lt;b&gt;Who&lt;/b&gt;&lt;/td&gt;</v>
       </c>
       <c r="J102" s="22" t="s">
-        <v>594</v>
+        <v>459</v>
       </c>
       <c r="K102" s="22" t="s">
-        <v>597</v>
-      </c>
-      <c r="L102" s="24" t="s">
-        <v>595</v>
+        <v>460</v>
+      </c>
+      <c r="L102" s="22" t="s">
+        <v>461</v>
       </c>
       <c r="M102" s="22" t="s">
-        <v>596</v>
+        <v>462</v>
       </c>
     </row>
     <row r="103" spans="1:18" ht="20.25">
       <c r="A103" s="6" t="str">
-        <f t="shared" si="18"/>
-        <v>&lt;tr&gt;&lt;td&gt;zero/1.0/&lt;/td&gt;&lt;td&gt;145209__lensflare8642__shotgun-sounds.mp3&lt;/td&gt;&lt;td&gt;https://freesound.org/s/145209/&lt;/td&gt;&lt;td&gt;lensflare8642&lt;/td&gt;</v>
-      </c>
-      <c r="J103" s="14" t="s">
-        <v>463</v>
+        <f t="shared" ref="A103:A129" si="18">"&lt;tr&gt;&lt;td&gt;"&amp;J103&amp;"&lt;/td&gt;&lt;td&gt;"&amp;K103&amp;"&lt;/td&gt;&lt;td&gt;"&amp;L103&amp;"&lt;/td&gt;&lt;td&gt;"&amp;M103&amp;"&lt;/td&gt;"</f>
+        <v>&lt;tr&gt;&lt;td&gt;N/A&lt;/td&gt;&lt;td&gt;GW170817-template.wav&lt;/td&gt;&lt;td&gt;https://www.gw-openscience.org/audiogwtc1/&lt;/td&gt;&lt;td&gt;LIGO detectors&lt;/td&gt;</v>
+      </c>
+      <c r="J103" s="22" t="s">
+        <v>594</v>
       </c>
       <c r="K103" s="22" t="s">
-        <v>468</v>
+        <v>597</v>
       </c>
       <c r="L103" s="24" t="s">
-        <v>469</v>
-      </c>
-      <c r="M103" s="23" t="s">
-        <v>470</v>
-      </c>
-      <c r="R103" t="str">
-        <f>"| "&amp;J103&amp;" | "&amp;K103&amp;" | "&amp;L103&amp;" | "&amp;M103&amp;" |"</f>
-        <v>| zero/1.0/ | 145209__lensflare8642__shotgun-sounds.mp3 | https://freesound.org/s/145209/ | lensflare8642 |</v>
+        <v>595</v>
+      </c>
+      <c r="M103" s="22" t="s">
+        <v>596</v>
       </c>
     </row>
     <row r="104" spans="1:18" ht="20.25">
       <c r="A104" s="6" t="str">
         <f t="shared" si="18"/>
-        <v>&lt;tr&gt;&lt;td&gt;zero/1.0/&lt;/td&gt;&lt;td&gt;162814__timgormly__spaceship-4.aiff&lt;/td&gt;&lt;td&gt;https://freesound.org/s/162814/&lt;/td&gt;&lt;td&gt;timgormly&lt;/td&gt;</v>
-      </c>
-      <c r="J104" s="36" t="s">
+        <v>&lt;tr&gt;&lt;td&gt;zero/1.0/&lt;/td&gt;&lt;td&gt;145209__lensflare8642__shotgun-sounds.mp3&lt;/td&gt;&lt;td&gt;https://freesound.org/s/145209/&lt;/td&gt;&lt;td&gt;lensflare8642&lt;/td&gt;</v>
+      </c>
+      <c r="J104" s="14" t="s">
         <v>463</v>
       </c>
-      <c r="K104" s="6" t="s">
-        <v>492</v>
-      </c>
-      <c r="L104" t="s">
-        <v>543</v>
+      <c r="K104" s="22" t="s">
+        <v>468</v>
+      </c>
+      <c r="L104" s="24" t="s">
+        <v>469</v>
       </c>
       <c r="M104" s="23" t="s">
-        <v>532</v>
+        <v>470</v>
       </c>
       <c r="R104" t="str">
         <f>"| "&amp;J104&amp;" | "&amp;K104&amp;" | "&amp;L104&amp;" | "&amp;M104&amp;" |"</f>
-        <v>| zero/1.0/ | 162814__timgormly__spaceship-4.aiff | https://freesound.org/s/162814/ | timgormly |</v>
+        <v>| zero/1.0/ | 145209__lensflare8642__shotgun-sounds.mp3 | https://freesound.org/s/145209/ | lensflare8642 |</v>
       </c>
     </row>
     <row r="105" spans="1:18" ht="20.25">
       <c r="A105" s="6" t="str">
         <f t="shared" si="18"/>
-        <v>&lt;tr&gt;&lt;td&gt;by-nc/3.0/&lt;/td&gt;&lt;td&gt;165483__timbre__glitch-voice-ep-mp3.mp3&lt;/td&gt;&lt;td&gt;https://freesound.org/s/165483/&lt;/td&gt;&lt;td&gt;timbre&lt;/td&gt;</v>
+        <v>&lt;tr&gt;&lt;td&gt;zero/1.0/&lt;/td&gt;&lt;td&gt;162814__timgormly__spaceship-4.aiff&lt;/td&gt;&lt;td&gt;https://freesound.org/s/162814/&lt;/td&gt;&lt;td&gt;timgormly&lt;/td&gt;</v>
       </c>
       <c r="J105" s="36" t="s">
-        <v>483</v>
+        <v>463</v>
       </c>
       <c r="K105" s="6" t="s">
-        <v>491</v>
+        <v>492</v>
       </c>
       <c r="L105" t="s">
-        <v>542</v>
+        <v>543</v>
       </c>
       <c r="M105" s="23" t="s">
-        <v>531</v>
+        <v>532</v>
       </c>
       <c r="R105" t="str">
         <f>"| "&amp;J105&amp;" | "&amp;K105&amp;" | "&amp;L105&amp;" | "&amp;M105&amp;" |"</f>
-        <v>| by-nc/3.0/ | 165483__timbre__glitch-voice-ep-mp3.mp3 | https://freesound.org/s/165483/ | timbre |</v>
+        <v>| zero/1.0/ | 162814__timgormly__spaceship-4.aiff | https://freesound.org/s/162814/ | timgormly |</v>
       </c>
     </row>
     <row r="106" spans="1:18" ht="20.25">
       <c r="A106" s="6" t="str">
         <f t="shared" si="18"/>
-        <v>&lt;tr&gt;&lt;td&gt;by/3.0/&lt;/td&gt;&lt;td&gt;169292__lazr2012__haywirefusionator.ogg&lt;/td&gt;&lt;td&gt;https://freesound.org/s/169292/&lt;/td&gt;&lt;td&gt;lazr2012&lt;/td&gt;</v>
+        <v>&lt;tr&gt;&lt;td&gt;by-nc/3.0/&lt;/td&gt;&lt;td&gt;165483__timbre__glitch-voice-ep-mp3.mp3&lt;/td&gt;&lt;td&gt;https://freesound.org/s/165483/&lt;/td&gt;&lt;td&gt;timbre&lt;/td&gt;</v>
       </c>
       <c r="J106" s="36" t="s">
-        <v>471</v>
+        <v>483</v>
       </c>
       <c r="K106" s="6" t="s">
-        <v>489</v>
+        <v>491</v>
       </c>
       <c r="L106" t="s">
-        <v>541</v>
+        <v>542</v>
       </c>
       <c r="M106" s="23" t="s">
-        <v>530</v>
+        <v>531</v>
       </c>
       <c r="R106" t="str">
         <f>"| "&amp;J106&amp;" | "&amp;K106&amp;" | "&amp;L106&amp;" | "&amp;M106&amp;" |"</f>
-        <v>| by/3.0/ | 169292__lazr2012__haywirefusionator.ogg | https://freesound.org/s/169292/ | lazr2012 |</v>
+        <v>| by-nc/3.0/ | 165483__timbre__glitch-voice-ep-mp3.mp3 | https://freesound.org/s/165483/ | timbre |</v>
       </c>
     </row>
     <row r="107" spans="1:18" ht="20.25">
       <c r="A107" s="6" t="str">
         <f t="shared" si="18"/>
-        <v>&lt;tr&gt;&lt;td&gt;zero/1.0/&lt;/td&gt;&lt;td&gt;170136__lazr2012__machinery-bo.flac&lt;/td&gt;&lt;td&gt;https://freesound.org/s/170136/&lt;/td&gt;&lt;td&gt;lazr2012&lt;/td&gt;</v>
+        <v>&lt;tr&gt;&lt;td&gt;by/3.0/&lt;/td&gt;&lt;td&gt;169292__lazr2012__haywirefusionator.ogg&lt;/td&gt;&lt;td&gt;https://freesound.org/s/169292/&lt;/td&gt;&lt;td&gt;lazr2012&lt;/td&gt;</v>
       </c>
       <c r="J107" s="36" t="s">
-        <v>463</v>
+        <v>471</v>
       </c>
       <c r="K107" s="6" t="s">
-        <v>487</v>
+        <v>489</v>
       </c>
       <c r="L107" t="s">
-        <v>540</v>
+        <v>541</v>
       </c>
       <c r="M107" s="23" t="s">
         <v>530</v>
       </c>
-      <c r="Q107" s="24"/>
       <c r="R107" t="str">
         <f>"| "&amp;J107&amp;" | "&amp;K107&amp;" | "&amp;L107&amp;" | "&amp;M107&amp;" |"</f>
-        <v>| zero/1.0/ | 170136__lazr2012__machinery-bo.flac | https://freesound.org/s/170136/ | lazr2012 |</v>
+        <v>| by/3.0/ | 169292__lazr2012__haywirefusionator.ogg | https://freesound.org/s/169292/ | lazr2012 |</v>
       </c>
     </row>
     <row r="108" spans="1:18" ht="20.25">
       <c r="A108" s="6" t="str">
         <f t="shared" si="18"/>
-        <v>&lt;tr&gt;&lt;td&gt;by-nc/3.0/&lt;/td&gt;&lt;td&gt;179281__timbre__boingy-sweep.flac&lt;/td&gt;&lt;td&gt;https://freesound.org/s/179281/&lt;/td&gt;&lt;td&gt;Timbre&lt;/td&gt;</v>
-      </c>
-      <c r="J108" s="14" t="s">
-        <v>483</v>
-      </c>
-      <c r="K108" s="4" t="s">
-        <v>484</v>
-      </c>
-      <c r="L108" s="24" t="s">
-        <v>485</v>
+        <v>&lt;tr&gt;&lt;td&gt;zero/1.0/&lt;/td&gt;&lt;td&gt;170136__lazr2012__machinery-bo.flac&lt;/td&gt;&lt;td&gt;https://freesound.org/s/170136/&lt;/td&gt;&lt;td&gt;lazr2012&lt;/td&gt;</v>
+      </c>
+      <c r="J108" s="36" t="s">
+        <v>463</v>
+      </c>
+      <c r="K108" s="6" t="s">
+        <v>487</v>
+      </c>
+      <c r="L108" t="s">
+        <v>540</v>
       </c>
       <c r="M108" s="23" t="s">
-        <v>486</v>
-      </c>
+        <v>530</v>
+      </c>
+      <c r="Q108" s="24"/>
       <c r="R108" t="str">
-        <f t="shared" ref="R108:R109" si="19">"| "&amp;J108&amp;" | "&amp;K108&amp;" | "&amp;L108&amp;" | "&amp;M108&amp;" |"</f>
-        <v>| by-nc/3.0/ | 179281__timbre__boingy-sweep.flac | https://freesound.org/s/179281/ | Timbre |</v>
+        <f>"| "&amp;J108&amp;" | "&amp;K108&amp;" | "&amp;L108&amp;" | "&amp;M108&amp;" |"</f>
+        <v>| zero/1.0/ | 170136__lazr2012__machinery-bo.flac | https://freesound.org/s/170136/ | lazr2012 |</v>
       </c>
     </row>
     <row r="109" spans="1:18" ht="20.25">
       <c r="A109" s="6" t="str">
         <f t="shared" si="18"/>
-        <v>&lt;tr&gt;&lt;td&gt;by/3.0/&lt;/td&gt;&lt;td&gt;216096__richerlandtv__u-f-o.mp3&lt;/td&gt;&lt;td&gt;https://freesound.org/s/216096/&lt;/td&gt;&lt;td&gt;RICHERlandTV&lt;/td&gt;</v>
+        <v>&lt;tr&gt;&lt;td&gt;by-nc/3.0/&lt;/td&gt;&lt;td&gt;179281__timbre__boingy-sweep.flac&lt;/td&gt;&lt;td&gt;https://freesound.org/s/179281/&lt;/td&gt;&lt;td&gt;Timbre&lt;/td&gt;</v>
       </c>
       <c r="J109" s="14" t="s">
-        <v>471</v>
+        <v>483</v>
       </c>
       <c r="K109" s="4" t="s">
-        <v>472</v>
+        <v>484</v>
       </c>
       <c r="L109" s="24" t="s">
-        <v>473</v>
+        <v>485</v>
       </c>
       <c r="M109" s="23" t="s">
-        <v>474</v>
+        <v>486</v>
       </c>
       <c r="R109" t="str">
-        <f t="shared" si="19"/>
-        <v>| by/3.0/ | 216096__richerlandtv__u-f-o.mp3 | https://freesound.org/s/216096/ | RICHERlandTV |</v>
+        <f t="shared" ref="R109:R110" si="19">"| "&amp;J109&amp;" | "&amp;K109&amp;" | "&amp;L109&amp;" | "&amp;M109&amp;" |"</f>
+        <v>| by-nc/3.0/ | 179281__timbre__boingy-sweep.flac | https://freesound.org/s/179281/ | Timbre |</v>
       </c>
     </row>
     <row r="110" spans="1:18" ht="20.25">
       <c r="A110" s="6" t="str">
         <f t="shared" si="18"/>
-        <v>&lt;tr&gt;&lt;td&gt;by/3.0/&lt;/td&gt;&lt;td&gt;221875__hero-of-the-winds__spring-boing.wav&lt;/td&gt;&lt;td&gt;https://freesound.org/s/221875/&lt;/td&gt;&lt;td&gt;hero-of-the-winds&lt;/td&gt;</v>
-      </c>
-      <c r="J110" s="36" t="s">
+        <v>&lt;tr&gt;&lt;td&gt;by/3.0/&lt;/td&gt;&lt;td&gt;216096__richerlandtv__u-f-o.mp3&lt;/td&gt;&lt;td&gt;https://freesound.org/s/216096/&lt;/td&gt;&lt;td&gt;RICHERlandTV&lt;/td&gt;</v>
+      </c>
+      <c r="J110" s="14" t="s">
         <v>471</v>
       </c>
-      <c r="K110" s="6" t="s">
-        <v>458</v>
-      </c>
-      <c r="L110" t="s">
-        <v>537</v>
+      <c r="K110" s="4" t="s">
+        <v>472</v>
+      </c>
+      <c r="L110" s="24" t="s">
+        <v>473</v>
       </c>
       <c r="M110" s="23" t="s">
-        <v>523</v>
+        <v>474</v>
       </c>
       <c r="R110" t="str">
-        <f t="shared" ref="R110:R128" si="20">"| "&amp;J110&amp;" | "&amp;K110&amp;" | "&amp;L110&amp;" | "&amp;M110&amp;" |"</f>
-        <v>| by/3.0/ | 221875__hero-of-the-winds__spring-boing.wav | https://freesound.org/s/221875/ | hero-of-the-winds |</v>
+        <f t="shared" si="19"/>
+        <v>| by/3.0/ | 216096__richerlandtv__u-f-o.mp3 | https://freesound.org/s/216096/ | RICHERlandTV |</v>
       </c>
     </row>
     <row r="111" spans="1:18" ht="20.25">
       <c r="A111" s="6" t="str">
         <f t="shared" si="18"/>
-        <v>&lt;tr&gt;&lt;td&gt;by/3.0/&lt;/td&gt;&lt;td&gt;240297__jalastram__abstract-guitar-sfx-003.wav&lt;/td&gt;&lt;td&gt;https://freesound.org/s/240297/&lt;/td&gt;&lt;td&gt;jalastram&lt;/td&gt;</v>
-      </c>
-      <c r="J111" s="31" t="s">
+        <v>&lt;tr&gt;&lt;td&gt;by/3.0/&lt;/td&gt;&lt;td&gt;221875__hero-of-the-winds__spring-boing.wav&lt;/td&gt;&lt;td&gt;https://freesound.org/s/221875/&lt;/td&gt;&lt;td&gt;hero-of-the-winds&lt;/td&gt;</v>
+      </c>
+      <c r="J111" s="36" t="s">
         <v>471</v>
       </c>
       <c r="K111" s="6" t="s">
-        <v>453</v>
-      </c>
-      <c r="L111" s="24" t="s">
-        <v>538</v>
+        <v>458</v>
+      </c>
+      <c r="L111" t="s">
+        <v>537</v>
       </c>
       <c r="M111" s="23" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
       <c r="R111" t="str">
-        <f t="shared" si="20"/>
-        <v>| by/3.0/ | 240297__jalastram__abstract-guitar-sfx-003.wav | https://freesound.org/s/240297/ | jalastram |</v>
+        <f t="shared" ref="R111:R129" si="20">"| "&amp;J111&amp;" | "&amp;K111&amp;" | "&amp;L111&amp;" | "&amp;M111&amp;" |"</f>
+        <v>| by/3.0/ | 221875__hero-of-the-winds__spring-boing.wav | https://freesound.org/s/221875/ | hero-of-the-winds |</v>
       </c>
     </row>
     <row r="112" spans="1:18" ht="20.25">
       <c r="A112" s="6" t="str">
         <f t="shared" si="18"/>
-        <v>&lt;tr&gt;&lt;td&gt;by/3.0/&lt;/td&gt;&lt;td&gt;272068__ichbinjager__shotgun-action.wav&lt;/td&gt;&lt;td&gt;https://freesound.org/s/272068/&lt;/td&gt;&lt;td&gt;IchBinJager&lt;/td&gt;</v>
-      </c>
-      <c r="J112" s="23" t="s">
+        <v>&lt;tr&gt;&lt;td&gt;by/3.0/&lt;/td&gt;&lt;td&gt;240297__jalastram__abstract-guitar-sfx-003.wav&lt;/td&gt;&lt;td&gt;https://freesound.org/s/240297/&lt;/td&gt;&lt;td&gt;jalastram&lt;/td&gt;</v>
+      </c>
+      <c r="J112" s="31" t="s">
         <v>471</v>
       </c>
-      <c r="K112" t="s">
-        <v>505</v>
+      <c r="K112" s="6" t="s">
+        <v>453</v>
       </c>
       <c r="L112" s="24" t="s">
-        <v>507</v>
+        <v>538</v>
       </c>
       <c r="M112" s="23" t="s">
-        <v>504</v>
+        <v>524</v>
       </c>
       <c r="R112" t="str">
         <f t="shared" si="20"/>
-        <v>| by/3.0/ | 272068__ichbinjager__shotgun-action.wav | https://freesound.org/s/272068/ | IchBinJager |</v>
+        <v>| by/3.0/ | 240297__jalastram__abstract-guitar-sfx-003.wav | https://freesound.org/s/240297/ | jalastram |</v>
       </c>
     </row>
     <row r="113" spans="1:18" ht="20.25">
       <c r="A113" s="6" t="str">
         <f t="shared" si="18"/>
-        <v>&lt;tr&gt;&lt;td&gt;by/3.0/&lt;/td&gt;&lt;td&gt;275537__wjoojoo__contact-mic-on-satellite-dish04.wav&lt;/td&gt;&lt;td&gt;https://freesound.org/s/275537/&lt;/td&gt;&lt;td&gt;wjoojoo&lt;/td&gt;</v>
-      </c>
-      <c r="J113" s="31" t="s">
+        <v>&lt;tr&gt;&lt;td&gt;by/3.0/&lt;/td&gt;&lt;td&gt;272068__ichbinjager__shotgun-action.wav&lt;/td&gt;&lt;td&gt;https://freesound.org/s/272068/&lt;/td&gt;&lt;td&gt;IchBinJager&lt;/td&gt;</v>
+      </c>
+      <c r="J113" s="23" t="s">
         <v>471</v>
       </c>
-      <c r="K113" s="6" t="s">
-        <v>451</v>
-      </c>
-      <c r="L113" t="s">
-        <v>534</v>
+      <c r="K113" t="s">
+        <v>505</v>
+      </c>
+      <c r="L113" s="24" t="s">
+        <v>507</v>
       </c>
       <c r="M113" s="23" t="s">
-        <v>525</v>
+        <v>504</v>
       </c>
       <c r="R113" t="str">
         <f t="shared" si="20"/>
-        <v>| by/3.0/ | 275537__wjoojoo__contact-mic-on-satellite-dish04.wav | https://freesound.org/s/275537/ | wjoojoo |</v>
+        <v>| by/3.0/ | 272068__ichbinjager__shotgun-action.wav | https://freesound.org/s/272068/ | IchBinJager |</v>
       </c>
     </row>
     <row r="114" spans="1:18" ht="20.25">
       <c r="A114" s="6" t="str">
         <f t="shared" si="18"/>
-        <v>&lt;tr&gt;&lt;td&gt;zero/1.0/&lt;/td&gt;&lt;td&gt;352852__josepharaoh99__game-style-laser-beam.wav&lt;/td&gt;&lt;td&gt;https://freesound.org/s/352852/&lt;/td&gt;&lt;td&gt;josepharaoh99&lt;/td&gt;</v>
+        <v>&lt;tr&gt;&lt;td&gt;by/3.0/&lt;/td&gt;&lt;td&gt;275537__wjoojoo__contact-mic-on-satellite-dish04.wav&lt;/td&gt;&lt;td&gt;https://freesound.org/s/275537/&lt;/td&gt;&lt;td&gt;wjoojoo&lt;/td&gt;</v>
       </c>
       <c r="J114" s="31" t="s">
-        <v>463</v>
+        <v>471</v>
       </c>
       <c r="K114" s="6" t="s">
-        <v>449</v>
+        <v>451</v>
       </c>
       <c r="L114" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
       <c r="M114" s="23" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="R114" t="str">
         <f t="shared" si="20"/>
-        <v>| zero/1.0/ | 352852__josepharaoh99__game-style-laser-beam.wav | https://freesound.org/s/352852/ | josepharaoh99 |</v>
+        <v>| by/3.0/ | 275537__wjoojoo__contact-mic-on-satellite-dish04.wav | https://freesound.org/s/275537/ | wjoojoo |</v>
       </c>
     </row>
     <row r="115" spans="1:18" ht="20.25">
       <c r="A115" s="6" t="str">
         <f t="shared" si="18"/>
-        <v>&lt;tr&gt;&lt;td&gt;zero/1.0/&lt;/td&gt;&lt;td&gt;380886__morganpurkis__doom-shotgun-2017.wav&lt;/td&gt;&lt;td&gt;https://freesound.org/s/380886/&lt;/td&gt;&lt;td&gt;morganpurkis&lt;/td&gt;</v>
-      </c>
-      <c r="J115" s="23" t="s">
+        <v>&lt;tr&gt;&lt;td&gt;zero/1.0/&lt;/td&gt;&lt;td&gt;352852__josepharaoh99__game-style-laser-beam.wav&lt;/td&gt;&lt;td&gt;https://freesound.org/s/352852/&lt;/td&gt;&lt;td&gt;josepharaoh99&lt;/td&gt;</v>
+      </c>
+      <c r="J115" s="31" t="s">
         <v>463</v>
       </c>
-      <c r="K115" t="s">
-        <v>501</v>
-      </c>
-      <c r="L115" s="24" t="s">
-        <v>502</v>
+      <c r="K115" s="6" t="s">
+        <v>449</v>
+      </c>
+      <c r="L115" t="s">
+        <v>535</v>
       </c>
       <c r="M115" s="23" t="s">
-        <v>499</v>
+        <v>526</v>
       </c>
       <c r="R115" t="str">
         <f t="shared" si="20"/>
-        <v>| zero/1.0/ | 380886__morganpurkis__doom-shotgun-2017.wav | https://freesound.org/s/380886/ | morganpurkis |</v>
+        <v>| zero/1.0/ | 352852__josepharaoh99__game-style-laser-beam.wav | https://freesound.org/s/352852/ | josepharaoh99 |</v>
       </c>
     </row>
     <row r="116" spans="1:18" ht="20.25">
       <c r="A116" s="6" t="str">
         <f t="shared" si="18"/>
-        <v>&lt;tr&gt;&lt;td&gt;by/3.0/&lt;/td&gt;&lt;td&gt;383205__spiceprogram__loading-sound.wav&lt;/td&gt;&lt;td&gt;https://freesound.org/s/383205/&lt;/td&gt;&lt;td&gt;SpiceProgram&lt;/td&gt;</v>
-      </c>
-      <c r="J116" s="25" t="s">
-        <v>471</v>
-      </c>
-      <c r="K116" s="23" t="s">
-        <v>447</v>
+        <v>&lt;tr&gt;&lt;td&gt;zero/1.0/&lt;/td&gt;&lt;td&gt;380886__morganpurkis__doom-shotgun-2017.wav&lt;/td&gt;&lt;td&gt;https://freesound.org/s/380886/&lt;/td&gt;&lt;td&gt;morganpurkis&lt;/td&gt;</v>
+      </c>
+      <c r="J116" s="23" t="s">
+        <v>463</v>
+      </c>
+      <c r="K116" t="s">
+        <v>501</v>
       </c>
       <c r="L116" s="24" t="s">
-        <v>481</v>
+        <v>502</v>
       </c>
       <c r="M116" s="23" t="s">
-        <v>482</v>
+        <v>499</v>
       </c>
       <c r="R116" t="str">
         <f t="shared" si="20"/>
-        <v>| by/3.0/ | 383205__spiceprogram__loading-sound.wav | https://freesound.org/s/383205/ | SpiceProgram |</v>
+        <v>| zero/1.0/ | 380886__morganpurkis__doom-shotgun-2017.wav | https://freesound.org/s/380886/ | morganpurkis |</v>
       </c>
     </row>
     <row r="117" spans="1:18" ht="20.25">
       <c r="A117" s="6" t="str">
         <f t="shared" si="18"/>
-        <v>&lt;tr&gt;&lt;td&gt;zero/1.0/&lt;/td&gt;&lt;td&gt;383760__deleted-user-7146007__laboratory-mad-scientist-science-fiction-sci-fi.wav&lt;/td&gt;&lt;td&gt;https://freesound.org/s/383760/&lt;/td&gt;&lt;td&gt;deleted-user-7146007&lt;/td&gt;</v>
-      </c>
-      <c r="J117" s="30" t="s">
-        <v>463</v>
-      </c>
-      <c r="K117" s="17" t="s">
-        <v>445</v>
-      </c>
-      <c r="L117" t="s">
-        <v>533</v>
+        <v>&lt;tr&gt;&lt;td&gt;by/3.0/&lt;/td&gt;&lt;td&gt;383205__spiceprogram__loading-sound.wav&lt;/td&gt;&lt;td&gt;https://freesound.org/s/383205/&lt;/td&gt;&lt;td&gt;SpiceProgram&lt;/td&gt;</v>
+      </c>
+      <c r="J117" s="25" t="s">
+        <v>471</v>
+      </c>
+      <c r="K117" s="23" t="s">
+        <v>447</v>
+      </c>
+      <c r="L117" s="24" t="s">
+        <v>481</v>
       </c>
       <c r="M117" s="23" t="s">
-        <v>527</v>
+        <v>482</v>
       </c>
       <c r="R117" t="str">
         <f t="shared" si="20"/>
-        <v>| zero/1.0/ | 383760__deleted-user-7146007__laboratory-mad-scientist-science-fiction-sci-fi.wav | https://freesound.org/s/383760/ | deleted-user-7146007 |</v>
+        <v>| by/3.0/ | 383205__spiceprogram__loading-sound.wav | https://freesound.org/s/383205/ | SpiceProgram |</v>
       </c>
     </row>
     <row r="118" spans="1:18" ht="20.25">
       <c r="A118" s="6" t="str">
         <f t="shared" si="18"/>
-        <v>&lt;tr&gt;&lt;td&gt;zero/1.0/&lt;/td&gt;&lt;td&gt;397254__screamstudio__loading.wav&lt;/td&gt;&lt;td&gt;https://freesound.org/s/397254/&lt;/td&gt;&lt;td&gt;ScreamStudio&lt;/td&gt;</v>
-      </c>
-      <c r="J118" s="27" t="s">
+        <v>&lt;tr&gt;&lt;td&gt;zero/1.0/&lt;/td&gt;&lt;td&gt;383760__deleted-user-7146007__laboratory-mad-scientist-science-fiction-sci-fi.wav&lt;/td&gt;&lt;td&gt;https://freesound.org/s/383760/&lt;/td&gt;&lt;td&gt;deleted-user-7146007&lt;/td&gt;</v>
+      </c>
+      <c r="J118" s="30" t="s">
         <v>463</v>
       </c>
-      <c r="K118" s="30" t="s">
-        <v>437</v>
-      </c>
-      <c r="L118" s="24" t="s">
-        <v>466</v>
+      <c r="K118" s="17" t="s">
+        <v>445</v>
+      </c>
+      <c r="L118" t="s">
+        <v>533</v>
       </c>
       <c r="M118" s="23" t="s">
-        <v>467</v>
+        <v>527</v>
       </c>
       <c r="R118" t="str">
         <f t="shared" si="20"/>
-        <v>| zero/1.0/ | 397254__screamstudio__loading.wav | https://freesound.org/s/397254/ | ScreamStudio |</v>
+        <v>| zero/1.0/ | 383760__deleted-user-7146007__laboratory-mad-scientist-science-fiction-sci-fi.wav | https://freesound.org/s/383760/ | deleted-user-7146007 |</v>
       </c>
     </row>
     <row r="119" spans="1:18" ht="20.25">
       <c r="A119" s="6" t="str">
         <f t="shared" si="18"/>
-        <v>&lt;tr&gt;&lt;td&gt;zero/1.0/&lt;/td&gt;&lt;td&gt;404068__swordofkings128__backyard-gate-open.wav&lt;/td&gt;&lt;td&gt;https://freesound.org/s/404068/&lt;/td&gt;&lt;td&gt;swordofkings128&lt;/td&gt;</v>
-      </c>
-      <c r="J119" s="30" t="s">
+        <v>&lt;tr&gt;&lt;td&gt;zero/1.0/&lt;/td&gt;&lt;td&gt;397254__screamstudio__loading.wav&lt;/td&gt;&lt;td&gt;https://freesound.org/s/397254/&lt;/td&gt;&lt;td&gt;ScreamStudio&lt;/td&gt;</v>
+      </c>
+      <c r="J119" s="27" t="s">
         <v>463</v>
       </c>
-      <c r="K119" s="17" t="s">
-        <v>510</v>
+      <c r="K119" s="30" t="s">
+        <v>437</v>
       </c>
       <c r="L119" s="24" t="s">
-        <v>515</v>
+        <v>466</v>
       </c>
       <c r="M119" s="23" t="s">
-        <v>511</v>
+        <v>467</v>
       </c>
       <c r="R119" t="str">
         <f t="shared" si="20"/>
-        <v>| zero/1.0/ | 404068__swordofkings128__backyard-gate-open.wav | https://freesound.org/s/404068/ | swordofkings128 |</v>
+        <v>| zero/1.0/ | 397254__screamstudio__loading.wav | https://freesound.org/s/397254/ | ScreamStudio |</v>
       </c>
     </row>
     <row r="120" spans="1:18" ht="20.25">
       <c r="A120" s="6" t="str">
         <f t="shared" si="18"/>
-        <v>&lt;tr&gt;&lt;td&gt;zero/1.0/&lt;/td&gt;&lt;td&gt;407052__sojan__power-charge.flac&lt;/td&gt;&lt;td&gt;https://freesound.org/s/193610/&lt;/td&gt;&lt;td&gt;crashoverride61088&lt;/td&gt;</v>
-      </c>
-      <c r="J120" s="27" t="s">
+        <v>&lt;tr&gt;&lt;td&gt;zero/1.0/&lt;/td&gt;&lt;td&gt;404068__swordofkings128__backyard-gate-open.wav&lt;/td&gt;&lt;td&gt;https://freesound.org/s/404068/&lt;/td&gt;&lt;td&gt;swordofkings128&lt;/td&gt;</v>
+      </c>
+      <c r="J120" s="30" t="s">
         <v>463</v>
       </c>
-      <c r="K120" s="30" t="s">
-        <v>439</v>
+      <c r="K120" s="17" t="s">
+        <v>510</v>
       </c>
       <c r="L120" s="24" t="s">
-        <v>464</v>
+        <v>515</v>
       </c>
       <c r="M120" s="23" t="s">
-        <v>465</v>
+        <v>511</v>
       </c>
       <c r="R120" t="str">
         <f t="shared" si="20"/>
-        <v>| zero/1.0/ | 407052__sojan__power-charge.flac | https://freesound.org/s/193610/ | crashoverride61088 |</v>
+        <v>| zero/1.0/ | 404068__swordofkings128__backyard-gate-open.wav | https://freesound.org/s/404068/ | swordofkings128 |</v>
       </c>
     </row>
     <row r="121" spans="1:18" ht="20.25">
       <c r="A121" s="6" t="str">
         <f t="shared" si="18"/>
-        <v>&lt;tr&gt;&lt;td&gt;by/3.0/&lt;/td&gt;&lt;td&gt;417131__cuddlenucks__science-fiction-noise-3.wav&lt;/td&gt;&lt;td&gt;https://freesound.org/s/417131/&lt;/td&gt;&lt;td&gt;cuddlenucks&lt;/td&gt;</v>
-      </c>
-      <c r="J121" s="30" t="s">
-        <v>471</v>
-      </c>
-      <c r="K121" s="17" t="s">
-        <v>443</v>
-      </c>
-      <c r="L121" t="s">
-        <v>539</v>
+        <v>&lt;tr&gt;&lt;td&gt;zero/1.0/&lt;/td&gt;&lt;td&gt;407052__sojan__power-charge.flac&lt;/td&gt;&lt;td&gt;https://freesound.org/s/193610/&lt;/td&gt;&lt;td&gt;crashoverride61088&lt;/td&gt;</v>
+      </c>
+      <c r="J121" s="27" t="s">
+        <v>463</v>
+      </c>
+      <c r="K121" s="30" t="s">
+        <v>439</v>
+      </c>
+      <c r="L121" s="24" t="s">
+        <v>464</v>
       </c>
       <c r="M121" s="23" t="s">
-        <v>528</v>
+        <v>465</v>
       </c>
       <c r="R121" t="str">
         <f t="shared" si="20"/>
-        <v>| by/3.0/ | 417131__cuddlenucks__science-fiction-noise-3.wav | https://freesound.org/s/417131/ | cuddlenucks |</v>
+        <v>| zero/1.0/ | 407052__sojan__power-charge.flac | https://freesound.org/s/193610/ | crashoverride61088 |</v>
       </c>
     </row>
     <row r="122" spans="1:18" ht="20.25">
       <c r="A122" s="6" t="str">
         <f t="shared" si="18"/>
-        <v>&lt;tr&gt;&lt;td&gt;by/3.0/&lt;/td&gt;&lt;td&gt;417363__xcreenplay__boing-massive-kick.wav&lt;/td&gt;&lt;td&gt;https://freesound.org/s/417363/&lt;/td&gt;&lt;td&gt;xcreenplay&lt;/td&gt;</v>
+        <v>&lt;tr&gt;&lt;td&gt;by/3.0/&lt;/td&gt;&lt;td&gt;417131__cuddlenucks__science-fiction-noise-3.wav&lt;/td&gt;&lt;td&gt;https://freesound.org/s/417131/&lt;/td&gt;&lt;td&gt;cuddlenucks&lt;/td&gt;</v>
       </c>
       <c r="J122" s="30" t="s">
         <v>471</v>
       </c>
       <c r="K122" s="17" t="s">
-        <v>441</v>
+        <v>443</v>
       </c>
       <c r="L122" t="s">
-        <v>536</v>
+        <v>539</v>
       </c>
       <c r="M122" s="23" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
       <c r="R122" t="str">
         <f t="shared" si="20"/>
-        <v>| by/3.0/ | 417363__xcreenplay__boing-massive-kick.wav | https://freesound.org/s/417363/ | xcreenplay |</v>
+        <v>| by/3.0/ | 417131__cuddlenucks__science-fiction-noise-3.wav | https://freesound.org/s/417131/ | cuddlenucks |</v>
       </c>
     </row>
     <row r="123" spans="1:18" ht="20.25">
       <c r="A123" s="6" t="str">
         <f t="shared" si="18"/>
-        <v>&lt;tr&gt;&lt;td&gt;by/3.0/&lt;/td&gt;&lt;td&gt;431117__inspectorj__door-front-opening-a.wav&lt;/td&gt;&lt;td&gt;https://freesound.org/s/431117/&lt;/td&gt;&lt;td&gt;inspectorj&lt;/td&gt;</v>
-      </c>
-      <c r="J123" s="23" t="s">
+        <v>&lt;tr&gt;&lt;td&gt;by/3.0/&lt;/td&gt;&lt;td&gt;417363__xcreenplay__boing-massive-kick.wav&lt;/td&gt;&lt;td&gt;https://freesound.org/s/417363/&lt;/td&gt;&lt;td&gt;xcreenplay&lt;/td&gt;</v>
+      </c>
+      <c r="J123" s="30" t="s">
         <v>471</v>
       </c>
       <c r="K123" s="17" t="s">
-        <v>508</v>
-      </c>
-      <c r="L123" s="24" t="s">
-        <v>514</v>
+        <v>441</v>
+      </c>
+      <c r="L123" t="s">
+        <v>536</v>
       </c>
       <c r="M123" s="23" t="s">
-        <v>509</v>
+        <v>529</v>
       </c>
       <c r="R123" t="str">
         <f t="shared" si="20"/>
-        <v>| by/3.0/ | 431117__inspectorj__door-front-opening-a.wav | https://freesound.org/s/431117/ | inspectorj |</v>
+        <v>| by/3.0/ | 417363__xcreenplay__boing-massive-kick.wav | https://freesound.org/s/417363/ | xcreenplay |</v>
       </c>
     </row>
     <row r="124" spans="1:18" ht="20.25">
       <c r="A124" s="6" t="str">
         <f t="shared" si="18"/>
-        <v>&lt;tr&gt;&lt;td&gt;zero/1.0/&lt;/td&gt;&lt;td&gt;500418__dj-somar__intro-reverso-craver-microbrute.wav&lt;/td&gt;&lt;td&gt;https://freesound.org/s/500418/&lt;/td&gt;&lt;td&gt;DJ_SoMaR&lt;/td&gt;</v>
-      </c>
-      <c r="J124" s="30" t="s">
-        <v>463</v>
+        <v>&lt;tr&gt;&lt;td&gt;by/3.0/&lt;/td&gt;&lt;td&gt;431117__inspectorj__door-front-opening-a.wav&lt;/td&gt;&lt;td&gt;https://freesound.org/s/431117/&lt;/td&gt;&lt;td&gt;inspectorj&lt;/td&gt;</v>
+      </c>
+      <c r="J124" s="23" t="s">
+        <v>471</v>
       </c>
       <c r="K124" s="17" t="s">
-        <v>497</v>
+        <v>508</v>
       </c>
       <c r="L124" s="24" t="s">
-        <v>503</v>
+        <v>514</v>
       </c>
       <c r="M124" s="23" t="s">
-        <v>498</v>
+        <v>509</v>
       </c>
       <c r="R124" t="str">
         <f t="shared" si="20"/>
-        <v>| zero/1.0/ | 500418__dj-somar__intro-reverso-craver-microbrute.wav | https://freesound.org/s/500418/ | DJ_SoMaR |</v>
+        <v>| by/3.0/ | 431117__inspectorj__door-front-opening-a.wav | https://freesound.org/s/431117/ | inspectorj |</v>
       </c>
     </row>
     <row r="125" spans="1:18" ht="20.25">
       <c r="A125" s="6" t="str">
         <f t="shared" si="18"/>
-        <v>&lt;tr&gt;&lt;td&gt;by/3.0/&lt;/td&gt;&lt;td&gt;7967__cfork__boing-raw.aiff&lt;/td&gt;&lt;td&gt;https://freesound.org/s/7967/&lt;/td&gt;&lt;td&gt;cfork&lt;/td&gt;</v>
-      </c>
-      <c r="J125" s="27" t="s">
-        <v>471</v>
-      </c>
-      <c r="K125" s="30" t="s">
-        <v>478</v>
+        <v>&lt;tr&gt;&lt;td&gt;zero/1.0/&lt;/td&gt;&lt;td&gt;500418__dj-somar__intro-reverso-craver-microbrute.wav&lt;/td&gt;&lt;td&gt;https://freesound.org/s/500418/&lt;/td&gt;&lt;td&gt;DJ_SoMaR&lt;/td&gt;</v>
+      </c>
+      <c r="J125" s="30" t="s">
+        <v>463</v>
+      </c>
+      <c r="K125" s="17" t="s">
+        <v>497</v>
       </c>
       <c r="L125" s="24" t="s">
-        <v>479</v>
+        <v>503</v>
       </c>
       <c r="M125" s="23" t="s">
-        <v>480</v>
+        <v>498</v>
       </c>
       <c r="R125" t="str">
         <f t="shared" si="20"/>
-        <v>| by/3.0/ | 7967__cfork__boing-raw.aiff | https://freesound.org/s/7967/ | cfork |</v>
+        <v>| zero/1.0/ | 500418__dj-somar__intro-reverso-craver-microbrute.wav | https://freesound.org/s/500418/ | DJ_SoMaR |</v>
       </c>
     </row>
     <row r="126" spans="1:18" ht="20.25">
       <c r="A126" s="6" t="str">
         <f t="shared" si="18"/>
-        <v>&lt;tr&gt;&lt;td&gt;by/3.0/&lt;/td&gt;&lt;td&gt;88635__uair01__bicycle-picture-in-spectrum.wav&lt;/td&gt;&lt;td&gt;https://freesound.org/s/88635/&lt;/td&gt;&lt;td&gt;uair01&lt;/td&gt;</v>
-      </c>
-      <c r="J126" s="25" t="s">
+        <v>&lt;tr&gt;&lt;td&gt;by/3.0/&lt;/td&gt;&lt;td&gt;7967__cfork__boing-raw.aiff&lt;/td&gt;&lt;td&gt;https://freesound.org/s/7967/&lt;/td&gt;&lt;td&gt;cfork&lt;/td&gt;</v>
+      </c>
+      <c r="J126" s="27" t="s">
         <v>471</v>
       </c>
       <c r="K126" s="30" t="s">
-        <v>475</v>
+        <v>478</v>
       </c>
       <c r="L126" s="24" t="s">
-        <v>476</v>
+        <v>479</v>
       </c>
       <c r="M126" s="23" t="s">
-        <v>477</v>
+        <v>480</v>
       </c>
       <c r="R126" t="str">
         <f t="shared" si="20"/>
-        <v>| by/3.0/ | 88635__uair01__bicycle-picture-in-spectrum.wav | https://freesound.org/s/88635/ | uair01 |</v>
+        <v>| by/3.0/ | 7967__cfork__boing-raw.aiff | https://freesound.org/s/7967/ | cfork |</v>
       </c>
     </row>
     <row r="127" spans="1:18" ht="20.25">
       <c r="A127" s="6" t="str">
         <f t="shared" si="18"/>
-        <v>&lt;tr&gt;&lt;td&gt;by-nc/3.0/&lt;/td&gt;&lt;td&gt;91296__timbre__bwaang-2-reverb.mp3&lt;/td&gt;&lt;td&gt;https://freesound.org/s/91296/&lt;/td&gt;&lt;td&gt;timbre&lt;/td&gt;</v>
-      </c>
-      <c r="J127" s="30" t="s">
-        <v>483</v>
-      </c>
-      <c r="K127" s="17" t="s">
-        <v>495</v>
-      </c>
-      <c r="L127" t="s">
-        <v>544</v>
+        <v>&lt;tr&gt;&lt;td&gt;by/3.0/&lt;/td&gt;&lt;td&gt;88635__uair01__bicycle-picture-in-spectrum.wav&lt;/td&gt;&lt;td&gt;https://freesound.org/s/88635/&lt;/td&gt;&lt;td&gt;uair01&lt;/td&gt;</v>
+      </c>
+      <c r="J127" s="25" t="s">
+        <v>471</v>
+      </c>
+      <c r="K127" s="30" t="s">
+        <v>475</v>
+      </c>
+      <c r="L127" s="24" t="s">
+        <v>476</v>
       </c>
       <c r="M127" s="23" t="s">
-        <v>531</v>
+        <v>477</v>
       </c>
       <c r="R127" t="str">
         <f t="shared" si="20"/>
-        <v>| by-nc/3.0/ | 91296__timbre__bwaang-2-reverb.mp3 | https://freesound.org/s/91296/ | timbre |</v>
+        <v>| by/3.0/ | 88635__uair01__bicycle-picture-in-spectrum.wav | https://freesound.org/s/88635/ | uair01 |</v>
       </c>
     </row>
     <row r="128" spans="1:18" ht="20.25">
       <c r="A128" s="6" t="str">
         <f t="shared" si="18"/>
-        <v>&lt;tr&gt;&lt;td&gt;by/3.0/&lt;/td&gt;&lt;td&gt;96964__gabisaraceni__porta-abrindo-5.wav&lt;/td&gt;&lt;td&gt;https://freesound.org/s/96964/&lt;/td&gt;&lt;td&gt;gabisaraceni&lt;/td&gt;</v>
+        <v>&lt;tr&gt;&lt;td&gt;by-nc/3.0/&lt;/td&gt;&lt;td&gt;91296__timbre__bwaang-2-reverb.mp3&lt;/td&gt;&lt;td&gt;https://freesound.org/s/91296/&lt;/td&gt;&lt;td&gt;timbre&lt;/td&gt;</v>
       </c>
       <c r="J128" s="30" t="s">
-        <v>471</v>
+        <v>483</v>
       </c>
       <c r="K128" s="17" t="s">
-        <v>512</v>
-      </c>
-      <c r="L128" s="24" t="s">
-        <v>516</v>
+        <v>495</v>
+      </c>
+      <c r="L128" t="s">
+        <v>544</v>
       </c>
       <c r="M128" s="23" t="s">
-        <v>513</v>
+        <v>531</v>
       </c>
       <c r="R128" t="str">
         <f t="shared" si="20"/>
+        <v>| by-nc/3.0/ | 91296__timbre__bwaang-2-reverb.mp3 | https://freesound.org/s/91296/ | timbre |</v>
+      </c>
+    </row>
+    <row r="129" spans="1:18" ht="20.25">
+      <c r="A129" s="6" t="str">
+        <f t="shared" si="18"/>
+        <v>&lt;tr&gt;&lt;td&gt;by/3.0/&lt;/td&gt;&lt;td&gt;96964__gabisaraceni__porta-abrindo-5.wav&lt;/td&gt;&lt;td&gt;https://freesound.org/s/96964/&lt;/td&gt;&lt;td&gt;gabisaraceni&lt;/td&gt;</v>
+      </c>
+      <c r="J129" s="30" t="s">
+        <v>471</v>
+      </c>
+      <c r="K129" s="17" t="s">
+        <v>512</v>
+      </c>
+      <c r="L129" s="24" t="s">
+        <v>516</v>
+      </c>
+      <c r="M129" s="23" t="s">
+        <v>513</v>
+      </c>
+      <c r="R129" t="str">
+        <f t="shared" si="20"/>
         <v>| by/3.0/ | 96964__gabisaraceni__porta-abrindo-5.wav | https://freesound.org/s/96964/ | gabisaraceni |</v>
       </c>
     </row>
-    <row r="129" spans="1:12">
-      <c r="A129" s="6" t="s">
+    <row r="130" spans="1:18">
+      <c r="A130" s="6" t="s">
         <v>585</v>
       </c>
     </row>
-    <row r="130" spans="1:12">
-      <c r="A130" t="s">
+    <row r="131" spans="1:18">
+      <c r="A131" t="s">
         <v>600</v>
       </c>
     </row>
-    <row r="131" spans="1:12">
-      <c r="A131" s="6" t="s">
+    <row r="132" spans="1:18">
+      <c r="A132" s="6" t="s">
         <v>584</v>
       </c>
     </row>
-    <row r="132" spans="1:12" ht="15.75" thickBot="1">
-      <c r="A132" t="s">
+    <row r="133" spans="1:18" ht="15.75" thickBot="1">
+      <c r="A133" t="s">
         <v>586</v>
       </c>
     </row>
-    <row r="133" spans="1:12" ht="18" thickBot="1">
-      <c r="A133" s="6" t="str">
-        <f>"&lt;tr&gt;&lt;td&gt;&lt;b&gt;"&amp;J133&amp;"&lt;/b&gt;&lt;/td&gt;&lt;td&gt;&lt;b&gt;"&amp;K133&amp;"&lt;/b&gt;&lt;/td&gt;&lt;td&gt;&lt;b&gt;"&amp;L133&amp;"&lt;/b&gt;&lt;/td&gt;"</f>
+    <row r="134" spans="1:18" ht="18" thickBot="1">
+      <c r="A134" s="6" t="str">
+        <f>"&lt;tr&gt;&lt;td&gt;&lt;b&gt;"&amp;J134&amp;"&lt;/b&gt;&lt;/td&gt;&lt;td&gt;&lt;b&gt;"&amp;K134&amp;"&lt;/b&gt;&lt;/td&gt;&lt;td&gt;&lt;b&gt;"&amp;L134&amp;"&lt;/b&gt;&lt;/td&gt;"</f>
         <v>&lt;tr&gt;&lt;td&gt;&lt;b&gt;Tag&lt;/b&gt;&lt;/td&gt;&lt;td&gt;&lt;b&gt;Name&lt;/b&gt;&lt;/td&gt;&lt;td&gt;&lt;b&gt;URL&lt;/b&gt;&lt;/td&gt;</v>
       </c>
-      <c r="J133" s="42" t="s">
+      <c r="J134" s="42" t="s">
         <v>459</v>
       </c>
-      <c r="K133" s="42" t="s">
+      <c r="K134" s="42" t="s">
         <v>587</v>
       </c>
-      <c r="L133" s="42" t="s">
+      <c r="L134" s="42" t="s">
         <v>461</v>
       </c>
     </row>
-    <row r="134" spans="1:12" ht="45.75" thickBot="1">
-      <c r="A134" s="6" t="str">
-        <f>"&lt;tr&gt;&lt;td&gt;"&amp;J134&amp;"&lt;/td&gt;&lt;td&gt;"&amp;K134&amp;"&lt;/td&gt;&lt;td&gt;"&amp;L134&amp;"&lt;/td&gt;"</f>
-        <v>&lt;tr&gt;&lt;td&gt;zero/1.0/&lt;/td&gt;&lt;td&gt;Creative Commons 0 License&lt;/td&gt;&lt;td&gt;https://creativecommons.org/publicdomain/zero/1.0/&lt;/td&gt;</v>
-      </c>
-      <c r="J134" s="43" t="s">
-        <v>463</v>
-      </c>
-      <c r="K134" s="43" t="s">
-        <v>588</v>
-      </c>
-      <c r="L134" s="44" t="s">
-        <v>589</v>
-      </c>
-    </row>
-    <row r="135" spans="1:12" ht="30.75" thickBot="1">
+    <row r="135" spans="1:18" ht="45.75" thickBot="1">
       <c r="A135" s="6" t="str">
         <f>"&lt;tr&gt;&lt;td&gt;"&amp;J135&amp;"&lt;/td&gt;&lt;td&gt;"&amp;K135&amp;"&lt;/td&gt;&lt;td&gt;"&amp;L135&amp;"&lt;/td&gt;"</f>
-        <v>&lt;tr&gt;&lt;td&gt;by/3.0/&lt;/td&gt;&lt;td&gt;Creative Commons Attribution License&lt;/td&gt;&lt;td&gt;https://creativecommons.org/licenses/by/3.0/&lt;/td&gt;</v>
-      </c>
-      <c r="J135" s="45" t="s">
-        <v>471</v>
-      </c>
-      <c r="K135" s="45" t="s">
-        <v>590</v>
-      </c>
-      <c r="L135" s="46" t="s">
-        <v>591</v>
-      </c>
-    </row>
-    <row r="136" spans="1:12" ht="30.75" thickBot="1">
+        <v>&lt;tr&gt;&lt;td&gt;zero/1.0/&lt;/td&gt;&lt;td&gt;Creative Commons 0 License&lt;/td&gt;&lt;td&gt;https://creativecommons.org/publicdomain/zero/1.0/&lt;/td&gt;</v>
+      </c>
+      <c r="J135" s="43" t="s">
+        <v>463</v>
+      </c>
+      <c r="K135" s="43" t="s">
+        <v>588</v>
+      </c>
+      <c r="L135" s="44" t="s">
+        <v>589</v>
+      </c>
+    </row>
+    <row r="136" spans="1:18" ht="30.75" thickBot="1">
       <c r="A136" s="6" t="str">
         <f>"&lt;tr&gt;&lt;td&gt;"&amp;J136&amp;"&lt;/td&gt;&lt;td&gt;"&amp;K136&amp;"&lt;/td&gt;&lt;td&gt;"&amp;L136&amp;"&lt;/td&gt;"</f>
+        <v>&lt;tr&gt;&lt;td&gt;by/3.0/&lt;/td&gt;&lt;td&gt;Creative Commons Attribution License&lt;/td&gt;&lt;td&gt;https://creativecommons.org/licenses/by/3.0/&lt;/td&gt;</v>
+      </c>
+      <c r="J136" s="45" t="s">
+        <v>471</v>
+      </c>
+      <c r="K136" s="45" t="s">
+        <v>590</v>
+      </c>
+      <c r="L136" s="46" t="s">
+        <v>591</v>
+      </c>
+    </row>
+    <row r="137" spans="1:18" ht="30.75" thickBot="1">
+      <c r="A137" s="6" t="str">
+        <f>"&lt;tr&gt;&lt;td&gt;"&amp;J137&amp;"&lt;/td&gt;&lt;td&gt;"&amp;K137&amp;"&lt;/td&gt;&lt;td&gt;"&amp;L137&amp;"&lt;/td&gt;"</f>
         <v>&lt;tr&gt;&lt;td&gt;by-nc/3.0/&lt;/td&gt;&lt;td&gt;Creative Commons Attribution Noncommercial License&lt;/td&gt;&lt;td&gt;https://creativecommons.org/licenses/by-nc/3.0/&lt;/td&gt;</v>
       </c>
-      <c r="J136" s="43" t="s">
+      <c r="J137" s="43" t="s">
         <v>483</v>
       </c>
-      <c r="K136" s="43" t="s">
+      <c r="K137" s="43" t="s">
         <v>592</v>
       </c>
-      <c r="L136" s="44" t="s">
+      <c r="L137" s="44" t="s">
         <v>593</v>
       </c>
     </row>
-    <row r="137" spans="1:12">
-      <c r="A137" s="6" t="s">
+    <row r="138" spans="1:18">
+      <c r="A138" s="6" t="s">
         <v>585</v>
       </c>
     </row>
-    <row r="145" spans="3:5">
-      <c r="C145" t="s">
+    <row r="146" spans="3:5">
+      <c r="C146" t="s">
         <v>693</v>
       </c>
-      <c r="D145" s="24" t="s">
+      <c r="D146" s="24" t="s">
         <v>692</v>
       </c>
-      <c r="E145" s="24" t="s">
+      <c r="E146" s="24" t="s">
         <v>691</v>
       </c>
     </row>
-    <row r="152" spans="3:5">
-      <c r="C152" t="s">
+    <row r="153" spans="3:5">
+      <c r="C153" t="s">
         <v>706</v>
       </c>
-      <c r="D152" s="24" t="s">
+      <c r="D153" s="24" t="s">
         <v>705</v>
       </c>
-      <c r="E152" s="24" t="s">
+      <c r="E153" s="24" t="s">
         <v>698</v>
       </c>
     </row>
-    <row r="162" spans="2:3">
-      <c r="C162" s="13" t="s">
+    <row r="163" spans="2:3">
+      <c r="C163" s="13" t="s">
         <v>4437</v>
       </c>
     </row>
-    <row r="164" spans="2:3">
-      <c r="C164" t="s">
+    <row r="165" spans="2:3">
+      <c r="C165" t="s">
         <v>4439</v>
-      </c>
-    </row>
-    <row r="165" spans="2:3">
-      <c r="B165">
-        <v>1</v>
-      </c>
-      <c r="C165" t="s">
-        <v>4445</v>
       </c>
     </row>
     <row r="166" spans="2:3">
       <c r="B166">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C166" t="s">
-        <v>4444</v>
+        <v>4445</v>
       </c>
     </row>
     <row r="167" spans="2:3">
       <c r="B167">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C167" t="s">
-        <v>4446</v>
+        <v>4444</v>
       </c>
     </row>
     <row r="168" spans="2:3">
       <c r="B168">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C168" t="s">
-        <v>4447</v>
+        <v>4446</v>
       </c>
     </row>
     <row r="169" spans="2:3">
       <c r="B169">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C169" t="s">
-        <v>4448</v>
+        <v>4447</v>
       </c>
     </row>
     <row r="170" spans="2:3">
       <c r="B170">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C170" t="s">
-        <v>4449</v>
+        <v>4448</v>
       </c>
     </row>
     <row r="171" spans="2:3">
       <c r="B171">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C171" t="s">
-        <v>4450</v>
+        <v>4449</v>
       </c>
     </row>
     <row r="172" spans="2:3">
       <c r="B172">
+        <v>7</v>
+      </c>
+      <c r="C172" t="s">
+        <v>4450</v>
+      </c>
+    </row>
+    <row r="173" spans="2:3">
+      <c r="B173">
         <v>8</v>
       </c>
-      <c r="C172" t="s">
+      <c r="C173" t="s">
         <v>4451</v>
       </c>
     </row>
-    <row r="174" spans="2:3">
-      <c r="C174" t="s">
+    <row r="175" spans="2:3">
+      <c r="C175" t="s">
         <v>4438</v>
-      </c>
-    </row>
-    <row r="175" spans="2:3">
-      <c r="B175">
-        <v>1</v>
-      </c>
-      <c r="C175" s="90" t="s">
-        <v>6005</v>
       </c>
     </row>
     <row r="176" spans="2:3">
       <c r="B176">
+        <v>1</v>
+      </c>
+      <c r="C176" s="90" t="s">
+        <v>6005</v>
+      </c>
+    </row>
+    <row r="177" spans="2:4">
+      <c r="B177">
         <v>2</v>
       </c>
-      <c r="C176" s="90" t="s">
+      <c r="C177" s="90" t="s">
         <v>4443</v>
       </c>
     </row>
-    <row r="178" spans="3:4">
-      <c r="D178" s="9"/>
-    </row>
-    <row r="183" spans="3:4">
-      <c r="C183" t="s">
+    <row r="179" spans="2:4">
+      <c r="D179" s="9"/>
+    </row>
+    <row r="184" spans="2:4">
+      <c r="C184" t="s">
         <v>4440</v>
       </c>
     </row>
-    <row r="184" spans="3:4">
-      <c r="C184" t="s">
+    <row r="185" spans="2:4">
+      <c r="C185" t="s">
         <v>4442</v>
       </c>
     </row>
-    <row r="185" spans="3:4">
-      <c r="C185" t="s">
+    <row r="186" spans="2:4">
+      <c r="C186" t="s">
         <v>4441</v>
       </c>
     </row>
-    <row r="189" spans="3:4">
-      <c r="D189" s="9"/>
+    <row r="190" spans="2:4">
+      <c r="D190" s="9"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:H73" xr:uid="{D49867B0-9605-4DAD-A171-997D81FF01DA}"/>
-  <sortState ref="D166:D190">
-    <sortCondition ref="D166:D190"/>
+  <autoFilter ref="A1:H74" xr:uid="{D49867B0-9605-4DAD-A171-997D81FF01DA}"/>
+  <sortState ref="D167:D191">
+    <sortCondition ref="D167:D191"/>
   </sortState>
   <hyperlinks>
-    <hyperlink ref="L120" r:id="rId1" xr:uid="{0389BFEF-2278-1C4C-AFFD-40911D54BA38}"/>
-    <hyperlink ref="L118" r:id="rId2" xr:uid="{6DC6DCC3-96F7-244A-A515-6ACC236B66A6}"/>
-    <hyperlink ref="L103" r:id="rId3" xr:uid="{CCE745AF-D2B8-1E45-81C2-27CEF6C5B2AF}"/>
-    <hyperlink ref="L109" r:id="rId4" xr:uid="{FC7F966A-1EC2-DE4A-875D-CA9E5FD25210}"/>
-    <hyperlink ref="L126" r:id="rId5" xr:uid="{0DB3DAF8-4FD8-5441-A5EE-FDB2E3108255}"/>
-    <hyperlink ref="L125" r:id="rId6" xr:uid="{6722E195-E4EF-1D49-A046-EFE49EC89CB6}"/>
-    <hyperlink ref="L116" r:id="rId7" xr:uid="{35EA502B-43EE-5648-92D3-03388141605B}"/>
-    <hyperlink ref="L108" r:id="rId8" xr:uid="{F628B53D-420C-0844-AF06-3CBF155582C6}"/>
-    <hyperlink ref="L115" r:id="rId9" xr:uid="{FA1B324F-1513-1343-9CCE-E23AFD154FFD}"/>
-    <hyperlink ref="L124" r:id="rId10" xr:uid="{C5AA4A87-0C8F-9A4C-974F-82A19E89F99C}"/>
-    <hyperlink ref="L112" r:id="rId11" xr:uid="{E1112DD8-8BE8-BD47-9002-F00DDA38363C}"/>
-    <hyperlink ref="L123" r:id="rId12" xr:uid="{4D774EC1-CC16-C24F-88F2-E9E20B8A8FC0}"/>
-    <hyperlink ref="L115:L116" r:id="rId13" display="https://freesound.org/s//" xr:uid="{5FB99E8B-AEFC-6A45-851E-E3C683DC5AC1}"/>
-    <hyperlink ref="L119" r:id="rId14" xr:uid="{E2EACC90-D2ED-AF4A-9302-ADD31B56C321}"/>
-    <hyperlink ref="L128" r:id="rId15" xr:uid="{13F37B0F-8A53-0B4F-8FE7-132D2186D638}"/>
-    <hyperlink ref="L111" r:id="rId16" xr:uid="{FA55BAC7-078A-8944-9FB5-42D7B041E218}"/>
+    <hyperlink ref="L121" r:id="rId1" xr:uid="{0389BFEF-2278-1C4C-AFFD-40911D54BA38}"/>
+    <hyperlink ref="L119" r:id="rId2" xr:uid="{6DC6DCC3-96F7-244A-A515-6ACC236B66A6}"/>
+    <hyperlink ref="L104" r:id="rId3" xr:uid="{CCE745AF-D2B8-1E45-81C2-27CEF6C5B2AF}"/>
+    <hyperlink ref="L110" r:id="rId4" xr:uid="{FC7F966A-1EC2-DE4A-875D-CA9E5FD25210}"/>
+    <hyperlink ref="L127" r:id="rId5" xr:uid="{0DB3DAF8-4FD8-5441-A5EE-FDB2E3108255}"/>
+    <hyperlink ref="L126" r:id="rId6" xr:uid="{6722E195-E4EF-1D49-A046-EFE49EC89CB6}"/>
+    <hyperlink ref="L117" r:id="rId7" xr:uid="{35EA502B-43EE-5648-92D3-03388141605B}"/>
+    <hyperlink ref="L109" r:id="rId8" xr:uid="{F628B53D-420C-0844-AF06-3CBF155582C6}"/>
+    <hyperlink ref="L116" r:id="rId9" xr:uid="{FA1B324F-1513-1343-9CCE-E23AFD154FFD}"/>
+    <hyperlink ref="L125" r:id="rId10" xr:uid="{C5AA4A87-0C8F-9A4C-974F-82A19E89F99C}"/>
+    <hyperlink ref="L113" r:id="rId11" xr:uid="{E1112DD8-8BE8-BD47-9002-F00DDA38363C}"/>
+    <hyperlink ref="L124" r:id="rId12" xr:uid="{4D774EC1-CC16-C24F-88F2-E9E20B8A8FC0}"/>
+    <hyperlink ref="L116:L117" r:id="rId13" display="https://freesound.org/s//" xr:uid="{5FB99E8B-AEFC-6A45-851E-E3C683DC5AC1}"/>
+    <hyperlink ref="L120" r:id="rId14" xr:uid="{E2EACC90-D2ED-AF4A-9302-ADD31B56C321}"/>
+    <hyperlink ref="L129" r:id="rId15" xr:uid="{13F37B0F-8A53-0B4F-8FE7-132D2186D638}"/>
+    <hyperlink ref="L112" r:id="rId16" xr:uid="{FA55BAC7-078A-8944-9FB5-42D7B041E218}"/>
     <hyperlink ref="H27" r:id="rId17" xr:uid="{4419FB35-315D-4DE4-9E5C-9B20E33A87FF}"/>
     <hyperlink ref="H22" r:id="rId18" xr:uid="{0ABC5FB6-8ADD-42B9-BF56-61A08BCA415C}"/>
     <hyperlink ref="H25" r:id="rId19" xr:uid="{189EA614-1A03-48EB-A1CB-FFAA9A4096B3}"/>
@@ -80151,22 +80189,23 @@
     <hyperlink ref="H28" r:id="rId42" xr:uid="{9A5F93C5-437C-488C-B3D7-22BAEE17A695}"/>
     <hyperlink ref="H26" r:id="rId43" xr:uid="{5BFD487A-D636-4DDD-B229-99F5CBDC0BE1}"/>
     <hyperlink ref="H23" r:id="rId44" xr:uid="{46A4F8EE-A89B-4A07-8D5D-E50FDDE0611E}"/>
-    <hyperlink ref="H90" r:id="rId45" xr:uid="{5B231739-C8F4-4D4E-B946-7A383ECBBB35}"/>
-    <hyperlink ref="H91" r:id="rId46" xr:uid="{6D8EAE93-D71D-4499-8388-86B77E8848FB}"/>
+    <hyperlink ref="H91" r:id="rId45" xr:uid="{5B231739-C8F4-4D4E-B946-7A383ECBBB35}"/>
+    <hyperlink ref="H92" r:id="rId46" xr:uid="{6D8EAE93-D71D-4499-8388-86B77E8848FB}"/>
     <hyperlink ref="H8" r:id="rId47" xr:uid="{2AE693E7-7449-4538-80A8-30A52F2A22F5}"/>
     <hyperlink ref="H7" r:id="rId48" xr:uid="{2FE1FB4D-693E-4830-8337-658393F68B92}"/>
     <hyperlink ref="H13" r:id="rId49" xr:uid="{DE9970E0-9BDB-45D1-93FA-3F6E016EDFDA}"/>
-    <hyperlink ref="L134" r:id="rId50" xr:uid="{643921F6-79ED-48CE-BC1D-7689B067914F}"/>
-    <hyperlink ref="L135" r:id="rId51" xr:uid="{5EB50EDD-6F80-49BD-9E94-C3F33E3E21E7}"/>
-    <hyperlink ref="L136" r:id="rId52" xr:uid="{3C3C642F-1CE9-4D06-A8F2-3D9A9371558D}"/>
-    <hyperlink ref="L102" r:id="rId53" xr:uid="{EAAF1456-48F9-4E52-8F61-7A6218C1AD87}"/>
-    <hyperlink ref="E145" r:id="rId54" xr:uid="{39B9B4E4-D455-4AB5-A866-4483392BA542}"/>
-    <hyperlink ref="D145" r:id="rId55" xr:uid="{53F0CD4A-267F-4EBB-A9F0-6B230EE74F90}"/>
-    <hyperlink ref="D152" r:id="rId56" xr:uid="{564063E4-ECA1-4F39-BC33-11B6AD635788}"/>
-    <hyperlink ref="E152" r:id="rId57" xr:uid="{71D99FD1-6BA5-4C5C-86BA-0F0C9A8663A2}"/>
+    <hyperlink ref="L135" r:id="rId50" xr:uid="{643921F6-79ED-48CE-BC1D-7689B067914F}"/>
+    <hyperlink ref="L136" r:id="rId51" xr:uid="{5EB50EDD-6F80-49BD-9E94-C3F33E3E21E7}"/>
+    <hyperlink ref="L137" r:id="rId52" xr:uid="{3C3C642F-1CE9-4D06-A8F2-3D9A9371558D}"/>
+    <hyperlink ref="L103" r:id="rId53" xr:uid="{EAAF1456-48F9-4E52-8F61-7A6218C1AD87}"/>
+    <hyperlink ref="E146" r:id="rId54" xr:uid="{39B9B4E4-D455-4AB5-A866-4483392BA542}"/>
+    <hyperlink ref="D146" r:id="rId55" xr:uid="{53F0CD4A-267F-4EBB-A9F0-6B230EE74F90}"/>
+    <hyperlink ref="D153" r:id="rId56" xr:uid="{564063E4-ECA1-4F39-BC33-11B6AD635788}"/>
+    <hyperlink ref="E153" r:id="rId57" xr:uid="{71D99FD1-6BA5-4C5C-86BA-0F0C9A8663A2}"/>
+    <hyperlink ref="H41" r:id="rId58" xr:uid="{6BF5EAAA-3B1C-4BD6-A82F-83B009FDB86E}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId58"/>
+  <pageSetup orientation="portrait" r:id="rId59"/>
 </worksheet>
 </file>
 
@@ -81843,8 +81882,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B7BCD6B9-C154-4F9D-B8BC-4D842A94058B}">
   <dimension ref="A1:AX30"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+    <sheetView tabSelected="1" topLeftCell="O1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="U24" sqref="U24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -82141,14 +82180,14 @@
         <v>606</v>
       </c>
       <c r="M6" s="55">
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="N6" s="55" t="s">
-        <v>487</v>
+        <v>6450</v>
       </c>
       <c r="O6" s="55" t="str">
         <f>Y6&amp;M6&amp;" };"</f>
-        <v>/* 1 SOUND */ { 4, 4, 5, 4, 2, 3 };</v>
+        <v>/* 1 SOUND */ { 4, 4, 5, 4, 2, 9 };</v>
       </c>
       <c r="T6" t="str">
         <f>"/* "&amp;A6&amp;" "&amp;B6&amp;" */ { "</f>
@@ -82889,7 +82928,7 @@
         <v>2</v>
       </c>
       <c r="U23">
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="V23">
         <v>1</v>
@@ -82953,47 +82992,47 @@
       </c>
       <c r="AN23" t="str">
         <f t="shared" ref="AN23:AN24" si="18">AM23&amp;", "&amp;U23</f>
-        <v>/* 1 SOUND */    4, 4, 5, 4, 2, 3</v>
+        <v>/* 1 SOUND */    4, 4, 5, 4, 2, 9</v>
       </c>
       <c r="AO23" t="str">
         <f t="shared" ref="AO23:AO24" si="19">AN23&amp;", "&amp;V23</f>
-        <v>/* 1 SOUND */    4, 4, 5, 4, 2, 3, 1</v>
+        <v>/* 1 SOUND */    4, 4, 5, 4, 2, 9, 1</v>
       </c>
       <c r="AP23" t="str">
         <f t="shared" ref="AP23:AP24" si="20">AO23&amp;", "&amp;W23</f>
-        <v>/* 1 SOUND */    4, 4, 5, 4, 2, 3, 1, 1</v>
+        <v>/* 1 SOUND */    4, 4, 5, 4, 2, 9, 1, 1</v>
       </c>
       <c r="AQ23" t="str">
         <f t="shared" ref="AQ23:AQ24" si="21">AP23&amp;", "&amp;X23</f>
-        <v>/* 1 SOUND */    4, 4, 5, 4, 2, 3, 1, 1, 1</v>
+        <v>/* 1 SOUND */    4, 4, 5, 4, 2, 9, 1, 1, 1</v>
       </c>
       <c r="AR23" t="str">
         <f t="shared" ref="AR23:AR24" si="22">AQ23&amp;", "&amp;Y23</f>
-        <v>/* 1 SOUND */    4, 4, 5, 4, 2, 3, 1, 1, 1, 1</v>
+        <v>/* 1 SOUND */    4, 4, 5, 4, 2, 9, 1, 1, 1, 1</v>
       </c>
       <c r="AS23" t="str">
         <f t="shared" ref="AS23:AS24" si="23">AR23&amp;", "&amp;Z23</f>
-        <v>/* 1 SOUND */    4, 4, 5, 4, 2, 3, 1, 1, 1, 1, 1</v>
+        <v>/* 1 SOUND */    4, 4, 5, 4, 2, 9, 1, 1, 1, 1, 1</v>
       </c>
       <c r="AT23" t="str">
         <f t="shared" ref="AT23:AT24" si="24">AS23&amp;", "&amp;AA23</f>
-        <v>/* 1 SOUND */    4, 4, 5, 4, 2, 3, 1, 1, 1, 1, 1, 1</v>
+        <v>/* 1 SOUND */    4, 4, 5, 4, 2, 9, 1, 1, 1, 1, 1, 1</v>
       </c>
       <c r="AU23" t="str">
         <f t="shared" ref="AU23:AU24" si="25">AT23&amp;", "&amp;AB23</f>
-        <v>/* 1 SOUND */    4, 4, 5, 4, 2, 3, 1, 1, 1, 1, 1, 1, 1</v>
+        <v>/* 1 SOUND */    4, 4, 5, 4, 2, 9, 1, 1, 1, 1, 1, 1, 1</v>
       </c>
       <c r="AV23" t="str">
         <f t="shared" ref="AV23:AV24" si="26">AU23&amp;", "&amp;AC23</f>
-        <v>/* 1 SOUND */    4, 4, 5, 4, 2, 3, 1, 1, 1, 1, 1, 1, 1, 1</v>
+        <v>/* 1 SOUND */    4, 4, 5, 4, 2, 9, 1, 1, 1, 1, 1, 1, 1, 1</v>
       </c>
       <c r="AW23" t="str">
         <f t="shared" ref="AW23:AW24" si="27">AV23&amp;", "&amp;AD23</f>
-        <v>/* 1 SOUND */    4, 4, 5, 4, 2, 3, 1, 1, 1, 1, 1, 1, 1, 1, 1</v>
+        <v>/* 1 SOUND */    4, 4, 5, 4, 2, 9, 1, 1, 1, 1, 1, 1, 1, 1, 1</v>
       </c>
       <c r="AX23" t="str">
         <f t="shared" ref="AX23:AX24" si="28">AW23&amp;", "&amp;AE23</f>
-        <v>/* 1 SOUND */    4, 4, 5, 4, 2, 3, 1, 1, 1, 1, 1, 1, 1, 1, 1, 25</v>
+        <v>/* 1 SOUND */    4, 4, 5, 4, 2, 9, 1, 1, 1, 1, 1, 1, 1, 1, 1, 25</v>
       </c>
     </row>
     <row r="24" spans="16:50">

</xml_diff>

<commit_message>
for some reason Cassini Saturn sounds don't play on YX5200
</commit_message>
<xml_diff>
--- a/RBG_arduino/StateTable_minimal.xlsx
+++ b/RBG_arduino/StateTable_minimal.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub-Mark-MDO47\RubberBandGun\RBG_arduino\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52A0A78D-35AD-478E-8CC7-5141C370236B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C154D99F-C903-48C3-B67E-E452CE88EEFA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21840" activeTab="6" xr2:uid="{CCADFEE4-B0E1-4363-9617-1683960BED03}"/>
+    <workbookView xWindow="11805" yWindow="3780" windowWidth="25965" windowHeight="16875" activeTab="6" xr2:uid="{CCADFEE4-B0E1-4363-9617-1683960BED03}"/>
   </bookViews>
   <sheets>
     <sheet name="StateTable" sheetId="1" r:id="rId1"/>
@@ -19768,10 +19768,10 @@
     <t>http://www-pw.physics.uiowa.edu/space-audio/cassini/SKR1/SKR-03-324.wav</t>
   </si>
   <si>
-    <t>Cassini sounds of Saturn radio waves</t>
-  </si>
-  <si>
     <t>NASA Cassini University of Iowa</t>
+  </si>
+  <si>
+    <t>Cassini sounds of Saturn radio waves. THIS SOUND DOES NOT WORK FOR SOME REASON</t>
   </si>
 </sst>
 </file>
@@ -20391,15 +20391,6 @@
       <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="164" fontId="19" fillId="10" borderId="3" xfId="8" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="11" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
     </xf>
@@ -20411,6 +20402,15 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="11" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="10">
@@ -24052,7 +24052,7 @@
       </c>
     </row>
     <row r="129" spans="1:12" ht="45">
-      <c r="A129" s="91" t="s">
+      <c r="A129" s="88" t="s">
         <v>6036</v>
       </c>
       <c r="B129" s="63" t="s">
@@ -24461,7 +24461,7 @@
     </row>
     <row r="152" spans="1:11">
       <c r="K152" s="9" t="str">
-        <f t="shared" ref="K146:K162" si="11">IF(LEN(C152),VLOOKUP(C152,mROW,3,FALSE),"")</f>
+        <f t="shared" ref="K152:K162" si="11">IF(LEN(C152),VLOOKUP(C152,mROW,3,FALSE),"")</f>
         <v/>
       </c>
     </row>
@@ -76472,8 +76472,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A827A58D-C8A4-4858-A89B-E853C083564F}">
   <dimension ref="A1:AK190"/>
   <sheetViews>
-    <sheetView topLeftCell="A23" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D44" sqref="D44"/>
+    <sheetView topLeftCell="A30" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C35" sqref="C35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
@@ -77647,7 +77647,7 @@
         <v>642</v>
       </c>
     </row>
-    <row r="41" spans="1:11" ht="20.25">
+    <row r="41" spans="1:11" ht="30">
       <c r="A41" s="55" t="s">
         <v>455</v>
       </c>
@@ -77658,7 +77658,7 @@
         <v>6450</v>
       </c>
       <c r="D41" s="52" t="s">
-        <v>6452</v>
+        <v>6453</v>
       </c>
       <c r="E41" s="52" t="s">
         <v>455</v>
@@ -77667,7 +77667,7 @@
         <v>594</v>
       </c>
       <c r="G41" s="57" t="s">
-        <v>6453</v>
+        <v>6452</v>
       </c>
       <c r="H41" s="54" t="s">
         <v>6451</v>
@@ -79030,10 +79030,10 @@
       <c r="B78" s="70">
         <v>109</v>
       </c>
-      <c r="C78" s="92" t="s">
+      <c r="C78" s="89" t="s">
         <v>5542</v>
       </c>
-      <c r="D78" s="93" t="s">
+      <c r="D78" s="90" t="s">
         <v>5539</v>
       </c>
       <c r="E78" s="69" t="s">
@@ -79061,31 +79061,31 @@
       </c>
     </row>
     <row r="79" spans="1:11">
-      <c r="A79" s="91" t="s">
+      <c r="A79" s="88" t="s">
         <v>694</v>
       </c>
-      <c r="B79" s="91" t="s">
+      <c r="B79" s="88" t="s">
         <v>694</v>
       </c>
-      <c r="C79" s="91" t="s">
+      <c r="C79" s="88" t="s">
         <v>694</v>
       </c>
-      <c r="D79" s="91" t="s">
+      <c r="D79" s="88" t="s">
         <v>694</v>
       </c>
-      <c r="E79" s="91" t="s">
+      <c r="E79" s="88" t="s">
         <v>694</v>
       </c>
-      <c r="F79" s="91" t="s">
+      <c r="F79" s="88" t="s">
         <v>694</v>
       </c>
-      <c r="G79" s="91" t="s">
+      <c r="G79" s="88" t="s">
         <v>694</v>
       </c>
-      <c r="H79" s="91" t="s">
+      <c r="H79" s="88" t="s">
         <v>694</v>
       </c>
-      <c r="I79" s="91" t="s">
+      <c r="I79" s="88" t="s">
         <v>694</v>
       </c>
     </row>
@@ -80106,7 +80106,7 @@
       <c r="B176">
         <v>1</v>
       </c>
-      <c r="C176" s="90" t="s">
+      <c r="C176" s="87" t="s">
         <v>6005</v>
       </c>
     </row>
@@ -80114,7 +80114,7 @@
       <c r="B177">
         <v>2</v>
       </c>
-      <c r="C177" s="90" t="s">
+      <c r="C177" s="87" t="s">
         <v>4443</v>
       </c>
     </row>
@@ -81883,7 +81883,7 @@
   <dimension ref="A1:AX30"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="O1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="U24" sqref="U24"/>
+      <selection activeCell="V34" sqref="V34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -81948,38 +81948,38 @@
       <c r="N1" s="81" t="s">
         <v>4482</v>
       </c>
-      <c r="O1" s="87" t="s">
+      <c r="O1" s="91" t="s">
         <v>4485</v>
       </c>
     </row>
     <row r="2" spans="1:25" ht="16.5" thickTop="1" thickBot="1">
       <c r="A2" s="83"/>
       <c r="B2" s="59"/>
-      <c r="C2" s="87" t="s">
+      <c r="C2" s="91" t="s">
         <v>45</v>
       </c>
-      <c r="D2" s="87"/>
-      <c r="E2" s="87" t="s">
+      <c r="D2" s="91"/>
+      <c r="E2" s="91" t="s">
         <v>44</v>
       </c>
-      <c r="F2" s="87"/>
-      <c r="G2" s="87" t="s">
+      <c r="F2" s="91"/>
+      <c r="G2" s="91" t="s">
         <v>33</v>
       </c>
-      <c r="H2" s="87"/>
-      <c r="I2" s="87" t="s">
+      <c r="H2" s="91"/>
+      <c r="I2" s="91" t="s">
         <v>34</v>
       </c>
-      <c r="J2" s="87"/>
-      <c r="K2" s="87" t="s">
+      <c r="J2" s="91"/>
+      <c r="K2" s="91" t="s">
         <v>32</v>
       </c>
-      <c r="L2" s="87"/>
-      <c r="M2" s="87" t="s">
+      <c r="L2" s="91"/>
+      <c r="M2" s="91" t="s">
         <v>601</v>
       </c>
-      <c r="N2" s="87"/>
-      <c r="O2" s="88"/>
+      <c r="N2" s="91"/>
+      <c r="O2" s="92"/>
     </row>
     <row r="3" spans="1:25" ht="16.5" thickTop="1" thickBot="1">
       <c r="A3" s="59">
@@ -82180,14 +82180,14 @@
         <v>606</v>
       </c>
       <c r="M6" s="55">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="N6" s="55" t="s">
-        <v>6450</v>
+        <v>487</v>
       </c>
       <c r="O6" s="55" t="str">
         <f>Y6&amp;M6&amp;" };"</f>
-        <v>/* 1 SOUND */ { 4, 4, 5, 4, 2, 9 };</v>
+        <v>/* 1 SOUND */ { 4, 4, 5, 4, 2, 3 };</v>
       </c>
       <c r="T6" t="str">
         <f>"/* "&amp;A6&amp;" "&amp;B6&amp;" */ { "</f>
@@ -82928,7 +82928,7 @@
         <v>2</v>
       </c>
       <c r="U23">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="V23">
         <v>1</v>
@@ -82992,47 +82992,47 @@
       </c>
       <c r="AN23" t="str">
         <f t="shared" ref="AN23:AN24" si="18">AM23&amp;", "&amp;U23</f>
-        <v>/* 1 SOUND */    4, 4, 5, 4, 2, 9</v>
+        <v>/* 1 SOUND */    4, 4, 5, 4, 2, 3</v>
       </c>
       <c r="AO23" t="str">
         <f t="shared" ref="AO23:AO24" si="19">AN23&amp;", "&amp;V23</f>
-        <v>/* 1 SOUND */    4, 4, 5, 4, 2, 9, 1</v>
+        <v>/* 1 SOUND */    4, 4, 5, 4, 2, 3, 1</v>
       </c>
       <c r="AP23" t="str">
         <f t="shared" ref="AP23:AP24" si="20">AO23&amp;", "&amp;W23</f>
-        <v>/* 1 SOUND */    4, 4, 5, 4, 2, 9, 1, 1</v>
+        <v>/* 1 SOUND */    4, 4, 5, 4, 2, 3, 1, 1</v>
       </c>
       <c r="AQ23" t="str">
         <f t="shared" ref="AQ23:AQ24" si="21">AP23&amp;", "&amp;X23</f>
-        <v>/* 1 SOUND */    4, 4, 5, 4, 2, 9, 1, 1, 1</v>
+        <v>/* 1 SOUND */    4, 4, 5, 4, 2, 3, 1, 1, 1</v>
       </c>
       <c r="AR23" t="str">
         <f t="shared" ref="AR23:AR24" si="22">AQ23&amp;", "&amp;Y23</f>
-        <v>/* 1 SOUND */    4, 4, 5, 4, 2, 9, 1, 1, 1, 1</v>
+        <v>/* 1 SOUND */    4, 4, 5, 4, 2, 3, 1, 1, 1, 1</v>
       </c>
       <c r="AS23" t="str">
         <f t="shared" ref="AS23:AS24" si="23">AR23&amp;", "&amp;Z23</f>
-        <v>/* 1 SOUND */    4, 4, 5, 4, 2, 9, 1, 1, 1, 1, 1</v>
+        <v>/* 1 SOUND */    4, 4, 5, 4, 2, 3, 1, 1, 1, 1, 1</v>
       </c>
       <c r="AT23" t="str">
         <f t="shared" ref="AT23:AT24" si="24">AS23&amp;", "&amp;AA23</f>
-        <v>/* 1 SOUND */    4, 4, 5, 4, 2, 9, 1, 1, 1, 1, 1, 1</v>
+        <v>/* 1 SOUND */    4, 4, 5, 4, 2, 3, 1, 1, 1, 1, 1, 1</v>
       </c>
       <c r="AU23" t="str">
         <f t="shared" ref="AU23:AU24" si="25">AT23&amp;", "&amp;AB23</f>
-        <v>/* 1 SOUND */    4, 4, 5, 4, 2, 9, 1, 1, 1, 1, 1, 1, 1</v>
+        <v>/* 1 SOUND */    4, 4, 5, 4, 2, 3, 1, 1, 1, 1, 1, 1, 1</v>
       </c>
       <c r="AV23" t="str">
         <f t="shared" ref="AV23:AV24" si="26">AU23&amp;", "&amp;AC23</f>
-        <v>/* 1 SOUND */    4, 4, 5, 4, 2, 9, 1, 1, 1, 1, 1, 1, 1, 1</v>
+        <v>/* 1 SOUND */    4, 4, 5, 4, 2, 3, 1, 1, 1, 1, 1, 1, 1, 1</v>
       </c>
       <c r="AW23" t="str">
         <f t="shared" ref="AW23:AW24" si="27">AV23&amp;", "&amp;AD23</f>
-        <v>/* 1 SOUND */    4, 4, 5, 4, 2, 9, 1, 1, 1, 1, 1, 1, 1, 1, 1</v>
+        <v>/* 1 SOUND */    4, 4, 5, 4, 2, 3, 1, 1, 1, 1, 1, 1, 1, 1, 1</v>
       </c>
       <c r="AX23" t="str">
         <f t="shared" ref="AX23:AX24" si="28">AW23&amp;", "&amp;AE23</f>
-        <v>/* 1 SOUND */    4, 4, 5, 4, 2, 9, 1, 1, 1, 1, 1, 1, 1, 1, 1, 25</v>
+        <v>/* 1 SOUND */    4, 4, 5, 4, 2, 3, 1, 1, 1, 1, 1, 1, 1, 1, 1, 25</v>
       </c>
     </row>
     <row r="24" spans="16:50">
@@ -83759,10 +83759,10 @@
       <c r="F19" t="s">
         <v>5994</v>
       </c>
-      <c r="K19" s="89" t="s">
+      <c r="K19" s="93" t="s">
         <v>6004</v>
       </c>
-      <c r="L19" s="89"/>
+      <c r="L19" s="93"/>
     </row>
     <row r="20" spans="2:12" ht="18">
       <c r="B20">

</xml_diff>

<commit_message>
needed to resample Cassini Saturn sounds to standard bit rate
</commit_message>
<xml_diff>
--- a/RBG_arduino/StateTable_minimal.xlsx
+++ b/RBG_arduino/StateTable_minimal.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub-Mark-MDO47\RubberBandGun\RBG_arduino\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C154D99F-C903-48C3-B67E-E452CE88EEFA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E75F04AE-B663-4744-8CBA-6016831F2A98}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="11805" yWindow="3780" windowWidth="25965" windowHeight="16875" activeTab="6" xr2:uid="{CCADFEE4-B0E1-4363-9617-1683960BED03}"/>
   </bookViews>
@@ -19771,7 +19771,7 @@
     <t>NASA Cassini University of Iowa</t>
   </si>
   <si>
-    <t>Cassini sounds of Saturn radio waves. THIS SOUND DOES NOT WORK FOR SOME REASON</t>
+    <t>Cassini sounds of Saturn radio waves. Needed to resample to standard bitrate to make this work</t>
   </si>
 </sst>
 </file>
@@ -76473,7 +76473,7 @@
   <dimension ref="A1:AK190"/>
   <sheetViews>
     <sheetView topLeftCell="A30" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C35" sqref="C35"/>
+      <selection activeCell="C41" sqref="C41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
@@ -81882,8 +81882,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B7BCD6B9-C154-4F9D-B8BC-4D842A94058B}">
   <dimension ref="A1:AX30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="O1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="V34" sqref="V34"/>
+    <sheetView tabSelected="1" topLeftCell="N1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="U24" sqref="U24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -82180,14 +82180,14 @@
         <v>606</v>
       </c>
       <c r="M6" s="55">
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="N6" s="55" t="s">
-        <v>487</v>
+        <v>6450</v>
       </c>
       <c r="O6" s="55" t="str">
         <f>Y6&amp;M6&amp;" };"</f>
-        <v>/* 1 SOUND */ { 4, 4, 5, 4, 2, 3 };</v>
+        <v>/* 1 SOUND */ { 4, 4, 5, 4, 2, 9 };</v>
       </c>
       <c r="T6" t="str">
         <f>"/* "&amp;A6&amp;" "&amp;B6&amp;" */ { "</f>
@@ -82928,7 +82928,7 @@
         <v>2</v>
       </c>
       <c r="U23">
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="V23">
         <v>1</v>
@@ -82992,47 +82992,47 @@
       </c>
       <c r="AN23" t="str">
         <f t="shared" ref="AN23:AN24" si="18">AM23&amp;", "&amp;U23</f>
-        <v>/* 1 SOUND */    4, 4, 5, 4, 2, 3</v>
+        <v>/* 1 SOUND */    4, 4, 5, 4, 2, 9</v>
       </c>
       <c r="AO23" t="str">
         <f t="shared" ref="AO23:AO24" si="19">AN23&amp;", "&amp;V23</f>
-        <v>/* 1 SOUND */    4, 4, 5, 4, 2, 3, 1</v>
+        <v>/* 1 SOUND */    4, 4, 5, 4, 2, 9, 1</v>
       </c>
       <c r="AP23" t="str">
         <f t="shared" ref="AP23:AP24" si="20">AO23&amp;", "&amp;W23</f>
-        <v>/* 1 SOUND */    4, 4, 5, 4, 2, 3, 1, 1</v>
+        <v>/* 1 SOUND */    4, 4, 5, 4, 2, 9, 1, 1</v>
       </c>
       <c r="AQ23" t="str">
         <f t="shared" ref="AQ23:AQ24" si="21">AP23&amp;", "&amp;X23</f>
-        <v>/* 1 SOUND */    4, 4, 5, 4, 2, 3, 1, 1, 1</v>
+        <v>/* 1 SOUND */    4, 4, 5, 4, 2, 9, 1, 1, 1</v>
       </c>
       <c r="AR23" t="str">
         <f t="shared" ref="AR23:AR24" si="22">AQ23&amp;", "&amp;Y23</f>
-        <v>/* 1 SOUND */    4, 4, 5, 4, 2, 3, 1, 1, 1, 1</v>
+        <v>/* 1 SOUND */    4, 4, 5, 4, 2, 9, 1, 1, 1, 1</v>
       </c>
       <c r="AS23" t="str">
         <f t="shared" ref="AS23:AS24" si="23">AR23&amp;", "&amp;Z23</f>
-        <v>/* 1 SOUND */    4, 4, 5, 4, 2, 3, 1, 1, 1, 1, 1</v>
+        <v>/* 1 SOUND */    4, 4, 5, 4, 2, 9, 1, 1, 1, 1, 1</v>
       </c>
       <c r="AT23" t="str">
         <f t="shared" ref="AT23:AT24" si="24">AS23&amp;", "&amp;AA23</f>
-        <v>/* 1 SOUND */    4, 4, 5, 4, 2, 3, 1, 1, 1, 1, 1, 1</v>
+        <v>/* 1 SOUND */    4, 4, 5, 4, 2, 9, 1, 1, 1, 1, 1, 1</v>
       </c>
       <c r="AU23" t="str">
         <f t="shared" ref="AU23:AU24" si="25">AT23&amp;", "&amp;AB23</f>
-        <v>/* 1 SOUND */    4, 4, 5, 4, 2, 3, 1, 1, 1, 1, 1, 1, 1</v>
+        <v>/* 1 SOUND */    4, 4, 5, 4, 2, 9, 1, 1, 1, 1, 1, 1, 1</v>
       </c>
       <c r="AV23" t="str">
         <f t="shared" ref="AV23:AV24" si="26">AU23&amp;", "&amp;AC23</f>
-        <v>/* 1 SOUND */    4, 4, 5, 4, 2, 3, 1, 1, 1, 1, 1, 1, 1, 1</v>
+        <v>/* 1 SOUND */    4, 4, 5, 4, 2, 9, 1, 1, 1, 1, 1, 1, 1, 1</v>
       </c>
       <c r="AW23" t="str">
         <f t="shared" ref="AW23:AW24" si="27">AV23&amp;", "&amp;AD23</f>
-        <v>/* 1 SOUND */    4, 4, 5, 4, 2, 3, 1, 1, 1, 1, 1, 1, 1, 1, 1</v>
+        <v>/* 1 SOUND */    4, 4, 5, 4, 2, 9, 1, 1, 1, 1, 1, 1, 1, 1, 1</v>
       </c>
       <c r="AX23" t="str">
         <f t="shared" ref="AX23:AX24" si="28">AW23&amp;", "&amp;AE23</f>
-        <v>/* 1 SOUND */    4, 4, 5, 4, 2, 3, 1, 1, 1, 1, 1, 1, 1, 1, 1, 25</v>
+        <v>/* 1 SOUND */    4, 4, 5, 4, 2, 9, 1, 1, 1, 1, 1, 1, 1, 1, 1, 25</v>
       </c>
     </row>
     <row r="24" spans="16:50">

</xml_diff>

<commit_message>
go back to power-on after shooting
</commit_message>
<xml_diff>
--- a/RBG_arduino/StateTable_minimal.xlsx
+++ b/RBG_arduino/StateTable_minimal.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub-Mark-MDO47\RubberBandGun\RBG_arduino\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E75F04AE-B663-4744-8CBA-6016831F2A98}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9C5EBDE-090F-4E5A-BA6C-3FB26E4FDE3F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11805" yWindow="3780" windowWidth="25965" windowHeight="16875" activeTab="6" xr2:uid="{CCADFEE4-B0E1-4363-9617-1683960BED03}"/>
+    <workbookView xWindow="11805" yWindow="3780" windowWidth="25965" windowHeight="16875" xr2:uid="{CCADFEE4-B0E1-4363-9617-1683960BED03}"/>
   </bookViews>
   <sheets>
     <sheet name="StateTable" sheetId="1" r:id="rId1"/>
@@ -49,7 +49,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8753" uniqueCount="6454">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8754" uniqueCount="6455">
   <si>
     <t>trigOnly</t>
   </si>
@@ -19772,6 +19772,9 @@
   </si>
   <si>
     <t>Cassini sounds of Saturn radio waves. Needed to resample to standard bitrate to make this work</t>
+  </si>
+  <si>
+    <t>#define mROW_MENU_CLOSED 12</t>
   </si>
 </sst>
 </file>
@@ -20742,9 +20745,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{90E8DFC6-94F4-4A82-A874-2F16F2CF0145}">
   <dimension ref="A1:AB162"/>
   <sheetViews>
-    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A119" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D30" sqref="D30"/>
+    <sheetView tabSelected="1" topLeftCell="K1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="X37" sqref="X37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
@@ -21454,7 +21457,7 @@
         <v>35</v>
       </c>
       <c r="C21" s="34" t="s">
-        <v>412</v>
+        <v>413</v>
       </c>
       <c r="D21" s="33" t="s">
         <v>601</v>
@@ -21473,7 +21476,7 @@
       <c r="J21" s="32"/>
       <c r="K21" s="9" t="str">
         <f t="shared" si="0"/>
-        <v>#define mROW_MENU_CLOSED 11</v>
+        <v>#define mROW_MENU_OPEN 9</v>
       </c>
       <c r="V21" t="s">
         <v>4498</v>
@@ -21537,7 +21540,7 @@
       <c r="J23" s="32"/>
       <c r="K23" s="9" t="str">
         <f t="shared" si="0"/>
-        <v>#define mROW_MENU_CLOSED 11</v>
+        <v>#define mROW_MENU_CLOSED 12</v>
       </c>
       <c r="V23" t="s">
         <v>658</v>
@@ -21574,7 +21577,7 @@
       <c r="J24" s="32"/>
       <c r="K24" s="9" t="str">
         <f t="shared" si="0"/>
-        <v>#define mROW_MENU_CLOSED 11</v>
+        <v>#define mROW_MENU_CLOSED 12</v>
       </c>
       <c r="V24" t="s">
         <v>656</v>
@@ -21611,7 +21614,7 @@
       <c r="J25" s="32"/>
       <c r="K25" s="9" t="str">
         <f t="shared" si="0"/>
-        <v>#define mROW_MENU_CLOSED 11</v>
+        <v>#define mROW_MENU_CLOSED 12</v>
       </c>
       <c r="V25" t="s">
         <v>655</v>
@@ -21843,7 +21846,7 @@
       <c r="E34" s="3"/>
       <c r="I34" s="9"/>
       <c r="J34" s="9" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="K34" s="9" t="str">
         <f t="shared" si="0"/>
@@ -21912,10 +21915,10 @@
         <v>412</v>
       </c>
       <c r="W36">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="X36" t="s">
-        <v>618</v>
+        <v>6454</v>
       </c>
     </row>
     <row r="37" spans="1:28">
@@ -22448,7 +22451,7 @@
         <v>708</v>
       </c>
       <c r="I59" s="61" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="J59" s="9"/>
       <c r="K59" s="9" t="str">
@@ -22824,7 +22827,7 @@
         <v>708</v>
       </c>
       <c r="I78" s="61" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="K78" s="9" t="str">
         <f t="shared" si="1"/>
@@ -23130,6 +23133,9 @@
       </c>
     </row>
     <row r="91" spans="1:24">
+      <c r="B91" t="s">
+        <v>602</v>
+      </c>
       <c r="C91" s="12" t="s">
         <v>656</v>
       </c>
@@ -23137,7 +23143,7 @@
         <v>708</v>
       </c>
       <c r="I91" s="61" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="K91" s="9" t="str">
         <f t="shared" si="1"/>
@@ -23602,7 +23608,7 @@
         <v>708</v>
       </c>
       <c r="I109" s="61" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="K109" s="9" t="str">
         <f t="shared" si="1"/>
@@ -24156,7 +24162,7 @@
         <v>708</v>
       </c>
       <c r="I133" s="61" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="K133" s="9" t="str">
         <f t="shared" si="10"/>
@@ -76472,8 +76478,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A827A58D-C8A4-4858-A89B-E853C083564F}">
   <dimension ref="A1:AK190"/>
   <sheetViews>
-    <sheetView topLeftCell="A30" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C41" sqref="C41"/>
+    <sheetView topLeftCell="A45" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="D58" sqref="D58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
@@ -80215,7 +80221,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C58" sqref="C58"/>
+      <selection pane="bottomLeft" activeCell="C51" sqref="C51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -81882,8 +81888,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B7BCD6B9-C154-4F9D-B8BC-4D842A94058B}">
   <dimension ref="A1:AX30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="N1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="U24" sqref="U24"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="A24" sqref="A24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>

</xml_diff>

<commit_message>
change green button for red button
</commit_message>
<xml_diff>
--- a/RBG_arduino/StateTable_minimal.xlsx
+++ b/RBG_arduino/StateTable_minimal.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub-Mark-MDO47\RubberBandGun\RBG_arduino\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56DE7CFB-E3E3-47A1-8223-D3817EE2F246}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B3EF6FD-DC67-497D-98B8-23CDA07EA310}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21840" xr2:uid="{CCADFEE4-B0E1-4363-9617-1683960BED03}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21840" activeTab="4" xr2:uid="{CCADFEE4-B0E1-4363-9617-1683960BED03}"/>
   </bookViews>
   <sheets>
     <sheet name="StateTable" sheetId="1" r:id="rId1"/>
@@ -20066,7 +20066,7 @@
     <xf numFmtId="0" fontId="19" fillId="10" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="10" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="96">
+  <cellXfs count="95">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -20267,17 +20267,14 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="2" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="19" fillId="10" borderId="3" xfId="8" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="11" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="10" borderId="3" xfId="8" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="3" xfId="5" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="10">
@@ -20609,7 +20606,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{90E8DFC6-94F4-4A82-A874-2F16F2CF0145}">
   <dimension ref="A1:AB162"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="C10" sqref="C10"/>
     </sheetView>
@@ -76342,8 +76339,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A827A58D-C8A4-4858-A89B-E853C083564F}">
   <dimension ref="A1:AK192"/>
   <sheetViews>
-    <sheetView topLeftCell="A74" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="H77" sqref="H77"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A46" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D77" sqref="D77"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
@@ -77590,7 +77588,7 @@
       <c r="C43" s="50" t="s">
         <v>669</v>
       </c>
-      <c r="D43" s="94" t="s">
+      <c r="D43" s="92" t="s">
         <v>6420</v>
       </c>
       <c r="E43" s="56" t="s">
@@ -77627,7 +77625,7 @@
       <c r="C44" s="50" t="s">
         <v>670</v>
       </c>
-      <c r="D44" s="94" t="s">
+      <c r="D44" s="92" t="s">
         <v>6421</v>
       </c>
       <c r="E44" s="56" t="s">
@@ -77664,7 +77662,7 @@
       <c r="C45" s="50" t="s">
         <v>671</v>
       </c>
-      <c r="D45" s="94" t="s">
+      <c r="D45" s="92" t="s">
         <v>6422</v>
       </c>
       <c r="E45" s="56" t="s">
@@ -77701,7 +77699,7 @@
       <c r="C46" s="50" t="s">
         <v>4431</v>
       </c>
-      <c r="D46" s="94" t="s">
+      <c r="D46" s="92" t="s">
         <v>6423</v>
       </c>
       <c r="E46" s="56" t="s">
@@ -78676,7 +78674,7 @@
       <c r="C72" s="75" t="s">
         <v>4458</v>
       </c>
-      <c r="D72" s="95" t="s">
+      <c r="D72" s="92" t="s">
         <v>6424</v>
       </c>
       <c r="E72" s="56" t="s">
@@ -78714,7 +78712,7 @@
       <c r="C73" s="75" t="s">
         <v>4459</v>
       </c>
-      <c r="D73" s="95" t="s">
+      <c r="D73" s="92" t="s">
         <v>6425</v>
       </c>
       <c r="E73" s="56" t="s">
@@ -78752,7 +78750,7 @@
       <c r="C74" s="75" t="s">
         <v>4460</v>
       </c>
-      <c r="D74" s="95" t="s">
+      <c r="D74" s="92" t="s">
         <v>6426</v>
       </c>
       <c r="E74" s="56" t="s">
@@ -78866,7 +78864,7 @@
       <c r="C77" s="75" t="s">
         <v>5990</v>
       </c>
-      <c r="D77" s="94" t="s">
+      <c r="D77" s="92" t="s">
         <v>6427</v>
       </c>
       <c r="E77" s="56" t="s">
@@ -78942,7 +78940,7 @@
       <c r="C79" s="75" t="s">
         <v>5524</v>
       </c>
-      <c r="D79" s="94" t="s">
+      <c r="D79" s="92" t="s">
         <v>6428</v>
       </c>
       <c r="E79" s="56" t="s">
@@ -81894,38 +81892,38 @@
       <c r="N1" s="81" t="s">
         <v>4471</v>
       </c>
-      <c r="O1" s="92" t="s">
+      <c r="O1" s="93" t="s">
         <v>4474</v>
       </c>
     </row>
     <row r="2" spans="1:25" ht="16.5" thickTop="1" thickBot="1">
       <c r="A2" s="83"/>
       <c r="B2" s="59"/>
-      <c r="C2" s="92" t="s">
+      <c r="C2" s="93" t="s">
         <v>45</v>
       </c>
-      <c r="D2" s="92"/>
-      <c r="E2" s="92" t="s">
+      <c r="D2" s="93"/>
+      <c r="E2" s="93" t="s">
         <v>44</v>
       </c>
-      <c r="F2" s="92"/>
-      <c r="G2" s="92" t="s">
+      <c r="F2" s="93"/>
+      <c r="G2" s="93" t="s">
         <v>33</v>
       </c>
-      <c r="H2" s="92"/>
-      <c r="I2" s="92" t="s">
+      <c r="H2" s="93"/>
+      <c r="I2" s="93" t="s">
         <v>34</v>
       </c>
-      <c r="J2" s="92"/>
-      <c r="K2" s="92" t="s">
+      <c r="J2" s="93"/>
+      <c r="K2" s="93" t="s">
         <v>32</v>
       </c>
-      <c r="L2" s="92"/>
-      <c r="M2" s="92" t="s">
+      <c r="L2" s="93"/>
+      <c r="M2" s="93" t="s">
         <v>601</v>
       </c>
-      <c r="N2" s="92"/>
-      <c r="O2" s="93"/>
+      <c r="N2" s="93"/>
+      <c r="O2" s="94"/>
     </row>
     <row r="3" spans="1:25" ht="16.5" thickTop="1" thickBot="1">
       <c r="A3" s="59">

</xml_diff>

<commit_message>
minor update plus some comments
</commit_message>
<xml_diff>
--- a/RBG_arduino/StateTable_minimal.xlsx
+++ b/RBG_arduino/StateTable_minimal.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub-Mark-MDO47\RubberBandGun\RBG_arduino\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B3EF6FD-DC67-497D-98B8-23CDA07EA310}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1E9580D-3C64-4DBF-805E-C384C85D80F3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21840" activeTab="4" xr2:uid="{CCADFEE4-B0E1-4363-9617-1683960BED03}"/>
+    <workbookView xWindow="2640" yWindow="7725" windowWidth="15795" windowHeight="10545" activeTab="4" xr2:uid="{CCADFEE4-B0E1-4363-9617-1683960BED03}"/>
   </bookViews>
   <sheets>
     <sheet name="StateTable" sheetId="1" r:id="rId1"/>
@@ -76337,11 +76337,12 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A827A58D-C8A4-4858-A89B-E853C083564F}">
+  <sheetPr filterMode="1"/>
   <dimension ref="A1:AK192"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A46" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D77" sqref="D77"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D46" sqref="D46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
@@ -76398,7 +76399,7 @@
         <v>552</v>
       </c>
     </row>
-    <row r="2" spans="1:37" ht="21" thickTop="1">
+    <row r="2" spans="1:37" ht="21" hidden="1" thickTop="1">
       <c r="A2" s="50" t="s">
         <v>457</v>
       </c>
@@ -76426,7 +76427,7 @@
       <c r="I2" s="22"/>
       <c r="AK2" s="23"/>
     </row>
-    <row r="3" spans="1:37" ht="30">
+    <row r="3" spans="1:37" ht="30.75" hidden="1" thickTop="1">
       <c r="A3" s="50" t="s">
         <v>457</v>
       </c>
@@ -76454,7 +76455,7 @@
       <c r="I3" s="22"/>
       <c r="AK3" s="23"/>
     </row>
-    <row r="4" spans="1:37" ht="20.25">
+    <row r="4" spans="1:37" ht="21" hidden="1" thickTop="1">
       <c r="A4" s="55" t="s">
         <v>457</v>
       </c>
@@ -76482,7 +76483,7 @@
       <c r="I4" s="22"/>
       <c r="AK4" s="23"/>
     </row>
-    <row r="5" spans="1:37" ht="20.25">
+    <row r="5" spans="1:37" ht="21" hidden="1" thickTop="1">
       <c r="A5" s="55" t="s">
         <v>457</v>
       </c>
@@ -76510,7 +76511,7 @@
       <c r="I5" s="22"/>
       <c r="AK5" s="23"/>
     </row>
-    <row r="6" spans="1:37" ht="30">
+    <row r="6" spans="1:37" ht="30.75" hidden="1" thickTop="1">
       <c r="A6" s="55" t="s">
         <v>457</v>
       </c>
@@ -76538,7 +76539,7 @@
       <c r="I6" s="22"/>
       <c r="AK6" s="23"/>
     </row>
-    <row r="7" spans="1:37" ht="30">
+    <row r="7" spans="1:37" ht="30.75" hidden="1" thickTop="1">
       <c r="A7" s="55" t="s">
         <v>457</v>
       </c>
@@ -76566,7 +76567,7 @@
       <c r="I7" s="22"/>
       <c r="AK7" s="23"/>
     </row>
-    <row r="8" spans="1:37" ht="21" thickBot="1">
+    <row r="8" spans="1:37" ht="21" hidden="1" thickTop="1">
       <c r="A8" s="50" t="s">
         <v>456</v>
       </c>
@@ -76593,7 +76594,7 @@
       </c>
       <c r="AK8" s="23"/>
     </row>
-    <row r="9" spans="1:37" ht="21.75" thickTop="1" thickBot="1">
+    <row r="9" spans="1:37" ht="21.75" hidden="1" thickTop="1" thickBot="1">
       <c r="A9" s="50" t="s">
         <v>456</v>
       </c>
@@ -76621,7 +76622,7 @@
       <c r="I9" s="22"/>
       <c r="AK9" s="23"/>
     </row>
-    <row r="10" spans="1:37" ht="31.5" thickTop="1" thickBot="1">
+    <row r="10" spans="1:37" ht="30.75" hidden="1" thickTop="1">
       <c r="A10" s="55" t="s">
         <v>456</v>
       </c>
@@ -76649,7 +76650,7 @@
       <c r="I10" s="23"/>
       <c r="AK10" s="23"/>
     </row>
-    <row r="11" spans="1:37" ht="31.5" thickTop="1" thickBot="1">
+    <row r="11" spans="1:37" ht="31.5" hidden="1" thickTop="1" thickBot="1">
       <c r="A11" s="55" t="s">
         <v>456</v>
       </c>
@@ -76677,7 +76678,7 @@
       <c r="I11" s="23"/>
       <c r="AK11" s="23"/>
     </row>
-    <row r="12" spans="1:37" ht="21" thickTop="1">
+    <row r="12" spans="1:37" ht="21" hidden="1" thickTop="1">
       <c r="A12" s="55" t="s">
         <v>456</v>
       </c>
@@ -76705,7 +76706,7 @@
       <c r="I12" s="23"/>
       <c r="AK12" s="23"/>
     </row>
-    <row r="13" spans="1:37" ht="30">
+    <row r="13" spans="1:37" ht="30.75" hidden="1" thickTop="1">
       <c r="A13" s="55" t="s">
         <v>456</v>
       </c>
@@ -76732,7 +76733,7 @@
       </c>
       <c r="I13" s="23"/>
     </row>
-    <row r="14" spans="1:37" ht="30">
+    <row r="14" spans="1:37" ht="30.75" hidden="1" thickTop="1">
       <c r="A14" s="55" t="s">
         <v>456</v>
       </c>
@@ -76759,7 +76760,7 @@
       </c>
       <c r="I14" s="23"/>
     </row>
-    <row r="15" spans="1:37" ht="30">
+    <row r="15" spans="1:37" ht="30.75" hidden="1" thickTop="1">
       <c r="A15" s="55" t="s">
         <v>456</v>
       </c>
@@ -76786,7 +76787,7 @@
       </c>
       <c r="I15" s="23"/>
     </row>
-    <row r="16" spans="1:37" ht="20.25">
+    <row r="16" spans="1:37" ht="21" hidden="1" thickTop="1">
       <c r="A16" s="55" t="s">
         <v>456</v>
       </c>
@@ -76813,7 +76814,7 @@
       </c>
       <c r="I16" s="23"/>
     </row>
-    <row r="17" spans="1:37" ht="20.25">
+    <row r="17" spans="1:37" ht="21" hidden="1" thickTop="1">
       <c r="A17" s="50" t="s">
         <v>3</v>
       </c>
@@ -76841,7 +76842,7 @@
       <c r="I17" s="23"/>
       <c r="AK17" s="23"/>
     </row>
-    <row r="18" spans="1:37" ht="20.25">
+    <row r="18" spans="1:37" ht="21" hidden="1" thickTop="1">
       <c r="A18" s="50" t="s">
         <v>3</v>
       </c>
@@ -76869,7 +76870,7 @@
       <c r="I18" s="23"/>
       <c r="AK18" s="23"/>
     </row>
-    <row r="19" spans="1:37" ht="20.25">
+    <row r="19" spans="1:37" ht="21" hidden="1" thickTop="1">
       <c r="A19" s="50" t="s">
         <v>3</v>
       </c>
@@ -76897,7 +76898,7 @@
       <c r="I19" s="23"/>
       <c r="AK19" s="23"/>
     </row>
-    <row r="20" spans="1:37" ht="20.25">
+    <row r="20" spans="1:37" ht="21" hidden="1" thickTop="1">
       <c r="A20" s="50" t="s">
         <v>3</v>
       </c>
@@ -76924,7 +76925,7 @@
       </c>
       <c r="I20" s="23"/>
     </row>
-    <row r="21" spans="1:37" ht="30">
+    <row r="21" spans="1:37" ht="30.75" hidden="1" thickTop="1">
       <c r="A21" s="55" t="s">
         <v>3</v>
       </c>
@@ -76951,7 +76952,7 @@
       </c>
       <c r="I21" s="23"/>
     </row>
-    <row r="22" spans="1:37" ht="20.25">
+    <row r="22" spans="1:37" ht="21" hidden="1" thickTop="1">
       <c r="A22" s="50" t="s">
         <v>3</v>
       </c>
@@ -76978,7 +76979,7 @@
       </c>
       <c r="I22" s="23"/>
     </row>
-    <row r="23" spans="1:37" ht="20.25">
+    <row r="23" spans="1:37" ht="21" hidden="1" thickTop="1">
       <c r="A23" s="50" t="s">
         <v>494</v>
       </c>
@@ -77005,7 +77006,7 @@
       </c>
       <c r="I23" s="23"/>
     </row>
-    <row r="24" spans="1:37" ht="20.25">
+    <row r="24" spans="1:37" ht="21" hidden="1" thickTop="1">
       <c r="A24" s="50" t="s">
         <v>494</v>
       </c>
@@ -77032,7 +77033,7 @@
       </c>
       <c r="I24" s="23"/>
     </row>
-    <row r="25" spans="1:37" ht="20.25">
+    <row r="25" spans="1:37" ht="21" hidden="1" thickTop="1">
       <c r="A25" s="50" t="s">
         <v>494</v>
       </c>
@@ -77059,7 +77060,7 @@
       </c>
       <c r="I25" s="23"/>
     </row>
-    <row r="26" spans="1:37" ht="20.25">
+    <row r="26" spans="1:37" ht="21" hidden="1" thickTop="1">
       <c r="A26" s="50" t="s">
         <v>494</v>
       </c>
@@ -77086,7 +77087,7 @@
       </c>
       <c r="I26" s="23"/>
     </row>
-    <row r="27" spans="1:37" ht="30">
+    <row r="27" spans="1:37" ht="30.75" hidden="1" thickTop="1">
       <c r="A27" s="55" t="s">
         <v>494</v>
       </c>
@@ -77113,7 +77114,7 @@
       </c>
       <c r="I27" s="23"/>
     </row>
-    <row r="28" spans="1:37" ht="20.25">
+    <row r="28" spans="1:37" ht="21" hidden="1" thickTop="1">
       <c r="A28" s="50" t="s">
         <v>494</v>
       </c>
@@ -77140,7 +77141,7 @@
       </c>
       <c r="I28" s="23"/>
     </row>
-    <row r="29" spans="1:37" ht="30">
+    <row r="29" spans="1:37" ht="30.75" hidden="1" thickTop="1">
       <c r="A29" s="55" t="s">
         <v>580</v>
       </c>
@@ -77177,7 +77178,7 @@
         <v>#define mEFCT_PWRON_LFOOF                 41 // This is the awesome FOOF Rubber Band Gun, darling.</v>
       </c>
     </row>
-    <row r="30" spans="1:37" ht="30">
+    <row r="30" spans="1:37" ht="30.75" hidden="1" thickTop="1">
       <c r="A30" s="55" t="s">
         <v>580</v>
       </c>
@@ -77214,7 +77215,7 @@
         <v>#define mEFCT_PWRON_MFOOF                 42 // This is the awesome FOOF Rubber Band Gun.</v>
       </c>
     </row>
-    <row r="31" spans="1:37" ht="30">
+    <row r="31" spans="1:37" ht="30.75" hidden="1" thickTop="1">
       <c r="A31" s="55" t="s">
         <v>580</v>
       </c>
@@ -77255,7 +77256,7 @@
         <v xml:space="preserve">                </v>
       </c>
     </row>
-    <row r="32" spans="1:37" ht="30">
+    <row r="32" spans="1:37" ht="30.75" hidden="1" thickTop="1">
       <c r="A32" s="55" t="s">
         <v>580</v>
       </c>
@@ -77293,7 +77294,7 @@
       </c>
       <c r="N32" s="24"/>
     </row>
-    <row r="33" spans="1:11" ht="20.25">
+    <row r="33" spans="1:11" ht="21" hidden="1" thickTop="1">
       <c r="A33" s="50" t="s">
         <v>455</v>
       </c>
@@ -77320,7 +77321,7 @@
       </c>
       <c r="I33" s="23"/>
     </row>
-    <row r="34" spans="1:11" ht="20.25">
+    <row r="34" spans="1:11" ht="21" hidden="1" thickTop="1">
       <c r="A34" s="50" t="s">
         <v>455</v>
       </c>
@@ -77347,7 +77348,7 @@
       </c>
       <c r="I34" s="23"/>
     </row>
-    <row r="35" spans="1:11" ht="30">
+    <row r="35" spans="1:11" ht="30.75" hidden="1" thickTop="1">
       <c r="A35" s="50" t="s">
         <v>455</v>
       </c>
@@ -77374,7 +77375,7 @@
       </c>
       <c r="I35" s="23"/>
     </row>
-    <row r="36" spans="1:11" ht="30">
+    <row r="36" spans="1:11" ht="30.75" hidden="1" thickTop="1">
       <c r="A36" s="50" t="s">
         <v>455</v>
       </c>
@@ -77401,7 +77402,7 @@
       </c>
       <c r="I36" s="23"/>
     </row>
-    <row r="37" spans="1:11" ht="30">
+    <row r="37" spans="1:11" ht="30.75" hidden="1" thickTop="1">
       <c r="A37" s="55" t="s">
         <v>455</v>
       </c>
@@ -77428,7 +77429,7 @@
       </c>
       <c r="I37" s="23"/>
     </row>
-    <row r="38" spans="1:11" ht="20.25">
+    <row r="38" spans="1:11" ht="21" hidden="1" thickTop="1">
       <c r="A38" s="55" t="s">
         <v>455</v>
       </c>
@@ -77455,7 +77456,7 @@
       </c>
       <c r="I38" s="23"/>
     </row>
-    <row r="39" spans="1:11" ht="30">
+    <row r="39" spans="1:11" ht="30.75" hidden="1" thickTop="1">
       <c r="A39" s="55" t="s">
         <v>455</v>
       </c>
@@ -77482,7 +77483,7 @@
       </c>
       <c r="I39" s="23"/>
     </row>
-    <row r="40" spans="1:11" ht="30">
+    <row r="40" spans="1:11" ht="30.75" hidden="1" thickTop="1">
       <c r="A40" s="55" t="s">
         <v>455</v>
       </c>
@@ -77515,7 +77516,7 @@
         <v>641</v>
       </c>
     </row>
-    <row r="41" spans="1:11" ht="30">
+    <row r="41" spans="1:11" ht="30.75" hidden="1" thickTop="1">
       <c r="A41" s="55" t="s">
         <v>455</v>
       </c>
@@ -77541,7 +77542,7 @@
         <v>6406</v>
       </c>
     </row>
-    <row r="42" spans="1:11" ht="120">
+    <row r="42" spans="1:11" ht="120.75" thickTop="1">
       <c r="A42" s="56" t="s">
         <v>583</v>
       </c>
@@ -77726,7 +77727,7 @@
         <v>#define mEFCT_UNIQ_CFG_LED2CHOOSE         66 // This is an LED pattern you can choose. As always, press trigger by itself to go forward to next step or to cycle through choices. To select a choice, first hold down any combination of Yellow or Red button then press trigger. To exit configuration, hold down Green button then press trigger.</v>
       </c>
     </row>
-    <row r="47" spans="1:11" ht="30">
+    <row r="47" spans="1:11" ht="30" hidden="1">
       <c r="A47" s="56" t="s">
         <v>583</v>
       </c>
@@ -77763,7 +77764,7 @@
         <v>#define mEFCT_UNIQ_CFG_ACCEPT             67 // Your choice has been saved into the running settings.</v>
       </c>
     </row>
-    <row r="48" spans="1:11" ht="30">
+    <row r="48" spans="1:11" ht="30" hidden="1">
       <c r="A48" s="56" t="s">
         <v>583</v>
       </c>
@@ -77800,7 +77801,7 @@
         <v>#define mEFCT_UNIQ_NOT_IMPL               68 // This feature is not yet implemented.</v>
       </c>
     </row>
-    <row r="49" spans="1:12" ht="20.25">
+    <row r="49" spans="1:12" ht="20.25" hidden="1">
       <c r="A49" s="56" t="s">
         <v>583</v>
       </c>
@@ -77837,7 +77838,7 @@
         <v>#define mEFCT_UNIQ_SILENCE                69 // silence</v>
       </c>
     </row>
-    <row r="50" spans="1:12" ht="30">
+    <row r="50" spans="1:12" ht="30" hidden="1">
       <c r="A50" s="56" t="s">
         <v>583</v>
       </c>
@@ -77874,7 +77875,7 @@
         <v>#define mEFCT_UNIQ_CFG_WINDUP_DESCRIP     71 // The effect happens during wind-up to shooting.</v>
       </c>
     </row>
-    <row r="51" spans="1:12" ht="30">
+    <row r="51" spans="1:12" ht="30" hidden="1">
       <c r="A51" s="56" t="s">
         <v>583</v>
       </c>
@@ -77911,7 +77912,7 @@
         <v>#define mEFCT_UNIQ_CFG_SHOOT_DESCRIP      72 // The effect happens during shooting itself.</v>
       </c>
     </row>
-    <row r="52" spans="1:12" ht="30">
+    <row r="52" spans="1:12" ht="30" hidden="1">
       <c r="A52" s="69" t="s">
         <v>583</v>
       </c>
@@ -77948,7 +77949,7 @@
         <v>#define mEFCT_UNIQ_CFG_OPEN_DESCRIP       73 // The effect happens during opening of the barrel.</v>
       </c>
     </row>
-    <row r="53" spans="1:12" ht="30">
+    <row r="53" spans="1:12" ht="30" hidden="1">
       <c r="A53" s="56" t="s">
         <v>583</v>
       </c>
@@ -77985,7 +77986,7 @@
         <v>#define mEFCT_UNIQ_CFG_LKLOD_DESCRIP      74 // The effect happens during lock-and-load of the barrel.</v>
       </c>
     </row>
-    <row r="54" spans="1:12" ht="30">
+    <row r="54" spans="1:12" ht="30" hidden="1">
       <c r="A54" s="56" t="s">
         <v>583</v>
       </c>
@@ -78022,7 +78023,7 @@
         <v>#define mEFCT_UNIQ_CFG_PWRON_DESCRIP      75 // The effect happens during initial power-on.</v>
       </c>
     </row>
-    <row r="55" spans="1:12" ht="30">
+    <row r="55" spans="1:12" ht="30" hidden="1">
       <c r="A55" s="56" t="s">
         <v>583</v>
       </c>
@@ -78059,7 +78060,7 @@
         <v>#define mEFCT_UNIQ_CFG_WAIT_DESCRIP       76 // The effect happens when waiting to shoot.</v>
       </c>
     </row>
-    <row r="56" spans="1:12" ht="20.25">
+    <row r="56" spans="1:12" ht="20.25" hidden="1">
       <c r="A56" s="56" t="s">
         <v>583</v>
       </c>
@@ -78096,7 +78097,7 @@
         <v>#define mEFCT_UNIQ_CFG_SOUNDS_DESCRIP     81 // The category is SOUNDS.</v>
       </c>
     </row>
-    <row r="57" spans="1:12" ht="30">
+    <row r="57" spans="1:12" ht="30" hidden="1">
       <c r="A57" s="56" t="s">
         <v>583</v>
       </c>
@@ -78133,7 +78134,7 @@
         <v>#define mEFCT_UNIQ_CFG_LEDPTRN_DESCRIP    82 // The category is L. E. D. PATTERNS.</v>
       </c>
     </row>
-    <row r="58" spans="1:12" ht="30">
+    <row r="58" spans="1:12" ht="30" hidden="1">
       <c r="A58" s="56" t="s">
         <v>583</v>
       </c>
@@ -78170,7 +78171,7 @@
         <v>#define mEFCT_UNIQ_CFG_CPY_RST_DESCRIP    83 // The category is configuration resets and copying.</v>
       </c>
     </row>
-    <row r="59" spans="1:12" ht="30">
+    <row r="59" spans="1:12" ht="30" hidden="1">
       <c r="A59" s="56" t="s">
         <v>583</v>
       </c>
@@ -78207,7 +78208,7 @@
         <v>#define mEFCT_UNIQ_CFG_ADVANCED_DESCRIP   84 // The category is advanced settings.</v>
       </c>
     </row>
-    <row r="60" spans="1:12" ht="30">
+    <row r="60" spans="1:12" ht="30" hidden="1">
       <c r="A60" s="56" t="s">
         <v>583</v>
       </c>
@@ -78246,7 +78247,7 @@
       </c>
       <c r="L60" s="65"/>
     </row>
-    <row r="61" spans="1:12" ht="45">
+    <row r="61" spans="1:12" ht="45" hidden="1">
       <c r="A61" s="56" t="s">
         <v>583</v>
       </c>
@@ -78285,7 +78286,7 @@
       </c>
       <c r="L61" s="65"/>
     </row>
-    <row r="62" spans="1:12" ht="45">
+    <row r="62" spans="1:12" ht="45" hidden="1">
       <c r="A62" s="56" t="s">
         <v>583</v>
       </c>
@@ -78323,7 +78324,7 @@
         <v>#define mEFCT_UNIQ_CFG_SORRY_NO_PASSWORD  88 // Sorry, I don't have a password, but you dance very well. Please press trigger.</v>
       </c>
     </row>
-    <row r="63" spans="1:12" ht="285">
+    <row r="63" spans="1:12" ht="285" hidden="1">
       <c r="A63" s="56" t="s">
         <v>583</v>
       </c>
@@ -78360,7 +78361,7 @@
         <v>#define mEFCT_UNIQ_CFG_CREDITS            89 // The FOOF Science Fiction Rubber Band Gun was originally conceived by Mark and Keith. The hardware implementation was designed and built by Jim. The software and most of the sounds were generated by Mark. Some build information is at Git Hub dot Com slash Mark Dash Em Dee Oh Forty Seven dot Com slash Rubber Band Gun. Some sounds are recordings of Mark's family. Many of the Sci Fi sounds are transmogrified versions of Creative Commons sounds stored on Free Sound dot Org. Other Sci Fi sounds originated from El Eye Gee Oh gravity wave detections of stellar events found at Gee Double You Dash Open Science dot Org slash Audio Gee Double You Tee See One. The robotic voice sounds were generated using the eSpeak text to speech program found on eSpeak dot Source Forge dot net. See the Git Hub page for more attributions.</v>
       </c>
     </row>
-    <row r="64" spans="1:12" ht="45">
+    <row r="64" spans="1:12" ht="45" hidden="1">
       <c r="A64" s="56" t="s">
         <v>583</v>
       </c>
@@ -78398,7 +78399,7 @@
         <v>#define mEFCT_UNIQ_CFG_MGMT_01            91 // Erase the running setting only and reset the running setting to the factory settings.</v>
       </c>
     </row>
-    <row r="65" spans="1:11" ht="45">
+    <row r="65" spans="1:11" ht="45" hidden="1">
       <c r="A65" s="56" t="s">
         <v>583</v>
       </c>
@@ -78436,7 +78437,7 @@
         <v>#define mEFCT_UNIQ_CFG_MGMT_02            92 // Erase the running setting and erase all saved auxilliary settings and reset to the factory settings.</v>
       </c>
     </row>
-    <row r="66" spans="1:11" ht="45">
+    <row r="66" spans="1:11" ht="45" hidden="1">
       <c r="A66" s="56" t="s">
         <v>583</v>
       </c>
@@ -78474,7 +78475,7 @@
         <v>#define mEFCT_UNIQ_CFG_MGMT_03            93 // Copy the running setting and overwrite into saved auxilliary setting number one.</v>
       </c>
     </row>
-    <row r="67" spans="1:11" ht="45">
+    <row r="67" spans="1:11" ht="45" hidden="1">
       <c r="A67" s="56" t="s">
         <v>583</v>
       </c>
@@ -78512,7 +78513,7 @@
         <v>#define mEFCT_UNIQ_CFG_MGMT_04            94 // Copy the running setting and overwrite into saved auxilliary setting number two.</v>
       </c>
     </row>
-    <row r="68" spans="1:11" ht="45">
+    <row r="68" spans="1:11" ht="45" hidden="1">
       <c r="A68" s="56" t="s">
         <v>583</v>
       </c>
@@ -78550,7 +78551,7 @@
         <v>#define mEFCT_UNIQ_CFG_MGMT_05            95 // Copy the running setting and overwrite into saved auxilliary setting number three.</v>
       </c>
     </row>
-    <row r="69" spans="1:11" ht="45">
+    <row r="69" spans="1:11" ht="45" hidden="1">
       <c r="A69" s="56" t="s">
         <v>583</v>
       </c>
@@ -78588,7 +78589,7 @@
         <v>#define mEFCT_UNIQ_CFG_MGMT_06            96 // Copy the saved auxilliary setting number one and overwrite into the running setting.</v>
       </c>
     </row>
-    <row r="70" spans="1:11" ht="45">
+    <row r="70" spans="1:11" ht="45" hidden="1">
       <c r="A70" s="56" t="s">
         <v>583</v>
       </c>
@@ -78626,7 +78627,7 @@
         <v>#define mEFCT_UNIQ_CFG_MGMT_07            97 // Copy the saved auxilliary setting number two and overwrite into the running setting.</v>
       </c>
     </row>
-    <row r="71" spans="1:11" ht="45">
+    <row r="71" spans="1:11" ht="45" hidden="1">
       <c r="A71" s="56" t="s">
         <v>583</v>
       </c>
@@ -78778,7 +78779,7 @@
         <v>#define mEFCT_UNIQ_CFG_ADVANCED_03       103 // Hear Rubber Band Gun credits. As always, press trigger by itself to go forward to next step or to cycle through choices. To select a choice, first hold down any combination of Yellow or Red button then press trigger. To exit configuration, hold down Green button then press trigger.</v>
       </c>
     </row>
-    <row r="75" spans="1:11" ht="20.25">
+    <row r="75" spans="1:11" ht="20.25" hidden="1">
       <c r="A75" s="56" t="s">
         <v>583</v>
       </c>
@@ -78816,7 +78817,7 @@
         <v>#define mEFCT_UNIQ_SHOOT_UNUSED          104 // Unused Sound File.</v>
       </c>
     </row>
-    <row r="76" spans="1:11" ht="30">
+    <row r="76" spans="1:11" ht="30" hidden="1">
       <c r="A76" s="56" t="s">
         <v>583</v>
       </c>
@@ -78892,7 +78893,7 @@
         <v>#define mEFCT_UNIQ_CFG_ADVANCED          106 // Now choose which ADVANCED configuration category: Demo Mode, Time Travel and Teleportation, or Credits. As always, press trigger by itself to go forward to next step or to cycle through choices. To select a choice, first hold down any combination of Yellow or Red button then press trigger. To exit configuration, hold down Green button then press trigger.</v>
       </c>
     </row>
-    <row r="78" spans="1:11" ht="30">
+    <row r="78" spans="1:11" ht="30" hidden="1">
       <c r="A78" s="56" t="s">
         <v>583</v>
       </c>
@@ -78967,7 +78968,7 @@
         <v>#define mEFCT_UNIQ_CFG_CPY_RST           108 // Now choose the, factory reset, or, configuration, copy, option. This list cycles through the options one by one. As always, press trigger by itself to go forward to next step or to cycle through choices. To select a choice, first hold down any combination of Yellow or Red button then press trigger. To exit configuration, hold down Green button then press trigger.</v>
       </c>
     </row>
-    <row r="80" spans="1:11" ht="45">
+    <row r="80" spans="1:11" ht="45" hidden="1">
       <c r="A80" s="69" t="s">
         <v>583</v>
       </c>
@@ -79004,7 +79005,7 @@
         <v>#define mEFCT_UNIQ_CFG_CPY_RST_ACCEPT    109 // Your, factory reset, or, configuration copy, option, has been accepted. Rebooting.</v>
       </c>
     </row>
-    <row r="81" spans="1:18">
+    <row r="81" spans="1:18" hidden="1">
       <c r="A81" s="87" t="s">
         <v>693</v>
       </c>
@@ -79033,32 +79034,32 @@
         <v>693</v>
       </c>
     </row>
-    <row r="82" spans="1:18">
+    <row r="82" spans="1:18" hidden="1">
       <c r="K82" t="s">
         <v>562</v>
       </c>
     </row>
-    <row r="83" spans="1:18">
+    <row r="83" spans="1:18" hidden="1">
       <c r="K83" t="s">
         <v>563</v>
       </c>
     </row>
-    <row r="84" spans="1:18">
+    <row r="84" spans="1:18" hidden="1">
       <c r="K84" t="s">
         <v>564</v>
       </c>
     </row>
-    <row r="85" spans="1:18">
+    <row r="85" spans="1:18" hidden="1">
       <c r="K85" t="s">
         <v>565</v>
       </c>
     </row>
-    <row r="86" spans="1:18">
+    <row r="86" spans="1:18" hidden="1">
       <c r="K86" t="s">
         <v>566</v>
       </c>
     </row>
-    <row r="87" spans="1:18">
+    <row r="87" spans="1:18" hidden="1">
       <c r="K87" t="s">
         <v>567</v>
       </c>
@@ -79066,7 +79067,7 @@
         <v>545</v>
       </c>
     </row>
-    <row r="88" spans="1:18">
+    <row r="88" spans="1:18" hidden="1">
       <c r="K88" t="s">
         <v>568</v>
       </c>
@@ -79074,7 +79075,7 @@
         <v>546</v>
       </c>
     </row>
-    <row r="89" spans="1:18">
+    <row r="89" spans="1:18" hidden="1">
       <c r="K89" t="s">
         <v>569</v>
       </c>
@@ -80084,7 +80085,32 @@
       <c r="D192" s="9"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:H89" xr:uid="{D49867B0-9605-4DAD-A171-997D81FF01DA}"/>
+  <autoFilter xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" ref="A1:H89" xr:uid="{D49867B0-9605-4DAD-A171-997D81FF01DA}">
+    <filterColumn colId="3">
+      <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+        <mc:Choice Requires="x14">
+          <filters>
+            <x14:filter val="mdo47 recording of &quot;Demo mode: Switch through the saved configurations each time you shoot. Power cycle to exit demo mode. As always, press trigger by itself to go forward to next step or to cycle through choices. To select a choice, first hold down any combination of Yellow or Red button then press trigger. To exit configuration, hold down Green button then press trigger.&quot;"/>
+            <x14:filter val="mdo47 recording of &quot;Enable time travel and teleportation capabilities (requires password). As always, press trigger by itself to go forward to next step or to cycle through choices. To select a choice, first hold down any combination of Yellow or Red button then press trigger. To exit configuration, hold down Green button then press trigger.&quot;"/>
+            <x14:filter val="mdo47 recording of &quot;Hear Rubber Band Gun credits. As always, press trigger by itself to go forward to next step or to cycle through choices. To select a choice, first hold down any combination of Yellow or Red button then press trigger. To exit configuration, hold down Green button then press trigger.&quot;"/>
+            <x14:filter val="mdo47 recording of &quot;Now choose the effect itself. This list cycles through the effects one by one. As always, press trigger by itself to go forward to next step or to cycle through choices. To select a choice, first hold down any combination of Yellow or Red button then press trigger. To exit configuration, hold down Green button then press trigger.&quot;"/>
+            <x14:filter val="mdo47 recording of &quot;Now choose the, factory reset, or, configuration, copy, option. This list cycles through the options one by one. As always, press trigger by itself to go forward to next step or to cycle through choices. To select a choice, first hold down any combination of Yellow or Red button then press trigger. To exit configuration, hold down Green button then press trigger.&quot;"/>
+            <x14:filter val="mdo47 recording of &quot;Now choose when the effect happens. This list includes when powering-on, when shooting, etc. As always, press trigger by itself to go forward to next step or to cycle through choices. To select a choice, first hold down any combination of Yellow or Red button then press trigger. To exit configuration, hold down Green button then press trigger.&quot;"/>
+            <x14:filter val="mdo47 recording of &quot;Now choose which ADVANCED configuration category: Demo Mode, Time Travel and Teleportation, or Credits. As always, press trigger by itself to go forward to next step or to cycle through choices. To select a choice, first hold down any combination of Yellow or Red button then press trigger. To exit configuration, hold down Green button then press trigger.&quot;"/>
+            <x14:filter val="mdo47 recording of &quot;Now choose which configuration category: sound effects, LED pattern effects, configuration resets and copying, or advanced settings. As always, press trigger by itself to go forward to next step or to cycle through choices. To select a choice, first hold down any combination of Yellow or Red button then press trigger. To exit configuration, hold down Green button then press trigger.&quot;"/>
+            <x14:filter val="mdo47 recording of &quot;This is an LED pattern you can choose. As always, press trigger by itself to go forward to next step or to cycle through choices. To select a choice, first hold down any combination of Yellow or Red button then press trigger. To exit configuration, hold down Green button then press trigger.&quot;"/>
+            <x14:filter val="mdo47 recording of &quot;Welcome to the FOOF Rubber Band Gun configuration! Your call is important to us. Press trigger by itself to go forward to next step or to cycle through choices. To select a choice, first hold down any combination of Yellow or Red button then press trigger. To exit configuration, hold down Green button then press trigger.&quot;"/>
+          </filters>
+        </mc:Choice>
+        <mc:Fallback>
+          <customFilters>
+            <customFilter val=""/>
+            <customFilter operator="notEqual" val=" "/>
+          </customFilters>
+        </mc:Fallback>
+      </mc:AlternateContent>
+    </filterColumn>
+  </autoFilter>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="D169:D193">
     <sortCondition ref="D169:D193"/>
   </sortState>

</xml_diff>

<commit_message>
add info on LED pattern generation
</commit_message>
<xml_diff>
--- a/RBG_arduino/StateTable_minimal.xlsx
+++ b/RBG_arduino/StateTable_minimal.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23231"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub-Mark-MDO47\RubberBandGun\RBG_arduino\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F74EC5E2-AF72-4F92-A29C-3CEAAD2CAECD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8271A6D-EABF-4852-AA4E-E50DB238B71A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21840" activeTab="6" xr2:uid="{CCADFEE4-B0E1-4363-9617-1683960BED03}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21840" activeTab="5" xr2:uid="{CCADFEE4-B0E1-4363-9617-1683960BED03}"/>
   </bookViews>
   <sheets>
     <sheet name="StateTable" sheetId="1" r:id="rId1"/>
@@ -23,11 +23,11 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">debugging!$A$5359:$B$5769</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">LEDpatterns!$A$1:$M$61</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">LEDpatterns!$A$8:$M$68</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">Sounds!$A$1:$H$92</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">StateTable!$A$1:$K$162</definedName>
     <definedName name="gain2N3904">#REF!</definedName>
-    <definedName name="LEDlookup">LEDpatterns!$I$2:$J$31</definedName>
+    <definedName name="LEDlookup">LEDpatterns!$I$9:$J$38</definedName>
     <definedName name="mROW">StateTable!$V$2:$X$45</definedName>
     <definedName name="prev">Sounds!$AK$2:$AK$19</definedName>
     <definedName name="yxcmd">'YX5200 info'!$A$2:$C$44</definedName>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8761" uniqueCount="6440">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8794" uniqueCount="6464">
   <si>
     <t>trigOnly</t>
   </si>
@@ -19654,6 +19654,78 @@
   </si>
   <si>
     <t>windup, open, lock/load</t>
+  </si>
+  <si>
+    <t>FastLED is the library I use for controlling these color addressable LEDs</t>
+  </si>
+  <si>
+    <t>https://www.arduino.cc/reference/en/libraries/fastled/</t>
+  </si>
+  <si>
+    <t>https://github.com/FastLED/FastLED</t>
+  </si>
+  <si>
+    <t>If you are new to FastLED, look at this famous demo code to see how easy it can be</t>
+  </si>
+  <si>
+    <t>https://github.com/FastLED/FastLED/blob/master/examples/DemoReel100/DemoReel100.ino</t>
+  </si>
+  <si>
+    <t>In the RBG I use four unmodified routines from DemoReel100. These routines take no parameters.</t>
+  </si>
+  <si>
+    <t>bpm</t>
+  </si>
+  <si>
+    <t>confetti</t>
+  </si>
+  <si>
+    <t>juggle</t>
+  </si>
+  <si>
+    <t>rainbowWithGlitter</t>
+  </si>
+  <si>
+    <t>I also use three modified routines from DemoReel100. The first routine takes no parameters, but the other two take a parameter.</t>
+  </si>
+  <si>
+    <t>RBG_bpm_rings</t>
+  </si>
+  <si>
+    <t>RBG_confetti_fadeby</t>
+  </si>
+  <si>
+    <t>RBG_juggle_numdot_ring</t>
+  </si>
+  <si>
+    <t>I also use two routines of my own invention; these routines take parameter(s).</t>
+  </si>
+  <si>
+    <t>RBG_diskDownTheDrainOrRotate</t>
+  </si>
+  <si>
+    <t>RBG_RailGunEffect</t>
+  </si>
+  <si>
+    <t>The LED patterns can string these routines together to make one composite pattern.</t>
+  </si>
+  <si>
+    <t>FYI diskDownTheDrainOrRotate was originally written for the Graduation Cap project https://github.com/Mark-MDO47/GraduationCap2017.</t>
+  </si>
+  <si>
+    <t>FYI diskDownTheDrainOrRotate was originally written for the Graduation Cap project</t>
+  </si>
+  <si>
+    <t>https://github.com/Mark-MDO47/GraduationCap2017</t>
+  </si>
+  <si>
+    <t>bpm, confetti, juggle, rainbowWithGlitter</t>
+  </si>
+  <si>
+    <t>RBG_bpm_rings, RBG_confetti_fadeby, RBG_juggle_numdot_ring</t>
+  </si>
+  <si>
+    <t>RBG_diskDownTheDrainOrRotate, RBG_RailGunEffect</t>
   </si>
 </sst>
 </file>
@@ -20078,7 +20150,7 @@
     <xf numFmtId="0" fontId="19" fillId="10" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="10" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="95">
+  <cellXfs count="102">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -20287,6 +20359,25 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="11" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="7" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="7" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="7" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="10">
@@ -20620,7 +20711,7 @@
   <sheetViews>
     <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="M9" sqref="M9"/>
+      <selection pane="bottomLeft" activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
@@ -80257,11 +80348,11 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D01D897F-FD6B-401C-A7DE-9A4CCEE4EB37}">
-  <dimension ref="A1:P62"/>
+  <dimension ref="A1:P100"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C51" sqref="C51"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="8" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A7" sqref="A7:XFD7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -80274,1653 +80365,1814 @@
     <col min="9" max="9" width="20.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" ht="16.5" thickTop="1" thickBot="1">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:16" ht="17.25">
+      <c r="A1" s="101" t="s">
+        <v>6440</v>
+      </c>
+      <c r="E1" s="100" t="s">
+        <v>6441</v>
+      </c>
+      <c r="G1" s="100" t="s">
+        <v>6442</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16" ht="17.25">
+      <c r="A2" s="101" t="s">
+        <v>6443</v>
+      </c>
+      <c r="F2" s="100" t="s">
+        <v>6444</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" ht="17.25">
+      <c r="A3" s="101" t="s">
+        <v>6445</v>
+      </c>
+      <c r="G3" s="101" t="s">
+        <v>6461</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" ht="17.25">
+      <c r="A4" s="101" t="s">
+        <v>6450</v>
+      </c>
+      <c r="G4" s="101" t="s">
+        <v>6462</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" ht="17.25">
+      <c r="A5" s="101" t="s">
+        <v>6454</v>
+      </c>
+      <c r="G5" s="101" t="s">
+        <v>6463</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" ht="17.25">
+      <c r="A6" s="101" t="s">
+        <v>6457</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16" ht="18" thickBot="1">
+      <c r="A7" s="98" t="s">
+        <v>6459</v>
+      </c>
+      <c r="F7" s="24" t="s">
+        <v>6460</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16" ht="16.5" thickTop="1" thickBot="1">
+      <c r="A8" s="1" t="s">
         <v>721</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B8" s="1" t="s">
         <v>722</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C8" s="1" t="s">
         <v>587</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D8" s="1" t="s">
         <v>731</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E8" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="F1" s="76" t="s">
+      <c r="F8" s="76" t="s">
         <v>723</v>
       </c>
-      <c r="G1" s="76" t="s">
+      <c r="G8" s="76" t="s">
         <v>4422</v>
       </c>
-      <c r="H1" s="77" t="s">
+      <c r="H8" s="77" t="s">
         <v>744</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="I8" s="1" t="s">
         <v>745</v>
       </c>
-      <c r="J1" s="76" t="s">
+      <c r="J8" s="76" t="s">
         <v>561</v>
       </c>
-      <c r="K1" s="76" t="s">
+      <c r="K8" s="76" t="s">
         <v>4421</v>
       </c>
-      <c r="L1" s="76" t="s">
+      <c r="L8" s="76" t="s">
         <v>745</v>
       </c>
-      <c r="M1" s="76" t="s">
+      <c r="M8" s="76" t="s">
         <v>561</v>
       </c>
-      <c r="P1" t="s">
+      <c r="P8" t="s">
         <v>764</v>
       </c>
     </row>
-    <row r="2" spans="1:16" ht="15.75" thickTop="1">
-      <c r="A2">
+    <row r="9" spans="1:16" ht="15.75" thickTop="1">
+      <c r="A9">
         <v>1</v>
       </c>
-      <c r="B2">
-        <f t="shared" ref="B2:B33" si="0">VLOOKUP(H2,LEDlookup,2,FALSE)</f>
+      <c r="B9">
+        <f t="shared" ref="B9:B40" si="0">VLOOKUP(H9,LEDlookup,2,FALSE)</f>
         <v>7</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C9" t="s">
         <v>734</v>
       </c>
-      <c r="E2" t="s">
+      <c r="E9" t="s">
         <v>743</v>
       </c>
-      <c r="F2" t="s">
+      <c r="F9" t="s">
         <v>45</v>
       </c>
-      <c r="G2" t="s">
+      <c r="G9" t="s">
         <v>736</v>
       </c>
-      <c r="H2" t="str">
-        <f>C2&amp;"|"&amp;D2</f>
+      <c r="H9" t="str">
+        <f>C9&amp;"|"&amp;D9</f>
         <v>RBG_juggle_numdot_ring(5); RBG_confetti_fadeby(128);|</v>
       </c>
-      <c r="I2" t="s">
+      <c r="I9" t="s">
         <v>747</v>
       </c>
-      <c r="J2">
+      <c r="J9">
         <v>254</v>
       </c>
-      <c r="L2" t="s">
+      <c r="L9" t="s">
         <v>748</v>
       </c>
-      <c r="M2">
+      <c r="M9">
         <v>1</v>
       </c>
-      <c r="P2" t="str">
-        <f>P1&amp;B2&amp;", "</f>
+      <c r="P9" t="str">
+        <f>P8&amp;B9&amp;", "</f>
         <v xml:space="preserve">static const uint8_t lookupLEDpatternTbl[] PROGMEM = { 7, </v>
       </c>
     </row>
-    <row r="3" spans="1:16">
-      <c r="A3">
+    <row r="10" spans="1:16">
+      <c r="A10">
         <v>2</v>
       </c>
-      <c r="B3">
+      <c r="B10">
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C10" t="s">
         <v>727</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D10" t="s">
         <v>728</v>
       </c>
-      <c r="E3" t="s">
+      <c r="E10" t="s">
         <v>737</v>
       </c>
-      <c r="F3" t="s">
+      <c r="F10" t="s">
         <v>45</v>
       </c>
-      <c r="G3" t="s">
+      <c r="G10" t="s">
         <v>733</v>
       </c>
-      <c r="H3" t="str">
-        <f t="shared" ref="H3:H60" si="1">C3&amp;"|"&amp;D3</f>
+      <c r="H10" t="str">
+        <f t="shared" ref="H10:H67" si="1">C10&amp;"|"&amp;D10</f>
         <v>RBG_diskDownTheDrainOrRotate(2);|RBG_ringRotateAndFade(mNONE, 0, windup1BrightSpots); numSteps</v>
       </c>
-      <c r="I3" t="s">
+      <c r="I10" t="s">
         <v>763</v>
       </c>
-      <c r="J3">
+      <c r="J10">
         <v>12</v>
       </c>
-      <c r="L3" t="s">
+      <c r="L10" t="s">
         <v>749</v>
       </c>
-      <c r="M3">
+      <c r="M10">
         <v>2</v>
       </c>
-      <c r="P3" t="str">
-        <f t="shared" ref="P3:P60" si="2">P2&amp;B3&amp;", "</f>
+      <c r="P10" t="str">
+        <f t="shared" ref="P10:P67" si="2">P9&amp;B10&amp;", "</f>
         <v xml:space="preserve">static const uint8_t lookupLEDpatternTbl[] PROGMEM = { 7, 5, </v>
       </c>
     </row>
-    <row r="4" spans="1:16">
-      <c r="A4">
+    <row r="11" spans="1:16">
+      <c r="A11">
         <v>3</v>
       </c>
-      <c r="B4">
+      <c r="B11">
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C11" t="s">
         <v>735</v>
       </c>
-      <c r="F4" t="s">
+      <c r="F11" t="s">
         <v>45</v>
       </c>
-      <c r="H4" t="str">
+      <c r="H11" t="str">
         <f t="shared" si="1"/>
         <v>rainbowWithGlitter();|</v>
       </c>
-      <c r="I4" t="s">
+      <c r="I11" t="s">
         <v>748</v>
       </c>
-      <c r="J4">
+      <c r="J11">
         <v>1</v>
       </c>
-      <c r="L4" t="s">
+      <c r="L11" t="s">
         <v>750</v>
       </c>
-      <c r="M4">
+      <c r="M11">
         <v>3</v>
       </c>
-      <c r="P4" t="str">
+      <c r="P11" t="str">
         <f t="shared" si="2"/>
         <v xml:space="preserve">static const uint8_t lookupLEDpatternTbl[] PROGMEM = { 7, 5, 2, </v>
       </c>
     </row>
-    <row r="5" spans="1:16">
-      <c r="A5">
+    <row r="12" spans="1:16">
+      <c r="A12">
         <v>4</v>
       </c>
-      <c r="B5">
+      <c r="B12">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C12" t="s">
         <v>739</v>
       </c>
-      <c r="F5" t="s">
+      <c r="F12" t="s">
         <v>45</v>
       </c>
-      <c r="H5" t="str">
+      <c r="H12" t="str">
         <f t="shared" si="1"/>
         <v>juggle();|</v>
       </c>
-      <c r="I5" t="s">
+      <c r="I12" t="s">
         <v>749</v>
       </c>
-      <c r="J5">
+      <c r="J12">
         <v>2</v>
       </c>
-      <c r="L5" t="s">
+      <c r="L12" t="s">
         <v>751</v>
       </c>
-      <c r="M5">
+      <c r="M12">
         <v>4</v>
       </c>
-      <c r="P5" t="str">
+      <c r="P12" t="str">
         <f t="shared" si="2"/>
         <v xml:space="preserve">static const uint8_t lookupLEDpatternTbl[] PROGMEM = { 7, 5, 2, 1, </v>
       </c>
     </row>
-    <row r="6" spans="1:16">
-      <c r="A6">
+    <row r="13" spans="1:16">
+      <c r="A13">
         <v>5</v>
       </c>
-      <c r="B6">
+      <c r="B13">
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C13" t="s">
         <v>741</v>
       </c>
-      <c r="E6" t="s">
+      <c r="E13" t="s">
         <v>742</v>
       </c>
-      <c r="F6" t="s">
+      <c r="F13" t="s">
         <v>45</v>
       </c>
-      <c r="H6" t="str">
+      <c r="H13" t="str">
         <f t="shared" si="1"/>
         <v>RBG_juggle_numdot_ring(-4);|</v>
       </c>
-      <c r="I6" t="s">
+      <c r="I13" t="s">
         <v>750</v>
       </c>
-      <c r="J6">
+      <c r="J13">
         <v>3</v>
       </c>
-      <c r="L6" t="s">
+      <c r="L13" t="s">
         <v>752</v>
       </c>
-      <c r="M6">
+      <c r="M13">
         <v>5</v>
       </c>
-      <c r="P6" t="str">
+      <c r="P13" t="str">
         <f t="shared" si="2"/>
         <v xml:space="preserve">static const uint8_t lookupLEDpatternTbl[] PROGMEM = { 7, 5, 2, 1, 6, </v>
       </c>
     </row>
-    <row r="7" spans="1:16">
-      <c r="A7">
+    <row r="14" spans="1:16">
+      <c r="A14">
         <v>6</v>
       </c>
-      <c r="B7">
+      <c r="B14">
         <f t="shared" si="0"/>
         <v>11</v>
       </c>
-      <c r="C7" t="s">
+      <c r="C14" t="s">
         <v>746</v>
       </c>
-      <c r="F7" t="s">
+      <c r="F14" t="s">
         <v>45</v>
       </c>
-      <c r="H7" t="str">
+      <c r="H14" t="str">
         <f t="shared" si="1"/>
         <v>RBG_confetti_fadeby(128);|</v>
       </c>
-      <c r="I7" t="s">
+      <c r="I14" t="s">
         <v>756</v>
       </c>
-      <c r="J7">
+      <c r="J14">
         <v>11</v>
       </c>
-      <c r="L7" t="s">
+      <c r="L14" t="s">
         <v>753</v>
       </c>
-      <c r="M7">
+      <c r="M14">
         <v>6</v>
       </c>
-      <c r="P7" t="str">
+      <c r="P14" t="str">
         <f t="shared" si="2"/>
         <v xml:space="preserve">static const uint8_t lookupLEDpatternTbl[] PROGMEM = { 7, 5, 2, 1, 6, 11, </v>
       </c>
     </row>
-    <row r="8" spans="1:16">
-      <c r="A8">
+    <row r="15" spans="1:16">
+      <c r="A15">
         <v>7</v>
       </c>
-      <c r="B8">
+      <c r="B15">
         <f t="shared" si="0"/>
         <v>12</v>
       </c>
-      <c r="C8" t="s">
+      <c r="C15" t="s">
         <v>762</v>
       </c>
-      <c r="F8" t="s">
+      <c r="F15" t="s">
         <v>45</v>
       </c>
-      <c r="H8" t="str">
+      <c r="H15" t="str">
         <f t="shared" si="1"/>
         <v>bpm();|</v>
       </c>
-      <c r="I8" t="s">
+      <c r="I15" t="s">
         <v>751</v>
       </c>
-      <c r="J8">
+      <c r="J15">
         <v>4</v>
       </c>
-      <c r="L8" t="s">
+      <c r="L15" t="s">
         <v>754</v>
       </c>
-      <c r="M8">
+      <c r="M15">
         <v>7</v>
       </c>
-      <c r="P8" t="str">
+      <c r="P15" t="str">
         <f t="shared" si="2"/>
         <v xml:space="preserve">static const uint8_t lookupLEDpatternTbl[] PROGMEM = { 7, 5, 2, 1, 6, 11, 12, </v>
       </c>
     </row>
-    <row r="9" spans="1:16">
-      <c r="A9">
+    <row r="16" spans="1:16">
+      <c r="A16">
         <v>8</v>
       </c>
-      <c r="B9">
+      <c r="B16">
         <f t="shared" si="0"/>
         <v>254</v>
       </c>
-      <c r="F9" t="s">
+      <c r="F16" t="s">
         <v>45</v>
       </c>
-      <c r="H9" t="str">
+      <c r="H16" t="str">
         <f t="shared" si="1"/>
         <v>|</v>
       </c>
-      <c r="I9" t="s">
+      <c r="I16" t="s">
         <v>752</v>
       </c>
-      <c r="J9">
+      <c r="J16">
         <v>5</v>
       </c>
-      <c r="L9" t="s">
+      <c r="L16" t="s">
         <v>755</v>
       </c>
-      <c r="M9">
+      <c r="M16">
         <v>8</v>
       </c>
-      <c r="P9" t="str">
+      <c r="P16" t="str">
         <f t="shared" si="2"/>
         <v xml:space="preserve">static const uint8_t lookupLEDpatternTbl[] PROGMEM = { 7, 5, 2, 1, 6, 11, 12, 254, </v>
       </c>
     </row>
-    <row r="10" spans="1:16">
-      <c r="A10">
+    <row r="17" spans="1:16">
+      <c r="A17">
         <v>9</v>
       </c>
-      <c r="B10">
+      <c r="B17">
         <f t="shared" si="0"/>
         <v>254</v>
       </c>
-      <c r="F10" t="s">
+      <c r="F17" t="s">
         <v>45</v>
       </c>
-      <c r="H10" t="str">
+      <c r="H17" t="str">
         <f t="shared" si="1"/>
         <v>|</v>
       </c>
-      <c r="I10" t="s">
+      <c r="I17" t="s">
         <v>753</v>
       </c>
-      <c r="J10">
+      <c r="J17">
         <v>6</v>
       </c>
-      <c r="L10" t="s">
+      <c r="L17" t="s">
         <v>760</v>
       </c>
-      <c r="M10">
+      <c r="M17">
         <v>9</v>
       </c>
-      <c r="P10" t="str">
+      <c r="P17" t="str">
         <f t="shared" si="2"/>
         <v xml:space="preserve">static const uint8_t lookupLEDpatternTbl[] PROGMEM = { 7, 5, 2, 1, 6, 11, 12, 254, 254, </v>
       </c>
     </row>
-    <row r="11" spans="1:16">
-      <c r="A11" t="s">
+    <row r="18" spans="1:16">
+      <c r="A18" t="s">
         <v>724</v>
       </c>
-      <c r="B11" t="str">
+      <c r="B18" t="str">
         <f t="shared" si="0"/>
         <v>skip</v>
       </c>
-      <c r="C11" t="s">
+      <c r="C18" t="s">
         <v>724</v>
       </c>
-      <c r="D11" t="s">
+      <c r="D18" t="s">
         <v>724</v>
       </c>
-      <c r="E11" t="s">
+      <c r="E18" t="s">
         <v>724</v>
       </c>
-      <c r="F11" t="s">
+      <c r="F18" t="s">
         <v>724</v>
       </c>
-      <c r="H11" t="str">
+      <c r="H18" t="str">
         <f t="shared" si="1"/>
         <v>skip|skip</v>
       </c>
-      <c r="I11" t="s">
+      <c r="I18" t="s">
         <v>754</v>
       </c>
-      <c r="J11">
+      <c r="J18">
         <v>7</v>
       </c>
-      <c r="L11" t="s">
+      <c r="L18" t="s">
         <v>761</v>
       </c>
-      <c r="M11">
+      <c r="M18">
         <v>10</v>
       </c>
-      <c r="P11" t="str">
+      <c r="P18" t="str">
         <f t="shared" si="2"/>
         <v xml:space="preserve">static const uint8_t lookupLEDpatternTbl[] PROGMEM = { 7, 5, 2, 1, 6, 11, 12, 254, 254, skip, </v>
       </c>
     </row>
-    <row r="12" spans="1:16">
-      <c r="A12">
+    <row r="19" spans="1:16">
+      <c r="A19">
         <v>11</v>
       </c>
-      <c r="B12">
+      <c r="B19">
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
-      <c r="C12" t="s">
+      <c r="C19" t="s">
         <v>732</v>
       </c>
-      <c r="F12" t="s">
+      <c r="F19" t="s">
         <v>44</v>
       </c>
-      <c r="H12" t="str">
+      <c r="H19" t="str">
         <f t="shared" si="1"/>
         <v>RBG_RailGunEffect(tmpInit, &amp;led_BLUE);|</v>
       </c>
-      <c r="I12" t="s">
+      <c r="I19" t="s">
         <v>755</v>
       </c>
-      <c r="J12">
+      <c r="J19">
         <v>8</v>
       </c>
-      <c r="L12" t="s">
+      <c r="L19" t="s">
         <v>756</v>
       </c>
-      <c r="M12">
+      <c r="M19">
         <v>11</v>
       </c>
-      <c r="P12" t="str">
+      <c r="P19" t="str">
         <f t="shared" si="2"/>
         <v xml:space="preserve">static const uint8_t lookupLEDpatternTbl[] PROGMEM = { 7, 5, 2, 1, 6, 11, 12, 254, 254, skip, 8, </v>
       </c>
     </row>
-    <row r="13" spans="1:16">
-      <c r="A13">
+    <row r="20" spans="1:16">
+      <c r="A20">
         <v>12</v>
       </c>
-      <c r="B13">
+      <c r="B20">
         <f t="shared" si="0"/>
         <v>9</v>
       </c>
-      <c r="C13" t="s">
+      <c r="C20" t="s">
         <v>758</v>
       </c>
-      <c r="F13" t="s">
+      <c r="F20" t="s">
         <v>44</v>
       </c>
-      <c r="H13" t="str">
+      <c r="H20" t="str">
         <f t="shared" si="1"/>
         <v>RBG_RailGunEffect(tmpInit, &amp;led_RED);|</v>
       </c>
-      <c r="I13" t="s">
+      <c r="I20" t="s">
         <v>761</v>
       </c>
-      <c r="J13">
+      <c r="J20">
         <v>10</v>
       </c>
-      <c r="L13" t="s">
+      <c r="L20" t="s">
         <v>763</v>
       </c>
-      <c r="M13">
+      <c r="M20">
         <v>12</v>
       </c>
-      <c r="P13" t="str">
+      <c r="P20" t="str">
         <f t="shared" si="2"/>
         <v xml:space="preserve">static const uint8_t lookupLEDpatternTbl[] PROGMEM = { 7, 5, 2, 1, 6, 11, 12, 254, 254, skip, 8, 9, </v>
       </c>
     </row>
-    <row r="14" spans="1:16">
-      <c r="A14">
+    <row r="21" spans="1:16">
+      <c r="A21">
         <v>13</v>
       </c>
-      <c r="B14">
+      <c r="B21">
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
-      <c r="C14" t="s">
+      <c r="C21" t="s">
         <v>759</v>
       </c>
-      <c r="F14" t="s">
+      <c r="F21" t="s">
         <v>44</v>
       </c>
-      <c r="H14" t="str">
+      <c r="H21" t="str">
         <f t="shared" si="1"/>
         <v>RBG_RailGunEffect(tmpInit, &amp;led_GREEN);|</v>
       </c>
-      <c r="I14" t="s">
+      <c r="I21" t="s">
         <v>760</v>
       </c>
-      <c r="J14">
+      <c r="J21">
         <v>9</v>
       </c>
-      <c r="L14" t="s">
+      <c r="L21" t="s">
         <v>766</v>
       </c>
-      <c r="M14">
+      <c r="M21">
         <v>13</v>
       </c>
-      <c r="P14" t="str">
+      <c r="P21" t="str">
         <f t="shared" si="2"/>
         <v xml:space="preserve">static const uint8_t lookupLEDpatternTbl[] PROGMEM = { 7, 5, 2, 1, 6, 11, 12, 254, 254, skip, 8, 9, 10, </v>
       </c>
     </row>
-    <row r="15" spans="1:16">
-      <c r="A15">
+    <row r="22" spans="1:16">
+      <c r="A22">
         <v>14</v>
       </c>
-      <c r="B15">
+      <c r="B22">
         <f t="shared" si="0"/>
         <v>11</v>
       </c>
-      <c r="C15" t="s">
+      <c r="C22" t="s">
         <v>746</v>
       </c>
-      <c r="F15" t="s">
+      <c r="F22" t="s">
         <v>44</v>
       </c>
-      <c r="H15" t="str">
+      <c r="H22" t="str">
         <f t="shared" si="1"/>
         <v>RBG_confetti_fadeby(128);|</v>
       </c>
-      <c r="I15" t="s">
+      <c r="I22" t="s">
         <v>757</v>
       </c>
-      <c r="J15" t="s">
+      <c r="J22" t="s">
         <v>724</v>
       </c>
-      <c r="P15" t="str">
+      <c r="P22" t="str">
         <f t="shared" si="2"/>
         <v xml:space="preserve">static const uint8_t lookupLEDpatternTbl[] PROGMEM = { 7, 5, 2, 1, 6, 11, 12, 254, 254, skip, 8, 9, 10, 11, </v>
       </c>
     </row>
-    <row r="16" spans="1:16">
-      <c r="A16">
+    <row r="23" spans="1:16">
+      <c r="A23">
         <v>15</v>
       </c>
-      <c r="B16">
+      <c r="B23">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="C16" t="s">
+      <c r="C23" t="s">
         <v>739</v>
       </c>
-      <c r="F16" t="s">
+      <c r="F23" t="s">
         <v>44</v>
       </c>
-      <c r="H16" t="str">
+      <c r="H23" t="str">
         <f t="shared" si="1"/>
         <v>juggle();|</v>
       </c>
-      <c r="I16" t="s">
+      <c r="I23" t="s">
         <v>766</v>
       </c>
-      <c r="J16">
+      <c r="J23">
         <v>13</v>
       </c>
-      <c r="P16" t="str">
+      <c r="P23" t="str">
         <f t="shared" si="2"/>
         <v xml:space="preserve">static const uint8_t lookupLEDpatternTbl[] PROGMEM = { 7, 5, 2, 1, 6, 11, 12, 254, 254, skip, 8, 9, 10, 11, 1, </v>
       </c>
     </row>
-    <row r="17" spans="1:16">
-      <c r="A17">
+    <row r="24" spans="1:16">
+      <c r="A24">
         <v>16</v>
       </c>
-      <c r="B17">
+      <c r="B24">
         <f t="shared" si="0"/>
         <v>7</v>
       </c>
-      <c r="C17" t="s">
+      <c r="C24" t="s">
         <v>734</v>
       </c>
-      <c r="F17" t="s">
+      <c r="F24" t="s">
         <v>44</v>
       </c>
-      <c r="H17" t="str">
+      <c r="H24" t="str">
         <f t="shared" si="1"/>
         <v>RBG_juggle_numdot_ring(5); RBG_confetti_fadeby(128);|</v>
       </c>
-      <c r="P17" t="str">
+      <c r="P24" t="str">
         <f t="shared" si="2"/>
         <v xml:space="preserve">static const uint8_t lookupLEDpatternTbl[] PROGMEM = { 7, 5, 2, 1, 6, 11, 12, 254, 254, skip, 8, 9, 10, 11, 1, 7, </v>
       </c>
     </row>
-    <row r="18" spans="1:16">
-      <c r="A18">
+    <row r="25" spans="1:16">
+      <c r="A25">
         <v>17</v>
       </c>
-      <c r="B18">
+      <c r="B25">
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="C18" t="s">
+      <c r="C25" t="s">
         <v>727</v>
       </c>
-      <c r="D18" t="s">
+      <c r="D25" t="s">
         <v>728</v>
       </c>
-      <c r="F18" t="s">
+      <c r="F25" t="s">
         <v>44</v>
       </c>
-      <c r="H18" t="str">
+      <c r="H25" t="str">
         <f t="shared" si="1"/>
         <v>RBG_diskDownTheDrainOrRotate(2);|RBG_ringRotateAndFade(mNONE, 0, windup1BrightSpots); numSteps</v>
       </c>
-      <c r="P18" t="str">
+      <c r="P25" t="str">
         <f t="shared" si="2"/>
         <v xml:space="preserve">static const uint8_t lookupLEDpatternTbl[] PROGMEM = { 7, 5, 2, 1, 6, 11, 12, 254, 254, skip, 8, 9, 10, 11, 1, 7, 5, </v>
       </c>
     </row>
-    <row r="19" spans="1:16">
-      <c r="A19">
+    <row r="26" spans="1:16">
+      <c r="A26">
         <v>18</v>
       </c>
-      <c r="B19">
+      <c r="B26">
         <f t="shared" si="0"/>
         <v>12</v>
       </c>
-      <c r="C19" t="s">
+      <c r="C26" t="s">
         <v>762</v>
       </c>
-      <c r="F19" t="s">
+      <c r="F26" t="s">
         <v>44</v>
       </c>
-      <c r="H19" t="str">
+      <c r="H26" t="str">
         <f t="shared" si="1"/>
         <v>bpm();|</v>
       </c>
-      <c r="P19" t="str">
+      <c r="P26" t="str">
         <f t="shared" si="2"/>
         <v xml:space="preserve">static const uint8_t lookupLEDpatternTbl[] PROGMEM = { 7, 5, 2, 1, 6, 11, 12, 254, 254, skip, 8, 9, 10, 11, 1, 7, 5, 12, </v>
       </c>
     </row>
-    <row r="20" spans="1:16">
-      <c r="A20">
+    <row r="27" spans="1:16">
+      <c r="A27">
         <v>19</v>
       </c>
-      <c r="B20">
+      <c r="B27">
         <f t="shared" si="0"/>
         <v>254</v>
       </c>
-      <c r="F20" t="s">
+      <c r="F27" t="s">
         <v>724</v>
       </c>
-      <c r="H20" t="str">
+      <c r="H27" t="str">
         <f t="shared" si="1"/>
         <v>|</v>
       </c>
-      <c r="P20" t="str">
+      <c r="P27" t="str">
         <f t="shared" si="2"/>
         <v xml:space="preserve">static const uint8_t lookupLEDpatternTbl[] PROGMEM = { 7, 5, 2, 1, 6, 11, 12, 254, 254, skip, 8, 9, 10, 11, 1, 7, 5, 12, 254, </v>
       </c>
     </row>
-    <row r="21" spans="1:16">
-      <c r="A21" t="s">
+    <row r="28" spans="1:16">
+      <c r="A28" t="s">
         <v>724</v>
       </c>
-      <c r="B21" t="str">
+      <c r="B28" t="str">
         <f t="shared" si="0"/>
         <v>skip</v>
       </c>
-      <c r="C21" t="s">
+      <c r="C28" t="s">
         <v>724</v>
       </c>
-      <c r="D21" t="s">
+      <c r="D28" t="s">
         <v>724</v>
       </c>
-      <c r="E21" t="s">
+      <c r="E28" t="s">
         <v>724</v>
       </c>
-      <c r="F21" t="s">
+      <c r="F28" t="s">
         <v>33</v>
       </c>
-      <c r="H21" t="str">
+      <c r="H28" t="str">
         <f t="shared" si="1"/>
         <v>skip|skip</v>
       </c>
-      <c r="P21" t="str">
+      <c r="P28" t="str">
         <f t="shared" si="2"/>
         <v xml:space="preserve">static const uint8_t lookupLEDpatternTbl[] PROGMEM = { 7, 5, 2, 1, 6, 11, 12, 254, 254, skip, 8, 9, 10, 11, 1, 7, 5, 12, 254, skip, </v>
       </c>
     </row>
-    <row r="22" spans="1:16">
-      <c r="A22">
+    <row r="29" spans="1:16">
+      <c r="A29">
         <v>21</v>
       </c>
-      <c r="B22">
+      <c r="B29">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="C22" t="s">
+      <c r="C29" t="s">
         <v>730</v>
       </c>
-      <c r="D22" t="s">
+      <c r="D29" t="s">
         <v>729</v>
       </c>
-      <c r="E22" t="s">
+      <c r="E29" t="s">
         <v>738</v>
       </c>
-      <c r="F22" t="s">
+      <c r="F29" t="s">
         <v>33</v>
       </c>
-      <c r="H22" t="str">
+      <c r="H29" t="str">
         <f t="shared" si="1"/>
         <v>RBG_diskDownTheDrainOrRotate(-1);|RBG_ringRotateAndFade(mNONE, 0, windup1BrightSpots); &amp; drain()</v>
       </c>
-      <c r="P22" t="str">
+      <c r="P29" t="str">
         <f t="shared" si="2"/>
         <v xml:space="preserve">static const uint8_t lookupLEDpatternTbl[] PROGMEM = { 7, 5, 2, 1, 6, 11, 12, 254, 254, skip, 8, 9, 10, 11, 1, 7, 5, 12, 254, skip, 4, </v>
       </c>
     </row>
-    <row r="23" spans="1:16">
-      <c r="A23">
+    <row r="30" spans="1:16">
+      <c r="A30">
         <v>22</v>
       </c>
-      <c r="B23">
+      <c r="B30">
         <f t="shared" si="0"/>
         <v>11</v>
       </c>
-      <c r="C23" t="s">
+      <c r="C30" t="s">
         <v>746</v>
       </c>
-      <c r="F23" t="s">
+      <c r="F30" t="s">
         <v>33</v>
       </c>
-      <c r="H23" t="str">
+      <c r="H30" t="str">
         <f t="shared" si="1"/>
         <v>RBG_confetti_fadeby(128);|</v>
       </c>
-      <c r="P23" t="str">
+      <c r="P30" t="str">
         <f t="shared" si="2"/>
         <v xml:space="preserve">static const uint8_t lookupLEDpatternTbl[] PROGMEM = { 7, 5, 2, 1, 6, 11, 12, 254, 254, skip, 8, 9, 10, 11, 1, 7, 5, 12, 254, skip, 4, 11, </v>
       </c>
     </row>
-    <row r="24" spans="1:16">
-      <c r="A24">
+    <row r="31" spans="1:16">
+      <c r="A31">
         <v>23</v>
       </c>
-      <c r="B24">
+      <c r="B31">
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
-      <c r="C24" t="s">
+      <c r="C31" t="s">
         <v>735</v>
       </c>
-      <c r="F24" t="s">
+      <c r="F31" t="s">
         <v>33</v>
       </c>
-      <c r="H24" t="str">
+      <c r="H31" t="str">
         <f t="shared" si="1"/>
         <v>rainbowWithGlitter();|</v>
       </c>
-      <c r="P24" t="str">
+      <c r="P31" t="str">
         <f t="shared" si="2"/>
         <v xml:space="preserve">static const uint8_t lookupLEDpatternTbl[] PROGMEM = { 7, 5, 2, 1, 6, 11, 12, 254, 254, skip, 8, 9, 10, 11, 1, 7, 5, 12, 254, skip, 4, 11, 2, </v>
       </c>
     </row>
-    <row r="25" spans="1:16">
-      <c r="A25">
+    <row r="32" spans="1:16">
+      <c r="A32">
         <v>24</v>
       </c>
-      <c r="B25">
+      <c r="B32">
         <f t="shared" si="0"/>
         <v>7</v>
       </c>
-      <c r="C25" t="s">
+      <c r="C32" t="s">
         <v>734</v>
       </c>
-      <c r="F25" t="s">
+      <c r="F32" t="s">
         <v>33</v>
       </c>
-      <c r="H25" t="str">
+      <c r="H32" t="str">
         <f t="shared" si="1"/>
         <v>RBG_juggle_numdot_ring(5); RBG_confetti_fadeby(128);|</v>
       </c>
-      <c r="P25" t="str">
+      <c r="P32" t="str">
         <f t="shared" si="2"/>
         <v xml:space="preserve">static const uint8_t lookupLEDpatternTbl[] PROGMEM = { 7, 5, 2, 1, 6, 11, 12, 254, 254, skip, 8, 9, 10, 11, 1, 7, 5, 12, 254, skip, 4, 11, 2, 7, </v>
       </c>
     </row>
-    <row r="26" spans="1:16">
-      <c r="A26">
+    <row r="33" spans="1:16">
+      <c r="A33">
         <v>25</v>
       </c>
-      <c r="B26">
+      <c r="B33">
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="C26" t="s">
+      <c r="C33" t="s">
         <v>727</v>
       </c>
-      <c r="D26" t="s">
+      <c r="D33" t="s">
         <v>728</v>
       </c>
-      <c r="F26" t="s">
+      <c r="F33" t="s">
         <v>33</v>
       </c>
-      <c r="H26" t="str">
+      <c r="H33" t="str">
         <f t="shared" si="1"/>
         <v>RBG_diskDownTheDrainOrRotate(2);|RBG_ringRotateAndFade(mNONE, 0, windup1BrightSpots); numSteps</v>
       </c>
-      <c r="P26" t="str">
+      <c r="P33" t="str">
         <f t="shared" si="2"/>
         <v xml:space="preserve">static const uint8_t lookupLEDpatternTbl[] PROGMEM = { 7, 5, 2, 1, 6, 11, 12, 254, 254, skip, 8, 9, 10, 11, 1, 7, 5, 12, 254, skip, 4, 11, 2, 7, 5, </v>
       </c>
     </row>
-    <row r="27" spans="1:16">
-      <c r="A27">
+    <row r="34" spans="1:16">
+      <c r="A34">
         <v>26</v>
       </c>
-      <c r="B27">
+      <c r="B34">
         <f t="shared" si="0"/>
         <v>13</v>
       </c>
-      <c r="C27" t="s">
+      <c r="C34" t="s">
         <v>765</v>
       </c>
-      <c r="F27" t="s">
+      <c r="F34" t="s">
         <v>33</v>
       </c>
-      <c r="H27" t="str">
+      <c r="H34" t="str">
         <f t="shared" si="1"/>
         <v>confetti();|</v>
       </c>
-      <c r="P27" t="str">
+      <c r="P34" t="str">
         <f t="shared" si="2"/>
         <v xml:space="preserve">static const uint8_t lookupLEDpatternTbl[] PROGMEM = { 7, 5, 2, 1, 6, 11, 12, 254, 254, skip, 8, 9, 10, 11, 1, 7, 5, 12, 254, skip, 4, 11, 2, 7, 5, 13, </v>
       </c>
     </row>
-    <row r="28" spans="1:16">
-      <c r="A28">
+    <row r="35" spans="1:16">
+      <c r="A35">
         <v>27</v>
       </c>
-      <c r="B28">
+      <c r="B35">
         <f t="shared" si="0"/>
         <v>254</v>
       </c>
-      <c r="F28" t="s">
+      <c r="F35" t="s">
         <v>33</v>
       </c>
-      <c r="H28" t="str">
+      <c r="H35" t="str">
         <f t="shared" si="1"/>
         <v>|</v>
       </c>
-      <c r="P28" t="str">
+      <c r="P35" t="str">
         <f t="shared" si="2"/>
         <v xml:space="preserve">static const uint8_t lookupLEDpatternTbl[] PROGMEM = { 7, 5, 2, 1, 6, 11, 12, 254, 254, skip, 8, 9, 10, 11, 1, 7, 5, 12, 254, skip, 4, 11, 2, 7, 5, 13, 254, </v>
       </c>
     </row>
-    <row r="29" spans="1:16">
-      <c r="A29">
+    <row r="36" spans="1:16">
+      <c r="A36">
         <v>28</v>
       </c>
-      <c r="B29">
+      <c r="B36">
         <f t="shared" si="0"/>
         <v>254</v>
       </c>
-      <c r="F29" t="s">
+      <c r="F36" t="s">
         <v>33</v>
       </c>
-      <c r="H29" t="str">
+      <c r="H36" t="str">
         <f t="shared" si="1"/>
         <v>|</v>
       </c>
-      <c r="P29" t="str">
+      <c r="P36" t="str">
         <f t="shared" si="2"/>
         <v xml:space="preserve">static const uint8_t lookupLEDpatternTbl[] PROGMEM = { 7, 5, 2, 1, 6, 11, 12, 254, 254, skip, 8, 9, 10, 11, 1, 7, 5, 12, 254, skip, 4, 11, 2, 7, 5, 13, 254, 254, </v>
       </c>
     </row>
-    <row r="30" spans="1:16">
-      <c r="A30">
+    <row r="37" spans="1:16">
+      <c r="A37">
         <v>29</v>
       </c>
-      <c r="B30">
+      <c r="B37">
         <f t="shared" si="0"/>
         <v>254</v>
       </c>
-      <c r="F30" t="s">
+      <c r="F37" t="s">
         <v>33</v>
       </c>
-      <c r="H30" t="str">
+      <c r="H37" t="str">
         <f t="shared" si="1"/>
         <v>|</v>
       </c>
-      <c r="P30" t="str">
+      <c r="P37" t="str">
         <f t="shared" si="2"/>
         <v xml:space="preserve">static const uint8_t lookupLEDpatternTbl[] PROGMEM = { 7, 5, 2, 1, 6, 11, 12, 254, 254, skip, 8, 9, 10, 11, 1, 7, 5, 12, 254, skip, 4, 11, 2, 7, 5, 13, 254, 254, 254, </v>
       </c>
     </row>
-    <row r="31" spans="1:16">
-      <c r="A31" t="s">
+    <row r="38" spans="1:16">
+      <c r="A38" t="s">
         <v>724</v>
       </c>
-      <c r="B31" t="str">
+      <c r="B38" t="str">
         <f t="shared" si="0"/>
         <v>skip</v>
       </c>
-      <c r="C31" t="s">
+      <c r="C38" t="s">
         <v>724</v>
       </c>
-      <c r="D31" t="s">
+      <c r="D38" t="s">
         <v>724</v>
       </c>
-      <c r="E31" t="s">
+      <c r="E38" t="s">
         <v>724</v>
       </c>
-      <c r="F31" t="s">
+      <c r="F38" t="s">
         <v>724</v>
       </c>
-      <c r="H31" t="str">
+      <c r="H38" t="str">
         <f t="shared" si="1"/>
         <v>skip|skip</v>
       </c>
-      <c r="P31" t="str">
+      <c r="P38" t="str">
         <f t="shared" si="2"/>
         <v xml:space="preserve">static const uint8_t lookupLEDpatternTbl[] PROGMEM = { 7, 5, 2, 1, 6, 11, 12, 254, 254, skip, 8, 9, 10, 11, 1, 7, 5, 12, 254, skip, 4, 11, 2, 7, 5, 13, 254, 254, 254, skip, </v>
       </c>
     </row>
-    <row r="32" spans="1:16">
-      <c r="A32">
+    <row r="39" spans="1:16">
+      <c r="A39">
         <v>31</v>
       </c>
-      <c r="B32">
+      <c r="B39">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="C32" t="s">
+      <c r="C39" t="s">
         <v>730</v>
       </c>
-      <c r="D32" t="s">
+      <c r="D39" t="s">
         <v>729</v>
       </c>
-      <c r="E32" t="s">
+      <c r="E39" t="s">
         <v>738</v>
       </c>
-      <c r="F32" t="s">
+      <c r="F39" t="s">
         <v>34</v>
       </c>
-      <c r="H32" t="str">
+      <c r="H39" t="str">
         <f t="shared" si="1"/>
         <v>RBG_diskDownTheDrainOrRotate(-1);|RBG_ringRotateAndFade(mNONE, 0, windup1BrightSpots); &amp; drain()</v>
       </c>
-      <c r="P32" t="str">
+      <c r="P39" t="str">
         <f t="shared" si="2"/>
         <v xml:space="preserve">static const uint8_t lookupLEDpatternTbl[] PROGMEM = { 7, 5, 2, 1, 6, 11, 12, 254, 254, skip, 8, 9, 10, 11, 1, 7, 5, 12, 254, skip, 4, 11, 2, 7, 5, 13, 254, 254, 254, skip, 4, </v>
       </c>
     </row>
-    <row r="33" spans="1:16">
-      <c r="A33">
+    <row r="40" spans="1:16">
+      <c r="A40">
         <v>32</v>
       </c>
-      <c r="B33">
+      <c r="B40">
         <f t="shared" si="0"/>
         <v>11</v>
       </c>
-      <c r="C33" t="s">
+      <c r="C40" t="s">
         <v>746</v>
       </c>
-      <c r="F33" t="s">
+      <c r="F40" t="s">
         <v>34</v>
       </c>
-      <c r="H33" t="str">
+      <c r="H40" t="str">
         <f t="shared" si="1"/>
         <v>RBG_confetti_fadeby(128);|</v>
       </c>
-      <c r="P33" t="str">
+      <c r="P40" t="str">
         <f t="shared" si="2"/>
         <v xml:space="preserve">static const uint8_t lookupLEDpatternTbl[] PROGMEM = { 7, 5, 2, 1, 6, 11, 12, 254, 254, skip, 8, 9, 10, 11, 1, 7, 5, 12, 254, skip, 4, 11, 2, 7, 5, 13, 254, 254, 254, skip, 4, 11, </v>
       </c>
     </row>
-    <row r="34" spans="1:16">
-      <c r="A34">
+    <row r="41" spans="1:16">
+      <c r="A41">
         <v>33</v>
       </c>
-      <c r="B34">
-        <f t="shared" ref="B34:B60" si="3">VLOOKUP(H34,LEDlookup,2,FALSE)</f>
+      <c r="B41">
+        <f t="shared" ref="B41:B67" si="3">VLOOKUP(H41,LEDlookup,2,FALSE)</f>
         <v>2</v>
       </c>
-      <c r="C34" t="s">
+      <c r="C41" t="s">
         <v>735</v>
       </c>
-      <c r="F34" t="s">
+      <c r="F41" t="s">
         <v>34</v>
       </c>
-      <c r="H34" t="str">
+      <c r="H41" t="str">
         <f t="shared" si="1"/>
         <v>rainbowWithGlitter();|</v>
       </c>
-      <c r="P34" t="str">
+      <c r="P41" t="str">
         <f t="shared" si="2"/>
         <v xml:space="preserve">static const uint8_t lookupLEDpatternTbl[] PROGMEM = { 7, 5, 2, 1, 6, 11, 12, 254, 254, skip, 8, 9, 10, 11, 1, 7, 5, 12, 254, skip, 4, 11, 2, 7, 5, 13, 254, 254, 254, skip, 4, 11, 2, </v>
       </c>
     </row>
-    <row r="35" spans="1:16">
-      <c r="A35">
+    <row r="42" spans="1:16">
+      <c r="A42">
         <v>34</v>
       </c>
-      <c r="B35">
+      <c r="B42">
         <f t="shared" si="3"/>
         <v>7</v>
       </c>
-      <c r="C35" t="s">
+      <c r="C42" t="s">
         <v>734</v>
       </c>
-      <c r="F35" t="s">
+      <c r="F42" t="s">
         <v>34</v>
       </c>
-      <c r="H35" t="str">
+      <c r="H42" t="str">
         <f t="shared" si="1"/>
         <v>RBG_juggle_numdot_ring(5); RBG_confetti_fadeby(128);|</v>
       </c>
-      <c r="P35" t="str">
+      <c r="P42" t="str">
         <f t="shared" si="2"/>
         <v xml:space="preserve">static const uint8_t lookupLEDpatternTbl[] PROGMEM = { 7, 5, 2, 1, 6, 11, 12, 254, 254, skip, 8, 9, 10, 11, 1, 7, 5, 12, 254, skip, 4, 11, 2, 7, 5, 13, 254, 254, 254, skip, 4, 11, 2, 7, </v>
       </c>
     </row>
-    <row r="36" spans="1:16">
-      <c r="A36">
+    <row r="43" spans="1:16">
+      <c r="A43">
         <v>35</v>
       </c>
-      <c r="B36">
+      <c r="B43">
         <f t="shared" si="3"/>
         <v>5</v>
       </c>
-      <c r="C36" t="s">
+      <c r="C43" t="s">
         <v>727</v>
       </c>
-      <c r="D36" t="s">
+      <c r="D43" t="s">
         <v>728</v>
       </c>
-      <c r="F36" t="s">
+      <c r="F43" t="s">
         <v>34</v>
       </c>
-      <c r="H36" t="str">
+      <c r="H43" t="str">
         <f t="shared" si="1"/>
         <v>RBG_diskDownTheDrainOrRotate(2);|RBG_ringRotateAndFade(mNONE, 0, windup1BrightSpots); numSteps</v>
       </c>
-      <c r="P36" t="str">
+      <c r="P43" t="str">
         <f t="shared" si="2"/>
         <v xml:space="preserve">static const uint8_t lookupLEDpatternTbl[] PROGMEM = { 7, 5, 2, 1, 6, 11, 12, 254, 254, skip, 8, 9, 10, 11, 1, 7, 5, 12, 254, skip, 4, 11, 2, 7, 5, 13, 254, 254, 254, skip, 4, 11, 2, 7, 5, </v>
       </c>
     </row>
-    <row r="37" spans="1:16">
-      <c r="A37">
+    <row r="44" spans="1:16">
+      <c r="A44">
         <v>36</v>
       </c>
-      <c r="B37">
+      <c r="B44">
         <f t="shared" si="3"/>
         <v>13</v>
       </c>
-      <c r="C37" t="s">
+      <c r="C44" t="s">
         <v>765</v>
       </c>
-      <c r="F37" t="s">
+      <c r="F44" t="s">
         <v>34</v>
       </c>
-      <c r="H37" t="str">
+      <c r="H44" t="str">
         <f t="shared" si="1"/>
         <v>confetti();|</v>
       </c>
-      <c r="P37" t="str">
+      <c r="P44" t="str">
         <f t="shared" si="2"/>
         <v xml:space="preserve">static const uint8_t lookupLEDpatternTbl[] PROGMEM = { 7, 5, 2, 1, 6, 11, 12, 254, 254, skip, 8, 9, 10, 11, 1, 7, 5, 12, 254, skip, 4, 11, 2, 7, 5, 13, 254, 254, 254, skip, 4, 11, 2, 7, 5, 13, </v>
       </c>
     </row>
-    <row r="38" spans="1:16">
-      <c r="A38">
+    <row r="45" spans="1:16">
+      <c r="A45">
         <v>37</v>
       </c>
-      <c r="B38">
+      <c r="B45">
         <f t="shared" si="3"/>
         <v>254</v>
       </c>
-      <c r="F38" t="s">
+      <c r="F45" t="s">
         <v>34</v>
       </c>
-      <c r="H38" t="str">
+      <c r="H45" t="str">
         <f t="shared" si="1"/>
         <v>|</v>
       </c>
-      <c r="P38" t="str">
+      <c r="P45" t="str">
         <f t="shared" si="2"/>
         <v xml:space="preserve">static const uint8_t lookupLEDpatternTbl[] PROGMEM = { 7, 5, 2, 1, 6, 11, 12, 254, 254, skip, 8, 9, 10, 11, 1, 7, 5, 12, 254, skip, 4, 11, 2, 7, 5, 13, 254, 254, 254, skip, 4, 11, 2, 7, 5, 13, 254, </v>
       </c>
     </row>
-    <row r="39" spans="1:16">
-      <c r="A39">
+    <row r="46" spans="1:16">
+      <c r="A46">
         <v>38</v>
       </c>
-      <c r="B39">
+      <c r="B46">
         <f t="shared" si="3"/>
         <v>254</v>
       </c>
-      <c r="F39" t="s">
+      <c r="F46" t="s">
         <v>34</v>
       </c>
-      <c r="H39" t="str">
+      <c r="H46" t="str">
         <f t="shared" si="1"/>
         <v>|</v>
       </c>
-      <c r="P39" t="str">
+      <c r="P46" t="str">
         <f t="shared" si="2"/>
         <v xml:space="preserve">static const uint8_t lookupLEDpatternTbl[] PROGMEM = { 7, 5, 2, 1, 6, 11, 12, 254, 254, skip, 8, 9, 10, 11, 1, 7, 5, 12, 254, skip, 4, 11, 2, 7, 5, 13, 254, 254, 254, skip, 4, 11, 2, 7, 5, 13, 254, 254, </v>
       </c>
     </row>
-    <row r="40" spans="1:16">
-      <c r="A40">
+    <row r="47" spans="1:16">
+      <c r="A47">
         <v>39</v>
       </c>
-      <c r="B40">
+      <c r="B47">
         <f t="shared" si="3"/>
         <v>254</v>
       </c>
-      <c r="F40" t="s">
+      <c r="F47" t="s">
         <v>34</v>
       </c>
-      <c r="H40" t="str">
+      <c r="H47" t="str">
         <f t="shared" si="1"/>
         <v>|</v>
       </c>
-      <c r="P40" t="str">
+      <c r="P47" t="str">
         <f t="shared" si="2"/>
         <v xml:space="preserve">static const uint8_t lookupLEDpatternTbl[] PROGMEM = { 7, 5, 2, 1, 6, 11, 12, 254, 254, skip, 8, 9, 10, 11, 1, 7, 5, 12, 254, skip, 4, 11, 2, 7, 5, 13, 254, 254, 254, skip, 4, 11, 2, 7, 5, 13, 254, 254, 254, </v>
       </c>
     </row>
-    <row r="41" spans="1:16">
-      <c r="A41" t="s">
+    <row r="48" spans="1:16">
+      <c r="A48" t="s">
         <v>724</v>
       </c>
-      <c r="B41" t="str">
+      <c r="B48" t="str">
         <f t="shared" si="3"/>
         <v>skip</v>
       </c>
-      <c r="C41" t="s">
+      <c r="C48" t="s">
         <v>724</v>
       </c>
-      <c r="D41" t="s">
+      <c r="D48" t="s">
         <v>724</v>
       </c>
-      <c r="E41" t="s">
+      <c r="E48" t="s">
         <v>724</v>
       </c>
-      <c r="F41" t="s">
+      <c r="F48" t="s">
         <v>724</v>
       </c>
-      <c r="H41" t="str">
+      <c r="H48" t="str">
         <f t="shared" si="1"/>
         <v>skip|skip</v>
       </c>
-      <c r="P41" t="str">
+      <c r="P48" t="str">
         <f t="shared" si="2"/>
         <v xml:space="preserve">static const uint8_t lookupLEDpatternTbl[] PROGMEM = { 7, 5, 2, 1, 6, 11, 12, 254, 254, skip, 8, 9, 10, 11, 1, 7, 5, 12, 254, skip, 4, 11, 2, 7, 5, 13, 254, 254, 254, skip, 4, 11, 2, 7, 5, 13, 254, 254, 254, skip, </v>
       </c>
     </row>
-    <row r="42" spans="1:16">
-      <c r="A42">
+    <row r="49" spans="1:16">
+      <c r="A49">
         <v>41</v>
       </c>
-      <c r="B42">
+      <c r="B49">
         <f t="shared" si="3"/>
         <v>5</v>
       </c>
-      <c r="C42" t="s">
+      <c r="C49" t="s">
         <v>727</v>
       </c>
-      <c r="D42" t="s">
+      <c r="D49" t="s">
         <v>728</v>
       </c>
-      <c r="F42" t="s">
+      <c r="F49" t="s">
         <v>32</v>
       </c>
-      <c r="H42" t="str">
+      <c r="H49" t="str">
         <f t="shared" si="1"/>
         <v>RBG_diskDownTheDrainOrRotate(2);|RBG_ringRotateAndFade(mNONE, 0, windup1BrightSpots); numSteps</v>
       </c>
-      <c r="P42" t="str">
+      <c r="P49" t="str">
         <f t="shared" si="2"/>
         <v xml:space="preserve">static const uint8_t lookupLEDpatternTbl[] PROGMEM = { 7, 5, 2, 1, 6, 11, 12, 254, 254, skip, 8, 9, 10, 11, 1, 7, 5, 12, 254, skip, 4, 11, 2, 7, 5, 13, 254, 254, 254, skip, 4, 11, 2, 7, 5, 13, 254, 254, 254, skip, 5, </v>
       </c>
     </row>
-    <row r="43" spans="1:16">
-      <c r="A43">
+    <row r="50" spans="1:16">
+      <c r="A50">
         <v>42</v>
       </c>
-      <c r="B43">
+      <c r="B50">
         <f t="shared" si="3"/>
         <v>6</v>
       </c>
-      <c r="C43" t="s">
+      <c r="C50" t="s">
         <v>741</v>
       </c>
-      <c r="E43" t="s">
+      <c r="E50" t="s">
         <v>742</v>
       </c>
-      <c r="F43" t="s">
+      <c r="F50" t="s">
         <v>32</v>
       </c>
-      <c r="H43" t="str">
+      <c r="H50" t="str">
         <f t="shared" si="1"/>
         <v>RBG_juggle_numdot_ring(-4);|</v>
       </c>
-      <c r="P43" t="str">
+      <c r="P50" t="str">
         <f t="shared" si="2"/>
         <v xml:space="preserve">static const uint8_t lookupLEDpatternTbl[] PROGMEM = { 7, 5, 2, 1, 6, 11, 12, 254, 254, skip, 8, 9, 10, 11, 1, 7, 5, 12, 254, skip, 4, 11, 2, 7, 5, 13, 254, 254, 254, skip, 4, 11, 2, 7, 5, 13, 254, 254, 254, skip, 5, 6, </v>
       </c>
     </row>
-    <row r="44" spans="1:16">
-      <c r="A44">
+    <row r="51" spans="1:16">
+      <c r="A51">
         <v>43</v>
       </c>
-      <c r="B44">
+      <c r="B51">
         <f t="shared" si="3"/>
         <v>3</v>
       </c>
-      <c r="C44" t="s">
+      <c r="C51" t="s">
         <v>740</v>
       </c>
-      <c r="F44" t="s">
+      <c r="F51" t="s">
         <v>32</v>
       </c>
-      <c r="H44" t="str">
+      <c r="H51" t="str">
         <f t="shared" si="1"/>
         <v>RBG_bpm_rings();|</v>
       </c>
-      <c r="P44" t="str">
+      <c r="P51" t="str">
         <f t="shared" si="2"/>
         <v xml:space="preserve">static const uint8_t lookupLEDpatternTbl[] PROGMEM = { 7, 5, 2, 1, 6, 11, 12, 254, 254, skip, 8, 9, 10, 11, 1, 7, 5, 12, 254, skip, 4, 11, 2, 7, 5, 13, 254, 254, 254, skip, 4, 11, 2, 7, 5, 13, 254, 254, 254, skip, 5, 6, 3, </v>
       </c>
     </row>
-    <row r="45" spans="1:16">
-      <c r="A45">
+    <row r="52" spans="1:16">
+      <c r="A52">
         <v>44</v>
       </c>
-      <c r="B45">
+      <c r="B52">
         <f t="shared" si="3"/>
         <v>1</v>
       </c>
-      <c r="C45" t="s">
+      <c r="C52" t="s">
         <v>739</v>
       </c>
-      <c r="F45" t="s">
+      <c r="F52" t="s">
         <v>32</v>
       </c>
-      <c r="H45" t="str">
+      <c r="H52" t="str">
         <f t="shared" si="1"/>
         <v>juggle();|</v>
       </c>
-      <c r="P45" t="str">
+      <c r="P52" t="str">
         <f t="shared" si="2"/>
         <v xml:space="preserve">static const uint8_t lookupLEDpatternTbl[] PROGMEM = { 7, 5, 2, 1, 6, 11, 12, 254, 254, skip, 8, 9, 10, 11, 1, 7, 5, 12, 254, skip, 4, 11, 2, 7, 5, 13, 254, 254, 254, skip, 4, 11, 2, 7, 5, 13, 254, 254, 254, skip, 5, 6, 3, 1, </v>
       </c>
     </row>
-    <row r="46" spans="1:16">
-      <c r="A46">
+    <row r="53" spans="1:16">
+      <c r="A53">
         <v>45</v>
       </c>
-      <c r="B46">
+      <c r="B53">
         <f t="shared" si="3"/>
         <v>11</v>
       </c>
-      <c r="C46" t="s">
+      <c r="C53" t="s">
         <v>746</v>
       </c>
-      <c r="F46" t="s">
+      <c r="F53" t="s">
         <v>32</v>
       </c>
-      <c r="H46" t="str">
+      <c r="H53" t="str">
         <f t="shared" si="1"/>
         <v>RBG_confetti_fadeby(128);|</v>
       </c>
-      <c r="P46" t="str">
+      <c r="P53" t="str">
         <f t="shared" si="2"/>
         <v xml:space="preserve">static const uint8_t lookupLEDpatternTbl[] PROGMEM = { 7, 5, 2, 1, 6, 11, 12, 254, 254, skip, 8, 9, 10, 11, 1, 7, 5, 12, 254, skip, 4, 11, 2, 7, 5, 13, 254, 254, 254, skip, 4, 11, 2, 7, 5, 13, 254, 254, 254, skip, 5, 6, 3, 1, 11, </v>
       </c>
     </row>
-    <row r="47" spans="1:16">
-      <c r="A47">
+    <row r="54" spans="1:16">
+      <c r="A54">
         <v>46</v>
       </c>
-      <c r="B47">
+      <c r="B54">
         <f t="shared" si="3"/>
         <v>2</v>
       </c>
-      <c r="C47" t="s">
+      <c r="C54" t="s">
         <v>735</v>
       </c>
-      <c r="F47" t="s">
+      <c r="F54" t="s">
         <v>32</v>
       </c>
-      <c r="H47" t="str">
+      <c r="H54" t="str">
         <f t="shared" si="1"/>
         <v>rainbowWithGlitter();|</v>
       </c>
-      <c r="P47" t="str">
+      <c r="P54" t="str">
         <f t="shared" si="2"/>
         <v xml:space="preserve">static const uint8_t lookupLEDpatternTbl[] PROGMEM = { 7, 5, 2, 1, 6, 11, 12, 254, 254, skip, 8, 9, 10, 11, 1, 7, 5, 12, 254, skip, 4, 11, 2, 7, 5, 13, 254, 254, 254, skip, 4, 11, 2, 7, 5, 13, 254, 254, 254, skip, 5, 6, 3, 1, 11, 2, </v>
       </c>
     </row>
-    <row r="48" spans="1:16">
-      <c r="A48">
+    <row r="55" spans="1:16">
+      <c r="A55">
         <v>47</v>
       </c>
-      <c r="B48">
+      <c r="B55">
         <f t="shared" si="3"/>
         <v>7</v>
       </c>
-      <c r="C48" t="s">
+      <c r="C55" t="s">
         <v>734</v>
       </c>
-      <c r="F48" t="s">
+      <c r="F55" t="s">
         <v>32</v>
       </c>
-      <c r="H48" t="str">
+      <c r="H55" t="str">
         <f t="shared" si="1"/>
         <v>RBG_juggle_numdot_ring(5); RBG_confetti_fadeby(128);|</v>
       </c>
-      <c r="P48" t="str">
+      <c r="P55" t="str">
         <f t="shared" si="2"/>
         <v xml:space="preserve">static const uint8_t lookupLEDpatternTbl[] PROGMEM = { 7, 5, 2, 1, 6, 11, 12, 254, 254, skip, 8, 9, 10, 11, 1, 7, 5, 12, 254, skip, 4, 11, 2, 7, 5, 13, 254, 254, 254, skip, 4, 11, 2, 7, 5, 13, 254, 254, 254, skip, 5, 6, 3, 1, 11, 2, 7, </v>
       </c>
     </row>
-    <row r="49" spans="1:16">
-      <c r="A49">
+    <row r="56" spans="1:16">
+      <c r="A56">
         <v>48</v>
       </c>
-      <c r="B49">
+      <c r="B56">
         <f t="shared" si="3"/>
         <v>254</v>
       </c>
-      <c r="F49" t="s">
+      <c r="F56" t="s">
         <v>32</v>
       </c>
-      <c r="H49" t="str">
+      <c r="H56" t="str">
         <f t="shared" si="1"/>
         <v>|</v>
       </c>
-      <c r="P49" t="str">
+      <c r="P56" t="str">
         <f t="shared" si="2"/>
         <v xml:space="preserve">static const uint8_t lookupLEDpatternTbl[] PROGMEM = { 7, 5, 2, 1, 6, 11, 12, 254, 254, skip, 8, 9, 10, 11, 1, 7, 5, 12, 254, skip, 4, 11, 2, 7, 5, 13, 254, 254, 254, skip, 4, 11, 2, 7, 5, 13, 254, 254, 254, skip, 5, 6, 3, 1, 11, 2, 7, 254, </v>
       </c>
     </row>
-    <row r="50" spans="1:16">
-      <c r="A50">
+    <row r="57" spans="1:16">
+      <c r="A57">
         <v>49</v>
       </c>
-      <c r="B50">
+      <c r="B57">
         <f t="shared" si="3"/>
         <v>254</v>
       </c>
-      <c r="F50" t="s">
+      <c r="F57" t="s">
         <v>32</v>
       </c>
-      <c r="H50" t="str">
+      <c r="H57" t="str">
         <f t="shared" si="1"/>
         <v>|</v>
       </c>
-      <c r="P50" t="str">
+      <c r="P57" t="str">
         <f t="shared" si="2"/>
         <v xml:space="preserve">static const uint8_t lookupLEDpatternTbl[] PROGMEM = { 7, 5, 2, 1, 6, 11, 12, 254, 254, skip, 8, 9, 10, 11, 1, 7, 5, 12, 254, skip, 4, 11, 2, 7, 5, 13, 254, 254, 254, skip, 4, 11, 2, 7, 5, 13, 254, 254, 254, skip, 5, 6, 3, 1, 11, 2, 7, 254, 254, </v>
       </c>
     </row>
-    <row r="51" spans="1:16">
-      <c r="A51" t="s">
+    <row r="58" spans="1:16">
+      <c r="A58" t="s">
         <v>724</v>
       </c>
-      <c r="B51" t="str">
+      <c r="B58" t="str">
         <f t="shared" si="3"/>
         <v>skip</v>
       </c>
-      <c r="C51" t="s">
+      <c r="C58" t="s">
         <v>724</v>
       </c>
-      <c r="D51" t="s">
+      <c r="D58" t="s">
         <v>724</v>
       </c>
-      <c r="E51" t="s">
+      <c r="E58" t="s">
         <v>724</v>
       </c>
-      <c r="F51" t="s">
+      <c r="F58" t="s">
         <v>724</v>
       </c>
-      <c r="H51" t="str">
+      <c r="H58" t="str">
         <f t="shared" si="1"/>
         <v>skip|skip</v>
       </c>
-      <c r="P51" t="str">
+      <c r="P58" t="str">
         <f t="shared" si="2"/>
         <v xml:space="preserve">static const uint8_t lookupLEDpatternTbl[] PROGMEM = { 7, 5, 2, 1, 6, 11, 12, 254, 254, skip, 8, 9, 10, 11, 1, 7, 5, 12, 254, skip, 4, 11, 2, 7, 5, 13, 254, 254, 254, skip, 4, 11, 2, 7, 5, 13, 254, 254, 254, skip, 5, 6, 3, 1, 11, 2, 7, 254, 254, skip, </v>
       </c>
     </row>
-    <row r="52" spans="1:16">
-      <c r="A52">
+    <row r="59" spans="1:16">
+      <c r="A59">
         <v>51</v>
       </c>
-      <c r="B52">
+      <c r="B59">
         <f t="shared" si="3"/>
         <v>6</v>
       </c>
-      <c r="C52" t="s">
+      <c r="C59" t="s">
         <v>741</v>
       </c>
-      <c r="E52" t="s">
+      <c r="E59" t="s">
         <v>742</v>
       </c>
-      <c r="F52" t="s">
+      <c r="F59" t="s">
         <v>601</v>
       </c>
-      <c r="H52" t="str">
+      <c r="H59" t="str">
         <f t="shared" si="1"/>
         <v>RBG_juggle_numdot_ring(-4);|</v>
       </c>
-      <c r="P52" t="str">
+      <c r="P59" t="str">
         <f t="shared" si="2"/>
         <v xml:space="preserve">static const uint8_t lookupLEDpatternTbl[] PROGMEM = { 7, 5, 2, 1, 6, 11, 12, 254, 254, skip, 8, 9, 10, 11, 1, 7, 5, 12, 254, skip, 4, 11, 2, 7, 5, 13, 254, 254, 254, skip, 4, 11, 2, 7, 5, 13, 254, 254, 254, skip, 5, 6, 3, 1, 11, 2, 7, 254, 254, skip, 6, </v>
       </c>
     </row>
-    <row r="53" spans="1:16">
-      <c r="A53">
+    <row r="60" spans="1:16">
+      <c r="A60">
         <v>52</v>
       </c>
-      <c r="B53">
+      <c r="B60">
         <f t="shared" si="3"/>
         <v>3</v>
       </c>
-      <c r="C53" t="s">
+      <c r="C60" t="s">
         <v>740</v>
       </c>
-      <c r="F53" t="s">
+      <c r="F60" t="s">
         <v>601</v>
       </c>
-      <c r="H53" t="str">
+      <c r="H60" t="str">
         <f t="shared" si="1"/>
         <v>RBG_bpm_rings();|</v>
       </c>
-      <c r="P53" t="str">
+      <c r="P60" t="str">
         <f t="shared" si="2"/>
         <v xml:space="preserve">static const uint8_t lookupLEDpatternTbl[] PROGMEM = { 7, 5, 2, 1, 6, 11, 12, 254, 254, skip, 8, 9, 10, 11, 1, 7, 5, 12, 254, skip, 4, 11, 2, 7, 5, 13, 254, 254, 254, skip, 4, 11, 2, 7, 5, 13, 254, 254, 254, skip, 5, 6, 3, 1, 11, 2, 7, 254, 254, skip, 6, 3, </v>
       </c>
     </row>
-    <row r="54" spans="1:16">
-      <c r="A54">
+    <row r="61" spans="1:16">
+      <c r="A61">
         <v>53</v>
       </c>
-      <c r="B54">
+      <c r="B61">
         <f t="shared" si="3"/>
         <v>5</v>
       </c>
-      <c r="C54" t="s">
+      <c r="C61" t="s">
         <v>727</v>
       </c>
-      <c r="D54" t="s">
+      <c r="D61" t="s">
         <v>728</v>
       </c>
-      <c r="E54" t="s">
+      <c r="E61" t="s">
         <v>737</v>
       </c>
-      <c r="F54" t="s">
+      <c r="F61" t="s">
         <v>601</v>
       </c>
-      <c r="H54" t="str">
+      <c r="H61" t="str">
         <f t="shared" si="1"/>
         <v>RBG_diskDownTheDrainOrRotate(2);|RBG_ringRotateAndFade(mNONE, 0, windup1BrightSpots); numSteps</v>
       </c>
-      <c r="P54" t="str">
+      <c r="P61" t="str">
         <f t="shared" si="2"/>
         <v xml:space="preserve">static const uint8_t lookupLEDpatternTbl[] PROGMEM = { 7, 5, 2, 1, 6, 11, 12, 254, 254, skip, 8, 9, 10, 11, 1, 7, 5, 12, 254, skip, 4, 11, 2, 7, 5, 13, 254, 254, 254, skip, 4, 11, 2, 7, 5, 13, 254, 254, 254, skip, 5, 6, 3, 1, 11, 2, 7, 254, 254, skip, 6, 3, 5, </v>
       </c>
     </row>
-    <row r="55" spans="1:16">
-      <c r="A55">
+    <row r="62" spans="1:16">
+      <c r="A62">
         <v>54</v>
       </c>
-      <c r="B55">
+      <c r="B62">
         <f t="shared" si="3"/>
         <v>1</v>
       </c>
-      <c r="C55" t="s">
+      <c r="C62" t="s">
         <v>739</v>
       </c>
-      <c r="F55" t="s">
+      <c r="F62" t="s">
         <v>601</v>
       </c>
-      <c r="H55" t="str">
+      <c r="H62" t="str">
         <f t="shared" si="1"/>
         <v>juggle();|</v>
       </c>
-      <c r="P55" t="str">
+      <c r="P62" t="str">
         <f t="shared" si="2"/>
         <v xml:space="preserve">static const uint8_t lookupLEDpatternTbl[] PROGMEM = { 7, 5, 2, 1, 6, 11, 12, 254, 254, skip, 8, 9, 10, 11, 1, 7, 5, 12, 254, skip, 4, 11, 2, 7, 5, 13, 254, 254, 254, skip, 4, 11, 2, 7, 5, 13, 254, 254, 254, skip, 5, 6, 3, 1, 11, 2, 7, 254, 254, skip, 6, 3, 5, 1, </v>
       </c>
     </row>
-    <row r="56" spans="1:16">
-      <c r="A56">
+    <row r="63" spans="1:16">
+      <c r="A63">
         <v>55</v>
       </c>
-      <c r="B56">
+      <c r="B63">
         <f t="shared" si="3"/>
         <v>11</v>
       </c>
-      <c r="C56" t="s">
+      <c r="C63" t="s">
         <v>746</v>
       </c>
-      <c r="F56" t="s">
+      <c r="F63" t="s">
         <v>601</v>
       </c>
-      <c r="H56" t="str">
+      <c r="H63" t="str">
         <f t="shared" si="1"/>
         <v>RBG_confetti_fadeby(128);|</v>
       </c>
-      <c r="P56" t="str">
+      <c r="P63" t="str">
         <f t="shared" si="2"/>
         <v xml:space="preserve">static const uint8_t lookupLEDpatternTbl[] PROGMEM = { 7, 5, 2, 1, 6, 11, 12, 254, 254, skip, 8, 9, 10, 11, 1, 7, 5, 12, 254, skip, 4, 11, 2, 7, 5, 13, 254, 254, 254, skip, 4, 11, 2, 7, 5, 13, 254, 254, 254, skip, 5, 6, 3, 1, 11, 2, 7, 254, 254, skip, 6, 3, 5, 1, 11, </v>
       </c>
     </row>
-    <row r="57" spans="1:16">
-      <c r="A57">
+    <row r="64" spans="1:16">
+      <c r="A64">
         <v>56</v>
       </c>
-      <c r="B57">
+      <c r="B64">
         <f t="shared" si="3"/>
         <v>2</v>
       </c>
-      <c r="C57" t="s">
+      <c r="C64" t="s">
         <v>735</v>
       </c>
-      <c r="F57" t="s">
+      <c r="F64" t="s">
         <v>601</v>
       </c>
-      <c r="H57" t="str">
+      <c r="H64" t="str">
         <f t="shared" si="1"/>
         <v>rainbowWithGlitter();|</v>
       </c>
-      <c r="P57" t="str">
+      <c r="P64" t="str">
         <f t="shared" si="2"/>
         <v xml:space="preserve">static const uint8_t lookupLEDpatternTbl[] PROGMEM = { 7, 5, 2, 1, 6, 11, 12, 254, 254, skip, 8, 9, 10, 11, 1, 7, 5, 12, 254, skip, 4, 11, 2, 7, 5, 13, 254, 254, 254, skip, 4, 11, 2, 7, 5, 13, 254, 254, 254, skip, 5, 6, 3, 1, 11, 2, 7, 254, 254, skip, 6, 3, 5, 1, 11, 2, </v>
       </c>
     </row>
-    <row r="58" spans="1:16">
-      <c r="A58">
+    <row r="65" spans="1:16">
+      <c r="A65">
         <v>57</v>
       </c>
-      <c r="B58">
+      <c r="B65">
         <f t="shared" si="3"/>
         <v>7</v>
       </c>
-      <c r="C58" t="s">
+      <c r="C65" t="s">
         <v>734</v>
       </c>
-      <c r="F58" t="s">
+      <c r="F65" t="s">
         <v>601</v>
       </c>
-      <c r="H58" t="str">
+      <c r="H65" t="str">
         <f t="shared" si="1"/>
         <v>RBG_juggle_numdot_ring(5); RBG_confetti_fadeby(128);|</v>
       </c>
-      <c r="P58" t="str">
+      <c r="P65" t="str">
         <f t="shared" si="2"/>
         <v xml:space="preserve">static const uint8_t lookupLEDpatternTbl[] PROGMEM = { 7, 5, 2, 1, 6, 11, 12, 254, 254, skip, 8, 9, 10, 11, 1, 7, 5, 12, 254, skip, 4, 11, 2, 7, 5, 13, 254, 254, 254, skip, 4, 11, 2, 7, 5, 13, 254, 254, 254, skip, 5, 6, 3, 1, 11, 2, 7, 254, 254, skip, 6, 3, 5, 1, 11, 2, 7, </v>
       </c>
     </row>
-    <row r="59" spans="1:16">
-      <c r="A59">
+    <row r="66" spans="1:16">
+      <c r="A66">
         <v>58</v>
       </c>
-      <c r="B59">
+      <c r="B66">
         <f t="shared" si="3"/>
         <v>254</v>
       </c>
-      <c r="F59" t="s">
+      <c r="F66" t="s">
         <v>601</v>
       </c>
-      <c r="H59" t="str">
+      <c r="H66" t="str">
         <f t="shared" si="1"/>
         <v>|</v>
       </c>
-      <c r="P59" t="str">
+      <c r="P66" t="str">
         <f t="shared" si="2"/>
         <v xml:space="preserve">static const uint8_t lookupLEDpatternTbl[] PROGMEM = { 7, 5, 2, 1, 6, 11, 12, 254, 254, skip, 8, 9, 10, 11, 1, 7, 5, 12, 254, skip, 4, 11, 2, 7, 5, 13, 254, 254, 254, skip, 4, 11, 2, 7, 5, 13, 254, 254, 254, skip, 5, 6, 3, 1, 11, 2, 7, 254, 254, skip, 6, 3, 5, 1, 11, 2, 7, 254, </v>
       </c>
     </row>
-    <row r="60" spans="1:16" ht="15.75" thickBot="1">
-      <c r="A60">
+    <row r="67" spans="1:16" ht="15.75" thickBot="1">
+      <c r="A67">
         <v>59</v>
       </c>
-      <c r="B60">
+      <c r="B67">
         <f t="shared" si="3"/>
         <v>254</v>
       </c>
-      <c r="F60" t="s">
+      <c r="F67" t="s">
         <v>601</v>
       </c>
-      <c r="H60" t="str">
+      <c r="H67" t="str">
         <f t="shared" si="1"/>
         <v>|</v>
       </c>
-      <c r="P60" t="str">
+      <c r="P67" t="str">
         <f t="shared" si="2"/>
         <v xml:space="preserve">static const uint8_t lookupLEDpatternTbl[] PROGMEM = { 7, 5, 2, 1, 6, 11, 12, 254, 254, skip, 8, 9, 10, 11, 1, 7, 5, 12, 254, skip, 4, 11, 2, 7, 5, 13, 254, 254, 254, skip, 4, 11, 2, 7, 5, 13, 254, 254, 254, skip, 5, 6, 3, 1, 11, 2, 7, 254, 254, skip, 6, 3, 5, 1, 11, 2, 7, 254, 254, </v>
       </c>
     </row>
-    <row r="61" spans="1:16" ht="16.5" thickTop="1" thickBot="1">
-      <c r="A61" s="1" t="s">
+    <row r="68" spans="1:16" ht="16.5" thickTop="1" thickBot="1">
+      <c r="A68" s="1" t="s">
         <v>725</v>
       </c>
-      <c r="B61" s="1" t="s">
+      <c r="B68" s="1" t="s">
         <v>725</v>
       </c>
-      <c r="C61" s="1" t="s">
+      <c r="C68" s="1" t="s">
         <v>725</v>
       </c>
-      <c r="D61" s="1" t="s">
+      <c r="D68" s="1" t="s">
         <v>725</v>
       </c>
-      <c r="E61" s="1" t="s">
+      <c r="E68" s="1" t="s">
         <v>725</v>
       </c>
-      <c r="F61" s="1" t="s">
+      <c r="F68" s="1" t="s">
         <v>725</v>
       </c>
     </row>
-    <row r="62" spans="1:16" ht="15.75" thickTop="1">
-      <c r="P62" t="str">
-        <f>SUBSTITUTE(SUBSTITUTE(P60,"skip","254")&amp;"};",", }"," }")</f>
+    <row r="69" spans="1:16" ht="15.75" thickTop="1">
+      <c r="P69" t="str">
+        <f>SUBSTITUTE(SUBSTITUTE(P67,"skip","254")&amp;"};",", }"," }")</f>
         <v>static const uint8_t lookupLEDpatternTbl[] PROGMEM = { 7, 5, 2, 1, 6, 11, 12, 254, 254, 254, 8, 9, 10, 11, 1, 7, 5, 12, 254, 254, 4, 11, 2, 7, 5, 13, 254, 254, 254, 254, 4, 11, 2, 7, 5, 13, 254, 254, 254, 254, 5, 6, 3, 1, 11, 2, 7, 254, 254, 254, 6, 3, 5, 1, 11, 2, 7, 254, 254 };</v>
       </c>
     </row>
+    <row r="82" spans="3:3" ht="51.75">
+      <c r="C82" s="95" t="s">
+        <v>6440</v>
+      </c>
+    </row>
+    <row r="83" spans="3:3" ht="30">
+      <c r="C83" s="96" t="s">
+        <v>6441</v>
+      </c>
+    </row>
+    <row r="84" spans="3:3">
+      <c r="C84" s="96" t="s">
+        <v>6442</v>
+      </c>
+    </row>
+    <row r="85" spans="3:3" ht="51.75">
+      <c r="C85" s="95" t="s">
+        <v>6443</v>
+      </c>
+    </row>
+    <row r="86" spans="3:3" ht="45">
+      <c r="C86" s="96" t="s">
+        <v>6444</v>
+      </c>
+    </row>
+    <row r="87" spans="3:3" ht="69">
+      <c r="C87" s="95" t="s">
+        <v>6445</v>
+      </c>
+    </row>
+    <row r="88" spans="3:3" ht="17.25">
+      <c r="C88" s="97" t="s">
+        <v>6446</v>
+      </c>
+    </row>
+    <row r="89" spans="3:3" ht="17.25">
+      <c r="C89" s="97" t="s">
+        <v>6447</v>
+      </c>
+    </row>
+    <row r="90" spans="3:3" ht="17.25">
+      <c r="C90" s="97" t="s">
+        <v>6448</v>
+      </c>
+    </row>
+    <row r="91" spans="3:3" ht="17.25">
+      <c r="C91" s="97" t="s">
+        <v>6449</v>
+      </c>
+    </row>
+    <row r="92" spans="3:3" ht="69">
+      <c r="C92" s="95" t="s">
+        <v>6450</v>
+      </c>
+    </row>
+    <row r="93" spans="3:3" ht="17.25">
+      <c r="C93" s="97" t="s">
+        <v>6451</v>
+      </c>
+    </row>
+    <row r="94" spans="3:3" ht="17.25">
+      <c r="C94" s="97" t="s">
+        <v>6452</v>
+      </c>
+    </row>
+    <row r="95" spans="3:3" ht="17.25">
+      <c r="C95" s="97" t="s">
+        <v>6453</v>
+      </c>
+    </row>
+    <row r="96" spans="3:3" ht="51.75">
+      <c r="C96" s="95" t="s">
+        <v>6454</v>
+      </c>
+    </row>
+    <row r="97" spans="3:3" ht="34.5">
+      <c r="C97" s="97" t="s">
+        <v>6455</v>
+      </c>
+    </row>
+    <row r="98" spans="3:3" ht="17.25">
+      <c r="C98" s="97" t="s">
+        <v>6456</v>
+      </c>
+    </row>
+    <row r="99" spans="3:3" ht="51.75">
+      <c r="C99" s="95" t="s">
+        <v>6457</v>
+      </c>
+    </row>
+    <row r="100" spans="3:3" ht="60">
+      <c r="C100" s="99" t="s">
+        <v>6458</v>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:M61" xr:uid="{5F43EA48-57E3-4717-B62B-57CBAB53DAAC}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="L2:M13">
-    <sortCondition ref="M2:M13"/>
+  <autoFilter ref="A8:M68" xr:uid="{5F43EA48-57E3-4717-B62B-57CBAB53DAAC}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="C82:C138">
+    <sortCondition ref="C82:C138"/>
   </sortState>
+  <hyperlinks>
+    <hyperlink ref="C83" r:id="rId1" xr:uid="{A4DE2DF6-FC3D-44A4-A845-9421CEF6A897}"/>
+    <hyperlink ref="C84" r:id="rId2" xr:uid="{3FFA6709-E399-4F9F-9569-608473B66B5F}"/>
+    <hyperlink ref="C86" r:id="rId3" xr:uid="{4A11A8AE-9487-4E79-A281-566AEB92E051}"/>
+    <hyperlink ref="C100" r:id="rId4" display="https://github.com/Mark-MDO47/GraduationCap2017" xr:uid="{BD957AB6-D9D3-4470-93D1-AF565570ACFE}"/>
+    <hyperlink ref="E1" r:id="rId5" xr:uid="{7ED12776-9590-4126-9385-BFCBFD5350E9}"/>
+    <hyperlink ref="G1" r:id="rId6" xr:uid="{D0A522B9-9F2C-4E9D-83FE-2D2CFF31963B}"/>
+    <hyperlink ref="F2" r:id="rId7" xr:uid="{684CD521-996A-4EBA-80F9-B655E6ABAF15}"/>
+    <hyperlink ref="F7" r:id="rId8" xr:uid="{4B71CD86-BD91-44FF-A59A-E552B20A441A}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId9"/>
 </worksheet>
 </file>
 
@@ -81928,7 +82180,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B7BCD6B9-C154-4F9D-B8BC-4D842A94058B}">
   <dimension ref="A1:AX30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView topLeftCell="G1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="O3" sqref="O3:O13"/>
     </sheetView>
   </sheetViews>

</xml_diff>